<commit_message>
region GL manual fix x4
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -67,7 +67,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"needs" + 0.007*"leaders" + 0.006*"practice" + 0.005*"within" + 0.005*"11" + 0.004*"plans" + 0.004*"senior" + 0.004*"15" + 0.004*"family"', '0.022*"’" + 0.008*"within" + 0.007*"leaders" + 0.007*"needs" + 0.007*"Barnsley" + 0.006*"practice" + 0.004*"2023" + 0.004*"response" + 0.004*"senior" + 0.004*"appropriate"', '0.019*"’" + 0.009*"needs" + 0.007*"leaders" + 0.006*"Barnsley" + 0.006*"practice" + 0.005*"within" + 0.005*"plans" + 0.004*"understand" + 0.004*"response" + 0.004*"September"']</t>
+    <t>['0.020*"’" + 0.007*"needs" + 0.007*"within" + 0.006*"Barnsley" + 0.006*"leaders" + 0.006*"response" + 0.005*"practice" + 0.005*"11" + 0.005*"plans" + 0.004*"15"', '0.017*"’" + 0.010*"leaders" + 0.009*"needs" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"within" + 0.005*"understand" + 0.004*"2023" + 0.004*"11" + 0.004*"plans"', '0.019*"’" + 0.007*"needs" + 0.007*"within" + 0.006*"leaders" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"quality" + 0.005*"2023" + 0.004*"plans" + 0.004*"senior"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -106,7 +106,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"well" + 0.006*"practice" + 0.005*"receive" + 0.005*"Bath" + 0.005*"leaders" + 0.005*"East" + 0.005*"‘" + 0.004*"effective" + 0.004*"needs"', '0.018*"’" + 0.008*"well" + 0.005*"needs" + 0.005*"clear" + 0.005*"practice" + 0.005*"plans" + 0.004*"receive" + 0.004*"4" + 0.004*"2022" + 0.004*"leaders"', '0.018*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"impact" + 0.005*"effective" + 0.005*"leaders" + 0.005*"Somerset" + 0.005*"practice" + 0.005*"North"']</t>
+    <t>['0.020*"’" + 0.010*"well" + 0.007*"practice" + 0.006*"needs" + 0.005*"4" + 0.005*"leaders" + 0.005*"plans" + 0.005*"impact" + 0.005*"clear" + 0.005*"Somerset"', '0.018*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"plans" + 0.005*"East" + 0.005*"protection" + 0.004*"leaders" + 0.004*"‘" + 0.004*"2022"', '0.014*"’" + 0.009*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"effective" + 0.005*"leaders" + 0.005*"receive" + 0.005*"Bath" + 0.004*"North" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -151,7 +151,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.006*"needs" + 0.006*"ensure" + 0.006*"supported" + 0.006*"plans" + 0.005*"well" + 0.005*"good" + 0.004*"Bedford" + 0.004*"need" + 0.004*"progress"', '0.018*"’" + 0.008*"needs" + 0.005*"ensure" + 0.005*"Bedford" + 0.005*"progress" + 0.005*"relationships" + 0.004*"well" + 0.004*"plans" + 0.004*"made" + 0.004*"education"', '0.018*"’" + 0.007*"ensure" + 0.006*"well" + 0.006*"needs" + 0.006*"Bedford" + 0.005*"good" + 0.005*"family" + 0.005*"plans" + 0.005*"education" + 0.005*"Borough"']</t>
+    <t>['0.018*"’" + 0.007*"needs" + 0.006*"ensure" + 0.006*"Bedford" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"supported" + 0.005*"Borough" + 0.005*"family"', '0.015*"’" + 0.005*"needs" + 0.005*"well" + 0.005*"ensure" + 0.005*"good" + 0.005*"plans" + 0.004*"Bedford" + 0.004*"supported" + 0.004*"need" + 0.004*"education"', '0.022*"’" + 0.007*"needs" + 0.007*"ensure" + 0.006*"well" + 0.005*"plans" + 0.005*"supported" + 0.005*"good" + 0.005*"made" + 0.005*"relationships" + 0.005*"15"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -193,7 +193,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"needs" + 0.006*"Birmingham" + 0.006*"well" + 0.006*"plans" + 0.006*"trust" + 0.005*"progress" + 0.004*"effective" + 0.004*"risk" + 0.004*"leaders"', '0.014*"’" + 0.011*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"effective" + 0.006*"progress" + 0.006*"Birmingham" + 0.005*"3" + 0.005*"trust" + 0.005*"appropriate"', '0.016*"’" + 0.008*"effective" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"trust" + 0.005*"appropriate" + 0.005*"Birmingham" + 0.005*"3"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.008*"effective" + 0.006*"well" + 0.006*"Birmingham" + 0.006*"plans" + 0.005*"trust" + 0.005*"3" + 0.004*"leaders" + 0.004*"20"', '0.015*"’" + 0.009*"needs" + 0.007*"effective" + 0.007*"well" + 0.006*"plans" + 0.006*"appropriate" + 0.005*"3" + 0.005*"progress" + 0.005*"risk" + 0.005*"trust"', '0.017*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Birmingham" + 0.006*"progress" + 0.006*"plans" + 0.006*"trust" + 0.005*"effective" + 0.005*"risk" + 0.005*"appropriate"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -232,7 +232,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"practice" + 0.007*"needs" + 0.007*"Darwen" + 0.006*"impact" + 0.006*"Blackburn" + 0.006*"quality" + 0.005*"well" + 0.005*"2022" + 0.005*"planning"', '0.017*"’" + 0.008*"needs" + 0.008*"quality" + 0.007*"practice" + 0.007*"well" + 0.007*"impact" + 0.006*"Darwen" + 0.006*"result" + 0.005*"planning" + 0.005*"Blackburn"', '0.011*"’" + 0.009*"Blackburn" + 0.007*"needs" + 0.007*"quality" + 0.006*"Darwen" + 0.005*"means" + 0.005*"practice" + 0.005*"well" + 0.005*"plans" + 0.005*"24"']</t>
+    <t>['0.009*"’" + 0.006*"practice" + 0.005*"quality" + 0.005*"needs" + 0.004*"impact" + 0.004*"well" + 0.004*"Blackburn" + 0.004*"plans" + 0.004*"Darwen" + 0.004*"means"', '0.011*"’" + 0.007*"practice" + 0.007*"well" + 0.007*"Darwen" + 0.007*"needs" + 0.006*"quality" + 0.006*"means" + 0.006*"Blackburn" + 0.005*"result" + 0.005*"impact"', '0.018*"’" + 0.009*"needs" + 0.008*"Blackburn" + 0.008*"quality" + 0.007*"practice" + 0.007*"impact" + 0.007*"Darwen" + 0.006*"well" + 0.006*"planning" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -271,7 +271,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"well" + 0.009*"needs" + 0.006*"Blackpool" + 0.005*"supported" + 0.004*"2022" + 0.004*"effective" + 0.004*"practice" + 0.004*"16" + 0.004*"response"', '0.021*"’" + 0.009*"needs" + 0.008*"Blackpool" + 0.008*"well" + 0.006*"effective" + 0.006*"practice" + 0.005*"5" + 0.005*"plans" + 0.005*"16" + 0.005*"experiences"', '0.014*"’" + 0.013*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.006*"effective" + 0.005*"plans" + 0.005*"quality" + 0.005*"carers" + 0.005*"good" + 0.005*"supported"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"Blackpool" + 0.005*"plans" + 0.005*"effective" + 0.005*"quality" + 0.005*"practice" + 0.004*"16" + 0.004*"need"', '0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"Blackpool" + 0.006*"effective" + 0.005*"plans" + 0.005*"16" + 0.005*"progress" + 0.004*"quality" + 0.004*"experiences"', '0.017*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"Blackpool" + 0.006*"supported" + 0.006*"practice" + 0.005*"experiences" + 0.005*"5" + 0.005*"16" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>350</t>
@@ -295,7 +295,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"Bolton" + 0.005*"supported" + 0.004*"planning" + 0.004*"2023" + 0.004*"strong" + 0.004*"11"', '0.017*"’" + 0.009*"well" + 0.009*"needs" + 0.006*"plans" + 0.006*"Bolton" + 0.005*"supported" + 0.005*"September" + 0.004*"11" + 0.004*"strong" + 0.004*"effective"', '0.023*"’" + 0.010*"Bolton" + 0.010*"needs" + 0.009*"plans" + 0.008*"well" + 0.007*"need" + 0.006*"supported" + 0.006*"planning" + 0.005*"response" + 0.005*"timely"']</t>
+    <t>['0.016*"’" + 0.008*"well" + 0.008*"Bolton" + 0.007*"plans" + 0.006*"needs" + 0.005*"planning" + 0.004*"need" + 0.004*"11" + 0.004*"risk" + 0.004*"strong"', '0.019*"’" + 0.011*"needs" + 0.008*"Bolton" + 0.007*"well" + 0.006*"plans" + 0.005*"effective" + 0.005*"11" + 0.005*"protection" + 0.005*"strong" + 0.005*"need"', '0.020*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"plans" + 0.008*"Bolton" + 0.007*"supported" + 0.006*"need" + 0.005*"planning" + 0.005*"response" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -331,7 +331,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"quality" + 0.005*"risk" + 0.005*"practice" + 0.005*"progress" + 0.005*"well" + 0.005*"Christchurch" + 0.005*"Bournemouth" + 0.004*"impact" + 0.004*"Poole"', '0.015*"’" + 0.007*"quality" + 0.005*"practice" + 0.005*"progress" + 0.004*"impact" + 0.004*"6" + 0.004*"17" + 0.004*"risk" + 0.004*"Poole" + 0.004*"Christchurch"', '0.021*"’" + 0.006*"practice" + 0.006*"17" + 0.005*"However" + 0.005*"progress" + 0.005*"time" + 0.005*"quality" + 0.005*"Poole" + 0.005*"6" + 0.004*"Bournemouth"']</t>
+    <t>['0.013*"’" + 0.005*"quality" + 0.004*"17" + 0.004*"well" + 0.004*"Poole" + 0.004*"6" + 0.004*"right" + 0.004*"practice" + 0.003*"However" + 0.003*"2021"', '0.014*"’" + 0.006*"quality" + 0.005*"practice" + 0.005*"Christchurch" + 0.005*"Bournemouth" + 0.005*"17" + 0.005*"progress" + 0.005*"many" + 0.005*"6" + 0.004*"Poole"', '0.023*"’" + 0.007*"practice" + 0.006*"progress" + 0.006*"quality" + 0.006*"time" + 0.005*"impact" + 0.005*"risk" + 0.005*"number" + 0.004*"However" + 0.004*"Bournemouth"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -370,7 +370,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"Bracknell" + 0.006*"good" + 0.005*"provided" + 0.005*"Forest" + 0.005*"needs" + 0.005*"risk" + 0.005*"impact" + 0.004*"effective" + 0.004*"plans"', '0.013*"’" + 0.008*"Forest" + 0.007*"risk" + 0.007*"quality" + 0.007*"well" + 0.006*"plans" + 0.006*"Bracknell" + 0.006*"needs" + 0.006*"good" + 0.005*"need"', '0.020*"’" + 0.008*"needs" + 0.007*"Bracknell" + 0.007*"effective" + 0.007*"progress" + 0.006*"Forest" + 0.006*"risk" + 0.006*"good" + 0.006*"quality" + 0.005*"need"']</t>
+    <t>['0.019*"’" + 0.008*"risk" + 0.006*"Forest" + 0.006*"Bracknell" + 0.005*"leaders" + 0.005*"quality" + 0.005*"plans" + 0.005*"impact" + 0.005*"provided" + 0.005*"progress"', '0.017*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"Forest" + 0.006*"good" + 0.006*"quality" + 0.006*"provided" + 0.006*"positive" + 0.006*"Bracknell" + 0.005*"progress"', '0.013*"’" + 0.008*"Bracknell" + 0.007*"risk" + 0.006*"needs" + 0.006*"Forest" + 0.006*"good" + 0.006*"quality" + 0.006*"well" + 0.005*"plans" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>846</t>
@@ -403,7 +403,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.008*"good" + 0.006*"well" + 0.006*"recording" + 0.005*"leaders" + 0.005*"need" + 0.005*"However" + 0.005*"plans" + 0.004*"ensure"', '0.014*"’" + 0.011*"needs" + 0.009*"good" + 0.006*"well" + 0.006*"leaders" + 0.005*"plans" + 0.005*"recording" + 0.005*"However" + 0.004*"need" + 0.004*"strong"', '0.014*"’" + 0.008*"good" + 0.008*"needs" + 0.006*"recording" + 0.005*"leaders" + 0.005*"well" + 0.005*"need" + 0.005*"timely" + 0.005*"Hove" + 0.004*"improve"']</t>
+    <t>['0.015*"’" + 0.008*"good" + 0.008*"needs" + 0.006*"leaders" + 0.005*"well" + 0.005*"need" + 0.005*"recording" + 0.004*"plans" + 0.004*"ensure" + 0.004*"improve"', '0.015*"’" + 0.010*"needs" + 0.007*"good" + 0.007*"recording" + 0.006*"well" + 0.005*"leaders" + 0.005*"need" + 0.005*"plans" + 0.005*"Hove" + 0.005*"arrangements"', '0.011*"’" + 0.009*"good" + 0.009*"needs" + 0.006*"recording" + 0.005*"plans" + 0.005*"well" + 0.005*"However" + 0.005*"leaders" + 0.004*"effectively" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -436,7 +436,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.007*"Bristol" + 0.007*"good" + 0.006*"needs" + 0.005*"health" + 0.005*"need" + 0.005*"progress" + 0.004*"leaders" + 0.004*"receive"', '0.019*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"Bristol" + 0.006*"good" + 0.006*"plans" + 0.005*"always" + 0.005*"health" + 0.005*"16" + 0.005*"progress"', '0.020*"’" + 0.009*"good" + 0.009*"well" + 0.007*"needs" + 0.007*"Bristol" + 0.005*"progress" + 0.005*"need" + 0.005*"health" + 0.005*"receive" + 0.005*"leaders"']</t>
+    <t>['0.024*"’" + 0.009*"good" + 0.008*"well" + 0.007*"needs" + 0.007*"Bristol" + 0.005*"need" + 0.005*"plans" + 0.005*"16" + 0.005*"receive" + 0.005*"health"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"Bristol" + 0.006*"health" + 0.005*"progress" + 0.005*"good" + 0.005*"leaders" + 0.004*"January" + 0.004*"plans"', '0.017*"’" + 0.010*"well" + 0.009*"good" + 0.008*"Bristol" + 0.007*"needs" + 0.005*"progress" + 0.005*"health" + 0.004*"need" + 0.004*"2023" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -463,7 +463,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"plans" + 0.005*"Buckinghamshire" + 0.004*"number" + 0.004*"6" + 0.004*"many" + 0.004*"December" + 0.004*"17" + 0.003*"2021" + 0.003*"protection"', '0.015*"’" + 0.005*"plans" + 0.004*"protection" + 0.004*"number" + 0.004*"17" + 0.004*"December" + 0.004*"6" + 0.004*"many" + 0.004*"2021" + 0.004*"Buckinghamshire"', '0.011*"’" + 0.005*"number" + 0.005*"17" + 0.005*"Buckinghamshire" + 0.004*"practice" + 0.004*"plans" + 0.004*"needs" + 0.004*"well" + 0.004*"many" + 0.004*"protection"']</t>
+    <t>['0.015*"’" + 0.005*"plans" + 0.005*"number" + 0.005*"Buckinghamshire" + 0.005*"17" + 0.004*"6" + 0.004*"2021" + 0.004*"many" + 0.004*"December" + 0.004*"well"', '0.012*"’" + 0.005*"plans" + 0.005*"number" + 0.004*"Buckinghamshire" + 0.004*"protection" + 0.004*"6" + 0.004*"practice" + 0.004*"17" + 0.003*"December" + 0.003*"2021"', '0.013*"’" + 0.005*"17" + 0.004*"many" + 0.004*"plans" + 0.004*"number" + 0.004*"needs" + 0.004*"protection" + 0.004*"practice" + 0.004*"Buckinghamshire" + 0.004*"teams"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -499,7 +499,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"needs" + 0.006*"protection" + 0.005*"2021" + 0.005*"impact" + 0.005*"practice" + 0.005*"need" + 0.004*"response" + 0.004*"Bury" + 0.004*"team"', '0.011*"’" + 0.008*"2021" + 0.007*"protection" + 0.007*"needs" + 0.006*"practice" + 0.005*"team" + 0.005*"delay" + 0.005*"impact" + 0.005*"November" + 0.005*"risk"', '0.012*"’" + 0.007*"team" + 0.006*"2021" + 0.005*"protection" + 0.005*"quality" + 0.005*"needs" + 0.005*"practice" + 0.005*"need" + 0.005*"risk" + 0.005*"October"']</t>
+    <t>['0.011*"’" + 0.007*"2021" + 0.007*"practice" + 0.006*"team" + 0.006*"protection" + 0.006*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"Bury" + 0.005*"impact"', '0.014*"’" + 0.007*"needs" + 0.007*"protection" + 0.006*"2021" + 0.006*"team" + 0.005*"risk" + 0.005*"need" + 0.005*"practice" + 0.005*"impact" + 0.005*"progress"', '0.009*"’" + 0.007*"needs" + 0.006*"protection" + 0.006*"2021" + 0.005*"impact" + 0.005*"new" + 0.005*"5" + 0.005*"drift" + 0.005*"timely" + 0.004*"team"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -529,7 +529,7 @@
     <t>0.1954</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"well" + 0.005*"good" + 0.005*"protection" + 0.004*"effective" + 0.004*"Calderdale" + 0.004*"‘" + 0.004*"inform" + 0.004*"need" + 0.004*"needs"', '0.016*"’" + 0.008*"well" + 0.005*"practice" + 0.005*"good" + 0.004*"Calderdale" + 0.004*"effective" + 0.004*"needs" + 0.004*"protection" + 0.003*"risk" + 0.003*"inform"', '0.014*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"Calderdale" + 0.005*"good" + 0.005*"carers" + 0.005*"effective" + 0.005*"protection" + 0.005*"‘" + 0.004*"education"']</t>
+    <t>['0.013*"’" + 0.007*"well" + 0.005*"Calderdale" + 0.005*"effective" + 0.004*"protection" + 0.004*"need" + 0.004*"inform" + 0.004*"‘" + 0.004*"good" + 0.003*"practice"', '0.009*"’" + 0.007*"well" + 0.005*"good" + 0.005*"practice" + 0.005*"effective" + 0.004*"protection" + 0.004*"Calderdale" + 0.004*"carers" + 0.004*"education" + 0.004*"leaders"', '0.019*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"good" + 0.006*"Calderdale" + 0.004*"‘" + 0.004*"carers" + 0.004*"protection" + 0.004*"education" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -562,7 +562,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"good" + 0.006*"need" + 0.006*"teams" + 0.006*"progress" + 0.006*"impact" + 0.005*"quality" + 0.005*"However"', '0.010*"’" + 0.008*"impact" + 0.007*"good" + 0.007*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"effective" + 0.005*"need" + 0.005*"teams" + 0.005*"practice"', '0.017*"’" + 0.012*"well" + 0.010*"good" + 0.008*"need" + 0.008*"teams" + 0.007*"plans" + 0.007*"impact" + 0.007*"needs" + 0.007*"quality" + 0.006*"However"']</t>
+    <t>['0.015*"’" + 0.011*"well" + 0.010*"good" + 0.009*"need" + 0.008*"plans" + 0.007*"needs" + 0.007*"teams" + 0.006*"impact" + 0.006*"However" + 0.006*"quality"', '0.013*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"teams" + 0.008*"good" + 0.008*"impact" + 0.006*"plans" + 0.006*"need" + 0.006*"quality" + 0.005*"effective"', '0.014*"’" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"need" + 0.006*"impact" + 0.005*"progress" + 0.005*"quality" + 0.005*"plans" + 0.005*"However"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -592,7 +592,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"well" + 0.007*"good" + 0.007*"progress" + 0.007*"plans" + 0.006*"Central" + 0.006*"need" + 0.006*"needs" + 0.005*"carers" + 0.004*"Bedfordshire"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"need" + 0.007*"carers" + 0.006*"good" + 0.005*"effective" + 0.005*"plans" + 0.005*"progress" + 0.005*"Bedfordshire"', '0.013*"’" + 0.007*"carers" + 0.006*"needs" + 0.006*"well" + 0.005*"need" + 0.005*"information" + 0.005*"good" + 0.005*"Bedfordshire" + 0.005*"plans" + 0.005*"number"']</t>
+    <t>['0.017*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"need" + 0.007*"good" + 0.006*"carers" + 0.006*"Central" + 0.006*"plans" + 0.006*"progress" + 0.005*"Bedfordshire"', '0.017*"’" + 0.011*"well" + 0.007*"needs" + 0.007*"carers" + 0.006*"need" + 0.006*"good" + 0.006*"progress" + 0.005*"number" + 0.005*"effective" + 0.005*"protection"', '0.012*"’" + 0.008*"well" + 0.007*"plans" + 0.005*"needs" + 0.005*"Bedfordshire" + 0.005*"need" + 0.004*"progress" + 0.004*"carers" + 0.004*"education" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -628,7 +628,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"good" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"need" + 0.006*"ensure" + 0.006*"However" + 0.006*"timely" + 0.005*"progress"', '0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"practice" + 0.007*"plans" + 0.006*"good" + 0.006*"supported" + 0.006*"always" + 0.005*"need" + 0.005*"accommodation"', '0.013*"’" + 0.007*"good" + 0.007*"well" + 0.007*"plans" + 0.006*"practice" + 0.006*"needs" + 0.006*"effective" + 0.005*"always" + 0.005*"carers" + 0.005*"supported"']</t>
+    <t>['0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"practice" + 0.006*"always" + 0.005*"accommodation" + 0.005*"ensure" + 0.005*"carers" + 0.005*"However"', '0.012*"’" + 0.008*"needs" + 0.008*"plans" + 0.008*"good" + 0.008*"well" + 0.007*"practice" + 0.006*"risk" + 0.006*"supported" + 0.006*"need" + 0.006*"However"', '0.011*"’" + 0.008*"well" + 0.007*"good" + 0.006*"plans" + 0.005*"needs" + 0.005*"supported" + 0.005*"need" + 0.005*"effective" + 0.005*"practice" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -664,7 +664,7 @@
     <t>0.1816</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"practice" + 0.005*"However" + 0.004*"learning" + 0.004*"receive" + 0.004*"effectively" + 0.004*"timely" + 0.004*"impact"', '0.022*"’" + 0.008*"well" + 0.007*"needs" + 0.004*"effective" + 0.004*"always" + 0.004*"information" + 0.004*"plans" + 0.004*"order" + 0.004*"impact" + 0.004*"learning"', '0.018*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"plans" + 0.004*"order" + 0.004*"impact" + 0.004*"effectively" + 0.004*"always" + 0.004*"progress"']</t>
+    <t>['0.024*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"order" + 0.005*"always" + 0.004*"timely" + 0.004*"effective" + 0.004*"learning" + 0.004*"impact"', '0.021*"’" + 0.007*"needs" + 0.007*"well" + 0.004*"impact" + 0.004*"effective" + 0.004*"effectively" + 0.004*"progress" + 0.004*"plans" + 0.004*"early" + 0.004*"including"', '0.019*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"receive" + 0.004*"plans" + 0.004*"always" + 0.004*"effectively" + 0.004*"small" + 0.004*"learning"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -700,7 +700,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.008*"plans" + 0.005*"need" + 0.005*"risk" + 0.005*"2" + 0.005*"needs" + 0.005*"impact" + 0.005*"Bradford" + 0.004*"quality" + 0.004*"lack"', '0.021*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"Bradford" + 0.005*"2" + 0.005*"quality" + 0.005*"November" + 0.004*"practice" + 0.004*"21" + 0.004*"risk"', '0.013*"’" + 0.005*"plans" + 0.004*"Bradford" + 0.004*"◼" + 0.004*"impact" + 0.004*"needs" + 0.004*"lack" + 0.004*"2022" + 0.004*"21" + 0.003*"2"']</t>
+    <t>['0.018*"’" + 0.007*"plans" + 0.005*"Bradford" + 0.005*"need" + 0.005*"needs" + 0.005*"practice" + 0.004*"quality" + 0.004*"risk" + 0.004*"Borough" + 0.004*"City"', '0.018*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"impact" + 0.005*"risk" + 0.004*"need" + 0.004*"lack" + 0.004*"◼" + 0.004*"Bradford" + 0.004*"November"', '0.024*"’" + 0.006*"plans" + 0.006*"2" + 0.005*"2022" + 0.005*"Bradford" + 0.005*"quality" + 0.004*"21" + 0.004*"needs" + 0.004*"Council" + 0.004*"many"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -733,7 +733,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.012*"needs" + 0.010*"well" + 0.007*"effective" + 0.007*"ensure" + 0.006*"plans" + 0.005*"clear" + 0.005*"good" + 0.005*"experiences" + 0.005*"progress"', '0.009*"needs" + 0.008*"ensure" + 0.008*"’" + 0.008*"well" + 0.007*"clear" + 0.006*"effective" + 0.005*"progress" + 0.005*"practice" + 0.004*"good" + 0.004*"timely"', '0.013*"’" + 0.013*"needs" + 0.011*"well" + 0.010*"ensure" + 0.007*"progress" + 0.006*"effective" + 0.006*"good" + 0.006*"clear" + 0.006*"plans" + 0.006*"within"']</t>
+    <t>['0.013*"well" + 0.012*"’" + 0.010*"ensure" + 0.010*"needs" + 0.008*"effective" + 0.007*"progress" + 0.007*"clear" + 0.006*"good" + 0.005*"experiences" + 0.005*"plans"', '0.011*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"ensure" + 0.006*"effective" + 0.005*"good" + 0.004*"plans" + 0.004*"clear" + 0.004*"individual" + 0.004*"progress"', '0.014*"needs" + 0.012*"’" + 0.008*"well" + 0.008*"ensure" + 0.007*"clear" + 0.006*"plans" + 0.006*"effective" + 0.006*"progress" + 0.005*"good" + 0.005*"within"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -769,7 +769,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"November" + 0.006*"plans" + 0.006*"Wakefield" + 0.006*"quality" + 0.006*"receive" + 0.005*"practice" + 0.005*"leaders" + 0.005*"19"', '0.019*"’" + 0.009*"leaders" + 0.009*"quality" + 0.007*"well" + 0.007*"Wakefield" + 0.007*"effective" + 0.006*"November" + 0.006*"good" + 0.006*"needs" + 0.006*"receive"', '0.017*"’" + 0.009*"Wakefield" + 0.009*"good" + 0.008*"November" + 0.007*"well" + 0.007*"effective" + 0.007*"plans" + 0.007*"quality" + 0.006*"leaders" + 0.006*"practice"']</t>
+    <t>['0.016*"’" + 0.010*"November" + 0.008*"leaders" + 0.007*"well" + 0.006*"Wakefield" + 0.006*"effective" + 0.006*"plans" + 0.005*"practice" + 0.005*"progress" + 0.005*"quality"', '0.020*"’" + 0.008*"quality" + 0.008*"well" + 0.008*"effective" + 0.008*"Wakefield" + 0.007*"good" + 0.007*"leaders" + 0.006*"practice" + 0.006*"plans" + 0.006*"needs"', '0.012*"’" + 0.009*"Wakefield" + 0.008*"quality" + 0.007*"good" + 0.007*"leaders" + 0.007*"well" + 0.007*"November" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -799,7 +799,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"effective" + 0.005*"March" + 0.005*"However" + 0.005*"York" + 0.005*"plans" + 0.005*"education" + 0.005*"need"', '0.019*"’" + 0.008*"quality" + 0.008*"March" + 0.007*"needs" + 0.007*"effective" + 0.006*"ensure" + 0.006*"However" + 0.006*"York" + 0.005*"7" + 0.005*"well"', '0.009*"’" + 0.007*"March" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"good" + 0.005*"ensure" + 0.004*"well" + 0.004*"plans" + 0.004*"York"']</t>
+    <t>['0.014*"’" + 0.009*"quality" + 0.007*"needs" + 0.006*"March" + 0.006*"effective" + 0.006*"practice" + 0.006*"ensure" + 0.006*"York" + 0.006*"plans" + 0.005*"However"', '0.020*"’" + 0.007*"needs" + 0.007*"March" + 0.006*"effective" + 0.005*"quality" + 0.005*"ensure" + 0.005*"7" + 0.005*"However" + 0.005*"training" + 0.004*"well"', '0.010*"’" + 0.008*"March" + 0.008*"needs" + 0.005*"effective" + 0.005*"York" + 0.005*"However" + 0.005*"need" + 0.005*"well" + 0.005*"good" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -835,7 +835,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.012*"well" + 0.010*"’" + 0.009*"quality" + 0.008*"effective" + 0.008*"leaders" + 0.007*"good" + 0.006*"plans" + 0.005*"timely" + 0.005*"arrangements" + 0.004*"experiences"', '0.018*"well" + 0.014*"’" + 0.011*"effective" + 0.010*"quality" + 0.009*"leaders" + 0.006*"arrangements" + 0.006*"plans" + 0.006*"highly" + 0.005*"timely" + 0.005*"Senior"', '0.011*"well" + 0.011*"’" + 0.010*"quality" + 0.007*"leaders" + 0.006*"good" + 0.006*"timely" + 0.005*"plans" + 0.005*"effective" + 0.004*"arrangements" + 0.004*"senior"']</t>
+    <t>['0.016*"well" + 0.014*"’" + 0.011*"quality" + 0.010*"effective" + 0.010*"leaders" + 0.006*"plans" + 0.006*"good" + 0.006*"arrangements" + 0.005*"ensure" + 0.005*"timely"', '0.013*"well" + 0.011*"’" + 0.009*"quality" + 0.007*"effective" + 0.006*"leaders" + 0.006*"timely" + 0.006*"good" + 0.005*"plans" + 0.005*"high" + 0.004*"highly"', '0.014*"well" + 0.010*"’" + 0.008*"leaders" + 0.008*"effective" + 0.008*"quality" + 0.007*"arrangements" + 0.006*"timely" + 0.006*"plans" + 0.005*"highly" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -865,7 +865,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.015*"Scilly" + 0.015*"Isles" + 0.010*"practice" + 0.010*"information" + 0.008*"need" + 0.008*"protection" + 0.008*"needs" + 0.007*"quality" + 0.006*"11"', '0.021*"’" + 0.010*"Isles" + 0.010*"Scilly" + 0.009*"need" + 0.008*"information" + 0.008*"place" + 0.006*"practice" + 0.005*"risks" + 0.005*"protection" + 0.005*"13"', '0.015*"’" + 0.008*"Isles" + 0.007*"Scilly" + 0.007*"information" + 0.006*"practice" + 0.006*"needs" + 0.005*"need" + 0.005*"protection" + 0.004*"July" + 0.004*"strategic"']</t>
+    <t>['0.015*"’" + 0.010*"Scilly" + 0.008*"Isles" + 0.008*"information" + 0.007*"need" + 0.007*"protection" + 0.006*"practice" + 0.006*"place" + 0.005*"strategic" + 0.005*"needs"', '0.026*"’" + 0.015*"Isles" + 0.013*"Scilly" + 0.011*"practice" + 0.010*"information" + 0.008*"need" + 0.007*"needs" + 0.007*"quality" + 0.007*"protection" + 0.006*"risks"', '0.017*"’" + 0.012*"Scilly" + 0.009*"Isles" + 0.008*"need" + 0.007*"needs" + 0.007*"information" + 0.006*"place" + 0.006*"practice" + 0.006*"protection" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -901,7 +901,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"well" + 0.009*"needs" + 0.008*"Coventry" + 0.007*"supported" + 0.006*"plans" + 0.005*"strong" + 0.005*"family" + 0.005*"need" + 0.004*"clear"', '0.017*"’" + 0.009*"Coventry" + 0.008*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"supported" + 0.006*"family" + 0.005*"strong" + 0.005*"need" + 0.005*"1"', '0.020*"’" + 0.007*"supported" + 0.007*"Coventry" + 0.007*"well" + 0.007*"family" + 0.006*"needs" + 0.005*"strong" + 0.005*"need" + 0.005*"plans" + 0.005*"20"']</t>
+    <t>['0.022*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"Coventry" + 0.007*"supported" + 0.006*"strong" + 0.006*"plans" + 0.005*"need" + 0.005*"family" + 0.004*"PAs"', '0.018*"’" + 0.009*"Coventry" + 0.008*"well" + 0.007*"needs" + 0.007*"supported" + 0.006*"family" + 0.006*"plans" + 0.006*"need" + 0.005*"use" + 0.005*"1"', '0.017*"’" + 0.006*"Coventry" + 0.006*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"strong" + 0.006*"supported" + 0.005*"family" + 0.004*"July" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -940,7 +940,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.008*"well" + 0.007*"Darlington" + 0.007*"practice" + 0.006*"October" + 0.006*"needs" + 0.006*"leaders" + 0.005*"supported" + 0.005*"plans" + 0.005*"effective"', '0.014*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"October" + 0.007*"practice" + 0.007*"leaders" + 0.005*"quality" + 0.005*"effective" + 0.005*"10" + 0.004*"21"', '0.013*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"October" + 0.005*"well" + 0.005*"Darlington" + 0.004*"quality" + 0.004*"effective" + 0.004*"protection" + 0.004*"supported"']</t>
+    <t>['0.019*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"October" + 0.007*"Darlington" + 0.006*"leaders" + 0.005*"practice" + 0.005*"family" + 0.005*"quality" + 0.005*"effective"', '0.012*"’" + 0.006*"Darlington" + 0.006*"leaders" + 0.006*"effective" + 0.005*"practice" + 0.005*"needs" + 0.005*"well" + 0.005*"October" + 0.005*"quality" + 0.005*"10"', '0.022*"’" + 0.009*"well" + 0.008*"leaders" + 0.008*"practice" + 0.007*"October" + 0.007*"needs" + 0.005*"supported" + 0.005*"Darlington" + 0.005*"education" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -979,7 +979,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"needs" + 0.007*"Derby" + 0.006*"progress" + 0.006*"receive" + 0.006*"oversight" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"well" + 0.005*"need"', '0.021*"’" + 0.011*"needs" + 0.008*"Derby" + 0.006*"quality" + 0.006*"receive" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.005*"appropriate" + 0.005*"progress"', '0.022*"’" + 0.008*"needs" + 0.008*"quality" + 0.007*"Derby" + 0.006*"plans" + 0.006*"receive" + 0.006*"leaders" + 0.006*"good" + 0.005*"progress" + 0.005*"appropriate"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.007*"Derby" + 0.006*"receive" + 0.006*"quality" + 0.006*"appropriate" + 0.005*"leaders" + 0.005*"progress" + 0.005*"need" + 0.005*"plans"', '0.022*"’" + 0.011*"needs" + 0.006*"Derby" + 0.006*"plans" + 0.005*"leaders" + 0.005*"receive" + 0.005*"quality" + 0.005*"progress" + 0.005*"good" + 0.004*"well"', '0.022*"’" + 0.009*"needs" + 0.008*"Derby" + 0.007*"quality" + 0.006*"well" + 0.006*"receive" + 0.006*"progress" + 0.006*"need" + 0.006*"plans" + 0.006*"good"']</t>
   </si>
   <si>
     <t>830</t>
@@ -1006,7 +1006,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.005*"need" + 0.005*"needs" + 0.005*"plans" + 0.005*"10" + 0.005*"good" + 0.005*"practice" + 0.004*"November"', '0.013*"’" + 0.007*"Derbyshire" + 0.006*"well" + 0.005*"positive" + 0.005*"health" + 0.005*"number" + 0.005*"good" + 0.004*"plans" + 0.004*"education" + 0.004*"effective"', '0.016*"’" + 0.009*"well" + 0.007*"Derbyshire" + 0.005*"plans" + 0.005*"positive" + 0.005*"health" + 0.005*"needs" + 0.005*"leaders" + 0.005*"effective" + 0.004*"education"']</t>
+    <t>['0.010*"’" + 0.005*"well" + 0.005*"Derbyshire" + 0.005*"10" + 0.004*"education" + 0.004*"effective" + 0.004*"positive" + 0.004*"plans" + 0.004*"health" + 0.004*"number"', '0.015*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.005*"positive" + 0.005*"health" + 0.005*"need" + 0.005*"good" + 0.005*"effective" + 0.005*"leaders" + 0.004*"practice"', '0.015*"’" + 0.009*"well" + 0.008*"Derbyshire" + 0.006*"plans" + 0.006*"needs" + 0.005*"10" + 0.004*"good" + 0.004*"November" + 0.004*"leaders" + 0.004*"number"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1036,7 +1036,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.005*"well" + 0.005*"leaders" + 0.004*"areas" + 0.004*"health" + 0.004*"risk" + 0.004*"case" + 0.004*"protection" + 0.004*"progress" + 0.004*"quality"', '0.008*"’" + 0.005*"progress" + 0.005*"well" + 0.004*"Devon" + 0.004*"risk" + 0.004*"leaders" + 0.004*"health" + 0.004*"plans" + 0.004*"areas" + 0.004*"case"', '0.011*"’" + 0.007*"well" + 0.005*"health" + 0.005*"risk" + 0.004*"leaders" + 0.004*"risks" + 0.004*"need" + 0.004*"practice" + 0.004*"including" + 0.004*"progress"']</t>
+    <t>['0.008*"’" + 0.006*"leaders" + 0.006*"well" + 0.005*"risk" + 0.005*"health" + 0.004*"risks" + 0.004*"early" + 0.004*"time" + 0.004*"progress" + 0.004*"practice"', '0.011*"’" + 0.007*"well" + 0.005*"progress" + 0.005*"health" + 0.005*"Devon" + 0.005*"risk" + 0.004*"leaders" + 0.004*"living" + 0.004*"case" + 0.004*"areas"', '0.008*"’" + 0.004*"protection" + 0.004*"well" + 0.004*"leaders" + 0.004*"health" + 0.004*"risk" + 0.003*"areas" + 0.003*"case" + 0.003*"need" + 0.003*"risks"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1069,7 +1069,7 @@
     <t>0.1512</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.005*"well" + 0.005*"progress" + 0.005*"Doncaster" + 0.004*"Trust" + 0.004*"quality" + 0.004*"many" + 0.004*"information" + 0.004*"arrangements" + 0.004*"plans"', '0.024*"’" + 0.007*"well" + 0.007*"leaders" + 0.006*"Doncaster" + 0.005*"records" + 0.005*"quality" + 0.005*"protection" + 0.005*"progress" + 0.005*"February" + 0.004*"25"', '0.019*"’" + 0.007*"well" + 0.006*"Doncaster" + 0.006*"many" + 0.005*"plans" + 0.005*"oversight" + 0.005*"arrangements" + 0.005*"records" + 0.005*"information" + 0.004*"effective"']</t>
+    <t>['0.022*"’" + 0.008*"well" + 0.007*"Doncaster" + 0.006*"records" + 0.006*"plans" + 0.005*"leaders" + 0.005*"quality" + 0.005*"protection" + 0.004*"information" + 0.004*"14"', '0.019*"’" + 0.006*"progress" + 0.006*"well" + 0.005*"Doncaster" + 0.005*"many" + 0.005*"oversight" + 0.004*"information" + 0.004*"quality" + 0.004*"February" + 0.004*"arrangements"', '0.019*"’" + 0.005*"well" + 0.005*"Doncaster" + 0.005*"progress" + 0.005*"many" + 0.005*"leaders" + 0.005*"oversight" + 0.004*"arrangements" + 0.004*"25" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>838</t>
@@ -1096,7 +1096,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.005*"Dorset" + 0.005*"well" + 0.005*"arrangements" + 0.004*"good" + 0.004*"needs" + 0.004*"change" + 0.003*"October" + 0.003*"quality" + 0.003*"practice"', '0.012*"’" + 0.007*"Dorset" + 0.006*"good" + 0.005*"well" + 0.005*"needs" + 0.005*"including" + 0.004*"impact" + 0.004*"2021" + 0.004*"October" + 0.004*"Senior"', '0.019*"’" + 0.009*"Dorset" + 0.007*"good" + 0.006*"well" + 0.005*"8" + 0.005*"arrangements" + 0.004*"27" + 0.004*"need" + 0.004*"needs" + 0.004*"leaders"']</t>
+    <t>['0.013*"’" + 0.006*"Dorset" + 0.006*"good" + 0.005*"arrangements" + 0.005*"well" + 0.004*"8" + 0.004*"needs" + 0.004*"27" + 0.004*"leaders" + 0.004*"home"', '0.014*"’" + 0.008*"Dorset" + 0.006*"good" + 0.006*"well" + 0.005*"change" + 0.005*"October" + 0.005*"needs" + 0.004*"including" + 0.004*"arrangements" + 0.004*"impact"', '0.014*"’" + 0.008*"Dorset" + 0.006*"well" + 0.006*"good" + 0.004*"needs" + 0.004*"quality" + 0.004*"2021" + 0.004*"8" + 0.004*"impact" + 0.004*"arrangements"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1123,7 +1123,7 @@
     <t>13/01/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.013*"needs" + 0.006*"well" + 0.006*"Dudley" + 0.006*"always" + 0.005*"plans" + 0.005*"However" + 0.005*"arrangements" + 0.005*"oversight" + 0.004*"31"', '0.015*"’" + 0.010*"Dudley" + 0.010*"needs" + 0.006*"arrangements" + 0.006*"quality" + 0.006*"plans" + 0.005*"ensure" + 0.005*"always" + 0.005*"oversight" + 0.005*"management"', '0.010*"needs" + 0.009*"’" + 0.007*"Dudley" + 0.006*"well" + 0.005*"ensure" + 0.004*"always" + 0.004*"plans" + 0.004*"enough" + 0.004*"November" + 0.004*"timely"']</t>
+    <t>['0.015*"’" + 0.014*"needs" + 0.010*"Dudley" + 0.006*"well" + 0.006*"plans" + 0.006*"always" + 0.005*"quality" + 0.005*"arrangements" + 0.005*"ensure" + 0.005*"management"', '0.017*"’" + 0.009*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.006*"arrangements" + 0.006*"always" + 0.005*"plans" + 0.005*"oversight" + 0.005*"However" + 0.005*"October"', '0.011*"’" + 0.009*"needs" + 0.006*"Dudley" + 0.004*"enough" + 0.004*"well" + 0.004*"ensure" + 0.004*"arrangements" + 0.004*"11" + 0.003*"However" + 0.003*"plans"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1159,7 +1159,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"needs" + 0.007*"May" + 0.006*"well" + 0.005*"ensure" + 0.005*"Durham" + 0.005*"plans" + 0.004*"family" + 0.004*"number" + 0.004*"risks"', '0.014*"’" + 0.011*"needs" + 0.007*"plans" + 0.007*"Durham" + 0.007*"well" + 0.006*"May" + 0.006*"leaders" + 0.005*"practice" + 0.005*"ensure" + 0.005*"supported"', '0.014*"’" + 0.011*"needs" + 0.008*"Durham" + 0.007*"May" + 0.007*"well" + 0.007*"ensure" + 0.006*"practice" + 0.006*"plans" + 0.005*"risks" + 0.004*"carers"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.007*"Durham" + 0.006*"well" + 0.006*"plans" + 0.006*"May" + 0.006*"ensure" + 0.004*"20" + 0.004*"number" + 0.004*"meetings"', '0.014*"’" + 0.010*"needs" + 0.008*"May" + 0.008*"Durham" + 0.007*"plans" + 0.006*"practice" + 0.006*"well" + 0.006*"risks" + 0.005*"ensure" + 0.005*"family"', '0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"May" + 0.006*"ensure" + 0.006*"Durham" + 0.006*"plans" + 0.005*"practice" + 0.004*"leaders" + 0.004*"appropriate"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1195,7 +1195,7 @@
     <t>0.1646</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"needs" + 0.008*"well" + 0.007*"Riding" + 0.007*"plans" + 0.006*"progress" + 0.005*"East" + 0.005*"30" + 0.005*"education" + 0.005*"10"', '0.015*"’" + 0.011*"plans" + 0.009*"well" + 0.008*"progress" + 0.008*"needs" + 0.007*"East" + 0.005*"10" + 0.005*"partners" + 0.005*"Riding" + 0.005*"good"', '0.012*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"Riding" + 0.006*"East" + 0.005*"well" + 0.005*"progress" + 0.004*"January" + 0.004*"information" + 0.004*"February"']</t>
+    <t>['0.011*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"progress" + 0.006*"East" + 0.005*"plans" + 0.004*"10" + 0.004*"education" + 0.004*"experiences" + 0.004*"partners"', '0.019*"’" + 0.011*"needs" + 0.009*"plans" + 0.007*"well" + 0.007*"progress" + 0.006*"East" + 0.006*"Riding" + 0.005*"information" + 0.005*"10" + 0.005*"partners"', '0.016*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"Riding" + 0.008*"needs" + 0.007*"progress" + 0.006*"East" + 0.005*"practice" + 0.005*"30" + 0.005*"training"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1222,7 +1222,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"need" + 0.005*"‘" + 0.004*"plans" + 0.004*"specialist" + 0.004*"family" + 0.004*"Sussex"', '0.010*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"practice" + 0.005*"Sussex" + 0.005*"need" + 0.004*"supported" + 0.004*"East" + 0.004*"plans" + 0.004*"senior"', '0.011*"’" + 0.010*"well" + 0.007*"practice" + 0.007*"needs" + 0.005*"need" + 0.005*"East" + 0.005*"senior" + 0.004*"Sussex" + 0.004*"‘" + 0.004*"quality"']</t>
+    <t>['0.014*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"Sussex" + 0.005*"need" + 0.005*"plans" + 0.004*"senior" + 0.004*"East" + 0.004*"‘"', '0.008*"well" + 0.008*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"need" + 0.004*"East" + 0.004*"carers" + 0.004*"plans" + 0.004*"senior" + 0.004*"receive"', '0.011*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"needs" + 0.004*"‘" + 0.004*"need" + 0.004*"Sussex" + 0.004*"effective" + 0.003*"senior" + 0.003*"East"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1258,7 +1258,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"well" + 0.006*"progress" + 0.005*"plans" + 0.005*"supported" + 0.004*"needs" + 0.004*"risk" + 0.004*"Essex" + 0.004*"parents" + 0.004*"understand"', '0.011*"’" + 0.006*"needs" + 0.005*"need" + 0.005*"plans" + 0.005*"well" + 0.005*"progress" + 0.005*"risk" + 0.005*"understand" + 0.004*"‘" + 0.004*"family"', '0.020*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"progress" + 0.006*"plans" + 0.006*"family" + 0.005*"Essex" + 0.005*"leaders" + 0.005*"experiences" + 0.005*"advisers"']</t>
+    <t>['0.013*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"progress" + 0.005*"understand" + 0.005*"experiences" + 0.005*"parents" + 0.005*"plans" + 0.004*"quality" + 0.004*"Essex"', '0.022*"’" + 0.007*"progress" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"family" + 0.005*"Essex" + 0.005*"risk" + 0.005*"leaders" + 0.005*"understand"', '0.017*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"‘" + 0.005*"progress" + 0.005*"family" + 0.005*"experiences" + 0.005*"supported" + 0.004*"helped"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1294,7 +1294,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.010*"effective" + 0.009*"’" + 0.007*"good" + 0.007*"quality" + 0.006*"practice" + 0.006*"timely" + 0.006*"well" + 0.005*"needs" + 0.005*"plans" + 0.005*"improve"', '0.017*"’" + 0.007*"needs" + 0.006*"effective" + 0.006*"good" + 0.006*"practice" + 0.006*"quality" + 0.006*"well" + 0.005*"early" + 0.004*"home" + 0.004*"need"', '0.014*"’" + 0.008*"effective" + 0.007*"practice" + 0.007*"good" + 0.006*"needs" + 0.005*"quality" + 0.005*"timely" + 0.005*"well" + 0.004*"need" + 0.004*"focus"']</t>
+    <t>['0.013*"’" + 0.007*"effective" + 0.007*"quality" + 0.007*"good" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"timely" + 0.005*"need"', '0.016*"’" + 0.007*"effective" + 0.007*"practice" + 0.007*"good" + 0.007*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"timely" + 0.005*"early" + 0.005*"improve"', '0.012*"effective" + 0.010*"’" + 0.007*"good" + 0.007*"practice" + 0.006*"timely" + 0.005*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"plans" + 0.004*"protection"']</t>
   </si>
   <si>
     <t>916</t>
@@ -1324,7 +1324,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"needs" + 0.008*"2022" + 0.007*"February" + 0.007*"well" + 0.006*"plans" + 0.005*"progress" + 0.005*"18" + 0.005*"appropriate" + 0.004*"effective"', '0.015*"’" + 0.008*"plans" + 0.007*"needs" + 0.006*"February" + 0.006*"2022" + 0.005*"Gloucestershire" + 0.004*"leaders" + 0.004*"progress" + 0.004*"accommodation" + 0.004*"need"', '0.017*"’" + 0.008*"needs" + 0.006*"February" + 0.006*"2022" + 0.006*"Gloucestershire" + 0.006*"well" + 0.005*"good" + 0.005*"plans" + 0.005*"appropriate" + 0.005*"experienced"']</t>
+    <t>['0.021*"’" + 0.009*"needs" + 0.008*"2022" + 0.008*"plans" + 0.007*"February" + 0.007*"well" + 0.006*"progress" + 0.006*"Gloucestershire" + 0.005*"timely" + 0.005*"good"', '0.013*"’" + 0.007*"needs" + 0.005*"February" + 0.004*"well" + 0.004*"appropriate" + 0.004*"2022" + 0.004*"plans" + 0.004*"protection" + 0.004*"need" + 0.004*"progress"', '0.016*"’" + 0.008*"needs" + 0.007*"2022" + 0.007*"February" + 0.006*"plans" + 0.005*"experienced" + 0.005*"appropriate" + 0.005*"18" + 0.005*"Gloucestershire" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1351,7 +1351,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"planning" + 0.006*"practice" + 0.006*"risk" + 0.006*"plans" + 0.006*"good" + 0.006*"progress" + 0.006*"need"', '0.010*"well" + 0.009*"needs" + 0.008*"’" + 0.008*"plans" + 0.008*"practice" + 0.007*"need" + 0.007*"good" + 0.007*"risk" + 0.006*"always" + 0.005*"cases"', '0.016*"’" + 0.011*"well" + 0.010*"practice" + 0.008*"needs" + 0.008*"plans" + 0.007*"always" + 0.006*"risk" + 0.006*"need" + 0.006*"planning" + 0.006*"quality"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"plans" + 0.007*"practice" + 0.006*"planning" + 0.006*"effective" + 0.006*"always" + 0.006*"risk" + 0.006*"need"', '0.010*"well" + 0.010*"practice" + 0.009*"’" + 0.009*"needs" + 0.008*"risk" + 0.007*"plans" + 0.006*"need" + 0.006*"good" + 0.006*"always" + 0.006*"planning"', '0.014*"’" + 0.010*"well" + 0.008*"practice" + 0.007*"need" + 0.007*"needs" + 0.007*"plans" + 0.007*"good" + 0.006*"planning" + 0.006*"effective" + 0.006*"oversight"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1378,7 +1378,7 @@
     <t>0.187</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.009*"needs" + 0.006*"well" + 0.005*"strong" + 0.005*"plans" + 0.005*"quality" + 0.004*"home" + 0.004*"Hampshire" + 0.004*"leaders" + 0.004*"progress"', '0.018*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.005*"quality" + 0.004*"leaders" + 0.004*"improve" + 0.004*"home" + 0.004*"Hampshire" + 0.003*"health"', '0.011*"’" + 0.006*"needs" + 0.006*"plans" + 0.004*"leaders" + 0.004*"well" + 0.004*"highly" + 0.004*"strong" + 0.004*"quality" + 0.003*"carers" + 0.003*"health"']</t>
+    <t>['0.021*"’" + 0.008*"needs" + 0.007*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"highly" + 0.004*"leaders" + 0.004*"strong" + 0.004*"improve" + 0.004*"need"', '0.016*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"home" + 0.005*"Hampshire" + 0.004*"quality" + 0.004*"strong" + 0.004*"leaders" + 0.003*"‘"', '0.017*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"quality" + 0.004*"leaders" + 0.004*"strong" + 0.004*"home" + 0.004*"carers" + 0.004*"improve"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1411,7 +1411,7 @@
     <t>0.2081</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"quality" + 0.005*"strong" + 0.004*"progress" + 0.004*"needs" + 0.004*"timely" + 0.004*"good" + 0.004*"plans" + 0.004*"Senior"', '0.016*"’" + 0.010*"well" + 0.007*"quality" + 0.005*"good" + 0.005*"plans" + 0.005*"strong" + 0.005*"team" + 0.005*"need" + 0.004*"early" + 0.004*"experiences"', '0.016*"’" + 0.009*"well" + 0.007*"quality" + 0.006*"strong" + 0.005*"impact" + 0.005*"good" + 0.005*"practice" + 0.005*"education" + 0.005*"progress" + 0.004*"early"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"strong" + 0.004*"early" + 0.004*"education" + 0.004*"good" + 0.004*"need" + 0.004*"impact" + 0.004*"practice"', '0.015*"’" + 0.010*"well" + 0.007*"quality" + 0.006*"good" + 0.005*"plans" + 0.005*"education" + 0.004*"practice" + 0.004*"strong" + 0.004*"experiences" + 0.004*"impact"', '0.015*"’" + 0.008*"well" + 0.006*"progress" + 0.006*"strong" + 0.005*"quality" + 0.005*"good" + 0.005*"early" + 0.004*"plans" + 0.004*"impact" + 0.004*"improve"']</t>
   </si>
   <si>
     <t>884</t>
@@ -1438,7 +1438,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.005*"lack" + 0.004*"impact" + 0.004*"needs" + 0.004*"Herefordshire" + 0.004*"practice" + 0.004*"progress" + 0.004*"quality" + 0.004*"18" + 0.004*"many"', '0.015*"’" + 0.006*"practice" + 0.006*"needs" + 0.006*"plans" + 0.006*"Herefordshire" + 0.005*"impact" + 0.005*"lack" + 0.004*"oversight" + 0.004*"many" + 0.004*"progress"', '0.019*"’" + 0.006*"practice" + 0.006*"Herefordshire" + 0.005*"lack" + 0.005*"many" + 0.004*"impact" + 0.004*"18" + 0.004*"carers" + 0.004*"agency" + 0.004*"quality"']</t>
+    <t>['0.023*"’" + 0.006*"practice" + 0.006*"lack" + 0.006*"needs" + 0.006*"Herefordshire" + 0.006*"impact" + 0.004*"carers" + 0.004*"July" + 0.004*"risk" + 0.004*"18"', '0.015*"’" + 0.005*"many" + 0.005*"quality" + 0.005*"lack" + 0.005*"practice" + 0.004*"Herefordshire" + 0.004*"impact" + 0.004*"need" + 0.004*"plans" + 0.004*"progress"', '0.009*"’" + 0.005*"Herefordshire" + 0.005*"many" + 0.005*"practice" + 0.005*"needs" + 0.004*"plans" + 0.004*"including" + 0.004*"identified" + 0.004*"18" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>919</t>
@@ -1465,7 +1465,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.007*"Hertfordshire" + 0.006*"well" + 0.006*"receive" + 0.005*"needs" + 0.005*"plans" + 0.005*"need" + 0.004*"Leaders" + 0.004*"23" + 0.004*"2023"', '0.024*"’" + 0.007*"well" + 0.006*"Hertfordshire" + 0.006*"needs" + 0.005*"receive" + 0.005*"2023" + 0.005*"‘" + 0.004*"effective" + 0.004*"risk" + 0.004*"27"', '0.018*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Hertfordshire" + 0.004*"leaders" + 0.004*"positive" + 0.004*"plans" + 0.004*"27" + 0.004*"23" + 0.003*"need"']</t>
+    <t>['0.015*"’" + 0.005*"Hertfordshire" + 0.005*"well" + 0.005*"needs" + 0.003*"leaders" + 0.003*"receive" + 0.003*"working" + 0.003*"‘" + 0.003*"supported" + 0.003*"Leaders"', '0.024*"’" + 0.008*"Hertfordshire" + 0.007*"needs" + 0.007*"well" + 0.006*"receive" + 0.006*"plans" + 0.005*"positive" + 0.005*"need" + 0.005*"2023" + 0.004*"risk"', '0.026*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"27" + 0.005*"Hertfordshire" + 0.005*"receive" + 0.004*"family" + 0.004*"23" + 0.004*"leaders" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1492,7 +1492,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"leaders" + 0.007*"needs" + 0.006*"well" + 0.006*"supported" + 0.006*"3" + 0.006*"progress" + 0.006*"protection" + 0.006*"plans" + 0.005*"good"', '0.015*"’" + 0.009*"leaders" + 0.005*"plans" + 0.005*"PAs" + 0.005*"needs" + 0.005*"Senior" + 0.004*"time" + 0.004*"practice" + 0.004*"good" + 0.004*"well"', '0.013*"’" + 0.005*"leaders" + 0.005*"well" + 0.005*"Isle" + 0.005*"Wight" + 0.004*"PAs" + 0.004*"improve" + 0.004*"Senior" + 0.004*"practice" + 0.004*"October"']</t>
+    <t>['0.017*"’" + 0.009*"leaders" + 0.005*"Senior" + 0.005*"Isle" + 0.005*"plans" + 0.005*"well" + 0.005*"Wight" + 0.005*"needs" + 0.005*"good" + 0.005*"improve"', '0.014*"’" + 0.008*"leaders" + 0.005*"needs" + 0.005*"practice" + 0.005*"supported" + 0.004*"Wight" + 0.004*"2023" + 0.004*"progress" + 0.004*"protection" + 0.004*"good"', '0.020*"’" + 0.008*"leaders" + 0.007*"well" + 0.006*"needs" + 0.006*"3" + 0.006*"PAs" + 0.006*"Isle" + 0.006*"progress" + 0.005*"Senior" + 0.005*"information"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1513,7 +1513,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"Kent" + 0.006*"well" + 0.006*"needs" + 0.006*"supported" + 0.005*"progress" + 0.005*"Council" + 0.005*"council" + 0.004*"practice" + 0.004*"including"', '0.017*"’" + 0.009*"Kent" + 0.007*"needs" + 0.007*"Council" + 0.006*"well" + 0.006*"supported" + 0.005*"County" + 0.005*"practice" + 0.004*"progress" + 0.004*"need"', '0.013*"’" + 0.010*"Kent" + 0.009*"needs" + 0.006*"County" + 0.005*"well" + 0.005*"Council" + 0.005*"leaders" + 0.005*"supported" + 0.004*"progress" + 0.004*"impact"']</t>
+    <t>['0.018*"’" + 0.007*"Kent" + 0.006*"supported" + 0.005*"well" + 0.005*"progress" + 0.005*"needs" + 0.005*"Council" + 0.004*"practice" + 0.004*"9" + 0.003*"plans"', '0.012*"’" + 0.009*"Kent" + 0.007*"needs" + 0.006*"Council" + 0.006*"County" + 0.006*"well" + 0.005*"supported" + 0.005*"practice" + 0.004*"ensure" + 0.004*"progress"', '0.021*"’" + 0.012*"Kent" + 0.009*"needs" + 0.007*"well" + 0.007*"Council" + 0.006*"County" + 0.005*"supported" + 0.005*"progress" + 0.005*"leaders" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1540,7 +1540,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"number" + 0.007*"well" + 0.006*"planning" + 0.006*"need" + 0.006*"Hull" + 0.006*"protection" + 0.006*"practice" + 0.005*"oversight" + 0.005*"small"', '0.015*"’" + 0.007*"number" + 0.007*"protection" + 0.006*"planning" + 0.005*"well" + 0.005*"Hull" + 0.005*"need" + 0.005*"management" + 0.005*"progress" + 0.005*"practice"', '0.016*"’" + 0.007*"planning" + 0.007*"practice" + 0.007*"risks" + 0.006*"number" + 0.006*"well" + 0.005*"management" + 0.005*"teams" + 0.005*"oversight" + 0.005*"agency"']</t>
+    <t>['0.017*"’" + 0.008*"planning" + 0.008*"number" + 0.007*"need" + 0.007*"Hull" + 0.007*"protection" + 0.006*"well" + 0.006*"risks" + 0.006*"practice" + 0.005*"small"', '0.012*"’" + 0.006*"planning" + 0.006*"practice" + 0.006*"management" + 0.005*"small" + 0.005*"number" + 0.005*"protection" + 0.005*"November" + 0.005*"well" + 0.004*"Hull"', '0.017*"’" + 0.007*"number" + 0.006*"practice" + 0.006*"well" + 0.005*"planning" + 0.005*"protection" + 0.005*"oversight" + 0.005*"risks" + 0.005*"management" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1570,7 +1570,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"good" + 0.006*"quality" + 0.006*"practice" + 0.005*"permanence" + 0.005*"needs" + 0.005*"Senior" + 0.005*"training" + 0.005*"risk" + 0.004*"response"', '0.011*"’" + 0.007*"practice" + 0.006*"good" + 0.006*"well" + 0.006*"quality" + 0.006*"protection" + 0.006*"Senior" + 0.005*"needs" + 0.005*"permanence" + 0.005*"plans"', '0.013*"’" + 0.007*"quality" + 0.006*"plans" + 0.005*"practice" + 0.005*"permanence" + 0.005*"well" + 0.004*"good" + 0.004*"training" + 0.004*"senior" + 0.004*"need"']</t>
+    <t>['0.011*"’" + 0.007*"good" + 0.006*"practice" + 0.006*"quality" + 0.006*"plans" + 0.005*"permanence" + 0.005*"Senior" + 0.005*"training" + 0.005*"well" + 0.004*"needs"', '0.012*"’" + 0.006*"quality" + 0.006*"good" + 0.006*"practice" + 0.005*"permanence" + 0.005*"plans" + 0.005*"protection" + 0.005*"needs" + 0.005*"senior" + 0.004*"need"', '0.012*"’" + 0.007*"quality" + 0.007*"well" + 0.006*"practice" + 0.005*"protection" + 0.005*"training" + 0.005*"Senior" + 0.005*"needs" + 0.004*"good" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1609,7 +1609,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.007*"progress" + 0.006*"plans" + 0.006*"quality" + 0.005*"needs" + 0.005*"experiences" + 0.004*"22" + 0.004*"2021" + 0.004*"often" + 0.004*"Knowsley"', '0.020*"’" + 0.010*"progress" + 0.008*"quality" + 0.007*"needs" + 0.007*"plans" + 0.006*"Knowsley" + 0.006*"2021" + 0.006*"impact" + 0.005*"good" + 0.005*"need"', '0.012*"’" + 0.008*"needs" + 0.008*"plans" + 0.007*"progress" + 0.006*"Knowsley" + 0.006*"2021" + 0.006*"experiences" + 0.005*"abuse" + 0.005*"quality" + 0.005*"need"']</t>
+    <t>['0.010*"’" + 0.007*"progress" + 0.007*"quality" + 0.005*"plans" + 0.005*"needs" + 0.004*"abuse" + 0.004*"Knowsley" + 0.004*"place" + 0.004*"October" + 0.004*"good"', '0.019*"’" + 0.010*"progress" + 0.008*"needs" + 0.008*"plans" + 0.007*"Knowsley" + 0.007*"quality" + 0.007*"2021" + 0.006*"good" + 0.006*"22" + 0.006*"experiences"', '0.012*"’" + 0.008*"plans" + 0.008*"needs" + 0.007*"quality" + 0.006*"progress" + 0.006*"Knowsley" + 0.005*"need" + 0.005*"2021" + 0.005*"education" + 0.005*"11"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1639,7 +1639,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.007*"Lancashire" + 0.007*"needs" + 0.006*"supported" + 0.006*"need" + 0.005*"live" + 0.005*"practice" + 0.005*"positive" + 0.005*"plans"', '0.017*"’" + 0.010*"well" + 0.007*"need" + 0.006*"needs" + 0.005*"parents" + 0.005*"practice" + 0.005*"positive" + 0.005*"plans" + 0.005*"supported" + 0.005*"28"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.008*"need" + 0.006*"Lancashire" + 0.006*"health" + 0.006*"plans" + 0.006*"progress" + 0.005*"number" + 0.005*"positive"']</t>
+    <t>['0.019*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"need" + 0.005*"supported" + 0.005*"plans" + 0.005*"Lancashire" + 0.005*"oversight" + 0.005*"live" + 0.004*"practice"', '0.017*"’" + 0.008*"well" + 0.008*"need" + 0.007*"Lancashire" + 0.006*"needs" + 0.006*"9" + 0.005*"supported" + 0.005*"practice" + 0.005*"plans" + 0.005*"28"', '0.012*"’" + 0.010*"well" + 0.008*"needs" + 0.007*"need" + 0.006*"Lancashire" + 0.005*"positive" + 0.005*"parents" + 0.005*"plans" + 0.005*"homes" + 0.005*"health"']</t>
   </si>
   <si>
     <t>383</t>
@@ -1663,7 +1663,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"Leeds" + 0.008*"needs" + 0.007*"well" + 0.006*"risk" + 0.005*"protection" + 0.005*"ensure" + 0.005*"2022" + 0.005*"practice" + 0.005*"benefit"', '0.010*"’" + 0.006*"needs" + 0.005*"risk" + 0.005*"Leeds" + 0.004*"4" + 0.004*"practice" + 0.004*"well" + 0.004*"plans" + 0.004*"supported" + 0.003*"ensure"', '0.012*"’" + 0.006*"needs" + 0.005*"practice" + 0.004*"well" + 0.004*"Leeds" + 0.004*"plans" + 0.004*"risk" + 0.004*"ensure" + 0.004*"supported" + 0.004*"March"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"21" + 0.004*"practice" + 0.004*"plans" + 0.004*"including" + 0.004*"March" + 0.004*"2022"', '0.017*"’" + 0.009*"needs" + 0.008*"Leeds" + 0.007*"well" + 0.005*"ensure" + 0.005*"risk" + 0.005*"4" + 0.005*"protection" + 0.005*"practice" + 0.005*"making"', '0.016*"’" + 0.006*"risk" + 0.006*"Leeds" + 0.005*"well" + 0.004*"practice" + 0.004*"plans" + 0.004*"protection" + 0.004*"benefit" + 0.004*"supported" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1696,7 +1696,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.010*"well" + 0.009*"2021" + 0.009*"Leicester" + 0.008*"needs" + 0.007*"good" + 0.006*"number" + 0.006*"ensure" + 0.006*"20" + 0.006*"1"', '0.008*"’" + 0.005*"needs" + 0.005*"2021" + 0.005*"well" + 0.004*"Leicester" + 0.004*"September" + 0.004*"good" + 0.004*"number" + 0.003*"quality" + 0.003*"October"', '0.014*"’" + 0.008*"2021" + 0.008*"well" + 0.008*"Leicester" + 0.006*"ensure" + 0.006*"good" + 0.006*"needs" + 0.005*"City" + 0.005*"progress" + 0.005*"1"']</t>
+    <t>['0.023*"’" + 0.011*"well" + 0.009*"Leicester" + 0.009*"2021" + 0.008*"needs" + 0.008*"good" + 0.007*"ensure" + 0.006*"number" + 0.005*"1" + 0.005*"October"', '0.017*"’" + 0.009*"2021" + 0.007*"well" + 0.007*"needs" + 0.007*"Leicester" + 0.006*"including" + 0.005*"20" + 0.005*"1" + 0.005*"number" + 0.005*"good"', '0.018*"’" + 0.007*"well" + 0.007*"2021" + 0.007*"Leicester" + 0.005*"20" + 0.005*"including" + 0.004*"1" + 0.004*"high" + 0.004*"number" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1729,7 +1729,7 @@
     <t>0.1666</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.008*"well" + 0.008*"good" + 0.006*"quality" + 0.006*"effective" + 0.005*"practice" + 0.005*"needs" + 0.005*"need" + 0.004*"protection" + 0.004*"education"', '0.013*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"good" + 0.006*"effective" + 0.006*"impact" + 0.005*"need" + 0.005*"practice" + 0.005*"risk"', '0.011*"’" + 0.009*"good" + 0.008*"needs" + 0.008*"effective" + 0.006*"well" + 0.005*"practice" + 0.005*"quality" + 0.005*"impact" + 0.004*"education" + 0.004*"leaders"']</t>
+    <t>['0.011*"’" + 0.007*"good" + 0.007*"well" + 0.006*"practice" + 0.006*"quality" + 0.006*"impact" + 0.006*"need" + 0.006*"needs" + 0.005*"effective" + 0.005*"risk"', '0.013*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"effective" + 0.006*"quality" + 0.006*"good" + 0.004*"risk" + 0.004*"education" + 0.004*"practice" + 0.004*"impact"', '0.010*"’" + 0.009*"good" + 0.009*"well" + 0.007*"effective" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.004*"education" + 0.004*"need" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1759,7 +1759,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"Lincolnshire" + 0.005*"needs" + 0.005*"progress" + 0.004*"well" + 0.004*"24" + 0.003*"April" + 0.003*"plans" + 0.003*"carers" + 0.003*"family"', '0.027*"’" + 0.009*"Lincolnshire" + 0.008*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"family" + 0.005*"progress" + 0.004*"need" + 0.004*"28" + 0.004*"education"', '0.016*"’" + 0.006*"Lincolnshire" + 0.006*"well" + 0.005*"needs" + 0.005*"plans" + 0.005*"24" + 0.004*"family" + 0.004*"working" + 0.004*"progress" + 0.004*"need"']</t>
+    <t>['0.025*"’" + 0.009*"Lincolnshire" + 0.008*"needs" + 0.006*"well" + 0.005*"family" + 0.005*"need" + 0.005*"plans" + 0.005*"progress" + 0.004*"24" + 0.004*"April"', '0.017*"’" + 0.005*"well" + 0.005*"Lincolnshire" + 0.005*"plans" + 0.004*"needs" + 0.004*"24" + 0.004*"2023" + 0.003*"28" + 0.003*"effective" + 0.003*"family"', '0.020*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"well" + 0.004*"28" + 0.004*"family" + 0.004*"24" + 0.003*"effective"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1789,7 +1789,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"practice" + 0.008*"needs" + 0.007*"need" + 0.006*"quality" + 0.006*"always" + 0.005*"Liverpool" + 0.005*"PAs" + 0.005*"protection" + 0.005*"24"', '0.019*"’" + 0.007*"needs" + 0.006*"Liverpool" + 0.006*"need" + 0.005*"always" + 0.005*"practice" + 0.005*"2023" + 0.005*"quality" + 0.004*"protection" + 0.004*"lack"', '0.018*"’" + 0.007*"always" + 0.006*"needs" + 0.006*"practice" + 0.005*"senior" + 0.005*"Liverpool" + 0.005*"quality" + 0.005*"need" + 0.005*"protection" + 0.005*"timely"']</t>
+    <t>['0.020*"’" + 0.007*"practice" + 0.007*"needs" + 0.006*"always" + 0.006*"quality" + 0.006*"Liverpool" + 0.005*"24" + 0.005*"need" + 0.005*"timely" + 0.005*"protection"', '0.019*"’" + 0.008*"needs" + 0.007*"need" + 0.007*"always" + 0.006*"Liverpool" + 0.006*"practice" + 0.005*"met" + 0.005*"quality" + 0.005*"protection" + 0.005*"PAs"', '0.019*"’" + 0.007*"practice" + 0.007*"need" + 0.006*"needs" + 0.006*"always" + 0.006*"Liverpool" + 0.005*"quality" + 0.005*"protection" + 0.005*"planning" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1822,7 +1822,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.005*"plans" + 0.005*"good" + 0.005*"well" + 0.005*"planning" + 0.005*"carers" + 0.005*"information" + 0.004*"Dagenham" + 0.004*"Barking" + 0.004*"timely"', '0.023*"’" + 0.012*"needs" + 0.006*"carers" + 0.006*"well" + 0.005*"progress" + 0.005*"plans" + 0.005*"practice" + 0.004*"ensure" + 0.004*"good" + 0.004*"Dagenham"', '0.023*"’" + 0.007*"good" + 0.007*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"London" + 0.005*"July" + 0.005*"carers" + 0.005*"information" + 0.004*"well"']</t>
+    <t>['0.026*"’" + 0.009*"needs" + 0.007*"good" + 0.006*"carers" + 0.006*"plans" + 0.005*"practice" + 0.005*"well" + 0.005*"information" + 0.005*"Borough" + 0.005*"progress"', '0.020*"’" + 0.007*"needs" + 0.006*"plans" + 0.005*"good" + 0.005*"well" + 0.004*"information" + 0.004*"carers" + 0.004*"Barking" + 0.004*"progress" + 0.004*"10"', '0.019*"’" + 0.007*"needs" + 0.005*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"ensure" + 0.004*"2023" + 0.004*"progress" + 0.004*"21" + 0.004*"carers"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -1858,7 +1858,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"good" + 0.008*"needs" + 0.008*"well" + 0.008*"progress" + 0.007*"need" + 0.006*"ensure" + 0.006*"quality" + 0.006*"clear" + 0.005*"plans"', '0.014*"’" + 0.011*"needs" + 0.010*"need" + 0.009*"good" + 0.008*"well" + 0.006*"plans" + 0.006*"ensure" + 0.005*"clear" + 0.005*"risk" + 0.005*"progress"', '0.014*"’" + 0.009*"good" + 0.009*"well" + 0.009*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"need" + 0.005*"clear" + 0.005*"risk" + 0.005*"meetings"']</t>
+    <t>['0.019*"’" + 0.012*"needs" + 0.010*"good" + 0.008*"well" + 0.008*"need" + 0.006*"ensure" + 0.006*"plans" + 0.006*"progress" + 0.005*"clear" + 0.005*"risk"', '0.012*"’" + 0.010*"well" + 0.010*"good" + 0.008*"needs" + 0.007*"progress" + 0.006*"plans" + 0.006*"need" + 0.006*"quality" + 0.006*"ensure" + 0.006*"clear"', '0.010*"’" + 0.009*"need" + 0.008*"needs" + 0.007*"good" + 0.006*"well" + 0.005*"progress" + 0.005*"clear" + 0.005*"plans" + 0.005*"effective" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>303</t>
@@ -1876,7 +1876,7 @@
     <t>06/02/2023</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"well" + 0.006*"Bexley" + 0.005*"need" + 0.005*"10" + 0.004*"plans" + 0.004*"practice" + 0.004*"including"', '0.023*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.006*"need" + 0.005*"6" + 0.005*"effective" + 0.005*"Bexley" + 0.005*"10" + 0.004*"education"', '0.018*"’" + 0.006*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"need" + 0.005*"Bexley" + 0.005*"plans" + 0.004*"including" + 0.004*"practice" + 0.004*"clear"']</t>
+    <t>['0.014*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"need" + 0.005*"Bexley" + 0.005*"plans" + 0.004*"clear" + 0.004*"10" + 0.004*"practice"', '0.026*"’" + 0.007*"well" + 0.006*"need" + 0.006*"needs" + 0.006*"effective" + 0.005*"Bexley" + 0.005*"plans" + 0.005*"6" + 0.004*"make" + 0.004*"oversight"', '0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"effective" + 0.005*"10" + 0.005*"need" + 0.004*"including" + 0.004*"Bexley" + 0.004*"6"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -1903,7 +1903,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"well" + 0.008*"leaders" + 0.007*"progress" + 0.006*"practice" + 0.006*"good" + 0.006*"quality" + 0.006*"Brent" + 0.006*"plans" + 0.006*"information"', '0.018*"’" + 0.009*"well" + 0.008*"plans" + 0.007*"leaders" + 0.006*"progress" + 0.006*"number" + 0.006*"senior" + 0.006*"needs" + 0.005*"quality" + 0.005*"Brent"', '0.011*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"good" + 0.005*"small" + 0.005*"plans" + 0.005*"However" + 0.005*"number" + 0.005*"Brent" + 0.004*"progress"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.007*"progress" + 0.006*"leaders" + 0.006*"number" + 0.006*"plans" + 0.005*"quality" + 0.005*"good" + 0.005*"practice" + 0.005*"timely"', '0.015*"’" + 0.010*"leaders" + 0.007*"plans" + 0.007*"good" + 0.006*"well" + 0.006*"quality" + 0.006*"number" + 0.006*"progress" + 0.005*"senior" + 0.005*"practice"', '0.019*"’" + 0.010*"well" + 0.007*"plans" + 0.006*"Brent" + 0.006*"progress" + 0.005*"leaders" + 0.005*"senior" + 0.005*"information" + 0.005*"good" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -1936,7 +1936,7 @@
     <t>0.1941</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"Bromley" + 0.006*"well" + 0.005*"needs" + 0.004*"leaders" + 0.004*"practice" + 0.004*"plans" + 0.004*"strong" + 0.004*"helping" + 0.004*"YPAs"', '0.023*"’" + 0.009*"Bromley" + 0.008*"needs" + 0.008*"well" + 0.007*"plans" + 0.006*"leaders" + 0.006*"education" + 0.005*"health" + 0.005*"practice" + 0.005*"17"', '0.014*"’" + 0.008*"Bromley" + 0.006*"well" + 0.006*"needs" + 0.005*"practice" + 0.004*"plans" + 0.004*"leaders" + 0.004*"health" + 0.003*"November" + 0.003*"carers"']</t>
+    <t>['0.016*"’" + 0.009*"Bromley" + 0.008*"needs" + 0.007*"well" + 0.005*"plans" + 0.005*"practice" + 0.004*"education" + 0.004*"health" + 0.004*"progress" + 0.004*"leaders"', '0.017*"’" + 0.009*"Bromley" + 0.007*"well" + 0.006*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.004*"access" + 0.004*"13" + 0.004*"practice" + 0.004*"17"', '0.025*"’" + 0.009*"Bromley" + 0.006*"plans" + 0.006*"well" + 0.006*"practice" + 0.006*"needs" + 0.005*"leaders" + 0.005*"health" + 0.005*"education" + 0.004*"17"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -1966,7 +1966,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.005*"’" + 0.005*"well" + 0.005*"Camden" + 0.004*"25" + 0.004*"practice" + 0.004*"leaders" + 0.004*"meetings" + 0.004*"appropriate" + 0.003*"health" + 0.003*"needs"', '0.012*"’" + 0.008*"Camden" + 0.006*"practice" + 0.006*"leaders" + 0.006*"needs" + 0.005*"response" + 0.005*"29" + 0.005*"appropriate" + 0.005*"protection" + 0.004*"well"', '0.012*"’" + 0.008*"leaders" + 0.007*"Camden" + 0.007*"practice" + 0.006*"well" + 0.006*"protection" + 0.005*"needs" + 0.004*"response" + 0.004*"progress" + 0.004*"good"']</t>
+    <t>['0.014*"’" + 0.008*"Camden" + 0.007*"practice" + 0.006*"leaders" + 0.006*"needs" + 0.005*"well" + 0.005*"appropriate" + 0.005*"response" + 0.005*"25" + 0.004*"protection"', '0.010*"’" + 0.007*"Camden" + 0.007*"leaders" + 0.005*"response" + 0.005*"practice" + 0.005*"protection" + 0.005*"well" + 0.004*"progress" + 0.004*"2022" + 0.004*"needs"', '0.006*"’" + 0.006*"practice" + 0.005*"well" + 0.005*"leaders" + 0.005*"protection" + 0.005*"Camden" + 0.004*"meetings" + 0.004*"needs" + 0.004*"29" + 0.004*"appropriate"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -1993,7 +1993,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"Croydon" + 0.004*"plans" + 0.004*"ensure" + 0.004*"arrangements" + 0.004*"improved" + 0.004*"quality" + 0.004*"good"', '0.014*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"health" + 0.006*"need" + 0.006*"Croydon" + 0.005*"quality" + 0.005*"Senior" + 0.005*"effective" + 0.005*"plans"', '0.012*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"Senior" + 0.006*"quality" + 0.006*"Croydon" + 0.006*"need" + 0.006*"good" + 0.005*"ensure" + 0.005*"education"']</t>
+    <t>['0.008*"’" + 0.006*"needs" + 0.006*"Senior" + 0.005*"well" + 0.005*"ensure" + 0.004*"Croydon" + 0.004*"quality" + 0.004*"need" + 0.004*"education" + 0.004*"effective"', '0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"need" + 0.006*"Croydon" + 0.006*"health" + 0.006*"plans" + 0.005*"effective" + 0.005*"risk" + 0.005*"quality"', '0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"ensure" + 0.006*"quality" + 0.006*"Senior" + 0.006*"Croydon" + 0.005*"education" + 0.005*"improved"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2026,7 +2026,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"quality" + 0.007*"needs" + 0.005*"Ealing" + 0.005*"experiences" + 0.005*"risk" + 0.005*"progress" + 0.004*"good" + 0.004*"family" + 0.004*"management"', '0.010*"’" + 0.010*"quality" + 0.008*"good" + 0.007*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"well" + 0.005*"experiences" + 0.004*"risk" + 0.004*"Ealing"', '0.012*"’" + 0.010*"quality" + 0.006*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"progress" + 0.005*"risk" + 0.005*"oversight" + 0.004*"need" + 0.004*"provide"']</t>
+    <t>['0.006*"’" + 0.005*"quality" + 0.005*"needs" + 0.005*"good" + 0.004*"risk" + 0.004*"oversight" + 0.004*"progress" + 0.003*"family" + 0.003*"experiences" + 0.003*"provide"', '0.013*"’" + 0.012*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.005*"risk" + 0.005*"progress" + 0.005*"experiences" + 0.005*"well" + 0.004*"need"', '0.010*"’" + 0.009*"quality" + 0.007*"needs" + 0.005*"good" + 0.005*"management" + 0.005*"progress" + 0.005*"Ealing" + 0.005*"plans" + 0.004*"oversight" + 0.004*"family"']</t>
   </si>
   <si>
     <t>308</t>
@@ -2053,7 +2053,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.009*"needs" + 0.007*"practice" + 0.007*"good" + 0.007*"ensure" + 0.006*"Enfield" + 0.006*"clear" + 0.005*"improve" + 0.005*"range" + 0.005*"quality"', '0.016*"’" + 0.008*"needs" + 0.008*"good" + 0.008*"ensure" + 0.007*"practice" + 0.007*"clear" + 0.006*"effective" + 0.006*"timely" + 0.006*"quality" + 0.006*"Enfield"', '0.013*"’" + 0.008*"effective" + 0.008*"practice" + 0.008*"leaders" + 0.008*"ensure" + 0.008*"needs" + 0.007*"quality" + 0.006*"Enfield" + 0.006*"good" + 0.006*"clear"']</t>
+    <t>['0.010*"’" + 0.008*"needs" + 0.008*"ensure" + 0.008*"good" + 0.008*"effective" + 0.007*"Enfield" + 0.007*"practice" + 0.007*"clear" + 0.006*"timely" + 0.006*"quality"', '0.015*"’" + 0.006*"ensure" + 0.006*"needs" + 0.006*"good" + 0.005*"Enfield" + 0.005*"timely" + 0.005*"practice" + 0.005*"arrangements" + 0.005*"clear" + 0.005*"leaders"', '0.016*"’" + 0.010*"needs" + 0.009*"practice" + 0.008*"ensure" + 0.007*"good" + 0.007*"effective" + 0.007*"quality" + 0.006*"clear" + 0.006*"leaders" + 0.006*"improve"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2083,7 +2083,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"plans" + 0.007*"good" + 0.006*"information" + 0.006*"need" + 0.005*"range" + 0.005*"timely" + 0.005*"progress"', '0.010*"’" + 0.009*"well" + 0.007*"good" + 0.007*"range" + 0.006*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"need" + 0.005*"effective" + 0.005*"quality"', '0.012*"’" + 0.009*"good" + 0.008*"plans" + 0.008*"well" + 0.007*"need" + 0.006*"ensure" + 0.006*"needs" + 0.005*"consistently" + 0.005*"range" + 0.005*"risk"']</t>
+    <t>['0.011*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"need" + 0.006*"good" + 0.006*"ensure" + 0.006*"progress" + 0.006*"range" + 0.005*"risk"', '0.013*"’" + 0.008*"well" + 0.008*"good" + 0.008*"plans" + 0.008*"needs" + 0.007*"range" + 0.005*"need" + 0.005*"risk" + 0.005*"quality" + 0.004*"risks"', '0.012*"’" + 0.010*"well" + 0.009*"good" + 0.008*"needs" + 0.007*"plans" + 0.006*"need" + 0.005*"timely" + 0.005*"progress" + 0.005*"consistently" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2119,7 +2119,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"practice" + 0.007*"number" + 0.006*"within" + 0.006*"small" + 0.006*"quality" + 0.006*"needs" + 0.005*"plans" + 0.005*"planning" + 0.005*"However"', '0.013*"’" + 0.013*"practice" + 0.007*"effective" + 0.006*"planning" + 0.006*"including" + 0.006*"number" + 0.005*"leaders" + 0.005*"plans" + 0.005*"needs" + 0.005*"quality"', '0.014*"’" + 0.009*"practice" + 0.006*"planning" + 0.006*"number" + 0.006*"plans" + 0.005*"effective" + 0.005*"needs" + 0.005*"including" + 0.005*"within" + 0.005*"making"']</t>
+    <t>['0.017*"’" + 0.009*"practice" + 0.006*"within" + 0.006*"quality" + 0.006*"planning" + 0.005*"needs" + 0.005*"including" + 0.005*"number" + 0.005*"effective" + 0.005*"carers"', '0.011*"practice" + 0.009*"’" + 0.006*"within" + 0.006*"leaders" + 0.006*"planning" + 0.006*"plans" + 0.005*"number" + 0.005*"protection" + 0.005*"effective" + 0.005*"needs"', '0.013*"’" + 0.009*"practice" + 0.008*"number" + 0.007*"effective" + 0.006*"planning" + 0.006*"needs" + 0.006*"need" + 0.006*"plans" + 0.006*"including" + 0.006*"However"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2149,7 +2149,7 @@
     <t>0.2054</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"shared" + 0.006*"arrangements" + 0.005*"effective" + 0.005*"improve" + 0.005*"appropriate" + 0.005*"ensure"', '0.010*"’" + 0.010*"needs" + 0.007*"effective" + 0.007*"well" + 0.006*"good" + 0.006*"arrangements" + 0.005*"appropriate" + 0.005*"ensure" + 0.005*"education" + 0.005*"leaders"', '0.013*"’" + 0.010*"effective" + 0.008*"needs" + 0.007*"well" + 0.007*"appropriate" + 0.006*"ensure" + 0.006*"good" + 0.006*"leaders" + 0.005*"risk" + 0.005*"improve"']</t>
+    <t>['0.011*"’" + 0.008*"effective" + 0.006*"needs" + 0.006*"well" + 0.006*"appropriate" + 0.006*"leaders" + 0.005*"arrangements" + 0.005*"plans" + 0.005*"good" + 0.005*"risk"', '0.012*"’" + 0.009*"needs" + 0.008*"effective" + 0.008*"well" + 0.007*"appropriate" + 0.006*"ensure" + 0.006*"good" + 0.005*"family" + 0.005*"shared" + 0.005*"leaders"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"effective" + 0.007*"good" + 0.006*"arrangements" + 0.006*"ensure" + 0.005*"appropriate" + 0.005*"improve" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2173,7 +2173,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Haringey" + 0.007*"plans" + 0.006*"well" + 0.005*"good" + 0.005*"progress" + 0.005*"need" + 0.004*"needs" + 0.004*"education" + 0.004*"timely"', '0.016*"’" + 0.010*"needs" + 0.009*"Haringey" + 0.006*"plans" + 0.006*"good" + 0.005*"well" + 0.005*"risk" + 0.005*"need" + 0.004*"education" + 0.004*"Leaders"', '0.016*"’" + 0.007*"needs" + 0.007*"Haringey" + 0.007*"plans" + 0.006*"well" + 0.006*"progress" + 0.005*"need" + 0.005*"good" + 0.004*"training" + 0.004*"impact"']</t>
+    <t>['0.020*"’" + 0.010*"Haringey" + 0.010*"needs" + 0.009*"plans" + 0.007*"well" + 0.006*"good" + 0.005*"need" + 0.005*"education" + 0.004*"24" + 0.004*"progress"', '0.008*"’" + 0.006*"needs" + 0.005*"good" + 0.005*"Haringey" + 0.005*"plans" + 0.004*"well" + 0.004*"progress" + 0.003*"education" + 0.003*"risk" + 0.003*"need"', '0.014*"’" + 0.008*"Haringey" + 0.006*"need" + 0.005*"progress" + 0.005*"plans" + 0.005*"needs" + 0.005*"well" + 0.005*"risk" + 0.004*"impact" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2203,7 +2203,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"needs" + 0.006*"good" + 0.005*"well" + 0.004*"plans" + 0.004*"impact" + 0.004*"experiences" + 0.003*"protection" + 0.003*"team" + 0.003*"early"', '0.012*"good" + 0.012*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"impact" + 0.006*"practice" + 0.006*"protection" + 0.006*"need" + 0.005*"plans" + 0.005*"early"', '0.013*"’" + 0.012*"good" + 0.009*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"protection" + 0.005*"early" + 0.005*"experiences" + 0.004*"practice"']</t>
+    <t>['0.015*"’" + 0.014*"good" + 0.011*"well" + 0.007*"needs" + 0.007*"plans" + 0.006*"early" + 0.006*"practice" + 0.006*"impact" + 0.005*"need" + 0.005*"school"', '0.009*"’" + 0.008*"good" + 0.007*"needs" + 0.005*"need" + 0.005*"experiences" + 0.005*"impact" + 0.005*"practice" + 0.005*"well" + 0.004*"protection" + 0.004*"team"', '0.009*"needs" + 0.009*"’" + 0.008*"good" + 0.008*"well" + 0.006*"protection" + 0.005*"impact" + 0.004*"experiences" + 0.004*"planning" + 0.004*"need" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2233,7 +2233,7 @@
     <t>0.2113</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"needs" + 0.008*"quality" + 0.008*"good" + 0.007*"need" + 0.006*"well" + 0.006*"plans" + 0.005*"meetings" + 0.005*"practice" + 0.005*"progress"', '0.008*"good" + 0.008*"need" + 0.007*"’" + 0.007*"well" + 0.006*"quality" + 0.006*"needs" + 0.006*"plans" + 0.006*"practice" + 0.005*"meetings" + 0.004*"consistently"', '0.011*"’" + 0.008*"needs" + 0.007*"good" + 0.007*"quality" + 0.006*"plans" + 0.006*"need" + 0.006*"well" + 0.006*"meetings" + 0.005*"number" + 0.005*"practice"']</t>
+    <t>['0.009*"needs" + 0.009*"’" + 0.008*"need" + 0.007*"quality" + 0.007*"plans" + 0.006*"good" + 0.006*"practice" + 0.006*"meetings" + 0.005*"well" + 0.005*"clear"', '0.010*"’" + 0.008*"good" + 0.007*"well" + 0.006*"practice" + 0.006*"needs" + 0.006*"quality" + 0.006*"need" + 0.005*"plans" + 0.005*"appropriate" + 0.005*"consistently"', '0.012*"’" + 0.009*"good" + 0.008*"quality" + 0.007*"need" + 0.007*"well" + 0.006*"needs" + 0.006*"meetings" + 0.006*"plans" + 0.005*"consistently" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>312</t>
@@ -2266,7 +2266,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Hillingdon" + 0.006*"plans" + 0.005*"team" + 0.005*"6" + 0.005*"need" + 0.004*"leaders" + 0.004*"PAs"', '0.014*"’" + 0.009*"needs" + 0.008*"plans" + 0.006*"Hillingdon" + 0.005*"team" + 0.005*"need" + 0.004*"October" + 0.004*"well" + 0.004*"2" + 0.004*"carers"', '0.020*"’" + 0.010*"needs" + 0.010*"Hillingdon" + 0.009*"plans" + 0.009*"well" + 0.005*"2" + 0.004*"experiences" + 0.004*"6" + 0.004*"understand" + 0.004*"timely"']</t>
+    <t>['0.018*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"Hillingdon" + 0.007*"needs" + 0.004*"team" + 0.004*"need" + 0.004*"PAs" + 0.004*"2023" + 0.003*"appropriate"', '0.016*"’" + 0.010*"needs" + 0.007*"plans" + 0.007*"Hillingdon" + 0.006*"well" + 0.005*"experiences" + 0.004*"October" + 0.004*"team" + 0.004*"6" + 0.004*"family"', '0.019*"’" + 0.011*"needs" + 0.009*"Hillingdon" + 0.008*"well" + 0.008*"plans" + 0.005*"need" + 0.005*"team" + 0.005*"2" + 0.005*"6" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2296,7 +2296,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"Hounslow" + 0.006*"plans" + 0.005*"timely" + 0.004*"experiences" + 0.004*"education" + 0.004*"16"', '0.012*"’" + 0.007*"needs" + 0.007*"Hounslow" + 0.006*"well" + 0.006*"effective" + 0.005*"timely" + 0.004*"October" + 0.004*"strong" + 0.003*"health" + 0.003*"plans"', '0.022*"’" + 0.014*"needs" + 0.012*"well" + 0.008*"effective" + 0.007*"timely" + 0.007*"Hounslow" + 0.006*"plans" + 0.005*"progress" + 0.005*"oversight" + 0.005*"experiences"']</t>
+    <t>['0.018*"’" + 0.010*"needs" + 0.008*"Hounslow" + 0.007*"well" + 0.007*"effective" + 0.006*"plans" + 0.006*"timely" + 0.004*"2023" + 0.004*"16" + 0.004*"leaders"', '0.026*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"effective" + 0.006*"timely" + 0.006*"Hounslow" + 0.005*"progress" + 0.005*"plans" + 0.005*"20" + 0.005*"experiences"', '0.013*"’" + 0.012*"needs" + 0.011*"well" + 0.007*"Hounslow" + 0.007*"effective" + 0.006*"timely" + 0.005*"plans" + 0.005*"oversight" + 0.005*"strong" + 0.004*"16"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2326,7 +2326,7 @@
     <t>0.1842</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.009*"needs" + 0.007*"well" + 0.005*"highly" + 0.005*"plans" + 0.005*"leaders" + 0.004*"quality" + 0.004*"Senior" + 0.004*"practice" + 0.004*"good"', '0.013*"needs" + 0.013*"’" + 0.010*"well" + 0.007*"plans" + 0.007*"good" + 0.007*"highly" + 0.006*"quality" + 0.005*"Islington" + 0.005*"practice" + 0.004*"need"', '0.014*"’" + 0.012*"well" + 0.010*"needs" + 0.007*"effective" + 0.007*"plans" + 0.006*"leaders" + 0.006*"good" + 0.006*"quality" + 0.005*"risk" + 0.005*"highly"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"highly" + 0.007*"plans" + 0.006*"school" + 0.005*"quality" + 0.005*"good" + 0.005*"Islington" + 0.005*"effective"', '0.010*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"good" + 0.005*"plans" + 0.005*"effective" + 0.005*"highly" + 0.004*"Islington" + 0.004*"quality" + 0.003*"lives"', '0.013*"’" + 0.012*"well" + 0.012*"needs" + 0.007*"plans" + 0.007*"leaders" + 0.006*"quality" + 0.006*"good" + 0.006*"effective" + 0.005*"highly" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2359,7 +2359,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"well" + 0.010*"needs" + 0.006*"Lambeth" + 0.006*"plans" + 0.006*"good" + 0.006*"impact" + 0.005*"4" + 0.004*"Leaders" + 0.004*"progress"', '0.015*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"progress" + 0.006*"plans" + 0.006*"Lambeth" + 0.005*"number" + 0.005*"4"', '0.015*"’" + 0.009*"plans" + 0.009*"needs" + 0.007*"good" + 0.006*"Lambeth" + 0.006*"well" + 0.006*"leaders" + 0.006*"progress" + 0.006*"impact" + 0.006*"need"']</t>
+    <t>['0.017*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"good" + 0.006*"Lambeth" + 0.006*"need" + 0.005*"progress" + 0.005*"arrangements" + 0.004*"carers"', '0.014*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"good" + 0.007*"Lambeth" + 0.007*"impact" + 0.006*"plans" + 0.006*"progress" + 0.005*"4" + 0.005*"need"', '0.014*"’" + 0.009*"needs" + 0.008*"plans" + 0.008*"well" + 0.006*"good" + 0.006*"need" + 0.006*"progress" + 0.006*"Lambeth" + 0.005*"impact" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2389,7 +2389,7 @@
     <t>0.1538</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"well" + 0.006*"However" + 0.006*"quality" + 0.005*"impact" + 0.005*"appropriate" + 0.005*"needs" + 0.005*"timely" + 0.004*"progress" + 0.004*"changes"', '0.007*"’" + 0.006*"However" + 0.006*"appropriate" + 0.006*"quality" + 0.006*"timely" + 0.005*"impact" + 0.005*"well" + 0.004*"clear" + 0.004*"effective" + 0.004*"practice"', '0.010*"’" + 0.006*"quality" + 0.006*"timely" + 0.006*"However" + 0.006*"well" + 0.004*"needs" + 0.004*"cases" + 0.004*"progress" + 0.004*"good" + 0.004*"oversight"']</t>
+    <t>['0.010*"’" + 0.007*"well" + 0.006*"However" + 0.006*"quality" + 0.005*"needs" + 0.005*"information" + 0.005*"appropriate" + 0.004*"early" + 0.004*"timely" + 0.004*"education"', '0.009*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"timely" + 0.006*"However" + 0.006*"impact" + 0.005*"appropriate" + 0.004*"needs" + 0.004*"oversight" + 0.004*"progress"', '0.008*"’" + 0.006*"However" + 0.006*"timely" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"impact" + 0.004*"well" + 0.004*"progress" + 0.004*"needs" + 0.004*"changes"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2410,7 +2410,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"Merton" + 0.005*"good" + 0.005*"family" + 0.004*"impact" + 0.004*"across" + 0.004*"4" + 0.004*"ensure"', '0.017*"’" + 0.008*"well" + 0.007*"Merton" + 0.005*"plans" + 0.005*"information" + 0.004*"needs" + 0.004*"early" + 0.004*"2022" + 0.004*"leaders" + 0.004*"access"', '0.013*"’" + 0.008*"well" + 0.006*"Merton" + 0.006*"needs" + 0.006*"progress" + 0.005*"plans" + 0.004*"4" + 0.004*"across" + 0.004*"education" + 0.004*"information"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.007*"Merton" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.004*"good" + 0.004*"leaders" + 0.004*"education" + 0.004*"information"', '0.012*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"Merton" + 0.005*"family" + 0.005*"progress" + 0.004*"risk" + 0.004*"4" + 0.004*"practice" + 0.004*"2022"', '0.017*"’" + 0.007*"well" + 0.006*"Merton" + 0.005*"needs" + 0.005*"plans" + 0.005*"ensure" + 0.005*"family" + 0.004*"across" + 0.004*"4" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2428,7 +2428,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50192878</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"needs" + 0.007*"Newham" + 0.007*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"progress" + 0.005*"practice" + 0.005*"good" + 0.005*"ensure"', '0.020*"’" + 0.008*"needs" + 0.007*"practice" + 0.006*"Newham" + 0.006*"progress" + 0.006*"need" + 0.006*"plans" + 0.005*"good" + 0.004*"effective" + 0.004*"planning"', '0.017*"’" + 0.008*"needs" + 0.007*"Newham" + 0.007*"progress" + 0.006*"need" + 0.006*"plans" + 0.006*"practice" + 0.005*"effective" + 0.005*"risks" + 0.005*"good"']</t>
+    <t>['0.021*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"plans" + 0.006*"effective" + 0.006*"progress" + 0.006*"need" + 0.005*"early" + 0.004*"18"', '0.021*"’" + 0.008*"needs" + 0.007*"progress" + 0.007*"plans" + 0.006*"Newham" + 0.006*"effective" + 0.006*"good" + 0.006*"practice" + 0.006*"need" + 0.005*"risks"', '0.013*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"need" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective" + 0.004*"good" + 0.004*"Leaders"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2455,7 +2455,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.007*"well" + 0.005*"need" + 0.005*"Redbridge" + 0.005*"including" + 0.005*"needs" + 0.005*"effective" + 0.005*"strong" + 0.004*"highly" + 0.004*"progress"', '0.009*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"strong" + 0.005*"effective" + 0.005*"needs" + 0.005*"risk" + 0.005*"receive" + 0.004*"ensure" + 0.004*"need"', '0.009*"practice" + 0.007*"needs" + 0.007*"need" + 0.007*"’" + 0.006*"well" + 0.005*"risk" + 0.005*"Redbridge" + 0.005*"effective" + 0.005*"strong" + 0.005*"team"']</t>
+    <t>['0.005*"’" + 0.005*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"Redbridge" + 0.004*"need" + 0.004*"risk" + 0.004*"team" + 0.004*"ensure" + 0.004*"strong"', '0.009*"’" + 0.007*"well" + 0.007*"practice" + 0.006*"needs" + 0.006*"strong" + 0.006*"need" + 0.005*"progress" + 0.005*"including" + 0.005*"risk" + 0.005*"Redbridge"', '0.007*"practice" + 0.007*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"need" + 0.005*"well" + 0.005*"Redbridge" + 0.005*"strong" + 0.005*"risk" + 0.004*"team"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2479,7 +2479,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"well" + 0.008*"needs" + 0.007*"Richmond" + 0.006*"need" + 0.005*"team" + 0.005*"additional" + 0.005*"good" + 0.005*"31" + 0.005*"January"', '0.016*"’" + 0.011*"well" + 0.009*"Richmond" + 0.008*"supported" + 0.007*"needs" + 0.006*"good" + 0.005*"ensure" + 0.005*"need" + 0.005*"team" + 0.005*"4"', '0.016*"’" + 0.008*"well" + 0.007*"Richmond" + 0.007*"needs" + 0.006*"team" + 0.006*"need" + 0.005*"good" + 0.005*"supported" + 0.005*"upon" + 0.005*"Thames"']</t>
+    <t>['0.018*"’" + 0.013*"well" + 0.010*"Richmond" + 0.007*"needs" + 0.007*"supported" + 0.007*"team" + 0.006*"need" + 0.006*"good" + 0.005*"4" + 0.005*"additional"', '0.011*"’" + 0.007*"Richmond" + 0.007*"well" + 0.006*"needs" + 0.005*"supported" + 0.005*"strong" + 0.004*"team" + 0.004*"need" + 0.004*"upon" + 0.004*"range"', '0.016*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"Richmond" + 0.006*"good" + 0.005*"need" + 0.005*"supported" + 0.005*"31" + 0.005*"team" + 0.004*"strong"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2506,7 +2506,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"Southwark" + 0.006*"needs" + 0.006*"good" + 0.006*"well" + 0.005*"plans" + 0.005*"Leaders" + 0.005*"need" + 0.005*"progress" + 0.004*"strong"', '0.025*"’" + 0.010*"Southwark" + 0.009*"good" + 0.009*"well" + 0.008*"needs" + 0.006*"progress" + 0.006*"need" + 0.006*"strong" + 0.006*"effective" + 0.006*"leaders"', '0.011*"’" + 0.008*"Southwark" + 0.007*"good" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"plans" + 0.005*"progress" + 0.005*"need" + 0.004*"improve"']</t>
+    <t>['0.021*"’" + 0.009*"Southwark" + 0.009*"well" + 0.007*"good" + 0.007*"progress" + 0.007*"needs" + 0.006*"need" + 0.005*"leaders" + 0.005*"plans" + 0.005*"strong"', '0.015*"’" + 0.009*"good" + 0.008*"needs" + 0.008*"Southwark" + 0.007*"well" + 0.006*"receive" + 0.005*"Leaders" + 0.005*"practice" + 0.005*"plans" + 0.005*"progress"', '0.018*"’" + 0.011*"Southwark" + 0.008*"good" + 0.007*"well" + 0.006*"effective" + 0.006*"needs" + 0.006*"plans" + 0.006*"need" + 0.006*"strong" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2533,7 +2533,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"well" + 0.005*"progress" + 0.005*"effective" + 0.005*"Sutton" + 0.005*"receive" + 0.004*"‘" + 0.004*"good" + 0.004*"6" + 0.004*"10"', '0.016*"’" + 0.006*"needs" + 0.005*"Sutton" + 0.005*"well" + 0.004*"6" + 0.004*"good" + 0.004*"10" + 0.004*"leaders" + 0.004*"receive" + 0.003*"progress"', '0.018*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Sutton" + 0.006*"progress" + 0.005*"effective" + 0.005*"receive" + 0.005*"good" + 0.005*"need" + 0.004*"understand"']</t>
+    <t>['0.011*"’" + 0.006*"well" + 0.005*"effective" + 0.005*"Sutton" + 0.004*"receive" + 0.004*"progress" + 0.004*"needs" + 0.004*"need" + 0.004*"good" + 0.004*"2021"', '0.017*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"receive" + 0.004*"Sutton" + 0.004*"10" + 0.004*"2021" + 0.004*"effective" + 0.004*"leaders"', '0.020*"’" + 0.007*"Sutton" + 0.007*"progress" + 0.006*"well" + 0.006*"needs" + 0.006*"6" + 0.005*"effective" + 0.005*"supported" + 0.005*"receive" + 0.005*"‘"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2560,7 +2560,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"good" + 0.007*"practice" + 0.007*"effective" + 0.006*"plans" + 0.006*"‘" + 0.006*"progress" + 0.005*"early" + 0.005*"needs" + 0.005*"carers"', '0.011*"’" + 0.007*"good" + 0.006*"well" + 0.006*"plans" + 0.005*"‘" + 0.005*"effective" + 0.005*"including" + 0.005*"need" + 0.004*"early" + 0.004*"example"', '0.012*"’" + 0.006*"need" + 0.006*"well" + 0.006*"effective" + 0.005*"plans" + 0.005*"good" + 0.004*"‘" + 0.004*"education" + 0.004*"practice" + 0.004*"including"']</t>
+    <t>['0.018*"’" + 0.007*"good" + 0.007*"effective" + 0.005*"‘" + 0.005*"including" + 0.005*"early" + 0.005*"need" + 0.005*"plans" + 0.004*"carers" + 0.004*"well"', '0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.006*"practice" + 0.005*"effective" + 0.005*"‘" + 0.005*"need" + 0.005*"needs"', '0.010*"’" + 0.006*"‘" + 0.006*"plans" + 0.006*"good" + 0.005*"effective" + 0.005*"need" + 0.005*"practice" + 0.005*"well" + 0.005*"needs" + 0.005*"early"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2587,7 +2587,7 @@
     <t>11/03/19</t>
   </si>
   <si>
-    <t>['0.010*"well" + 0.010*"’" + 0.008*"needs" + 0.007*"good" + 0.006*"need" + 0.005*"effective" + 0.005*"plans" + 0.004*"timely" + 0.004*"protection" + 0.004*"clear"', '0.018*"’" + 0.009*"well" + 0.009*"effective" + 0.008*"needs" + 0.008*"good" + 0.006*"need" + 0.005*"plans" + 0.005*"timely" + 0.004*"information" + 0.004*"risk"', '0.016*"well" + 0.014*"’" + 0.009*"needs" + 0.009*"good" + 0.007*"effective" + 0.006*"need" + 0.006*"plans" + 0.005*"risk" + 0.005*"timely" + 0.005*"progress"']</t>
+    <t>['0.010*"’" + 0.010*"well" + 0.007*"effective" + 0.006*"need" + 0.005*"needs" + 0.005*"good" + 0.004*"timely" + 0.003*"plans" + 0.003*"actions" + 0.003*"information"', '0.018*"’" + 0.014*"well" + 0.010*"needs" + 0.010*"good" + 0.008*"effective" + 0.007*"need" + 0.006*"plans" + 0.006*"timely" + 0.005*"risk" + 0.005*"ensure"', '0.012*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"effective" + 0.005*"plans" + 0.004*"risk" + 0.004*"practice" + 0.004*"timely" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2611,7 +2611,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"well" + 0.006*"Senior" + 0.006*"needs" + 0.006*"practice" + 0.005*"Wandsworth" + 0.005*"protection" + 0.005*"ensure" + 0.005*"quality" + 0.005*"effective"', '0.012*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"Wandsworth" + 0.005*"supported" + 0.005*"Senior" + 0.005*"7" + 0.005*"needs" + 0.005*"receive" + 0.005*"improve"', '0.011*"’" + 0.008*"well" + 0.006*"progress" + 0.005*"team" + 0.005*"needs" + 0.005*"protection" + 0.004*"practice" + 0.004*"However" + 0.004*"supported" + 0.004*"quality"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.005*"progress" + 0.005*"well" + 0.005*"18" + 0.005*"Wandsworth" + 0.005*"Senior" + 0.004*"supported" + 0.004*"timely" + 0.004*"practice"', '0.013*"’" + 0.007*"well" + 0.007*"protection" + 0.006*"effective" + 0.006*"good" + 0.005*"Senior" + 0.005*"progress" + 0.005*"needs" + 0.005*"quality" + 0.005*"supported"', '0.011*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"needs" + 0.005*"Wandsworth" + 0.005*"progress" + 0.005*"ensure" + 0.005*"quality" + 0.005*"7" + 0.005*"18"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2632,7 +2632,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.005*"practice" + 0.005*"highly" + 0.004*"well" + 0.004*"many" + 0.004*"across" + 0.004*"direct" + 0.004*"interventions" + 0.003*"family"', '0.014*"’" + 0.008*"practice" + 0.005*"highly" + 0.005*"well" + 0.004*"needs" + 0.004*"across" + 0.004*"skilled" + 0.004*"high" + 0.004*"many" + 0.003*"plans"', '0.012*"’" + 0.007*"highly" + 0.006*"practice" + 0.006*"well" + 0.005*"needs" + 0.004*"many" + 0.004*"family" + 0.004*"shared" + 0.003*"across" + 0.003*"protection"']</t>
+    <t>['0.015*"’" + 0.007*"needs" + 0.007*"practice" + 0.007*"highly" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.004*"skilled" + 0.004*"quality" + 0.004*"shared"', '0.011*"’" + 0.006*"needs" + 0.006*"practice" + 0.005*"highly" + 0.004*"well" + 0.003*"high" + 0.003*"family" + 0.003*"early" + 0.003*"direct" + 0.003*"across"', '0.010*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"highly" + 0.004*"across" + 0.004*"many" + 0.004*"needs" + 0.004*"direct" + 0.004*"family" + 0.003*"shared"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2662,7 +2662,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"needs" + 0.007*"need" + 0.006*"effective" + 0.006*"Luton" + 0.006*"plans" + 0.005*"impact" + 0.005*"good" + 0.005*"progress" + 0.005*"leaders"', '0.016*"’" + 0.006*"good" + 0.006*"plans" + 0.005*"impact" + 0.005*"Luton" + 0.005*"effective" + 0.005*"quality" + 0.005*"need" + 0.005*"progress" + 0.005*"ensure"', '0.016*"’" + 0.007*"need" + 0.006*"needs" + 0.006*"plans" + 0.005*"Luton" + 0.005*"receive" + 0.005*"ensure" + 0.005*"progress" + 0.004*"effective" + 0.004*"well"']</t>
+    <t>['0.018*"’" + 0.006*"needs" + 0.005*"effective" + 0.005*"quality" + 0.005*"receive" + 0.005*"progress" + 0.005*"ensure" + 0.005*"need" + 0.005*"leaders" + 0.005*"impact"', '0.014*"’" + 0.007*"plans" + 0.005*"need" + 0.005*"effective" + 0.005*"progress" + 0.005*"Luton" + 0.005*"impact" + 0.005*"needs" + 0.004*"11" + 0.004*"well"', '0.019*"’" + 0.008*"need" + 0.007*"Luton" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"well" + 0.005*"effective" + 0.005*"impact" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2689,7 +2689,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Manchester" + 0.007*"needs" + 0.006*"supported" + 0.006*"always" + 0.005*"plans" + 0.005*"effective" + 0.005*"disabled" + 0.004*"protection" + 0.004*"well"', '0.022*"’" + 0.011*"Manchester" + 0.009*"needs" + 0.008*"well" + 0.008*"always" + 0.006*"education" + 0.006*"supported" + 0.005*"plans" + 0.005*"protection" + 0.005*"progress"', '0.024*"’" + 0.011*"Manchester" + 0.011*"needs" + 0.007*"supported" + 0.007*"well" + 0.006*"always" + 0.006*"plans" + 0.005*"disabled" + 0.005*"protection" + 0.005*"effective"']</t>
+    <t>['0.015*"’" + 0.010*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.007*"always" + 0.005*"education" + 0.005*"effective" + 0.005*"progress" + 0.005*"supported" + 0.005*"risk"', '0.014*"’" + 0.009*"Manchester" + 0.007*"supported" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"21" + 0.005*"information" + 0.005*"family" + 0.004*"protection"', '0.030*"’" + 0.011*"Manchester" + 0.011*"needs" + 0.007*"always" + 0.007*"supported" + 0.007*"well" + 0.006*"plans" + 0.006*"quality" + 0.005*"protection" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -2716,7 +2716,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"practice" + 0.007*"quality" + 0.007*"Medway" + 0.007*"well" + 0.006*"leaders" + 0.005*"needs" + 0.005*"oversight" + 0.005*"impact" + 0.004*"progress"', '0.013*"’" + 0.009*"well" + 0.007*"Medway" + 0.007*"quality" + 0.007*"practice" + 0.006*"leaders" + 0.005*"risk" + 0.005*"needs" + 0.005*"Senior" + 0.004*"experiences"', '0.018*"’" + 0.011*"Medway" + 0.009*"practice" + 0.008*"quality" + 0.007*"oversight" + 0.007*"impact" + 0.007*"needs" + 0.007*"well" + 0.006*"leaders" + 0.006*"experiences"']</t>
+    <t>['0.015*"’" + 0.010*"Medway" + 0.007*"practice" + 0.006*"impact" + 0.005*"experiences" + 0.005*"quality" + 0.005*"well" + 0.005*"oversight" + 0.005*"needs" + 0.005*"Senior"', '0.010*"’" + 0.008*"Medway" + 0.008*"quality" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.006*"oversight" + 0.006*"leaders" + 0.005*"Senior" + 0.005*"impact"', '0.020*"’" + 0.009*"well" + 0.009*"quality" + 0.009*"Medway" + 0.009*"practice" + 0.007*"leaders" + 0.007*"needs" + 0.006*"good" + 0.006*"oversight" + 0.006*"impact"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -2737,7 +2737,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"well" + 0.006*"Middlesbrough" + 0.006*"progress" + 0.005*"practice" + 0.005*"plans" + 0.005*"place" + 0.005*"impact"', '0.014*"’" + 0.008*"effective" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.006*"place" + 0.006*"Middlesbrough" + 0.005*"24" + 0.005*"progress"', '0.013*"’" + 0.009*"plans" + 0.009*"Middlesbrough" + 0.006*"effective" + 0.006*"well" + 0.005*"needs" + 0.005*"progress" + 0.004*"March" + 0.004*"good" + 0.004*"practice"']</t>
+    <t>['0.011*"’" + 0.008*"Middlesbrough" + 0.007*"practice" + 0.007*"plans" + 0.006*"needs" + 0.005*"well" + 0.005*"effective" + 0.005*"good" + 0.005*"24" + 0.005*"progress"', '0.015*"’" + 0.008*"effective" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.005*"progress" + 0.005*"13" + 0.005*"Middlesbrough" + 0.005*"place" + 0.005*"good"', '0.015*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.006*"well" + 0.005*"progress" + 0.005*"means" + 0.005*"practice" + 0.005*"needs" + 0.004*"24"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -2761,7 +2761,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"Keynes" + 0.006*"Milton" + 0.005*"practice" + 0.005*"good" + 0.005*"well" + 0.005*"leaders" + 0.004*"need" + 0.004*"quality" + 0.004*"effective"', '0.012*"’" + 0.006*"Keynes" + 0.006*"Milton" + 0.005*"well" + 0.005*"need" + 0.005*"5" + 0.005*"plans" + 0.005*"25" + 0.004*"practice" + 0.004*"leaders"', '0.018*"’" + 0.006*"need" + 0.006*"Milton" + 0.006*"well" + 0.006*"Keynes" + 0.005*"25" + 0.005*"October" + 0.005*"plans" + 0.005*"carers" + 0.004*"5"']</t>
+    <t>['0.014*"’" + 0.006*"Milton" + 0.006*"Keynes" + 0.005*"need" + 0.005*"practice" + 0.005*"well" + 0.005*"October" + 0.005*"needs" + 0.004*"25" + 0.004*"leaders"', '0.015*"’" + 0.007*"Keynes" + 0.006*"well" + 0.006*"Milton" + 0.006*"need" + 0.005*"impact" + 0.005*"November" + 0.005*"plans" + 0.005*"leaders" + 0.005*"team"', '0.017*"’" + 0.005*"well" + 0.005*"good" + 0.005*"Milton" + 0.005*"need" + 0.004*"25" + 0.004*"Keynes" + 0.004*"plans" + 0.004*"carers" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -2785,7 +2785,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"plans" + 0.007*"protection" + 0.007*"needs" + 0.006*"well" + 0.006*"good" + 0.006*"ensure" + 0.005*"response" + 0.005*"management" + 0.005*"Newcastle"', '0.017*"’" + 0.012*"plans" + 0.008*"needs" + 0.007*"good" + 0.006*"making" + 0.006*"protection" + 0.006*"Newcastle" + 0.006*"well" + 0.005*"progress" + 0.005*"planning"', '0.018*"’" + 0.011*"plans" + 0.009*"Newcastle" + 0.008*"needs" + 0.007*"good" + 0.007*"well" + 0.007*"progress" + 0.007*"protection" + 0.006*"need" + 0.006*"2021"']</t>
+    <t>['0.017*"’" + 0.010*"plans" + 0.008*"needs" + 0.007*"Newcastle" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.005*"ensure" + 0.005*"management" + 0.005*"need"', '0.017*"’" + 0.010*"plans" + 0.009*"needs" + 0.008*"good" + 0.008*"protection" + 0.007*"Newcastle" + 0.006*"progress" + 0.006*"management" + 0.006*"need" + 0.006*"planning"', '0.012*"’" + 0.011*"plans" + 0.007*"well" + 0.007*"protection" + 0.006*"making" + 0.006*"Newcastle" + 0.006*"needs" + 0.005*"progress" + 0.005*"10" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -2806,7 +2806,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"Norfolk" + 0.006*"needs" + 0.006*"well" + 0.005*"carers" + 0.005*"plans" + 0.005*"supported" + 0.004*"progress" + 0.004*"practice" + 0.004*"information"', '0.017*"’" + 0.008*"Norfolk" + 0.008*"well" + 0.007*"carers" + 0.006*"practice" + 0.005*"supported" + 0.005*"range" + 0.005*"effective" + 0.005*"needs" + 0.004*"plans"', '0.015*"’" + 0.010*"well" + 0.007*"Norfolk" + 0.007*"needs" + 0.006*"practice" + 0.006*"carers" + 0.005*"supported" + 0.005*"18" + 0.005*"leaders" + 0.004*"including"']</t>
+    <t>['0.015*"’" + 0.009*"Norfolk" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"supported" + 0.005*"carers" + 0.005*"including" + 0.005*"range" + 0.005*"18"', '0.013*"’" + 0.006*"well" + 0.006*"Norfolk" + 0.005*"carers" + 0.005*"supported" + 0.004*"plans" + 0.004*"leaders" + 0.004*"practice" + 0.004*"needs" + 0.004*"range"', '0.021*"’" + 0.009*"well" + 0.008*"Norfolk" + 0.007*"carers" + 0.006*"practice" + 0.006*"needs" + 0.005*"supported" + 0.005*"effective" + 0.005*"plans" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -2836,7 +2836,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"leaders" + 0.007*"practice" + 0.007*"needs" + 0.006*"planning" + 0.006*"risk" + 0.005*"many" + 0.005*"2021" + 0.005*"plans" + 0.005*"oversight"', '0.007*"’" + 0.006*"practice" + 0.006*"planning" + 0.005*"risk" + 0.005*"needs" + 0.004*"leaders" + 0.004*"many" + 0.004*"East" + 0.004*"delay" + 0.004*"Council"', '0.017*"’" + 0.009*"practice" + 0.008*"risk" + 0.007*"need" + 0.006*"leaders" + 0.006*"needs" + 0.006*"planning" + 0.005*"North" + 0.005*"quality" + 0.005*"Lincolnshire"']</t>
+    <t>['0.015*"’" + 0.010*"practice" + 0.009*"risk" + 0.008*"leaders" + 0.007*"needs" + 0.007*"planning" + 0.006*"need" + 0.005*"North" + 0.005*"quality" + 0.005*"East"', '0.011*"’" + 0.005*"practice" + 0.005*"planning" + 0.005*"needs" + 0.005*"Lincolnshire" + 0.005*"leaders" + 0.004*"2021" + 0.004*"need" + 0.004*"risk" + 0.004*"senior"', '0.014*"’" + 0.006*"leaders" + 0.005*"plans" + 0.005*"practice" + 0.005*"planning" + 0.005*"many" + 0.005*"October" + 0.005*"needs" + 0.004*"risk" + 0.004*"oversight"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -2863,7 +2863,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"‘" + 0.006*"North" + 0.006*"family" + 0.006*"well" + 0.005*"leaders" + 0.005*"10" + 0.005*"approach" + 0.005*"need" + 0.005*"protection"', '0.020*"’" + 0.006*"‘" + 0.006*"Lincolnshire" + 0.006*"North" + 0.005*"family" + 0.005*"approach" + 0.005*"need" + 0.004*"10" + 0.004*"team" + 0.004*"leaders"', '0.017*"’" + 0.006*"family" + 0.006*"‘" + 0.005*"Lincolnshire" + 0.005*"well" + 0.005*"leaders" + 0.005*"approach" + 0.004*"October" + 0.004*"2022" + 0.004*"need"']</t>
+    <t>['0.025*"’" + 0.008*"‘" + 0.006*"North" + 0.006*"Lincolnshire" + 0.006*"leaders" + 0.006*"approach" + 0.005*"family" + 0.005*"protection" + 0.005*"10" + 0.005*"need"', '0.016*"’" + 0.005*"‘" + 0.005*"well" + 0.005*"family" + 0.004*"North" + 0.004*"14" + 0.004*"leaders" + 0.004*"team" + 0.004*"approach" + 0.004*"Lincolnshire"', '0.017*"’" + 0.007*"family" + 0.007*"‘" + 0.005*"well" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"10" + 0.005*"approach" + 0.005*"North" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>940</t>
@@ -2893,7 +2893,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"practice" + 0.005*"Leaders" + 0.005*"impact" + 0.005*"NCT"', '0.013*"’" + 0.007*"well" + 0.007*"North" + 0.006*"quality" + 0.005*"need" + 0.005*"practice" + 0.005*"NCT" + 0.004*"plans" + 0.004*"impact" + 0.004*"Northamptonshire"', '0.015*"’" + 0.008*"Northamptonshire" + 0.006*"well" + 0.005*"Leaders" + 0.004*"North" + 0.004*"quality" + 0.004*"3" + 0.004*"impact" + 0.004*"plans" + 0.004*"needs"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.005*"However" + 0.005*"quality" + 0.005*"practice" + 0.005*"Northamptonshire" + 0.004*"North" + 0.004*"impact" + 0.004*"needs" + 0.004*"2022"', '0.023*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.006*"quality" + 0.006*"impact" + 0.005*"needs" + 0.005*"Leaders" + 0.005*"NCT" + 0.005*"e"', '0.013*"’" + 0.010*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.005*"practice" + 0.005*"quality" + 0.005*"need" + 0.005*"NCT" + 0.005*"3" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -2917,7 +2917,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"quality" + 0.005*"progress" + 0.005*"North" + 0.005*"always" + 0.005*"number" + 0.005*"well" + 0.004*"plans" + 0.004*"practice" + 0.004*"needs"', '0.018*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"always" + 0.006*"practice" + 0.006*"North" + 0.006*"need" + 0.006*"Somerset" + 0.006*"risk" + 0.006*"number"', '0.017*"’" + 0.008*"quality" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"number" + 0.005*"North" + 0.005*"always" + 0.005*"practice" + 0.005*"experienced" + 0.004*"progress"']</t>
+    <t>['0.020*"’" + 0.007*"always" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"progress" + 0.006*"need" + 0.006*"North" + 0.006*"quality" + 0.006*"practice" + 0.005*"number"', '0.013*"’" + 0.008*"quality" + 0.006*"always" + 0.006*"risk" + 0.006*"needs" + 0.005*"North" + 0.005*"practice" + 0.005*"experienced" + 0.005*"number" + 0.005*"need"', '0.016*"’" + 0.009*"quality" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"number" + 0.005*"North" + 0.005*"risk" + 0.005*"well" + 0.005*"practice" + 0.005*"oversight"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -2941,7 +2941,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"need" + 0.005*"quality" + 0.005*"needs" + 0.005*"make" + 0.005*"impact" + 0.004*"protection" + 0.004*"clear"', '0.017*"’" + 0.006*"well" + 0.005*"make" + 0.005*"leaders" + 0.005*"need" + 0.004*"needs" + 0.004*"quality" + 0.004*"experiences" + 0.004*"foster" + 0.004*"impact"', '0.013*"’" + 0.005*"leaders" + 0.005*"need" + 0.005*"progress" + 0.005*"well" + 0.004*"early" + 0.004*"quality" + 0.004*"impact" + 0.003*"make" + 0.003*"needs"']</t>
+    <t>['0.019*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"need" + 0.005*"quality" + 0.005*"make" + 0.005*"needs" + 0.004*"impact" + 0.004*"clear" + 0.004*"early"', '0.014*"’" + 0.004*"leaders" + 0.004*"need" + 0.004*"quality" + 0.004*"needs" + 0.004*"well" + 0.003*"good" + 0.003*"impact" + 0.003*"make" + 0.003*"foster"', '0.013*"’" + 0.006*"well" + 0.005*"need" + 0.005*"leaders" + 0.005*"make" + 0.005*"understand" + 0.004*"needs" + 0.004*"impact" + 0.004*"early" + 0.004*"way"']</t>
   </si>
   <si>
     <t>815</t>
@@ -2965,7 +2965,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"family" + 0.006*"Yorkshire" + 0.006*"needs" + 0.005*"‘" + 0.005*"North" + 0.004*"3" + 0.004*"7"', '0.020*"’" + 0.008*"well" + 0.007*"North" + 0.006*"needs" + 0.005*"Yorkshire" + 0.005*"practice" + 0.005*"family" + 0.004*"‘" + 0.004*"3" + 0.004*"supported"', '0.021*"’" + 0.009*"well" + 0.007*"North" + 0.007*"Yorkshire" + 0.006*"practice" + 0.005*"family" + 0.005*"needs" + 0.005*"‘" + 0.004*"3" + 0.004*"supported"']</t>
+    <t>['0.020*"’" + 0.008*"well" + 0.007*"North" + 0.006*"family" + 0.006*"Yorkshire" + 0.006*"practice" + 0.005*"needs" + 0.004*"3" + 0.004*"‘" + 0.004*"supported"', '0.021*"’" + 0.009*"well" + 0.007*"North" + 0.007*"practice" + 0.006*"Yorkshire" + 0.006*"family" + 0.005*"needs" + 0.005*"supported" + 0.005*"‘" + 0.004*"need"', '0.020*"’" + 0.007*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.006*"needs" + 0.005*"North" + 0.005*"‘" + 0.004*"7" + 0.004*"2023" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -2989,7 +2989,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.010*"well" + 0.010*"needs" + 0.008*"good" + 0.007*"experiences" + 0.007*"need" + 0.006*"impact" + 0.005*"practice" + 0.005*"quality" + 0.005*"leaders"', '0.020*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"good" + 0.005*"need" + 0.005*"practice" + 0.005*"effective" + 0.005*"impact" + 0.005*"education" + 0.004*"always"', '0.020*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"good" + 0.006*"need" + 0.005*"experiences" + 0.005*"quality" + 0.004*"practice" + 0.004*"education" + 0.004*"always"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"impact" + 0.005*"need" + 0.004*"experiences" + 0.004*"quality" + 0.004*"education" + 0.004*"progress"', '0.028*"’" + 0.013*"needs" + 0.011*"well" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.006*"experiences" + 0.006*"education" + 0.005*"leaders" + 0.005*"impact"', '0.016*"’" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"experiences" + 0.006*"quality" + 0.005*"need" + 0.005*"impact" + 0.004*"practice" + 0.004*"always"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3016,7 +3016,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"Nottingham" + 0.006*"effective" + 0.005*"impact" + 0.005*"However" + 0.005*"2022" + 0.004*"practice" + 0.004*"oversight"', '0.012*"’" + 0.006*"needs" + 0.005*"Nottingham" + 0.005*"oversight" + 0.005*"impact" + 0.005*"protection" + 0.005*"City" + 0.005*"effective" + 0.005*"risk" + 0.005*"plans"', '0.014*"’" + 0.009*"needs" + 0.005*"11" + 0.005*"Nottingham" + 0.005*"effective" + 0.005*"plans" + 0.005*"City" + 0.004*"impact" + 0.004*"consistently" + 0.004*"oversight"']</t>
+    <t>['0.016*"’" + 0.006*"effective" + 0.006*"needs" + 0.006*"Nottingham" + 0.005*"oversight" + 0.005*"practice" + 0.005*"City" + 0.005*"impact" + 0.005*"11" + 0.005*"plans"', '0.010*"’" + 0.007*"needs" + 0.004*"Nottingham" + 0.004*"11" + 0.004*"impact" + 0.004*"risk" + 0.004*"effective" + 0.004*"plans" + 0.004*"City" + 0.003*"However"', '0.014*"’" + 0.010*"needs" + 0.007*"plans" + 0.006*"Nottingham" + 0.005*"impact" + 0.005*"effective" + 0.005*"2022" + 0.004*"oversight" + 0.004*"July" + 0.004*"11"']</t>
   </si>
   <si>
     <t>891</t>
@@ -3034,7 +3034,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"well" + 0.006*"practice" + 0.005*"areas" + 0.005*"plans" + 0.005*"quality" + 0.005*"progress" + 0.005*"made" + 0.005*"ensure" + 0.004*"receive"', '0.014*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"receive" + 0.005*"ensure" + 0.005*"carers" + 0.005*"progress" + 0.005*"plans" + 0.005*"e"', '0.011*"’" + 0.009*"practice" + 0.006*"well" + 0.006*"needs" + 0.005*"quality" + 0.005*"receive" + 0.005*"ensure" + 0.005*"plans" + 0.004*"carers" + 0.004*"made"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"e" + 0.006*"receive" + 0.006*"progress" + 0.005*"made" + 0.005*"quality" + 0.005*"needs" + 0.005*"ensure"', '0.012*"’" + 0.008*"well" + 0.008*"practice" + 0.007*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.005*"receive" + 0.005*"areas" + 0.005*"carers" + 0.005*"made"', '0.013*"’" + 0.008*"practice" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.004*"progress" + 0.004*"quality" + 0.004*"made" + 0.004*"number" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3067,7 +3067,7 @@
     <t>0.176</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.009*"good" + 0.008*"practice" + 0.007*"well" + 0.007*"quality" + 0.006*"effective" + 0.006*"progress" + 0.006*"needs" + 0.006*"planning" + 0.006*"plans"', '0.009*"good" + 0.008*"needs" + 0.008*"effective" + 0.008*"’" + 0.007*"practice" + 0.007*"progress" + 0.006*"well" + 0.006*"planning" + 0.005*"plans" + 0.005*"information"', '0.012*"’" + 0.011*"needs" + 0.010*"practice" + 0.009*"good" + 0.008*"effective" + 0.007*"quality" + 0.006*"planning" + 0.006*"plans" + 0.006*"progress" + 0.005*"well"']</t>
+    <t>['0.010*"needs" + 0.010*"practice" + 0.009*"’" + 0.009*"good" + 0.008*"progress" + 0.006*"effective" + 0.006*"planning" + 0.006*"quality" + 0.006*"plans" + 0.005*"well"', '0.008*"effective" + 0.008*"’" + 0.008*"good" + 0.007*"needs" + 0.007*"practice" + 0.006*"quality" + 0.006*"planning" + 0.006*"progress" + 0.005*"well" + 0.004*"place"', '0.013*"’" + 0.010*"good" + 0.009*"effective" + 0.009*"needs" + 0.008*"practice" + 0.008*"well" + 0.007*"plans" + 0.007*"quality" + 0.006*"planning" + 0.006*"risk"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3097,7 +3097,7 @@
     <t>0.1848</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.012*"needs" + 0.007*"good" + 0.006*"number" + 0.005*"early" + 0.005*"plans" + 0.005*"education" + 0.005*"effective" + 0.005*"response" + 0.004*"Oxfordshire"', '0.012*"’" + 0.006*"needs" + 0.006*"number" + 0.006*"good" + 0.005*"early" + 0.005*"response" + 0.004*"practice" + 0.004*"Oxfordshire" + 0.004*"quality" + 0.004*"plans"', '0.014*"’" + 0.008*"needs" + 0.006*"good" + 0.006*"number" + 0.006*"protection" + 0.005*"early" + 0.005*"plans" + 0.005*"quality" + 0.004*"response" + 0.004*"Oxfordshire"']</t>
+    <t>['0.012*"’" + 0.010*"needs" + 0.007*"number" + 0.006*"good" + 0.005*"early" + 0.005*"live" + 0.004*"education" + 0.004*"plans" + 0.004*"response" + 0.004*"quality"', '0.014*"’" + 0.008*"needs" + 0.006*"good" + 0.005*"number" + 0.005*"protection" + 0.005*"early" + 0.005*"response" + 0.004*"plans" + 0.004*"education" + 0.004*"practice"', '0.014*"’" + 0.009*"needs" + 0.007*"good" + 0.005*"protection" + 0.005*"early" + 0.005*"number" + 0.005*"plans" + 0.005*"response" + 0.005*"effective" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3127,7 +3127,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"practice" + 0.006*"planning" + 0.006*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"need" + 0.005*"quality" + 0.005*"number" + 0.005*"risk"', '0.013*"’" + 0.008*"practice" + 0.007*"well" + 0.007*"good" + 0.007*"needs" + 0.006*"risk" + 0.006*"planning" + 0.005*"progress" + 0.005*"quality" + 0.005*"effective"', '0.016*"’" + 0.007*"well" + 0.007*"risk" + 0.006*"progress" + 0.006*"effective" + 0.006*"practice" + 0.006*"needs" + 0.005*"good" + 0.005*"quality" + 0.005*"including"']</t>
+    <t>['0.015*"’" + 0.008*"good" + 0.008*"practice" + 0.006*"well" + 0.006*"risk" + 0.006*"progress" + 0.006*"effective" + 0.005*"planning" + 0.005*"needs" + 0.004*"quality"', '0.013*"’" + 0.008*"needs" + 0.007*"practice" + 0.006*"well" + 0.006*"planning" + 0.006*"risk" + 0.005*"need" + 0.005*"effective" + 0.005*"progress" + 0.005*"including"', '0.014*"’" + 0.008*"well" + 0.007*"risk" + 0.006*"planning" + 0.006*"practice" + 0.006*"good" + 0.006*"needs" + 0.005*"quality" + 0.005*"need" + 0.005*"including"']</t>
   </si>
   <si>
     <t>879</t>
@@ -3154,7 +3154,7 @@
     <t>0.1594</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"well" + 0.008*"good" + 0.008*"However" + 0.006*"needs" + 0.006*"quality" + 0.005*"progress" + 0.005*"result" + 0.005*"number" + 0.004*"plans"', '0.016*"’" + 0.009*"well" + 0.008*"quality" + 0.008*"good" + 0.008*"However" + 0.007*"progress" + 0.007*"needs" + 0.006*"timely" + 0.006*"leaders" + 0.005*"effective"', '0.014*"’" + 0.010*"However" + 0.010*"good" + 0.010*"needs" + 0.009*"quality" + 0.008*"well" + 0.007*"timely" + 0.006*"progress" + 0.006*"plans" + 0.006*"effective"']</t>
+    <t>['0.013*"’" + 0.010*"However" + 0.009*"well" + 0.009*"good" + 0.009*"needs" + 0.009*"quality" + 0.007*"progress" + 0.006*"timely" + 0.006*"plans" + 0.006*"leaders"', '0.013*"’" + 0.008*"well" + 0.007*"good" + 0.006*"However" + 0.006*"quality" + 0.006*"result" + 0.005*"needs" + 0.005*"timely" + 0.005*"plans" + 0.004*"protection"', '0.017*"’" + 0.010*"However" + 0.009*"good" + 0.009*"well" + 0.008*"needs" + 0.008*"quality" + 0.007*"progress" + 0.006*"effective" + 0.006*"number" + 0.006*"timely"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3184,7 +3184,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.010*"care-experienced" + 0.008*"well" + 0.007*"family" + 0.007*"Portsmouth" + 0.005*"needs" + 0.005*"practice" + 0.005*"19" + 0.005*"foster" + 0.005*"plans"', '0.015*"’" + 0.006*"well" + 0.006*"care-experienced" + 0.006*"Portsmouth" + 0.005*"needs" + 0.004*"plans" + 0.004*"need" + 0.004*"practice" + 0.004*"family" + 0.004*"leaders"', '0.019*"’" + 0.009*"needs" + 0.007*"care-experienced" + 0.007*"Portsmouth" + 0.007*"health" + 0.006*"well" + 0.006*"plans" + 0.005*"risk" + 0.005*"leaders" + 0.005*"15"']</t>
+    <t>['0.011*"’" + 0.008*"care-experienced" + 0.007*"well" + 0.005*"Portsmouth" + 0.005*"needs" + 0.005*"plans" + 0.004*"leaders" + 0.004*"health" + 0.004*"family" + 0.004*"practice"', '0.019*"’" + 0.007*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"well" + 0.005*"family" + 0.005*"plans" + 0.005*"health" + 0.005*"risk" + 0.005*"15"', '0.018*"’" + 0.009*"well" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"family" + 0.006*"health" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3217,7 +3217,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"number" + 0.006*"quality" + 0.006*"plans" + 0.006*"good" + 0.005*"well" + 0.005*"However" + 0.005*"practice" + 0.005*"effective" + 0.005*"needs"', '0.019*"’" + 0.008*"well" + 0.006*"good" + 0.006*"quality" + 0.006*"need" + 0.006*"effective" + 0.006*"plans" + 0.005*"number" + 0.005*"timely" + 0.005*"always"', '0.014*"’" + 0.008*"number" + 0.007*"quality" + 0.006*"plans" + 0.005*"well" + 0.005*"timely" + 0.005*"practice" + 0.005*"need" + 0.004*"effective" + 0.004*"needs"']</t>
+    <t>['0.018*"’" + 0.008*"number" + 0.007*"quality" + 0.007*"plans" + 0.007*"good" + 0.007*"well" + 0.006*"need" + 0.006*"effective" + 0.005*"timely" + 0.005*"practice"', '0.014*"’" + 0.006*"quality" + 0.006*"plans" + 0.005*"effective" + 0.005*"well" + 0.005*"need" + 0.005*"number" + 0.005*"good" + 0.005*"practice" + 0.004*"always"', '0.015*"’" + 0.007*"well" + 0.007*"number" + 0.006*"quality" + 0.005*"However" + 0.005*"carers" + 0.005*"plans" + 0.005*"arrangements" + 0.005*"timely" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3238,7 +3238,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"plans" + 0.006*"leaders" + 0.005*"However" + 0.005*"consistently" + 0.005*"needs" + 0.004*"Cleveland" + 0.004*"2022" + 0.004*"practice" + 0.004*"July"', '0.016*"’" + 0.007*"However" + 0.006*"plans" + 0.006*"leaders" + 0.006*"needs" + 0.006*"2022" + 0.005*"consistently" + 0.005*"risk" + 0.005*"practice" + 0.005*"20"', '0.022*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"carers" + 0.005*"Redcar" + 0.005*"consistently" + 0.005*"20" + 0.005*"plans" + 0.005*"risk" + 0.005*"practice"']</t>
+    <t>['0.019*"’" + 0.007*"leaders" + 0.005*"Cleveland" + 0.005*"20" + 0.005*"consistently" + 0.005*"plans" + 0.005*"2022" + 0.005*"risk" + 0.005*"Redcar" + 0.005*"However"', '0.014*"’" + 0.006*"However" + 0.006*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"Redcar" + 0.005*"consistently" + 0.005*"1" + 0.005*"carers" + 0.005*"2022"', '0.019*"’" + 0.006*"needs" + 0.006*"leaders" + 0.006*"However" + 0.005*"plans" + 0.005*"consistently" + 0.005*"practice" + 0.005*"20" + 0.004*"2022" + 0.004*"Cleveland"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3265,7 +3265,7 @@
     <t>0.1837</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"experienced" + 0.010*"practice" + 0.008*"needs" + 0.005*"plans" + 0.005*"response" + 0.004*"PAs" + 0.004*"consistently" + 0.004*"2023" + 0.004*"Rochdale"', '0.027*"’" + 0.009*"needs" + 0.008*"experienced" + 0.007*"practice" + 0.007*"plans" + 0.006*"response" + 0.006*"quality" + 0.006*"good" + 0.006*"consistently" + 0.006*"Rochdale"', '0.017*"’" + 0.010*"experienced" + 0.007*"practice" + 0.006*"response" + 0.006*"consistently" + 0.006*"good" + 0.005*"well" + 0.005*"3" + 0.005*"needs" + 0.005*"plans"']</t>
+    <t>['0.026*"’" + 0.011*"practice" + 0.011*"experienced" + 0.009*"needs" + 0.006*"response" + 0.006*"consistently" + 0.005*"plans" + 0.005*"quality" + 0.005*"good" + 0.004*"well"', '0.018*"’" + 0.009*"experienced" + 0.007*"plans" + 0.007*"response" + 0.006*"practice" + 0.006*"needs" + 0.006*"quality" + 0.005*"consistently" + 0.005*"Rochdale" + 0.005*"3"', '0.015*"’" + 0.008*"experienced" + 0.007*"needs" + 0.005*"practice" + 0.005*"good" + 0.005*"well" + 0.005*"plans" + 0.005*"PAs" + 0.005*"Rochdale" + 0.004*"23"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3289,7 +3289,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"Rotherham" + 0.006*"needs" + 0.005*"well" + 0.005*"clear" + 0.005*"good" + 0.004*"ensure" + 0.004*"Metropolitan" + 0.004*"Borough" + 0.004*"plans"', '0.017*"’" + 0.010*"Rotherham" + 0.007*"needs" + 0.006*"good" + 0.005*"However" + 0.005*"Council" + 0.005*"ensure" + 0.005*"well" + 0.004*"plans" + 0.004*"27"', '0.016*"’" + 0.006*"needs" + 0.006*"Rotherham" + 0.006*"well" + 0.005*"Council" + 0.005*"plans" + 0.004*"good" + 0.004*"ensure" + 0.004*"July" + 0.004*"Borough"']</t>
+    <t>['0.017*"’" + 0.009*"Rotherham" + 0.006*"needs" + 0.005*"good" + 0.005*"well" + 0.005*"ensure" + 0.005*"Council" + 0.005*"plans" + 0.004*"1" + 0.004*"However"', '0.014*"’" + 0.005*"Council" + 0.005*"Rotherham" + 0.005*"well" + 0.005*"needs" + 0.004*"plans" + 0.004*"July" + 0.004*"27" + 0.004*"However" + 0.004*"Metropolitan"', '0.014*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"ensure" + 0.006*"good" + 0.005*"well" + 0.005*"However" + 0.004*"clear" + 0.004*"plans" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3313,7 +3313,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.010*"well" + 0.009*"’" + 0.007*"practice" + 0.006*"highly" + 0.005*"needs" + 0.005*"strong" + 0.004*"high" + 0.004*"leaders" + 0.004*"effective" + 0.004*"progress"', '0.017*"well" + 0.013*"practice" + 0.012*"’" + 0.007*"highly" + 0.006*"strong" + 0.006*"needs" + 0.005*"leaders" + 0.005*"effective" + 0.005*"high" + 0.004*"need"', '0.012*"’" + 0.012*"well" + 0.010*"practice" + 0.008*"highly" + 0.007*"strong" + 0.006*"effective" + 0.005*"needs" + 0.005*"professionals" + 0.005*"leaders" + 0.004*"range"']</t>
+    <t>['0.013*"’" + 0.011*"well" + 0.008*"practice" + 0.006*"highly" + 0.006*"strong" + 0.005*"progress" + 0.005*"timely" + 0.004*"leaders" + 0.004*"needs" + 0.004*"effective"', '0.017*"well" + 0.012*"practice" + 0.011*"’" + 0.007*"strong" + 0.007*"highly" + 0.006*"effective" + 0.005*"needs" + 0.005*"leaders" + 0.004*"high" + 0.004*"professionals"', '0.011*"practice" + 0.011*"’" + 0.011*"well" + 0.008*"highly" + 0.007*"needs" + 0.006*"strong" + 0.005*"leaders" + 0.005*"high" + 0.005*"effective" + 0.004*"professionals"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3340,7 +3340,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"well" + 0.008*"plans" + 0.007*"needs" + 0.005*"good" + 0.005*"clear" + 0.005*"risk" + 0.005*"supported" + 0.005*"need" + 0.005*"appropriate"', '0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.005*"good" + 0.004*"practice" + 0.004*"effective" + 0.004*"need" + 0.004*"Kingston" + 0.004*"risk"', '0.013*"’" + 0.009*"plans" + 0.008*"needs" + 0.008*"well" + 0.005*"effective" + 0.005*"good" + 0.004*"progress" + 0.004*"parents" + 0.004*"practice" + 0.004*"clear"']</t>
+    <t>['0.012*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"needs" + 0.005*"good" + 0.005*"effective" + 0.005*"clear" + 0.005*"practice" + 0.004*"risk" + 0.004*"progress"', '0.013*"’" + 0.009*"plans" + 0.007*"needs" + 0.007*"well" + 0.005*"need" + 0.004*"good" + 0.004*"appropriate" + 0.004*"Kingston" + 0.004*"progress" + 0.004*"range"', '0.015*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"good" + 0.005*"practice" + 0.005*"effective" + 0.004*"clear" + 0.004*"supported" + 0.004*"parents"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3367,7 +3367,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.005*"quality" + 0.005*"well" + 0.004*"needs" + 0.004*"information" + 0.004*"use" + 0.004*"plans" + 0.004*"always" + 0.004*"benefit" + 0.003*"management"', '0.009*"’" + 0.006*"well" + 0.005*"plans" + 0.005*"quality" + 0.005*"needs" + 0.004*"However" + 0.004*"changes" + 0.003*"information" + 0.003*"actions" + 0.003*"always"', '0.012*"’" + 0.005*"well" + 0.005*"needs" + 0.005*"effective" + 0.005*"quality" + 0.005*"plans" + 0.005*"benefit" + 0.004*"use" + 0.004*"health" + 0.004*"information"']</t>
+    <t>['0.011*"’" + 0.006*"well" + 0.005*"quality" + 0.005*"information" + 0.004*"needs" + 0.004*"plans" + 0.004*"actions" + 0.004*"always" + 0.004*"effective" + 0.003*"use"', '0.009*"’" + 0.006*"well" + 0.005*"plans" + 0.005*"needs" + 0.004*"use" + 0.004*"benefit" + 0.004*"quality" + 0.004*"informed" + 0.004*"health" + 0.004*"effective"', '0.014*"’" + 0.005*"quality" + 0.005*"needs" + 0.005*"well" + 0.004*"plans" + 0.004*"benefit" + 0.004*"management" + 0.004*"However" + 0.004*"effective" + 0.004*"use"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3388,7 +3388,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.012*"well" + 0.012*"’" + 0.009*"needs" + 0.008*"good" + 0.007*"effective" + 0.006*"ensure" + 0.006*"need" + 0.006*"team" + 0.005*"practice" + 0.005*"protection"', '0.015*"’" + 0.010*"needs" + 0.009*"well" + 0.008*"team" + 0.008*"good" + 0.008*"need" + 0.007*"enough" + 0.007*"practice" + 0.007*"protection" + 0.006*"plans"', '0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"good" + 0.006*"practice" + 0.005*"team" + 0.005*"need" + 0.005*"plans" + 0.004*"family" + 0.004*"ensure"']</t>
+    <t>['0.015*"’" + 0.011*"needs" + 0.011*"well" + 0.008*"need" + 0.007*"good" + 0.007*"practice" + 0.006*"effective" + 0.006*"ensure" + 0.006*"team" + 0.005*"family"', '0.011*"’" + 0.010*"well" + 0.010*"needs" + 0.008*"good" + 0.007*"team" + 0.006*"plans" + 0.006*"need" + 0.006*"practice" + 0.005*"protection" + 0.005*"enough"', '0.012*"’" + 0.008*"well" + 0.007*"good" + 0.007*"team" + 0.006*"enough" + 0.006*"protection" + 0.006*"needs" + 0.005*"plans" + 0.005*"practice" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3412,7 +3412,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"needs" + 0.007*"effective" + 0.006*"Salford" + 0.006*"well" + 0.006*"plans" + 0.005*"practice" + 0.005*"10" + 0.005*"6" + 0.004*"progress"', '0.014*"’" + 0.009*"plans" + 0.008*"needs" + 0.007*"well" + 0.005*"quality" + 0.005*"planning" + 0.005*"effective" + 0.005*"practice" + 0.005*"appropriate" + 0.004*"progress"', '0.015*"’" + 0.008*"well" + 0.008*"plans" + 0.008*"effective" + 0.007*"Salford" + 0.006*"needs" + 0.005*"planning" + 0.005*"leaders" + 0.005*"experiences" + 0.005*"practice"']</t>
+    <t>['0.012*"’" + 0.007*"needs" + 0.007*"effective" + 0.006*"plans" + 0.005*"well" + 0.005*"Salford" + 0.005*"10" + 0.004*"quality" + 0.004*"practice" + 0.004*"planning"', '0.014*"’" + 0.009*"plans" + 0.008*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"Salford" + 0.006*"planning" + 0.005*"progress" + 0.005*"leaders" + 0.005*"practice"', '0.014*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"Salford" + 0.005*"experiences" + 0.005*"appropriate" + 0.005*"practice" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3433,7 +3433,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"plans" + 0.006*"needs" + 0.006*"Sandwell" + 0.005*"quality" + 0.005*"changes" + 0.004*"Trust" + 0.004*"well" + 0.004*"9" + 0.004*"education"', '0.016*"’" + 0.010*"needs" + 0.008*"Sandwell" + 0.008*"plans" + 0.007*"well" + 0.006*"education" + 0.005*"effective" + 0.005*"Trust" + 0.005*"quality" + 0.005*"progress"', '0.013*"’" + 0.008*"well" + 0.007*"Sandwell" + 0.007*"quality" + 0.006*"needs" + 0.006*"plans" + 0.005*"number" + 0.005*"20" + 0.004*"progress" + 0.004*"May"']</t>
+    <t>['0.011*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Sandwell" + 0.005*"quality" + 0.005*"education" + 0.004*"effective" + 0.004*"good" + 0.004*"changes"', '0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"Sandwell" + 0.005*"quality" + 0.005*"plans" + 0.005*"number" + 0.004*"progress" + 0.004*"many" + 0.004*"effective"', '0.015*"’" + 0.009*"needs" + 0.009*"plans" + 0.008*"Sandwell" + 0.006*"well" + 0.006*"quality" + 0.006*"Trust" + 0.006*"20" + 0.005*"9" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3454,7 +3454,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.005*"protection" + 0.005*"practice" + 0.005*"planning" + 0.005*"plans" + 0.004*"management" + 0.004*"4" + 0.004*"including" + 0.004*"many"', '0.016*"’" + 0.009*"needs" + 0.007*"practice" + 0.005*"oversight" + 0.005*"lack" + 0.004*"including" + 0.004*"always" + 0.004*"◼" + 0.004*"response" + 0.004*"many"', '0.017*"’" + 0.011*"needs" + 0.007*"oversight" + 0.006*"practice" + 0.005*"including" + 0.005*"March" + 0.005*"protection" + 0.005*"management" + 0.005*"◼" + 0.005*"lack"']</t>
+    <t>['0.014*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"Sefton" + 0.005*"many" + 0.005*"protection" + 0.005*"including" + 0.005*"March" + 0.005*"◼" + 0.004*"21"', '0.015*"’" + 0.008*"needs" + 0.006*"practice" + 0.006*"oversight" + 0.005*"protection" + 0.005*"February" + 0.005*"4" + 0.005*"including" + 0.005*"lack" + 0.005*"need"', '0.019*"’" + 0.010*"needs" + 0.006*"oversight" + 0.006*"lack" + 0.006*"practice" + 0.005*"management" + 0.005*"many" + 0.005*"always" + 0.005*"timely" + 0.005*"including"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3484,7 +3484,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.012*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.006*"leaders" + 0.006*"health" + 0.006*"practice" + 0.005*"quality" + 0.005*"11" + 0.005*"adviser"', '0.013*"’" + 0.008*"Sheffield" + 0.007*"needs" + 0.006*"well" + 0.004*"health" + 0.004*"practice" + 0.004*"leaders" + 0.004*"experiences" + 0.004*"ensure" + 0.004*"effective"', '0.022*"’" + 0.011*"Sheffield" + 0.008*"needs" + 0.006*"practice" + 0.006*"leaders" + 0.005*"well" + 0.005*"good" + 0.005*"health" + 0.005*"mental" + 0.004*"quality"']</t>
+    <t>['0.022*"’" + 0.010*"Sheffield" + 0.009*"needs" + 0.006*"well" + 0.006*"practice" + 0.005*"leaders" + 0.005*"11" + 0.005*"adviser" + 0.004*"quality" + 0.004*"plans"', '0.017*"’" + 0.011*"Sheffield" + 0.009*"needs" + 0.007*"well" + 0.006*"health" + 0.006*"leaders" + 0.006*"practice" + 0.005*"quality" + 0.005*"experiences" + 0.004*"protection"', '0.022*"’" + 0.012*"Sheffield" + 0.007*"needs" + 0.007*"well" + 0.006*"leaders" + 0.005*"practice" + 0.005*"health" + 0.005*"good" + 0.004*"plans" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3511,7 +3511,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"needs" + 0.006*"Shropshire" + 0.006*"progress" + 0.006*"well" + 0.005*"plans" + 0.004*"need" + 0.004*"2022" + 0.004*"ensure" + 0.004*"making"', '0.018*"’" + 0.009*"needs" + 0.008*"Shropshire" + 0.008*"well" + 0.006*"making" + 0.006*"plans" + 0.006*"2022" + 0.006*"progress" + 0.005*"training" + 0.005*"7"', '0.018*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Shropshire" + 0.005*"progress" + 0.005*"7" + 0.005*"plans" + 0.004*"leaders" + 0.004*"2022" + 0.004*"making"']</t>
+    <t>['0.008*"’" + 0.007*"needs" + 0.006*"Shropshire" + 0.004*"progress" + 0.004*"making" + 0.004*"well" + 0.004*"2022" + 0.004*"plans" + 0.004*"leaders" + 0.004*"practice"', '0.016*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Shropshire" + 0.006*"plans" + 0.006*"progress" + 0.006*"11" + 0.005*"2022" + 0.005*"making" + 0.005*"training"', '0.024*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.006*"progress" + 0.005*"7" + 0.005*"plans" + 0.005*"making" + 0.005*"2022" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3532,7 +3532,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Slough" + 0.007*"practice" + 0.007*"needs" + 0.007*"quality" + 0.005*"plans" + 0.005*"3" + 0.005*"leaders" + 0.005*"supported" + 0.005*"need"', '0.012*"’" + 0.006*"plans" + 0.006*"Slough" + 0.005*"needs" + 0.005*"quality" + 0.005*"impact" + 0.005*"need" + 0.004*"3" + 0.004*"However" + 0.004*"practice"', '0.018*"’" + 0.008*"Slough" + 0.007*"plans" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"impact" + 0.005*"leaders" + 0.004*"January" + 0.004*"supported"']</t>
+    <t>['0.014*"’" + 0.009*"Slough" + 0.007*"plans" + 0.007*"quality" + 0.006*"practice" + 0.006*"3" + 0.006*"needs" + 0.005*"leaders" + 0.005*"senior" + 0.005*"impact"', '0.007*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"quality" + 0.005*"practice" + 0.004*"Slough" + 0.004*"timely" + 0.004*"However" + 0.004*"impact" + 0.003*"23"', '0.021*"’" + 0.008*"Slough" + 0.007*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"practice" + 0.005*"impact" + 0.005*"plans" + 0.005*"supported" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3553,7 +3553,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"lack" + 0.007*"2022" + 0.007*"Solihull" + 0.006*"need" + 0.006*"significant" + 0.005*"risk" + 0.005*"progress" + 0.004*"quality" + 0.004*"focus"', '0.018*"’" + 0.010*"lack" + 0.009*"2022" + 0.006*"risk" + 0.006*"need" + 0.006*"experiences" + 0.006*"Solihull" + 0.006*"practice" + 0.005*"quality" + 0.005*"significant"', '0.015*"’" + 0.011*"lack" + 0.009*"2022" + 0.006*"need" + 0.006*"quality" + 0.006*"practice" + 0.006*"Solihull" + 0.006*"risk" + 0.005*"effective" + 0.005*"means"']</t>
+    <t>['0.015*"’" + 0.007*"2022" + 0.007*"lack" + 0.006*"need" + 0.006*"effective" + 0.006*"experiences" + 0.005*"risk" + 0.005*"Solihull" + 0.005*"means" + 0.005*"practice"', '0.017*"’" + 0.011*"lack" + 0.008*"2022" + 0.006*"need" + 0.006*"quality" + 0.006*"Solihull" + 0.006*"practice" + 0.005*"risk" + 0.005*"experiences" + 0.005*"significant"', '0.014*"’" + 0.013*"lack" + 0.009*"2022" + 0.007*"Solihull" + 0.006*"risk" + 0.006*"need" + 0.006*"quality" + 0.005*"significant" + 0.005*"delay" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3574,7 +3574,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"good" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"leaders" + 0.006*"supported" + 0.006*"including" + 0.005*"number"', '0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"progress" + 0.005*"plans" + 0.005*"leaders" + 0.004*"practice" + 0.004*"understand" + 0.004*"good"', '0.019*"’" + 0.010*"needs" + 0.010*"well" + 0.007*"Somerset" + 0.005*"progress" + 0.005*"good" + 0.005*"need" + 0.005*"plans" + 0.005*"regularly" + 0.005*"family"']</t>
+    <t>['0.014*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"need" + 0.005*"understand" + 0.005*"Somerset" + 0.005*"leaders" + 0.004*"practice" + 0.004*"supported"', '0.020*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"Somerset" + 0.007*"good" + 0.006*"progress" + 0.006*"plans" + 0.005*"including" + 0.005*"number" + 0.005*"positive"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Somerset" + 0.007*"plans" + 0.006*"leaders" + 0.005*"supported" + 0.005*"practice" + 0.005*"family" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3595,7 +3595,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.011*"well" + 0.011*"quality" + 0.008*"’" + 0.008*"leaders" + 0.007*"plans" + 0.006*"progress" + 0.006*"needs" + 0.005*"timely" + 0.005*"good" + 0.005*"South"', '0.011*"quality" + 0.010*"well" + 0.008*"leaders" + 0.008*"’" + 0.007*"good" + 0.007*"plans" + 0.006*"timely" + 0.006*"needs" + 0.005*"Senior" + 0.005*"practice"', '0.011*"well" + 0.010*"’" + 0.009*"quality" + 0.009*"plans" + 0.008*"leaders" + 0.008*"good" + 0.006*"timely" + 0.005*"progress" + 0.005*"needs" + 0.005*"always"']</t>
+    <t>['0.012*"well" + 0.012*"quality" + 0.010*"leaders" + 0.009*"plans" + 0.009*"’" + 0.007*"good" + 0.006*"timely" + 0.005*"needs" + 0.005*"progress" + 0.005*"always"', '0.010*"quality" + 0.009*"well" + 0.008*"’" + 0.008*"leaders" + 0.007*"plans" + 0.007*"good" + 0.005*"needs" + 0.005*"timely" + 0.005*"practice" + 0.005*"Senior"', '0.010*"well" + 0.009*"’" + 0.008*"quality" + 0.007*"good" + 0.007*"timely" + 0.007*"leaders" + 0.006*"progress" + 0.006*"plans" + 0.006*"needs" + 0.005*"◼"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -3625,7 +3625,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"South" + 0.006*"Tyneside" + 0.005*"effective" + 0.005*"needs" + 0.005*"oversight" + 0.004*"However" + 0.004*"risk" + 0.004*"5" + 0.004*"14"', '0.031*"’" + 0.012*"needs" + 0.008*"Tyneside" + 0.008*"South" + 0.006*"carers" + 0.006*"9" + 0.006*"oversight" + 0.005*"management" + 0.005*"effective" + 0.005*"15"', '0.016*"’" + 0.007*"South" + 0.007*"needs" + 0.006*"Tyneside" + 0.005*"management" + 0.005*"However" + 0.005*"practice" + 0.004*"oversight" + 0.004*"leaders" + 0.004*"2023"']</t>
+    <t>['0.023*"’" + 0.009*"needs" + 0.008*"South" + 0.006*"However" + 0.006*"oversight" + 0.005*"effective" + 0.005*"Tyneside" + 0.005*"carers" + 0.005*"9" + 0.005*"February"', '0.026*"’" + 0.009*"Tyneside" + 0.008*"South" + 0.008*"needs" + 0.005*"management" + 0.005*"2022" + 0.005*"However" + 0.005*"effective" + 0.005*"homes" + 0.005*"2023"', '0.023*"’" + 0.010*"needs" + 0.007*"Tyneside" + 0.006*"South" + 0.006*"oversight" + 0.005*"14" + 0.005*"5" + 0.005*"carers" + 0.005*"risk" + 0.004*"9"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -3652,7 +3652,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"plans" + 0.004*"experiences" + 0.004*"improve" + 0.004*"needs" + 0.004*"Southampton" + 0.004*"June" + 0.004*"including" + 0.004*"progress" + 0.004*"leaders"', '0.014*"’" + 0.005*"Southampton" + 0.005*"plans" + 0.004*"well" + 0.004*"progress" + 0.004*"timely" + 0.004*"including" + 0.004*"good" + 0.004*"needs" + 0.004*"make"', '0.019*"’" + 0.006*"Southampton" + 0.006*"plans" + 0.005*"progress" + 0.005*"5" + 0.005*"improve" + 0.005*"16" + 0.005*"including" + 0.005*"needs" + 0.004*"2023"']</t>
+    <t>['0.013*"’" + 0.006*"improve" + 0.006*"Southampton" + 0.005*"progress" + 0.005*"plans" + 0.005*"June" + 0.005*"5" + 0.004*"provide" + 0.004*"2023" + 0.004*"experiences"', '0.021*"’" + 0.006*"plans" + 0.005*"Southampton" + 0.005*"needs" + 0.005*"including" + 0.005*"16" + 0.004*"timely" + 0.004*"experiences" + 0.004*"well" + 0.004*"2023"', '0.013*"’" + 0.006*"plans" + 0.005*"progress" + 0.005*"5" + 0.005*"Southampton" + 0.004*"experiences" + 0.004*"improve" + 0.004*"timely" + 0.004*"including" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -3682,7 +3682,7 @@
     <t>to requires improvement</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"quality" + 0.006*"planning" + 0.005*"leaders" + 0.005*"number" + 0.005*"always" + 0.005*"However" + 0.005*"within" + 0.004*"Southend" + 0.004*"carers"', '0.012*"’" + 0.009*"planning" + 0.008*"quality" + 0.008*"practice" + 0.006*"leaders" + 0.006*"always" + 0.006*"need" + 0.005*"protection" + 0.005*"number" + 0.005*"risk"', '0.017*"’" + 0.008*"planning" + 0.008*"practice" + 0.006*"leaders" + 0.006*"effective" + 0.005*"protection" + 0.005*"quality" + 0.005*"needs" + 0.005*"progress" + 0.005*"number"']</t>
+    <t>['0.013*"’" + 0.008*"planning" + 0.007*"practice" + 0.006*"leaders" + 0.006*"number" + 0.006*"quality" + 0.005*"within" + 0.005*"effective" + 0.005*"carers" + 0.005*"protection"', '0.013*"’" + 0.009*"planning" + 0.006*"practice" + 0.006*"protection" + 0.006*"quality" + 0.006*"leaders" + 0.005*"within" + 0.005*"good" + 0.005*"always" + 0.005*"needs"', '0.014*"’" + 0.008*"quality" + 0.007*"planning" + 0.007*"practice" + 0.006*"need" + 0.006*"leaders" + 0.005*"always" + 0.005*"effective" + 0.005*"number" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -3700,7 +3700,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.008*"Helens" + 0.007*"well" + 0.007*"St" + 0.006*"progress" + 0.006*"10" + 0.006*"receive" + 0.006*"need" + 0.005*"2023"', '0.014*"’" + 0.009*"Helens" + 0.007*"well" + 0.006*"21" + 0.006*"St" + 0.005*"risk" + 0.005*"10" + 0.005*"needs" + 0.005*"progress" + 0.005*"receive"', '0.019*"’" + 0.010*"St" + 0.007*"good" + 0.007*"needs" + 0.006*"Helens" + 0.006*"progress" + 0.006*"need" + 0.005*"well" + 0.005*"21" + 0.005*"receive"']</t>
+    <t>['0.018*"’" + 0.010*"St" + 0.008*"Helens" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.005*"receive" + 0.005*"risk" + 0.005*"10"', '0.013*"’" + 0.008*"needs" + 0.007*"St" + 0.007*"Helens" + 0.006*"well" + 0.006*"need" + 0.006*"10" + 0.006*"progress" + 0.006*"21" + 0.005*"receive"', '0.016*"’" + 0.008*"Helens" + 0.006*"St" + 0.006*"well" + 0.005*"progress" + 0.005*"effective" + 0.005*"risk" + 0.005*"needs" + 0.005*"21" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -3721,7 +3721,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.013*"needs" + 0.007*"quality" + 0.007*"Staffordshire" + 0.006*"progress" + 0.006*"practice" + 0.006*"oversight" + 0.005*"ensure" + 0.005*"plans" + 0.005*"health"', '0.014*"’" + 0.007*"needs" + 0.005*"quality" + 0.005*"health" + 0.005*"oversight" + 0.004*"progress" + 0.004*"ensure" + 0.004*"Staffordshire" + 0.004*"plans" + 0.004*"practice"', '0.018*"’" + 0.012*"needs" + 0.006*"health" + 0.006*"ensure" + 0.006*"practice" + 0.006*"oversight" + 0.005*"progress" + 0.005*"plans" + 0.005*"quality" + 0.005*"impact"']</t>
+    <t>['0.021*"’" + 0.010*"needs" + 0.007*"progress" + 0.006*"practice" + 0.006*"ensure" + 0.005*"quality" + 0.005*"oversight" + 0.005*"health" + 0.005*"6" + 0.005*"2023"', '0.014*"’" + 0.012*"needs" + 0.006*"health" + 0.006*"quality" + 0.006*"practice" + 0.006*"Staffordshire" + 0.006*"oversight" + 0.005*"plans" + 0.005*"ensure" + 0.005*"progress"', '0.017*"’" + 0.012*"needs" + 0.006*"quality" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.005*"ensure" + 0.005*"10" + 0.005*"impact" + 0.005*"progress" + 0.005*"health"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -3745,7 +3745,7 @@
     <t>18/05/22</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"Stockport" + 0.006*"practice" + 0.005*"plans" + 0.005*"risk" + 0.005*"team" + 0.004*"ensure" + 0.004*"28"', '0.010*"’" + 0.009*"well" + 0.008*"practice" + 0.007*"strong" + 0.007*"Stockport" + 0.006*"plans" + 0.005*"needs" + 0.005*"ensure" + 0.005*"risk" + 0.004*"leaders"', '0.014*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"Stockport" + 0.005*"needs" + 0.005*"risk" + 0.005*"strong" + 0.005*"leaders" + 0.005*"2022" + 0.004*"quality"']</t>
+    <t>['0.011*"’" + 0.007*"practice" + 0.007*"needs" + 0.007*"well" + 0.006*"Stockport" + 0.005*"strong" + 0.005*"risk" + 0.005*"quality" + 0.004*"ensure" + 0.004*"plans"', '0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.006*"risk" + 0.005*"Stockport" + 0.005*"needs" + 0.004*"team" + 0.004*"range" + 0.004*"ensure" + 0.004*"strong"', '0.012*"’" + 0.008*"well" + 0.008*"Stockport" + 0.007*"practice" + 0.007*"plans" + 0.006*"strong" + 0.006*"needs" + 0.005*"28" + 0.005*"ensure" + 0.005*"March"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -3778,7 +3778,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.008*"plans" + 0.007*"leaders" + 0.006*"good" + 0.006*"well" + 0.006*"on-Tees" + 0.005*"needs" + 0.005*"quality" + 0.005*"Stockton" + 0.005*"understand"', '0.016*"’" + 0.008*"leaders" + 0.008*"well" + 0.007*"quality" + 0.007*"plans" + 0.006*"Stockton" + 0.006*"senior" + 0.005*"needs" + 0.005*"good" + 0.005*"on-Tees"', '0.018*"’" + 0.010*"leaders" + 0.009*"plans" + 0.008*"needs" + 0.007*"on-Tees" + 0.007*"Stockton" + 0.005*"well" + 0.005*"good" + 0.005*"carers" + 0.005*"quality"']</t>
+    <t>['0.025*"’" + 0.010*"leaders" + 0.009*"plans" + 0.007*"well" + 0.007*"on-Tees" + 0.007*"needs" + 0.006*"Stockton" + 0.006*"quality" + 0.006*"17" + 0.005*"senior"', '0.012*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"Stockton" + 0.005*"good" + 0.005*"quality" + 0.004*"on-Tees" + 0.004*"progress"', '0.017*"’" + 0.008*"plans" + 0.007*"leaders" + 0.007*"needs" + 0.007*"quality" + 0.006*"Stockton" + 0.006*"good" + 0.006*"on-Tees" + 0.006*"well" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -3799,7 +3799,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.007*"on-Trent" + 0.007*"ensure" + 0.006*"well" + 0.006*"However" + 0.006*"plans" + 0.005*"protection" + 0.005*"Stoke" + 0.005*"progress"', '0.014*"’" + 0.007*"However" + 0.007*"Stoke" + 0.006*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.005*"on-Trent" + 0.005*"well" + 0.005*"effectively" + 0.004*"October"', '0.022*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"Stoke" + 0.007*"on-Trent" + 0.007*"plans" + 0.007*"protection" + 0.006*"However" + 0.005*"quality" + 0.005*"3"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.008*"on-Trent" + 0.008*"well" + 0.007*"plans" + 0.007*"However" + 0.007*"Stoke" + 0.006*"ensure" + 0.005*"protection" + 0.005*"quality"', '0.019*"’" + 0.007*"needs" + 0.007*"Stoke" + 0.007*"ensure" + 0.007*"However" + 0.007*"well" + 0.006*"on-Trent" + 0.006*"protection" + 0.006*"plans" + 0.005*"progress"', '0.013*"’" + 0.008*"needs" + 0.006*"Stoke" + 0.006*"on-Trent" + 0.006*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"protection" + 0.005*"However" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -3826,7 +3826,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"progress" + 0.005*"well" + 0.004*"good" + 0.004*"effective" + 0.004*"leaders" + 0.004*"Suffolk" + 0.004*"practice" + 0.003*"ensure" + 0.003*"needs"', '0.012*"’" + 0.005*"well" + 0.005*"progress" + 0.005*"ensure" + 0.004*"good" + 0.004*"practice" + 0.003*"new" + 0.003*"leaders" + 0.003*"needs" + 0.003*"experiences"', '0.014*"’" + 0.008*"well" + 0.007*"progress" + 0.006*"effective" + 0.006*"leaders" + 0.005*"good" + 0.005*"ensure" + 0.005*"practice" + 0.004*"carers" + 0.004*"need"']</t>
+    <t>['0.009*"’" + 0.007*"progress" + 0.007*"well" + 0.005*"effective" + 0.005*"good" + 0.005*"ensure" + 0.005*"leaders" + 0.004*"practice" + 0.004*"needs" + 0.004*"risk"', '0.017*"’" + 0.005*"effective" + 0.005*"leaders" + 0.005*"well" + 0.004*"ensure" + 0.004*"carers" + 0.004*"progress" + 0.004*"good" + 0.003*"high" + 0.003*"use"', '0.014*"’" + 0.007*"well" + 0.007*"progress" + 0.005*"good" + 0.005*"practice" + 0.004*"leaders" + 0.004*"ensure" + 0.004*"effective" + 0.004*"high" + 0.004*"Suffolk"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -3856,7 +3856,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"Sunderland" + 0.006*"needs" + 0.006*"well" + 0.006*"quality" + 0.006*"experienced" + 0.005*"robust" + 0.005*"cared" + 0.005*"family" + 0.004*"practice"', '0.013*"’" + 0.007*"well" + 0.006*"quality" + 0.005*"needs" + 0.005*"protection" + 0.004*"Sunderland" + 0.004*"TfC" + 0.004*"need" + 0.004*"experienced" + 0.004*"practice"', '0.018*"’" + 0.008*"well" + 0.008*"quality" + 0.007*"needs" + 0.005*"parents" + 0.005*"Sunderland" + 0.005*"practice" + 0.005*"good" + 0.005*"experienced" + 0.005*"protection"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"Sunderland" + 0.005*"TfC" + 0.004*"experienced" + 0.004*"risk" + 0.004*"need" + 0.004*"council"', '0.015*"’" + 0.008*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"Sunderland" + 0.005*"highly" + 0.005*"practice" + 0.005*"robust" + 0.004*"experienced" + 0.004*"protection"', '0.019*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"experienced" + 0.005*"well" + 0.005*"Sunderland" + 0.005*"good" + 0.005*"practice" + 0.005*"council" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -3883,7 +3883,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.008*"practice" + 0.007*"well" + 0.007*"progress" + 0.005*"17" + 0.005*"good" + 0.005*"However" + 0.005*"carers" + 0.004*"quality"', '0.012*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"practice" + 0.006*"plans" + 0.005*"carers" + 0.005*"However" + 0.005*"quality" + 0.004*"good" + 0.004*"17"', '0.014*"’" + 0.011*"well" + 0.009*"needs" + 0.008*"progress" + 0.007*"practice" + 0.006*"plans" + 0.006*"effective" + 0.005*"quality" + 0.005*"good" + 0.005*"17"']</t>
+    <t>['0.012*"’" + 0.012*"needs" + 0.010*"well" + 0.007*"practice" + 0.006*"progress" + 0.006*"17" + 0.005*"good" + 0.005*"quality" + 0.005*"plans" + 0.005*"carers"', '0.014*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"progress" + 0.006*"practice" + 0.005*"plans" + 0.005*"carers" + 0.005*"quality" + 0.005*"However" + 0.005*"effective"', '0.015*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"practice" + 0.006*"progress" + 0.006*"effective" + 0.005*"plans" + 0.005*"17" + 0.004*"good" + 0.004*"carers"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -3904,7 +3904,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.014*"needs" + 0.008*"Swindon" + 0.007*"well" + 0.007*"need" + 0.006*"plans" + 0.006*"impact" + 0.006*"always" + 0.006*"Council" + 0.005*"health"', '0.026*"’" + 0.011*"needs" + 0.010*"Swindon" + 0.009*"well" + 0.008*"need" + 0.006*"always" + 0.006*"effective" + 0.006*"plans" + 0.005*"home" + 0.005*"Council"', '0.020*"’" + 0.014*"needs" + 0.009*"need" + 0.009*"Swindon" + 0.007*"always" + 0.007*"well" + 0.007*"plans" + 0.006*"impact" + 0.005*"many" + 0.005*"28"']</t>
+    <t>['0.026*"’" + 0.016*"needs" + 0.011*"Swindon" + 0.010*"well" + 0.009*"need" + 0.008*"plans" + 0.006*"always" + 0.006*"impact" + 0.006*"effective" + 0.005*"education"', '0.020*"’" + 0.010*"needs" + 0.008*"need" + 0.007*"Swindon" + 0.006*"health" + 0.006*"always" + 0.005*"well" + 0.005*"impact" + 0.005*"effective" + 0.005*"many"', '0.015*"’" + 0.008*"needs" + 0.008*"need" + 0.007*"always" + 0.006*"well" + 0.006*"Swindon" + 0.005*"clear" + 0.004*"home" + 0.004*"28" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -3925,7 +3925,7 @@
     <t>0.1619</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"always" + 0.007*"plans" + 0.006*"impact" + 0.006*"good" + 0.006*"practice" + 0.005*"well" + 0.005*"need" + 0.004*"progress" + 0.004*"example"', '0.016*"’" + 0.006*"plans" + 0.005*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"good" + 0.005*"impact" + 0.005*"needs" + 0.004*"new" + 0.004*"need"', '0.015*"’" + 0.008*"plans" + 0.007*"impact" + 0.007*"progress" + 0.006*"always" + 0.006*"well" + 0.005*"good" + 0.005*"practice" + 0.005*"needs" + 0.004*"example"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.006*"impact" + 0.006*"always" + 0.006*"practice" + 0.006*"progress" + 0.005*"good" + 0.005*"well" + 0.005*"example" + 0.005*"needs"', '0.014*"’" + 0.006*"plans" + 0.006*"well" + 0.006*"progress" + 0.006*"impact" + 0.006*"always" + 0.005*"practice" + 0.005*"good" + 0.005*"need" + 0.005*"new"', '0.016*"’" + 0.007*"impact" + 0.007*"plans" + 0.007*"always" + 0.006*"good" + 0.006*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"needs" + 0.004*"However"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -3946,7 +3946,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"well" + 0.008*"effective" + 0.008*"needs" + 0.005*"ensure" + 0.005*"strong" + 0.005*"plans" + 0.005*"practice" + 0.005*"clear" + 0.004*"leaders"', '0.015*"’" + 0.011*"well" + 0.007*"needs" + 0.005*"strong" + 0.005*"plans" + 0.005*"effective" + 0.005*"planning" + 0.005*"ensure" + 0.005*"need" + 0.004*"practice"', '0.020*"’" + 0.013*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"need" + 0.005*"plans" + 0.005*"improve" + 0.005*"practice" + 0.005*"benefit" + 0.005*"strong"']</t>
+    <t>['0.020*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"effective" + 0.005*"ensure" + 0.005*"need" + 0.005*"strong" + 0.005*"plans" + 0.005*"practice" + 0.005*"planning"', '0.012*"’" + 0.010*"well" + 0.007*"effective" + 0.006*"needs" + 0.005*"plans" + 0.005*"strong" + 0.005*"improve" + 0.005*"practice" + 0.004*"leaders" + 0.004*"planning"', '0.015*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"ensure" + 0.005*"strong" + 0.004*"clear" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -3967,7 +3967,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"well" + 0.006*"carers" + 0.005*"need" + 0.005*"ensure" + 0.005*"practice" + 0.004*"needs" + 0.004*"parents" + 0.004*"leaders" + 0.004*"protect"', '0.014*"’" + 0.008*"well" + 0.006*"need" + 0.005*"carers" + 0.005*"needs" + 0.004*"effective" + 0.004*"Thurrock" + 0.004*"leaders" + 0.004*"practice" + 0.004*"vulnerable"', '0.010*"’" + 0.007*"well" + 0.004*"carers" + 0.004*"needs" + 0.003*"ensure" + 0.003*"need" + 0.003*"protection" + 0.003*"practice" + 0.003*"plans" + 0.003*"leaders"']</t>
+    <t>['0.013*"’" + 0.011*"well" + 0.005*"carers" + 0.004*"need" + 0.004*"plans" + 0.004*"ensure" + 0.004*"practice" + 0.004*"needs" + 0.004*"leaders" + 0.004*"Thurrock"', '0.015*"’" + 0.007*"well" + 0.005*"carers" + 0.005*"need" + 0.005*"needs" + 0.004*"effective" + 0.004*"ensure" + 0.004*"Thurrock" + 0.004*"practice" + 0.004*"leaders"', '0.011*"’" + 0.006*"well" + 0.006*"carers" + 0.005*"need" + 0.004*"needs" + 0.004*"protection" + 0.004*"practice" + 0.004*"ensure" + 0.004*"quality" + 0.004*"Thurrock"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -3988,7 +3988,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"well" + 0.004*"21" + 0.004*"needs" + 0.004*"Torbay" + 0.004*"timely" + 0.004*"2022" + 0.004*"good" + 0.004*"effective" + 0.004*"education"', '0.016*"’" + 0.007*"well" + 0.007*"Torbay" + 0.007*"effective" + 0.006*"good" + 0.006*"needs" + 0.005*"plans" + 0.005*"2022" + 0.005*"supported" + 0.004*"1"', '0.019*"’" + 0.012*"well" + 0.009*"Torbay" + 0.007*"needs" + 0.007*"good" + 0.005*"agencies" + 0.005*"progress" + 0.005*"team" + 0.005*"21" + 0.004*"timely"']</t>
+    <t>['0.015*"’" + 0.009*"well" + 0.009*"Torbay" + 0.007*"needs" + 0.006*"good" + 0.005*"effective" + 0.004*"team" + 0.004*"agencies" + 0.004*"supported" + 0.004*"21"', '0.020*"’" + 0.009*"well" + 0.007*"Torbay" + 0.006*"effective" + 0.006*"good" + 0.005*"needs" + 0.005*"team" + 0.005*"progress" + 0.005*"plans" + 0.004*"timely"', '0.013*"’" + 0.008*"well" + 0.005*"good" + 0.005*"needs" + 0.005*"Torbay" + 0.005*"timely" + 0.005*"21" + 0.004*"agencies" + 0.004*"quality" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4009,7 +4009,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"Trafford" + 0.006*"quality" + 0.005*"well" + 0.005*"team" + 0.004*"2" + 0.004*"leaders" + 0.004*"2022"', '0.018*"’" + 0.012*"needs" + 0.009*"Trafford" + 0.007*"quality" + 0.007*"well" + 0.006*"plans" + 0.006*"practice" + 0.006*"leaders" + 0.005*"placed" + 0.005*"impact"', '0.017*"’" + 0.008*"well" + 0.008*"needs" + 0.008*"Trafford" + 0.007*"plans" + 0.006*"leaders" + 0.006*"quality" + 0.005*"practice" + 0.005*"ensure" + 0.005*"impact"']</t>
+    <t>['0.016*"’" + 0.010*"needs" + 0.009*"Trafford" + 0.009*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"leaders" + 0.006*"impact" + 0.005*"placed" + 0.005*"practice"', '0.017*"’" + 0.009*"needs" + 0.007*"Trafford" + 0.007*"quality" + 0.007*"plans" + 0.006*"practice" + 0.006*"leaders" + 0.005*"well" + 0.005*"worker" + 0.005*"impact"', '0.015*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Trafford" + 0.006*"plans" + 0.006*"quality" + 0.005*"leaders" + 0.005*"2" + 0.004*"21" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4027,7 +4027,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50172854</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.005*"leaders" + 0.005*"well" + 0.005*"Walsall" + 0.005*"needs" + 0.004*"early" + 0.004*"4" + 0.003*"October" + 0.003*"need" + 0.003*"education"', '0.028*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"well" + 0.006*"Walsall" + 0.005*"oversight" + 0.005*"4" + 0.005*"information" + 0.005*"Senior" + 0.004*"15"', '0.017*"’" + 0.008*"leaders" + 0.007*"needs" + 0.005*"information" + 0.005*"Walsall" + 0.005*"positive" + 0.005*"well" + 0.005*"good" + 0.004*"Senior" + 0.004*"2021"']</t>
+    <t>['0.018*"’" + 0.007*"leaders" + 0.006*"well" + 0.006*"needs" + 0.005*"oversight" + 0.005*"Senior" + 0.004*"4" + 0.004*"information" + 0.004*"Walsall" + 0.004*"15"', '0.020*"’" + 0.006*"needs" + 0.005*"leaders" + 0.005*"well" + 0.005*"Walsall" + 0.004*"4" + 0.004*"good" + 0.004*"2021" + 0.004*"positive" + 0.004*"information"', '0.024*"’" + 0.009*"leaders" + 0.007*"Walsall" + 0.006*"needs" + 0.005*"well" + 0.005*"information" + 0.005*"4" + 0.005*"progress" + 0.004*"good" + 0.004*"Senior"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4045,7 +4045,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50101635</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"practice" + 0.005*"well" + 0.004*"plans" + 0.004*"number" + 0.004*"progress" + 0.004*"Senior" + 0.004*"small" + 0.004*"carers" + 0.004*"information"', '0.015*"’" + 0.009*"well" + 0.006*"practice" + 0.005*"Senior" + 0.005*"good" + 0.004*"plans" + 0.004*"carers" + 0.004*"number" + 0.004*"information" + 0.004*"senior"', '0.017*"’" + 0.007*"practice" + 0.005*"well" + 0.004*"number" + 0.004*"progress" + 0.004*"need" + 0.004*"plans" + 0.004*"Senior" + 0.004*"needs" + 0.004*"protection"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.007*"practice" + 0.006*"number" + 0.005*"plans" + 0.005*"Senior" + 0.005*"progress" + 0.004*"provided" + 0.004*"information" + 0.004*"need"', '0.011*"’" + 0.007*"practice" + 0.007*"well" + 0.004*"home" + 0.004*"senior" + 0.004*"plans" + 0.004*"good" + 0.004*"progress" + 0.004*"information" + 0.004*"carers"', '0.016*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"Senior" + 0.005*"good" + 0.004*"small" + 0.004*"number" + 0.004*"plans" + 0.003*"need" + 0.003*"needs"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4069,7 +4069,7 @@
     <t>03/12/2021</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.006*"Warwickshire" + 0.005*"plans" + 0.005*"practice" + 0.004*"clear" + 0.004*"needs" + 0.004*"Senior" + 0.004*"progress" + 0.004*"3"', '0.013*"’" + 0.007*"plans" + 0.007*"Warwickshire" + 0.007*"needs" + 0.006*"well" + 0.005*"good" + 0.005*"carers" + 0.005*"practice" + 0.005*"3" + 0.004*"progress"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"plans" + 0.005*"information" + 0.005*"practice" + 0.005*"Warwickshire" + 0.005*"good" + 0.004*"22" + 0.004*"clear"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.005*"Warwickshire" + 0.005*"plans" + 0.005*"carers" + 0.005*"22" + 0.004*"good" + 0.004*"3"', '0.011*"’" + 0.008*"plans" + 0.007*"Warwickshire" + 0.007*"well" + 0.006*"needs" + 0.005*"clear" + 0.004*"Senior" + 0.004*"information" + 0.004*"progress" + 0.004*"3"', '0.008*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.005*"practice" + 0.005*"good" + 0.005*"carers" + 0.005*"supported" + 0.004*"progress" + 0.004*"Warwickshire"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4096,7 +4096,7 @@
     <t>0.1667</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"West" + 0.007*"Berkshire" + 0.006*"well" + 0.005*"working" + 0.004*"plans" + 0.004*"early" + 0.004*"need" + 0.004*"March" + 0.004*"agency"', '0.017*"’" + 0.007*"West" + 0.005*"well" + 0.005*"needs" + 0.005*"Berkshire" + 0.005*"need" + 0.004*"14" + 0.004*"18" + 0.004*"education" + 0.004*"progress"', '0.013*"’" + 0.007*"Berkshire" + 0.006*"well" + 0.005*"West" + 0.004*"plans" + 0.004*"agency" + 0.004*"early" + 0.004*"14" + 0.004*"18" + 0.004*"education"']</t>
+    <t>['0.013*"’" + 0.006*"Berkshire" + 0.005*"West" + 0.005*"well" + 0.005*"need" + 0.004*"18" + 0.004*"plans" + 0.003*"needs" + 0.003*"early" + 0.003*"14"', '0.013*"’" + 0.007*"West" + 0.006*"well" + 0.006*"Berkshire" + 0.005*"14" + 0.004*"needs" + 0.004*"working" + 0.004*"agency" + 0.004*"early" + 0.004*"plans"', '0.017*"’" + 0.007*"Berkshire" + 0.006*"West" + 0.006*"well" + 0.004*"plans" + 0.004*"needs" + 0.004*"practice" + 0.004*"working" + 0.004*"18" + 0.004*"agency"']</t>
   </si>
   <si>
     <t>941</t>
@@ -4114,7 +4114,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"Northamptonshire" + 0.008*"quality" + 0.007*"well" + 0.007*"West" + 0.006*"practice" + 0.005*"needs" + 0.005*"plans" + 0.005*"3" + 0.005*"14"', '0.016*"’" + 0.006*"West" + 0.006*"quality" + 0.006*"Northamptonshire" + 0.006*"well" + 0.006*"practice" + 0.004*"needs" + 0.004*"experiences" + 0.004*"NCT" + 0.004*"However"', '0.012*"’" + 0.007*"Northamptonshire" + 0.006*"West" + 0.005*"NCT" + 0.005*"quality" + 0.005*"impact" + 0.004*"need" + 0.004*"needs" + 0.004*"3" + 0.004*"plans"']</t>
+    <t>['0.018*"’" + 0.007*"well" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"West" + 0.006*"needs" + 0.005*"NCT" + 0.005*"practice" + 0.004*"plans" + 0.004*"October"', '0.015*"’" + 0.007*"West" + 0.007*"Northamptonshire" + 0.006*"well" + 0.006*"quality" + 0.005*"practice" + 0.005*"NCT" + 0.004*"needs" + 0.004*"place" + 0.004*"experiences"', '0.019*"’" + 0.010*"Northamptonshire" + 0.007*"quality" + 0.006*"West" + 0.006*"practice" + 0.005*"impact" + 0.005*"3" + 0.005*"plans" + 0.005*"well" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4135,7 +4135,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"West" + 0.006*"Sussex" + 0.005*"practice" + 0.005*"needs" + 0.005*"number" + 0.005*"supported" + 0.005*"quality"', '0.011*"’" + 0.006*"needs" + 0.006*"plans" + 0.005*"well" + 0.004*"13" + 0.004*"Sussex" + 0.004*"West" + 0.004*"health" + 0.004*"24" + 0.003*"strong"', '0.011*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"number" + 0.005*"13" + 0.005*"plans" + 0.005*"quality" + 0.004*"March" + 0.004*"24" + 0.004*"West"']</t>
+    <t>['0.013*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"13" + 0.005*"West" + 0.005*"Sussex" + 0.004*"number" + 0.004*"health"', '0.017*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"supported" + 0.005*"West" + 0.005*"quality" + 0.005*"number" + 0.004*"actively"', '0.011*"’" + 0.006*"plans" + 0.005*"well" + 0.005*"health" + 0.005*"West" + 0.005*"13" + 0.005*"needs" + 0.005*"Sussex" + 0.004*"March" + 0.004*"clear"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4153,7 +4153,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"plans" + 0.007*"May" + 0.006*"needs" + 0.005*"quality" + 0.005*"Wigan" + 0.004*"practice" + 0.004*"leaders" + 0.004*"9" + 0.003*"good"', '0.013*"’" + 0.008*"practice" + 0.007*"Wigan" + 0.006*"May" + 0.006*"plans" + 0.006*"quality" + 0.006*"appropriate" + 0.005*"timely" + 0.005*"leaders" + 0.005*"needs"', '0.013*"’" + 0.009*"May" + 0.006*"needs" + 0.006*"practice" + 0.006*"plans" + 0.006*"appropriate" + 0.006*"Wigan" + 0.005*"quality" + 0.005*"increased" + 0.004*"leaders"']</t>
+    <t>['0.009*"’" + 0.005*"Wigan" + 0.005*"needs" + 0.005*"quality" + 0.005*"plans" + 0.005*"May" + 0.004*"leaders" + 0.004*"2022" + 0.004*"practice" + 0.004*"well"', '0.012*"’" + 0.008*"May" + 0.008*"practice" + 0.007*"plans" + 0.006*"needs" + 0.006*"Wigan" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"timely" + 0.005*"20"', '0.015*"’" + 0.008*"May" + 0.007*"plans" + 0.007*"practice" + 0.006*"quality" + 0.006*"needs" + 0.006*"appropriate" + 0.006*"Wigan" + 0.005*"leaders" + 0.005*"9"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4180,7 +4180,7 @@
     <t>12/12/23</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"including" + 0.006*"progress" + 0.006*"need" + 0.006*"Wiltshire" + 0.006*"risk" + 0.006*"parents" + 0.005*"plans"', '0.014*"’" + 0.011*"well" + 0.007*"need" + 0.006*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"quality" + 0.005*"Wiltshire" + 0.005*"supported" + 0.005*"parents"', '0.014*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"Wiltshire" + 0.005*"risk" + 0.005*"supported" + 0.005*"parents" + 0.005*"make" + 0.005*"including"']</t>
+    <t>['0.012*"’" + 0.011*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"Wiltshire" + 0.006*"supported" + 0.005*"ensure" + 0.005*"parents" + 0.005*"risk" + 0.005*"progress"', '0.022*"’" + 0.011*"well" + 0.007*"need" + 0.007*"progress" + 0.006*"needs" + 0.006*"including" + 0.006*"risk" + 0.006*"plans" + 0.006*"ensure" + 0.006*"Wiltshire"', '0.012*"well" + 0.011*"’" + 0.008*"needs" + 0.006*"parents" + 0.006*"Wiltshire" + 0.005*"progress" + 0.005*"including" + 0.005*"plans" + 0.005*"supported" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4210,7 +4210,7 @@
     <t>0.1719</t>
   </si>
   <si>
-    <t>['0.007*"quality" + 0.006*"practice" + 0.006*"good" + 0.006*"needs" + 0.005*"well" + 0.004*"progress" + 0.004*"place" + 0.004*"clear" + 0.004*"plans" + 0.004*"need"', '0.010*"’" + 0.009*"well" + 0.008*"quality" + 0.008*"practice" + 0.008*"good" + 0.008*"need" + 0.008*"plans" + 0.007*"needs" + 0.006*"ensure" + 0.006*"effective"', '0.009*"quality" + 0.009*"’" + 0.008*"good" + 0.008*"well" + 0.008*"progress" + 0.007*"needs" + 0.007*"practice" + 0.007*"need" + 0.006*"place" + 0.006*"plans"']</t>
+    <t>['0.009*"practice" + 0.009*"well" + 0.009*"’" + 0.009*"good" + 0.007*"need" + 0.007*"quality" + 0.007*"progress" + 0.006*"place" + 0.006*"ensure" + 0.005*"needs"', '0.008*"needs" + 0.008*"good" + 0.007*"quality" + 0.007*"’" + 0.007*"well" + 0.007*"practice" + 0.007*"need" + 0.006*"effective" + 0.006*"progress" + 0.006*"plans"', '0.012*"quality" + 0.009*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"progress" + 0.006*"practice" + 0.006*"good" + 0.006*"need" + 0.005*"place"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4231,7 +4231,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"effective" + 0.007*"plans" + 0.007*"needs" + 0.005*"provided" + 0.005*"quality" + 0.005*"progress" + 0.005*"experiences" + 0.004*"appropriate" + 0.004*"parents"', '0.012*"’" + 0.007*"progress" + 0.007*"plans" + 0.005*"well" + 0.005*"provided" + 0.005*"needs" + 0.005*"effective" + 0.005*"experiences" + 0.005*"impact" + 0.005*"6"', '0.013*"’" + 0.006*"plans" + 0.006*"well" + 0.006*"17" + 0.006*"needs" + 0.005*"effective" + 0.005*"Wokingham" + 0.004*"6" + 0.004*"good" + 0.004*"quality"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.005*"effective" + 0.004*"provided" + 0.004*"progress" + 0.004*"impact" + 0.004*"quality" + 0.004*"Wokingham"', '0.015*"’" + 0.008*"plans" + 0.007*"effective" + 0.007*"progress" + 0.006*"needs" + 0.005*"17" + 0.005*"quality" + 0.005*"experiences" + 0.005*"appropriate" + 0.005*"provided"', '0.011*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"provided" + 0.005*"6" + 0.005*"progress" + 0.005*"experiences" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4252,7 +4252,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"needs" + 0.005*"effective" + 0.005*"risks" + 0.004*"Wolverhampton" + 0.004*"risk" + 0.004*"quality" + 0.004*"supported" + 0.004*"leaders" + 0.004*"strong"', '0.014*"’" + 0.007*"needs" + 0.006*"risks" + 0.005*"effective" + 0.005*"plans" + 0.005*"Wolverhampton" + 0.005*"supported" + 0.005*"practice" + 0.004*"education" + 0.004*"City"', '0.016*"’" + 0.007*"needs" + 0.006*"Wolverhampton" + 0.006*"effective" + 0.006*"receive" + 0.005*"quality" + 0.005*"leaders" + 0.005*"plans" + 0.005*"risk" + 0.005*"strong"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.006*"Wolverhampton" + 0.005*"effective" + 0.005*"leaders" + 0.005*"strong" + 0.005*"risks" + 0.004*"well" + 0.004*"practice" + 0.004*"supported"', '0.016*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"Wolverhampton" + 0.006*"risks" + 0.005*"plans" + 0.005*"effective" + 0.005*"education" + 0.005*"receive" + 0.004*"leaders"', '0.013*"’" + 0.007*"effective" + 0.007*"needs" + 0.005*"plans" + 0.005*"Wolverhampton" + 0.005*"receive" + 0.004*"education" + 0.004*"risk" + 0.004*"City" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4279,7 +4279,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"well" + 0.008*"progress" + 0.007*"plans" + 0.007*"needs" + 0.006*"Worcestershire" + 0.006*"leaders" + 0.006*"ensure" + 0.005*"appropriate" + 0.005*"living"', '0.017*"’" + 0.007*"plans" + 0.007*"Worcestershire" + 0.007*"needs" + 0.006*"ensure" + 0.006*"leaders" + 0.005*"improve" + 0.005*"appropriate" + 0.005*"experiences" + 0.005*"well"', '0.017*"’" + 0.009*"well" + 0.009*"needs" + 0.009*"plans" + 0.007*"Worcestershire" + 0.007*"leaders" + 0.007*"progress" + 0.006*"appropriate" + 0.005*"ensure" + 0.005*"2023"']</t>
+    <t>['0.016*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"plans" + 0.007*"Worcestershire" + 0.006*"progress" + 0.006*"ensure" + 0.005*"leaders" + 0.005*"PAs" + 0.005*"improve"', '0.018*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"Worcestershire" + 0.006*"appropriate" + 0.006*"ensure" + 0.006*"leaders" + 0.005*"experiences"', '0.022*"’" + 0.008*"leaders" + 0.008*"plans" + 0.008*"well" + 0.007*"Worcestershire" + 0.007*"progress" + 0.006*"appropriate" + 0.006*"needs" + 0.005*"ensure" + 0.005*"improve"']</t>
   </si>
   <si>
     <t>urn</t>
@@ -10448,7 +10448,7 @@
         <v>859</v>
       </c>
       <c r="C84" t="s">
-        <v>33</v>
+        <v>231</v>
       </c>
       <c r="D84" t="s">
         <v>860</v>
@@ -10517,7 +10517,7 @@
         <v>867</v>
       </c>
       <c r="C85" t="s">
-        <v>62</v>
+        <v>231</v>
       </c>
       <c r="D85" t="s">
         <v>868</v>
@@ -12299,7 +12299,7 @@
         <v>1093</v>
       </c>
       <c r="C111" t="s">
-        <v>62</v>
+        <v>231</v>
       </c>
       <c r="D111" t="s">
         <v>1094</v>
@@ -12368,7 +12368,7 @@
         <v>1101</v>
       </c>
       <c r="C112" t="s">
-        <v>48</v>
+        <v>231</v>
       </c>
       <c r="D112" t="s">
         <v>1102</v>

</xml_diff>

<commit_message>
DtoI-1613 fix region codes
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -67,7 +67,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"needs" + 0.007*"within" + 0.006*"Barnsley" + 0.006*"leaders" + 0.006*"response" + 0.005*"practice" + 0.005*"11" + 0.005*"plans" + 0.004*"15"', '0.017*"’" + 0.010*"leaders" + 0.009*"needs" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"within" + 0.005*"understand" + 0.004*"2023" + 0.004*"11" + 0.004*"plans"', '0.019*"’" + 0.007*"needs" + 0.007*"within" + 0.006*"leaders" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"quality" + 0.005*"2023" + 0.004*"plans" + 0.004*"senior"']</t>
+    <t>['0.023*"’" + 0.008*"needs" + 0.007*"within" + 0.007*"leaders" + 0.006*"Barnsley" + 0.006*"practice" + 0.005*"senior" + 0.005*"15" + 0.004*"plans" + 0.004*"response"', '0.014*"’" + 0.007*"needs" + 0.006*"leaders" + 0.005*"within" + 0.005*"Barnsley" + 0.005*"response" + 0.005*"practice" + 0.005*"plans" + 0.004*"2023" + 0.004*"11"', '0.018*"’" + 0.009*"needs" + 0.009*"leaders" + 0.006*"practice" + 0.006*"within" + 0.005*"Barnsley" + 0.005*"progress" + 0.005*"understand" + 0.005*"11" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -106,7 +106,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"well" + 0.007*"practice" + 0.006*"needs" + 0.005*"4" + 0.005*"leaders" + 0.005*"plans" + 0.005*"impact" + 0.005*"clear" + 0.005*"Somerset"', '0.018*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"plans" + 0.005*"East" + 0.005*"protection" + 0.004*"leaders" + 0.004*"‘" + 0.004*"2022"', '0.014*"’" + 0.009*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"effective" + 0.005*"leaders" + 0.005*"receive" + 0.005*"Bath" + 0.004*"North" + 0.004*"education"']</t>
+    <t>['0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"4" + 0.005*"North" + 0.005*"practice" + 0.004*"receive" + 0.004*"clear" + 0.004*"East"', '0.017*"’" + 0.009*"well" + 0.007*"practice" + 0.006*"needs" + 0.006*"leaders" + 0.005*"effective" + 0.005*"East" + 0.005*"impact" + 0.004*"plans" + 0.004*"clear"', '0.018*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"Somerset" + 0.005*"impact" + 0.005*"Bath" + 0.005*"effective" + 0.005*"practice" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -151,7 +151,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"needs" + 0.006*"ensure" + 0.006*"Bedford" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"supported" + 0.005*"Borough" + 0.005*"family"', '0.015*"’" + 0.005*"needs" + 0.005*"well" + 0.005*"ensure" + 0.005*"good" + 0.005*"plans" + 0.004*"Bedford" + 0.004*"supported" + 0.004*"need" + 0.004*"education"', '0.022*"’" + 0.007*"needs" + 0.007*"ensure" + 0.006*"well" + 0.005*"plans" + 0.005*"supported" + 0.005*"good" + 0.005*"made" + 0.005*"relationships" + 0.005*"15"']</t>
+    <t>['0.015*"’" + 0.006*"Bedford" + 0.006*"well" + 0.005*"needs" + 0.005*"Borough" + 0.005*"ensure" + 0.005*"progress" + 0.005*"family" + 0.004*"2021" + 0.004*"relationships"', '0.025*"’" + 0.007*"needs" + 0.007*"ensure" + 0.006*"supported" + 0.005*"good" + 0.005*"progress" + 0.005*"well" + 0.005*"plans" + 0.005*"Bedford" + 0.005*"Borough"', '0.013*"’" + 0.008*"needs" + 0.006*"ensure" + 0.006*"well" + 0.006*"plans" + 0.005*"Bedford" + 0.005*"education" + 0.005*"good" + 0.005*"relationships" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -193,7 +193,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"needs" + 0.008*"effective" + 0.006*"well" + 0.006*"Birmingham" + 0.006*"plans" + 0.005*"trust" + 0.005*"3" + 0.004*"leaders" + 0.004*"20"', '0.015*"’" + 0.009*"needs" + 0.007*"effective" + 0.007*"well" + 0.006*"plans" + 0.006*"appropriate" + 0.005*"3" + 0.005*"progress" + 0.005*"risk" + 0.005*"trust"', '0.017*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Birmingham" + 0.006*"progress" + 0.006*"plans" + 0.006*"trust" + 0.005*"effective" + 0.005*"risk" + 0.005*"appropriate"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"effective" + 0.005*"Birmingham" + 0.005*"plans" + 0.005*"progress" + 0.004*"trust" + 0.004*"leaders" + 0.004*"appropriate"', '0.017*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"progress" + 0.005*"Birmingham" + 0.005*"3" + 0.005*"trust" + 0.005*"plans" + 0.005*"February"', '0.015*"’" + 0.009*"needs" + 0.007*"plans" + 0.006*"trust" + 0.006*"Birmingham" + 0.006*"effective" + 0.005*"timely" + 0.005*"3" + 0.005*"appropriate" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -232,7 +232,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.006*"practice" + 0.005*"quality" + 0.005*"needs" + 0.004*"impact" + 0.004*"well" + 0.004*"Blackburn" + 0.004*"plans" + 0.004*"Darwen" + 0.004*"means"', '0.011*"’" + 0.007*"practice" + 0.007*"well" + 0.007*"Darwen" + 0.007*"needs" + 0.006*"quality" + 0.006*"means" + 0.006*"Blackburn" + 0.005*"result" + 0.005*"impact"', '0.018*"’" + 0.009*"needs" + 0.008*"Blackburn" + 0.008*"quality" + 0.007*"practice" + 0.007*"impact" + 0.007*"Darwen" + 0.006*"well" + 0.006*"planning" + 0.006*"effective"']</t>
+    <t>['0.012*"’" + 0.006*"Darwen" + 0.006*"needs" + 0.006*"impact" + 0.006*"quality" + 0.006*"Blackburn" + 0.006*"well" + 0.005*"practice" + 0.004*"result" + 0.004*"plans"', '0.010*"’" + 0.007*"quality" + 0.007*"Blackburn" + 0.006*"well" + 0.006*"practice" + 0.006*"needs" + 0.006*"planning" + 0.005*"receive" + 0.005*"Darwen" + 0.005*"impact"', '0.017*"’" + 0.009*"practice" + 0.009*"needs" + 0.007*"Darwen" + 0.007*"Blackburn" + 0.007*"quality" + 0.006*"impact" + 0.006*"well" + 0.005*"means" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -271,7 +271,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"Blackpool" + 0.005*"plans" + 0.005*"effective" + 0.005*"quality" + 0.005*"practice" + 0.004*"16" + 0.004*"need"', '0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"Blackpool" + 0.006*"effective" + 0.005*"plans" + 0.005*"16" + 0.005*"progress" + 0.004*"quality" + 0.004*"experiences"', '0.017*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"Blackpool" + 0.006*"supported" + 0.006*"practice" + 0.005*"experiences" + 0.005*"5" + 0.005*"16" + 0.005*"progress"']</t>
+    <t>['0.017*"’" + 0.010*"needs" + 0.009*"well" + 0.006*"Blackpool" + 0.006*"effective" + 0.005*"quality" + 0.005*"16" + 0.005*"practice" + 0.005*"carers" + 0.005*"team"', '0.015*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.006*"supported" + 0.005*"progress" + 0.005*"practice" + 0.005*"effective" + 0.005*"plans" + 0.005*"5"', '0.018*"’" + 0.010*"needs" + 0.009*"well" + 0.008*"Blackpool" + 0.006*"plans" + 0.006*"effective" + 0.005*"16" + 0.005*"practice" + 0.005*"progress" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>350</t>
@@ -295,7 +295,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.008*"Bolton" + 0.007*"plans" + 0.006*"needs" + 0.005*"planning" + 0.004*"need" + 0.004*"11" + 0.004*"risk" + 0.004*"strong"', '0.019*"’" + 0.011*"needs" + 0.008*"Bolton" + 0.007*"well" + 0.006*"plans" + 0.005*"effective" + 0.005*"11" + 0.005*"protection" + 0.005*"strong" + 0.005*"need"', '0.020*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"plans" + 0.008*"Bolton" + 0.007*"supported" + 0.006*"need" + 0.005*"planning" + 0.005*"response" + 0.005*"effective"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Bolton" + 0.006*"planning" + 0.006*"plans" + 0.005*"2023" + 0.005*"need" + 0.005*"supported" + 0.005*"experiences"', '0.016*"’" + 0.011*"Bolton" + 0.010*"needs" + 0.007*"plans" + 0.007*"well" + 0.006*"supported" + 0.005*"strong" + 0.005*"need" + 0.005*"11" + 0.005*"effective"', '0.023*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"plans" + 0.006*"Bolton" + 0.005*"need" + 0.005*"planning" + 0.005*"effective" + 0.005*"supported" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -304,42 +304,42 @@
     <t>839</t>
   </si>
   <si>
+    <t>E06000058</t>
+  </si>
+  <si>
+    <t>bournemouth, christchurch &amp; poole</t>
+  </si>
+  <si>
+    <t>https://files.ofsted.gov.uk/v1/file/50177455</t>
+  </si>
+  <si>
+    <t>inadequate</t>
+  </si>
+  <si>
+    <t>06/12/2021</t>
+  </si>
+  <si>
+    <t>17/12/2021</t>
+  </si>
+  <si>
+    <t>11/02/22</t>
+  </si>
+  <si>
+    <t>0.153</t>
+  </si>
+  <si>
+    <t>['0.015*"’" + 0.005*"quality" + 0.005*"practice" + 0.005*"risk" + 0.005*"6" + 0.005*"impact" + 0.005*"right" + 0.004*"Poole" + 0.004*"2021" + 0.004*"progress"', '0.018*"’" + 0.005*"However" + 0.005*"quality" + 0.005*"Poole" + 0.005*"17" + 0.004*"practice" + 0.004*"progress" + 0.004*"number" + 0.004*"Bournemouth" + 0.004*"health"', '0.019*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"progress" + 0.005*"Christchurch" + 0.005*"Bournemouth" + 0.005*"well" + 0.005*"time" + 0.005*"impact" + 0.005*"risk"']</t>
+  </si>
+  <si>
+    <t>80436</t>
+  </si>
+  <si>
+    <t>867</t>
+  </si>
+  <si>
     <t>SE</t>
   </si>
   <si>
-    <t>E06000058</t>
-  </si>
-  <si>
-    <t>bournemouth, christchurch &amp; poole</t>
-  </si>
-  <si>
-    <t>https://files.ofsted.gov.uk/v1/file/50177455</t>
-  </si>
-  <si>
-    <t>inadequate</t>
-  </si>
-  <si>
-    <t>06/12/2021</t>
-  </si>
-  <si>
-    <t>17/12/2021</t>
-  </si>
-  <si>
-    <t>11/02/22</t>
-  </si>
-  <si>
-    <t>0.153</t>
-  </si>
-  <si>
-    <t>['0.013*"’" + 0.005*"quality" + 0.004*"17" + 0.004*"well" + 0.004*"Poole" + 0.004*"6" + 0.004*"right" + 0.004*"practice" + 0.003*"However" + 0.003*"2021"', '0.014*"’" + 0.006*"quality" + 0.005*"practice" + 0.005*"Christchurch" + 0.005*"Bournemouth" + 0.005*"17" + 0.005*"progress" + 0.005*"many" + 0.005*"6" + 0.004*"Poole"', '0.023*"’" + 0.007*"practice" + 0.006*"progress" + 0.006*"quality" + 0.006*"time" + 0.005*"impact" + 0.005*"risk" + 0.005*"number" + 0.004*"However" + 0.004*"Bournemouth"']</t>
-  </si>
-  <si>
-    <t>80436</t>
-  </si>
-  <si>
-    <t>867</t>
-  </si>
-  <si>
     <t>E06000036</t>
   </si>
   <si>
@@ -370,7 +370,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"risk" + 0.006*"Forest" + 0.006*"Bracknell" + 0.005*"leaders" + 0.005*"quality" + 0.005*"plans" + 0.005*"impact" + 0.005*"provided" + 0.005*"progress"', '0.017*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"Forest" + 0.006*"good" + 0.006*"quality" + 0.006*"provided" + 0.006*"positive" + 0.006*"Bracknell" + 0.005*"progress"', '0.013*"’" + 0.008*"Bracknell" + 0.007*"risk" + 0.006*"needs" + 0.006*"Forest" + 0.006*"good" + 0.006*"quality" + 0.006*"well" + 0.005*"plans" + 0.005*"progress"']</t>
+    <t>['0.015*"’" + 0.007*"Forest" + 0.007*"Bracknell" + 0.007*"need" + 0.007*"needs" + 0.006*"effective" + 0.006*"risk" + 0.006*"quality" + 0.005*"well" + 0.005*"leaders"', '0.012*"’" + 0.007*"good" + 0.006*"progress" + 0.005*"well" + 0.005*"risk" + 0.005*"quality" + 0.005*"Forest" + 0.005*"effective" + 0.005*"Bracknell" + 0.004*"need"', '0.020*"’" + 0.008*"needs" + 0.008*"Bracknell" + 0.007*"Forest" + 0.007*"risk" + 0.007*"quality" + 0.006*"plans" + 0.006*"provided" + 0.006*"good" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>846</t>
@@ -403,7 +403,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"good" + 0.008*"needs" + 0.006*"leaders" + 0.005*"well" + 0.005*"need" + 0.005*"recording" + 0.004*"plans" + 0.004*"ensure" + 0.004*"improve"', '0.015*"’" + 0.010*"needs" + 0.007*"good" + 0.007*"recording" + 0.006*"well" + 0.005*"leaders" + 0.005*"need" + 0.005*"plans" + 0.005*"Hove" + 0.005*"arrangements"', '0.011*"’" + 0.009*"good" + 0.009*"needs" + 0.006*"recording" + 0.005*"plans" + 0.005*"well" + 0.005*"However" + 0.005*"leaders" + 0.004*"effectively" + 0.004*"need"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.007*"good" + 0.006*"recording" + 0.005*"well" + 0.005*"However" + 0.005*"leaders" + 0.005*"timely" + 0.005*"Brighton" + 0.005*"plans"', '0.012*"’" + 0.009*"good" + 0.008*"needs" + 0.006*"recording" + 0.006*"need" + 0.006*"leaders" + 0.005*"well" + 0.005*"Senior" + 0.005*"supported" + 0.004*"plans"', '0.013*"’" + 0.009*"needs" + 0.009*"good" + 0.006*"well" + 0.005*"leaders" + 0.005*"plans" + 0.004*"recording" + 0.004*"Hove" + 0.004*"quality" + 0.004*"strong"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -436,7 +436,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.009*"good" + 0.008*"well" + 0.007*"needs" + 0.007*"Bristol" + 0.005*"need" + 0.005*"plans" + 0.005*"16" + 0.005*"receive" + 0.005*"health"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"Bristol" + 0.006*"health" + 0.005*"progress" + 0.005*"good" + 0.005*"leaders" + 0.004*"January" + 0.004*"plans"', '0.017*"’" + 0.010*"well" + 0.009*"good" + 0.008*"Bristol" + 0.007*"needs" + 0.005*"progress" + 0.005*"health" + 0.004*"need" + 0.004*"2023" + 0.004*"leaders"']</t>
+    <t>['0.018*"’" + 0.009*"well" + 0.008*"Bristol" + 0.007*"good" + 0.006*"needs" + 0.005*"health" + 0.005*"progress" + 0.005*"leaders" + 0.005*"16" + 0.005*"need"', '0.020*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"good" + 0.006*"Bristol" + 0.006*"progress" + 0.005*"health" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders"', '0.020*"’" + 0.008*"needs" + 0.008*"good" + 0.008*"well" + 0.007*"Bristol" + 0.005*"health" + 0.005*"16" + 0.005*"always" + 0.004*"progress" + 0.004*"27"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -463,7 +463,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.005*"plans" + 0.005*"number" + 0.005*"Buckinghamshire" + 0.005*"17" + 0.004*"6" + 0.004*"2021" + 0.004*"many" + 0.004*"December" + 0.004*"well"', '0.012*"’" + 0.005*"plans" + 0.005*"number" + 0.004*"Buckinghamshire" + 0.004*"protection" + 0.004*"6" + 0.004*"practice" + 0.004*"17" + 0.003*"December" + 0.003*"2021"', '0.013*"’" + 0.005*"17" + 0.004*"many" + 0.004*"plans" + 0.004*"number" + 0.004*"needs" + 0.004*"protection" + 0.004*"practice" + 0.004*"Buckinghamshire" + 0.004*"teams"']</t>
+    <t>['0.013*"’" + 0.006*"plans" + 0.005*"6" + 0.004*"number" + 0.004*"protection" + 0.004*"Buckinghamshire" + 0.004*"many" + 0.004*"17" + 0.004*"December" + 0.004*"needs"', '0.014*"’" + 0.005*"number" + 0.004*"17" + 0.004*"many" + 0.004*"well" + 0.004*"2021" + 0.004*"protection" + 0.003*"needs" + 0.003*"impact" + 0.003*"December"', '0.013*"’" + 0.006*"Buckinghamshire" + 0.005*"plans" + 0.005*"17" + 0.005*"number" + 0.004*"2021" + 0.004*"practice" + 0.004*"6" + 0.004*"many" + 0.004*"protection"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -499,7 +499,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"2021" + 0.007*"practice" + 0.006*"team" + 0.006*"protection" + 0.006*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"Bury" + 0.005*"impact"', '0.014*"’" + 0.007*"needs" + 0.007*"protection" + 0.006*"2021" + 0.006*"team" + 0.005*"risk" + 0.005*"need" + 0.005*"practice" + 0.005*"impact" + 0.005*"progress"', '0.009*"’" + 0.007*"needs" + 0.006*"protection" + 0.006*"2021" + 0.005*"impact" + 0.005*"new" + 0.005*"5" + 0.005*"drift" + 0.005*"timely" + 0.004*"team"']</t>
+    <t>['0.012*"’" + 0.008*"2021" + 0.007*"needs" + 0.007*"protection" + 0.007*"team" + 0.006*"practice" + 0.006*"quality" + 0.005*"risk" + 0.005*"need" + 0.005*"impact"', '0.011*"’" + 0.006*"needs" + 0.006*"2021" + 0.005*"protection" + 0.005*"practice" + 0.005*"team" + 0.005*"Bury" + 0.005*"new" + 0.004*"need" + 0.004*"impact"', '0.010*"’" + 0.006*"protection" + 0.006*"needs" + 0.005*"impact" + 0.005*"need" + 0.005*"2021" + 0.004*"risk" + 0.004*"Bury" + 0.004*"practice" + 0.004*"team"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -529,7 +529,7 @@
     <t>0.1954</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.005*"Calderdale" + 0.005*"effective" + 0.004*"protection" + 0.004*"need" + 0.004*"inform" + 0.004*"‘" + 0.004*"good" + 0.003*"practice"', '0.009*"’" + 0.007*"well" + 0.005*"good" + 0.005*"practice" + 0.005*"effective" + 0.004*"protection" + 0.004*"Calderdale" + 0.004*"carers" + 0.004*"education" + 0.004*"leaders"', '0.019*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"good" + 0.006*"Calderdale" + 0.004*"‘" + 0.004*"carers" + 0.004*"protection" + 0.004*"education" + 0.004*"needs"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"good" + 0.004*"Calderdale" + 0.004*"effective" + 0.004*"‘" + 0.004*"protection" + 0.003*"inform" + 0.003*"risk"', '0.017*"’" + 0.008*"well" + 0.005*"Calderdale" + 0.005*"protection" + 0.005*"good" + 0.005*"education" + 0.004*"practice" + 0.004*"need" + 0.004*"‘" + 0.004*"leaders"', '0.015*"’" + 0.008*"well" + 0.006*"practice" + 0.006*"Calderdale" + 0.006*"good" + 0.005*"effective" + 0.005*"carers" + 0.004*"needs" + 0.004*"protection" + 0.004*"‘"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -562,7 +562,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.011*"well" + 0.010*"good" + 0.009*"need" + 0.008*"plans" + 0.007*"needs" + 0.007*"teams" + 0.006*"impact" + 0.006*"However" + 0.006*"quality"', '0.013*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"teams" + 0.008*"good" + 0.008*"impact" + 0.006*"plans" + 0.006*"need" + 0.006*"quality" + 0.005*"effective"', '0.014*"’" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"need" + 0.006*"impact" + 0.005*"progress" + 0.005*"quality" + 0.005*"plans" + 0.005*"However"']</t>
+    <t>['0.016*"’" + 0.009*"well" + 0.009*"good" + 0.009*"impact" + 0.008*"needs" + 0.008*"need" + 0.007*"quality" + 0.006*"plans" + 0.006*"teams" + 0.005*"practice"', '0.013*"’" + 0.010*"well" + 0.008*"good" + 0.007*"teams" + 0.007*"needs" + 0.007*"plans" + 0.006*"need" + 0.006*"However" + 0.006*"effective" + 0.006*"progress"', '0.013*"’" + 0.009*"well" + 0.009*"good" + 0.008*"teams" + 0.007*"need" + 0.007*"needs" + 0.007*"plans" + 0.006*"impact" + 0.006*"However" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -592,7 +592,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"need" + 0.007*"good" + 0.006*"carers" + 0.006*"Central" + 0.006*"plans" + 0.006*"progress" + 0.005*"Bedfordshire"', '0.017*"’" + 0.011*"well" + 0.007*"needs" + 0.007*"carers" + 0.006*"need" + 0.006*"good" + 0.006*"progress" + 0.005*"number" + 0.005*"effective" + 0.005*"protection"', '0.012*"’" + 0.008*"well" + 0.007*"plans" + 0.005*"needs" + 0.005*"Bedfordshire" + 0.005*"need" + 0.004*"progress" + 0.004*"carers" + 0.004*"education" + 0.004*"supported"']</t>
+    <t>['0.014*"’" + 0.007*"well" + 0.007*"carers" + 0.006*"needs" + 0.005*"progress" + 0.005*"good" + 0.005*"need" + 0.004*"plans" + 0.004*"supported" + 0.004*"Bedfordshire"', '0.016*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"need" + 0.007*"plans" + 0.007*"good" + 0.006*"progress" + 0.006*"effective" + 0.006*"Central" + 0.005*"Bedfordshire"', '0.018*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"carers" + 0.005*"need" + 0.005*"good" + 0.005*"plans" + 0.004*"progress" + 0.004*"17" + 0.004*"Bedfordshire"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -628,7 +628,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"practice" + 0.006*"always" + 0.005*"accommodation" + 0.005*"ensure" + 0.005*"carers" + 0.005*"However"', '0.012*"’" + 0.008*"needs" + 0.008*"plans" + 0.008*"good" + 0.008*"well" + 0.007*"practice" + 0.006*"risk" + 0.006*"supported" + 0.006*"need" + 0.006*"However"', '0.011*"’" + 0.008*"well" + 0.007*"good" + 0.006*"plans" + 0.005*"needs" + 0.005*"supported" + 0.005*"need" + 0.005*"effective" + 0.005*"practice" + 0.004*"timely"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.007*"good" + 0.006*"always" + 0.006*"needs" + 0.006*"need" + 0.005*"practice" + 0.005*"plans" + 0.005*"However" + 0.005*"ensure"', '0.013*"’" + 0.008*"well" + 0.007*"good" + 0.007*"needs" + 0.007*"plans" + 0.007*"practice" + 0.006*"supported" + 0.006*"always" + 0.006*"carers" + 0.006*"need"', '0.014*"’" + 0.008*"needs" + 0.007*"good" + 0.007*"well" + 0.006*"plans" + 0.006*"practice" + 0.005*"quality" + 0.005*"effective" + 0.005*"ensure" + 0.005*"However"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -664,7 +664,7 @@
     <t>0.1816</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"order" + 0.005*"always" + 0.004*"timely" + 0.004*"effective" + 0.004*"learning" + 0.004*"impact"', '0.021*"’" + 0.007*"needs" + 0.007*"well" + 0.004*"impact" + 0.004*"effective" + 0.004*"effectively" + 0.004*"progress" + 0.004*"plans" + 0.004*"early" + 0.004*"including"', '0.019*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"receive" + 0.004*"plans" + 0.004*"always" + 0.004*"effectively" + 0.004*"small" + 0.004*"learning"']</t>
+    <t>['0.019*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"practice" + 0.005*"plans" + 0.004*"learning" + 0.004*"need" + 0.004*"early" + 0.004*"receive" + 0.004*"including"', '0.024*"’" + 0.007*"needs" + 0.007*"well" + 0.005*"effectively" + 0.005*"timely" + 0.005*"impact" + 0.004*"always" + 0.004*"order" + 0.004*"effective" + 0.004*"progress"', '0.021*"’" + 0.007*"well" + 0.005*"needs" + 0.004*"effective" + 0.004*"practice" + 0.004*"always" + 0.004*"order" + 0.004*"risk" + 0.004*"receive" + 0.004*"use"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -700,7 +700,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"plans" + 0.005*"Bradford" + 0.005*"need" + 0.005*"needs" + 0.005*"practice" + 0.004*"quality" + 0.004*"risk" + 0.004*"Borough" + 0.004*"City"', '0.018*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"impact" + 0.005*"risk" + 0.004*"need" + 0.004*"lack" + 0.004*"◼" + 0.004*"Bradford" + 0.004*"November"', '0.024*"’" + 0.006*"plans" + 0.006*"2" + 0.005*"2022" + 0.005*"Bradford" + 0.005*"quality" + 0.004*"21" + 0.004*"needs" + 0.004*"Council" + 0.004*"many"']</t>
+    <t>['0.017*"’" + 0.007*"plans" + 0.006*"Council" + 0.005*"risk" + 0.005*"needs" + 0.005*"2022" + 0.005*"City" + 0.005*"impact" + 0.004*"◼" + 0.004*"quality"', '0.015*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"2" + 0.004*"◼" + 0.004*"Bradford" + 0.004*"senior" + 0.004*"Borough" + 0.004*"quality" + 0.003*"risk"', '0.026*"’" + 0.006*"plans" + 0.006*"Bradford" + 0.005*"need" + 0.005*"2" + 0.005*"21" + 0.005*"practice" + 0.005*"impact" + 0.005*"quality" + 0.004*"However"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -733,7 +733,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.013*"well" + 0.012*"’" + 0.010*"ensure" + 0.010*"needs" + 0.008*"effective" + 0.007*"progress" + 0.007*"clear" + 0.006*"good" + 0.005*"experiences" + 0.005*"plans"', '0.011*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"ensure" + 0.006*"effective" + 0.005*"good" + 0.004*"plans" + 0.004*"clear" + 0.004*"individual" + 0.004*"progress"', '0.014*"needs" + 0.012*"’" + 0.008*"well" + 0.008*"ensure" + 0.007*"clear" + 0.006*"plans" + 0.006*"effective" + 0.006*"progress" + 0.005*"good" + 0.005*"within"']</t>
+    <t>['0.015*"needs" + 0.013*"’" + 0.012*"well" + 0.010*"ensure" + 0.007*"plans" + 0.006*"effective" + 0.006*"progress" + 0.006*"clear" + 0.006*"within" + 0.005*"good"', '0.012*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"ensure" + 0.007*"effective" + 0.007*"clear" + 0.007*"progress" + 0.006*"good" + 0.006*"supported" + 0.005*"individual"', '0.009*"’" + 0.007*"needs" + 0.007*"ensure" + 0.007*"well" + 0.006*"effective" + 0.005*"clear" + 0.005*"good" + 0.005*"within" + 0.005*"clearly" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -769,7 +769,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"November" + 0.008*"leaders" + 0.007*"well" + 0.006*"Wakefield" + 0.006*"effective" + 0.006*"plans" + 0.005*"practice" + 0.005*"progress" + 0.005*"quality"', '0.020*"’" + 0.008*"quality" + 0.008*"well" + 0.008*"effective" + 0.008*"Wakefield" + 0.007*"good" + 0.007*"leaders" + 0.006*"practice" + 0.006*"plans" + 0.006*"needs"', '0.012*"’" + 0.009*"Wakefield" + 0.008*"quality" + 0.007*"good" + 0.007*"leaders" + 0.007*"well" + 0.007*"November" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective"']</t>
+    <t>['0.014*"’" + 0.008*"quality" + 0.006*"effective" + 0.006*"good" + 0.006*"Wakefield" + 0.006*"leaders" + 0.005*"practice" + 0.005*"plans" + 0.005*"19" + 0.005*"well"', '0.018*"’" + 0.010*"well" + 0.009*"November" + 0.009*"Wakefield" + 0.009*"leaders" + 0.006*"effective" + 0.006*"receive" + 0.006*"quality" + 0.006*"needs" + 0.006*"plans"', '0.017*"’" + 0.008*"good" + 0.008*"quality" + 0.007*"Wakefield" + 0.007*"November" + 0.007*"effective" + 0.007*"plans" + 0.006*"well" + 0.006*"leaders" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -799,7 +799,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"quality" + 0.007*"needs" + 0.006*"March" + 0.006*"effective" + 0.006*"practice" + 0.006*"ensure" + 0.006*"York" + 0.006*"plans" + 0.005*"However"', '0.020*"’" + 0.007*"needs" + 0.007*"March" + 0.006*"effective" + 0.005*"quality" + 0.005*"ensure" + 0.005*"7" + 0.005*"However" + 0.005*"training" + 0.004*"well"', '0.010*"’" + 0.008*"March" + 0.008*"needs" + 0.005*"effective" + 0.005*"York" + 0.005*"However" + 0.005*"need" + 0.005*"well" + 0.005*"good" + 0.005*"quality"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.008*"March" + 0.007*"effective" + 0.006*"However" + 0.006*"quality" + 0.006*"supported" + 0.005*"York" + 0.005*"well" + 0.005*"plans"', '0.012*"’" + 0.008*"quality" + 0.005*"March" + 0.005*"ensure" + 0.005*"needs" + 0.005*"plans" + 0.005*"effective" + 0.004*"York" + 0.004*"However" + 0.004*"need"', '0.016*"’" + 0.008*"needs" + 0.007*"March" + 0.006*"quality" + 0.006*"effective" + 0.006*"well" + 0.006*"York" + 0.005*"ensure" + 0.005*"7" + 0.005*"However"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -835,7 +835,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.016*"well" + 0.014*"’" + 0.011*"quality" + 0.010*"effective" + 0.010*"leaders" + 0.006*"plans" + 0.006*"good" + 0.006*"arrangements" + 0.005*"ensure" + 0.005*"timely"', '0.013*"well" + 0.011*"’" + 0.009*"quality" + 0.007*"effective" + 0.006*"leaders" + 0.006*"timely" + 0.006*"good" + 0.005*"plans" + 0.005*"high" + 0.004*"highly"', '0.014*"well" + 0.010*"’" + 0.008*"leaders" + 0.008*"effective" + 0.008*"quality" + 0.007*"arrangements" + 0.006*"timely" + 0.006*"plans" + 0.005*"highly" + 0.005*"good"']</t>
+    <t>['0.013*"well" + 0.011*"’" + 0.010*"effective" + 0.010*"quality" + 0.008*"leaders" + 0.005*"highly" + 0.005*"good" + 0.005*"arrangements" + 0.004*"plans" + 0.004*"timely"', '0.015*"well" + 0.012*"’" + 0.010*"quality" + 0.008*"leaders" + 0.007*"effective" + 0.005*"timely" + 0.005*"arrangements" + 0.005*"highly" + 0.005*"plans" + 0.005*"good"', '0.016*"well" + 0.013*"’" + 0.009*"leaders" + 0.009*"effective" + 0.008*"quality" + 0.007*"plans" + 0.007*"good" + 0.006*"timely" + 0.006*"arrangements" + 0.005*"Senior"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -865,7 +865,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"Scilly" + 0.008*"Isles" + 0.008*"information" + 0.007*"need" + 0.007*"protection" + 0.006*"practice" + 0.006*"place" + 0.005*"strategic" + 0.005*"needs"', '0.026*"’" + 0.015*"Isles" + 0.013*"Scilly" + 0.011*"practice" + 0.010*"information" + 0.008*"need" + 0.007*"needs" + 0.007*"quality" + 0.007*"protection" + 0.006*"risks"', '0.017*"’" + 0.012*"Scilly" + 0.009*"Isles" + 0.008*"need" + 0.007*"needs" + 0.007*"information" + 0.006*"place" + 0.006*"practice" + 0.006*"protection" + 0.005*"quality"']</t>
+    <t>['0.021*"’" + 0.012*"Scilly" + 0.011*"Isles" + 0.009*"practice" + 0.008*"information" + 0.008*"need" + 0.006*"quality" + 0.006*"place" + 0.006*"needs" + 0.005*"protection"', '0.021*"’" + 0.014*"Scilly" + 0.010*"Isles" + 0.009*"information" + 0.008*"protection" + 0.008*"needs" + 0.008*"practice" + 0.008*"need" + 0.007*"risks" + 0.006*"place"', '0.020*"’" + 0.015*"Isles" + 0.010*"Scilly" + 0.009*"information" + 0.008*"practice" + 0.008*"need" + 0.006*"protection" + 0.006*"needs" + 0.006*"quality" + 0.006*"13"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -901,7 +901,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"Coventry" + 0.007*"supported" + 0.006*"strong" + 0.006*"plans" + 0.005*"need" + 0.005*"family" + 0.004*"PAs"', '0.018*"’" + 0.009*"Coventry" + 0.008*"well" + 0.007*"needs" + 0.007*"supported" + 0.006*"family" + 0.006*"plans" + 0.006*"need" + 0.005*"use" + 0.005*"1"', '0.017*"’" + 0.006*"Coventry" + 0.006*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"strong" + 0.006*"supported" + 0.005*"family" + 0.004*"July" + 0.004*"health"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.008*"plans" + 0.007*"Coventry" + 0.006*"needs" + 0.005*"strong" + 0.005*"family" + 0.004*"supported" + 0.004*"need" + 0.004*"PAs"', '0.017*"’" + 0.009*"well" + 0.009*"Coventry" + 0.007*"needs" + 0.007*"supported" + 0.006*"plans" + 0.005*"family" + 0.005*"need" + 0.005*"strong" + 0.005*"understand"', '0.022*"’" + 0.008*"Coventry" + 0.008*"needs" + 0.008*"supported" + 0.007*"family" + 0.006*"well" + 0.006*"strong" + 0.005*"need" + 0.005*"1" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -940,7 +940,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"October" + 0.007*"Darlington" + 0.006*"leaders" + 0.005*"practice" + 0.005*"family" + 0.005*"quality" + 0.005*"effective"', '0.012*"’" + 0.006*"Darlington" + 0.006*"leaders" + 0.006*"effective" + 0.005*"practice" + 0.005*"needs" + 0.005*"well" + 0.005*"October" + 0.005*"quality" + 0.005*"10"', '0.022*"’" + 0.009*"well" + 0.008*"leaders" + 0.008*"practice" + 0.007*"October" + 0.007*"needs" + 0.005*"supported" + 0.005*"Darlington" + 0.005*"education" + 0.005*"quality"']</t>
+    <t>['0.022*"’" + 0.007*"well" + 0.007*"October" + 0.007*"leaders" + 0.007*"Darlington" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"effective" + 0.005*"education"', '0.016*"’" + 0.008*"practice" + 0.007*"well" + 0.007*"needs" + 0.006*"October" + 0.006*"leaders" + 0.005*"Darlington" + 0.005*"10" + 0.005*"plans" + 0.004*"family"', '0.018*"’" + 0.009*"well" + 0.006*"leaders" + 0.006*"needs" + 0.005*"October" + 0.005*"supported" + 0.005*"effective" + 0.005*"practice" + 0.005*"quality" + 0.005*"Darlington"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -979,7 +979,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"needs" + 0.007*"Derby" + 0.006*"receive" + 0.006*"quality" + 0.006*"appropriate" + 0.005*"leaders" + 0.005*"progress" + 0.005*"need" + 0.005*"plans"', '0.022*"’" + 0.011*"needs" + 0.006*"Derby" + 0.006*"plans" + 0.005*"leaders" + 0.005*"receive" + 0.005*"quality" + 0.005*"progress" + 0.005*"good" + 0.004*"well"', '0.022*"’" + 0.009*"needs" + 0.008*"Derby" + 0.007*"quality" + 0.006*"well" + 0.006*"receive" + 0.006*"progress" + 0.006*"need" + 0.006*"plans" + 0.006*"good"']</t>
+    <t>['0.016*"’" + 0.010*"needs" + 0.007*"Derby" + 0.006*"receive" + 0.006*"leaders" + 0.005*"well" + 0.005*"progress" + 0.005*"need" + 0.005*"appropriate" + 0.005*"21"', '0.026*"’" + 0.009*"needs" + 0.008*"quality" + 0.007*"Derby" + 0.006*"plans" + 0.006*"receive" + 0.006*"appropriate" + 0.005*"progress" + 0.005*"good" + 0.005*"need"', '0.020*"’" + 0.009*"needs" + 0.007*"Derby" + 0.006*"plans" + 0.006*"quality" + 0.006*"progress" + 0.005*"leaders" + 0.005*"receive" + 0.005*"good" + 0.005*"need"']</t>
   </si>
   <si>
     <t>830</t>
@@ -1006,7 +1006,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"well" + 0.005*"Derbyshire" + 0.005*"10" + 0.004*"education" + 0.004*"effective" + 0.004*"positive" + 0.004*"plans" + 0.004*"health" + 0.004*"number"', '0.015*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.005*"positive" + 0.005*"health" + 0.005*"need" + 0.005*"good" + 0.005*"effective" + 0.005*"leaders" + 0.004*"practice"', '0.015*"’" + 0.009*"well" + 0.008*"Derbyshire" + 0.006*"plans" + 0.006*"needs" + 0.005*"10" + 0.004*"good" + 0.004*"November" + 0.004*"leaders" + 0.004*"number"']</t>
+    <t>['0.012*"’" + 0.007*"well" + 0.007*"positive" + 0.006*"Derbyshire" + 0.005*"needs" + 0.005*"10" + 0.005*"need" + 0.005*"health" + 0.005*"number" + 0.005*"education"', '0.014*"’" + 0.007*"Derbyshire" + 0.007*"well" + 0.006*"plans" + 0.005*"leaders" + 0.005*"effective" + 0.005*"health" + 0.004*"2023" + 0.004*"progress" + 0.004*"risk"', '0.016*"’" + 0.010*"well" + 0.006*"Derbyshire" + 0.005*"effective" + 0.005*"need" + 0.004*"needs" + 0.004*"30" + 0.004*"education" + 0.004*"plans" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1036,7 +1036,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.006*"leaders" + 0.006*"well" + 0.005*"risk" + 0.005*"health" + 0.004*"risks" + 0.004*"early" + 0.004*"time" + 0.004*"progress" + 0.004*"practice"', '0.011*"’" + 0.007*"well" + 0.005*"progress" + 0.005*"health" + 0.005*"Devon" + 0.005*"risk" + 0.004*"leaders" + 0.004*"living" + 0.004*"case" + 0.004*"areas"', '0.008*"’" + 0.004*"protection" + 0.004*"well" + 0.004*"leaders" + 0.004*"health" + 0.004*"risk" + 0.003*"areas" + 0.003*"case" + 0.003*"need" + 0.003*"risks"']</t>
+    <t>['0.008*"’" + 0.007*"well" + 0.005*"progress" + 0.005*"leaders" + 0.004*"risk" + 0.004*"case" + 0.004*"risks" + 0.004*"protection" + 0.004*"needs" + 0.004*"living"', '0.012*"’" + 0.006*"health" + 0.006*"well" + 0.006*"leaders" + 0.005*"risk" + 0.004*"Devon" + 0.004*"plans" + 0.004*"living" + 0.004*"quality" + 0.004*"time"', '0.007*"’" + 0.005*"well" + 0.004*"risk" + 0.004*"progress" + 0.004*"protection" + 0.004*"health" + 0.004*"Devon" + 0.004*"time" + 0.003*"practice" + 0.003*"early"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1069,7 +1069,7 @@
     <t>0.1512</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"well" + 0.007*"Doncaster" + 0.006*"records" + 0.006*"plans" + 0.005*"leaders" + 0.005*"quality" + 0.005*"protection" + 0.004*"information" + 0.004*"14"', '0.019*"’" + 0.006*"progress" + 0.006*"well" + 0.005*"Doncaster" + 0.005*"many" + 0.005*"oversight" + 0.004*"information" + 0.004*"quality" + 0.004*"February" + 0.004*"arrangements"', '0.019*"’" + 0.005*"well" + 0.005*"Doncaster" + 0.005*"progress" + 0.005*"many" + 0.005*"leaders" + 0.005*"oversight" + 0.004*"arrangements" + 0.004*"25" + 0.004*"quality"']</t>
+    <t>['0.021*"’" + 0.007*"Doncaster" + 0.006*"well" + 0.006*"records" + 0.006*"arrangements" + 0.005*"quality" + 0.005*"protection" + 0.005*"progress" + 0.005*"oversight" + 0.005*"leaders"', '0.015*"’" + 0.006*"well" + 0.006*"many" + 0.005*"leaders" + 0.005*"Doncaster" + 0.004*"progress" + 0.004*"information" + 0.004*"2022" + 0.004*"oversight" + 0.004*"plans"', '0.023*"’" + 0.007*"well" + 0.005*"many" + 0.005*"progress" + 0.004*"information" + 0.004*"plans" + 0.004*"effective" + 0.004*"Doncaster" + 0.004*"quality" + 0.004*"council"']</t>
   </si>
   <si>
     <t>838</t>
@@ -1096,7 +1096,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"Dorset" + 0.006*"good" + 0.005*"arrangements" + 0.005*"well" + 0.004*"8" + 0.004*"needs" + 0.004*"27" + 0.004*"leaders" + 0.004*"home"', '0.014*"’" + 0.008*"Dorset" + 0.006*"good" + 0.006*"well" + 0.005*"change" + 0.005*"October" + 0.005*"needs" + 0.004*"including" + 0.004*"arrangements" + 0.004*"impact"', '0.014*"’" + 0.008*"Dorset" + 0.006*"well" + 0.006*"good" + 0.004*"needs" + 0.004*"quality" + 0.004*"2021" + 0.004*"8" + 0.004*"impact" + 0.004*"arrangements"']</t>
+    <t>['0.010*"’" + 0.008*"Dorset" + 0.006*"well" + 0.005*"good" + 0.005*"needs" + 0.004*"8" + 0.004*"need" + 0.004*"protection" + 0.004*"27" + 0.004*"2021"', '0.018*"’" + 0.007*"Dorset" + 0.007*"good" + 0.006*"well" + 0.005*"arrangements" + 0.005*"needs" + 0.005*"including" + 0.004*"quality" + 0.004*"impact" + 0.004*"October"', '0.012*"’" + 0.007*"Dorset" + 0.005*"good" + 0.005*"well" + 0.004*"arrangements" + 0.004*"October" + 0.004*"8" + 0.004*"change" + 0.004*"quality" + 0.003*"leaders"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1123,7 +1123,7 @@
     <t>13/01/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.014*"needs" + 0.010*"Dudley" + 0.006*"well" + 0.006*"plans" + 0.006*"always" + 0.005*"quality" + 0.005*"arrangements" + 0.005*"ensure" + 0.005*"management"', '0.017*"’" + 0.009*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.006*"arrangements" + 0.006*"always" + 0.005*"plans" + 0.005*"oversight" + 0.005*"However" + 0.005*"October"', '0.011*"’" + 0.009*"needs" + 0.006*"Dudley" + 0.004*"enough" + 0.004*"well" + 0.004*"ensure" + 0.004*"arrangements" + 0.004*"11" + 0.003*"However" + 0.003*"plans"']</t>
+    <t>['0.013*"needs" + 0.012*"’" + 0.006*"Dudley" + 0.006*"ensure" + 0.005*"plans" + 0.005*"always" + 0.004*"arrangements" + 0.004*"oversight" + 0.004*"31" + 0.004*"October"', '0.016*"’" + 0.010*"needs" + 0.009*"Dudley" + 0.006*"well" + 0.005*"arrangements" + 0.005*"always" + 0.005*"quality" + 0.005*"oversight" + 0.005*"plans" + 0.005*"However"', '0.017*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.005*"plans" + 0.005*"always" + 0.005*"arrangements" + 0.004*"quality" + 0.004*"receive" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1159,7 +1159,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"needs" + 0.007*"Durham" + 0.006*"well" + 0.006*"plans" + 0.006*"May" + 0.006*"ensure" + 0.004*"20" + 0.004*"number" + 0.004*"meetings"', '0.014*"’" + 0.010*"needs" + 0.008*"May" + 0.008*"Durham" + 0.007*"plans" + 0.006*"practice" + 0.006*"well" + 0.006*"risks" + 0.005*"ensure" + 0.005*"family"', '0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"May" + 0.006*"ensure" + 0.006*"Durham" + 0.006*"plans" + 0.005*"practice" + 0.004*"leaders" + 0.004*"appropriate"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"Durham" + 0.005*"ensure" + 0.005*"progress" + 0.005*"May" + 0.004*"family" + 0.004*"effective"', '0.016*"’" + 0.011*"needs" + 0.009*"May" + 0.007*"Durham" + 0.007*"well" + 0.006*"ensure" + 0.006*"plans" + 0.005*"practice" + 0.005*"risks" + 0.004*"making"', '0.012*"’" + 0.011*"needs" + 0.007*"Durham" + 0.007*"plans" + 0.006*"May" + 0.006*"well" + 0.006*"ensure" + 0.006*"practice" + 0.005*"protection" + 0.005*"10"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1195,7 +1195,7 @@
     <t>0.1646</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"progress" + 0.006*"East" + 0.005*"plans" + 0.004*"10" + 0.004*"education" + 0.004*"experiences" + 0.004*"partners"', '0.019*"’" + 0.011*"needs" + 0.009*"plans" + 0.007*"well" + 0.007*"progress" + 0.006*"East" + 0.006*"Riding" + 0.005*"information" + 0.005*"10" + 0.005*"partners"', '0.016*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"Riding" + 0.008*"needs" + 0.007*"progress" + 0.006*"East" + 0.005*"practice" + 0.005*"30" + 0.005*"training"']</t>
+    <t>['0.020*"’" + 0.010*"needs" + 0.009*"plans" + 0.009*"well" + 0.007*"progress" + 0.007*"Riding" + 0.006*"East" + 0.005*"partners" + 0.005*"education" + 0.005*"10"', '0.015*"’" + 0.007*"East" + 0.007*"plans" + 0.007*"needs" + 0.007*"progress" + 0.007*"Riding" + 0.006*"well" + 0.005*"practice" + 0.005*"good" + 0.005*"place"', '0.012*"’" + 0.011*"needs" + 0.009*"plans" + 0.009*"well" + 0.006*"progress" + 0.005*"10" + 0.005*"East" + 0.005*"2023" + 0.005*"partners" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1222,7 +1222,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"Sussex" + 0.005*"need" + 0.005*"plans" + 0.004*"senior" + 0.004*"East" + 0.004*"‘"', '0.008*"well" + 0.008*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"need" + 0.004*"East" + 0.004*"carers" + 0.004*"plans" + 0.004*"senior" + 0.004*"receive"', '0.011*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"needs" + 0.004*"‘" + 0.004*"need" + 0.004*"Sussex" + 0.004*"effective" + 0.003*"senior" + 0.003*"East"']</t>
+    <t>['0.010*"’" + 0.008*"practice" + 0.007*"well" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"need" + 0.004*"East" + 0.004*"receive" + 0.004*"‘" + 0.003*"supported"', '0.011*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"practice" + 0.005*"need" + 0.005*"Sussex" + 0.004*"senior" + 0.004*"plans" + 0.004*"specialist" + 0.004*"‘"', '0.013*"’" + 0.010*"well" + 0.006*"needs" + 0.005*"need" + 0.004*"practice" + 0.004*"plans" + 0.004*"senior" + 0.004*"‘" + 0.004*"East" + 0.004*"specialist"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1258,7 +1258,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"progress" + 0.005*"understand" + 0.005*"experiences" + 0.005*"parents" + 0.005*"plans" + 0.004*"quality" + 0.004*"Essex"', '0.022*"’" + 0.007*"progress" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"family" + 0.005*"Essex" + 0.005*"risk" + 0.005*"leaders" + 0.005*"understand"', '0.017*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"‘" + 0.005*"progress" + 0.005*"family" + 0.005*"experiences" + 0.005*"supported" + 0.004*"helped"']</t>
+    <t>['0.017*"’" + 0.007*"well" + 0.006*"progress" + 0.006*"plans" + 0.005*"family" + 0.005*"needs" + 0.005*"parents" + 0.005*"leaders" + 0.005*"access" + 0.004*"‘"', '0.019*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"progress" + 0.005*"helped" + 0.005*"understand" + 0.005*"risk" + 0.005*"Essex" + 0.005*"family" + 0.005*"experiences"', '0.017*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"progress" + 0.006*"needs" + 0.005*"experiences" + 0.005*"family" + 0.005*"Essex" + 0.005*"need" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1294,7 +1294,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"effective" + 0.007*"quality" + 0.007*"good" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"timely" + 0.005*"need"', '0.016*"’" + 0.007*"effective" + 0.007*"practice" + 0.007*"good" + 0.007*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"timely" + 0.005*"early" + 0.005*"improve"', '0.012*"effective" + 0.010*"’" + 0.007*"good" + 0.007*"practice" + 0.006*"timely" + 0.005*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"plans" + 0.004*"protection"']</t>
+    <t>['0.007*"effective" + 0.006*"’" + 0.006*"needs" + 0.006*"good" + 0.006*"practice" + 0.005*"quality" + 0.005*"well" + 0.004*"focus" + 0.004*"improve" + 0.004*"early"', '0.011*"’" + 0.007*"practice" + 0.007*"good" + 0.006*"quality" + 0.006*"effective" + 0.006*"needs" + 0.005*"need" + 0.005*"well" + 0.005*"plans" + 0.005*"timely"', '0.019*"’" + 0.010*"effective" + 0.007*"good" + 0.006*"timely" + 0.006*"quality" + 0.006*"practice" + 0.006*"well" + 0.006*"needs" + 0.005*"early" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>916</t>
@@ -1324,7 +1324,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"needs" + 0.008*"2022" + 0.008*"plans" + 0.007*"February" + 0.007*"well" + 0.006*"progress" + 0.006*"Gloucestershire" + 0.005*"timely" + 0.005*"good"', '0.013*"’" + 0.007*"needs" + 0.005*"February" + 0.004*"well" + 0.004*"appropriate" + 0.004*"2022" + 0.004*"plans" + 0.004*"protection" + 0.004*"need" + 0.004*"progress"', '0.016*"’" + 0.008*"needs" + 0.007*"2022" + 0.007*"February" + 0.006*"plans" + 0.005*"experienced" + 0.005*"appropriate" + 0.005*"18" + 0.005*"Gloucestershire" + 0.005*"protection"']</t>
+    <t>['0.011*"’" + 0.009*"needs" + 0.007*"February" + 0.005*"plans" + 0.005*"2022" + 0.005*"good" + 0.005*"progress" + 0.004*"experienced" + 0.004*"well" + 0.004*"effective"', '0.011*"’" + 0.007*"2022" + 0.005*"February" + 0.005*"plans" + 0.005*"well" + 0.004*"family" + 0.004*"needs" + 0.004*"Gloucestershire" + 0.004*"leaders" + 0.004*"experienced"', '0.023*"’" + 0.010*"needs" + 0.008*"plans" + 0.008*"2022" + 0.007*"February" + 0.006*"well" + 0.006*"progress" + 0.006*"Gloucestershire" + 0.005*"protection" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1351,7 +1351,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"plans" + 0.007*"practice" + 0.006*"planning" + 0.006*"effective" + 0.006*"always" + 0.006*"risk" + 0.006*"need"', '0.010*"well" + 0.010*"practice" + 0.009*"’" + 0.009*"needs" + 0.008*"risk" + 0.007*"plans" + 0.006*"need" + 0.006*"good" + 0.006*"always" + 0.006*"planning"', '0.014*"’" + 0.010*"well" + 0.008*"practice" + 0.007*"need" + 0.007*"needs" + 0.007*"plans" + 0.007*"good" + 0.006*"planning" + 0.006*"effective" + 0.006*"oversight"']</t>
+    <t>['0.011*"’" + 0.009*"practice" + 0.009*"well" + 0.007*"plans" + 0.006*"needs" + 0.006*"effective" + 0.006*"response" + 0.006*"planning" + 0.006*"risk" + 0.006*"means"', '0.011*"well" + 0.009*"’" + 0.008*"always" + 0.007*"needs" + 0.007*"good" + 0.006*"effective" + 0.006*"need" + 0.006*"plans" + 0.006*"planning" + 0.006*"quality"', '0.014*"’" + 0.010*"well" + 0.010*"needs" + 0.009*"practice" + 0.009*"plans" + 0.008*"risk" + 0.007*"need" + 0.006*"good" + 0.006*"planning" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1378,7 +1378,7 @@
     <t>0.187</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.008*"needs" + 0.007*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"highly" + 0.004*"leaders" + 0.004*"strong" + 0.004*"improve" + 0.004*"need"', '0.016*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"home" + 0.005*"Hampshire" + 0.004*"quality" + 0.004*"strong" + 0.004*"leaders" + 0.003*"‘"', '0.017*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"quality" + 0.004*"leaders" + 0.004*"strong" + 0.004*"home" + 0.004*"carers" + 0.004*"improve"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.005*"quality" + 0.005*"plans" + 0.004*"well" + 0.004*"leaders" + 0.004*"strong" + 0.004*"home" + 0.003*"progress" + 0.003*"health"', '0.019*"’" + 0.010*"needs" + 0.006*"well" + 0.006*"plans" + 0.004*"Hampshire" + 0.004*"home" + 0.004*"improve" + 0.004*"quality" + 0.004*"strong" + 0.004*"highly"', '0.022*"’" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"leaders" + 0.004*"strong" + 0.004*"quality" + 0.004*"need" + 0.004*"highly" + 0.004*"home"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1411,7 +1411,7 @@
     <t>0.2081</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"strong" + 0.004*"early" + 0.004*"education" + 0.004*"good" + 0.004*"need" + 0.004*"impact" + 0.004*"practice"', '0.015*"’" + 0.010*"well" + 0.007*"quality" + 0.006*"good" + 0.005*"plans" + 0.005*"education" + 0.004*"practice" + 0.004*"strong" + 0.004*"experiences" + 0.004*"impact"', '0.015*"’" + 0.008*"well" + 0.006*"progress" + 0.006*"strong" + 0.005*"quality" + 0.005*"good" + 0.005*"early" + 0.004*"plans" + 0.004*"impact" + 0.004*"improve"']</t>
+    <t>['0.018*"’" + 0.009*"well" + 0.005*"quality" + 0.005*"good" + 0.004*"education" + 0.004*"strong" + 0.004*"practice" + 0.004*"early" + 0.004*"team" + 0.004*"effective"', '0.015*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"strong" + 0.004*"needs" + 0.004*"plans" + 0.004*"‘" + 0.004*"good" + 0.004*"health" + 0.004*"practice"', '0.015*"’" + 0.009*"well" + 0.007*"quality" + 0.006*"strong" + 0.005*"progress" + 0.005*"good" + 0.005*"early" + 0.005*"impact" + 0.005*"plans" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>884</t>
@@ -1438,7 +1438,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.006*"practice" + 0.006*"lack" + 0.006*"needs" + 0.006*"Herefordshire" + 0.006*"impact" + 0.004*"carers" + 0.004*"July" + 0.004*"risk" + 0.004*"18"', '0.015*"’" + 0.005*"many" + 0.005*"quality" + 0.005*"lack" + 0.005*"practice" + 0.004*"Herefordshire" + 0.004*"impact" + 0.004*"need" + 0.004*"plans" + 0.004*"progress"', '0.009*"’" + 0.005*"Herefordshire" + 0.005*"many" + 0.005*"practice" + 0.005*"needs" + 0.004*"plans" + 0.004*"including" + 0.004*"identified" + 0.004*"18" + 0.004*"progress"']</t>
+    <t>['0.019*"’" + 0.007*"practice" + 0.005*"impact" + 0.005*"Herefordshire" + 0.004*"plans" + 0.004*"many" + 0.004*"lack" + 0.004*"quality" + 0.004*"18" + 0.004*"2022"', '0.019*"’" + 0.006*"Herefordshire" + 0.005*"lack" + 0.005*"needs" + 0.005*"practice" + 0.005*"many" + 0.004*"across" + 0.004*"impact" + 0.004*"need" + 0.004*"progress"', '0.012*"’" + 0.005*"lack" + 0.005*"needs" + 0.005*"Herefordshire" + 0.004*"impact" + 0.004*"carers" + 0.004*"practice" + 0.004*"many" + 0.004*"quality" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>919</t>
@@ -1465,7 +1465,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.005*"Hertfordshire" + 0.005*"well" + 0.005*"needs" + 0.003*"leaders" + 0.003*"receive" + 0.003*"working" + 0.003*"‘" + 0.003*"supported" + 0.003*"Leaders"', '0.024*"’" + 0.008*"Hertfordshire" + 0.007*"needs" + 0.007*"well" + 0.006*"receive" + 0.006*"plans" + 0.005*"positive" + 0.005*"need" + 0.005*"2023" + 0.004*"risk"', '0.026*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"27" + 0.005*"Hertfordshire" + 0.005*"receive" + 0.004*"family" + 0.004*"23" + 0.004*"leaders" + 0.004*"effective"']</t>
+    <t>['0.027*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Hertfordshire" + 0.006*"receive" + 0.005*"plans" + 0.005*"risk" + 0.005*"effective" + 0.004*"need" + 0.004*"23"', '0.019*"’" + 0.006*"Hertfordshire" + 0.006*"needs" + 0.005*"well" + 0.004*"receive" + 0.004*"leaders" + 0.004*"training" + 0.004*"working" + 0.004*"27" + 0.004*"‘"', '0.021*"’" + 0.006*"Hertfordshire" + 0.005*"well" + 0.005*"plans" + 0.005*"needs" + 0.004*"receive" + 0.004*"leaders" + 0.004*"positive" + 0.004*"Leaders" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1492,7 +1492,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"leaders" + 0.005*"Senior" + 0.005*"Isle" + 0.005*"plans" + 0.005*"well" + 0.005*"Wight" + 0.005*"needs" + 0.005*"good" + 0.005*"improve"', '0.014*"’" + 0.008*"leaders" + 0.005*"needs" + 0.005*"practice" + 0.005*"supported" + 0.004*"Wight" + 0.004*"2023" + 0.004*"progress" + 0.004*"protection" + 0.004*"good"', '0.020*"’" + 0.008*"leaders" + 0.007*"well" + 0.006*"needs" + 0.006*"3" + 0.006*"PAs" + 0.006*"Isle" + 0.006*"progress" + 0.005*"Senior" + 0.005*"information"']</t>
+    <t>['0.020*"’" + 0.010*"leaders" + 0.007*"well" + 0.006*"supported" + 0.005*"needs" + 0.005*"Isle" + 0.005*"Senior" + 0.005*"progress" + 0.005*"good" + 0.005*"practice"', '0.019*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"plans" + 0.006*"3" + 0.006*"well" + 0.005*"Wight" + 0.005*"Isle" + 0.005*"progress" + 0.005*"information"', '0.012*"’" + 0.006*"leaders" + 0.004*"supported" + 0.004*"needs" + 0.004*"Wight" + 0.004*"progress" + 0.004*"3" + 0.004*"Senior" + 0.004*"improve" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1513,7 +1513,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"Kent" + 0.006*"supported" + 0.005*"well" + 0.005*"progress" + 0.005*"needs" + 0.005*"Council" + 0.004*"practice" + 0.004*"9" + 0.003*"plans"', '0.012*"’" + 0.009*"Kent" + 0.007*"needs" + 0.006*"Council" + 0.006*"County" + 0.006*"well" + 0.005*"supported" + 0.005*"practice" + 0.004*"ensure" + 0.004*"progress"', '0.021*"’" + 0.012*"Kent" + 0.009*"needs" + 0.007*"well" + 0.007*"Council" + 0.006*"County" + 0.005*"supported" + 0.005*"progress" + 0.005*"leaders" + 0.004*"impact"']</t>
+    <t>['0.018*"’" + 0.013*"Kent" + 0.007*"needs" + 0.006*"Council" + 0.006*"well" + 0.006*"supported" + 0.005*"practice" + 0.005*"County" + 0.004*"progress" + 0.004*"appropriate"', '0.019*"’" + 0.010*"Kent" + 0.006*"needs" + 0.006*"Council" + 0.005*"well" + 0.005*"supported" + 0.005*"leaders" + 0.005*"County" + 0.004*"progress" + 0.004*"impact"', '0.017*"’" + 0.008*"needs" + 0.007*"Kent" + 0.007*"well" + 0.006*"supported" + 0.005*"County" + 0.005*"Council" + 0.005*"progress" + 0.004*"including" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1540,7 +1540,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"planning" + 0.008*"number" + 0.007*"need" + 0.007*"Hull" + 0.007*"protection" + 0.006*"well" + 0.006*"risks" + 0.006*"practice" + 0.005*"small"', '0.012*"’" + 0.006*"planning" + 0.006*"practice" + 0.006*"management" + 0.005*"small" + 0.005*"number" + 0.005*"protection" + 0.005*"November" + 0.005*"well" + 0.004*"Hull"', '0.017*"’" + 0.007*"number" + 0.006*"practice" + 0.006*"well" + 0.005*"planning" + 0.005*"protection" + 0.005*"oversight" + 0.005*"risks" + 0.005*"management" + 0.005*"progress"']</t>
+    <t>['0.014*"’" + 0.006*"management" + 0.006*"planning" + 0.006*"number" + 0.006*"small" + 0.006*"well" + 0.005*"practice" + 0.005*"teams" + 0.005*"right" + 0.005*"need"', '0.018*"’" + 0.007*"protection" + 0.006*"number" + 0.006*"planning" + 0.006*"risks" + 0.006*"practice" + 0.006*"Hull" + 0.006*"agency" + 0.005*"well" + 0.005*"management"', '0.015*"’" + 0.008*"number" + 0.007*"planning" + 0.007*"need" + 0.006*"well" + 0.006*"protection" + 0.006*"practice" + 0.006*"Hull" + 0.005*"risks" + 0.005*"25"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1570,7 +1570,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"good" + 0.006*"practice" + 0.006*"quality" + 0.006*"plans" + 0.005*"permanence" + 0.005*"Senior" + 0.005*"training" + 0.005*"well" + 0.004*"needs"', '0.012*"’" + 0.006*"quality" + 0.006*"good" + 0.006*"practice" + 0.005*"permanence" + 0.005*"plans" + 0.005*"protection" + 0.005*"needs" + 0.005*"senior" + 0.004*"need"', '0.012*"’" + 0.007*"quality" + 0.007*"well" + 0.006*"practice" + 0.005*"protection" + 0.005*"training" + 0.005*"Senior" + 0.005*"needs" + 0.004*"good" + 0.004*"plans"']</t>
+    <t>['0.010*"’" + 0.006*"good" + 0.006*"quality" + 0.006*"Senior" + 0.006*"protection" + 0.006*"plans" + 0.005*"needs" + 0.005*"permanence" + 0.005*"practice" + 0.005*"training"', '0.009*"’" + 0.006*"quality" + 0.006*"practice" + 0.005*"plans" + 0.005*"permanence" + 0.005*"well" + 0.005*"good" + 0.005*"training" + 0.004*"last" + 0.004*"senior"', '0.015*"’" + 0.007*"practice" + 0.007*"quality" + 0.006*"good" + 0.006*"well" + 0.005*"needs" + 0.005*"need" + 0.005*"senior" + 0.005*"permanence" + 0.005*"Senior"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1609,7 +1609,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"progress" + 0.007*"quality" + 0.005*"plans" + 0.005*"needs" + 0.004*"abuse" + 0.004*"Knowsley" + 0.004*"place" + 0.004*"October" + 0.004*"good"', '0.019*"’" + 0.010*"progress" + 0.008*"needs" + 0.008*"plans" + 0.007*"Knowsley" + 0.007*"quality" + 0.007*"2021" + 0.006*"good" + 0.006*"22" + 0.006*"experiences"', '0.012*"’" + 0.008*"plans" + 0.008*"needs" + 0.007*"quality" + 0.006*"progress" + 0.006*"Knowsley" + 0.005*"need" + 0.005*"2021" + 0.005*"education" + 0.005*"11"']</t>
+    <t>['0.010*"’" + 0.007*"progress" + 0.005*"Knowsley" + 0.005*"quality" + 0.005*"needs" + 0.005*"11" + 0.004*"2021" + 0.004*"experiences" + 0.004*"October" + 0.004*"plans"', '0.013*"’" + 0.008*"progress" + 0.007*"plans" + 0.007*"quality" + 0.007*"2021" + 0.007*"needs" + 0.005*"need" + 0.005*"experiences" + 0.005*"Knowsley" + 0.005*"October"', '0.018*"’" + 0.009*"progress" + 0.008*"plans" + 0.008*"needs" + 0.007*"quality" + 0.007*"Knowsley" + 0.005*"good" + 0.005*"abuse" + 0.005*"22" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1639,7 +1639,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"need" + 0.005*"supported" + 0.005*"plans" + 0.005*"Lancashire" + 0.005*"oversight" + 0.005*"live" + 0.004*"practice"', '0.017*"’" + 0.008*"well" + 0.008*"need" + 0.007*"Lancashire" + 0.006*"needs" + 0.006*"9" + 0.005*"supported" + 0.005*"practice" + 0.005*"plans" + 0.005*"28"', '0.012*"’" + 0.010*"well" + 0.008*"needs" + 0.007*"need" + 0.006*"Lancashire" + 0.005*"positive" + 0.005*"parents" + 0.005*"plans" + 0.005*"homes" + 0.005*"health"']</t>
+    <t>['0.015*"’" + 0.009*"well" + 0.007*"need" + 0.007*"needs" + 0.005*"supported" + 0.005*"Lancashire" + 0.005*"positive" + 0.005*"health" + 0.004*"plans" + 0.004*"homes"', '0.018*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"need" + 0.007*"Lancashire" + 0.006*"supported" + 0.006*"practice" + 0.006*"positive" + 0.005*"parents" + 0.005*"health"', '0.015*"’" + 0.007*"need" + 0.007*"well" + 0.006*"plans" + 0.006*"Lancashire" + 0.006*"needs" + 0.005*"9" + 0.005*"live" + 0.005*"homes" + 0.005*"number"']</t>
   </si>
   <si>
     <t>383</t>
@@ -1663,7 +1663,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"21" + 0.004*"practice" + 0.004*"plans" + 0.004*"including" + 0.004*"March" + 0.004*"2022"', '0.017*"’" + 0.009*"needs" + 0.008*"Leeds" + 0.007*"well" + 0.005*"ensure" + 0.005*"risk" + 0.005*"4" + 0.005*"protection" + 0.005*"practice" + 0.005*"making"', '0.016*"’" + 0.006*"risk" + 0.006*"Leeds" + 0.005*"well" + 0.004*"practice" + 0.004*"plans" + 0.004*"protection" + 0.004*"benefit" + 0.004*"supported" + 0.004*"2022"']</t>
+    <t>['0.013*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"risk" + 0.005*"protection" + 0.005*"4" + 0.004*"2022" + 0.004*"practice" + 0.004*"21"', '0.017*"’" + 0.007*"Leeds" + 0.007*"needs" + 0.006*"ensure" + 0.005*"risk" + 0.005*"practice" + 0.005*"well" + 0.004*"plans" + 0.004*"21" + 0.004*"benefit"', '0.017*"’" + 0.008*"Leeds" + 0.008*"needs" + 0.007*"well" + 0.005*"risk" + 0.004*"plans" + 0.004*"including" + 0.004*"practice" + 0.004*"2022" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1696,7 +1696,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.011*"well" + 0.009*"Leicester" + 0.009*"2021" + 0.008*"needs" + 0.008*"good" + 0.007*"ensure" + 0.006*"number" + 0.005*"1" + 0.005*"October"', '0.017*"’" + 0.009*"2021" + 0.007*"well" + 0.007*"needs" + 0.007*"Leicester" + 0.006*"including" + 0.005*"20" + 0.005*"1" + 0.005*"number" + 0.005*"good"', '0.018*"’" + 0.007*"well" + 0.007*"2021" + 0.007*"Leicester" + 0.005*"20" + 0.005*"including" + 0.004*"1" + 0.004*"high" + 0.004*"number" + 0.004*"good"']</t>
+    <t>['0.019*"’" + 0.009*"Leicester" + 0.009*"well" + 0.006*"2021" + 0.006*"needs" + 0.005*"1" + 0.005*"number" + 0.005*"Council" + 0.005*"ensure" + 0.005*"October"', '0.019*"’" + 0.011*"2021" + 0.008*"well" + 0.007*"good" + 0.006*"Leicester" + 0.006*"needs" + 0.006*"ensure" + 0.006*"number" + 0.005*"1" + 0.005*"including"', '0.022*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Leicester" + 0.007*"2021" + 0.007*"good" + 0.006*"ensure" + 0.006*"20" + 0.005*"number" + 0.005*"circumstances"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1729,7 +1729,7 @@
     <t>0.1666</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"good" + 0.007*"well" + 0.006*"practice" + 0.006*"quality" + 0.006*"impact" + 0.006*"need" + 0.006*"needs" + 0.005*"effective" + 0.005*"risk"', '0.013*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"effective" + 0.006*"quality" + 0.006*"good" + 0.004*"risk" + 0.004*"education" + 0.004*"practice" + 0.004*"impact"', '0.010*"’" + 0.009*"good" + 0.009*"well" + 0.007*"effective" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.004*"education" + 0.004*"need" + 0.004*"progress"']</t>
+    <t>['0.010*"’" + 0.007*"needs" + 0.006*"effective" + 0.006*"well" + 0.006*"good" + 0.005*"practice" + 0.005*"education" + 0.005*"risk" + 0.004*"impact" + 0.004*"quality"', '0.010*"’" + 0.007*"well" + 0.006*"good" + 0.005*"quality" + 0.005*"needs" + 0.004*"leaders" + 0.004*"need" + 0.004*"effective" + 0.003*"progress" + 0.003*"practice"', '0.013*"’" + 0.009*"good" + 0.009*"well" + 0.008*"effective" + 0.007*"needs" + 0.007*"quality" + 0.007*"practice" + 0.006*"impact" + 0.005*"need" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1759,7 +1759,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.009*"Lincolnshire" + 0.008*"needs" + 0.006*"well" + 0.005*"family" + 0.005*"need" + 0.005*"plans" + 0.005*"progress" + 0.004*"24" + 0.004*"April"', '0.017*"’" + 0.005*"well" + 0.005*"Lincolnshire" + 0.005*"plans" + 0.004*"needs" + 0.004*"24" + 0.004*"2023" + 0.003*"28" + 0.003*"effective" + 0.003*"family"', '0.020*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"well" + 0.004*"28" + 0.004*"family" + 0.004*"24" + 0.003*"effective"']</t>
+    <t>['0.022*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.007*"well" + 0.005*"plans" + 0.004*"need" + 0.004*"2023" + 0.004*"progress" + 0.004*"family" + 0.004*"education"', '0.023*"’" + 0.008*"Lincolnshire" + 0.006*"needs" + 0.006*"well" + 0.005*"progress" + 0.005*"plans" + 0.005*"24" + 0.004*"family" + 0.004*"28" + 0.004*"number"', '0.018*"’" + 0.006*"needs" + 0.005*"Lincolnshire" + 0.004*"family" + 0.004*"progress" + 0.004*"well" + 0.004*"offer" + 0.004*"need" + 0.004*"effective" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1789,7 +1789,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"practice" + 0.007*"needs" + 0.006*"always" + 0.006*"quality" + 0.006*"Liverpool" + 0.005*"24" + 0.005*"need" + 0.005*"timely" + 0.005*"protection"', '0.019*"’" + 0.008*"needs" + 0.007*"need" + 0.007*"always" + 0.006*"Liverpool" + 0.006*"practice" + 0.005*"met" + 0.005*"quality" + 0.005*"protection" + 0.005*"PAs"', '0.019*"’" + 0.007*"practice" + 0.007*"need" + 0.006*"needs" + 0.006*"always" + 0.006*"Liverpool" + 0.005*"quality" + 0.005*"protection" + 0.005*"planning" + 0.005*"well"']</t>
+    <t>['0.022*"’" + 0.008*"practice" + 0.008*"needs" + 0.007*"need" + 0.007*"Liverpool" + 0.006*"always" + 0.005*"quality" + 0.005*"protection" + 0.005*"harm" + 0.005*"13"', '0.020*"’" + 0.006*"need" + 0.006*"needs" + 0.006*"always" + 0.005*"practice" + 0.005*"quality" + 0.005*"PAs" + 0.004*"timely" + 0.004*"13" + 0.004*"met"', '0.013*"’" + 0.006*"needs" + 0.006*"always" + 0.006*"Liverpool" + 0.006*"quality" + 0.005*"practice" + 0.005*"protection" + 0.005*"need" + 0.004*"24" + 0.004*"response"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1822,7 +1822,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.009*"needs" + 0.007*"good" + 0.006*"carers" + 0.006*"plans" + 0.005*"practice" + 0.005*"well" + 0.005*"information" + 0.005*"Borough" + 0.005*"progress"', '0.020*"’" + 0.007*"needs" + 0.006*"plans" + 0.005*"good" + 0.005*"well" + 0.004*"information" + 0.004*"carers" + 0.004*"Barking" + 0.004*"progress" + 0.004*"10"', '0.019*"’" + 0.007*"needs" + 0.005*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"ensure" + 0.004*"2023" + 0.004*"progress" + 0.004*"21" + 0.004*"carers"']</t>
+    <t>['0.023*"’" + 0.007*"needs" + 0.005*"plans" + 0.005*"well" + 0.005*"information" + 0.004*"good" + 0.004*"London" + 0.004*"practice" + 0.004*"planning" + 0.004*"carers"', '0.025*"’" + 0.010*"needs" + 0.007*"good" + 0.006*"carers" + 0.006*"progress" + 0.006*"plans" + 0.006*"practice" + 0.005*"well" + 0.005*"information" + 0.005*"timely"', '0.014*"’" + 0.006*"needs" + 0.005*"plans" + 0.004*"well" + 0.004*"planning" + 0.004*"ensure" + 0.004*"carers" + 0.004*"10" + 0.004*"practice" + 0.004*"Dagenham"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -1858,7 +1858,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.012*"needs" + 0.010*"good" + 0.008*"well" + 0.008*"need" + 0.006*"ensure" + 0.006*"plans" + 0.006*"progress" + 0.005*"clear" + 0.005*"risk"', '0.012*"’" + 0.010*"well" + 0.010*"good" + 0.008*"needs" + 0.007*"progress" + 0.006*"plans" + 0.006*"need" + 0.006*"quality" + 0.006*"ensure" + 0.006*"clear"', '0.010*"’" + 0.009*"need" + 0.008*"needs" + 0.007*"good" + 0.006*"well" + 0.005*"progress" + 0.005*"clear" + 0.005*"plans" + 0.005*"effective" + 0.005*"risk"']</t>
+    <t>['0.015*"’" + 0.010*"good" + 0.009*"needs" + 0.009*"well" + 0.007*"need" + 0.006*"effective" + 0.006*"progress" + 0.006*"ensure" + 0.006*"plans" + 0.005*"clear"', '0.013*"’" + 0.009*"needs" + 0.007*"good" + 0.007*"clear" + 0.006*"well" + 0.006*"need" + 0.005*"risk" + 0.005*"ensure" + 0.005*"progress" + 0.005*"plans"', '0.014*"’" + 0.010*"needs" + 0.010*"good" + 0.010*"well" + 0.009*"need" + 0.007*"progress" + 0.007*"plans" + 0.006*"quality" + 0.005*"clear" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>303</t>
@@ -1876,7 +1876,7 @@
     <t>06/02/2023</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"need" + 0.005*"Bexley" + 0.005*"plans" + 0.004*"clear" + 0.004*"10" + 0.004*"practice"', '0.026*"’" + 0.007*"well" + 0.006*"need" + 0.006*"needs" + 0.006*"effective" + 0.005*"Bexley" + 0.005*"plans" + 0.005*"6" + 0.004*"make" + 0.004*"oversight"', '0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"effective" + 0.005*"10" + 0.005*"need" + 0.004*"including" + 0.004*"Bexley" + 0.004*"6"']</t>
+    <t>['0.024*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"need" + 0.006*"plans" + 0.005*"effective" + 0.005*"Bexley" + 0.005*"10" + 0.004*"make" + 0.004*"practice"', '0.019*"’" + 0.006*"effective" + 0.005*"needs" + 0.005*"Bexley" + 0.005*"well" + 0.005*"6" + 0.005*"February" + 0.005*"plans" + 0.004*"need" + 0.004*"including"', '0.014*"’" + 0.006*"well" + 0.005*"need" + 0.005*"Bexley" + 0.005*"needs" + 0.005*"plans" + 0.004*"clear" + 0.004*"including" + 0.004*"10" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -1903,7 +1903,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.007*"progress" + 0.006*"leaders" + 0.006*"number" + 0.006*"plans" + 0.005*"quality" + 0.005*"good" + 0.005*"practice" + 0.005*"timely"', '0.015*"’" + 0.010*"leaders" + 0.007*"plans" + 0.007*"good" + 0.006*"well" + 0.006*"quality" + 0.006*"number" + 0.006*"progress" + 0.005*"senior" + 0.005*"practice"', '0.019*"’" + 0.010*"well" + 0.007*"plans" + 0.006*"Brent" + 0.006*"progress" + 0.005*"leaders" + 0.005*"senior" + 0.005*"information" + 0.005*"good" + 0.005*"family"']</t>
+    <t>['0.014*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"progress" + 0.006*"practice" + 0.006*"good" + 0.005*"quality" + 0.005*"However" + 0.005*"plans" + 0.005*"number"', '0.023*"’" + 0.010*"well" + 0.008*"plans" + 0.008*"leaders" + 0.007*"good" + 0.007*"senior" + 0.006*"Brent" + 0.006*"progress" + 0.006*"quality" + 0.006*"number"', '0.012*"’" + 0.007*"leaders" + 0.007*"well" + 0.006*"progress" + 0.005*"needs" + 0.005*"number" + 0.005*"Brent" + 0.005*"plans" + 0.005*"20" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -1936,7 +1936,7 @@
     <t>0.1941</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Bromley" + 0.008*"needs" + 0.007*"well" + 0.005*"plans" + 0.005*"practice" + 0.004*"education" + 0.004*"health" + 0.004*"progress" + 0.004*"leaders"', '0.017*"’" + 0.009*"Bromley" + 0.007*"well" + 0.006*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.004*"access" + 0.004*"13" + 0.004*"practice" + 0.004*"17"', '0.025*"’" + 0.009*"Bromley" + 0.006*"plans" + 0.006*"well" + 0.006*"practice" + 0.006*"needs" + 0.005*"leaders" + 0.005*"health" + 0.005*"education" + 0.004*"17"']</t>
+    <t>['0.022*"’" + 0.011*"Bromley" + 0.009*"well" + 0.006*"plans" + 0.006*"needs" + 0.006*"practice" + 0.005*"leaders" + 0.005*"health" + 0.004*"17" + 0.004*"quality"', '0.018*"’" + 0.008*"Bromley" + 0.007*"needs" + 0.006*"plans" + 0.005*"health" + 0.005*"education" + 0.005*"leaders" + 0.005*"YPAs" + 0.004*"practice" + 0.004*"well"', '0.019*"’" + 0.008*"Bromley" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.004*"practice" + 0.004*"progress" + 0.004*"education" + 0.004*"November" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -1966,7 +1966,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Camden" + 0.007*"practice" + 0.006*"leaders" + 0.006*"needs" + 0.005*"well" + 0.005*"appropriate" + 0.005*"response" + 0.005*"25" + 0.004*"protection"', '0.010*"’" + 0.007*"Camden" + 0.007*"leaders" + 0.005*"response" + 0.005*"practice" + 0.005*"protection" + 0.005*"well" + 0.004*"progress" + 0.004*"2022" + 0.004*"needs"', '0.006*"’" + 0.006*"practice" + 0.005*"well" + 0.005*"leaders" + 0.005*"protection" + 0.005*"Camden" + 0.004*"meetings" + 0.004*"needs" + 0.004*"29" + 0.004*"appropriate"']</t>
+    <t>['0.010*"’" + 0.007*"Camden" + 0.006*"well" + 0.005*"practice" + 0.005*"25" + 0.005*"needs" + 0.005*"leaders" + 0.005*"29" + 0.004*"April" + 0.004*"response"', '0.010*"’" + 0.006*"leaders" + 0.006*"Camden" + 0.006*"practice" + 0.005*"protection" + 0.005*"response" + 0.004*"progress" + 0.004*"well" + 0.004*"needs" + 0.004*"2022"', '0.012*"’" + 0.007*"Camden" + 0.007*"leaders" + 0.006*"practice" + 0.006*"protection" + 0.005*"well" + 0.005*"needs" + 0.005*"appropriate" + 0.004*"response" + 0.004*"29"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -1993,7 +1993,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.006*"needs" + 0.006*"Senior" + 0.005*"well" + 0.005*"ensure" + 0.004*"Croydon" + 0.004*"quality" + 0.004*"need" + 0.004*"education" + 0.004*"effective"', '0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"need" + 0.006*"Croydon" + 0.006*"health" + 0.006*"plans" + 0.005*"effective" + 0.005*"risk" + 0.005*"quality"', '0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"ensure" + 0.006*"quality" + 0.006*"Senior" + 0.006*"Croydon" + 0.005*"education" + 0.005*"improved"']</t>
+    <t>['0.011*"’" + 0.010*"well" + 0.006*"needs" + 0.005*"Senior" + 0.005*"Croydon" + 0.005*"effective" + 0.005*"quality" + 0.005*"need" + 0.005*"ensure" + 0.004*"plans"', '0.010*"’" + 0.006*"good" + 0.006*"needs" + 0.005*"health" + 0.005*"Senior" + 0.005*"Croydon" + 0.005*"quality" + 0.005*"well" + 0.004*"need" + 0.004*"arrangements"', '0.013*"’" + 0.009*"needs" + 0.006*"ensure" + 0.006*"well" + 0.006*"need" + 0.006*"Croydon" + 0.006*"quality" + 0.005*"health" + 0.005*"However" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2026,7 +2026,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.006*"’" + 0.005*"quality" + 0.005*"needs" + 0.005*"good" + 0.004*"risk" + 0.004*"oversight" + 0.004*"progress" + 0.003*"family" + 0.003*"experiences" + 0.003*"provide"', '0.013*"’" + 0.012*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.005*"risk" + 0.005*"progress" + 0.005*"experiences" + 0.005*"well" + 0.004*"need"', '0.010*"’" + 0.009*"quality" + 0.007*"needs" + 0.005*"good" + 0.005*"management" + 0.005*"progress" + 0.005*"Ealing" + 0.005*"plans" + 0.004*"oversight" + 0.004*"family"']</t>
+    <t>['0.009*"’" + 0.007*"quality" + 0.005*"good" + 0.005*"risk" + 0.005*"needs" + 0.004*"plans" + 0.004*"need" + 0.004*"appropriately" + 0.004*"management" + 0.004*"family"', '0.011*"’" + 0.011*"quality" + 0.008*"needs" + 0.006*"progress" + 0.006*"plans" + 0.006*"good" + 0.006*"well" + 0.005*"risk" + 0.005*"experiences" + 0.005*"oversight"', '0.011*"’" + 0.010*"quality" + 0.007*"needs" + 0.007*"good" + 0.005*"Ealing" + 0.005*"management" + 0.004*"always" + 0.004*"leaders" + 0.004*"experiences" + 0.004*"protection"']</t>
   </si>
   <si>
     <t>308</t>
@@ -2053,7 +2053,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"needs" + 0.008*"ensure" + 0.008*"good" + 0.008*"effective" + 0.007*"Enfield" + 0.007*"practice" + 0.007*"clear" + 0.006*"timely" + 0.006*"quality"', '0.015*"’" + 0.006*"ensure" + 0.006*"needs" + 0.006*"good" + 0.005*"Enfield" + 0.005*"timely" + 0.005*"practice" + 0.005*"arrangements" + 0.005*"clear" + 0.005*"leaders"', '0.016*"’" + 0.010*"needs" + 0.009*"practice" + 0.008*"ensure" + 0.007*"good" + 0.007*"effective" + 0.007*"quality" + 0.006*"clear" + 0.006*"leaders" + 0.006*"improve"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.007*"ensure" + 0.007*"good" + 0.007*"practice" + 0.007*"effective" + 0.007*"clear" + 0.006*"leaders" + 0.006*"Enfield" + 0.005*"improve"', '0.011*"’" + 0.010*"needs" + 0.008*"ensure" + 0.007*"good" + 0.007*"quality" + 0.007*"effective" + 0.007*"practice" + 0.006*"Enfield" + 0.006*"clear" + 0.006*"progress"', '0.017*"’" + 0.009*"practice" + 0.007*"Enfield" + 0.007*"good" + 0.006*"needs" + 0.006*"quality" + 0.006*"ensure" + 0.006*"timely" + 0.006*"effective" + 0.006*"clear"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2083,7 +2083,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"need" + 0.006*"good" + 0.006*"ensure" + 0.006*"progress" + 0.006*"range" + 0.005*"risk"', '0.013*"’" + 0.008*"well" + 0.008*"good" + 0.008*"plans" + 0.008*"needs" + 0.007*"range" + 0.005*"need" + 0.005*"risk" + 0.005*"quality" + 0.004*"risks"', '0.012*"’" + 0.010*"well" + 0.009*"good" + 0.008*"needs" + 0.007*"plans" + 0.006*"need" + 0.005*"timely" + 0.005*"progress" + 0.005*"consistently" + 0.005*"quality"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.008*"good" + 0.007*"plans" + 0.006*"need" + 0.006*"needs" + 0.005*"range" + 0.005*"progress" + 0.004*"timely" + 0.004*"Senior"', '0.014*"’" + 0.010*"well" + 0.008*"good" + 0.008*"plans" + 0.008*"needs" + 0.006*"range" + 0.006*"need" + 0.006*"ensure" + 0.005*"progress" + 0.005*"information"', '0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"need" + 0.006*"range" + 0.005*"quality" + 0.005*"progress" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2119,7 +2119,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"practice" + 0.006*"within" + 0.006*"quality" + 0.006*"planning" + 0.005*"needs" + 0.005*"including" + 0.005*"number" + 0.005*"effective" + 0.005*"carers"', '0.011*"practice" + 0.009*"’" + 0.006*"within" + 0.006*"leaders" + 0.006*"planning" + 0.006*"plans" + 0.005*"number" + 0.005*"protection" + 0.005*"effective" + 0.005*"needs"', '0.013*"’" + 0.009*"practice" + 0.008*"number" + 0.007*"effective" + 0.006*"planning" + 0.006*"needs" + 0.006*"need" + 0.006*"plans" + 0.006*"including" + 0.006*"However"']</t>
+    <t>['0.013*"’" + 0.011*"practice" + 0.007*"number" + 0.007*"effective" + 0.006*"planning" + 0.006*"needs" + 0.006*"quality" + 0.006*"plans" + 0.006*"However" + 0.005*"within"', '0.012*"’" + 0.009*"practice" + 0.006*"number" + 0.006*"including" + 0.005*"plans" + 0.005*"within" + 0.005*"needs" + 0.005*"However" + 0.005*"effective" + 0.005*"small"', '0.014*"’" + 0.008*"practice" + 0.007*"planning" + 0.006*"within" + 0.006*"need" + 0.006*"small" + 0.005*"including" + 0.005*"quality" + 0.005*"number" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2149,7 +2149,7 @@
     <t>0.2054</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"effective" + 0.006*"needs" + 0.006*"well" + 0.006*"appropriate" + 0.006*"leaders" + 0.005*"arrangements" + 0.005*"plans" + 0.005*"good" + 0.005*"risk"', '0.012*"’" + 0.009*"needs" + 0.008*"effective" + 0.008*"well" + 0.007*"appropriate" + 0.006*"ensure" + 0.006*"good" + 0.005*"family" + 0.005*"shared" + 0.005*"leaders"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"effective" + 0.007*"good" + 0.006*"arrangements" + 0.006*"ensure" + 0.005*"appropriate" + 0.005*"improve" + 0.005*"timely"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.008*"effective" + 0.008*"well" + 0.006*"good" + 0.006*"shared" + 0.006*"plans" + 0.005*"appropriate" + 0.005*"ensure" + 0.005*"leaders"', '0.012*"’" + 0.008*"effective" + 0.008*"well" + 0.007*"needs" + 0.007*"appropriate" + 0.006*"good" + 0.006*"arrangements" + 0.005*"ensure" + 0.005*"risk" + 0.005*"improve"', '0.010*"’" + 0.007*"needs" + 0.007*"effective" + 0.007*"well" + 0.005*"good" + 0.005*"arrangements" + 0.005*"appropriate" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2173,7 +2173,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"Haringey" + 0.010*"needs" + 0.009*"plans" + 0.007*"well" + 0.006*"good" + 0.005*"need" + 0.005*"education" + 0.004*"24" + 0.004*"progress"', '0.008*"’" + 0.006*"needs" + 0.005*"good" + 0.005*"Haringey" + 0.005*"plans" + 0.004*"well" + 0.004*"progress" + 0.003*"education" + 0.003*"risk" + 0.003*"need"', '0.014*"’" + 0.008*"Haringey" + 0.006*"need" + 0.005*"progress" + 0.005*"plans" + 0.005*"needs" + 0.005*"well" + 0.005*"risk" + 0.004*"impact" + 0.004*"supported"']</t>
+    <t>['0.010*"’" + 0.007*"Haringey" + 0.007*"needs" + 0.006*"plans" + 0.005*"well" + 0.005*"progress" + 0.005*"good" + 0.005*"need" + 0.004*"supported" + 0.004*"education"', '0.020*"’" + 0.009*"needs" + 0.008*"Haringey" + 0.008*"plans" + 0.006*"good" + 0.005*"need" + 0.005*"well" + 0.005*"24" + 0.004*"education" + 0.004*"progress"', '0.015*"’" + 0.009*"Haringey" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.005*"good" + 0.005*"progress" + 0.004*"need" + 0.004*"risk" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2203,7 +2203,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.014*"good" + 0.011*"well" + 0.007*"needs" + 0.007*"plans" + 0.006*"early" + 0.006*"practice" + 0.006*"impact" + 0.005*"need" + 0.005*"school"', '0.009*"’" + 0.008*"good" + 0.007*"needs" + 0.005*"need" + 0.005*"experiences" + 0.005*"impact" + 0.005*"practice" + 0.005*"well" + 0.004*"protection" + 0.004*"team"', '0.009*"needs" + 0.009*"’" + 0.008*"good" + 0.008*"well" + 0.006*"protection" + 0.005*"impact" + 0.004*"experiences" + 0.004*"planning" + 0.004*"need" + 0.004*"plans"']</t>
+    <t>['0.015*"’" + 0.011*"good" + 0.009*"needs" + 0.008*"well" + 0.006*"plans" + 0.006*"impact" + 0.005*"protection" + 0.005*"practice" + 0.005*"school" + 0.005*"need"', '0.010*"good" + 0.009*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"experiences" + 0.006*"early" + 0.005*"impact" + 0.005*"plans" + 0.005*"practice" + 0.005*"need"', '0.010*"good" + 0.010*"’" + 0.009*"well" + 0.006*"needs" + 0.005*"need" + 0.004*"plans" + 0.004*"impact" + 0.004*"practice" + 0.004*"early" + 0.004*"protection"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2233,7 +2233,7 @@
     <t>0.2113</t>
   </si>
   <si>
-    <t>['0.009*"needs" + 0.009*"’" + 0.008*"need" + 0.007*"quality" + 0.007*"plans" + 0.006*"good" + 0.006*"practice" + 0.006*"meetings" + 0.005*"well" + 0.005*"clear"', '0.010*"’" + 0.008*"good" + 0.007*"well" + 0.006*"practice" + 0.006*"needs" + 0.006*"quality" + 0.006*"need" + 0.005*"plans" + 0.005*"appropriate" + 0.005*"consistently"', '0.012*"’" + 0.009*"good" + 0.008*"quality" + 0.007*"need" + 0.007*"well" + 0.006*"needs" + 0.006*"meetings" + 0.006*"plans" + 0.005*"consistently" + 0.005*"progress"']</t>
+    <t>['0.012*"’" + 0.009*"good" + 0.008*"quality" + 0.006*"needs" + 0.006*"meetings" + 0.006*"well" + 0.006*"plans" + 0.006*"need" + 0.005*"practice" + 0.004*"consistently"', '0.010*"’" + 0.007*"good" + 0.006*"need" + 0.006*"needs" + 0.006*"consistently" + 0.005*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"quality" + 0.005*"meetings"', '0.009*"needs" + 0.009*"need" + 0.009*"’" + 0.007*"well" + 0.007*"quality" + 0.007*"plans" + 0.007*"good" + 0.006*"practice" + 0.005*"meetings" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>312</t>
@@ -2266,7 +2266,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"Hillingdon" + 0.007*"needs" + 0.004*"team" + 0.004*"need" + 0.004*"PAs" + 0.004*"2023" + 0.003*"appropriate"', '0.016*"’" + 0.010*"needs" + 0.007*"plans" + 0.007*"Hillingdon" + 0.006*"well" + 0.005*"experiences" + 0.004*"October" + 0.004*"team" + 0.004*"6" + 0.004*"family"', '0.019*"’" + 0.011*"needs" + 0.009*"Hillingdon" + 0.008*"well" + 0.008*"plans" + 0.005*"need" + 0.005*"team" + 0.005*"2" + 0.005*"6" + 0.004*"leaders"']</t>
+    <t>['0.023*"’" + 0.011*"needs" + 0.009*"Hillingdon" + 0.009*"well" + 0.007*"plans" + 0.005*"team" + 0.005*"6" + 0.005*"need" + 0.004*"practice" + 0.004*"leaders"', '0.011*"’" + 0.008*"Hillingdon" + 0.007*"plans" + 0.006*"needs" + 0.006*"well" + 0.004*"2" + 0.004*"team" + 0.004*"October" + 0.003*"improve" + 0.003*"2023"', '0.015*"’" + 0.009*"plans" + 0.009*"needs" + 0.007*"well" + 0.005*"Hillingdon" + 0.005*"need" + 0.005*"2" + 0.004*"carers" + 0.004*"team" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2296,7 +2296,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"needs" + 0.008*"Hounslow" + 0.007*"well" + 0.007*"effective" + 0.006*"plans" + 0.006*"timely" + 0.004*"2023" + 0.004*"16" + 0.004*"leaders"', '0.026*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"effective" + 0.006*"timely" + 0.006*"Hounslow" + 0.005*"progress" + 0.005*"plans" + 0.005*"20" + 0.005*"experiences"', '0.013*"’" + 0.012*"needs" + 0.011*"well" + 0.007*"Hounslow" + 0.007*"effective" + 0.006*"timely" + 0.005*"plans" + 0.005*"oversight" + 0.005*"strong" + 0.004*"16"']</t>
+    <t>['0.019*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"effective" + 0.007*"Hounslow" + 0.005*"plans" + 0.005*"oversight" + 0.005*"timely" + 0.004*"20" + 0.004*"training"', '0.019*"’" + 0.012*"needs" + 0.009*"well" + 0.007*"effective" + 0.007*"Hounslow" + 0.006*"timely" + 0.005*"plans" + 0.004*"strong" + 0.004*"progress" + 0.004*"training"', '0.021*"’" + 0.012*"well" + 0.011*"needs" + 0.007*"timely" + 0.007*"effective" + 0.007*"Hounslow" + 0.006*"plans" + 0.005*"experiences" + 0.005*"16" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2326,7 +2326,7 @@
     <t>0.1842</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"highly" + 0.007*"plans" + 0.006*"school" + 0.005*"quality" + 0.005*"good" + 0.005*"Islington" + 0.005*"effective"', '0.010*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"good" + 0.005*"plans" + 0.005*"effective" + 0.005*"highly" + 0.004*"Islington" + 0.004*"quality" + 0.003*"lives"', '0.013*"’" + 0.012*"well" + 0.012*"needs" + 0.007*"plans" + 0.007*"leaders" + 0.006*"quality" + 0.006*"good" + 0.006*"effective" + 0.005*"highly" + 0.005*"practice"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.010*"well" + 0.007*"highly" + 0.007*"plans" + 0.006*"leaders" + 0.006*"quality" + 0.005*"Islington" + 0.005*"practice" + 0.005*"good"', '0.012*"’" + 0.010*"needs" + 0.006*"well" + 0.005*"quality" + 0.005*"good" + 0.005*"plans" + 0.005*"leaders" + 0.004*"effective" + 0.004*"carers" + 0.004*"Islington"', '0.013*"well" + 0.011*"’" + 0.011*"needs" + 0.007*"good" + 0.007*"plans" + 0.006*"effective" + 0.006*"highly" + 0.005*"risk" + 0.005*"quality" + 0.005*"Islington"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2359,7 +2359,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"good" + 0.006*"Lambeth" + 0.006*"need" + 0.005*"progress" + 0.005*"arrangements" + 0.004*"carers"', '0.014*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"good" + 0.007*"Lambeth" + 0.007*"impact" + 0.006*"plans" + 0.006*"progress" + 0.005*"4" + 0.005*"need"', '0.014*"’" + 0.009*"needs" + 0.008*"plans" + 0.008*"well" + 0.006*"good" + 0.006*"need" + 0.006*"progress" + 0.006*"Lambeth" + 0.005*"impact" + 0.005*"leaders"']</t>
+    <t>['0.019*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"good" + 0.008*"plans" + 0.006*"progress" + 0.006*"impact" + 0.006*"Lambeth" + 0.005*"leaders" + 0.005*"November"', '0.013*"’" + 0.011*"needs" + 0.007*"well" + 0.007*"plans" + 0.007*"Lambeth" + 0.006*"good" + 0.006*"need" + 0.005*"progress" + 0.005*"impact" + 0.005*"leaders"', '0.012*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.007*"Lambeth" + 0.006*"need" + 0.005*"good" + 0.005*"Leaders" + 0.004*"progress" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2389,7 +2389,7 @@
     <t>0.1538</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"well" + 0.006*"However" + 0.006*"quality" + 0.005*"needs" + 0.005*"information" + 0.005*"appropriate" + 0.004*"early" + 0.004*"timely" + 0.004*"education"', '0.009*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"timely" + 0.006*"However" + 0.006*"impact" + 0.005*"appropriate" + 0.004*"needs" + 0.004*"oversight" + 0.004*"progress"', '0.008*"’" + 0.006*"However" + 0.006*"timely" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"impact" + 0.004*"well" + 0.004*"progress" + 0.004*"needs" + 0.004*"changes"']</t>
+    <t>['0.007*"’" + 0.006*"well" + 0.005*"However" + 0.005*"quality" + 0.005*"timely" + 0.005*"appropriate" + 0.004*"needs" + 0.004*"impact" + 0.004*"information" + 0.004*"good"', '0.010*"’" + 0.007*"However" + 0.006*"quality" + 0.005*"appropriate" + 0.005*"impact" + 0.005*"well" + 0.005*"timely" + 0.004*"clear" + 0.004*"plans" + 0.004*"needs"', '0.010*"’" + 0.008*"well" + 0.006*"quality" + 0.006*"timely" + 0.005*"However" + 0.005*"appropriate" + 0.005*"needs" + 0.004*"impact" + 0.004*"progress" + 0.004*"oversight"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2410,7 +2410,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.007*"Merton" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.004*"good" + 0.004*"leaders" + 0.004*"education" + 0.004*"information"', '0.012*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"Merton" + 0.005*"family" + 0.005*"progress" + 0.004*"risk" + 0.004*"4" + 0.004*"practice" + 0.004*"2022"', '0.017*"’" + 0.007*"well" + 0.006*"Merton" + 0.005*"needs" + 0.005*"plans" + 0.005*"ensure" + 0.005*"family" + 0.004*"across" + 0.004*"4" + 0.004*"good"']</t>
+    <t>['0.016*"’" + 0.008*"Merton" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"family" + 0.005*"early" + 0.004*"progress" + 0.004*"4" + 0.004*"education"', '0.008*"’" + 0.005*"well" + 0.004*"Merton" + 0.004*"progress" + 0.003*"good" + 0.003*"ensure" + 0.003*"family" + 0.003*"Leaders" + 0.003*"plans" + 0.003*"across"', '0.020*"’" + 0.010*"well" + 0.006*"needs" + 0.005*"Merton" + 0.004*"progress" + 0.004*"2022" + 0.004*"family" + 0.004*"good" + 0.004*"plans" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2428,7 +2428,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50192878</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"plans" + 0.006*"effective" + 0.006*"progress" + 0.006*"need" + 0.005*"early" + 0.004*"18"', '0.021*"’" + 0.008*"needs" + 0.007*"progress" + 0.007*"plans" + 0.006*"Newham" + 0.006*"effective" + 0.006*"good" + 0.006*"practice" + 0.006*"need" + 0.005*"risks"', '0.013*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"need" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective" + 0.004*"good" + 0.004*"Leaders"']</t>
+    <t>['0.023*"’" + 0.010*"needs" + 0.007*"Newham" + 0.007*"effective" + 0.007*"progress" + 0.006*"plans" + 0.006*"practice" + 0.006*"need" + 0.005*"good" + 0.005*"Leaders"', '0.017*"’" + 0.007*"Newham" + 0.007*"needs" + 0.006*"need" + 0.006*"practice" + 0.006*"progress" + 0.006*"plans" + 0.005*"effective" + 0.005*"good" + 0.005*"18"', '0.014*"’" + 0.006*"Newham" + 0.005*"practice" + 0.005*"plans" + 0.005*"need" + 0.005*"needs" + 0.005*"progress" + 0.004*"effective" + 0.004*"good" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2455,7 +2455,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.005*"’" + 0.005*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"Redbridge" + 0.004*"need" + 0.004*"risk" + 0.004*"team" + 0.004*"ensure" + 0.004*"strong"', '0.009*"’" + 0.007*"well" + 0.007*"practice" + 0.006*"needs" + 0.006*"strong" + 0.006*"need" + 0.005*"progress" + 0.005*"including" + 0.005*"risk" + 0.005*"Redbridge"', '0.007*"practice" + 0.007*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"need" + 0.005*"well" + 0.005*"Redbridge" + 0.005*"strong" + 0.005*"risk" + 0.004*"team"']</t>
+    <t>['0.007*"need" + 0.007*"’" + 0.007*"practice" + 0.005*"risk" + 0.005*"effective" + 0.005*"well" + 0.005*"strong" + 0.005*"progress" + 0.005*"Redbridge" + 0.005*"ensure"', '0.010*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.006*"strong" + 0.005*"including" + 0.005*"effective" + 0.005*"need" + 0.005*"risk" + 0.004*"team"', '0.007*"practice" + 0.007*"needs" + 0.006*"well" + 0.006*"Redbridge" + 0.006*"’" + 0.005*"need" + 0.005*"effective" + 0.005*"including" + 0.004*"strong" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2479,7 +2479,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.013*"well" + 0.010*"Richmond" + 0.007*"needs" + 0.007*"supported" + 0.007*"team" + 0.006*"need" + 0.006*"good" + 0.005*"4" + 0.005*"additional"', '0.011*"’" + 0.007*"Richmond" + 0.007*"well" + 0.006*"needs" + 0.005*"supported" + 0.005*"strong" + 0.004*"team" + 0.004*"need" + 0.004*"upon" + 0.004*"range"', '0.016*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"Richmond" + 0.006*"good" + 0.005*"need" + 0.005*"supported" + 0.005*"31" + 0.005*"team" + 0.004*"strong"']</t>
+    <t>['0.017*"’" + 0.012*"well" + 0.011*"Richmond" + 0.007*"needs" + 0.007*"good" + 0.007*"supported" + 0.006*"team" + 0.006*"need" + 0.005*"ensure" + 0.005*"January"', '0.018*"’" + 0.012*"well" + 0.008*"needs" + 0.007*"Richmond" + 0.006*"supported" + 0.006*"team" + 0.006*"need" + 0.005*"4" + 0.005*"good" + 0.005*"31"', '0.010*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"Richmond" + 0.005*"need" + 0.004*"ensure" + 0.004*"additional" + 0.004*"supported" + 0.004*"good" + 0.004*"strong"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2506,7 +2506,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"Southwark" + 0.009*"well" + 0.007*"good" + 0.007*"progress" + 0.007*"needs" + 0.006*"need" + 0.005*"leaders" + 0.005*"plans" + 0.005*"strong"', '0.015*"’" + 0.009*"good" + 0.008*"needs" + 0.008*"Southwark" + 0.007*"well" + 0.006*"receive" + 0.005*"Leaders" + 0.005*"practice" + 0.005*"plans" + 0.005*"progress"', '0.018*"’" + 0.011*"Southwark" + 0.008*"good" + 0.007*"well" + 0.006*"effective" + 0.006*"needs" + 0.006*"plans" + 0.006*"need" + 0.006*"strong" + 0.005*"progress"']</t>
+    <t>['0.016*"’" + 0.008*"Southwark" + 0.007*"good" + 0.006*"needs" + 0.005*"plans" + 0.005*"well" + 0.005*"risks" + 0.004*"effective" + 0.004*"Leaders" + 0.004*"progress"', '0.022*"’" + 0.010*"Southwark" + 0.010*"well" + 0.009*"good" + 0.008*"needs" + 0.007*"need" + 0.007*"progress" + 0.006*"strong" + 0.006*"receive" + 0.006*"leaders"', '0.013*"’" + 0.008*"Southwark" + 0.007*"needs" + 0.007*"good" + 0.005*"Leaders" + 0.005*"progress" + 0.005*"plans" + 0.005*"effective" + 0.005*"well" + 0.005*"receive"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2533,7 +2533,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.005*"effective" + 0.005*"Sutton" + 0.004*"receive" + 0.004*"progress" + 0.004*"needs" + 0.004*"need" + 0.004*"good" + 0.004*"2021"', '0.017*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"receive" + 0.004*"Sutton" + 0.004*"10" + 0.004*"2021" + 0.004*"effective" + 0.004*"leaders"', '0.020*"’" + 0.007*"Sutton" + 0.007*"progress" + 0.006*"well" + 0.006*"needs" + 0.006*"6" + 0.005*"effective" + 0.005*"supported" + 0.005*"receive" + 0.005*"‘"']</t>
+    <t>['0.010*"’" + 0.005*"well" + 0.004*"needs" + 0.004*"receive" + 0.004*"need" + 0.004*"progress" + 0.003*"Sutton" + 0.003*"home" + 0.003*"good" + 0.003*"6"', '0.019*"’" + 0.007*"well" + 0.006*"Sutton" + 0.006*"needs" + 0.005*"6" + 0.005*"progress" + 0.005*"10" + 0.005*"good" + 0.004*"effective" + 0.004*"understand"', '0.018*"’" + 0.008*"well" + 0.006*"Sutton" + 0.006*"needs" + 0.006*"effective" + 0.006*"progress" + 0.005*"receive" + 0.005*"good" + 0.004*"December" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2560,7 +2560,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"good" + 0.007*"effective" + 0.005*"‘" + 0.005*"including" + 0.005*"early" + 0.005*"need" + 0.005*"plans" + 0.004*"carers" + 0.004*"well"', '0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.006*"practice" + 0.005*"effective" + 0.005*"‘" + 0.005*"need" + 0.005*"needs"', '0.010*"’" + 0.006*"‘" + 0.006*"plans" + 0.006*"good" + 0.005*"effective" + 0.005*"need" + 0.005*"practice" + 0.005*"well" + 0.005*"needs" + 0.005*"early"']</t>
+    <t>['0.017*"’" + 0.008*"good" + 0.007*"effective" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"need" + 0.005*"including" + 0.005*"‘" + 0.005*"progress"', '0.017*"’" + 0.006*"plans" + 0.006*"practice" + 0.006*"good" + 0.005*"well" + 0.005*"‘" + 0.005*"need" + 0.005*"progress" + 0.005*"effective" + 0.004*"education"', '0.009*"’" + 0.007*"‘" + 0.006*"effective" + 0.006*"good" + 0.005*"early" + 0.005*"well" + 0.005*"plans" + 0.005*"practice" + 0.004*"need" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2587,7 +2587,7 @@
     <t>11/03/19</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.010*"well" + 0.007*"effective" + 0.006*"need" + 0.005*"needs" + 0.005*"good" + 0.004*"timely" + 0.003*"plans" + 0.003*"actions" + 0.003*"information"', '0.018*"’" + 0.014*"well" + 0.010*"needs" + 0.010*"good" + 0.008*"effective" + 0.007*"need" + 0.006*"plans" + 0.006*"timely" + 0.005*"risk" + 0.005*"ensure"', '0.012*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"effective" + 0.005*"plans" + 0.004*"risk" + 0.004*"practice" + 0.004*"timely" + 0.004*"need"']</t>
+    <t>['0.017*"’" + 0.014*"well" + 0.010*"needs" + 0.009*"good" + 0.007*"effective" + 0.006*"need" + 0.006*"plans" + 0.005*"timely" + 0.005*"risk" + 0.004*"protection"', '0.014*"’" + 0.011*"well" + 0.008*"needs" + 0.008*"effective" + 0.007*"good" + 0.005*"need" + 0.005*"plans" + 0.005*"ensure" + 0.004*"progress" + 0.004*"information"', '0.010*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"good" + 0.007*"effective" + 0.006*"need" + 0.005*"timely" + 0.004*"plans" + 0.004*"risk" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2611,7 +2611,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"needs" + 0.005*"progress" + 0.005*"well" + 0.005*"18" + 0.005*"Wandsworth" + 0.005*"Senior" + 0.004*"supported" + 0.004*"timely" + 0.004*"practice"', '0.013*"’" + 0.007*"well" + 0.007*"protection" + 0.006*"effective" + 0.006*"good" + 0.005*"Senior" + 0.005*"progress" + 0.005*"needs" + 0.005*"quality" + 0.005*"supported"', '0.011*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"needs" + 0.005*"Wandsworth" + 0.005*"progress" + 0.005*"ensure" + 0.005*"quality" + 0.005*"7" + 0.005*"18"']</t>
+    <t>['0.009*"’" + 0.006*"progress" + 0.006*"needs" + 0.006*"protection" + 0.005*"Senior" + 0.005*"Wandsworth" + 0.005*"effective" + 0.005*"practice" + 0.005*"supported" + 0.004*"7"', '0.012*"’" + 0.008*"well" + 0.006*"practice" + 0.006*"progress" + 0.005*"supported" + 0.005*"Wandsworth" + 0.005*"quality" + 0.005*"Senior" + 0.005*"needs" + 0.005*"receive"', '0.014*"’" + 0.007*"well" + 0.006*"ensure" + 0.005*"team" + 0.005*"needs" + 0.005*"protection" + 0.005*"7" + 0.005*"effective" + 0.005*"Senior" + 0.005*"Wandsworth"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2632,7 +2632,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.007*"practice" + 0.007*"highly" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.004*"skilled" + 0.004*"quality" + 0.004*"shared"', '0.011*"’" + 0.006*"needs" + 0.006*"practice" + 0.005*"highly" + 0.004*"well" + 0.003*"high" + 0.003*"family" + 0.003*"early" + 0.003*"direct" + 0.003*"across"', '0.010*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"highly" + 0.004*"across" + 0.004*"many" + 0.004*"needs" + 0.004*"direct" + 0.004*"family" + 0.003*"shared"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.007*"highly" + 0.005*"well" + 0.005*"practice" + 0.004*"many" + 0.004*"interventions" + 0.003*"across" + 0.003*"plans" + 0.003*"family"', '0.010*"’" + 0.006*"practice" + 0.005*"needs" + 0.005*"well" + 0.005*"highly" + 0.004*"across" + 0.003*"shared" + 0.003*"direct" + 0.003*"plans" + 0.003*"many"', '0.014*"’" + 0.008*"practice" + 0.005*"highly" + 0.005*"well" + 0.005*"needs" + 0.004*"many" + 0.004*"family" + 0.004*"across" + 0.004*"skilled" + 0.004*"high"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2662,7 +2662,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.006*"needs" + 0.005*"effective" + 0.005*"quality" + 0.005*"receive" + 0.005*"progress" + 0.005*"ensure" + 0.005*"need" + 0.005*"leaders" + 0.005*"impact"', '0.014*"’" + 0.007*"plans" + 0.005*"need" + 0.005*"effective" + 0.005*"progress" + 0.005*"Luton" + 0.005*"impact" + 0.005*"needs" + 0.004*"11" + 0.004*"well"', '0.019*"’" + 0.008*"need" + 0.007*"Luton" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"well" + 0.005*"effective" + 0.005*"impact" + 0.005*"ensure"']</t>
+    <t>['0.016*"’" + 0.008*"needs" + 0.007*"need" + 0.006*"good" + 0.006*"quality" + 0.005*"Luton" + 0.005*"progress" + 0.005*"effective" + 0.005*"ensure" + 0.005*"plans"', '0.015*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"impact" + 0.006*"plans" + 0.005*"Luton" + 0.005*"need" + 0.005*"receive" + 0.005*"good" + 0.005*"2022"', '0.020*"’" + 0.007*"need" + 0.007*"plans" + 0.006*"Luton" + 0.005*"effective" + 0.005*"ensure" + 0.005*"well" + 0.005*"progress" + 0.004*"good" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2689,7 +2689,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.007*"always" + 0.005*"education" + 0.005*"effective" + 0.005*"progress" + 0.005*"supported" + 0.005*"risk"', '0.014*"’" + 0.009*"Manchester" + 0.007*"supported" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"21" + 0.005*"information" + 0.005*"family" + 0.004*"protection"', '0.030*"’" + 0.011*"Manchester" + 0.011*"needs" + 0.007*"always" + 0.007*"supported" + 0.007*"well" + 0.006*"plans" + 0.006*"quality" + 0.005*"protection" + 0.005*"education"']</t>
+    <t>['0.016*"’" + 0.012*"Manchester" + 0.008*"needs" + 0.007*"always" + 0.006*"well" + 0.006*"supported" + 0.006*"plans" + 0.005*"quality" + 0.005*"21" + 0.005*"family"', '0.026*"’" + 0.011*"Manchester" + 0.010*"needs" + 0.007*"well" + 0.007*"supported" + 0.006*"education" + 0.006*"plans" + 0.005*"1" + 0.005*"effective" + 0.005*"family"', '0.018*"’" + 0.010*"needs" + 0.008*"Manchester" + 0.008*"always" + 0.007*"well" + 0.006*"effective" + 0.006*"supported" + 0.006*"protection" + 0.006*"disabled" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -2716,7 +2716,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"Medway" + 0.007*"practice" + 0.006*"impact" + 0.005*"experiences" + 0.005*"quality" + 0.005*"well" + 0.005*"oversight" + 0.005*"needs" + 0.005*"Senior"', '0.010*"’" + 0.008*"Medway" + 0.008*"quality" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.006*"oversight" + 0.006*"leaders" + 0.005*"Senior" + 0.005*"impact"', '0.020*"’" + 0.009*"well" + 0.009*"quality" + 0.009*"Medway" + 0.009*"practice" + 0.007*"leaders" + 0.007*"needs" + 0.006*"good" + 0.006*"oversight" + 0.006*"impact"']</t>
+    <t>['0.015*"’" + 0.011*"Medway" + 0.009*"practice" + 0.007*"well" + 0.007*"leaders" + 0.007*"quality" + 0.006*"needs" + 0.006*"impact" + 0.006*"experiences" + 0.006*"good"', '0.011*"’" + 0.008*"Medway" + 0.007*"well" + 0.006*"leaders" + 0.005*"oversight" + 0.005*"quality" + 0.005*"practice" + 0.005*"impact" + 0.004*"improve" + 0.004*"experiences"', '0.020*"’" + 0.009*"quality" + 0.009*"practice" + 0.008*"well" + 0.008*"Medway" + 0.007*"needs" + 0.007*"oversight" + 0.006*"clear" + 0.006*"progress" + 0.006*"risk"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -2737,7 +2737,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"Middlesbrough" + 0.007*"practice" + 0.007*"plans" + 0.006*"needs" + 0.005*"well" + 0.005*"effective" + 0.005*"good" + 0.005*"24" + 0.005*"progress"', '0.015*"’" + 0.008*"effective" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.005*"progress" + 0.005*"13" + 0.005*"Middlesbrough" + 0.005*"place" + 0.005*"good"', '0.015*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.006*"well" + 0.005*"progress" + 0.005*"means" + 0.005*"practice" + 0.005*"needs" + 0.004*"24"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"Middlesbrough" + 0.007*"effective" + 0.006*"well" + 0.006*"progress" + 0.005*"practice" + 0.005*"24" + 0.005*"March"', '0.014*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.005*"needs" + 0.005*"place" + 0.005*"progress" + 0.005*"risk" + 0.004*"practice"', '0.010*"’" + 0.007*"practice" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.004*"needs" + 0.004*"impact" + 0.004*"13"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -2761,7 +2761,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"Milton" + 0.006*"Keynes" + 0.005*"need" + 0.005*"practice" + 0.005*"well" + 0.005*"October" + 0.005*"needs" + 0.004*"25" + 0.004*"leaders"', '0.015*"’" + 0.007*"Keynes" + 0.006*"well" + 0.006*"Milton" + 0.006*"need" + 0.005*"impact" + 0.005*"November" + 0.005*"plans" + 0.005*"leaders" + 0.005*"team"', '0.017*"’" + 0.005*"well" + 0.005*"good" + 0.005*"Milton" + 0.005*"need" + 0.004*"25" + 0.004*"Keynes" + 0.004*"plans" + 0.004*"carers" + 0.004*"leaders"']</t>
+    <t>['0.015*"’" + 0.006*"Keynes" + 0.006*"practice" + 0.006*"well" + 0.005*"need" + 0.005*"5" + 0.005*"Milton" + 0.005*"effective" + 0.005*"plans" + 0.004*"25"', '0.014*"’" + 0.006*"well" + 0.006*"Milton" + 0.005*"need" + 0.005*"2021" + 0.004*"Keynes" + 0.004*"team" + 0.004*"good" + 0.004*"plans" + 0.004*"effective"', '0.016*"’" + 0.007*"Milton" + 0.006*"Keynes" + 0.005*"need" + 0.005*"well" + 0.005*"25" + 0.005*"leaders" + 0.005*"good" + 0.005*"October" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -2785,7 +2785,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.010*"plans" + 0.008*"needs" + 0.007*"Newcastle" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.005*"ensure" + 0.005*"management" + 0.005*"need"', '0.017*"’" + 0.010*"plans" + 0.009*"needs" + 0.008*"good" + 0.008*"protection" + 0.007*"Newcastle" + 0.006*"progress" + 0.006*"management" + 0.006*"need" + 0.006*"planning"', '0.012*"’" + 0.011*"plans" + 0.007*"well" + 0.007*"protection" + 0.006*"making" + 0.006*"Newcastle" + 0.006*"needs" + 0.005*"progress" + 0.005*"10" + 0.005*"ensure"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"Newcastle" + 0.006*"well" + 0.006*"good" + 0.006*"progress" + 0.006*"protection" + 0.005*"making" + 0.005*"management"', '0.011*"’" + 0.009*"needs" + 0.008*"plans" + 0.007*"protection" + 0.006*"good" + 0.005*"Newcastle" + 0.005*"response" + 0.005*"need" + 0.005*"well" + 0.005*"planning"', '0.020*"’" + 0.014*"plans" + 0.008*"Newcastle" + 0.007*"well" + 0.007*"needs" + 0.007*"protection" + 0.007*"good" + 0.007*"progress" + 0.006*"ensure" + 0.006*"making"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -2806,7 +2806,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"Norfolk" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"supported" + 0.005*"carers" + 0.005*"including" + 0.005*"range" + 0.005*"18"', '0.013*"’" + 0.006*"well" + 0.006*"Norfolk" + 0.005*"carers" + 0.005*"supported" + 0.004*"plans" + 0.004*"leaders" + 0.004*"practice" + 0.004*"needs" + 0.004*"range"', '0.021*"’" + 0.009*"well" + 0.008*"Norfolk" + 0.007*"carers" + 0.006*"practice" + 0.006*"needs" + 0.005*"supported" + 0.005*"effective" + 0.005*"plans" + 0.005*"family"']</t>
+    <t>['0.011*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"needs" + 0.005*"supported" + 0.004*"carers" + 0.004*"plans" + 0.004*"Norfolk" + 0.003*"including" + 0.003*"2022"', '0.015*"’" + 0.007*"Norfolk" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.005*"supported" + 0.005*"carers" + 0.004*"7" + 0.004*"information" + 0.004*"18"', '0.021*"’" + 0.010*"Norfolk" + 0.010*"well" + 0.007*"carers" + 0.006*"needs" + 0.005*"supported" + 0.005*"plans" + 0.005*"practice" + 0.005*"range" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -2836,7 +2836,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"practice" + 0.009*"risk" + 0.008*"leaders" + 0.007*"needs" + 0.007*"planning" + 0.006*"need" + 0.005*"North" + 0.005*"quality" + 0.005*"East"', '0.011*"’" + 0.005*"practice" + 0.005*"planning" + 0.005*"needs" + 0.005*"Lincolnshire" + 0.005*"leaders" + 0.004*"2021" + 0.004*"need" + 0.004*"risk" + 0.004*"senior"', '0.014*"’" + 0.006*"leaders" + 0.005*"plans" + 0.005*"practice" + 0.005*"planning" + 0.005*"many" + 0.005*"October" + 0.005*"needs" + 0.004*"risk" + 0.004*"oversight"']</t>
+    <t>['0.012*"’" + 0.008*"practice" + 0.008*"risk" + 0.006*"leaders" + 0.006*"planning" + 0.005*"needs" + 0.005*"need" + 0.005*"October" + 0.004*"delay" + 0.004*"harm"', '0.016*"’" + 0.007*"planning" + 0.007*"practice" + 0.006*"risk" + 0.006*"needs" + 0.006*"leaders" + 0.005*"many" + 0.005*"need" + 0.005*"East" + 0.005*"oversight"', '0.014*"’" + 0.009*"practice" + 0.007*"leaders" + 0.006*"needs" + 0.006*"risk" + 0.005*"Lincolnshire" + 0.005*"planning" + 0.005*"need" + 0.005*"North" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -2863,7 +2863,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.008*"‘" + 0.006*"North" + 0.006*"Lincolnshire" + 0.006*"leaders" + 0.006*"approach" + 0.005*"family" + 0.005*"protection" + 0.005*"10" + 0.005*"need"', '0.016*"’" + 0.005*"‘" + 0.005*"well" + 0.005*"family" + 0.004*"North" + 0.004*"14" + 0.004*"leaders" + 0.004*"team" + 0.004*"approach" + 0.004*"Lincolnshire"', '0.017*"’" + 0.007*"family" + 0.007*"‘" + 0.005*"well" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"10" + 0.005*"approach" + 0.005*"North" + 0.004*"leaders"']</t>
+    <t>['0.023*"’" + 0.008*"‘" + 0.006*"Lincolnshire" + 0.006*"family" + 0.005*"approach" + 0.005*"leaders" + 0.005*"well" + 0.005*"need" + 0.004*"North" + 0.004*"October"', '0.021*"’" + 0.006*"family" + 0.006*"North" + 0.006*"‘" + 0.005*"approach" + 0.005*"council" + 0.005*"plans" + 0.005*"need" + 0.005*"Lincolnshire" + 0.004*"needs"', '0.017*"’" + 0.006*"‘" + 0.006*"10" + 0.006*"leaders" + 0.006*"well" + 0.005*"family" + 0.005*"North" + 0.005*"Lincolnshire" + 0.005*"need" + 0.004*"approach"']</t>
   </si>
   <si>
     <t>940</t>
@@ -2893,7 +2893,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"well" + 0.005*"However" + 0.005*"quality" + 0.005*"practice" + 0.005*"Northamptonshire" + 0.004*"North" + 0.004*"impact" + 0.004*"needs" + 0.004*"2022"', '0.023*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.006*"quality" + 0.006*"impact" + 0.005*"needs" + 0.005*"Leaders" + 0.005*"NCT" + 0.005*"e"', '0.013*"’" + 0.010*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.005*"practice" + 0.005*"quality" + 0.005*"need" + 0.005*"NCT" + 0.005*"3" + 0.004*"2022"']</t>
+    <t>['0.020*"’" + 0.010*"Northamptonshire" + 0.008*"North" + 0.006*"Leaders" + 0.006*"practice" + 0.005*"quality" + 0.005*"needs" + 0.005*"impact" + 0.005*"well" + 0.005*"NCT"', '0.019*"’" + 0.008*"Northamptonshire" + 0.007*"well" + 0.006*"quality" + 0.005*"3" + 0.005*"practice" + 0.005*"North" + 0.005*"impact" + 0.004*"NCT" + 0.004*"e"', '0.011*"’" + 0.007*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.005*"quality" + 0.005*"need" + 0.005*"needs" + 0.005*"NCT" + 0.004*"plans" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -2917,7 +2917,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"always" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"progress" + 0.006*"need" + 0.006*"North" + 0.006*"quality" + 0.006*"practice" + 0.005*"number"', '0.013*"’" + 0.008*"quality" + 0.006*"always" + 0.006*"risk" + 0.006*"needs" + 0.005*"North" + 0.005*"practice" + 0.005*"experienced" + 0.005*"number" + 0.005*"need"', '0.016*"’" + 0.009*"quality" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"number" + 0.005*"North" + 0.005*"risk" + 0.005*"well" + 0.005*"practice" + 0.005*"oversight"']</t>
+    <t>['0.016*"’" + 0.007*"North" + 0.007*"Somerset" + 0.006*"quality" + 0.006*"needs" + 0.005*"number" + 0.005*"always" + 0.005*"plans" + 0.005*"risk" + 0.004*"need"', '0.014*"’" + 0.008*"quality" + 0.007*"needs" + 0.007*"always" + 0.006*"practice" + 0.006*"number" + 0.006*"risk" + 0.005*"well" + 0.005*"North" + 0.004*"24"', '0.019*"’" + 0.007*"quality" + 0.007*"Somerset" + 0.007*"needs" + 0.006*"progress" + 0.006*"need" + 0.006*"experienced" + 0.006*"always" + 0.006*"practice" + 0.005*"North"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -2941,7 +2941,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"need" + 0.005*"quality" + 0.005*"make" + 0.005*"needs" + 0.004*"impact" + 0.004*"clear" + 0.004*"early"', '0.014*"’" + 0.004*"leaders" + 0.004*"need" + 0.004*"quality" + 0.004*"needs" + 0.004*"well" + 0.003*"good" + 0.003*"impact" + 0.003*"make" + 0.003*"foster"', '0.013*"’" + 0.006*"well" + 0.005*"need" + 0.005*"leaders" + 0.005*"make" + 0.005*"understand" + 0.004*"needs" + 0.004*"impact" + 0.004*"early" + 0.004*"way"']</t>
+    <t>['0.017*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"needs" + 0.004*"quality" + 0.004*"impact" + 0.004*"working" + 0.004*"clear" + 0.004*"early" + 0.003*"need"', '0.014*"’" + 0.007*"well" + 0.006*"leaders" + 0.006*"make" + 0.005*"need" + 0.005*"quality" + 0.004*"early" + 0.004*"impact" + 0.004*"needs" + 0.004*"clear"', '0.016*"’" + 0.007*"well" + 0.007*"need" + 0.005*"quality" + 0.005*"make" + 0.004*"impact" + 0.004*"leaders" + 0.004*"protection" + 0.004*"needs" + 0.004*"early"']</t>
   </si>
   <si>
     <t>815</t>
@@ -2965,7 +2965,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"well" + 0.007*"North" + 0.006*"family" + 0.006*"Yorkshire" + 0.006*"practice" + 0.005*"needs" + 0.004*"3" + 0.004*"‘" + 0.004*"supported"', '0.021*"’" + 0.009*"well" + 0.007*"North" + 0.007*"practice" + 0.006*"Yorkshire" + 0.006*"family" + 0.005*"needs" + 0.005*"supported" + 0.005*"‘" + 0.004*"need"', '0.020*"’" + 0.007*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.006*"needs" + 0.005*"North" + 0.005*"‘" + 0.004*"7" + 0.004*"2023" + 0.004*"ensure"']</t>
+    <t>['0.015*"’" + 0.010*"well" + 0.008*"practice" + 0.007*"North" + 0.006*"Yorkshire" + 0.006*"‘" + 0.006*"needs" + 0.005*"family" + 0.005*"3" + 0.004*"2023"', '0.022*"’" + 0.005*"North" + 0.005*"Yorkshire" + 0.004*"well" + 0.004*"planning" + 0.004*"‘" + 0.004*"practice" + 0.004*"Leaders" + 0.004*"3" + 0.004*"effective"', '0.024*"’" + 0.008*"well" + 0.007*"family" + 0.007*"Yorkshire" + 0.007*"needs" + 0.007*"North" + 0.005*"practice" + 0.004*"‘" + 0.004*"7" + 0.004*"3"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -2989,7 +2989,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"impact" + 0.005*"need" + 0.004*"experiences" + 0.004*"quality" + 0.004*"education" + 0.004*"progress"', '0.028*"’" + 0.013*"needs" + 0.011*"well" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.006*"experiences" + 0.006*"education" + 0.005*"leaders" + 0.005*"impact"', '0.016*"’" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"experiences" + 0.006*"quality" + 0.005*"need" + 0.005*"impact" + 0.004*"practice" + 0.004*"always"']</t>
+    <t>['0.025*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"good" + 0.005*"need" + 0.005*"experiences" + 0.005*"practice" + 0.005*"plans" + 0.005*"impact" + 0.005*"leaders"', '0.018*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"good" + 0.006*"need" + 0.006*"experiences" + 0.006*"education" + 0.005*"impact" + 0.005*"practice" + 0.004*"always"', '0.022*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"good" + 0.007*"need" + 0.006*"quality" + 0.005*"practice" + 0.005*"experiences" + 0.005*"impact" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3016,7 +3016,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.006*"effective" + 0.006*"needs" + 0.006*"Nottingham" + 0.005*"oversight" + 0.005*"practice" + 0.005*"City" + 0.005*"impact" + 0.005*"11" + 0.005*"plans"', '0.010*"’" + 0.007*"needs" + 0.004*"Nottingham" + 0.004*"11" + 0.004*"impact" + 0.004*"risk" + 0.004*"effective" + 0.004*"plans" + 0.004*"City" + 0.003*"However"', '0.014*"’" + 0.010*"needs" + 0.007*"plans" + 0.006*"Nottingham" + 0.005*"impact" + 0.005*"effective" + 0.005*"2022" + 0.004*"oversight" + 0.004*"July" + 0.004*"11"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.006*"Nottingham" + 0.005*"plans" + 0.005*"effective" + 0.005*"impact" + 0.005*"City" + 0.005*"risk" + 0.005*"consistently" + 0.005*"oversight"', '0.013*"’" + 0.007*"needs" + 0.006*"11" + 0.005*"effective" + 0.005*"However" + 0.005*"plans" + 0.004*"impact" + 0.004*"Nottingham" + 0.004*"oversight" + 0.004*"practice"', '0.013*"’" + 0.007*"needs" + 0.006*"Nottingham" + 0.006*"plans" + 0.005*"effective" + 0.004*"impact" + 0.004*"City" + 0.004*"oversight" + 0.004*"2022" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>891</t>
@@ -3034,7 +3034,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"e" + 0.006*"receive" + 0.006*"progress" + 0.005*"made" + 0.005*"quality" + 0.005*"needs" + 0.005*"ensure"', '0.012*"’" + 0.008*"well" + 0.008*"practice" + 0.007*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.005*"receive" + 0.005*"areas" + 0.005*"carers" + 0.005*"made"', '0.013*"’" + 0.008*"practice" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.004*"progress" + 0.004*"quality" + 0.004*"made" + 0.004*"number" + 0.004*"receive"']</t>
+    <t>['0.013*"’" + 0.007*"practice" + 0.006*"needs" + 0.006*"well" + 0.006*"receive" + 0.005*"ensure" + 0.005*"plans" + 0.005*"made" + 0.005*"e" + 0.005*"progress"', '0.012*"’" + 0.008*"practice" + 0.008*"well" + 0.006*"plans" + 0.005*"receive" + 0.005*"needs" + 0.005*"quality" + 0.005*"e" + 0.005*"progress" + 0.005*"placements"', '0.012*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"ensure" + 0.006*"needs" + 0.006*"carers" + 0.005*"made" + 0.005*"areas" + 0.005*"receive" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3067,7 +3067,7 @@
     <t>0.176</t>
   </si>
   <si>
-    <t>['0.010*"needs" + 0.010*"practice" + 0.009*"’" + 0.009*"good" + 0.008*"progress" + 0.006*"effective" + 0.006*"planning" + 0.006*"quality" + 0.006*"plans" + 0.005*"well"', '0.008*"effective" + 0.008*"’" + 0.008*"good" + 0.007*"needs" + 0.007*"practice" + 0.006*"quality" + 0.006*"planning" + 0.006*"progress" + 0.005*"well" + 0.004*"place"', '0.013*"’" + 0.010*"good" + 0.009*"effective" + 0.009*"needs" + 0.008*"practice" + 0.008*"well" + 0.007*"plans" + 0.007*"quality" + 0.006*"planning" + 0.006*"risk"']</t>
+    <t>['0.011*"needs" + 0.011*"’" + 0.010*"good" + 0.009*"effective" + 0.008*"practice" + 0.008*"quality" + 0.008*"planning" + 0.007*"progress" + 0.006*"well" + 0.006*"plans"', '0.009*"’" + 0.008*"good" + 0.007*"practice" + 0.006*"needs" + 0.005*"well" + 0.005*"effective" + 0.004*"plans" + 0.004*"progress" + 0.004*"risk" + 0.004*"information"', '0.012*"’" + 0.011*"practice" + 0.009*"good" + 0.008*"effective" + 0.007*"needs" + 0.007*"progress" + 0.007*"well" + 0.007*"quality" + 0.006*"plans" + 0.005*"planning"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3097,7 +3097,7 @@
     <t>0.1848</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.010*"needs" + 0.007*"number" + 0.006*"good" + 0.005*"early" + 0.005*"live" + 0.004*"education" + 0.004*"plans" + 0.004*"response" + 0.004*"quality"', '0.014*"’" + 0.008*"needs" + 0.006*"good" + 0.005*"number" + 0.005*"protection" + 0.005*"early" + 0.005*"response" + 0.004*"plans" + 0.004*"education" + 0.004*"practice"', '0.014*"’" + 0.009*"needs" + 0.007*"good" + 0.005*"protection" + 0.005*"early" + 0.005*"number" + 0.005*"plans" + 0.005*"response" + 0.005*"effective" + 0.005*"quality"']</t>
+    <t>['0.014*"’" + 0.010*"needs" + 0.007*"good" + 0.006*"number" + 0.006*"early" + 0.005*"Oxfordshire" + 0.005*"response" + 0.005*"protection" + 0.005*"quality" + 0.005*"plans"', '0.015*"’" + 0.009*"needs" + 0.006*"number" + 0.006*"good" + 0.006*"early" + 0.005*"response" + 0.004*"plans" + 0.004*"protection" + 0.004*"effective" + 0.004*"Oxfordshire"', '0.010*"’" + 0.008*"needs" + 0.005*"good" + 0.005*"number" + 0.004*"plans" + 0.004*"protection" + 0.004*"education" + 0.004*"effective" + 0.004*"practice" + 0.004*"including"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3127,7 +3127,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"good" + 0.008*"practice" + 0.006*"well" + 0.006*"risk" + 0.006*"progress" + 0.006*"effective" + 0.005*"planning" + 0.005*"needs" + 0.004*"quality"', '0.013*"’" + 0.008*"needs" + 0.007*"practice" + 0.006*"well" + 0.006*"planning" + 0.006*"risk" + 0.005*"need" + 0.005*"effective" + 0.005*"progress" + 0.005*"including"', '0.014*"’" + 0.008*"well" + 0.007*"risk" + 0.006*"planning" + 0.006*"practice" + 0.006*"good" + 0.006*"needs" + 0.005*"quality" + 0.005*"need" + 0.005*"including"']</t>
+    <t>['0.014*"’" + 0.008*"risk" + 0.006*"practice" + 0.006*"well" + 0.005*"progress" + 0.005*"needs" + 0.005*"planning" + 0.005*"need" + 0.004*"quality" + 0.004*"effective"', '0.016*"’" + 0.008*"well" + 0.008*"good" + 0.007*"needs" + 0.007*"effective" + 0.007*"practice" + 0.006*"planning" + 0.005*"progress" + 0.005*"need" + 0.005*"quality"', '0.010*"’" + 0.007*"practice" + 0.006*"needs" + 0.005*"good" + 0.005*"planning" + 0.005*"well" + 0.005*"risk" + 0.005*"including" + 0.004*"quality" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>879</t>
@@ -3154,7 +3154,7 @@
     <t>0.1594</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.010*"However" + 0.009*"well" + 0.009*"good" + 0.009*"needs" + 0.009*"quality" + 0.007*"progress" + 0.006*"timely" + 0.006*"plans" + 0.006*"leaders"', '0.013*"’" + 0.008*"well" + 0.007*"good" + 0.006*"However" + 0.006*"quality" + 0.006*"result" + 0.005*"needs" + 0.005*"timely" + 0.005*"plans" + 0.004*"protection"', '0.017*"’" + 0.010*"However" + 0.009*"good" + 0.009*"well" + 0.008*"needs" + 0.008*"quality" + 0.007*"progress" + 0.006*"effective" + 0.006*"number" + 0.006*"timely"']</t>
+    <t>['0.012*"’" + 0.009*"good" + 0.009*"well" + 0.008*"quality" + 0.007*"However" + 0.007*"needs" + 0.007*"progress" + 0.006*"result" + 0.005*"identified" + 0.005*"leaders"', '0.018*"’" + 0.011*"However" + 0.009*"well" + 0.009*"quality" + 0.009*"good" + 0.008*"needs" + 0.007*"progress" + 0.006*"timely" + 0.006*"number" + 0.006*"plans"', '0.013*"’" + 0.008*"good" + 0.008*"needs" + 0.007*"well" + 0.007*"However" + 0.006*"timely" + 0.006*"result" + 0.005*"quality" + 0.005*"effective" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3184,7 +3184,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"care-experienced" + 0.007*"well" + 0.005*"Portsmouth" + 0.005*"needs" + 0.005*"plans" + 0.004*"leaders" + 0.004*"health" + 0.004*"family" + 0.004*"practice"', '0.019*"’" + 0.007*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"well" + 0.005*"family" + 0.005*"plans" + 0.005*"health" + 0.005*"risk" + 0.005*"15"', '0.018*"’" + 0.009*"well" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"family" + 0.006*"health" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders"']</t>
+    <t>['0.018*"’" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.007*"well" + 0.006*"plans" + 0.005*"health" + 0.005*"family" + 0.005*"need" + 0.004*"leaders"', '0.012*"’" + 0.007*"care-experienced" + 0.006*"Portsmouth" + 0.005*"needs" + 0.005*"well" + 0.005*"family" + 0.005*"receive" + 0.004*"progress" + 0.004*"health" + 0.004*"plans"', '0.019*"’" + 0.009*"well" + 0.009*"care-experienced" + 0.007*"needs" + 0.006*"Portsmouth" + 0.006*"family" + 0.006*"leaders" + 0.005*"health" + 0.005*"plans" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3217,7 +3217,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"number" + 0.007*"quality" + 0.007*"plans" + 0.007*"good" + 0.007*"well" + 0.006*"need" + 0.006*"effective" + 0.005*"timely" + 0.005*"practice"', '0.014*"’" + 0.006*"quality" + 0.006*"plans" + 0.005*"effective" + 0.005*"well" + 0.005*"need" + 0.005*"number" + 0.005*"good" + 0.005*"practice" + 0.004*"always"', '0.015*"’" + 0.007*"well" + 0.007*"number" + 0.006*"quality" + 0.005*"However" + 0.005*"carers" + 0.005*"plans" + 0.005*"arrangements" + 0.005*"timely" + 0.004*"health"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.007*"quality" + 0.006*"well" + 0.006*"practice" + 0.006*"number" + 0.005*"good" + 0.005*"timely" + 0.005*"However" + 0.005*"health"', '0.018*"’" + 0.007*"well" + 0.007*"number" + 0.006*"good" + 0.006*"plans" + 0.005*"effective" + 0.005*"quality" + 0.005*"needs" + 0.005*"carers" + 0.005*"always"', '0.015*"’" + 0.008*"number" + 0.008*"quality" + 0.006*"need" + 0.006*"well" + 0.005*"effective" + 0.005*"However" + 0.005*"timely" + 0.005*"good" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3238,7 +3238,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"leaders" + 0.005*"Cleveland" + 0.005*"20" + 0.005*"consistently" + 0.005*"plans" + 0.005*"2022" + 0.005*"risk" + 0.005*"Redcar" + 0.005*"However"', '0.014*"’" + 0.006*"However" + 0.006*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"Redcar" + 0.005*"consistently" + 0.005*"1" + 0.005*"carers" + 0.005*"2022"', '0.019*"’" + 0.006*"needs" + 0.006*"leaders" + 0.006*"However" + 0.005*"plans" + 0.005*"consistently" + 0.005*"practice" + 0.005*"20" + 0.004*"2022" + 0.004*"Cleveland"']</t>
+    <t>['0.018*"’" + 0.006*"leaders" + 0.006*"needs" + 0.005*"plans" + 0.005*"However" + 0.005*"practice" + 0.004*"consistently" + 0.004*"response" + 0.004*"Cleveland" + 0.004*"carers"', '0.019*"’" + 0.007*"However" + 0.007*"plans" + 0.006*"leaders" + 0.006*"2022" + 0.005*"needs" + 0.005*"consistently" + 0.005*"practice" + 0.005*"risk" + 0.004*"20"', '0.015*"’" + 0.007*"leaders" + 0.006*"consistently" + 0.006*"needs" + 0.005*"20" + 0.005*"Cleveland" + 0.005*"carers" + 0.005*"Redcar" + 0.005*"July" + 0.004*"However"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3265,7 +3265,7 @@
     <t>0.1837</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.011*"practice" + 0.011*"experienced" + 0.009*"needs" + 0.006*"response" + 0.006*"consistently" + 0.005*"plans" + 0.005*"quality" + 0.005*"good" + 0.004*"well"', '0.018*"’" + 0.009*"experienced" + 0.007*"plans" + 0.007*"response" + 0.006*"practice" + 0.006*"needs" + 0.006*"quality" + 0.005*"consistently" + 0.005*"Rochdale" + 0.005*"3"', '0.015*"’" + 0.008*"experienced" + 0.007*"needs" + 0.005*"practice" + 0.005*"good" + 0.005*"well" + 0.005*"plans" + 0.005*"PAs" + 0.005*"Rochdale" + 0.004*"23"']</t>
+    <t>['0.023*"’" + 0.008*"experienced" + 0.006*"needs" + 0.006*"practice" + 0.006*"consistently" + 0.006*"response" + 0.005*"plans" + 0.005*"23" + 0.004*"leaders" + 0.004*"good"', '0.015*"’" + 0.008*"practice" + 0.007*"experienced" + 0.006*"plans" + 0.006*"needs" + 0.005*"progress" + 0.005*"Rochdale" + 0.004*"good" + 0.004*"3" + 0.004*"experiences"', '0.022*"’" + 0.012*"experienced" + 0.009*"needs" + 0.009*"practice" + 0.007*"response" + 0.006*"quality" + 0.006*"good" + 0.006*"plans" + 0.006*"consistently" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3289,7 +3289,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"Rotherham" + 0.006*"needs" + 0.005*"good" + 0.005*"well" + 0.005*"ensure" + 0.005*"Council" + 0.005*"plans" + 0.004*"1" + 0.004*"However"', '0.014*"’" + 0.005*"Council" + 0.005*"Rotherham" + 0.005*"well" + 0.005*"needs" + 0.004*"plans" + 0.004*"July" + 0.004*"27" + 0.004*"However" + 0.004*"Metropolitan"', '0.014*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"ensure" + 0.006*"good" + 0.005*"well" + 0.005*"However" + 0.004*"clear" + 0.004*"plans" + 0.004*"quality"']</t>
+    <t>['0.012*"’" + 0.007*"Rotherham" + 0.006*"needs" + 0.005*"well" + 0.005*"ensure" + 0.004*"plans" + 0.004*"However" + 0.003*"good" + 0.003*"Borough" + 0.003*"Council"', '0.014*"’" + 0.009*"Rotherham" + 0.006*"needs" + 0.005*"good" + 0.005*"plans" + 0.005*"1" + 0.004*"27" + 0.004*"clear" + 0.004*"However" + 0.004*"June"', '0.018*"’" + 0.009*"Rotherham" + 0.007*"needs" + 0.006*"well" + 0.006*"Council" + 0.005*"ensure" + 0.005*"good" + 0.005*"However" + 0.004*"Metropolitan" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3313,7 +3313,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"well" + 0.008*"practice" + 0.006*"highly" + 0.006*"strong" + 0.005*"progress" + 0.005*"timely" + 0.004*"leaders" + 0.004*"needs" + 0.004*"effective"', '0.017*"well" + 0.012*"practice" + 0.011*"’" + 0.007*"strong" + 0.007*"highly" + 0.006*"effective" + 0.005*"needs" + 0.005*"leaders" + 0.004*"high" + 0.004*"professionals"', '0.011*"practice" + 0.011*"’" + 0.011*"well" + 0.008*"highly" + 0.007*"needs" + 0.006*"strong" + 0.005*"leaders" + 0.005*"high" + 0.005*"effective" + 0.004*"professionals"']</t>
+    <t>['0.014*"well" + 0.012*"’" + 0.010*"practice" + 0.008*"highly" + 0.007*"strong" + 0.006*"leaders" + 0.006*"high" + 0.006*"effective" + 0.006*"needs" + 0.005*"professionals"', '0.012*"’" + 0.011*"practice" + 0.010*"well" + 0.007*"strong" + 0.006*"needs" + 0.005*"highly" + 0.004*"progress" + 0.004*"effective" + 0.004*"ensure" + 0.004*"range"', '0.016*"well" + 0.011*"practice" + 0.010*"’" + 0.008*"highly" + 0.006*"effective" + 0.005*"strong" + 0.005*"effectively" + 0.005*"leaders" + 0.005*"needs" + 0.004*"professionals"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3340,7 +3340,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"needs" + 0.005*"good" + 0.005*"effective" + 0.005*"clear" + 0.005*"practice" + 0.004*"risk" + 0.004*"progress"', '0.013*"’" + 0.009*"plans" + 0.007*"needs" + 0.007*"well" + 0.005*"need" + 0.004*"good" + 0.004*"appropriate" + 0.004*"Kingston" + 0.004*"progress" + 0.004*"range"', '0.015*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"good" + 0.005*"practice" + 0.005*"effective" + 0.004*"clear" + 0.004*"supported" + 0.004*"parents"']</t>
+    <t>['0.011*"’" + 0.008*"well" + 0.006*"plans" + 0.006*"needs" + 0.004*"good" + 0.004*"parents" + 0.004*"progress" + 0.004*"effective" + 0.004*"practice" + 0.004*"supported"', '0.015*"’" + 0.009*"plans" + 0.008*"well" + 0.008*"needs" + 0.005*"effective" + 0.005*"good" + 0.005*"need" + 0.005*"practice" + 0.005*"risk" + 0.004*"appropriate"', '0.013*"’" + 0.010*"well" + 0.008*"plans" + 0.008*"needs" + 0.006*"good" + 0.005*"clear" + 0.004*"need" + 0.004*"risk" + 0.004*"effective" + 0.004*"parents"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3367,7 +3367,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.005*"quality" + 0.005*"information" + 0.004*"needs" + 0.004*"plans" + 0.004*"actions" + 0.004*"always" + 0.004*"effective" + 0.003*"use"', '0.009*"’" + 0.006*"well" + 0.005*"plans" + 0.005*"needs" + 0.004*"use" + 0.004*"benefit" + 0.004*"quality" + 0.004*"informed" + 0.004*"health" + 0.004*"effective"', '0.014*"’" + 0.005*"quality" + 0.005*"needs" + 0.005*"well" + 0.004*"plans" + 0.004*"benefit" + 0.004*"management" + 0.004*"However" + 0.004*"effective" + 0.004*"use"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.005*"quality" + 0.004*"plans" + 0.004*"benefit" + 0.004*"needs" + 0.004*"effective" + 0.004*"use" + 0.004*"timely" + 0.004*"early"', '0.014*"’" + 0.005*"well" + 0.004*"plans" + 0.004*"needs" + 0.004*"information" + 0.004*"quality" + 0.004*"use" + 0.004*"However" + 0.004*"actions" + 0.004*"management"', '0.012*"’" + 0.006*"needs" + 0.006*"well" + 0.005*"quality" + 0.004*"plans" + 0.004*"effective" + 0.004*"However" + 0.004*"information" + 0.004*"benefit" + 0.004*"informed"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3388,7 +3388,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.011*"needs" + 0.011*"well" + 0.008*"need" + 0.007*"good" + 0.007*"practice" + 0.006*"effective" + 0.006*"ensure" + 0.006*"team" + 0.005*"family"', '0.011*"’" + 0.010*"well" + 0.010*"needs" + 0.008*"good" + 0.007*"team" + 0.006*"plans" + 0.006*"need" + 0.006*"practice" + 0.005*"protection" + 0.005*"enough"', '0.012*"’" + 0.008*"well" + 0.007*"good" + 0.007*"team" + 0.006*"enough" + 0.006*"protection" + 0.006*"needs" + 0.005*"plans" + 0.005*"practice" + 0.005*"effective"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"good" + 0.007*"team" + 0.006*"practice" + 0.006*"need" + 0.005*"ensure" + 0.005*"plans" + 0.005*"enough"', '0.012*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"need" + 0.006*"effective" + 0.006*"good" + 0.006*"protection" + 0.006*"practice" + 0.005*"enough" + 0.005*"ensure"', '0.014*"’" + 0.012*"well" + 0.011*"needs" + 0.009*"good" + 0.007*"team" + 0.006*"plans" + 0.006*"need" + 0.006*"practice" + 0.006*"enough" + 0.006*"ensure"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3412,7 +3412,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"needs" + 0.007*"effective" + 0.006*"plans" + 0.005*"well" + 0.005*"Salford" + 0.005*"10" + 0.004*"quality" + 0.004*"practice" + 0.004*"planning"', '0.014*"’" + 0.009*"plans" + 0.008*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"Salford" + 0.006*"planning" + 0.005*"progress" + 0.005*"leaders" + 0.005*"practice"', '0.014*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"Salford" + 0.005*"experiences" + 0.005*"appropriate" + 0.005*"practice" + 0.005*"leaders"']</t>
+    <t>['0.009*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"Salford" + 0.005*"practice" + 0.004*"leaders" + 0.004*"6" + 0.004*"experiences"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"Salford" + 0.005*"quality" + 0.005*"ensure" + 0.005*"practice" + 0.004*"experiences" + 0.004*"effective"', '0.018*"’" + 0.008*"plans" + 0.008*"effective" + 0.008*"well" + 0.007*"needs" + 0.007*"planning" + 0.006*"Salford" + 0.005*"progress" + 0.005*"6" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3433,7 +3433,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Sandwell" + 0.005*"quality" + 0.005*"education" + 0.004*"effective" + 0.004*"good" + 0.004*"changes"', '0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"Sandwell" + 0.005*"quality" + 0.005*"plans" + 0.005*"number" + 0.004*"progress" + 0.004*"many" + 0.004*"effective"', '0.015*"’" + 0.009*"needs" + 0.009*"plans" + 0.008*"Sandwell" + 0.006*"well" + 0.006*"quality" + 0.006*"Trust" + 0.006*"20" + 0.005*"9" + 0.005*"progress"']</t>
+    <t>['0.012*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Sandwell" + 0.005*"plans" + 0.005*"number" + 0.004*"progress" + 0.004*"quality" + 0.004*"changes" + 0.004*"9"', '0.017*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"Sandwell" + 0.007*"quality" + 0.006*"well" + 0.006*"Trust" + 0.005*"20" + 0.005*"education" + 0.004*"progress"', '0.013*"’" + 0.008*"needs" + 0.008*"Sandwell" + 0.008*"plans" + 0.007*"well" + 0.005*"quality" + 0.005*"9" + 0.005*"20" + 0.004*"many" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3454,7 +3454,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"Sefton" + 0.005*"many" + 0.005*"protection" + 0.005*"including" + 0.005*"March" + 0.005*"◼" + 0.004*"21"', '0.015*"’" + 0.008*"needs" + 0.006*"practice" + 0.006*"oversight" + 0.005*"protection" + 0.005*"February" + 0.005*"4" + 0.005*"including" + 0.005*"lack" + 0.005*"need"', '0.019*"’" + 0.010*"needs" + 0.006*"oversight" + 0.006*"lack" + 0.006*"practice" + 0.005*"management" + 0.005*"many" + 0.005*"always" + 0.005*"timely" + 0.005*"including"']</t>
+    <t>['0.016*"’" + 0.010*"needs" + 0.007*"practice" + 0.006*"oversight" + 0.005*"protection" + 0.005*"March" + 0.005*"◼" + 0.005*"plans" + 0.005*"always" + 0.005*"many"', '0.015*"’" + 0.008*"needs" + 0.006*"oversight" + 0.005*"need" + 0.005*"including" + 0.005*"l" + 0.005*"lack" + 0.005*"management" + 0.005*"Sefton" + 0.005*"4"', '0.017*"’" + 0.011*"needs" + 0.007*"practice" + 0.005*"including" + 0.005*"response" + 0.005*"lack" + 0.005*"management" + 0.005*"always" + 0.005*"oversight" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3484,7 +3484,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"Sheffield" + 0.009*"needs" + 0.006*"well" + 0.006*"practice" + 0.005*"leaders" + 0.005*"11" + 0.005*"adviser" + 0.004*"quality" + 0.004*"plans"', '0.017*"’" + 0.011*"Sheffield" + 0.009*"needs" + 0.007*"well" + 0.006*"health" + 0.006*"leaders" + 0.006*"practice" + 0.005*"quality" + 0.005*"experiences" + 0.004*"protection"', '0.022*"’" + 0.012*"Sheffield" + 0.007*"needs" + 0.007*"well" + 0.006*"leaders" + 0.005*"practice" + 0.005*"health" + 0.005*"good" + 0.004*"plans" + 0.004*"effective"']</t>
+    <t>['0.027*"’" + 0.012*"Sheffield" + 0.011*"needs" + 0.007*"well" + 0.007*"health" + 0.006*"leaders" + 0.006*"practice" + 0.005*"quality" + 0.005*"22" + 0.005*"plans"', '0.011*"’" + 0.010*"Sheffield" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.005*"practice" + 0.004*"adviser" + 0.004*"receive" + 0.004*"effective" + 0.004*"experiences"', '0.019*"’" + 0.010*"Sheffield" + 0.007*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"leaders" + 0.005*"11" + 0.005*"health" + 0.005*"good" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3511,7 +3511,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"needs" + 0.006*"Shropshire" + 0.004*"progress" + 0.004*"making" + 0.004*"well" + 0.004*"2022" + 0.004*"plans" + 0.004*"leaders" + 0.004*"practice"', '0.016*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Shropshire" + 0.006*"plans" + 0.006*"progress" + 0.006*"11" + 0.005*"2022" + 0.005*"making" + 0.005*"training"', '0.024*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.006*"progress" + 0.005*"7" + 0.005*"plans" + 0.005*"making" + 0.005*"2022" + 0.004*"education"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.007*"Shropshire" + 0.006*"2022" + 0.006*"plans" + 0.005*"7" + 0.005*"well" + 0.005*"progress" + 0.005*"training" + 0.004*"practice"', '0.015*"’" + 0.008*"needs" + 0.007*"Shropshire" + 0.007*"well" + 0.006*"making" + 0.006*"progress" + 0.006*"plans" + 0.005*"11" + 0.005*"leaders" + 0.005*"effectively"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Shropshire" + 0.006*"progress" + 0.005*"making" + 0.004*"plans" + 0.004*"2022" + 0.004*"effective" + 0.004*"7"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3532,7 +3532,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"Slough" + 0.007*"plans" + 0.007*"quality" + 0.006*"practice" + 0.006*"3" + 0.006*"needs" + 0.005*"leaders" + 0.005*"senior" + 0.005*"impact"', '0.007*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"quality" + 0.005*"practice" + 0.004*"Slough" + 0.004*"timely" + 0.004*"However" + 0.004*"impact" + 0.003*"23"', '0.021*"’" + 0.008*"Slough" + 0.007*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"practice" + 0.005*"impact" + 0.005*"plans" + 0.005*"supported" + 0.005*"leaders"']</t>
+    <t>['0.012*"’" + 0.008*"Slough" + 0.006*"plans" + 0.005*"practice" + 0.004*"impact" + 0.004*"However" + 0.004*"February" + 0.004*"need" + 0.004*"PAs" + 0.004*"2023"', '0.018*"’" + 0.008*"needs" + 0.008*"Slough" + 0.007*"plans" + 0.007*"quality" + 0.006*"practice" + 0.005*"3" + 0.005*"leaders" + 0.005*"However" + 0.005*"timely"', '0.016*"’" + 0.008*"Slough" + 0.006*"quality" + 0.006*"needs" + 0.005*"practice" + 0.005*"impact" + 0.005*"leaders" + 0.005*"supported" + 0.005*"plans" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3553,7 +3553,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"2022" + 0.007*"lack" + 0.006*"need" + 0.006*"effective" + 0.006*"experiences" + 0.005*"risk" + 0.005*"Solihull" + 0.005*"means" + 0.005*"practice"', '0.017*"’" + 0.011*"lack" + 0.008*"2022" + 0.006*"need" + 0.006*"quality" + 0.006*"Solihull" + 0.006*"practice" + 0.005*"risk" + 0.005*"experiences" + 0.005*"significant"', '0.014*"’" + 0.013*"lack" + 0.009*"2022" + 0.007*"Solihull" + 0.006*"risk" + 0.006*"need" + 0.006*"quality" + 0.005*"significant" + 0.005*"delay" + 0.005*"timely"']</t>
+    <t>['0.015*"’" + 0.010*"lack" + 0.006*"practice" + 0.006*"risk" + 0.005*"2022" + 0.005*"experiences" + 0.005*"need" + 0.005*"significant" + 0.005*"11" + 0.005*"means"', '0.015*"’" + 0.012*"lack" + 0.009*"2022" + 0.007*"need" + 0.006*"quality" + 0.006*"Solihull" + 0.005*"progress" + 0.005*"experiences" + 0.005*"risk" + 0.005*"delay"', '0.016*"’" + 0.010*"lack" + 0.009*"2022" + 0.008*"Solihull" + 0.006*"risk" + 0.006*"need" + 0.006*"effective" + 0.005*"quality" + 0.005*"practice" + 0.005*"significant"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3574,7 +3574,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"need" + 0.005*"understand" + 0.005*"Somerset" + 0.005*"leaders" + 0.004*"practice" + 0.004*"supported"', '0.020*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"Somerset" + 0.007*"good" + 0.006*"progress" + 0.006*"plans" + 0.005*"including" + 0.005*"number" + 0.005*"positive"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Somerset" + 0.007*"plans" + 0.006*"leaders" + 0.005*"supported" + 0.005*"practice" + 0.005*"family" + 0.004*"good"']</t>
+    <t>['0.018*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"number" + 0.006*"plans" + 0.006*"Somerset" + 0.005*"effective" + 0.005*"good" + 0.005*"progress" + 0.005*"supported"', '0.016*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"Somerset" + 0.007*"good" + 0.006*"practice" + 0.006*"supported" + 0.006*"plans" + 0.005*"leaders" + 0.005*"progress"', '0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.006*"Somerset" + 0.006*"plans" + 0.006*"need" + 0.006*"leaders" + 0.005*"good" + 0.005*"including" + 0.005*"understand"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3595,7 +3595,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.012*"well" + 0.012*"quality" + 0.010*"leaders" + 0.009*"plans" + 0.009*"’" + 0.007*"good" + 0.006*"timely" + 0.005*"needs" + 0.005*"progress" + 0.005*"always"', '0.010*"quality" + 0.009*"well" + 0.008*"’" + 0.008*"leaders" + 0.007*"plans" + 0.007*"good" + 0.005*"needs" + 0.005*"timely" + 0.005*"practice" + 0.005*"Senior"', '0.010*"well" + 0.009*"’" + 0.008*"quality" + 0.007*"good" + 0.007*"timely" + 0.007*"leaders" + 0.006*"progress" + 0.006*"plans" + 0.006*"needs" + 0.005*"◼"']</t>
+    <t>['0.012*"quality" + 0.012*"well" + 0.008*"’" + 0.008*"plans" + 0.008*"leaders" + 0.007*"timely" + 0.006*"progress" + 0.006*"needs" + 0.006*"good" + 0.005*"always"', '0.011*"well" + 0.011*"quality" + 0.010*"’" + 0.009*"leaders" + 0.008*"good" + 0.008*"plans" + 0.006*"needs" + 0.006*"timely" + 0.005*"progress" + 0.005*"◼"', '0.008*"well" + 0.007*"leaders" + 0.006*"’" + 0.006*"plans" + 0.005*"quality" + 0.005*"good" + 0.005*"practice" + 0.005*"timely" + 0.004*"needs" + 0.004*"timeliness"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -3625,7 +3625,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.009*"needs" + 0.008*"South" + 0.006*"However" + 0.006*"oversight" + 0.005*"effective" + 0.005*"Tyneside" + 0.005*"carers" + 0.005*"9" + 0.005*"February"', '0.026*"’" + 0.009*"Tyneside" + 0.008*"South" + 0.008*"needs" + 0.005*"management" + 0.005*"2022" + 0.005*"However" + 0.005*"effective" + 0.005*"homes" + 0.005*"2023"', '0.023*"’" + 0.010*"needs" + 0.007*"Tyneside" + 0.006*"South" + 0.006*"oversight" + 0.005*"14" + 0.005*"5" + 0.005*"carers" + 0.005*"risk" + 0.004*"9"']</t>
+    <t>['0.027*"’" + 0.010*"needs" + 0.008*"Tyneside" + 0.007*"South" + 0.006*"However" + 0.005*"5" + 0.005*"management" + 0.005*"carers" + 0.005*"oversight" + 0.005*"14"', '0.017*"’" + 0.006*"needs" + 0.006*"South" + 0.005*"Tyneside" + 0.005*"oversight" + 0.005*"management" + 0.005*"However" + 0.005*"effective" + 0.004*"2022" + 0.004*"practice"', '0.026*"’" + 0.010*"needs" + 0.008*"South" + 0.008*"Tyneside" + 0.006*"effective" + 0.005*"oversight" + 0.005*"carers" + 0.005*"9" + 0.005*"practice" + 0.005*"December"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -3652,7 +3652,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"improve" + 0.006*"Southampton" + 0.005*"progress" + 0.005*"plans" + 0.005*"June" + 0.005*"5" + 0.004*"provide" + 0.004*"2023" + 0.004*"experiences"', '0.021*"’" + 0.006*"plans" + 0.005*"Southampton" + 0.005*"needs" + 0.005*"including" + 0.005*"16" + 0.004*"timely" + 0.004*"experiences" + 0.004*"well" + 0.004*"2023"', '0.013*"’" + 0.006*"plans" + 0.005*"progress" + 0.005*"5" + 0.005*"Southampton" + 0.004*"experiences" + 0.004*"improve" + 0.004*"timely" + 0.004*"including" + 0.004*"needs"']</t>
+    <t>['0.014*"’" + 0.005*"Southampton" + 0.005*"improve" + 0.005*"plans" + 0.004*"including" + 0.004*"experiences" + 0.004*"progress" + 0.004*"timely" + 0.004*"16" + 0.004*"make"', '0.014*"’" + 0.005*"progress" + 0.005*"plans" + 0.005*"Southampton" + 0.004*"experiences" + 0.004*"provide" + 0.004*"improve" + 0.004*"5" + 0.004*"good" + 0.004*"2023"', '0.019*"’" + 0.007*"plans" + 0.006*"Southampton" + 0.005*"needs" + 0.005*"5" + 0.005*"16" + 0.005*"including" + 0.005*"progress" + 0.004*"improve" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -3682,7 +3682,7 @@
     <t>to requires improvement</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"planning" + 0.007*"practice" + 0.006*"leaders" + 0.006*"number" + 0.006*"quality" + 0.005*"within" + 0.005*"effective" + 0.005*"carers" + 0.005*"protection"', '0.013*"’" + 0.009*"planning" + 0.006*"practice" + 0.006*"protection" + 0.006*"quality" + 0.006*"leaders" + 0.005*"within" + 0.005*"good" + 0.005*"always" + 0.005*"needs"', '0.014*"’" + 0.008*"quality" + 0.007*"planning" + 0.007*"practice" + 0.006*"need" + 0.006*"leaders" + 0.005*"always" + 0.005*"effective" + 0.005*"number" + 0.005*"risk"']</t>
+    <t>['0.014*"’" + 0.007*"planning" + 0.006*"quality" + 0.005*"practice" + 0.005*"number" + 0.005*"protection" + 0.005*"Southend" + 0.005*"always" + 0.005*"effective" + 0.005*"leaders"', '0.012*"’" + 0.010*"planning" + 0.008*"leaders" + 0.008*"quality" + 0.007*"practice" + 0.005*"within" + 0.005*"effective" + 0.005*"number" + 0.005*"carers" + 0.005*"needs"', '0.014*"’" + 0.007*"practice" + 0.007*"planning" + 0.006*"need" + 0.006*"always" + 0.006*"quality" + 0.006*"protection" + 0.005*"However" + 0.005*"well" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -3700,7 +3700,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"St" + 0.008*"Helens" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"progress" + 0.005*"receive" + 0.005*"risk" + 0.005*"10"', '0.013*"’" + 0.008*"needs" + 0.007*"St" + 0.007*"Helens" + 0.006*"well" + 0.006*"need" + 0.006*"10" + 0.006*"progress" + 0.006*"21" + 0.005*"receive"', '0.016*"’" + 0.008*"Helens" + 0.006*"St" + 0.006*"well" + 0.005*"progress" + 0.005*"effective" + 0.005*"risk" + 0.005*"needs" + 0.005*"21" + 0.004*"receive"']</t>
+    <t>['0.010*"’" + 0.008*"Helens" + 0.007*"St" + 0.007*"well" + 0.007*"needs" + 0.005*"good" + 0.005*"need" + 0.005*"receive" + 0.005*"21" + 0.004*"10"', '0.017*"’" + 0.008*"needs" + 0.008*"St" + 0.007*"progress" + 0.007*"Helens" + 0.007*"well" + 0.006*"10" + 0.006*"risk" + 0.006*"good" + 0.005*"need"', '0.019*"’" + 0.008*"Helens" + 0.008*"St" + 0.005*"well" + 0.005*"21" + 0.005*"receive" + 0.005*"needs" + 0.005*"progress" + 0.005*"risk" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -3721,7 +3721,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"needs" + 0.007*"progress" + 0.006*"practice" + 0.006*"ensure" + 0.005*"quality" + 0.005*"oversight" + 0.005*"health" + 0.005*"6" + 0.005*"2023"', '0.014*"’" + 0.012*"needs" + 0.006*"health" + 0.006*"quality" + 0.006*"practice" + 0.006*"Staffordshire" + 0.006*"oversight" + 0.005*"plans" + 0.005*"ensure" + 0.005*"progress"', '0.017*"’" + 0.012*"needs" + 0.006*"quality" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.005*"ensure" + 0.005*"10" + 0.005*"impact" + 0.005*"progress" + 0.005*"health"']</t>
+    <t>['0.015*"’" + 0.013*"needs" + 0.006*"quality" + 0.006*"progress" + 0.006*"oversight" + 0.006*"health" + 0.005*"plans" + 0.005*"ensure" + 0.005*"10" + 0.005*"Council"', '0.013*"’" + 0.009*"needs" + 0.006*"quality" + 0.005*"ensure" + 0.005*"Staffordshire" + 0.005*"practice" + 0.005*"progress" + 0.004*"plans" + 0.004*"health" + 0.004*"oversight"', '0.021*"’" + 0.012*"needs" + 0.007*"practice" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.006*"progress" + 0.006*"health" + 0.006*"ensure" + 0.006*"quality" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -3745,7 +3745,7 @@
     <t>18/05/22</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"practice" + 0.007*"needs" + 0.007*"well" + 0.006*"Stockport" + 0.005*"strong" + 0.005*"risk" + 0.005*"quality" + 0.004*"ensure" + 0.004*"plans"', '0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.006*"risk" + 0.005*"Stockport" + 0.005*"needs" + 0.004*"team" + 0.004*"range" + 0.004*"ensure" + 0.004*"strong"', '0.012*"’" + 0.008*"well" + 0.008*"Stockport" + 0.007*"practice" + 0.007*"plans" + 0.006*"strong" + 0.006*"needs" + 0.005*"28" + 0.005*"ensure" + 0.005*"March"']</t>
+    <t>['0.009*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"Stockport" + 0.005*"needs" + 0.005*"leaders" + 0.005*"strong" + 0.004*"risk" + 0.004*"28" + 0.003*"response"', '0.013*"’" + 0.010*"well" + 0.008*"practice" + 0.008*"Stockport" + 0.006*"needs" + 0.006*"plans" + 0.005*"strong" + 0.005*"risk" + 0.005*"ensure" + 0.005*"28"', '0.010*"’" + 0.007*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"strong" + 0.006*"Stockport" + 0.006*"plans" + 0.005*"ensure" + 0.005*"risk" + 0.005*"range"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -3778,7 +3778,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.010*"leaders" + 0.009*"plans" + 0.007*"well" + 0.007*"on-Tees" + 0.007*"needs" + 0.006*"Stockton" + 0.006*"quality" + 0.006*"17" + 0.005*"senior"', '0.012*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"Stockton" + 0.005*"good" + 0.005*"quality" + 0.004*"on-Tees" + 0.004*"progress"', '0.017*"’" + 0.008*"plans" + 0.007*"leaders" + 0.007*"needs" + 0.007*"quality" + 0.006*"Stockton" + 0.006*"good" + 0.006*"on-Tees" + 0.006*"well" + 0.005*"carers"']</t>
+    <t>['0.021*"’" + 0.010*"leaders" + 0.007*"well" + 0.007*"plans" + 0.005*"on-Tees" + 0.005*"good" + 0.005*"needs" + 0.005*"Stockton" + 0.004*"senior" + 0.004*"quality"', '0.022*"’" + 0.009*"plans" + 0.008*"needs" + 0.008*"leaders" + 0.007*"well" + 0.007*"on-Tees" + 0.006*"good" + 0.006*"Stockton" + 0.006*"quality" + 0.006*"17"', '0.013*"’" + 0.008*"plans" + 0.008*"leaders" + 0.007*"quality" + 0.006*"Stockton" + 0.005*"needs" + 0.005*"on-Tees" + 0.004*"well" + 0.004*"senior" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -3799,7 +3799,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"needs" + 0.008*"on-Trent" + 0.008*"well" + 0.007*"plans" + 0.007*"However" + 0.007*"Stoke" + 0.006*"ensure" + 0.005*"protection" + 0.005*"quality"', '0.019*"’" + 0.007*"needs" + 0.007*"Stoke" + 0.007*"ensure" + 0.007*"However" + 0.007*"well" + 0.006*"on-Trent" + 0.006*"protection" + 0.006*"plans" + 0.005*"progress"', '0.013*"’" + 0.008*"needs" + 0.006*"Stoke" + 0.006*"on-Trent" + 0.006*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"protection" + 0.005*"However" + 0.004*"leaders"']</t>
+    <t>['0.021*"’" + 0.009*"needs" + 0.008*"However" + 0.008*"plans" + 0.007*"Stoke" + 0.007*"on-Trent" + 0.007*"well" + 0.006*"ensure" + 0.006*"protection" + 0.005*"quality"', '0.015*"’" + 0.008*"needs" + 0.007*"on-Trent" + 0.007*"well" + 0.006*"Stoke" + 0.006*"protection" + 0.005*"ensure" + 0.005*"effectively" + 0.005*"progress" + 0.005*"However"', '0.013*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Stoke" + 0.006*"on-Trent" + 0.005*"However" + 0.005*"14" + 0.005*"progress" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -3826,7 +3826,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.007*"progress" + 0.007*"well" + 0.005*"effective" + 0.005*"good" + 0.005*"ensure" + 0.005*"leaders" + 0.004*"practice" + 0.004*"needs" + 0.004*"risk"', '0.017*"’" + 0.005*"effective" + 0.005*"leaders" + 0.005*"well" + 0.004*"ensure" + 0.004*"carers" + 0.004*"progress" + 0.004*"good" + 0.003*"high" + 0.003*"use"', '0.014*"’" + 0.007*"well" + 0.007*"progress" + 0.005*"good" + 0.005*"practice" + 0.004*"leaders" + 0.004*"ensure" + 0.004*"effective" + 0.004*"high" + 0.004*"Suffolk"']</t>
+    <t>['0.014*"’" + 0.007*"well" + 0.006*"progress" + 0.005*"leaders" + 0.005*"effective" + 0.005*"carers" + 0.005*"good" + 0.004*"need" + 0.004*"ensure" + 0.004*"needs"', '0.013*"’" + 0.006*"well" + 0.006*"progress" + 0.005*"effective" + 0.005*"ensure" + 0.004*"practice" + 0.004*"leaders" + 0.004*"good" + 0.004*"high" + 0.004*"Suffolk"', '0.012*"’" + 0.006*"well" + 0.006*"progress" + 0.005*"good" + 0.005*"effective" + 0.004*"practice" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"needs" + 0.003*"risk"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -3856,7 +3856,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"Sunderland" + 0.005*"TfC" + 0.004*"experienced" + 0.004*"risk" + 0.004*"need" + 0.004*"council"', '0.015*"’" + 0.008*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"Sunderland" + 0.005*"highly" + 0.005*"practice" + 0.005*"robust" + 0.004*"experienced" + 0.004*"protection"', '0.019*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"experienced" + 0.005*"well" + 0.005*"Sunderland" + 0.005*"good" + 0.005*"practice" + 0.005*"council" + 0.005*"protection"']</t>
+    <t>['0.013*"’" + 0.008*"Sunderland" + 0.007*"well" + 0.006*"needs" + 0.006*"quality" + 0.005*"council" + 0.005*"TfC" + 0.004*"experienced" + 0.004*"highly" + 0.004*"training"', '0.020*"’" + 0.008*"quality" + 0.007*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"Sunderland" + 0.005*"protection" + 0.005*"council" + 0.005*"good" + 0.005*"experienced"', '0.014*"’" + 0.007*"needs" + 0.007*"well" + 0.005*"quality" + 0.005*"experienced" + 0.005*"Sunderland" + 0.005*"parents" + 0.005*"TfC" + 0.004*"result" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -3883,7 +3883,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.012*"needs" + 0.010*"well" + 0.007*"practice" + 0.006*"progress" + 0.006*"17" + 0.005*"good" + 0.005*"quality" + 0.005*"plans" + 0.005*"carers"', '0.014*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"progress" + 0.006*"practice" + 0.005*"plans" + 0.005*"carers" + 0.005*"quality" + 0.005*"However" + 0.005*"effective"', '0.015*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"practice" + 0.006*"progress" + 0.006*"effective" + 0.005*"plans" + 0.005*"17" + 0.004*"good" + 0.004*"carers"']</t>
+    <t>['0.015*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"practice" + 0.006*"progress" + 0.006*"carers" + 0.005*"quality" + 0.005*"17" + 0.005*"good" + 0.005*"plans"', '0.015*"’" + 0.010*"needs" + 0.009*"well" + 0.008*"practice" + 0.007*"progress" + 0.005*"quality" + 0.005*"effective" + 0.005*"plans" + 0.005*"carers" + 0.005*"17"', '0.011*"’" + 0.010*"needs" + 0.009*"well" + 0.006*"plans" + 0.006*"practice" + 0.006*"good" + 0.005*"progress" + 0.005*"effective" + 0.005*"However" + 0.005*"17"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -3904,7 +3904,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.016*"needs" + 0.011*"Swindon" + 0.010*"well" + 0.009*"need" + 0.008*"plans" + 0.006*"always" + 0.006*"impact" + 0.006*"effective" + 0.005*"education"', '0.020*"’" + 0.010*"needs" + 0.008*"need" + 0.007*"Swindon" + 0.006*"health" + 0.006*"always" + 0.005*"well" + 0.005*"impact" + 0.005*"effective" + 0.005*"many"', '0.015*"’" + 0.008*"needs" + 0.008*"need" + 0.007*"always" + 0.006*"well" + 0.006*"Swindon" + 0.005*"clear" + 0.004*"home" + 0.004*"28" + 0.004*"health"']</t>
+    <t>['0.018*"’" + 0.012*"needs" + 0.008*"Swindon" + 0.007*"need" + 0.007*"well" + 0.007*"plans" + 0.006*"always" + 0.006*"impact" + 0.005*"Council" + 0.005*"many"', '0.023*"’" + 0.012*"needs" + 0.009*"Swindon" + 0.008*"well" + 0.008*"need" + 0.007*"always" + 0.006*"plans" + 0.005*"education" + 0.005*"impact" + 0.005*"effective"', '0.024*"’" + 0.014*"needs" + 0.009*"Swindon" + 0.009*"need" + 0.008*"well" + 0.006*"always" + 0.006*"plans" + 0.006*"health" + 0.006*"However" + 0.005*"lack"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -3925,7 +3925,7 @@
     <t>0.1619</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"plans" + 0.006*"impact" + 0.006*"always" + 0.006*"practice" + 0.006*"progress" + 0.005*"good" + 0.005*"well" + 0.005*"example" + 0.005*"needs"', '0.014*"’" + 0.006*"plans" + 0.006*"well" + 0.006*"progress" + 0.006*"impact" + 0.006*"always" + 0.005*"practice" + 0.005*"good" + 0.005*"need" + 0.005*"new"', '0.016*"’" + 0.007*"impact" + 0.007*"plans" + 0.007*"always" + 0.006*"good" + 0.006*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"needs" + 0.004*"However"']</t>
+    <t>['0.018*"’" + 0.008*"plans" + 0.006*"progress" + 0.006*"well" + 0.006*"practice" + 0.006*"always" + 0.006*"impact" + 0.005*"good" + 0.005*"need" + 0.005*"risk"', '0.012*"’" + 0.006*"always" + 0.005*"impact" + 0.005*"plans" + 0.005*"good" + 0.005*"progress" + 0.004*"quality" + 0.004*"well" + 0.004*"practice" + 0.004*"consistently"', '0.015*"’" + 0.008*"impact" + 0.007*"plans" + 0.006*"always" + 0.006*"good" + 0.006*"practice" + 0.006*"well" + 0.005*"progress" + 0.005*"needs" + 0.004*"example"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -3946,7 +3946,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"effective" + 0.005*"ensure" + 0.005*"need" + 0.005*"strong" + 0.005*"plans" + 0.005*"practice" + 0.005*"planning"', '0.012*"’" + 0.010*"well" + 0.007*"effective" + 0.006*"needs" + 0.005*"plans" + 0.005*"strong" + 0.005*"improve" + 0.005*"practice" + 0.004*"leaders" + 0.004*"planning"', '0.015*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"ensure" + 0.005*"strong" + 0.004*"clear" + 0.004*"practice"']</t>
+    <t>['0.013*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"effective" + 0.005*"need" + 0.005*"practice" + 0.005*"strong" + 0.004*"benefit" + 0.004*"plans" + 0.004*"improve"', '0.020*"’" + 0.011*"well" + 0.008*"needs" + 0.008*"effective" + 0.006*"ensure" + 0.006*"planning" + 0.006*"plans" + 0.005*"need" + 0.005*"strong" + 0.005*"timely"', '0.013*"’" + 0.011*"well" + 0.006*"plans" + 0.006*"needs" + 0.006*"effective" + 0.005*"strong" + 0.005*"clear" + 0.004*"practice" + 0.004*"highly" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -3967,7 +3967,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"well" + 0.005*"carers" + 0.004*"need" + 0.004*"plans" + 0.004*"ensure" + 0.004*"practice" + 0.004*"needs" + 0.004*"leaders" + 0.004*"Thurrock"', '0.015*"’" + 0.007*"well" + 0.005*"carers" + 0.005*"need" + 0.005*"needs" + 0.004*"effective" + 0.004*"ensure" + 0.004*"Thurrock" + 0.004*"practice" + 0.004*"leaders"', '0.011*"’" + 0.006*"well" + 0.006*"carers" + 0.005*"need" + 0.004*"needs" + 0.004*"protection" + 0.004*"practice" + 0.004*"ensure" + 0.004*"quality" + 0.004*"Thurrock"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.006*"carers" + 0.004*"need" + 0.004*"leaders" + 0.004*"Thurrock" + 0.004*"protection" + 0.004*"needs" + 0.003*"ensure" + 0.003*"effective"', '0.011*"’" + 0.008*"well" + 0.005*"carers" + 0.005*"need" + 0.005*"needs" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"impact" + 0.004*"effective" + 0.004*"Thurrock"', '0.013*"’" + 0.009*"well" + 0.006*"carers" + 0.005*"practice" + 0.005*"need" + 0.004*"needs" + 0.004*"ensure" + 0.004*"effective" + 0.004*"parents" + 0.004*"vulnerable"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -3988,7 +3988,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.009*"Torbay" + 0.007*"needs" + 0.006*"good" + 0.005*"effective" + 0.004*"team" + 0.004*"agencies" + 0.004*"supported" + 0.004*"21"', '0.020*"’" + 0.009*"well" + 0.007*"Torbay" + 0.006*"effective" + 0.006*"good" + 0.005*"needs" + 0.005*"team" + 0.005*"progress" + 0.005*"plans" + 0.004*"timely"', '0.013*"’" + 0.008*"well" + 0.005*"good" + 0.005*"needs" + 0.005*"Torbay" + 0.005*"timely" + 0.005*"21" + 0.004*"agencies" + 0.004*"quality" + 0.004*"2022"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.007*"Torbay" + 0.006*"needs" + 0.006*"effective" + 0.005*"good" + 0.005*"21" + 0.004*"education" + 0.004*"agencies" + 0.004*"1"', '0.015*"’" + 0.008*"well" + 0.008*"Torbay" + 0.005*"good" + 0.005*"needs" + 0.004*"progress" + 0.004*"quality" + 0.004*"timely" + 0.004*"effective" + 0.004*"2022"', '0.018*"’" + 0.010*"well" + 0.007*"Torbay" + 0.007*"good" + 0.006*"needs" + 0.005*"plans" + 0.005*"effective" + 0.004*"team" + 0.004*"2022" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4009,7 +4009,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"needs" + 0.009*"Trafford" + 0.009*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"leaders" + 0.006*"impact" + 0.005*"placed" + 0.005*"practice"', '0.017*"’" + 0.009*"needs" + 0.007*"Trafford" + 0.007*"quality" + 0.007*"plans" + 0.006*"practice" + 0.006*"leaders" + 0.005*"well" + 0.005*"worker" + 0.005*"impact"', '0.015*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Trafford" + 0.006*"plans" + 0.006*"quality" + 0.005*"leaders" + 0.005*"2" + 0.004*"21" + 0.004*"practice"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"Trafford" + 0.007*"quality" + 0.006*"plans" + 0.006*"leaders" + 0.005*"placed" + 0.005*"practice" + 0.005*"impact"', '0.014*"’" + 0.009*"Trafford" + 0.009*"needs" + 0.007*"well" + 0.006*"quality" + 0.005*"impact" + 0.005*"worker" + 0.005*"plans" + 0.005*"leaders" + 0.004*"practice"', '0.018*"’" + 0.010*"needs" + 0.009*"plans" + 0.007*"Trafford" + 0.007*"well" + 0.006*"quality" + 0.006*"practice" + 0.006*"leaders" + 0.005*"team" + 0.005*"21"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4027,7 +4027,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50172854</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"leaders" + 0.006*"well" + 0.006*"needs" + 0.005*"oversight" + 0.005*"Senior" + 0.004*"4" + 0.004*"information" + 0.004*"Walsall" + 0.004*"15"', '0.020*"’" + 0.006*"needs" + 0.005*"leaders" + 0.005*"well" + 0.005*"Walsall" + 0.004*"4" + 0.004*"good" + 0.004*"2021" + 0.004*"positive" + 0.004*"information"', '0.024*"’" + 0.009*"leaders" + 0.007*"Walsall" + 0.006*"needs" + 0.005*"well" + 0.005*"information" + 0.005*"4" + 0.005*"progress" + 0.004*"good" + 0.004*"Senior"']</t>
+    <t>['0.024*"’" + 0.008*"leaders" + 0.006*"Walsall" + 0.006*"needs" + 0.006*"well" + 0.005*"Senior" + 0.005*"4" + 0.005*"information" + 0.005*"oversight" + 0.005*"plans"', '0.018*"’" + 0.008*"needs" + 0.007*"leaders" + 0.006*"well" + 0.004*"Walsall" + 0.004*"4" + 0.004*"oversight" + 0.004*"good" + 0.004*"risk" + 0.004*"Senior"', '0.020*"’" + 0.006*"leaders" + 0.005*"needs" + 0.005*"Walsall" + 0.005*"well" + 0.005*"information" + 0.004*"4" + 0.004*"positive" + 0.004*"oversight" + 0.004*"Senior"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4045,7 +4045,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50101635</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"well" + 0.007*"practice" + 0.006*"number" + 0.005*"plans" + 0.005*"Senior" + 0.005*"progress" + 0.004*"provided" + 0.004*"information" + 0.004*"need"', '0.011*"’" + 0.007*"practice" + 0.007*"well" + 0.004*"home" + 0.004*"senior" + 0.004*"plans" + 0.004*"good" + 0.004*"progress" + 0.004*"information" + 0.004*"carers"', '0.016*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"Senior" + 0.005*"good" + 0.004*"small" + 0.004*"number" + 0.004*"plans" + 0.003*"need" + 0.003*"needs"']</t>
+    <t>['0.016*"’" + 0.006*"practice" + 0.005*"well" + 0.005*"Senior" + 0.004*"need" + 0.004*"plans" + 0.004*"home" + 0.004*"information" + 0.004*"number" + 0.004*"good"', '0.015*"’" + 0.008*"well" + 0.006*"practice" + 0.005*"number" + 0.004*"plans" + 0.004*"carers" + 0.004*"Senior" + 0.004*"progress" + 0.004*"good" + 0.004*"needs"', '0.011*"’" + 0.007*"practice" + 0.006*"well" + 0.004*"progress" + 0.004*"number" + 0.004*"plans" + 0.004*"Senior" + 0.004*"information" + 0.004*"needs" + 0.003*"carers"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4069,7 +4069,7 @@
     <t>03/12/2021</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.005*"Warwickshire" + 0.005*"plans" + 0.005*"carers" + 0.005*"22" + 0.004*"good" + 0.004*"3"', '0.011*"’" + 0.008*"plans" + 0.007*"Warwickshire" + 0.007*"well" + 0.006*"needs" + 0.005*"clear" + 0.004*"Senior" + 0.004*"information" + 0.004*"progress" + 0.004*"3"', '0.008*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.005*"practice" + 0.005*"good" + 0.005*"carers" + 0.005*"supported" + 0.004*"progress" + 0.004*"Warwickshire"']</t>
+    <t>['0.013*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"Warwickshire" + 0.006*"well" + 0.006*"good" + 0.005*"clear" + 0.005*"practice" + 0.004*"November" + 0.004*"3"', '0.010*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"plans" + 0.005*"carers" + 0.005*"benefit" + 0.005*"Warwickshire" + 0.004*"supported" + 0.004*"progress"', '0.011*"’" + 0.006*"needs" + 0.005*"Warwickshire" + 0.005*"well" + 0.005*"plans" + 0.004*"carers" + 0.004*"practice" + 0.004*"information" + 0.004*"effective" + 0.004*"December"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4096,7 +4096,7 @@
     <t>0.1667</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"Berkshire" + 0.005*"West" + 0.005*"well" + 0.005*"need" + 0.004*"18" + 0.004*"plans" + 0.003*"needs" + 0.003*"early" + 0.003*"14"', '0.013*"’" + 0.007*"West" + 0.006*"well" + 0.006*"Berkshire" + 0.005*"14" + 0.004*"needs" + 0.004*"working" + 0.004*"agency" + 0.004*"early" + 0.004*"plans"', '0.017*"’" + 0.007*"Berkshire" + 0.006*"West" + 0.006*"well" + 0.004*"plans" + 0.004*"needs" + 0.004*"practice" + 0.004*"working" + 0.004*"18" + 0.004*"agency"']</t>
+    <t>['0.012*"’" + 0.006*"well" + 0.005*"West" + 0.005*"plans" + 0.004*"18" + 0.004*"14" + 0.004*"Berkshire" + 0.004*"needs" + 0.003*"agency" + 0.003*"working"', '0.013*"’" + 0.008*"Berkshire" + 0.007*"West" + 0.007*"well" + 0.005*"need" + 0.005*"early" + 0.004*"needs" + 0.004*"education" + 0.004*"plans" + 0.004*"14"', '0.017*"’" + 0.006*"West" + 0.006*"Berkshire" + 0.005*"well" + 0.004*"agency" + 0.004*"March" + 0.004*"needs" + 0.004*"working" + 0.004*"need" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>941</t>
@@ -4114,7 +4114,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"West" + 0.006*"needs" + 0.005*"NCT" + 0.005*"practice" + 0.004*"plans" + 0.004*"October"', '0.015*"’" + 0.007*"West" + 0.007*"Northamptonshire" + 0.006*"well" + 0.006*"quality" + 0.005*"practice" + 0.005*"NCT" + 0.004*"needs" + 0.004*"place" + 0.004*"experiences"', '0.019*"’" + 0.010*"Northamptonshire" + 0.007*"quality" + 0.006*"West" + 0.006*"practice" + 0.005*"impact" + 0.005*"3" + 0.005*"plans" + 0.005*"well" + 0.004*"needs"']</t>
+    <t>['0.021*"’" + 0.008*"Northamptonshire" + 0.007*"quality" + 0.006*"practice" + 0.006*"West" + 0.006*"well" + 0.006*"needs" + 0.005*"impact" + 0.005*"3" + 0.005*"NCT"', '0.017*"’" + 0.007*"Northamptonshire" + 0.007*"well" + 0.007*"West" + 0.006*"quality" + 0.005*"needs" + 0.005*"practice" + 0.005*"plans" + 0.005*"NCT" + 0.004*"need"', '0.013*"’" + 0.008*"Northamptonshire" + 0.007*"quality" + 0.007*"West" + 0.005*"well" + 0.004*"2022" + 0.004*"impact" + 0.004*"practice" + 0.004*"14" + 0.004*"NCT"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4135,7 +4135,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"13" + 0.005*"West" + 0.005*"Sussex" + 0.004*"number" + 0.004*"health"', '0.017*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"supported" + 0.005*"West" + 0.005*"quality" + 0.005*"number" + 0.004*"actively"', '0.011*"’" + 0.006*"plans" + 0.005*"well" + 0.005*"health" + 0.005*"West" + 0.005*"13" + 0.005*"needs" + 0.005*"Sussex" + 0.004*"March" + 0.004*"clear"']</t>
+    <t>['0.018*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"well" + 0.006*"West" + 0.005*"Sussex" + 0.005*"13" + 0.005*"supported" + 0.005*"number" + 0.005*"quality"', '0.010*"’" + 0.006*"well" + 0.005*"Sussex" + 0.005*"plans" + 0.005*"West" + 0.004*"13" + 0.004*"quality" + 0.004*"needs" + 0.004*"supported" + 0.004*"advis"', '0.012*"’" + 0.006*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"practice" + 0.004*"number" + 0.004*"impact" + 0.004*"good" + 0.004*"health" + 0.004*"planning"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4153,7 +4153,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.005*"Wigan" + 0.005*"needs" + 0.005*"quality" + 0.005*"plans" + 0.005*"May" + 0.004*"leaders" + 0.004*"2022" + 0.004*"practice" + 0.004*"well"', '0.012*"’" + 0.008*"May" + 0.008*"practice" + 0.007*"plans" + 0.006*"needs" + 0.006*"Wigan" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"timely" + 0.005*"20"', '0.015*"’" + 0.008*"May" + 0.007*"plans" + 0.007*"practice" + 0.006*"quality" + 0.006*"needs" + 0.006*"appropriate" + 0.006*"Wigan" + 0.005*"leaders" + 0.005*"9"']</t>
+    <t>['0.014*"’" + 0.008*"May" + 0.008*"practice" + 0.007*"plans" + 0.007*"Wigan" + 0.006*"needs" + 0.006*"quality" + 0.006*"timely" + 0.005*"2022" + 0.005*"20"', '0.010*"’" + 0.006*"May" + 0.006*"appropriate" + 0.005*"quality" + 0.005*"plans" + 0.005*"leaders" + 0.004*"Wigan" + 0.004*"needs" + 0.004*"practice" + 0.004*"good"', '0.011*"’" + 0.006*"needs" + 0.006*"May" + 0.006*"plans" + 0.006*"appropriate" + 0.006*"quality" + 0.005*"practice" + 0.005*"Wigan" + 0.004*"leaders" + 0.004*"9"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4180,7 +4180,7 @@
     <t>12/12/23</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"Wiltshire" + 0.006*"supported" + 0.005*"ensure" + 0.005*"parents" + 0.005*"risk" + 0.005*"progress"', '0.022*"’" + 0.011*"well" + 0.007*"need" + 0.007*"progress" + 0.006*"needs" + 0.006*"including" + 0.006*"risk" + 0.006*"plans" + 0.006*"ensure" + 0.006*"Wiltshire"', '0.012*"well" + 0.011*"’" + 0.008*"needs" + 0.006*"parents" + 0.006*"Wiltshire" + 0.005*"progress" + 0.005*"including" + 0.005*"plans" + 0.005*"supported" + 0.005*"risk"']</t>
+    <t>['0.014*"’" + 0.010*"well" + 0.007*"progress" + 0.007*"risk" + 0.007*"Wiltshire" + 0.007*"need" + 0.007*"needs" + 0.006*"including" + 0.006*"parents" + 0.005*"ensure"', '0.015*"’" + 0.011*"well" + 0.006*"need" + 0.006*"needs" + 0.005*"Wiltshire" + 0.005*"quality" + 0.005*"parents" + 0.005*"plans" + 0.005*"supported" + 0.004*"risk"', '0.016*"’" + 0.013*"well" + 0.009*"needs" + 0.006*"need" + 0.006*"progress" + 0.005*"plans" + 0.005*"including" + 0.005*"supported" + 0.005*"quality" + 0.005*"parents"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4210,7 +4210,7 @@
     <t>0.1719</t>
   </si>
   <si>
-    <t>['0.009*"practice" + 0.009*"well" + 0.009*"’" + 0.009*"good" + 0.007*"need" + 0.007*"quality" + 0.007*"progress" + 0.006*"place" + 0.006*"ensure" + 0.005*"needs"', '0.008*"needs" + 0.008*"good" + 0.007*"quality" + 0.007*"’" + 0.007*"well" + 0.007*"practice" + 0.007*"need" + 0.006*"effective" + 0.006*"progress" + 0.006*"plans"', '0.012*"quality" + 0.009*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"progress" + 0.006*"practice" + 0.006*"good" + 0.006*"need" + 0.005*"place"']</t>
+    <t>['0.009*"quality" + 0.008*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"good" + 0.006*"need" + 0.006*"progress" + 0.006*"practice" + 0.006*"plans" + 0.005*"ensure"', '0.009*"practice" + 0.009*"well" + 0.008*"good" + 0.008*"plans" + 0.008*"’" + 0.007*"quality" + 0.007*"place" + 0.007*"need" + 0.007*"needs" + 0.006*"progress"', '0.010*"quality" + 0.009*"’" + 0.008*"good" + 0.007*"progress" + 0.007*"well" + 0.007*"need" + 0.006*"practice" + 0.006*"needs" + 0.006*"effective" + 0.006*"ensure"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4231,7 +4231,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.005*"effective" + 0.004*"provided" + 0.004*"progress" + 0.004*"impact" + 0.004*"quality" + 0.004*"Wokingham"', '0.015*"’" + 0.008*"plans" + 0.007*"effective" + 0.007*"progress" + 0.006*"needs" + 0.005*"17" + 0.005*"quality" + 0.005*"experiences" + 0.005*"appropriate" + 0.005*"provided"', '0.011*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"provided" + 0.005*"6" + 0.005*"progress" + 0.005*"experiences" + 0.004*"good"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.006*"progress" + 0.005*"plans" + 0.005*"provided" + 0.005*"6" + 0.005*"effective" + 0.005*"quality" + 0.005*"experiences" + 0.005*"well"', '0.012*"’" + 0.007*"plans" + 0.006*"effective" + 0.005*"needs" + 0.005*"provided" + 0.005*"well" + 0.005*"impact" + 0.005*"parents" + 0.005*"progress" + 0.004*"good"', '0.013*"’" + 0.008*"plans" + 0.007*"effective" + 0.006*"well" + 0.005*"needs" + 0.005*"progress" + 0.005*"17" + 0.004*"experiences" + 0.004*"quality" + 0.004*"provided"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4252,7 +4252,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.006*"Wolverhampton" + 0.005*"effective" + 0.005*"leaders" + 0.005*"strong" + 0.005*"risks" + 0.004*"well" + 0.004*"practice" + 0.004*"supported"', '0.016*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"Wolverhampton" + 0.006*"risks" + 0.005*"plans" + 0.005*"effective" + 0.005*"education" + 0.005*"receive" + 0.004*"leaders"', '0.013*"’" + 0.007*"effective" + 0.007*"needs" + 0.005*"plans" + 0.005*"Wolverhampton" + 0.005*"receive" + 0.004*"education" + 0.004*"risk" + 0.004*"City" + 0.004*"supported"']</t>
+    <t>['0.016*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"risks" + 0.005*"leaders" + 0.005*"Wolverhampton" + 0.005*"practice" + 0.005*"receive" + 0.005*"supported" + 0.005*"plans"', '0.013*"’" + 0.006*"Wolverhampton" + 0.006*"needs" + 0.006*"effective" + 0.005*"strong" + 0.005*"leaders" + 0.005*"plans" + 0.004*"risks" + 0.004*"education" + 0.004*"receive"', '0.014*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"quality" + 0.005*"plans" + 0.005*"City" + 0.005*"Wolverhampton" + 0.005*"risk" + 0.005*"receive" + 0.005*"risks"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4279,7 +4279,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"plans" + 0.007*"Worcestershire" + 0.006*"progress" + 0.006*"ensure" + 0.005*"leaders" + 0.005*"PAs" + 0.005*"improve"', '0.018*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"Worcestershire" + 0.006*"appropriate" + 0.006*"ensure" + 0.006*"leaders" + 0.005*"experiences"', '0.022*"’" + 0.008*"leaders" + 0.008*"plans" + 0.008*"well" + 0.007*"Worcestershire" + 0.007*"progress" + 0.006*"appropriate" + 0.006*"needs" + 0.005*"ensure" + 0.005*"improve"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"plans" + 0.005*"appropriate" + 0.004*"ensure" + 0.004*"Worcestershire" + 0.004*"leaders" + 0.004*"progress" + 0.004*"good"', '0.020*"’" + 0.009*"well" + 0.008*"ensure" + 0.007*"Worcestershire" + 0.007*"plans" + 0.006*"leaders" + 0.006*"needs" + 0.006*"appropriate" + 0.006*"progress" + 0.005*"PAs"', '0.021*"’" + 0.010*"plans" + 0.008*"needs" + 0.008*"progress" + 0.008*"well" + 0.008*"leaders" + 0.008*"Worcestershire" + 0.005*"appropriate" + 0.005*"15" + 0.005*"living"']</t>
   </si>
   <si>
     <t>urn</t>
@@ -5273,19 +5273,19 @@
         <v>95</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
         <v>96</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>97</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" t="s">
         <v>99</v>
-      </c>
-      <c r="G9" t="s">
-        <v>100</v>
       </c>
       <c r="H9" t="s">
         <v>37</v>
@@ -5294,32 +5294,32 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
         <v>101</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>102</v>
-      </c>
-      <c r="L9" t="s">
-        <v>103</v>
       </c>
       <c r="M9" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\2532287_bournemouth, christchurch &amp; poole", ".\export_data\inspection_reports\2532287_bournemouth, christchurch &amp; poole")</f>
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q9" t="s">
         <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S9" t="s">
         <v>28</v>
@@ -5331,18 +5331,18 @@
         <v>16</v>
       </c>
       <c r="V9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:22">
       <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" t="s">
         <v>106</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>107</v>
-      </c>
-      <c r="C10" t="s">
-        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>108</v>
@@ -5411,7 +5411,7 @@
         <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
         <v>120</v>
@@ -5549,7 +5549,7 @@
         <v>142</v>
       </c>
       <c r="C13" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
         <v>143</v>
@@ -5570,13 +5570,13 @@
         <v>146</v>
       </c>
       <c r="J13" t="s">
+        <v>100</v>
+      </c>
+      <c r="K13" t="s">
         <v>101</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>102</v>
-      </c>
-      <c r="L13" t="s">
-        <v>103</v>
       </c>
       <c r="M13" s="3">
         <f>HYPERLINK(".\.\export_data\inspection_reports\80442_buckinghamshire", ".\export_data\inspection_reports\80442_buckinghamshire")</f>
@@ -5630,7 +5630,7 @@
         <v>154</v>
       </c>
       <c r="G14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" t="s">
         <v>37</v>
@@ -5652,13 +5652,13 @@
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q14" t="s">
         <v>12</v>
@@ -6044,7 +6044,7 @@
         <v>221</v>
       </c>
       <c r="G20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
@@ -6066,16 +6066,16 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R20" t="s">
         <v>226</v>
@@ -6389,7 +6389,7 @@
         <v>278</v>
       </c>
       <c r="G25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
         <v>7</v>
@@ -6411,10 +6411,10 @@
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O25" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P25" t="s">
         <v>12</v>
@@ -6734,7 +6734,7 @@
         <v>335</v>
       </c>
       <c r="G30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H30" t="s">
         <v>37</v>
@@ -6756,16 +6756,16 @@
         <v>0</v>
       </c>
       <c r="N30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O30" t="s">
         <v>12</v>
       </c>
       <c r="P30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R30" t="s">
         <v>339</v>
@@ -6825,7 +6825,7 @@
         <v>0</v>
       </c>
       <c r="N31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O31" t="s">
         <v>12</v>
@@ -7136,7 +7136,7 @@
         <v>395</v>
       </c>
       <c r="C36" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
         <v>396</v>
@@ -7481,7 +7481,7 @@
         <v>447</v>
       </c>
       <c r="C41" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D41" t="s">
         <v>448</v>
@@ -7631,7 +7631,7 @@
         <v>469</v>
       </c>
       <c r="G43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H43" t="s">
         <v>37</v>
@@ -7653,16 +7653,16 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q43" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R43" t="s">
         <v>473</v>
@@ -7757,7 +7757,7 @@
         <v>485</v>
       </c>
       <c r="C45" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D45" t="s">
         <v>486</v>
@@ -7826,7 +7826,7 @@
         <v>494</v>
       </c>
       <c r="C46" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D46" t="s">
         <v>495</v>
@@ -8459,7 +8459,7 @@
         <v>586</v>
       </c>
       <c r="G55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H55" t="s">
         <v>37</v>
@@ -8481,13 +8481,13 @@
         <v>0</v>
       </c>
       <c r="N55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q55" t="s">
         <v>12</v>
@@ -10262,7 +10262,7 @@
         <v>725</v>
       </c>
       <c r="J81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K81" t="s">
         <v>836</v>
@@ -10586,7 +10586,7 @@
         <v>874</v>
       </c>
       <c r="C86" t="s">
-        <v>298</v>
+        <v>33</v>
       </c>
       <c r="D86" t="s">
         <v>875</v>
@@ -10655,7 +10655,7 @@
         <v>884</v>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D87" t="s">
         <v>885</v>
@@ -10724,7 +10724,7 @@
         <v>893</v>
       </c>
       <c r="C88" t="s">
-        <v>298</v>
+        <v>529</v>
       </c>
       <c r="D88" t="s">
         <v>894</v>
@@ -10793,7 +10793,7 @@
         <v>902</v>
       </c>
       <c r="C89" t="s">
-        <v>33</v>
+        <v>298</v>
       </c>
       <c r="D89" t="s">
         <v>903</v>
@@ -10862,7 +10862,7 @@
         <v>909</v>
       </c>
       <c r="C90" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="D90" t="s">
         <v>910</v>
@@ -10931,7 +10931,7 @@
         <v>917</v>
       </c>
       <c r="C91" t="s">
-        <v>2</v>
+        <v>298</v>
       </c>
       <c r="D91" t="s">
         <v>918</v>
@@ -11069,7 +11069,7 @@
         <v>932</v>
       </c>
       <c r="C93" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D93" t="s">
         <v>933</v>
@@ -11081,7 +11081,7 @@
         <v>935</v>
       </c>
       <c r="G93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H93" t="s">
         <v>37</v>
@@ -11103,16 +11103,16 @@
         <v>0</v>
       </c>
       <c r="N93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q93" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R93" t="s">
         <v>939</v>
@@ -11138,7 +11138,7 @@
         <v>942</v>
       </c>
       <c r="C94" t="s">
-        <v>298</v>
+        <v>2</v>
       </c>
       <c r="D94" t="s">
         <v>943</v>
@@ -11276,7 +11276,7 @@
         <v>961</v>
       </c>
       <c r="C96" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D96" t="s">
         <v>962</v>
@@ -11345,7 +11345,7 @@
         <v>969</v>
       </c>
       <c r="C97" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D97" t="s">
         <v>970</v>
@@ -11483,7 +11483,7 @@
         <v>985</v>
       </c>
       <c r="C99" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D99" t="s">
         <v>986</v>
@@ -11552,7 +11552,7 @@
         <v>993</v>
       </c>
       <c r="C100" t="s">
-        <v>62</v>
+        <v>311</v>
       </c>
       <c r="D100" t="s">
         <v>994</v>
@@ -11564,7 +11564,7 @@
         <v>996</v>
       </c>
       <c r="G100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H100" t="s">
         <v>524</v>
@@ -11583,10 +11583,10 @@
         <v>12</v>
       </c>
       <c r="O100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P100" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q100" t="s">
         <v>12</v>
@@ -11684,7 +11684,7 @@
         <v>1008</v>
       </c>
       <c r="C102" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D102" t="s">
         <v>1009</v>
@@ -11753,7 +11753,7 @@
         <v>1019</v>
       </c>
       <c r="C103" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="D103" t="s">
         <v>1020</v>
@@ -11822,7 +11822,7 @@
         <v>1029</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D104" t="s">
         <v>1030</v>
@@ -11960,7 +11960,7 @@
         <v>1048</v>
       </c>
       <c r="C106" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="D106" t="s">
         <v>1049</v>
@@ -12029,7 +12029,7 @@
         <v>1058</v>
       </c>
       <c r="C107" t="s">
-        <v>298</v>
+        <v>107</v>
       </c>
       <c r="D107" t="s">
         <v>1059</v>
@@ -12098,7 +12098,7 @@
         <v>1069</v>
       </c>
       <c r="C108" t="s">
-        <v>62</v>
+        <v>298</v>
       </c>
       <c r="D108" t="s">
         <v>1070</v>
@@ -12161,7 +12161,7 @@
         <v>1076</v>
       </c>
       <c r="C109" t="s">
-        <v>2</v>
+        <v>62</v>
       </c>
       <c r="D109" t="s">
         <v>1077</v>
@@ -12230,7 +12230,7 @@
         <v>1085</v>
       </c>
       <c r="C110" t="s">
-        <v>311</v>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
         <v>1086</v>
@@ -12437,7 +12437,7 @@
         <v>1110</v>
       </c>
       <c r="C113" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D113" t="s">
         <v>1111</v>
@@ -12506,7 +12506,7 @@
         <v>1119</v>
       </c>
       <c r="C114" t="s">
-        <v>2</v>
+        <v>311</v>
       </c>
       <c r="D114" t="s">
         <v>1120</v>
@@ -12575,7 +12575,7 @@
         <v>1126</v>
       </c>
       <c r="C115" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D115" t="s">
         <v>1127</v>
@@ -12644,7 +12644,7 @@
         <v>1134</v>
       </c>
       <c r="C116" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D116" t="s">
         <v>1135</v>
@@ -12713,7 +12713,7 @@
         <v>1141</v>
       </c>
       <c r="C117" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D117" t="s">
         <v>1142</v>
@@ -12725,7 +12725,7 @@
         <v>1144</v>
       </c>
       <c r="G117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H117" t="s">
         <v>37</v>
@@ -12747,16 +12747,16 @@
         <v>0</v>
       </c>
       <c r="N117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q117" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R117" t="s">
         <v>1145</v>
@@ -12782,7 +12782,7 @@
         <v>1148</v>
       </c>
       <c r="C118" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D118" t="s">
         <v>1149</v>
@@ -12851,7 +12851,7 @@
         <v>1158</v>
       </c>
       <c r="C119" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D119" t="s">
         <v>1159</v>
@@ -12920,7 +12920,7 @@
         <v>1167</v>
       </c>
       <c r="C120" t="s">
-        <v>298</v>
+        <v>107</v>
       </c>
       <c r="D120" t="s">
         <v>1168</v>
@@ -12954,7 +12954,7 @@
         <v>0</v>
       </c>
       <c r="N120" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O120" t="s">
         <v>12</v>
@@ -12989,7 +12989,7 @@
         <v>1174</v>
       </c>
       <c r="C121" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D121" t="s">
         <v>1175</v>
@@ -13001,7 +13001,7 @@
         <v>1177</v>
       </c>
       <c r="G121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H121" t="s">
         <v>37</v>
@@ -13023,16 +13023,16 @@
         <v>0</v>
       </c>
       <c r="N121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q121" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R121" t="s">
         <v>1178</v>
@@ -13058,7 +13058,7 @@
         <v>1181</v>
       </c>
       <c r="C122" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D122" t="s">
         <v>1182</v>
@@ -13127,7 +13127,7 @@
         <v>1188</v>
       </c>
       <c r="C123" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D123" t="s">
         <v>1189</v>
@@ -13196,7 +13196,7 @@
         <v>1195</v>
       </c>
       <c r="C124" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="D124" t="s">
         <v>1196</v>
@@ -13208,7 +13208,7 @@
         <v>1198</v>
       </c>
       <c r="G124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H124" t="s">
         <v>7</v>
@@ -13230,16 +13230,16 @@
         <v>0</v>
       </c>
       <c r="N124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O124" t="s">
         <v>12</v>
       </c>
       <c r="P124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q124" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R124" t="s">
         <v>1201</v>
@@ -13265,7 +13265,7 @@
         <v>1205</v>
       </c>
       <c r="C125" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D125" t="s">
         <v>1206</v>
@@ -13334,7 +13334,7 @@
         <v>1214</v>
       </c>
       <c r="C126" t="s">
-        <v>298</v>
+        <v>33</v>
       </c>
       <c r="D126" t="s">
         <v>1215</v>
@@ -13403,7 +13403,7 @@
         <v>1224</v>
       </c>
       <c r="C127" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="D127" t="s">
         <v>1225</v>
@@ -13472,7 +13472,7 @@
         <v>1230</v>
       </c>
       <c r="C128" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D128" t="s">
         <v>1231</v>
@@ -13541,7 +13541,7 @@
         <v>1237</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>62</v>
       </c>
       <c r="D129" t="s">
         <v>1238</v>
@@ -13610,7 +13610,7 @@
         <v>1245</v>
       </c>
       <c r="C130" t="s">
-        <v>96</v>
+        <v>298</v>
       </c>
       <c r="D130" t="s">
         <v>1246</v>
@@ -13679,7 +13679,7 @@
         <v>1256</v>
       </c>
       <c r="C131" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D131" t="s">
         <v>1257</v>
@@ -13748,7 +13748,7 @@
         <v>1263</v>
       </c>
       <c r="C132" t="s">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="D132" t="s">
         <v>1264</v>
@@ -13817,7 +13817,7 @@
         <v>1272</v>
       </c>
       <c r="C133" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="D133" t="s">
         <v>1273</v>
@@ -13886,7 +13886,7 @@
         <v>1282</v>
       </c>
       <c r="C134" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="D134" t="s">
         <v>1283</v>
@@ -13967,7 +13967,7 @@
         <v>1294</v>
       </c>
       <c r="G135" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H135" t="s">
         <v>37</v>
@@ -13989,16 +13989,16 @@
         <v>0</v>
       </c>
       <c r="N135" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="O135" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P135" t="s">
         <v>12</v>
       </c>
       <c r="Q135" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R135" t="s">
         <v>1295</v>
@@ -14093,7 +14093,7 @@
         <v>1305</v>
       </c>
       <c r="C137" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D137" t="s">
         <v>1306</v>
@@ -14162,7 +14162,7 @@
         <v>1312</v>
       </c>
       <c r="C138" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D138" t="s">
         <v>1313</v>
@@ -14231,7 +14231,7 @@
         <v>1319</v>
       </c>
       <c r="C139" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D139" t="s">
         <v>1320</v>
@@ -14300,7 +14300,7 @@
         <v>1326</v>
       </c>
       <c r="C140" t="s">
-        <v>529</v>
+        <v>62</v>
       </c>
       <c r="D140" t="s">
         <v>1327</v>
@@ -14438,7 +14438,7 @@
         <v>1339</v>
       </c>
       <c r="C142" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D142" t="s">
         <v>1340</v>
@@ -14507,7 +14507,7 @@
         <v>1345</v>
       </c>
       <c r="C143" t="s">
-        <v>96</v>
+        <v>48</v>
       </c>
       <c r="D143" t="s">
         <v>1346</v>
@@ -14576,7 +14576,7 @@
         <v>1353</v>
       </c>
       <c r="C144" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D144" t="s">
         <v>1354</v>
@@ -14714,7 +14714,7 @@
         <v>1368</v>
       </c>
       <c r="C146" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="D146" t="s">
         <v>1369</v>
@@ -14783,7 +14783,7 @@
         <v>1375</v>
       </c>
       <c r="C147" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D147" t="s">
         <v>1376</v>
@@ -14852,7 +14852,7 @@
         <v>1381</v>
       </c>
       <c r="C148" t="s">
-        <v>62</v>
+        <v>20</v>
       </c>
       <c r="D148" t="s">
         <v>1382</v>
@@ -14921,7 +14921,7 @@
         <v>1390</v>
       </c>
       <c r="C149" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="D149" t="s">
         <v>1391</v>
@@ -14990,7 +14990,7 @@
         <v>1400</v>
       </c>
       <c r="C150" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D150" t="s">
         <v>1401</v>
@@ -15128,7 +15128,7 @@
         <v>1414</v>
       </c>
       <c r="C152" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="D152" t="s">
         <v>1415</v>

</xml_diff>

<commit_message>
adds toggle to include full text in xlsx output
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -70,7 +70,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"needs" + 0.006*"Barnsley" + 0.006*"leaders" + 0.005*"senior" + 0.005*"practice" + 0.004*"response" + 0.004*"11" + 0.004*"need" + 0.003*"within"', '0.022*"’" + 0.009*"leaders" + 0.008*"needs" + 0.008*"within" + 0.006*"practice" + 0.006*"Barnsley" + 0.006*"plans" + 0.005*"15" + 0.004*"11" + 0.004*"2023"', '0.017*"’" + 0.010*"needs" + 0.006*"within" + 0.006*"leaders" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"understand" + 0.004*"response" + 0.004*"progress" + 0.004*"11"']</t>
+    <t>['0.018*"’" + 0.009*"leaders" + 0.008*"needs" + 0.007*"Barnsley" + 0.006*"within" + 0.006*"practice" + 0.005*"11" + 0.005*"plans" + 0.005*"response" + 0.004*"need"', '0.016*"’" + 0.008*"needs" + 0.006*"leaders" + 0.005*"Barnsley" + 0.005*"plans" + 0.005*"practice" + 0.004*"within" + 0.004*"15" + 0.004*"senior" + 0.004*"11"', '0.023*"’" + 0.008*"needs" + 0.007*"within" + 0.006*"practice" + 0.006*"leaders" + 0.005*"Barnsley" + 0.005*"senior" + 0.004*"2023" + 0.004*"experiences" + 0.004*"understand"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -115,7 +115,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"plans" + 0.005*"East" + 0.005*"North" + 0.005*"leaders" + 0.005*"receive" + 0.005*"impact"', '0.016*"’" + 0.009*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"clear" + 0.005*"effective" + 0.005*"leaders" + 0.005*"plans" + 0.004*"Somerset" + 0.004*"Bath"', '0.012*"’" + 0.006*"well" + 0.005*"needs" + 0.005*"practice" + 0.004*"plans" + 0.004*"leaders" + 0.004*"Bath" + 0.004*"protection" + 0.004*"effective" + 0.004*"impact"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.004*"practice" + 0.004*"needs" + 0.004*"plans" + 0.004*"receive" + 0.004*"2022" + 0.004*"effective" + 0.004*"clear" + 0.003*"‘"', '0.015*"’" + 0.008*"well" + 0.006*"plans" + 0.006*"needs" + 0.006*"practice" + 0.005*"effective" + 0.005*"East" + 0.005*"4" + 0.005*"Somerset" + 0.005*"Bath"', '0.022*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.005*"plans" + 0.005*"North" + 0.005*"impact" + 0.004*"effective" + 0.004*"protection"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -163,7 +163,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"Bedford" + 0.005*"supported" + 0.005*"ensure" + 0.005*"progress" + 0.005*"good" + 0.004*"family" + 0.004*"plans"', '0.018*"’" + 0.007*"ensure" + 0.006*"well" + 0.005*"needs" + 0.005*"Bedford" + 0.005*"plans" + 0.005*"family" + 0.005*"education" + 0.004*"made" + 0.004*"supported"', '0.023*"’" + 0.008*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.005*"good" + 0.005*"progress" + 0.005*"well" + 0.005*"supported" + 0.005*"Bedford" + 0.005*"Borough"']</t>
+    <t>['0.020*"’" + 0.007*"needs" + 0.007*"ensure" + 0.006*"Bedford" + 0.006*"well" + 0.006*"progress" + 0.005*"supported" + 0.005*"good" + 0.005*"plans" + 0.005*"family"', '0.015*"’" + 0.006*"well" + 0.006*"ensure" + 0.005*"needs" + 0.005*"plans" + 0.004*"good" + 0.004*"Borough" + 0.004*"education" + 0.004*"Bedford" + 0.004*"progress"', '0.019*"’" + 0.008*"needs" + 0.006*"ensure" + 0.005*"plans" + 0.005*"supported" + 0.005*"relationships" + 0.005*"well" + 0.005*"family" + 0.004*"Bedford" + 0.004*"15"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -208,7 +208,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"needs" + 0.007*"plans" + 0.006*"well" + 0.005*"timely" + 0.005*"leaders" + 0.005*"risk" + 0.005*"effective" + 0.005*"20" + 0.005*"3"', '0.017*"’" + 0.009*"needs" + 0.008*"Birmingham" + 0.007*"well" + 0.007*"effective" + 0.006*"progress" + 0.006*"trust" + 0.005*"plans" + 0.005*"3" + 0.005*"response"', '0.018*"’" + 0.009*"needs" + 0.007*"effective" + 0.006*"well" + 0.006*"plans" + 0.005*"trust" + 0.005*"appropriate" + 0.005*"progress" + 0.005*"risk" + 0.005*"March"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.007*"Birmingham" + 0.007*"effective" + 0.005*"trust" + 0.005*"well" + 0.005*"3" + 0.005*"response" + 0.005*"plans" + 0.004*"risk"', '0.015*"’" + 0.007*"needs" + 0.007*"progress" + 0.007*"plans" + 0.007*"well" + 0.006*"effective" + 0.006*"appropriate" + 0.006*"trust" + 0.005*"Birmingham" + 0.005*"3"', '0.017*"’" + 0.011*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"effective" + 0.005*"progress" + 0.005*"leaders" + 0.005*"risk" + 0.005*"ensure" + 0.005*"Birmingham"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -250,7 +250,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.007*"practice" + 0.007*"Darwen" + 0.007*"quality" + 0.007*"well" + 0.006*"Blackburn" + 0.005*"planning" + 0.005*"impact" + 0.005*"leaders"', '0.016*"’" + 0.008*"practice" + 0.007*"Blackburn" + 0.007*"needs" + 0.007*"quality" + 0.006*"impact" + 0.006*"well" + 0.006*"Darwen" + 0.005*"planning" + 0.005*"means"', '0.013*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"Darwen" + 0.006*"impact" + 0.006*"Blackburn" + 0.006*"practice" + 0.005*"well" + 0.005*"plans" + 0.005*"result"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.007*"Darwen" + 0.006*"Blackburn" + 0.006*"quality" + 0.006*"well" + 0.006*"practice" + 0.006*"impact" + 0.005*"receive" + 0.005*"result"', '0.015*"’" + 0.009*"practice" + 0.008*"quality" + 0.007*"needs" + 0.007*"Darwen" + 0.007*"Blackburn" + 0.006*"impact" + 0.006*"well" + 0.005*"planning" + 0.005*"means"', '0.012*"’" + 0.006*"needs" + 0.006*"Blackburn" + 0.006*"practice" + 0.006*"well" + 0.006*"quality" + 0.006*"impact" + 0.005*"number" + 0.004*"means" + 0.004*"planning"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -292,7 +292,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"needs" + 0.009*"well" + 0.006*"Blackpool" + 0.005*"quality" + 0.005*"16" + 0.005*"progress" + 0.005*"carers" + 0.004*"plans" + 0.004*"5"', '0.015*"’" + 0.012*"well" + 0.010*"needs" + 0.008*"Blackpool" + 0.006*"effective" + 0.005*"practice" + 0.005*"supported" + 0.005*"need" + 0.005*"quality" + 0.005*"good"', '0.020*"’" + 0.011*"needs" + 0.007*"Blackpool" + 0.007*"well" + 0.007*"effective" + 0.006*"plans" + 0.005*"experiences" + 0.005*"progress" + 0.005*"practice" + 0.005*"supported"']</t>
+    <t>['0.016*"’" + 0.011*"needs" + 0.009*"well" + 0.006*"Blackpool" + 0.005*"effective" + 0.005*"supported" + 0.005*"plans" + 0.005*"team" + 0.005*"carers" + 0.005*"good"', '0.018*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"Blackpool" + 0.006*"experiences" + 0.006*"effective" + 0.005*"supported" + 0.005*"practice" + 0.005*"16" + 0.004*"December"', '0.016*"’" + 0.012*"needs" + 0.010*"well" + 0.009*"Blackpool" + 0.006*"plans" + 0.006*"effective" + 0.005*"practice" + 0.005*"16" + 0.005*"quality" + 0.004*"5"']</t>
   </si>
   <si>
     <t>80432</t>
@@ -322,7 +322,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.007*"Bolton" + 0.007*"well" + 0.007*"plans" + 0.006*"11" + 0.006*"supported" + 0.005*"need" + 0.005*"planning" + 0.005*"September"', '0.022*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Bolton" + 0.007*"plans" + 0.005*"need" + 0.005*"response" + 0.005*"supported" + 0.005*"planning" + 0.004*"2023"', '0.019*"’" + 0.010*"needs" + 0.009*"Bolton" + 0.009*"well" + 0.008*"plans" + 0.006*"supported" + 0.005*"timely" + 0.005*"planning" + 0.005*"effective" + 0.005*"strong"']</t>
+    <t>['0.020*"’" + 0.011*"needs" + 0.009*"Bolton" + 0.009*"plans" + 0.008*"well" + 0.006*"supported" + 0.005*"strong" + 0.005*"need" + 0.005*"timely" + 0.005*"carers"', '0.022*"’" + 0.009*"Bolton" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.006*"planning" + 0.005*"effective" + 0.005*"need" + 0.005*"15" + 0.005*"supported"', '0.011*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"need" + 0.005*"Bolton" + 0.004*"response" + 0.004*"11" + 0.004*"planning" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -358,7 +358,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"impact" + 0.005*"quality" + 0.004*"Christchurch" + 0.004*"17" + 0.004*"time" + 0.004*"progress" + 0.003*"risk" + 0.003*"2021" + 0.003*"6"', '0.018*"’" + 0.005*"practice" + 0.005*"progress" + 0.005*"quality" + 0.005*"Poole" + 0.005*"time" + 0.005*"However" + 0.004*"Bournemouth" + 0.004*"risk" + 0.004*"17"', '0.021*"’" + 0.008*"quality" + 0.007*"practice" + 0.006*"progress" + 0.005*"Christchurch" + 0.005*"6" + 0.005*"Bournemouth" + 0.005*"impact" + 0.005*"risk" + 0.005*"Poole"']</t>
+    <t>['0.012*"’" + 0.006*"quality" + 0.005*"practice" + 0.005*"time" + 0.004*"impact" + 0.004*"risk" + 0.004*"progress" + 0.004*"However" + 0.004*"number" + 0.004*"Christchurch"', '0.016*"’" + 0.006*"quality" + 0.005*"practice" + 0.005*"17" + 0.005*"progress" + 0.005*"6" + 0.005*"risk" + 0.005*"Poole" + 0.005*"well" + 0.004*"right"', '0.024*"’" + 0.006*"practice" + 0.006*"quality" + 0.005*"progress" + 0.005*"time" + 0.005*"Bournemouth" + 0.005*"Christchurch" + 0.005*"Poole" + 0.004*"well" + 0.004*"many"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -403,7 +403,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.007*"good" + 0.007*"Forest" + 0.007*"Bracknell" + 0.006*"effective" + 0.006*"risk" + 0.005*"progress" + 0.005*"need" + 0.005*"impact"', '0.016*"’" + 0.007*"risk" + 0.007*"Forest" + 0.006*"well" + 0.006*"needs" + 0.006*"provided" + 0.006*"plans" + 0.005*"quality" + 0.005*"good" + 0.005*"Bracknell"', '0.018*"’" + 0.008*"Bracknell" + 0.007*"quality" + 0.007*"needs" + 0.006*"Forest" + 0.006*"good" + 0.006*"progress" + 0.005*"risk" + 0.005*"provided" + 0.005*"need"']</t>
+    <t>['0.010*"’" + 0.007*"provided" + 0.006*"Forest" + 0.006*"risk" + 0.006*"needs" + 0.006*"Bracknell" + 0.005*"progress" + 0.005*"well" + 0.005*"good" + 0.005*"positive"', '0.017*"’" + 0.007*"effective" + 0.007*"risk" + 0.006*"Forest" + 0.006*"Bracknell" + 0.006*"quality" + 0.006*"good" + 0.006*"plans" + 0.006*"needs" + 0.005*"need"', '0.020*"’" + 0.008*"needs" + 0.007*"Bracknell" + 0.007*"Forest" + 0.007*"quality" + 0.006*"good" + 0.006*"risk" + 0.006*"progress" + 0.005*"well" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80438</t>
@@ -442,7 +442,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"needs" + 0.008*"good" + 0.006*"well" + 0.006*"need" + 0.005*"recording" + 0.005*"quality" + 0.004*"plans" + 0.004*"effective" + 0.004*"leaders"', '0.014*"’" + 0.008*"needs" + 0.008*"good" + 0.007*"leaders" + 0.006*"well" + 0.005*"recording" + 0.004*"improve" + 0.004*"timely" + 0.004*"plans" + 0.004*"need"', '0.013*"’" + 0.009*"good" + 0.008*"needs" + 0.007*"recording" + 0.005*"leaders" + 0.005*"However" + 0.005*"plans" + 0.005*"Hove" + 0.005*"arrangements" + 0.005*"quality"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.007*"good" + 0.007*"recording" + 0.005*"leaders" + 0.005*"supported" + 0.005*"timely" + 0.005*"ensure" + 0.004*"arrangements" + 0.004*"Senior"', '0.012*"’" + 0.009*"needs" + 0.008*"good" + 0.006*"recording" + 0.005*"well" + 0.005*"leaders" + 0.005*"need" + 0.004*"including" + 0.004*"plans" + 0.004*"timely"', '0.011*"’" + 0.010*"good" + 0.008*"needs" + 0.007*"well" + 0.006*"leaders" + 0.005*"plans" + 0.005*"need" + 0.005*"However" + 0.005*"quality" + 0.005*"recording"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -478,7 +478,7 @@
     <t>0.1875</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"needs" + 0.008*"Bristol" + 0.008*"well" + 0.007*"good" + 0.004*"receive" + 0.004*"leaders" + 0.004*"risk" + 0.004*"health" + 0.004*"progress"', '0.020*"’" + 0.009*"good" + 0.009*"well" + 0.008*"Bristol" + 0.006*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"health" + 0.005*"leaders" + 0.005*"always"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"good" + 0.006*"Bristol" + 0.006*"health" + 0.005*"progress" + 0.005*"need" + 0.005*"plans" + 0.005*"27"']</t>
+    <t>['0.021*"’" + 0.008*"good" + 0.008*"well" + 0.008*"Bristol" + 0.008*"needs" + 0.006*"health" + 0.005*"progress" + 0.005*"always" + 0.005*"need" + 0.005*"leaders"', '0.017*"’" + 0.009*"well" + 0.007*"Bristol" + 0.007*"good" + 0.007*"needs" + 0.005*"receive" + 0.005*"progress" + 0.005*"health" + 0.004*"ensure" + 0.004*"always"', '0.020*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Bristol" + 0.007*"good" + 0.006*"plans" + 0.005*"16" + 0.005*"progress" + 0.005*"leaders" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -511,7 +511,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"number" + 0.005*"17" + 0.004*"6" + 0.004*"protection" + 0.004*"Buckinghamshire" + 0.004*"well" + 0.003*"plans" + 0.003*"practice" + 0.003*"many"', '0.012*"’" + 0.006*"plans" + 0.005*"17" + 0.004*"Buckinghamshire" + 0.004*"number" + 0.004*"2021" + 0.004*"many" + 0.004*"protection" + 0.004*"December" + 0.003*"impact"', '0.017*"’" + 0.005*"plans" + 0.005*"number" + 0.005*"Buckinghamshire" + 0.004*"6" + 0.004*"practice" + 0.004*"many" + 0.004*"December" + 0.004*"2021" + 0.004*"17"']</t>
+    <t>['0.015*"’" + 0.005*"plans" + 0.005*"Buckinghamshire" + 0.005*"17" + 0.005*"number" + 0.005*"6" + 0.004*"many" + 0.004*"protection" + 0.004*"December" + 0.004*"well"', '0.011*"’" + 0.005*"many" + 0.004*"practice" + 0.004*"needs" + 0.004*"plans" + 0.004*"17" + 0.004*"6" + 0.004*"number" + 0.004*"protection" + 0.004*"Buckinghamshire"', '0.014*"’" + 0.005*"number" + 0.005*"plans" + 0.004*"Buckinghamshire" + 0.004*"17" + 0.004*"small" + 0.004*"protection" + 0.004*"2021" + 0.003*"teams" + 0.003*"December"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -550,7 +550,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"practice" + 0.007*"needs" + 0.006*"team" + 0.006*"protection" + 0.006*"2021" + 0.005*"impact" + 0.005*"delay" + 0.005*"Bury" + 0.005*"new"', '0.012*"’" + 0.006*"2021" + 0.005*"needs" + 0.005*"protection" + 0.005*"risk" + 0.005*"quality" + 0.005*"need" + 0.004*"team" + 0.004*"practice" + 0.004*"Bury"', '0.012*"’" + 0.008*"protection" + 0.007*"2021" + 0.007*"needs" + 0.006*"need" + 0.005*"team" + 0.005*"impact" + 0.005*"risk" + 0.005*"quality" + 0.005*"Bury"']</t>
+    <t>['0.010*"’" + 0.006*"protection" + 0.005*"need" + 0.005*"2021" + 0.005*"practice" + 0.005*"Bury" + 0.005*"needs" + 0.005*"team" + 0.005*"impact" + 0.005*"25"', '0.009*"’" + 0.005*"team" + 0.005*"needs" + 0.005*"protection" + 0.005*"need" + 0.004*"risk" + 0.004*"delay" + 0.004*"quality" + 0.004*"October" + 0.004*"response"', '0.013*"’" + 0.008*"2021" + 0.008*"needs" + 0.007*"protection" + 0.007*"practice" + 0.006*"team" + 0.006*"impact" + 0.005*"quality" + 0.005*"risk" + 0.005*"Bury"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -583,7 +583,7 @@
     <t>0.1954</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"well" + 0.006*"practice" + 0.006*"good" + 0.005*"Calderdale" + 0.005*"effective" + 0.005*"protection" + 0.005*"need" + 0.004*"‘" + 0.004*"carers"', '0.015*"’" + 0.006*"well" + 0.005*"Calderdale" + 0.005*"inform" + 0.005*"protection" + 0.004*"good" + 0.004*"practice" + 0.004*"‘" + 0.004*"risk" + 0.004*"leaders"', '0.012*"’" + 0.007*"well" + 0.005*"practice" + 0.005*"Calderdale" + 0.005*"good" + 0.005*"education" + 0.004*"needs" + 0.004*"effective" + 0.004*"risk" + 0.004*"need"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.006*"practice" + 0.006*"good" + 0.005*"Calderdale" + 0.005*"protection" + 0.005*"effective" + 0.004*"‘" + 0.004*"carers" + 0.004*"inform"', '0.017*"’" + 0.009*"well" + 0.006*"Calderdale" + 0.006*"practice" + 0.005*"good" + 0.005*"education" + 0.005*"effective" + 0.004*"need" + 0.004*"‘" + 0.004*"risk"', '0.008*"’" + 0.006*"well" + 0.004*"protection" + 0.004*"practice" + 0.004*"Calderdale" + 0.003*"good" + 0.003*"needs" + 0.003*"‘" + 0.003*"need" + 0.003*"education"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -622,7 +622,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.008*"good" + 0.008*"plans" + 0.007*"needs" + 0.006*"However" + 0.006*"need" + 0.006*"teams" + 0.006*"impact" + 0.005*"effective"', '0.013*"’" + 0.011*"well" + 0.009*"good" + 0.008*"impact" + 0.008*"need" + 0.007*"needs" + 0.007*"teams" + 0.006*"effective" + 0.006*"progress" + 0.005*"plans"', '0.014*"’" + 0.009*"good" + 0.009*"well" + 0.007*"needs" + 0.007*"teams" + 0.007*"quality" + 0.007*"need" + 0.006*"impact" + 0.006*"plans" + 0.006*"However"']</t>
+    <t>['0.014*"’" + 0.010*"well" + 0.009*"need" + 0.009*"good" + 0.008*"needs" + 0.008*"teams" + 0.007*"impact" + 0.007*"plans" + 0.006*"However" + 0.006*"effective"', '0.013*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"plans" + 0.006*"need" + 0.006*"carers" + 0.006*"teams" + 0.005*"quality" + 0.005*"However"', '0.016*"’" + 0.010*"well" + 0.010*"good" + 0.007*"impact" + 0.007*"needs" + 0.007*"teams" + 0.006*"quality" + 0.006*"plans" + 0.006*"effective" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -655,7 +655,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"need" + 0.005*"carers" + 0.005*"progress" + 0.005*"Bedfordshire" + 0.005*"plans" + 0.005*"effective" + 0.005*"good"', '0.018*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"good" + 0.006*"carers" + 0.006*"need" + 0.006*"plans" + 0.005*"Central" + 0.005*"progress" + 0.005*"information"', '0.017*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"need" + 0.006*"plans" + 0.006*"good" + 0.006*"carers" + 0.005*"progress" + 0.004*"Bedfordshire" + 0.004*"Leaders"']</t>
+    <t>['0.019*"’" + 0.008*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"need" + 0.005*"carers" + 0.004*"effective" + 0.004*"protection"', '0.016*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"need" + 0.006*"good" + 0.006*"carers" + 0.005*"Bedfordshire" + 0.005*"plans" + 0.005*"Central" + 0.004*"number"', '0.014*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"carers" + 0.007*"need" + 0.006*"plans" + 0.006*"progress" + 0.006*"good" + 0.005*"Bedfordshire" + 0.005*"Central"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -694,7 +694,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.006*"good" + 0.006*"need" + 0.005*"always" + 0.005*"ensure" + 0.005*"However" + 0.005*"supported"', '0.011*"’" + 0.008*"good" + 0.008*"well" + 0.007*"practice" + 0.007*"needs" + 0.007*"plans" + 0.006*"ensure" + 0.005*"effective" + 0.005*"need" + 0.005*"carers"', '0.013*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"good" + 0.007*"practice" + 0.006*"supported" + 0.006*"always" + 0.006*"plans" + 0.005*"However" + 0.005*"need"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.008*"good" + 0.007*"plans" + 0.007*"supported" + 0.006*"needs" + 0.006*"practice" + 0.006*"always" + 0.006*"However" + 0.006*"risk"', '0.013*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"good" + 0.006*"practice" + 0.006*"plans" + 0.005*"need" + 0.005*"always" + 0.005*"effective" + 0.005*"supported"', '0.011*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"good" + 0.006*"ensure" + 0.006*"need" + 0.005*"practice" + 0.005*"plans" + 0.005*"effective" + 0.005*"However"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -733,7 +733,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"well" + 0.006*"practice" + 0.005*"needs" + 0.004*"plans" + 0.004*"impact" + 0.004*"always" + 0.004*"However" + 0.004*"effective" + 0.004*"learning"', '0.024*"’" + 0.007*"needs" + 0.006*"well" + 0.004*"practice" + 0.004*"effective" + 0.004*"impact" + 0.004*"information" + 0.004*"always" + 0.004*"timely" + 0.004*"learning"', '0.018*"’" + 0.008*"needs" + 0.008*"well" + 0.005*"effectively" + 0.005*"order" + 0.005*"plans" + 0.004*"receive" + 0.004*"timely" + 0.004*"effective" + 0.004*"early"']</t>
+    <t>['0.019*"’" + 0.007*"well" + 0.007*"needs" + 0.004*"effectively" + 0.004*"information" + 0.004*"always" + 0.004*"practice" + 0.004*"However" + 0.003*"use" + 0.003*"learning"', '0.024*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"plans" + 0.004*"impact" + 0.004*"effectively" + 0.004*"order" + 0.004*"timely" + 0.004*"learning"', '0.021*"’" + 0.008*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"effective" + 0.005*"order" + 0.004*"always" + 0.004*"impact" + 0.004*"intervention" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -772,7 +772,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"plans" + 0.006*"needs" + 0.005*"impact" + 0.005*"2" + 0.005*"risk" + 0.005*"Bradford" + 0.005*"December" + 0.005*"21" + 0.004*"quality"', '0.025*"’" + 0.007*"plans" + 0.006*"Bradford" + 0.005*"need" + 0.005*"2" + 0.005*"2022" + 0.005*"Council" + 0.004*"lack" + 0.004*"◼" + 0.004*"quality"', '0.015*"’" + 0.006*"plans" + 0.004*"quality" + 0.004*"However" + 0.004*"practice" + 0.004*"risk" + 0.004*"November" + 0.004*"needs" + 0.004*"worker" + 0.004*"Metropolitan"']</t>
+    <t>['0.022*"’" + 0.007*"plans" + 0.004*"November" + 0.004*"Bradford" + 0.004*"However" + 0.004*"senior" + 0.004*"◼" + 0.004*"experiences" + 0.004*"2022" + 0.004*"Borough"', '0.022*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"2" + 0.006*"Bradford" + 0.005*"risk" + 0.005*"quality" + 0.005*"need" + 0.005*"impact" + 0.004*"21"', '0.018*"’" + 0.006*"plans" + 0.005*"practice" + 0.005*"Council" + 0.004*"Bradford" + 0.004*"2" + 0.004*"impact" + 0.004*"progress" + 0.004*"changes" + 0.004*"December"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -808,7 +808,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"well" + 0.010*"ensure" + 0.009*"needs" + 0.006*"plans" + 0.006*"clear" + 0.006*"good" + 0.006*"effective" + 0.005*"progress" + 0.005*"individual"', '0.010*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"effective" + 0.007*"ensure" + 0.007*"progress" + 0.005*"clear" + 0.005*"good" + 0.005*"supported" + 0.004*"plans"', '0.016*"needs" + 0.011*"well" + 0.011*"’" + 0.008*"ensure" + 0.007*"clear" + 0.006*"effective" + 0.005*"practice" + 0.005*"good" + 0.005*"plans" + 0.005*"within"']</t>
+    <t>['0.010*"needs" + 0.009*"well" + 0.008*"’" + 0.007*"plans" + 0.006*"ensure" + 0.006*"clear" + 0.006*"effective" + 0.005*"good" + 0.005*"experiences" + 0.005*"progress"', '0.014*"’" + 0.012*"needs" + 0.010*"well" + 0.009*"ensure" + 0.008*"progress" + 0.006*"good" + 0.006*"clear" + 0.006*"practice" + 0.006*"supported" + 0.005*"effective"', '0.012*"’" + 0.011*"needs" + 0.011*"well" + 0.010*"ensure" + 0.008*"effective" + 0.007*"clear" + 0.005*"good" + 0.005*"within" + 0.005*"individual" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -847,7 +847,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"Wakefield" + 0.009*"well" + 0.008*"leaders" + 0.008*"November" + 0.007*"quality" + 0.007*"effective" + 0.007*"plans" + 0.006*"practice" + 0.006*"good"', '0.012*"’" + 0.007*"Wakefield" + 0.006*"November" + 0.006*"well" + 0.006*"quality" + 0.005*"effective" + 0.005*"leaders" + 0.005*"good" + 0.004*"plans" + 0.004*"2021"', '0.017*"’" + 0.009*"quality" + 0.008*"good" + 0.007*"leaders" + 0.007*"Wakefield" + 0.007*"well" + 0.007*"November" + 0.006*"effective" + 0.006*"needs" + 0.006*"progress"']</t>
+    <t>['0.012*"’" + 0.008*"Wakefield" + 0.007*"well" + 0.006*"quality" + 0.006*"effective" + 0.006*"good" + 0.005*"leaders" + 0.005*"November" + 0.005*"plans" + 0.005*"practice"', '0.020*"’" + 0.008*"quality" + 0.008*"Wakefield" + 0.008*"well" + 0.007*"November" + 0.007*"effective" + 0.007*"good" + 0.007*"leaders" + 0.006*"plans" + 0.006*"needs"', '0.017*"’" + 0.008*"leaders" + 0.008*"November" + 0.007*"Wakefield" + 0.007*"well" + 0.007*"quality" + 0.007*"good" + 0.006*"progress" + 0.006*"receive" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -880,7 +880,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.007*"quality" + 0.006*"ensure" + 0.006*"March" + 0.006*"effective" + 0.005*"well" + 0.005*"7" + 0.005*"plans" + 0.005*"supported"', '0.013*"’" + 0.008*"March" + 0.006*"needs" + 0.006*"quality" + 0.005*"effective" + 0.005*"However" + 0.005*"York" + 0.005*"appropriate" + 0.005*"plans" + 0.004*"good"', '0.016*"’" + 0.008*"needs" + 0.006*"March" + 0.006*"quality" + 0.006*"effective" + 0.006*"York" + 0.006*"However" + 0.006*"practice" + 0.005*"well" + 0.005*"ensure"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"March" + 0.006*"quality" + 0.006*"However" + 0.006*"good" + 0.005*"plans" + 0.005*"York" + 0.005*"training"', '0.015*"’" + 0.008*"quality" + 0.007*"needs" + 0.007*"March" + 0.006*"ensure" + 0.006*"York" + 0.005*"well" + 0.005*"effective" + 0.005*"However" + 0.005*"need"', '0.010*"’" + 0.006*"needs" + 0.006*"March" + 0.006*"quality" + 0.005*"plans" + 0.004*"education" + 0.004*"ensure" + 0.004*"effective" + 0.004*"York" + 0.004*"However"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -919,7 +919,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"well" + 0.010*"effective" + 0.008*"leaders" + 0.008*"quality" + 0.006*"timely" + 0.006*"plans" + 0.006*"arrangements" + 0.006*"good" + 0.005*"ensure"', '0.012*"’" + 0.010*"well" + 0.010*"effective" + 0.009*"quality" + 0.008*"leaders" + 0.006*"good" + 0.005*"plans" + 0.005*"arrangements" + 0.005*"highly" + 0.005*"Senior"', '0.022*"well" + 0.012*"quality" + 0.010*"’" + 0.008*"leaders" + 0.006*"effective" + 0.006*"plans" + 0.006*"timely" + 0.006*"good" + 0.005*"arrangements" + 0.005*"highly"']</t>
+    <t>['0.012*"well" + 0.009*"effective" + 0.009*"quality" + 0.009*"’" + 0.007*"leaders" + 0.005*"timely" + 0.005*"good" + 0.005*"highly" + 0.005*"arrangements" + 0.005*"plans"', '0.014*"well" + 0.012*"’" + 0.008*"effective" + 0.008*"leaders" + 0.007*"good" + 0.007*"quality" + 0.006*"arrangements" + 0.005*"timely" + 0.005*"ensure" + 0.005*"Senior"', '0.016*"well" + 0.014*"’" + 0.012*"quality" + 0.009*"leaders" + 0.008*"effective" + 0.008*"plans" + 0.006*"timely" + 0.006*"arrangements" + 0.005*"good" + 0.005*"high"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -952,7 +952,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.016*"Isles" + 0.015*"Scilly" + 0.009*"needs" + 0.009*"practice" + 0.009*"information" + 0.009*"need" + 0.007*"protection" + 0.007*"risks" + 0.006*"quality"', '0.012*"’" + 0.009*"Scilly" + 0.009*"need" + 0.008*"information" + 0.008*"practice" + 0.008*"Isles" + 0.007*"protection" + 0.006*"place" + 0.006*"quality" + 0.005*"lack"', '0.022*"’" + 0.010*"Isles" + 0.009*"Scilly" + 0.009*"information" + 0.008*"place" + 0.008*"practice" + 0.006*"need" + 0.005*"protection" + 0.005*"quality" + 0.005*"13"']</t>
+    <t>['0.012*"’" + 0.006*"Scilly" + 0.006*"practice" + 0.006*"information" + 0.006*"Isles" + 0.005*"protection" + 0.005*"need" + 0.004*"needs" + 0.004*"place" + 0.004*"enough"', '0.016*"’" + 0.013*"Scilly" + 0.011*"Isles" + 0.009*"need" + 0.008*"needs" + 0.007*"practice" + 0.007*"information" + 0.007*"protection" + 0.006*"2023" + 0.006*"place"', '0.027*"’" + 0.015*"Isles" + 0.014*"Scilly" + 0.011*"information" + 0.010*"practice" + 0.009*"need" + 0.007*"protection" + 0.007*"quality" + 0.007*"risks" + 0.007*"needs"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -991,7 +991,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.008*"well" + 0.008*"Coventry" + 0.008*"needs" + 0.006*"family" + 0.006*"strong" + 0.006*"plans" + 0.005*"supported" + 0.005*"June" + 0.004*"2022"', '0.012*"’" + 0.008*"supported" + 0.008*"well" + 0.007*"Coventry" + 0.006*"needs" + 0.005*"need" + 0.005*"strong" + 0.005*"family" + 0.004*"plans" + 0.004*"training"', '0.021*"’" + 0.008*"Coventry" + 0.008*"well" + 0.008*"needs" + 0.007*"plans" + 0.007*"supported" + 0.006*"need" + 0.006*"family" + 0.005*"strong" + 0.005*"1"']</t>
+    <t>['0.024*"’" + 0.009*"Coventry" + 0.008*"needs" + 0.007*"well" + 0.006*"supported" + 0.006*"strong" + 0.006*"plans" + 0.006*"family" + 0.005*"need" + 0.005*"PAs"', '0.014*"’" + 0.009*"well" + 0.007*"Coventry" + 0.007*"plans" + 0.007*"supported" + 0.006*"needs" + 0.006*"family" + 0.005*"need" + 0.005*"strong" + 0.004*"education"', '0.019*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Coventry" + 0.007*"supported" + 0.006*"family" + 0.005*"plans" + 0.005*"strong" + 0.005*"need" + 0.004*"1"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -1030,7 +1030,7 @@
     <t>0.1983</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"leaders" + 0.006*"quality" + 0.006*"October" + 0.005*"supported" + 0.005*"Darlington" + 0.004*"effective"', '0.017*"’" + 0.008*"well" + 0.008*"October" + 0.007*"needs" + 0.006*"leaders" + 0.006*"Darlington" + 0.006*"practice" + 0.005*"effective" + 0.005*"10" + 0.004*"21"', '0.021*"’" + 0.008*"leaders" + 0.007*"well" + 0.006*"practice" + 0.006*"Darlington" + 0.006*"October" + 0.006*"needs" + 0.005*"effective" + 0.004*"quality" + 0.004*"family"']</t>
+    <t>['0.024*"’" + 0.008*"October" + 0.008*"well" + 0.008*"Darlington" + 0.007*"needs" + 0.007*"leaders" + 0.007*"practice" + 0.005*"quality" + 0.005*"supported" + 0.005*"effective"', '0.015*"’" + 0.007*"well" + 0.006*"October" + 0.006*"needs" + 0.005*"leaders" + 0.005*"plans" + 0.004*"21" + 0.004*"Darlington" + 0.004*"practice" + 0.004*"understand"', '0.014*"’" + 0.008*"well" + 0.007*"leaders" + 0.006*"practice" + 0.006*"needs" + 0.005*"10" + 0.005*"effective" + 0.005*"October" + 0.005*"quality" + 0.004*"Darlington"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -1072,7 +1072,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"Derby" + 0.006*"receive" + 0.006*"needs" + 0.006*"quality" + 0.005*"plans" + 0.005*"progress" + 0.005*"good" + 0.005*"need" + 0.004*"appropriate"', '0.022*"’" + 0.011*"needs" + 0.007*"Derby" + 0.007*"quality" + 0.006*"need" + 0.006*"receive" + 0.006*"good" + 0.005*"well" + 0.005*"appropriate" + 0.005*"plans"', '0.024*"’" + 0.010*"needs" + 0.007*"Derby" + 0.006*"leaders" + 0.006*"quality" + 0.006*"receive" + 0.006*"views" + 0.006*"progress" + 0.006*"well" + 0.006*"plans"']</t>
+    <t>['0.021*"’" + 0.010*"needs" + 0.009*"Derby" + 0.007*"receive" + 0.006*"plans" + 0.006*"appropriate" + 0.006*"progress" + 0.006*"quality" + 0.006*"leaders" + 0.005*"good"', '0.022*"’" + 0.009*"needs" + 0.006*"Derby" + 0.006*"quality" + 0.006*"well" + 0.005*"plans" + 0.005*"need" + 0.005*"receive" + 0.005*"leaders" + 0.005*"good"', '0.020*"’" + 0.009*"needs" + 0.007*"quality" + 0.007*"receive" + 0.006*"Derby" + 0.006*"well" + 0.006*"good" + 0.006*"progress" + 0.005*"need" + 0.005*"oversight"']</t>
   </si>
   <si>
     <t>80460</t>
@@ -1105,7 +1105,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.008*"Derbyshire" + 0.006*"need" + 0.005*"education" + 0.005*"good" + 0.005*"10" + 0.005*"plans" + 0.005*"effective" + 0.005*"leaders"', '0.012*"’" + 0.007*"well" + 0.005*"education" + 0.005*"positive" + 0.004*"plans" + 0.004*"health" + 0.004*"Derbyshire" + 0.004*"needs" + 0.004*"effective" + 0.004*"good"', '0.012*"’" + 0.008*"well" + 0.007*"Derbyshire" + 0.005*"plans" + 0.005*"needs" + 0.005*"health" + 0.005*"October" + 0.004*"positive" + 0.004*"leaders" + 0.004*"10"']</t>
+    <t>['0.011*"’" + 0.007*"well" + 0.006*"plans" + 0.005*"Derbyshire" + 0.005*"2023" + 0.004*"need" + 0.004*"effective" + 0.004*"good" + 0.004*"education" + 0.004*"30"', '0.016*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.006*"needs" + 0.006*"10" + 0.005*"plans" + 0.005*"health" + 0.005*"education" + 0.005*"positive" + 0.005*"good"', '0.015*"’" + 0.008*"well" + 0.008*"Derbyshire" + 0.006*"leaders" + 0.005*"positive" + 0.005*"need" + 0.005*"effective" + 0.004*"number" + 0.004*"needs" + 0.004*"November"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1138,7 +1138,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"well" + 0.006*"health" + 0.005*"risk" + 0.005*"leaders" + 0.005*"case" + 0.004*"progress" + 0.004*"protection" + 0.004*"time" + 0.004*"Devon"', '0.009*"’" + 0.005*"well" + 0.005*"leaders" + 0.004*"health" + 0.004*"protection" + 0.004*"living" + 0.004*"progress" + 0.004*"risk" + 0.004*"including" + 0.004*"plans"', '0.007*"’" + 0.004*"well" + 0.004*"progress" + 0.004*"Devon" + 0.004*"risk" + 0.004*"leaders" + 0.004*"areas" + 0.004*"risks" + 0.004*"need" + 0.003*"health"']</t>
+    <t>['0.008*"’" + 0.005*"well" + 0.004*"leaders" + 0.004*"risk" + 0.004*"health" + 0.004*"protection" + 0.003*"need" + 0.003*"Devon" + 0.003*"risks" + 0.003*"lack"', '0.011*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"health" + 0.005*"leaders" + 0.005*"risk" + 0.004*"case" + 0.004*"protection" + 0.004*"time" + 0.004*"plans"', '0.008*"’" + 0.007*"well" + 0.005*"health" + 0.005*"risk" + 0.005*"progress" + 0.005*"leaders" + 0.005*"early" + 0.004*"Devon" + 0.004*"living" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1177,7 +1177,7 @@
     <t>0.1841</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.005*"Doncaster" + 0.005*"well" + 0.004*"leaders" + 0.004*"many" + 0.004*"Trust" + 0.004*"quality" + 0.004*"25" + 0.004*"progress" + 0.004*"experiences"', '0.023*"’" + 0.008*"well" + 0.007*"Doncaster" + 0.006*"many" + 0.005*"records" + 0.005*"plans" + 0.005*"leaders" + 0.005*"progress" + 0.005*"effective" + 0.005*"oversight"', '0.022*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"leaders" + 0.005*"records" + 0.005*"Doncaster" + 0.005*"arrangements" + 0.005*"quality" + 0.004*"information" + 0.004*"oversight"']</t>
+    <t>['0.021*"’" + 0.006*"progress" + 0.006*"Doncaster" + 0.005*"well" + 0.005*"February" + 0.005*"leaders" + 0.004*"information" + 0.004*"14" + 0.004*"quality" + 0.004*"oversight"', '0.019*"’" + 0.007*"well" + 0.006*"Doncaster" + 0.006*"many" + 0.006*"leaders" + 0.005*"plans" + 0.005*"records" + 0.005*"arrangements" + 0.005*"quality" + 0.005*"protection"', '0.020*"’" + 0.006*"well" + 0.005*"Doncaster" + 0.005*"records" + 0.004*"quality" + 0.004*"many" + 0.004*"effective" + 0.004*"protection" + 0.004*"progress" + 0.004*"information"']</t>
   </si>
   <si>
     <t>2532283</t>
@@ -1210,7 +1210,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"Dorset" + 0.005*"good" + 0.004*"well" + 0.003*"arrangements" + 0.003*"leaders" + 0.003*"needs" + 0.003*"September" + 0.003*"supported" + 0.003*"27"', '0.014*"’" + 0.008*"Dorset" + 0.006*"good" + 0.005*"well" + 0.005*"arrangements" + 0.004*"pandemic" + 0.004*"needs" + 0.004*"including" + 0.004*"8" + 0.004*"leaders"', '0.016*"’" + 0.008*"Dorset" + 0.007*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"impact" + 0.005*"8" + 0.005*"change" + 0.005*"2021" + 0.004*"arrangements"']</t>
+    <t>['0.016*"’" + 0.007*"Dorset" + 0.007*"good" + 0.006*"well" + 0.005*"arrangements" + 0.004*"leaders" + 0.004*"8" + 0.004*"change" + 0.004*"27" + 0.004*"October"', '0.012*"’" + 0.008*"Dorset" + 0.006*"well" + 0.005*"good" + 0.005*"quality" + 0.005*"needs" + 0.004*"8" + 0.004*"impact" + 0.004*"protection" + 0.004*"health"', '0.012*"’" + 0.008*"Dorset" + 0.006*"good" + 0.005*"well" + 0.005*"needs" + 0.004*"2021" + 0.004*"September" + 0.004*"27" + 0.004*"including" + 0.004*"arrangements"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1240,7 +1240,7 @@
     <t>13/01/23</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.012*"needs" + 0.009*"Dudley" + 0.006*"well" + 0.006*"arrangements" + 0.006*"always" + 0.005*"plans" + 0.005*"oversight" + 0.005*"practice" + 0.004*"enough"', '0.014*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.005*"plans" + 0.005*"always" + 0.005*"well" + 0.004*"quality" + 0.004*"ensure" + 0.004*"11" + 0.004*"experiences"', '0.013*"’" + 0.011*"needs" + 0.007*"Dudley" + 0.005*"arrangements" + 0.005*"well" + 0.005*"ensure" + 0.005*"plans" + 0.005*"31" + 0.005*"However" + 0.005*"always"']</t>
+    <t>['0.014*"’" + 0.010*"needs" + 0.008*"Dudley" + 0.006*"always" + 0.006*"well" + 0.005*"plans" + 0.005*"arrangements" + 0.004*"October" + 0.004*"However" + 0.004*"2022"', '0.015*"’" + 0.012*"needs" + 0.006*"Dudley" + 0.005*"well" + 0.005*"arrangements" + 0.005*"always" + 0.004*"31" + 0.004*"11" + 0.004*"plans" + 0.004*"oversight"', '0.015*"’" + 0.011*"needs" + 0.009*"Dudley" + 0.006*"ensure" + 0.006*"arrangements" + 0.005*"well" + 0.005*"oversight" + 0.005*"quality" + 0.005*"plans" + 0.004*"management"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1279,7 +1279,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"needs" + 0.008*"May" + 0.007*"Durham" + 0.007*"plans" + 0.006*"practice" + 0.006*"well" + 0.005*"ensure" + 0.005*"family" + 0.004*"carers"', '0.012*"’" + 0.010*"needs" + 0.006*"plans" + 0.006*"well" + 0.005*"ensure" + 0.005*"May" + 0.005*"practice" + 0.005*"10" + 0.005*"number" + 0.004*"Durham"', '0.017*"’" + 0.009*"needs" + 0.009*"Durham" + 0.008*"well" + 0.007*"May" + 0.006*"ensure" + 0.006*"plans" + 0.005*"risks" + 0.005*"leaders" + 0.005*"robust"']</t>
+    <t>['0.012*"’" + 0.011*"needs" + 0.008*"May" + 0.007*"well" + 0.006*"plans" + 0.006*"Durham" + 0.005*"ensure" + 0.004*"practice" + 0.004*"family" + 0.004*"10"', '0.015*"’" + 0.011*"needs" + 0.007*"May" + 0.007*"well" + 0.007*"ensure" + 0.006*"Durham" + 0.006*"plans" + 0.005*"practice" + 0.005*"number" + 0.005*"supported"', '0.015*"’" + 0.010*"needs" + 0.009*"Durham" + 0.007*"plans" + 0.006*"well" + 0.006*"May" + 0.005*"practice" + 0.005*"ensure" + 0.005*"making" + 0.004*"risks"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1318,7 +1318,7 @@
     <t>0.1646</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"needs" + 0.009*"plans" + 0.007*"well" + 0.007*"Riding" + 0.007*"progress" + 0.006*"East" + 0.005*"2023" + 0.005*"good" + 0.004*"practice"', '0.017*"’" + 0.011*"well" + 0.010*"needs" + 0.009*"plans" + 0.008*"progress" + 0.008*"East" + 0.006*"Riding" + 0.006*"10" + 0.005*"30" + 0.005*"place"', '0.013*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"progress" + 0.005*"well" + 0.005*"Riding" + 0.004*"East" + 0.004*"quality" + 0.004*"education" + 0.004*"10"']</t>
+    <t>['0.011*"’" + 0.008*"plans" + 0.007*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"partners" + 0.005*"Riding" + 0.005*"East" + 0.005*"good" + 0.005*"30"', '0.019*"’" + 0.011*"needs" + 0.009*"well" + 0.009*"plans" + 0.008*"progress" + 0.007*"East" + 0.006*"Riding" + 0.005*"January" + 0.005*"February" + 0.005*"10"', '0.017*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.007*"Riding" + 0.006*"progress" + 0.005*"East" + 0.004*"10" + 0.004*"30" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1351,7 +1351,7 @@
     <t>0.1738</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"East" + 0.005*"progress" + 0.005*"impact" + 0.005*"effective" + 0.005*"Sussex" + 0.005*"experiences"', '0.020*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.007*"East" + 0.006*"progress" + 0.006*"Sussex" + 0.006*"11" + 0.005*"including" + 0.005*"provide"', '0.013*"’" + 0.010*"well" + 0.008*"plans" + 0.007*"Sussex" + 0.007*"progress" + 0.006*"needs" + 0.006*"including" + 0.006*"East" + 0.006*"impact" + 0.005*"relationships"']</t>
+    <t>['0.020*"’" + 0.010*"well" + 0.009*"plans" + 0.008*"needs" + 0.007*"Sussex" + 0.007*"impact" + 0.006*"including" + 0.006*"progress" + 0.005*"East" + 0.005*"provide"', '0.015*"’" + 0.009*"well" + 0.008*"East" + 0.007*"plans" + 0.007*"needs" + 0.007*"progress" + 0.006*"Sussex" + 0.005*"including" + 0.005*"provide" + 0.005*"effective"', '0.013*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"progress" + 0.005*"East" + 0.005*"11" + 0.004*"impact" + 0.004*"including" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1390,7 +1390,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"well" + 0.007*"progress" + 0.006*"needs" + 0.006*"plans" + 0.005*"family" + 0.005*"risk" + 0.005*"understand" + 0.005*"Essex" + 0.004*"‘"', '0.019*"’" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"family" + 0.005*"progress" + 0.005*"helped" + 0.004*"risk" + 0.004*"30" + 0.004*"need"', '0.021*"’" + 0.007*"progress" + 0.006*"needs" + 0.006*"well" + 0.005*"experiences" + 0.005*"Essex" + 0.005*"plans" + 0.005*"supported" + 0.005*"parents" + 0.005*"understand"']</t>
+    <t>['0.012*"’" + 0.006*"progress" + 0.006*"well" + 0.005*"Essex" + 0.005*"plans" + 0.004*"understand" + 0.004*"needs" + 0.004*"experiences" + 0.004*"family" + 0.004*"new"', '0.020*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"progress" + 0.006*"leaders" + 0.006*"family" + 0.006*"plans" + 0.005*"supported" + 0.005*"experiences" + 0.005*"new"', '0.019*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"progress" + 0.006*"needs" + 0.005*"risk" + 0.005*"practice" + 0.005*"‘" + 0.005*"Essex" + 0.005*"parents"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1429,7 +1429,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"effective" + 0.006*"quality" + 0.006*"good" + 0.005*"timely" + 0.005*"well" + 0.005*"practice" + 0.004*"need" + 0.004*"progress" + 0.004*"needs"', '0.012*"’" + 0.010*"effective" + 0.007*"practice" + 0.007*"quality" + 0.006*"good" + 0.006*"needs" + 0.006*"well" + 0.005*"need" + 0.005*"home" + 0.004*"timely"', '0.013*"’" + 0.008*"effective" + 0.008*"good" + 0.007*"needs" + 0.006*"practice" + 0.006*"timely" + 0.006*"well" + 0.005*"improve" + 0.005*"quality" + 0.005*"progress"']</t>
+    <t>['0.014*"’" + 0.009*"effective" + 0.007*"practice" + 0.007*"quality" + 0.007*"needs" + 0.006*"good" + 0.006*"timely" + 0.005*"well" + 0.005*"early" + 0.004*"progress"', '0.014*"’" + 0.009*"effective" + 0.008*"good" + 0.007*"practice" + 0.007*"quality" + 0.006*"needs" + 0.006*"improve" + 0.006*"well" + 0.005*"timely" + 0.005*"team"', '0.012*"’" + 0.006*"effective" + 0.006*"good" + 0.005*"well" + 0.005*"need" + 0.004*"needs" + 0.004*"plans" + 0.004*"timely" + 0.004*"practice" + 0.004*"home"']</t>
   </si>
   <si>
     <t>80470</t>
@@ -1465,7 +1465,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.010*"needs" + 0.007*"plans" + 0.007*"February" + 0.006*"2022" + 0.006*"well" + 0.005*"appropriate" + 0.005*"18" + 0.005*"protection" + 0.004*"good"', '0.019*"’" + 0.008*"2022" + 0.007*"needs" + 0.007*"plans" + 0.007*"February" + 0.006*"progress" + 0.006*"well" + 0.005*"Gloucestershire" + 0.005*"protection" + 0.005*"timely"', '0.013*"’" + 0.008*"needs" + 0.006*"February" + 0.006*"2022" + 0.006*"experienced" + 0.005*"plans" + 0.005*"good" + 0.005*"progress" + 0.005*"leaders" + 0.005*"Gloucestershire"']</t>
+    <t>['0.012*"’" + 0.006*"2022" + 0.006*"needs" + 0.005*"February" + 0.005*"Gloucestershire" + 0.005*"good" + 0.004*"plans" + 0.004*"18" + 0.004*"experienced" + 0.004*"well"', '0.020*"’" + 0.011*"needs" + 0.007*"2022" + 0.007*"February" + 0.006*"plans" + 0.005*"progress" + 0.005*"leaders" + 0.005*"experienced" + 0.005*"appropriate" + 0.005*"protection"', '0.019*"’" + 0.008*"plans" + 0.008*"well" + 0.007*"February" + 0.007*"needs" + 0.006*"2022" + 0.006*"Gloucestershire" + 0.005*"18" + 0.005*"appropriate" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1495,7 +1495,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"well" + 0.009*"practice" + 0.008*"risk" + 0.007*"need" + 0.007*"plans" + 0.007*"needs" + 0.006*"planning" + 0.006*"always" + 0.005*"However"', '0.012*"’" + 0.011*"well" + 0.007*"needs" + 0.007*"plans" + 0.007*"practice" + 0.007*"planning" + 0.007*"good" + 0.006*"risk" + 0.006*"need" + 0.006*"quality"', '0.010*"’" + 0.010*"needs" + 0.009*"well" + 0.008*"practice" + 0.007*"plans" + 0.007*"good" + 0.006*"effective" + 0.006*"quality" + 0.006*"need" + 0.006*"always"']</t>
+    <t>['0.009*"well" + 0.009*"practice" + 0.009*"’" + 0.007*"risk" + 0.007*"plans" + 0.006*"planning" + 0.006*"good" + 0.006*"need" + 0.006*"needs" + 0.006*"effective"', '0.013*"’" + 0.011*"well" + 0.007*"plans" + 0.007*"risk" + 0.007*"practice" + 0.006*"needs" + 0.006*"always" + 0.005*"quality" + 0.005*"planning" + 0.005*"effective"', '0.013*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"need" + 0.008*"practice" + 0.007*"plans" + 0.007*"good" + 0.006*"planning" + 0.006*"effective" + 0.006*"risk"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1522,7 +1522,7 @@
     <t>0.1893</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"needs" + 0.006*"plans" + 0.005*"quality" + 0.005*"strong" + 0.005*"well" + 0.004*"leaders" + 0.004*"home" + 0.004*"health" + 0.004*"Hampshire"', '0.023*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"plans" + 0.004*"quality" + 0.004*"highly" + 0.004*"Hampshire" + 0.004*"leaders" + 0.004*"carers" + 0.003*"home"', '0.018*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"strong" + 0.005*"leaders" + 0.005*"plans" + 0.005*"improve" + 0.004*"home" + 0.004*"decisions" + 0.004*"need"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.005*"well" + 0.005*"improve" + 0.004*"leaders" + 0.004*"plans" + 0.004*"quality" + 0.004*"highly" + 0.003*"practice" + 0.003*"Hampshire"', '0.017*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.004*"quality" + 0.004*"leaders" + 0.004*"strong" + 0.004*"highly" + 0.004*"home" + 0.004*"health"', '0.023*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"well" + 0.005*"strong" + 0.005*"quality" + 0.005*"home" + 0.004*"leaders" + 0.004*"need" + 0.004*"Hampshire"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1558,7 +1558,7 @@
     <t>0.2081</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"well" + 0.006*"quality" + 0.005*"strong" + 0.005*"plans" + 0.005*"progress" + 0.004*"practice" + 0.004*"needs" + 0.004*"good" + 0.004*"timely"', '0.020*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"good" + 0.005*"plans" + 0.005*"strong" + 0.005*"progress" + 0.004*"early" + 0.004*"need" + 0.004*"education"', '0.012*"’" + 0.008*"well" + 0.006*"strong" + 0.006*"quality" + 0.005*"good" + 0.004*"impact" + 0.004*"needs" + 0.004*"timely" + 0.004*"practice" + 0.003*"health"']</t>
+    <t>['0.018*"’" + 0.011*"well" + 0.008*"quality" + 0.007*"strong" + 0.005*"plans" + 0.005*"good" + 0.004*"education" + 0.004*"practice" + 0.004*"improve" + 0.004*"needs"', '0.014*"’" + 0.008*"well" + 0.006*"quality" + 0.005*"good" + 0.004*"progress" + 0.004*"early" + 0.004*"plans" + 0.004*"impact" + 0.004*"timely" + 0.004*"education"', '0.015*"’" + 0.007*"well" + 0.006*"quality" + 0.005*"good" + 0.005*"strong" + 0.004*"progress" + 0.004*"early" + 0.004*"need" + 0.004*"health" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80474</t>
@@ -1591,7 +1591,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.007*"practice" + 0.006*"needs" + 0.005*"lack" + 0.005*"Herefordshire" + 0.005*"impact" + 0.004*"agency" + 0.004*"18" + 0.004*"progress" + 0.004*"plans"', '0.011*"’" + 0.006*"Herefordshire" + 0.005*"many" + 0.005*"quality" + 0.005*"lack" + 0.004*"practice" + 0.004*"impact" + 0.004*"oversight" + 0.004*"agency" + 0.004*"ensure"', '0.016*"’" + 0.005*"impact" + 0.005*"Herefordshire" + 0.005*"lack" + 0.005*"practice" + 0.005*"many" + 0.004*"plans" + 0.004*"18" + 0.004*"across" + 0.004*"management"']</t>
+    <t>['0.019*"’" + 0.006*"impact" + 0.006*"practice" + 0.005*"lack" + 0.005*"Herefordshire" + 0.005*"needs" + 0.005*"many" + 0.005*"18" + 0.005*"quality" + 0.005*"plans"', '0.016*"’" + 0.006*"practice" + 0.006*"Herefordshire" + 0.005*"lack" + 0.005*"needs" + 0.005*"progress" + 0.004*"2022" + 0.004*"agency" + 0.004*"29" + 0.004*"many"', '0.016*"’" + 0.004*"Herefordshire" + 0.004*"oversight" + 0.004*"impact" + 0.004*"many" + 0.004*"plans" + 0.004*"need" + 0.004*"practice" + 0.003*"management" + 0.003*"lack"']</t>
   </si>
   <si>
     <t>80475</t>
@@ -1624,7 +1624,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"Hertfordshire" + 0.006*"plans" + 0.005*"need" + 0.005*"receive" + 0.004*"risk" + 0.004*"‘" + 0.004*"23"', '0.019*"’" + 0.006*"Hertfordshire" + 0.005*"well" + 0.005*"needs" + 0.004*"receive" + 0.004*"plans" + 0.004*"effective" + 0.004*"risk" + 0.004*"January" + 0.004*"positive"', '0.024*"’" + 0.008*"Hertfordshire" + 0.006*"needs" + 0.006*"receive" + 0.006*"well" + 0.004*"leaders" + 0.004*"2023" + 0.004*"family" + 0.004*"27" + 0.004*"23"']</t>
+    <t>['0.022*"’" + 0.006*"Hertfordshire" + 0.006*"well" + 0.006*"needs" + 0.005*"receive" + 0.004*"2023" + 0.004*"risk" + 0.004*"plans" + 0.004*"leaders" + 0.004*"23"', '0.023*"’" + 0.007*"well" + 0.006*"Hertfordshire" + 0.006*"needs" + 0.006*"receive" + 0.005*"plans" + 0.005*"27" + 0.005*"23" + 0.004*"2023" + 0.004*"leaders"', '0.023*"’" + 0.007*"needs" + 0.006*"Hertfordshire" + 0.005*"well" + 0.005*"need" + 0.005*"receive" + 0.004*"positive" + 0.004*"January" + 0.004*"plans" + 0.004*"Leaders"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1654,7 +1654,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"leaders" + 0.005*"plans" + 0.005*"30" + 0.005*"well" + 0.005*"protection" + 0.005*"practice" + 0.004*"supported" + 0.004*"Senior" + 0.004*"November"', '0.015*"’" + 0.010*"leaders" + 0.006*"needs" + 0.005*"3" + 0.005*"November" + 0.005*"plans" + 0.005*"progress" + 0.005*"practice" + 0.005*"improve" + 0.005*"Senior"', '0.022*"’" + 0.009*"leaders" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"Isle" + 0.006*"Wight" + 0.005*"PAs" + 0.005*"good" + 0.005*"supported"']</t>
+    <t>['0.016*"’" + 0.007*"leaders" + 0.005*"Isle" + 0.005*"practice" + 0.005*"needs" + 0.005*"progress" + 0.005*"well" + 0.005*"plans" + 0.005*"time" + 0.005*"Wight"', '0.016*"’" + 0.010*"leaders" + 0.007*"needs" + 0.006*"PAs" + 0.006*"3" + 0.006*"Senior" + 0.006*"well" + 0.005*"supported" + 0.005*"protection" + 0.005*"Wight"', '0.020*"’" + 0.008*"leaders" + 0.006*"well" + 0.005*"supported" + 0.005*"plans" + 0.005*"improve" + 0.005*"Wight" + 0.005*"practice" + 0.005*"Isle" + 0.005*"needs"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1678,7 +1678,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"Kent" + 0.005*"Council" + 0.004*"needs" + 0.004*"supported" + 0.004*"practice" + 0.003*"progress" + 0.003*"impact" + 0.003*"well" + 0.003*"arrangements"', '0.021*"’" + 0.012*"Kent" + 0.009*"needs" + 0.007*"supported" + 0.006*"well" + 0.006*"progress" + 0.005*"Council" + 0.005*"County" + 0.005*"including" + 0.004*"practice"', '0.020*"’" + 0.009*"Kent" + 0.007*"well" + 0.007*"needs" + 0.007*"Council" + 0.006*"County" + 0.005*"supported" + 0.005*"practice" + 0.004*"plans" + 0.004*"leaders"']</t>
+    <t>['0.016*"’" + 0.010*"Kent" + 0.008*"needs" + 0.006*"practice" + 0.006*"Council" + 0.005*"supported" + 0.005*"well" + 0.004*"including" + 0.004*"leaders" + 0.004*"County"', '0.020*"’" + 0.009*"Kent" + 0.009*"needs" + 0.007*"Council" + 0.006*"supported" + 0.005*"well" + 0.004*"County" + 0.004*"ensure" + 0.004*"progress" + 0.004*"May"', '0.018*"’" + 0.010*"Kent" + 0.008*"well" + 0.006*"County" + 0.005*"supported" + 0.005*"progress" + 0.005*"needs" + 0.005*"Council" + 0.005*"leaders" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1708,7 +1708,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"need" + 0.007*"practice" + 0.006*"protection" + 0.006*"Hull" + 0.006*"planning" + 0.006*"number" + 0.006*"well" + 0.006*"impact" + 0.006*"risks"', '0.014*"’" + 0.006*"number" + 0.006*"planning" + 0.006*"oversight" + 0.006*"protection" + 0.005*"agency" + 0.005*"Hull" + 0.005*"well" + 0.005*"14" + 0.005*"management"', '0.019*"’" + 0.008*"number" + 0.007*"planning" + 0.006*"well" + 0.006*"management" + 0.006*"practice" + 0.005*"protection" + 0.005*"small" + 0.005*"risks" + 0.005*"progress"']</t>
+    <t>['0.012*"’" + 0.007*"planning" + 0.006*"number" + 0.006*"management" + 0.006*"well" + 0.006*"protection" + 0.006*"Hull" + 0.005*"need" + 0.005*"small" + 0.005*"needs"', '0.021*"’" + 0.007*"need" + 0.007*"Hull" + 0.006*"practice" + 0.006*"oversight" + 0.006*"planning" + 0.006*"risks" + 0.006*"protection" + 0.006*"number" + 0.005*"well"', '0.013*"’" + 0.008*"number" + 0.007*"practice" + 0.006*"planning" + 0.006*"well" + 0.005*"protection" + 0.005*"25" + 0.005*"November" + 0.004*"risks" + 0.004*"small"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1741,7 +1741,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"practice" + 0.006*"quality" + 0.006*"needs" + 0.005*"good" + 0.005*"well" + 0.005*"protection" + 0.005*"training" + 0.004*"senior" + 0.004*"risk"', '0.014*"’" + 0.007*"quality" + 0.007*"good" + 0.007*"practice" + 0.006*"permanence" + 0.006*"plans" + 0.006*"Senior" + 0.005*"well" + 0.005*"senior" + 0.005*"training"', '0.010*"’" + 0.006*"quality" + 0.005*"good" + 0.005*"practice" + 0.005*"need" + 0.004*"well" + 0.004*"protection" + 0.004*"plans" + 0.004*"training" + 0.004*"team"']</t>
+    <t>['0.013*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"well" + 0.006*"needs" + 0.006*"good" + 0.006*"Senior" + 0.005*"plans" + 0.005*"protection" + 0.005*"last"', '0.011*"’" + 0.005*"good" + 0.005*"quality" + 0.005*"training" + 0.005*"plans" + 0.005*"practice" + 0.005*"protection" + 0.004*"well" + 0.004*"team" + 0.004*"senior"', '0.010*"’" + 0.006*"permanence" + 0.006*"practice" + 0.006*"good" + 0.006*"quality" + 0.004*"senior" + 0.004*"plans" + 0.004*"Senior" + 0.004*"training" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1783,7 +1783,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"progress" + 0.008*"plans" + 0.007*"needs" + 0.006*"quality" + 0.006*"2021" + 0.006*"good" + 0.006*"Knowsley" + 0.005*"abuse" + 0.005*"need"', '0.011*"’" + 0.008*"progress" + 0.007*"plans" + 0.006*"needs" + 0.006*"Knowsley" + 0.005*"11" + 0.005*"quality" + 0.005*"impact" + 0.005*"2021" + 0.005*"experiences"', '0.017*"’" + 0.008*"progress" + 0.008*"quality" + 0.008*"needs" + 0.006*"plans" + 0.006*"Knowsley" + 0.006*"22" + 0.006*"2021" + 0.005*"experiences" + 0.005*"need"']</t>
+    <t>['0.017*"’" + 0.010*"progress" + 0.009*"needs" + 0.007*"quality" + 0.007*"plans" + 0.006*"2021" + 0.006*"good" + 0.006*"Knowsley" + 0.005*"domestic" + 0.005*"need"', '0.013*"’" + 0.006*"progress" + 0.006*"quality" + 0.006*"Knowsley" + 0.005*"plans" + 0.005*"need" + 0.005*"2021" + 0.005*"October" + 0.004*"effective" + 0.004*"experiences"', '0.013*"’" + 0.009*"plans" + 0.008*"progress" + 0.008*"needs" + 0.007*"quality" + 0.006*"Knowsley" + 0.006*"experiences" + 0.006*"2021" + 0.005*"abuse" + 0.005*"22"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1816,7 +1816,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"well" + 0.007*"need" + 0.006*"Lancashire" + 0.006*"health" + 0.005*"needs" + 0.005*"28" + 0.005*"supported" + 0.005*"live" + 0.004*"homes"', '0.018*"’" + 0.009*"needs" + 0.009*"well" + 0.007*"need" + 0.006*"Lancashire" + 0.006*"plans" + 0.006*"practice" + 0.006*"positive" + 0.005*"live" + 0.005*"number"', '0.016*"’" + 0.009*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"supported" + 0.005*"homes" + 0.005*"Lancashire" + 0.005*"plans" + 0.005*"practice" + 0.005*"positive"']</t>
+    <t>['0.019*"’" + 0.008*"well" + 0.008*"need" + 0.008*"needs" + 0.006*"plans" + 0.006*"Lancashire" + 0.005*"health" + 0.005*"information" + 0.005*"supported" + 0.005*"9"', '0.016*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"Lancashire" + 0.006*"need" + 0.006*"supported" + 0.006*"practice" + 0.005*"live" + 0.005*"homes" + 0.005*"progress"', '0.013*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"Lancashire" + 0.006*"need" + 0.006*"positive" + 0.005*"plans" + 0.004*"supported" + 0.004*"homes" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80481</t>
@@ -1846,7 +1846,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"needs" + 0.007*"Leeds" + 0.006*"well" + 0.005*"risk" + 0.005*"4" + 0.005*"practice" + 0.004*"ensure" + 0.004*"plans" + 0.004*"March"', '0.011*"’" + 0.006*"Leeds" + 0.005*"ensure" + 0.004*"needs" + 0.004*"risk" + 0.004*"protection" + 0.004*"well" + 0.004*"February" + 0.004*"21" + 0.003*"practice"', '0.018*"’" + 0.008*"Leeds" + 0.007*"needs" + 0.006*"well" + 0.006*"risk" + 0.005*"supported" + 0.005*"protection" + 0.005*"plans" + 0.005*"practice" + 0.004*"2022"']</t>
+    <t>['0.017*"’" + 0.009*"Leeds" + 0.008*"needs" + 0.006*"risk" + 0.006*"well" + 0.004*"21" + 0.004*"ensure" + 0.004*"practice" + 0.004*"protection" + 0.004*"supported"', '0.017*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"risk" + 0.005*"supported" + 0.005*"4" + 0.005*"protection" + 0.004*"practice" + 0.004*"plans"', '0.014*"’" + 0.006*"Leeds" + 0.006*"needs" + 0.006*"well" + 0.005*"March" + 0.005*"practice" + 0.005*"ensure" + 0.004*"making" + 0.004*"4" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1882,7 +1882,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"well" + 0.008*"2021" + 0.007*"Leicester" + 0.007*"needs" + 0.006*"good" + 0.006*"20" + 0.005*"Council" + 0.005*"ensure" + 0.005*"including"', '0.022*"’" + 0.008*"well" + 0.008*"Leicester" + 0.008*"2021" + 0.007*"needs" + 0.006*"ensure" + 0.006*"1" + 0.005*"good" + 0.005*"improve" + 0.005*"including"', '0.016*"’" + 0.009*"2021" + 0.008*"well" + 0.008*"Leicester" + 0.007*"number" + 0.006*"good" + 0.006*"needs" + 0.006*"ensure" + 0.005*"1" + 0.005*"high"']</t>
+    <t>['0.021*"’" + 0.010*"well" + 0.009*"2021" + 0.009*"Leicester" + 0.007*"needs" + 0.006*"good" + 0.006*"1" + 0.005*"ensure" + 0.005*"20" + 0.004*"October"', '0.014*"’" + 0.008*"well" + 0.007*"Leicester" + 0.007*"needs" + 0.006*"2021" + 0.006*"good" + 0.005*"number" + 0.005*"ensure" + 0.004*"City" + 0.004*"including"', '0.022*"’" + 0.009*"2021" + 0.008*"well" + 0.007*"Leicester" + 0.006*"needs" + 0.006*"ensure" + 0.006*"number" + 0.006*"good" + 0.006*"20" + 0.005*"1"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1918,7 +1918,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"good" + 0.006*"effective" + 0.006*"quality" + 0.005*"practice" + 0.005*"education" + 0.004*"impact" + 0.004*"leaders"', '0.012*"’" + 0.009*"well" + 0.008*"good" + 0.007*"effective" + 0.006*"needs" + 0.006*"quality" + 0.005*"impact" + 0.005*"need" + 0.005*"risk" + 0.005*"practice"', '0.012*"’" + 0.008*"good" + 0.007*"needs" + 0.006*"well" + 0.006*"practice" + 0.006*"quality" + 0.006*"effective" + 0.005*"education" + 0.005*"need" + 0.005*"impact"']</t>
+    <t>['0.009*"’" + 0.006*"good" + 0.006*"well" + 0.005*"needs" + 0.005*"quality" + 0.005*"impact" + 0.005*"education" + 0.004*"practice" + 0.004*"effective" + 0.004*"leaders"', '0.014*"’" + 0.009*"good" + 0.009*"well" + 0.008*"effective" + 0.007*"needs" + 0.006*"practice" + 0.006*"need" + 0.005*"quality" + 0.005*"impact" + 0.005*"education"', '0.009*"’" + 0.007*"well" + 0.007*"quality" + 0.007*"needs" + 0.006*"good" + 0.006*"effective" + 0.005*"practice" + 0.004*"impact" + 0.004*"need" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1951,7 +1951,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.004*"family" + 0.004*"plans" + 0.004*"28" + 0.004*"24" + 0.004*"April" + 0.004*"education"', '0.024*"’" + 0.008*"Lincolnshire" + 0.006*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"family" + 0.004*"progress" + 0.004*"24" + 0.004*"2023" + 0.004*"working"', '0.020*"’" + 0.007*"needs" + 0.006*"Lincolnshire" + 0.006*"progress" + 0.005*"well" + 0.005*"plans" + 0.004*"need" + 0.004*"family" + 0.004*"24" + 0.004*"effective"']</t>
+    <t>['0.019*"’" + 0.007*"Lincolnshire" + 0.007*"well" + 0.005*"needs" + 0.004*"plans" + 0.004*"family" + 0.004*"progress" + 0.004*"education" + 0.004*"April" + 0.004*"number"', '0.019*"’" + 0.007*"needs" + 0.007*"Lincolnshire" + 0.005*"plans" + 0.005*"family" + 0.004*"need" + 0.004*"well" + 0.004*"24" + 0.004*"28" + 0.004*"education"', '0.025*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"plans" + 0.005*"24" + 0.004*"family" + 0.004*"effective" + 0.004*"28"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1984,7 +1984,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"needs" + 0.007*"practice" + 0.007*"always" + 0.006*"need" + 0.005*"Liverpool" + 0.005*"quality" + 0.004*"met" + 0.004*"13" + 0.004*"timely"', '0.020*"’" + 0.007*"need" + 0.007*"practice" + 0.007*"Liverpool" + 0.007*"protection" + 0.006*"needs" + 0.006*"always" + 0.006*"quality" + 0.005*"harm" + 0.004*"13"', '0.016*"’" + 0.008*"needs" + 0.006*"always" + 0.006*"quality" + 0.005*"practice" + 0.005*"met" + 0.005*"need" + 0.005*"Liverpool" + 0.004*"senior" + 0.004*"24"']</t>
+    <t>['0.018*"’" + 0.006*"quality" + 0.006*"needs" + 0.006*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"Liverpool" + 0.005*"met" + 0.005*"protection" + 0.004*"24"', '0.023*"’" + 0.008*"needs" + 0.007*"practice" + 0.007*"need" + 0.007*"always" + 0.006*"Liverpool" + 0.005*"13" + 0.005*"quality" + 0.005*"protection" + 0.005*"24"', '0.015*"’" + 0.007*"needs" + 0.006*"need" + 0.006*"always" + 0.006*"Liverpool" + 0.006*"practice" + 0.005*"quality" + 0.005*"PAs" + 0.005*"protection" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -2020,7 +2020,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"good" + 0.005*"information" + 0.005*"carers" + 0.005*"progress" + 0.004*"practice" + 0.004*"well" + 0.004*"10"', '0.020*"’" + 0.006*"needs" + 0.006*"good" + 0.005*"plans" + 0.005*"well" + 0.005*"progress" + 0.005*"information" + 0.005*"carers" + 0.005*"practice" + 0.004*"planning"', '0.025*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"good" + 0.005*"carers" + 0.005*"well" + 0.005*"practice" + 0.005*"e" + 0.005*"ensure" + 0.005*"21"']</t>
+    <t>['0.020*"’" + 0.009*"needs" + 0.005*"good" + 0.005*"ensure" + 0.005*"carers" + 0.005*"practice" + 0.005*"10" + 0.004*"plans" + 0.004*"Barking" + 0.004*"e"', '0.021*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"information" + 0.005*"practice" + 0.004*"progress" + 0.004*"planning" + 0.004*"e"', '0.025*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"carers" + 0.006*"good" + 0.005*"21" + 0.005*"information" + 0.005*"progress" + 0.004*"practice" + 0.004*"London"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -2059,7 +2059,7 @@
     <t>0.2188</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"good" + 0.011*"needs" + 0.008*"well" + 0.008*"progress" + 0.008*"need" + 0.007*"plans" + 0.007*"ensure" + 0.006*"clear" + 0.005*"effective"', '0.016*"’" + 0.010*"well" + 0.009*"needs" + 0.009*"need" + 0.007*"good" + 0.006*"risk" + 0.006*"clear" + 0.005*"carers" + 0.005*"ensure" + 0.005*"quality"', '0.008*"’" + 0.007*"well" + 0.007*"good" + 0.006*"needs" + 0.005*"need" + 0.005*"plans" + 0.005*"progress" + 0.004*"quality" + 0.004*"appropriate" + 0.004*"ensure"']</t>
+    <t>['0.015*"’" + 0.010*"well" + 0.008*"good" + 0.008*"need" + 0.008*"needs" + 0.006*"ensure" + 0.006*"clear" + 0.006*"progress" + 0.005*"plans" + 0.005*"appropriate"', '0.013*"’" + 0.011*"needs" + 0.009*"good" + 0.009*"well" + 0.008*"need" + 0.007*"progress" + 0.007*"plans" + 0.005*"risk" + 0.005*"carers" + 0.005*"clear"', '0.014*"’" + 0.010*"good" + 0.008*"needs" + 0.007*"well" + 0.006*"need" + 0.006*"clear" + 0.006*"progress" + 0.005*"quality" + 0.005*"ensure" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80488</t>
@@ -2083,7 +2083,7 @@
     <t>06/02/2023</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"10" + 0.005*"clear" + 0.005*"plans" + 0.005*"Bexley" + 0.004*"effective" + 0.004*"need" + 0.004*"make"', '0.016*"’" + 0.007*"needs" + 0.006*"effective" + 0.006*"well" + 0.005*"Bexley" + 0.005*"plans" + 0.004*"need" + 0.004*"including" + 0.004*"helps" + 0.004*"level"', '0.026*"’" + 0.007*"need" + 0.006*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"plans" + 0.005*"Bexley" + 0.005*"progress" + 0.005*"practice" + 0.004*"6"']</t>
+    <t>['0.017*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"effective" + 0.005*"need" + 0.005*"Bexley" + 0.005*"10" + 0.004*"make" + 0.004*"oversight"', '0.017*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"need" + 0.005*"effective" + 0.005*"including" + 0.005*"Bexley" + 0.004*"clear" + 0.004*"make" + 0.004*"plans"', '0.024*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"Bexley" + 0.005*"2023" + 0.005*"need" + 0.005*"effective" + 0.005*"helps" + 0.005*"plans" + 0.004*"6"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -2113,7 +2113,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"well" + 0.008*"leaders" + 0.008*"plans" + 0.007*"progress" + 0.006*"good" + 0.006*"Brent" + 0.006*"number" + 0.005*"small" + 0.005*"timely"', '0.017*"’" + 0.008*"well" + 0.007*"leaders" + 0.006*"quality" + 0.006*"senior" + 0.006*"progress" + 0.005*"good" + 0.005*"Brent" + 0.005*"number" + 0.005*"plans"', '0.011*"’" + 0.008*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"progress" + 0.005*"number" + 0.005*"practice" + 0.005*"needs" + 0.005*"good" + 0.005*"range"']</t>
+    <t>['0.011*"’" + 0.008*"well" + 0.007*"Brent" + 0.007*"leaders" + 0.006*"progress" + 0.006*"practice" + 0.005*"good" + 0.005*"plans" + 0.005*"quality" + 0.005*"number"', '0.023*"’" + 0.010*"well" + 0.008*"leaders" + 0.008*"plans" + 0.007*"progress" + 0.006*"number" + 0.006*"good" + 0.006*"senior" + 0.006*"quality" + 0.005*"needs"', '0.011*"’" + 0.006*"well" + 0.005*"leaders" + 0.005*"progress" + 0.005*"plans" + 0.005*"good" + 0.004*"senior" + 0.004*"practice" + 0.004*"quality" + 0.004*"Brent"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -2149,7 +2149,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"Bromley" + 0.007*"well" + 0.007*"plans" + 0.006*"needs" + 0.006*"practice" + 0.005*"leaders" + 0.005*"education" + 0.005*"progress" + 0.004*"health"', '0.018*"’" + 0.008*"Bromley" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.005*"plans" + 0.004*"practice" + 0.004*"health" + 0.004*"strong" + 0.004*"access"', '0.022*"’" + 0.010*"Bromley" + 0.007*"needs" + 0.007*"well" + 0.005*"leaders" + 0.005*"education" + 0.005*"plans" + 0.005*"practice" + 0.004*"health" + 0.004*"YPAs"']</t>
+    <t>['0.017*"’" + 0.011*"Bromley" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"leaders" + 0.004*"practice" + 0.004*"education" + 0.004*"carers" + 0.004*"progress"', '0.020*"’" + 0.009*"needs" + 0.007*"Bromley" + 0.006*"plans" + 0.006*"well" + 0.005*"education" + 0.004*"health" + 0.004*"leaders" + 0.004*"practice" + 0.004*"2023"', '0.021*"’" + 0.009*"Bromley" + 0.008*"well" + 0.006*"leaders" + 0.006*"practice" + 0.005*"health" + 0.005*"needs" + 0.005*"17" + 0.005*"plans" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -2182,7 +2182,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"practice" + 0.007*"Camden" + 0.007*"leaders" + 0.006*"protection" + 0.006*"well" + 0.006*"appropriate" + 0.005*"needs" + 0.005*"25" + 0.004*"meetings"', '0.011*"’" + 0.007*"Camden" + 0.006*"leaders" + 0.006*"practice" + 0.005*"response" + 0.005*"well" + 0.005*"health" + 0.005*"29" + 0.005*"needs" + 0.004*"protection"', '0.009*"’" + 0.007*"Camden" + 0.005*"leaders" + 0.005*"well" + 0.005*"needs" + 0.004*"progress" + 0.004*"29" + 0.003*"25" + 0.003*"April" + 0.003*"practice"']</t>
+    <t>['0.009*"’" + 0.007*"leaders" + 0.007*"Camden" + 0.006*"well" + 0.005*"practice" + 0.004*"needs" + 0.004*"response" + 0.004*"protection" + 0.004*"appropriate" + 0.004*"April"', '0.012*"’" + 0.008*"Camden" + 0.006*"practice" + 0.006*"needs" + 0.006*"protection" + 0.005*"leaders" + 0.005*"response" + 0.004*"appropriate" + 0.004*"progress" + 0.004*"29"', '0.010*"’" + 0.007*"leaders" + 0.006*"practice" + 0.006*"Camden" + 0.006*"well" + 0.005*"25" + 0.005*"29" + 0.005*"protection" + 0.004*"response" + 0.004*"meetings"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -2212,7 +2212,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"Croydon" + 0.005*"good" + 0.005*"risk" + 0.005*"quality" + 0.005*"ensure" + 0.005*"plans" + 0.004*"need"', '0.013*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"quality" + 0.006*"Senior" + 0.006*"need" + 0.006*"effective" + 0.006*"Croydon" + 0.005*"plans" + 0.005*"ensure"', '0.012*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"ensure" + 0.005*"good" + 0.005*"Senior" + 0.005*"health" + 0.005*"improved" + 0.005*"Croydon" + 0.005*"education"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"quality" + 0.006*"Senior" + 0.006*"risk" + 0.006*"Croydon" + 0.006*"ensure" + 0.005*"need" + 0.005*"education"', '0.010*"’" + 0.006*"well" + 0.006*"Croydon" + 0.006*"needs" + 0.005*"good" + 0.005*"need" + 0.005*"ensure" + 0.005*"health" + 0.004*"Senior" + 0.004*"quality"', '0.010*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"need" + 0.005*"Croydon" + 0.005*"However" + 0.005*"effective" + 0.004*"oversight" + 0.004*"Senior" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2248,7 +2248,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"quality" + 0.007*"needs" + 0.005*"good" + 0.005*"Ealing" + 0.004*"progress" + 0.004*"experiences" + 0.004*"risk" + 0.004*"plans" + 0.004*"protection"', '0.012*"’" + 0.008*"quality" + 0.007*"good" + 0.006*"needs" + 0.005*"plans" + 0.005*"risk" + 0.005*"progress" + 0.005*"well" + 0.004*"oversight" + 0.004*"leaders"', '0.012*"quality" + 0.012*"’" + 0.007*"needs" + 0.007*"good" + 0.005*"plans" + 0.005*"progress" + 0.005*"risk" + 0.005*"experiences" + 0.005*"Ealing" + 0.004*"need"']</t>
+    <t>['0.009*"’" + 0.008*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"progress" + 0.005*"management" + 0.005*"Ealing" + 0.005*"risk" + 0.004*"family" + 0.004*"plans"', '0.012*"’" + 0.011*"quality" + 0.008*"needs" + 0.006*"good" + 0.005*"progress" + 0.005*"risk" + 0.004*"Ealing" + 0.004*"plans" + 0.004*"experiences" + 0.004*"leaders"', '0.012*"’" + 0.010*"quality" + 0.007*"good" + 0.006*"plans" + 0.006*"needs" + 0.005*"oversight" + 0.004*"risk" + 0.004*"well" + 0.004*"family" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80494</t>
@@ -2281,7 +2281,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"practice" + 0.009*"needs" + 0.008*"good" + 0.007*"effective" + 0.007*"quality" + 0.006*"leaders" + 0.006*"clear" + 0.006*"improve" + 0.006*"Enfield"', '0.011*"’" + 0.009*"ensure" + 0.008*"good" + 0.008*"needs" + 0.007*"timely" + 0.007*"effective" + 0.006*"clear" + 0.006*"Enfield" + 0.006*"practice" + 0.006*"leaders"', '0.015*"’" + 0.009*"needs" + 0.008*"ensure" + 0.007*"practice" + 0.006*"Enfield" + 0.006*"clear" + 0.006*"good" + 0.006*"quality" + 0.006*"timely" + 0.006*"appropriate"']</t>
+    <t>['0.010*"’" + 0.008*"practice" + 0.007*"ensure" + 0.007*"good" + 0.007*"needs" + 0.007*"effective" + 0.006*"timely" + 0.005*"clear" + 0.005*"quality" + 0.005*"Enfield"', '0.015*"’" + 0.008*"needs" + 0.007*"practice" + 0.007*"good" + 0.007*"ensure" + 0.007*"clear" + 0.007*"Enfield" + 0.006*"quality" + 0.006*"effective" + 0.006*"leaders"', '0.014*"’" + 0.010*"needs" + 0.008*"ensure" + 0.007*"practice" + 0.007*"good" + 0.006*"effective" + 0.006*"Enfield" + 0.006*"timely" + 0.006*"leaders" + 0.006*"clear"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2314,7 +2314,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"well" + 0.009*"needs" + 0.009*"good" + 0.007*"plans" + 0.006*"need" + 0.006*"range" + 0.005*"risks" + 0.005*"ensure" + 0.005*"quality"', '0.012*"’" + 0.010*"well" + 0.009*"plans" + 0.008*"good" + 0.007*"needs" + 0.006*"range" + 0.006*"need" + 0.006*"progress" + 0.006*"ensure" + 0.005*"risk"', '0.009*"’" + 0.008*"well" + 0.006*"need" + 0.006*"plans" + 0.006*"good" + 0.005*"needs" + 0.005*"range" + 0.004*"timely" + 0.004*"progress" + 0.004*"information"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.009*"good" + 0.007*"need" + 0.007*"needs" + 0.007*"plans" + 0.005*"risks" + 0.005*"timely" + 0.005*"quality" + 0.005*"range"', '0.014*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"plans" + 0.007*"good" + 0.006*"progress" + 0.006*"ensure" + 0.006*"range" + 0.005*"effective" + 0.005*"need"', '0.010*"’" + 0.009*"well" + 0.008*"plans" + 0.007*"good" + 0.006*"range" + 0.006*"needs" + 0.006*"need" + 0.005*"progress" + 0.005*"risk" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2353,7 +2353,7 @@
     <t>0.1417</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.009*"practice" + 0.007*"planning" + 0.006*"number" + 0.005*"within" + 0.005*"needs" + 0.005*"small" + 0.005*"progress" + 0.005*"However" + 0.005*"leaders"', '0.016*"’" + 0.011*"practice" + 0.007*"number" + 0.007*"effective" + 0.007*"needs" + 0.006*"planning" + 0.006*"plans" + 0.006*"including" + 0.006*"within" + 0.005*"making"', '0.013*"’" + 0.009*"practice" + 0.006*"effective" + 0.006*"quality" + 0.006*"plans" + 0.005*"number" + 0.005*"within" + 0.005*"including" + 0.005*"carers" + 0.005*"However"']</t>
+    <t>['0.012*"’" + 0.009*"practice" + 0.006*"planning" + 0.006*"within" + 0.006*"plans" + 0.006*"effective" + 0.005*"number" + 0.005*"needs" + 0.005*"making" + 0.005*"including"', '0.011*"’" + 0.009*"practice" + 0.006*"number" + 0.006*"leaders" + 0.005*"needs" + 0.005*"effective" + 0.005*"plans" + 0.005*"quality" + 0.005*"planning" + 0.004*"range"', '0.015*"’" + 0.010*"practice" + 0.007*"number" + 0.006*"planning" + 0.006*"within" + 0.006*"effective" + 0.006*"including" + 0.006*"However" + 0.006*"needs" + 0.006*"quality"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2386,7 +2386,7 @@
     <t>0.2054</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"needs" + 0.006*"appropriate" + 0.006*"good" + 0.006*"effective" + 0.006*"well" + 0.005*"arrangements" + 0.005*"ensure" + 0.005*"improve" + 0.004*"shared"', '0.013*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"effective" + 0.006*"leaders" + 0.005*"arrangements" + 0.005*"good" + 0.005*"ensure" + 0.005*"However" + 0.004*"appropriate"', '0.011*"’" + 0.011*"effective" + 0.009*"needs" + 0.008*"well" + 0.007*"appropriate" + 0.007*"good" + 0.006*"ensure" + 0.006*"education" + 0.005*"arrangements" + 0.005*"leaders"']</t>
+    <t>['0.012*"’" + 0.009*"effective" + 0.009*"needs" + 0.007*"well" + 0.006*"appropriate" + 0.006*"ensure" + 0.006*"leaders" + 0.005*"arrangements" + 0.005*"health" + 0.005*"shared"', '0.013*"’" + 0.008*"well" + 0.007*"effective" + 0.006*"needs" + 0.006*"good" + 0.005*"arrangements" + 0.005*"improve" + 0.005*"leaders" + 0.005*"quality" + 0.004*"need"', '0.011*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"effective" + 0.007*"appropriate" + 0.007*"good" + 0.006*"arrangements" + 0.006*"ensure" + 0.006*"education" + 0.006*"risk"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2410,7 +2410,7 @@
     <t>13/02/2023</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.006*"Haringey" + 0.006*"plans" + 0.005*"need" + 0.005*"24" + 0.004*"impact" + 0.004*"well" + 0.004*"good" + 0.004*"education"', '0.016*"’" + 0.010*"Haringey" + 0.007*"good" + 0.006*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"progress" + 0.006*"need" + 0.005*"education" + 0.004*"leaders"', '0.015*"’" + 0.009*"needs" + 0.008*"Haringey" + 0.008*"plans" + 0.006*"well" + 0.005*"good" + 0.005*"carers" + 0.004*"supported" + 0.004*"risk" + 0.004*"progress"']</t>
+    <t>['0.018*"’" + 0.007*"Haringey" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"progress" + 0.005*"good" + 0.004*"risk" + 0.004*"13" + 0.004*"education"', '0.016*"’" + 0.008*"Haringey" + 0.008*"needs" + 0.006*"plans" + 0.006*"need" + 0.005*"good" + 0.005*"well" + 0.004*"risk" + 0.004*"education" + 0.004*"impact"', '0.013*"’" + 0.010*"Haringey" + 0.008*"plans" + 0.008*"needs" + 0.006*"well" + 0.005*"good" + 0.005*"need" + 0.004*"timely" + 0.004*"progress" + 0.004*"February"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2443,7 +2443,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.009*"good" + 0.008*"well" + 0.008*"’" + 0.006*"needs" + 0.005*"impact" + 0.004*"protection" + 0.004*"practice" + 0.004*"school" + 0.004*"quality" + 0.004*"early"', '0.012*"’" + 0.011*"good" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"need" + 0.005*"practice" + 0.005*"protection" + 0.005*"early" + 0.005*"impact"', '0.013*"’" + 0.011*"good" + 0.009*"needs" + 0.008*"well" + 0.006*"impact" + 0.006*"experiences" + 0.005*"protection" + 0.005*"plans" + 0.005*"practice" + 0.005*"early"']</t>
+    <t>['0.011*"’" + 0.008*"well" + 0.008*"good" + 0.007*"needs" + 0.005*"plans" + 0.005*"practice" + 0.004*"protection" + 0.004*"need" + 0.004*"early" + 0.004*"impact"', '0.014*"good" + 0.013*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"plans" + 0.006*"impact" + 0.006*"need" + 0.006*"protection" + 0.005*"practice" + 0.005*"early"', '0.010*"’" + 0.008*"well" + 0.008*"good" + 0.008*"needs" + 0.006*"impact" + 0.006*"experiences" + 0.005*"practice" + 0.005*"protection" + 0.005*"need" + 0.004*"early"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2470,7 +2470,7 @@
     <t>16/02/24</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"Havering" + 0.008*"quality" + 0.006*"effective" + 0.005*"plans" + 0.004*"needs" + 0.004*"22" + 0.004*"well" + 0.004*"11" + 0.004*"practice"', '0.018*"’" + 0.011*"Havering" + 0.009*"quality" + 0.008*"plans" + 0.007*"oversight" + 0.006*"effective" + 0.005*"22" + 0.004*"practice" + 0.004*"December" + 0.004*"needs"', '0.021*"’" + 0.012*"Havering" + 0.009*"quality" + 0.007*"plans" + 0.005*"needs" + 0.005*"11" + 0.004*"many" + 0.004*"effective" + 0.004*"oversight" + 0.004*"well"']</t>
+    <t>['0.020*"’" + 0.012*"Havering" + 0.009*"quality" + 0.008*"plans" + 0.006*"effective" + 0.006*"oversight" + 0.005*"needs" + 0.004*"11" + 0.004*"practice" + 0.004*"22"', '0.015*"’" + 0.011*"Havering" + 0.010*"quality" + 0.007*"plans" + 0.005*"11" + 0.005*"needs" + 0.004*"oversight" + 0.004*"effective" + 0.004*"practice" + 0.004*"22"', '0.017*"’" + 0.010*"Havering" + 0.006*"plans" + 0.006*"quality" + 0.006*"effective" + 0.005*"oversight" + 0.004*"well" + 0.004*"needs" + 0.004*"many" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80501</t>
@@ -2509,7 +2509,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"needs" + 0.009*"plans" + 0.007*"well" + 0.007*"Hillingdon" + 0.004*"need" + 0.004*"2" + 0.004*"6" + 0.004*"leaders" + 0.004*"good"', '0.012*"’" + 0.010*"needs" + 0.007*"plans" + 0.006*"Hillingdon" + 0.005*"well" + 0.004*"team" + 0.004*"need" + 0.004*"carers" + 0.004*"understand" + 0.004*"6"', '0.022*"’" + 0.009*"Hillingdon" + 0.009*"needs" + 0.009*"well" + 0.007*"plans" + 0.006*"team" + 0.005*"need" + 0.005*"2" + 0.005*"6" + 0.004*"2023"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.006*"Hillingdon" + 0.006*"plans" + 0.006*"well" + 0.004*"6" + 0.004*"2" + 0.004*"team" + 0.004*"PAs" + 0.004*"understand"', '0.018*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"Hillingdon" + 0.006*"plans" + 0.005*"team" + 0.005*"need" + 0.004*"6" + 0.004*"experiences" + 0.004*"leaders"', '0.020*"’" + 0.010*"plans" + 0.008*"needs" + 0.008*"Hillingdon" + 0.007*"well" + 0.005*"need" + 0.004*"team" + 0.004*"leaders" + 0.004*"October" + 0.004*"2"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2542,7 +2542,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"needs" + 0.010*"well" + 0.007*"effective" + 0.006*"Hounslow" + 0.005*"timely" + 0.005*"plans" + 0.004*"oversight" + 0.004*"training" + 0.004*"progress"', '0.024*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"effective" + 0.006*"Hounslow" + 0.006*"plans" + 0.005*"education" + 0.005*"16" + 0.005*"timely" + 0.005*"strong"', '0.020*"’" + 0.012*"needs" + 0.011*"well" + 0.008*"Hounslow" + 0.008*"effective" + 0.008*"timely" + 0.005*"plans" + 0.005*"progress" + 0.005*"2023" + 0.004*"experiences"']</t>
+    <t>['0.024*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"plans" + 0.005*"Hounslow" + 0.005*"oversight" + 0.005*"regular" + 0.005*"timely" + 0.005*"2023"', '0.016*"’" + 0.012*"needs" + 0.011*"well" + 0.007*"effective" + 0.007*"Hounslow" + 0.006*"timely" + 0.006*"plans" + 0.005*"experiences" + 0.005*"strong" + 0.005*"16"', '0.019*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"Hounslow" + 0.007*"timely" + 0.007*"effective" + 0.005*"oversight" + 0.005*"progress" + 0.005*"plans" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2572,7 +2572,7 @@
     <t>0.209</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"well" + 0.011*"needs" + 0.007*"plans" + 0.007*"highly" + 0.006*"good" + 0.006*"quality" + 0.006*"leaders" + 0.005*"practice" + 0.005*"Islington"', '0.013*"needs" + 0.009*"well" + 0.009*"’" + 0.006*"plans" + 0.005*"effective" + 0.005*"good" + 0.005*"highly" + 0.005*"leaders" + 0.005*"quality" + 0.004*"risk"', '0.010*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"plans" + 0.005*"Islington" + 0.005*"highly" + 0.005*"good" + 0.005*"effective" + 0.005*"quality" + 0.005*"risk"']</t>
+    <t>['0.013*"’" + 0.013*"needs" + 0.007*"plans" + 0.007*"well" + 0.006*"good" + 0.005*"highly" + 0.005*"leaders" + 0.005*"effective" + 0.005*"Islington" + 0.004*"school"', '0.014*"’" + 0.012*"well" + 0.010*"needs" + 0.008*"plans" + 0.007*"quality" + 0.006*"highly" + 0.006*"effective" + 0.006*"leaders" + 0.006*"Islington" + 0.005*"good"', '0.011*"well" + 0.010*"needs" + 0.010*"’" + 0.006*"highly" + 0.006*"good" + 0.005*"quality" + 0.004*"risk" + 0.004*"practice" + 0.004*"leaders" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2605,7 +2605,7 @@
     <t>16/12/22</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Lambeth" + 0.006*"plans" + 0.006*"good" + 0.005*"impact" + 0.005*"leaders" + 0.005*"progress" + 0.004*"arrangements"', '0.015*"’" + 0.009*"well" + 0.009*"needs" + 0.006*"need" + 0.006*"good" + 0.006*"impact" + 0.005*"24" + 0.005*"Leaders" + 0.005*"number" + 0.005*"plans"', '0.017*"’" + 0.010*"needs" + 0.009*"plans" + 0.008*"well" + 0.007*"good" + 0.007*"Lambeth" + 0.007*"progress" + 0.006*"need" + 0.006*"leaders" + 0.005*"4"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"plans" + 0.005*"need" + 0.005*"Lambeth" + 0.005*"progress" + 0.005*"Leaders" + 0.005*"24"', '0.016*"’" + 0.010*"needs" + 0.007*"plans" + 0.007*"Lambeth" + 0.006*"well" + 0.005*"progress" + 0.005*"need" + 0.005*"November" + 0.005*"leaders" + 0.005*"good"', '0.016*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"plans" + 0.008*"good" + 0.007*"Lambeth" + 0.006*"impact" + 0.006*"progress" + 0.006*"need" + 0.006*"leaders"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2641,7 +2641,7 @@
     <t>0.1803</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"good" + 0.005*"plans" + 0.004*"Lewisham" + 0.004*"progress" + 0.004*"need" + 0.004*"benefit"', '0.012*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"needs" + 0.006*"Lewisham" + 0.006*"effective" + 0.005*"progress" + 0.005*"good" + 0.005*"4" + 0.005*"arrangements"', '0.021*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.007*"effective" + 0.006*"Lewisham" + 0.005*"progress" + 0.005*"leaders" + 0.005*"4" + 0.005*"arrangements"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"Lewisham" + 0.006*"plans" + 0.006*"leaders" + 0.005*"progress" + 0.005*"2023" + 0.005*"benefit"', '0.021*"’" + 0.008*"plans" + 0.008*"well" + 0.006*"progress" + 0.006*"needs" + 0.006*"Lewisham" + 0.006*"effective" + 0.005*"good" + 0.005*"4" + 0.005*"need"', '0.010*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"plans" + 0.005*"Lewisham" + 0.004*"4" + 0.004*"arrangements" + 0.004*"ensure" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2665,7 +2665,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"Merton" + 0.008*"well" + 0.005*"needs" + 0.005*"family" + 0.005*"progress" + 0.005*"helping" + 0.004*"4" + 0.004*"2022" + 0.004*"practice"', '0.009*"’" + 0.005*"well" + 0.004*"needs" + 0.004*"Merton" + 0.004*"plans" + 0.004*"progress" + 0.004*"health" + 0.003*"risk" + 0.003*"family" + 0.003*"early"', '0.018*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"Merton" + 0.006*"plans" + 0.005*"ensure" + 0.005*"good" + 0.004*"28" + 0.004*"information" + 0.004*"progress"']</t>
+    <t>['0.011*"’" + 0.006*"Merton" + 0.006*"well" + 0.006*"needs" + 0.004*"family" + 0.004*"4" + 0.004*"risk" + 0.004*"progress" + 0.004*"early" + 0.004*"good"', '0.019*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"plans" + 0.005*"needs" + 0.005*"family" + 0.005*"ensure" + 0.004*"across" + 0.004*"February" + 0.004*"helping"', '0.016*"’" + 0.009*"well" + 0.006*"Merton" + 0.006*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"good" + 0.004*"28" + 0.004*"education" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2686,7 +2686,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50192878</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"needs" + 0.007*"Newham" + 0.007*"need" + 0.006*"progress" + 0.006*"practice" + 0.005*"plans" + 0.005*"good" + 0.005*"effective" + 0.005*"receive"', '0.013*"’" + 0.007*"needs" + 0.007*"Newham" + 0.006*"plans" + 0.005*"need" + 0.005*"progress" + 0.004*"good" + 0.004*"effective" + 0.004*"practice" + 0.004*"Leaders"', '0.022*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"practice" + 0.006*"plans" + 0.006*"progress" + 0.006*"Newham" + 0.005*"need" + 0.005*"good" + 0.005*"18"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"Newham" + 0.006*"practice" + 0.006*"need" + 0.006*"effective" + 0.005*"progress" + 0.005*"good" + 0.004*"29"', '0.022*"’" + 0.009*"Newham" + 0.008*"needs" + 0.007*"plans" + 0.006*"need" + 0.006*"practice" + 0.006*"progress" + 0.006*"effective" + 0.005*"good" + 0.005*"18"', '0.019*"’" + 0.010*"needs" + 0.006*"progress" + 0.006*"practice" + 0.006*"effective" + 0.005*"need" + 0.005*"Newham" + 0.005*"Leaders" + 0.005*"plans" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2716,7 +2716,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.007*"practice" + 0.006*"need" + 0.006*"well" + 0.006*"needs" + 0.005*"Redbridge" + 0.005*"good" + 0.005*"effective" + 0.005*"risk" + 0.005*"team"', '0.007*"practice" + 0.007*"’" + 0.006*"effective" + 0.006*"well" + 0.006*"need" + 0.005*"needs" + 0.005*"risk" + 0.005*"Redbridge" + 0.005*"team" + 0.005*"strong"', '0.008*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"strong" + 0.006*"practice" + 0.005*"progress" + 0.005*"ensure" + 0.005*"including" + 0.005*"Redbridge" + 0.005*"need"']</t>
+    <t>['0.007*"well" + 0.007*"’" + 0.007*"need" + 0.007*"practice" + 0.006*"needs" + 0.006*"Redbridge" + 0.006*"strong" + 0.005*"progress" + 0.005*"effective" + 0.005*"including"', '0.008*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"effective" + 0.005*"risk" + 0.005*"need" + 0.004*"including" + 0.004*"provided" + 0.004*"Redbridge" + 0.004*"team"', '0.007*"’" + 0.007*"practice" + 0.007*"needs" + 0.005*"strong" + 0.005*"well" + 0.005*"effective" + 0.005*"risk" + 0.005*"Redbridge" + 0.005*"team" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2743,7 +2743,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"well" + 0.008*"needs" + 0.008*"Richmond" + 0.007*"supported" + 0.006*"need" + 0.006*"good" + 0.006*"team" + 0.005*"upon" + 0.005*"strong"', '0.012*"well" + 0.009*"’" + 0.009*"Richmond" + 0.006*"needs" + 0.005*"team" + 0.005*"need" + 0.005*"supported" + 0.005*"good" + 0.004*"ensure" + 0.004*"4"', '0.013*"’" + 0.010*"well" + 0.007*"Richmond" + 0.006*"needs" + 0.005*"team" + 0.005*"good" + 0.005*"supported" + 0.004*"January" + 0.004*"need" + 0.004*"additional"']</t>
+    <t>['0.015*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"Richmond" + 0.007*"supported" + 0.006*"team" + 0.006*"good" + 0.006*"need" + 0.005*"additional" + 0.005*"upon"', '0.016*"’" + 0.013*"well" + 0.008*"Richmond" + 0.006*"needs" + 0.005*"good" + 0.005*"January" + 0.005*"need" + 0.005*"supported" + 0.005*"team" + 0.004*"ensure"', '0.015*"’" + 0.009*"well" + 0.008*"Richmond" + 0.007*"needs" + 0.005*"supported" + 0.005*"need" + 0.005*"2022" + 0.005*"4" + 0.005*"team" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2773,7 +2773,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"needs" + 0.009*"good" + 0.009*"Southwark" + 0.008*"well" + 0.007*"plans" + 0.006*"strong" + 0.006*"Leaders" + 0.006*"leaders" + 0.005*"progress"', '0.022*"’" + 0.011*"Southwark" + 0.007*"progress" + 0.007*"good" + 0.007*"need" + 0.007*"well" + 0.005*"Leaders" + 0.005*"effective" + 0.005*"strong" + 0.005*"ensure"', '0.013*"’" + 0.007*"well" + 0.007*"Southwark" + 0.006*"good" + 0.006*"effective" + 0.005*"receive" + 0.005*"plans" + 0.005*"needs" + 0.005*"leaders" + 0.004*"30"']</t>
+    <t>['0.019*"’" + 0.010*"Southwark" + 0.007*"needs" + 0.007*"good" + 0.007*"well" + 0.006*"effective" + 0.006*"strong" + 0.005*"need" + 0.005*"progress" + 0.005*"Leaders"', '0.018*"’" + 0.009*"Southwark" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"plans" + 0.006*"practice" + 0.005*"receive" + 0.005*"strong"', '0.018*"’" + 0.009*"Southwark" + 0.009*"well" + 0.008*"good" + 0.008*"needs" + 0.006*"progress" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders" + 0.005*"Leaders"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2803,7 +2803,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"Sutton" + 0.004*"receive" + 0.004*"good" + 0.004*"December" + 0.004*"need" + 0.004*"6" + 0.004*"effective"', '0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"good" + 0.005*"Sutton" + 0.005*"effective" + 0.005*"need" + 0.005*"leaders" + 0.004*"progress" + 0.004*"receive"', '0.018*"’" + 0.007*"Sutton" + 0.007*"progress" + 0.006*"well" + 0.005*"effective" + 0.005*"receive" + 0.005*"6" + 0.005*"needs" + 0.005*"10" + 0.004*"good"']</t>
+    <t>['0.016*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"Sutton" + 0.005*"receive" + 0.004*"protection" + 0.004*"6" + 0.004*"needs" + 0.004*"effective" + 0.004*"need"', '0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"Sutton" + 0.005*"good" + 0.005*"6" + 0.005*"receive" + 0.004*"supported" + 0.004*"effective"', '0.015*"’" + 0.007*"well" + 0.006*"Sutton" + 0.006*"needs" + 0.005*"effective" + 0.005*"good" + 0.005*"understand" + 0.005*"receive" + 0.005*"leaders" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2833,7 +2833,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"good" + 0.006*"need" + 0.006*"needs" + 0.006*"‘" + 0.005*"including" + 0.005*"effective" + 0.005*"well" + 0.005*"plans" + 0.005*"practice"', '0.014*"’" + 0.008*"plans" + 0.007*"effective" + 0.007*"good" + 0.006*"well" + 0.005*"‘" + 0.005*"early" + 0.005*"need" + 0.005*"progress" + 0.004*"practice"', '0.014*"’" + 0.007*"good" + 0.007*"practice" + 0.006*"effective" + 0.006*"‘" + 0.005*"plans" + 0.005*"carers" + 0.005*"well" + 0.005*"early" + 0.005*"progress"']</t>
+    <t>['0.015*"’" + 0.006*"good" + 0.006*"‘" + 0.006*"effective" + 0.006*"progress" + 0.005*"practice" + 0.005*"need" + 0.005*"plans" + 0.005*"well" + 0.005*"needs"', '0.018*"’" + 0.008*"good" + 0.007*"plans" + 0.006*"well" + 0.006*"effective" + 0.006*"practice" + 0.006*"‘" + 0.005*"early" + 0.005*"need" + 0.005*"needs"', '0.009*"’" + 0.007*"plans" + 0.006*"effective" + 0.005*"well" + 0.005*"good" + 0.005*"need" + 0.004*"practice" + 0.004*"early" + 0.004*"including" + 0.004*"‘"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2866,7 +2866,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"well" + 0.007*"needs" + 0.007*"effective" + 0.007*"good" + 0.007*"need" + 0.006*"plans" + 0.004*"information" + 0.004*"receive" + 0.004*"risk"', '0.013*"’" + 0.010*"well" + 0.007*"needs" + 0.006*"good" + 0.005*"effective" + 0.005*"need" + 0.004*"risk" + 0.004*"plans" + 0.004*"actions" + 0.004*"timely"', '0.014*"’" + 0.013*"well" + 0.011*"needs" + 0.010*"good" + 0.008*"effective" + 0.006*"timely" + 0.006*"plans" + 0.006*"need" + 0.005*"risk" + 0.004*"protection"']</t>
+    <t>['0.016*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"good" + 0.006*"effective" + 0.006*"timely" + 0.006*"need" + 0.005*"plans" + 0.004*"information" + 0.004*"quality"', '0.013*"’" + 0.012*"well" + 0.009*"needs" + 0.007*"effective" + 0.006*"good" + 0.006*"plans" + 0.004*"need" + 0.004*"ensure" + 0.004*"timely" + 0.004*"protection"', '0.014*"’" + 0.013*"well" + 0.010*"good" + 0.010*"needs" + 0.008*"effective" + 0.007*"need" + 0.006*"risk" + 0.005*"plans" + 0.004*"timely" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2893,7 +2893,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.005*"well" + 0.005*"protection" + 0.005*"progress" + 0.005*"Wandsworth" + 0.005*"7" + 0.004*"good" + 0.004*"Senior" + 0.004*"practice" + 0.004*"alongside"', '0.013*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"protection" + 0.006*"practice" + 0.005*"Senior" + 0.005*"ing" + 0.005*"supported" + 0.005*"7"', '0.011*"’" + 0.006*"Wandsworth" + 0.005*"well" + 0.005*"needs" + 0.005*"effective" + 0.005*"quality" + 0.005*"ensure" + 0.005*"Senior" + 0.005*"practice" + 0.004*"18"']</t>
+    <t>['0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"effective" + 0.006*"protection" + 0.005*"progress" + 0.005*"practice" + 0.005*"quality" + 0.005*"Wandsworth" + 0.005*"ensure"', '0.007*"’" + 0.006*"protection" + 0.005*"well" + 0.005*"progress" + 0.004*"ensure" + 0.004*"effective" + 0.004*"practice" + 0.004*"Senior" + 0.004*"needs" + 0.004*"ing"', '0.012*"’" + 0.007*"well" + 0.007*"Senior" + 0.006*"Wandsworth" + 0.006*"needs" + 0.005*"progress" + 0.005*"supported" + 0.005*"practice" + 0.005*"7" + 0.005*"team"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2917,7 +2917,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"practice" + 0.005*"highly" + 0.004*"well" + 0.004*"across" + 0.004*"needs" + 0.004*"family" + 0.003*"high" + 0.003*"many" + 0.003*"shared"', '0.016*"’" + 0.007*"practice" + 0.007*"needs" + 0.006*"highly" + 0.006*"well" + 0.004*"many" + 0.004*"skilled" + 0.003*"across" + 0.003*"plans" + 0.003*"high"', '0.010*"’" + 0.007*"needs" + 0.007*"practice" + 0.005*"highly" + 0.005*"well" + 0.004*"family" + 0.004*"across" + 0.004*"many" + 0.004*"direct" + 0.004*"experiences"']</t>
+    <t>['0.012*"’" + 0.006*"needs" + 0.006*"practice" + 0.006*"highly" + 0.005*"well" + 0.005*"many" + 0.004*"shared" + 0.004*"skilled" + 0.003*"across" + 0.003*"family"', '0.014*"’" + 0.006*"needs" + 0.006*"practice" + 0.006*"highly" + 0.006*"well" + 0.004*"plans" + 0.003*"across" + 0.003*"family" + 0.003*"many" + 0.003*"interventions"', '0.012*"’" + 0.008*"practice" + 0.005*"highly" + 0.005*"needs" + 0.004*"well" + 0.004*"across" + 0.004*"high" + 0.004*"family" + 0.004*"Westminster" + 0.003*"plans"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2950,7 +2950,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.005*"needs" + 0.004*"plans" + 0.004*"need" + 0.004*"Luton" + 0.004*"impact" + 0.003*"receive" + 0.003*"22" + 0.003*"good" + 0.003*"July"', '0.016*"’" + 0.008*"needs" + 0.007*"need" + 0.006*"Luton" + 0.006*"plans" + 0.006*"good" + 0.006*"progress" + 0.005*"effective" + 0.005*"Leaders" + 0.005*"impact"', '0.021*"’" + 0.006*"need" + 0.006*"effective" + 0.006*"plans" + 0.006*"ensure" + 0.005*"Luton" + 0.005*"good" + 0.005*"needs" + 0.005*"impact" + 0.005*"quality"']</t>
+    <t>['0.018*"’" + 0.007*"needs" + 0.007*"need" + 0.006*"good" + 0.006*"plans" + 0.006*"progress" + 0.006*"Luton" + 0.005*"effective" + 0.005*"quality" + 0.005*"impact"', '0.016*"’" + 0.006*"plans" + 0.006*"Luton" + 0.005*"needs" + 0.005*"need" + 0.005*"ensure" + 0.005*"effective" + 0.005*"receive" + 0.004*"impact" + 0.004*"Leaders"', '0.017*"’" + 0.007*"need" + 0.006*"plans" + 0.006*"effective" + 0.005*"Luton" + 0.005*"needs" + 0.005*"good" + 0.004*"impact" + 0.004*"receive" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2977,7 +2977,7 @@
     <t>19/05/22</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.012*"needs" + 0.011*"Manchester" + 0.007*"always" + 0.007*"well" + 0.006*"supported" + 0.006*"education" + 0.006*"quality" + 0.005*"plans" + 0.005*"effective"', '0.025*"’" + 0.009*"Manchester" + 0.008*"needs" + 0.007*"always" + 0.007*"well" + 0.007*"supported" + 0.006*"protection" + 0.006*"disabled" + 0.006*"plans" + 0.005*"effective"', '0.015*"’" + 0.011*"Manchester" + 0.008*"needs" + 0.006*"supported" + 0.006*"well" + 0.005*"plans" + 0.004*"April" + 0.004*"education" + 0.004*"1" + 0.004*"effective"']</t>
+    <t>['0.018*"’" + 0.011*"Manchester" + 0.008*"needs" + 0.006*"well" + 0.005*"always" + 0.005*"protection" + 0.005*"plans" + 0.005*"supported" + 0.005*"family" + 0.005*"education"', '0.020*"’" + 0.012*"Manchester" + 0.010*"needs" + 0.009*"always" + 0.008*"well" + 0.008*"supported" + 0.006*"plans" + 0.006*"disabled" + 0.005*"quality" + 0.005*"1"', '0.025*"’" + 0.009*"needs" + 0.008*"Manchester" + 0.006*"supported" + 0.006*"education" + 0.006*"protection" + 0.005*"effective" + 0.005*"well" + 0.005*"progress" + 0.005*"21"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -3007,7 +3007,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"Medway" + 0.009*"practice" + 0.007*"well" + 0.007*"leaders" + 0.007*"quality" + 0.007*"needs" + 0.006*"oversight" + 0.006*"experiences" + 0.005*"impact"', '0.014*"’" + 0.009*"Medway" + 0.008*"well" + 0.007*"quality" + 0.007*"practice" + 0.006*"oversight" + 0.006*"good" + 0.006*"needs" + 0.005*"17" + 0.005*"risk"', '0.018*"’" + 0.009*"Medway" + 0.008*"quality" + 0.008*"practice" + 0.008*"well" + 0.007*"leaders" + 0.006*"impact" + 0.006*"needs" + 0.005*"progress" + 0.005*"28"']</t>
+    <t>['0.014*"’" + 0.010*"Medway" + 0.008*"quality" + 0.007*"practice" + 0.006*"leaders" + 0.006*"oversight" + 0.005*"28" + 0.005*"improve" + 0.005*"well" + 0.005*"17"', '0.017*"’" + 0.010*"Medway" + 0.008*"well" + 0.008*"practice" + 0.007*"quality" + 0.007*"leaders" + 0.006*"oversight" + 0.006*"impact" + 0.006*"needs" + 0.006*"experiences"', '0.016*"’" + 0.009*"well" + 0.009*"practice" + 0.008*"quality" + 0.008*"Medway" + 0.007*"needs" + 0.005*"leaders" + 0.005*"impact" + 0.005*"Senior" + 0.005*"oversight"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -3031,7 +3031,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"effective" + 0.007*"plans" + 0.006*"needs" + 0.006*"Middlesbrough" + 0.005*"practice" + 0.005*"place" + 0.005*"well" + 0.005*"progress" + 0.005*"24"', '0.017*"’" + 0.008*"Middlesbrough" + 0.008*"plans" + 0.007*"effective" + 0.007*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"practice" + 0.005*"good" + 0.005*"means"', '0.011*"’" + 0.007*"well" + 0.006*"effective" + 0.005*"Middlesbrough" + 0.005*"needs" + 0.005*"plans" + 0.005*"practice" + 0.005*"progress" + 0.004*"senior" + 0.004*"good"']</t>
+    <t>['0.015*"’" + 0.008*"plans" + 0.007*"Middlesbrough" + 0.007*"well" + 0.006*"effective" + 0.006*"needs" + 0.006*"practice" + 0.005*"progress" + 0.005*"place" + 0.005*"24"', '0.013*"’" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"progress" + 0.005*"place" + 0.005*"good" + 0.005*"13"', '0.012*"’" + 0.007*"effective" + 0.007*"plans" + 0.006*"practice" + 0.006*"well" + 0.006*"Middlesbrough" + 0.006*"needs" + 0.005*"progress" + 0.004*"24" + 0.004*"March"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -3058,7 +3058,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"Keynes" + 0.005*"Milton" + 0.005*"practice" + 0.005*"team" + 0.004*"plans" + 0.004*"need" + 0.004*"well" + 0.004*"needs" + 0.004*"25"', '0.017*"’" + 0.007*"Milton" + 0.006*"well" + 0.006*"Keynes" + 0.005*"need" + 0.005*"good" + 0.005*"leaders" + 0.005*"practice" + 0.005*"education" + 0.005*"October"', '0.015*"’" + 0.006*"well" + 0.006*"need" + 0.005*"25" + 0.005*"Keynes" + 0.005*"Milton" + 0.005*"practice" + 0.004*"good" + 0.004*"leaders" + 0.004*"family"']</t>
+    <t>['0.016*"’" + 0.007*"Keynes" + 0.006*"Milton" + 0.006*"plans" + 0.006*"well" + 0.005*"practice" + 0.005*"need" + 0.005*"25" + 0.004*"leaders" + 0.004*"needs"', '0.013*"’" + 0.005*"need" + 0.005*"Keynes" + 0.005*"Milton" + 0.005*"well" + 0.005*"good" + 0.004*"impact" + 0.004*"October" + 0.004*"2021" + 0.004*"leaders"', '0.015*"’" + 0.006*"well" + 0.006*"Milton" + 0.005*"need" + 0.005*"Keynes" + 0.005*"practice" + 0.005*"25" + 0.005*"good" + 0.004*"leaders" + 0.004*"5"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -3085,7 +3085,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"plans" + 0.008*"needs" + 0.006*"well" + 0.006*"Newcastle" + 0.005*"progress" + 0.005*"management" + 0.005*"good" + 0.005*"need" + 0.005*"ensure"', '0.015*"’" + 0.010*"plans" + 0.008*"good" + 0.007*"Newcastle" + 0.007*"protection" + 0.006*"progress" + 0.006*"needs" + 0.006*"making" + 0.005*"well" + 0.005*"December"', '0.019*"’" + 0.011*"plans" + 0.008*"needs" + 0.008*"protection" + 0.007*"Newcastle" + 0.007*"good" + 0.007*"well" + 0.006*"ensure" + 0.006*"response" + 0.006*"10"']</t>
+    <t>['0.017*"’" + 0.011*"plans" + 0.009*"needs" + 0.008*"Newcastle" + 0.006*"protection" + 0.006*"good" + 0.006*"response" + 0.006*"well" + 0.006*"progress" + 0.006*"10"', '0.018*"’" + 0.011*"plans" + 0.007*"Newcastle" + 0.007*"protection" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.006*"ensure" + 0.005*"progress" + 0.005*"2021"', '0.012*"’" + 0.008*"plans" + 0.007*"good" + 0.006*"needs" + 0.006*"well" + 0.006*"protection" + 0.006*"progress" + 0.005*"need" + 0.005*"making" + 0.005*"Newcastle"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -3109,7 +3109,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"Norfolk" + 0.009*"well" + 0.007*"carers" + 0.007*"practice" + 0.006*"needs" + 0.006*"supported" + 0.005*"plans" + 0.005*"information" + 0.004*"range"', '0.013*"’" + 0.008*"Norfolk" + 0.008*"well" + 0.006*"carers" + 0.006*"supported" + 0.005*"needs" + 0.005*"18" + 0.005*"plans" + 0.005*"practice" + 0.005*"including"', '0.013*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"Norfolk" + 0.004*"including" + 0.004*"leaders" + 0.004*"18" + 0.004*"carers" + 0.004*"practice" + 0.004*"supported"']</t>
+    <t>['0.015*"’" + 0.007*"Norfolk" + 0.007*"needs" + 0.007*"well" + 0.006*"carers" + 0.005*"practice" + 0.005*"supported" + 0.005*"effective" + 0.004*"information" + 0.004*"progress"', '0.020*"’" + 0.009*"well" + 0.009*"Norfolk" + 0.007*"carers" + 0.006*"practice" + 0.006*"supported" + 0.005*"needs" + 0.005*"range" + 0.005*"plans" + 0.005*"7"', '0.014*"’" + 0.007*"well" + 0.007*"Norfolk" + 0.005*"needs" + 0.005*"supported" + 0.004*"practice" + 0.004*"18" + 0.004*"carers" + 0.004*"progress" + 0.004*"including"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -3142,7 +3142,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"practice" + 0.007*"leaders" + 0.006*"needs" + 0.006*"risk" + 0.005*"2021" + 0.005*"need" + 0.005*"East" + 0.005*"planning" + 0.005*"Lincolnshire"', '0.013*"’" + 0.009*"practice" + 0.008*"risk" + 0.007*"needs" + 0.006*"leaders" + 0.006*"planning" + 0.006*"many" + 0.005*"October" + 0.005*"quality" + 0.005*"plans"', '0.011*"’" + 0.007*"planning" + 0.006*"risk" + 0.006*"leaders" + 0.006*"practice" + 0.005*"need" + 0.005*"needs" + 0.005*"many" + 0.004*"experiences" + 0.004*"harm"']</t>
+    <t>['0.010*"’" + 0.008*"practice" + 0.006*"leaders" + 0.006*"planning" + 0.005*"needs" + 0.005*"risk" + 0.005*"quality" + 0.005*"need" + 0.005*"North" + 0.004*"plans"', '0.016*"’" + 0.009*"practice" + 0.007*"risk" + 0.007*"needs" + 0.006*"many" + 0.006*"need" + 0.006*"planning" + 0.006*"leaders" + 0.005*"plans" + 0.005*"East"', '0.014*"’" + 0.007*"leaders" + 0.007*"risk" + 0.006*"planning" + 0.006*"needs" + 0.006*"practice" + 0.005*"2021" + 0.005*"oversight" + 0.005*"Lincolnshire" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -3172,7 +3172,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"‘" + 0.006*"leaders" + 0.006*"North" + 0.006*"Lincolnshire" + 0.005*"family" + 0.005*"approach" + 0.005*"10" + 0.005*"need" + 0.005*"team"', '0.021*"’" + 0.007*"‘" + 0.006*"family" + 0.005*"well" + 0.004*"North" + 0.004*"council" + 0.004*"14" + 0.004*"need" + 0.004*"protection" + 0.004*"approach"', '0.021*"’" + 0.007*"‘" + 0.006*"Lincolnshire" + 0.006*"well" + 0.006*"family" + 0.006*"approach" + 0.005*"North" + 0.005*"leaders" + 0.005*"10" + 0.005*"need"']</t>
+    <t>['0.015*"’" + 0.007*"‘" + 0.006*"family" + 0.006*"leaders" + 0.005*"Lincolnshire" + 0.005*"approach" + 0.005*"North" + 0.004*"team" + 0.004*"need" + 0.004*"plans"', '0.023*"’" + 0.006*"North" + 0.006*"‘" + 0.005*"Lincolnshire" + 0.005*"10" + 0.005*"need" + 0.005*"family" + 0.005*"well" + 0.005*"14" + 0.005*"needs"', '0.022*"’" + 0.008*"‘" + 0.007*"family" + 0.006*"well" + 0.005*"approach" + 0.005*"leaders" + 0.005*"Lincolnshire" + 0.005*"North" + 0.004*"need" + 0.004*"10"']</t>
   </si>
   <si>
     <t>2637539</t>
@@ -3208,7 +3208,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"Northamptonshire" + 0.008*"well" + 0.007*"North" + 0.006*"quality" + 0.005*"practice" + 0.005*"impact" + 0.005*"Leaders" + 0.005*"needs" + 0.005*"need"', '0.018*"’" + 0.007*"North" + 0.006*"Northamptonshire" + 0.006*"quality" + 0.005*"needs" + 0.005*"need" + 0.005*"experiences" + 0.005*"practice" + 0.005*"2022" + 0.004*"Leaders"', '0.014*"’" + 0.006*"Northamptonshire" + 0.006*"well" + 0.005*"quality" + 0.005*"North" + 0.005*"NCT" + 0.005*"practice" + 0.005*"impact" + 0.004*"3" + 0.004*"e"']</t>
+    <t>['0.019*"’" + 0.007*"Northamptonshire" + 0.007*"well" + 0.006*"quality" + 0.006*"practice" + 0.006*"North" + 0.005*"impact" + 0.005*"Leaders" + 0.005*"NCT" + 0.005*"experiences"', '0.018*"’" + 0.007*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.005*"practice" + 0.005*"NCT" + 0.005*"quality" + 0.004*"plans" + 0.004*"impact" + 0.004*"need"', '0.013*"’" + 0.010*"Northamptonshire" + 0.007*"North" + 0.006*"needs" + 0.006*"well" + 0.006*"Leaders" + 0.005*"quality" + 0.005*"plans" + 0.005*"personal" + 0.005*"2022"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -3235,7 +3235,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"quality" + 0.007*"needs" + 0.007*"North" + 0.006*"always" + 0.005*"number" + 0.005*"practice" + 0.005*"risk" + 0.005*"need" + 0.004*"well"', '0.021*"’" + 0.008*"quality" + 0.007*"Somerset" + 0.007*"always" + 0.007*"practice" + 0.006*"needs" + 0.005*"progress" + 0.005*"risk" + 0.005*"number" + 0.005*"need"', '0.015*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"number" + 0.005*"North" + 0.005*"Somerset" + 0.005*"progress" + 0.005*"experienced" + 0.005*"well" + 0.005*"need"']</t>
+    <t>['0.018*"’" + 0.007*"quality" + 0.006*"number" + 0.006*"needs" + 0.006*"always" + 0.006*"need" + 0.005*"Somerset" + 0.005*"well" + 0.005*"experienced" + 0.005*"risk"', '0.018*"’" + 0.008*"quality" + 0.007*"needs" + 0.006*"North" + 0.006*"always" + 0.005*"progress" + 0.005*"number" + 0.005*"Somerset" + 0.005*"practice" + 0.005*"risk"', '0.014*"’" + 0.007*"quality" + 0.006*"Somerset" + 0.006*"North" + 0.006*"needs" + 0.006*"practice" + 0.005*"always" + 0.005*"effective" + 0.005*"need" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -3262,7 +3262,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"well" + 0.005*"need" + 0.005*"impact" + 0.005*"make" + 0.005*"leaders" + 0.004*"early" + 0.003*"progress" + 0.003*"clear" + 0.003*"needs"', '0.017*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"need" + 0.005*"quality" + 0.004*"protection" + 0.004*"needs" + 0.004*"make" + 0.004*"family" + 0.004*"clear"', '0.015*"’" + 0.006*"well" + 0.005*"leaders" + 0.005*"quality" + 0.005*"make" + 0.005*"needs" + 0.005*"need" + 0.004*"progress" + 0.004*"impact" + 0.004*"experiences"']</t>
+    <t>['0.013*"’" + 0.006*"well" + 0.005*"leaders" + 0.005*"quality" + 0.005*"need" + 0.004*"needs" + 0.004*"experiences" + 0.004*"impact" + 0.003*"clear" + 0.003*"senior"', '0.020*"’" + 0.007*"well" + 0.006*"leaders" + 0.005*"need" + 0.005*"make" + 0.005*"needs" + 0.005*"impact" + 0.004*"quality" + 0.004*"early" + 0.004*"foster"', '0.011*"’" + 0.006*"well" + 0.006*"make" + 0.005*"need" + 0.004*"leaders" + 0.004*"quality" + 0.004*"early" + 0.004*"needs" + 0.004*"protection" + 0.003*"good"']</t>
   </si>
   <si>
     <t>80530</t>
@@ -3292,7 +3292,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"well" + 0.007*"North" + 0.006*"Yorkshire" + 0.006*"‘" + 0.005*"practice" + 0.005*"family" + 0.005*"needs" + 0.004*"3" + 0.004*"supported"', '0.014*"’" + 0.008*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.005*"North" + 0.005*"‘" + 0.005*"needs" + 0.005*"family" + 0.004*"3" + 0.004*"effective"', '0.024*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"needs" + 0.006*"family" + 0.006*"North" + 0.006*"Yorkshire" + 0.005*"supported" + 0.005*"7" + 0.004*"3"']</t>
+    <t>['0.022*"’" + 0.008*"well" + 0.007*"practice" + 0.007*"Yorkshire" + 0.006*"North" + 0.005*"needs" + 0.005*"family" + 0.005*"3" + 0.004*"supported" + 0.004*"carers"', '0.021*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"practice" + 0.006*"family" + 0.006*"North" + 0.005*"‘" + 0.005*"Yorkshire" + 0.004*"7" + 0.004*"2023"', '0.018*"’" + 0.008*"well" + 0.007*"North" + 0.006*"Yorkshire" + 0.006*"family" + 0.005*"needs" + 0.005*"‘" + 0.005*"practice" + 0.004*"3" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -3319,7 +3319,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.009*"well" + 0.009*"needs" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.005*"experiences" + 0.005*"impact" + 0.004*"quality" + 0.004*"leaders"', '0.019*"’" + 0.009*"needs" + 0.009*"well" + 0.006*"experiences" + 0.006*"education" + 0.006*"good" + 0.005*"leaders" + 0.005*"quality" + 0.004*"need" + 0.004*"always"', '0.022*"’" + 0.012*"needs" + 0.010*"well" + 0.008*"good" + 0.007*"need" + 0.006*"impact" + 0.006*"practice" + 0.005*"experiences" + 0.005*"quality" + 0.004*"plans"']</t>
+    <t>['0.022*"’" + 0.012*"needs" + 0.008*"good" + 0.007*"well" + 0.007*"need" + 0.006*"practice" + 0.006*"experiences" + 0.005*"impact" + 0.005*"leaders" + 0.005*"education"', '0.018*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"good" + 0.006*"experiences" + 0.005*"need" + 0.005*"practice" + 0.004*"quality" + 0.004*"supported" + 0.003*"early"', '0.025*"’" + 0.012*"well" + 0.009*"needs" + 0.008*"good" + 0.006*"need" + 0.006*"impact" + 0.005*"education" + 0.005*"experiences" + 0.005*"quality" + 0.005*"always"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3349,7 +3349,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.005*"effective" + 0.005*"Nottingham" + 0.005*"City" + 0.005*"plans" + 0.005*"oversight" + 0.004*"risk" + 0.004*"However" + 0.004*"11"', '0.011*"’" + 0.008*"needs" + 0.006*"effective" + 0.006*"plans" + 0.006*"Nottingham" + 0.005*"However" + 0.004*"11" + 0.004*"City" + 0.004*"impact" + 0.004*"protection"', '0.014*"’" + 0.007*"needs" + 0.006*"impact" + 0.006*"Nottingham" + 0.005*"plans" + 0.005*"11" + 0.005*"oversight" + 0.005*"effective" + 0.004*"risk" + 0.004*"2022"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.006*"Nottingham" + 0.005*"oversight" + 0.005*"risk" + 0.005*"plans" + 0.005*"2022" + 0.004*"practice" + 0.004*"effective" + 0.004*"However"', '0.011*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"Nottingham" + 0.005*"impact" + 0.005*"July" + 0.005*"11" + 0.005*"effective" + 0.004*"protection" + 0.004*"oversight"', '0.015*"’" + 0.007*"needs" + 0.007*"effective" + 0.006*"impact" + 0.005*"plans" + 0.005*"Nottingham" + 0.005*"City" + 0.005*"11" + 0.005*"However" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80534</t>
@@ -3373,7 +3373,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"practice" + 0.008*"well" + 0.005*"receive" + 0.005*"made" + 0.005*"ensure" + 0.005*"plans" + 0.005*"good" + 0.005*"progress" + 0.005*"needs"', '0.014*"’" + 0.009*"practice" + 0.008*"well" + 0.007*"needs" + 0.006*"receive" + 0.006*"ensure" + 0.005*"areas" + 0.005*"quality" + 0.005*"e" + 0.005*"progress"', '0.009*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"needs" + 0.005*"plans" + 0.004*"carers" + 0.004*"receive" + 0.004*"made" + 0.004*"progress" + 0.004*"ensure"']</t>
+    <t>['0.014*"’" + 0.007*"practice" + 0.007*"needs" + 0.006*"receive" + 0.006*"well" + 0.006*"ensure" + 0.005*"areas" + 0.005*"made" + 0.005*"progress" + 0.005*"quality"', '0.012*"’" + 0.009*"practice" + 0.009*"well" + 0.006*"needs" + 0.005*"quality" + 0.005*"plans" + 0.005*"progress" + 0.005*"e" + 0.005*"effective" + 0.005*"made"', '0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.006*"plans" + 0.005*"carers" + 0.005*"ensure" + 0.005*"receive" + 0.004*"needs" + 0.004*"made" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3406,7 +3406,7 @@
     <t>04/03/19</t>
   </si>
   <si>
-    <t>['0.010*"practice" + 0.010*"good" + 0.010*"needs" + 0.008*"’" + 0.007*"quality" + 0.007*"well" + 0.006*"effective" + 0.006*"progress" + 0.006*"planning" + 0.005*"plans"', '0.011*"’" + 0.011*"good" + 0.008*"needs" + 0.008*"effective" + 0.007*"practice" + 0.007*"progress" + 0.006*"planning" + 0.006*"well" + 0.006*"plans" + 0.006*"information"', '0.013*"’" + 0.009*"needs" + 0.009*"effective" + 0.009*"practice" + 0.007*"good" + 0.007*"quality" + 0.006*"progress" + 0.006*"plans" + 0.006*"planning" + 0.006*"well"']</t>
+    <t>['0.009*"’" + 0.008*"practice" + 0.008*"good" + 0.008*"effective" + 0.007*"well" + 0.007*"needs" + 0.007*"quality" + 0.006*"progress" + 0.005*"plans" + 0.005*"receive"', '0.008*"’" + 0.008*"practice" + 0.008*"good" + 0.008*"needs" + 0.007*"planning" + 0.007*"progress" + 0.005*"effective" + 0.005*"well" + 0.005*"plans" + 0.004*"quality"', '0.013*"’" + 0.011*"good" + 0.011*"needs" + 0.009*"effective" + 0.009*"practice" + 0.007*"quality" + 0.006*"plans" + 0.006*"well" + 0.006*"planning" + 0.006*"progress"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3439,7 +3439,7 @@
     <t>0.1755</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"Oxfordshire" + 0.005*"risk" + 0.005*"quality" + 0.005*"good" + 0.005*"12" + 0.005*"February" + 0.004*"leaders"', '0.020*"’" + 0.014*"needs" + 0.008*"Oxfordshire" + 0.007*"well" + 0.006*"supported" + 0.006*"risk" + 0.006*"practice" + 0.005*"receive" + 0.005*"progress" + 0.005*"quality"', '0.021*"’" + 0.007*"Oxfordshire" + 0.007*"needs" + 0.007*"good" + 0.006*"risk" + 0.006*"supported" + 0.005*"well" + 0.005*"23" + 0.005*"progress" + 0.005*"12"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.006*"Oxfordshire" + 0.006*"well" + 0.005*"quality" + 0.005*"supported" + 0.004*"12" + 0.004*"progress" + 0.004*"good" + 0.004*"February"', '0.020*"’" + 0.012*"needs" + 0.007*"risk" + 0.006*"well" + 0.006*"Oxfordshire" + 0.006*"supported" + 0.006*"progress" + 0.005*"quality" + 0.005*"good" + 0.005*"practice"', '0.020*"’" + 0.009*"needs" + 0.008*"Oxfordshire" + 0.007*"well" + 0.007*"good" + 0.005*"education" + 0.005*"leaders" + 0.005*"risk" + 0.005*"supported" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3469,7 +3469,7 @@
     <t>30/01/24</t>
   </si>
   <si>
-    <t>['0.011*"needs" + 0.010*"’" + 0.008*"Peterborough" + 0.005*"well" + 0.005*"progress" + 0.005*"plans" + 0.005*"receive" + 0.005*"need" + 0.004*"good" + 0.004*"2023"', '0.012*"’" + 0.010*"needs" + 0.008*"need" + 0.006*"2023" + 0.006*"progress" + 0.005*"plans" + 0.005*"8" + 0.005*"27" + 0.005*"Peterborough" + 0.005*"well"', '0.019*"’" + 0.016*"needs" + 0.007*"need" + 0.007*"Peterborough" + 0.007*"well" + 0.007*"2023" + 0.006*"supported" + 0.006*"progress" + 0.006*"8" + 0.005*"November"']</t>
+    <t>['0.013*"needs" + 0.012*"’" + 0.008*"Peterborough" + 0.007*"need" + 0.006*"2023" + 0.006*"progress" + 0.006*"8" + 0.005*"supported" + 0.005*"education" + 0.005*"receive"', '0.014*"’" + 0.012*"needs" + 0.007*"Peterborough" + 0.007*"need" + 0.006*"2023" + 0.006*"well" + 0.006*"lack" + 0.005*"progress" + 0.005*"December" + 0.005*"receive"', '0.017*"’" + 0.015*"needs" + 0.007*"plans" + 0.007*"well" + 0.007*"need" + 0.006*"progress" + 0.006*"8" + 0.006*"supported" + 0.006*"2023" + 0.005*"Peterborough"']</t>
   </si>
   <si>
     <t>80538</t>
@@ -3499,7 +3499,7 @@
     <t>15/03/24</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Plymouth" + 0.006*"practice" + 0.005*"22" + 0.005*"good" + 0.005*"education" + 0.005*"timely" + 0.005*"benefit"', '0.016*"’" + 0.009*"needs" + 0.008*"Plymouth" + 0.006*"well" + 0.005*"appropriate" + 0.005*"education" + 0.005*"plans" + 0.004*"2" + 0.004*"January" + 0.004*"practice"', '0.012*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"Plymouth" + 0.005*"appropriate" + 0.005*"plans" + 0.005*"ensure" + 0.005*"practice" + 0.004*"Council" + 0.004*"22"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"Plymouth" + 0.006*"practice" + 0.005*"education" + 0.005*"quality" + 0.005*"22" + 0.005*"2" + 0.004*"plans"', '0.010*"’" + 0.008*"needs" + 0.005*"Plymouth" + 0.005*"well" + 0.005*"timely" + 0.004*"practice" + 0.004*"education" + 0.004*"2" + 0.004*"leaders" + 0.004*"February"', '0.012*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"Plymouth" + 0.005*"risks" + 0.005*"plans" + 0.005*"appropriate" + 0.005*"January" + 0.005*"22" + 0.005*"2"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3532,7 +3532,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.008*"well" + 0.007*"care-experienced" + 0.007*"Portsmouth" + 0.007*"needs" + 0.006*"plans" + 0.006*"family" + 0.005*"leaders" + 0.005*"practice" + 0.005*"health"', '0.013*"’" + 0.007*"well" + 0.006*"Portsmouth" + 0.006*"care-experienced" + 0.006*"needs" + 0.005*"family" + 0.005*"progress" + 0.005*"health" + 0.005*"plans" + 0.004*"foster"', '0.015*"’" + 0.010*"care-experienced" + 0.006*"needs" + 0.006*"well" + 0.006*"Portsmouth" + 0.006*"health" + 0.005*"family" + 0.004*"practice" + 0.004*"2023" + 0.004*"need"']</t>
+    <t>['0.019*"’" + 0.008*"well" + 0.008*"care-experienced" + 0.008*"Portsmouth" + 0.007*"needs" + 0.006*"family" + 0.005*"practice" + 0.005*"health" + 0.005*"need" + 0.005*"risk"', '0.019*"’" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"Portsmouth" + 0.006*"health" + 0.005*"family" + 0.005*"carers" + 0.004*"foster"', '0.009*"’" + 0.007*"care-experienced" + 0.006*"Portsmouth" + 0.006*"plans" + 0.005*"needs" + 0.005*"well" + 0.004*"family" + 0.004*"health" + 0.004*"receive" + 0.003*"2023"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3568,7 +3568,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"well" + 0.007*"number" + 0.007*"quality" + 0.006*"need" + 0.006*"plans" + 0.006*"effective" + 0.006*"good" + 0.005*"timely" + 0.005*"practice"', '0.010*"’" + 0.008*"quality" + 0.006*"well" + 0.005*"number" + 0.005*"good" + 0.005*"However" + 0.005*"plans" + 0.004*"effective" + 0.004*"need" + 0.004*"timely"', '0.015*"’" + 0.008*"number" + 0.007*"plans" + 0.005*"quality" + 0.005*"good" + 0.005*"well" + 0.005*"always" + 0.005*"effective" + 0.005*"carers" + 0.005*"needs"']</t>
+    <t>['0.020*"’" + 0.007*"well" + 0.007*"number" + 0.007*"quality" + 0.007*"plans" + 0.006*"effective" + 0.006*"need" + 0.006*"good" + 0.006*"timely" + 0.005*"practice"', '0.012*"’" + 0.008*"number" + 0.007*"quality" + 0.006*"well" + 0.005*"plans" + 0.005*"good" + 0.005*"However" + 0.004*"need" + 0.004*"always" + 0.004*"practice"', '0.014*"’" + 0.006*"quality" + 0.006*"plans" + 0.006*"number" + 0.005*"well" + 0.005*"good" + 0.005*"carers" + 0.004*"need" + 0.004*"However" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3592,7 +3592,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"leaders" + 0.006*"plans" + 0.006*"However" + 0.005*"Cleveland" + 0.005*"2022" + 0.005*"risk" + 0.005*"20" + 0.005*"needs" + 0.005*"response"', '0.014*"’" + 0.006*"consistently" + 0.005*"needs" + 0.005*"However" + 0.005*"plans" + 0.005*"leaders" + 0.005*"practice" + 0.005*"1" + 0.004*"risk" + 0.004*"20"', '0.022*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"carers" + 0.006*"However" + 0.006*"plans" + 0.006*"consistently" + 0.005*"practice" + 0.005*"2022" + 0.005*"Redcar"']</t>
+    <t>['0.019*"’" + 0.007*"However" + 0.007*"needs" + 0.007*"leaders" + 0.006*"consistently" + 0.006*"plans" + 0.005*"2022" + 0.005*"Redcar" + 0.005*"carers" + 0.005*"practice"', '0.017*"’" + 0.006*"practice" + 0.005*"leaders" + 0.005*"plans" + 0.005*"20" + 0.004*"Cleveland" + 0.004*"consistently" + 0.004*"needs" + 0.004*"2022" + 0.004*"Redcar"', '0.015*"’" + 0.006*"plans" + 0.005*"20" + 0.005*"leaders" + 0.005*"risk" + 0.005*"consistently" + 0.004*"needs" + 0.004*"carers" + 0.004*"However" + 0.004*"Cleveland"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3622,7 +3622,7 @@
     <t>0.1837</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.013*"experienced" + 0.007*"needs" + 0.006*"practice" + 0.006*"plans" + 0.005*"consistently" + 0.005*"good" + 0.005*"well" + 0.005*"quality" + 0.005*"progress"', '0.015*"’" + 0.009*"needs" + 0.008*"experienced" + 0.008*"practice" + 0.007*"response" + 0.006*"plans" + 0.005*"consistently" + 0.005*"good" + 0.005*"Rochdale" + 0.005*"3"', '0.027*"’" + 0.009*"practice" + 0.008*"experienced" + 0.007*"needs" + 0.006*"response" + 0.006*"quality" + 0.005*"plans" + 0.005*"consistently" + 0.005*"23" + 0.005*"Rochdale"']</t>
+    <t>['0.022*"’" + 0.009*"experienced" + 0.009*"practice" + 0.006*"needs" + 0.006*"consistently" + 0.006*"plans" + 0.006*"Rochdale" + 0.005*"good" + 0.005*"quality" + 0.005*"3"', '0.017*"’" + 0.010*"experienced" + 0.010*"needs" + 0.008*"response" + 0.008*"practice" + 0.006*"good" + 0.006*"progress" + 0.006*"plans" + 0.005*"quality" + 0.005*"consistently"', '0.022*"’" + 0.009*"experienced" + 0.007*"needs" + 0.007*"practice" + 0.006*"plans" + 0.005*"response" + 0.005*"3" + 0.005*"Rochdale" + 0.005*"consistently" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3649,7 +3649,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"needs" + 0.006*"Rotherham" + 0.006*"well" + 0.005*"ensure" + 0.004*"receive" + 0.004*"good" + 0.004*"plans" + 0.004*"27" + 0.004*"However"', '0.019*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"Council" + 0.006*"well" + 0.005*"However" + 0.005*"ensure" + 0.005*"good" + 0.004*"plans" + 0.004*"2022"', '0.010*"’" + 0.008*"Rotherham" + 0.006*"good" + 0.005*"needs" + 0.004*"plans" + 0.004*"However" + 0.004*"ensure" + 0.004*"1" + 0.004*"progress" + 0.004*"well"']</t>
+    <t>['0.012*"’" + 0.007*"Rotherham" + 0.006*"good" + 0.006*"needs" + 0.005*"ensure" + 0.005*"well" + 0.005*"However" + 0.005*"Council" + 0.004*"Metropolitan" + 0.004*"clear"', '0.017*"’" + 0.010*"Rotherham" + 0.006*"needs" + 0.005*"good" + 0.005*"plans" + 0.005*"well" + 0.005*"Council" + 0.005*"ensure" + 0.004*"protection" + 0.004*"1"', '0.016*"’" + 0.008*"Rotherham" + 0.007*"needs" + 0.006*"well" + 0.005*"However" + 0.004*"ensure" + 0.004*"plans" + 0.004*"Council" + 0.004*"27" + 0.004*"Metropolitan"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3676,7 +3676,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.012*"well" + 0.011*"practice" + 0.010*"’" + 0.007*"highly" + 0.006*"strong" + 0.005*"leaders" + 0.005*"needs" + 0.004*"professionals" + 0.004*"effective" + 0.004*"high"', '0.012*"well" + 0.010*"practice" + 0.009*"’" + 0.007*"highly" + 0.005*"needs" + 0.005*"strong" + 0.004*"effective" + 0.004*"range" + 0.003*"professionals" + 0.003*"excellent"', '0.016*"well" + 0.014*"’" + 0.011*"practice" + 0.007*"highly" + 0.007*"strong" + 0.006*"effective" + 0.006*"needs" + 0.005*"leaders" + 0.005*"progress" + 0.005*"high"']</t>
+    <t>['0.009*"practice" + 0.008*"well" + 0.008*"strong" + 0.008*"’" + 0.007*"highly" + 0.006*"effective" + 0.005*"needs" + 0.005*"leaders" + 0.005*"high" + 0.004*"professionals"', '0.015*"’" + 0.015*"well" + 0.011*"practice" + 0.008*"highly" + 0.005*"professionals" + 0.005*"strong" + 0.005*"effective" + 0.005*"high" + 0.005*"needs" + 0.005*"leaders"', '0.016*"well" + 0.012*"practice" + 0.011*"’" + 0.006*"highly" + 0.006*"strong" + 0.006*"needs" + 0.005*"effective" + 0.005*"progress" + 0.005*"leaders" + 0.004*"effectively"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3706,7 +3706,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"well" + 0.006*"good" + 0.005*"need" + 0.004*"practice" + 0.004*"information" + 0.004*"clear" + 0.004*"supported"', '0.012*"’" + 0.009*"well" + 0.008*"plans" + 0.007*"needs" + 0.004*"effective" + 0.004*"good" + 0.004*"practice" + 0.004*"clear" + 0.004*"need" + 0.004*"supported"', '0.014*"’" + 0.010*"well" + 0.009*"plans" + 0.007*"needs" + 0.005*"parents" + 0.005*"effective" + 0.005*"good" + 0.004*"clear" + 0.004*"need" + 0.004*"risk"']</t>
+    <t>['0.014*"’" + 0.009*"well" + 0.008*"plans" + 0.007*"needs" + 0.006*"good" + 0.005*"effective" + 0.004*"practice" + 0.004*"supported" + 0.004*"Kingston" + 0.004*"understand"', '0.014*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"needs" + 0.005*"need" + 0.005*"clear" + 0.004*"risk" + 0.004*"practice" + 0.004*"appropriate" + 0.004*"parents"', '0.012*"’" + 0.010*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"good" + 0.005*"effective" + 0.005*"range" + 0.005*"parents" + 0.004*"clear" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3736,7 +3736,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.005*"plans" + 0.005*"well" + 0.004*"always" + 0.004*"needs" + 0.004*"quality" + 0.004*"case" + 0.004*"actions" + 0.004*"use" + 0.004*"benefit"', '0.011*"’" + 0.005*"well" + 0.005*"quality" + 0.005*"needs" + 0.005*"use" + 0.004*"information" + 0.004*"effective" + 0.004*"benefit" + 0.004*"health" + 0.004*"need"', '0.010*"’" + 0.006*"well" + 0.005*"quality" + 0.005*"needs" + 0.005*"plans" + 0.004*"effective" + 0.004*"information" + 0.004*"good" + 0.004*"However" + 0.004*"benefit"']</t>
+    <t>['0.009*"’" + 0.005*"well" + 0.004*"quality" + 0.004*"information" + 0.004*"benefit" + 0.004*"use" + 0.004*"good" + 0.004*"plans" + 0.003*"needs" + 0.003*"effective"', '0.007*"’" + 0.005*"needs" + 0.004*"well" + 0.004*"plans" + 0.004*"risk" + 0.004*"benefit" + 0.004*"use" + 0.003*"early" + 0.003*"information" + 0.003*"quality"', '0.016*"’" + 0.006*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"plans" + 0.005*"effective" + 0.004*"health" + 0.004*"actions" + 0.004*"case" + 0.004*"information"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3760,7 +3760,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"good" + 0.006*"practice" + 0.006*"effective" + 0.005*"protection" + 0.005*"need" + 0.005*"team" + 0.005*"ensure"', '0.011*"needs" + 0.011*"well" + 0.009*"’" + 0.008*"team" + 0.007*"good" + 0.006*"ensure" + 0.006*"need" + 0.006*"practice" + 0.005*"enough" + 0.005*"plans"', '0.015*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"need" + 0.008*"good" + 0.007*"practice" + 0.006*"plans" + 0.006*"team" + 0.006*"effective" + 0.006*"enough"']</t>
+    <t>['0.010*"well" + 0.009*"’" + 0.007*"needs" + 0.006*"team" + 0.006*"plans" + 0.005*"protection" + 0.005*"practice" + 0.005*"need" + 0.005*"enough" + 0.005*"good"', '0.012*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"need" + 0.006*"team" + 0.006*"good" + 0.006*"protection" + 0.006*"effective" + 0.006*"practice" + 0.006*"enough"', '0.016*"’" + 0.011*"well" + 0.010*"good" + 0.010*"needs" + 0.007*"need" + 0.007*"practice" + 0.007*"ensure" + 0.006*"team" + 0.006*"effective" + 0.005*"enough"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3787,7 +3787,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"effective" + 0.008*"plans" + 0.008*"needs" + 0.007*"well" + 0.007*"Salford" + 0.005*"6" + 0.005*"leaders" + 0.005*"practice" + 0.005*"quality"', '0.013*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"needs" + 0.006*"effective" + 0.005*"practice" + 0.005*"Salford" + 0.005*"planning" + 0.005*"10" + 0.004*"progress"', '0.012*"’" + 0.008*"plans" + 0.007*"needs" + 0.005*"well" + 0.005*"planning" + 0.005*"effective" + 0.005*"leaders" + 0.005*"Salford" + 0.004*"progress" + 0.004*"experiences"']</t>
+    <t>['0.018*"’" + 0.010*"plans" + 0.008*"needs" + 0.007*"well" + 0.007*"effective" + 0.006*"Salford" + 0.006*"practice" + 0.005*"experiences" + 0.005*"6" + 0.005*"10"', '0.008*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"Salford" + 0.005*"effective" + 0.004*"planning" + 0.004*"City" + 0.004*"Council" + 0.004*"plans" + 0.004*"2023"', '0.010*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"Salford" + 0.006*"effective" + 0.005*"planning" + 0.005*"2023" + 0.005*"leaders" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3811,7 +3811,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"needs" + 0.008*"plans" + 0.007*"Sandwell" + 0.007*"well" + 0.005*"quality" + 0.005*"number" + 0.005*"changes" + 0.005*"progress" + 0.005*"20"', '0.014*"’" + 0.006*"Sandwell" + 0.006*"plans" + 0.005*"needs" + 0.005*"well" + 0.005*"Trust" + 0.005*"9" + 0.004*"training" + 0.004*"20" + 0.004*"education"', '0.014*"’" + 0.008*"needs" + 0.008*"Sandwell" + 0.007*"well" + 0.007*"quality" + 0.007*"plans" + 0.005*"Trust" + 0.005*"education" + 0.004*"progress" + 0.004*"many"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.008*"Sandwell" + 0.007*"well" + 0.007*"plans" + 0.007*"quality" + 0.005*"20" + 0.005*"9" + 0.004*"Trust" + 0.004*"many"', '0.012*"’" + 0.007*"Sandwell" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.005*"9" + 0.005*"education" + 0.005*"Trust" + 0.004*"quality" + 0.004*"number"', '0.010*"’" + 0.008*"plans" + 0.007*"needs" + 0.006*"Sandwell" + 0.005*"Trust" + 0.005*"quality" + 0.005*"well" + 0.005*"changes" + 0.005*"progress" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3835,7 +3835,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.011*"needs" + 0.006*"including" + 0.006*"practice" + 0.006*"lack" + 0.005*"oversight" + 0.005*"protection" + 0.005*"many" + 0.005*"◼" + 0.005*"timely"', '0.013*"’" + 0.010*"needs" + 0.006*"practice" + 0.006*"oversight" + 0.005*"always" + 0.005*"protection" + 0.005*"lack" + 0.004*"timely" + 0.004*"management" + 0.004*"4"', '0.013*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"oversight" + 0.004*"plans" + 0.004*"management" + 0.004*"many" + 0.004*"21" + 0.004*"◼" + 0.004*"response"']</t>
+    <t>['0.015*"’" + 0.012*"needs" + 0.006*"practice" + 0.006*"management" + 0.006*"lack" + 0.005*"March" + 0.005*"many" + 0.005*"◼" + 0.005*"Sefton" + 0.005*"plans"', '0.017*"’" + 0.009*"needs" + 0.007*"practice" + 0.006*"oversight" + 0.006*"timely" + 0.005*"protection" + 0.005*"including" + 0.005*"lack" + 0.005*"many" + 0.005*"management"', '0.016*"’" + 0.007*"needs" + 0.006*"oversight" + 0.005*"4" + 0.005*"including" + 0.005*"protection" + 0.005*"always" + 0.005*"practice" + 0.004*"◼" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3868,7 +3868,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Sheffield" + 0.009*"needs" + 0.006*"well" + 0.005*"practice" + 0.004*"experiences" + 0.004*"leaders" + 0.004*"health" + 0.004*"plans" + 0.004*"good"', '0.017*"’" + 0.012*"Sheffield" + 0.007*"leaders" + 0.006*"needs" + 0.005*"health" + 0.005*"well" + 0.005*"11" + 0.005*"practice" + 0.004*"quality" + 0.004*"September"', '0.025*"’" + 0.011*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.006*"practice" + 0.006*"health" + 0.005*"leaders" + 0.005*"ensure" + 0.005*"quality" + 0.005*"experiences"']</t>
+    <t>['0.022*"’" + 0.011*"needs" + 0.010*"Sheffield" + 0.007*"well" + 0.006*"practice" + 0.005*"leaders" + 0.005*"health" + 0.005*"receive" + 0.005*"plans" + 0.004*"good"', '0.021*"’" + 0.013*"Sheffield" + 0.007*"needs" + 0.007*"well" + 0.006*"health" + 0.006*"leaders" + 0.006*"practice" + 0.005*"quality" + 0.005*"adviser" + 0.004*"experiences"', '0.016*"’" + 0.009*"Sheffield" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.004*"experiences" + 0.004*"leaders" + 0.004*"receive" + 0.004*"health" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3898,7 +3898,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.006*"plans" + 0.005*"effective" + 0.005*"progress" + 0.005*"11" + 0.004*"7" + 0.004*"2022"', '0.022*"’" + 0.010*"needs" + 0.007*"Shropshire" + 0.006*"progress" + 0.006*"well" + 0.006*"2022" + 0.006*"making" + 0.005*"plans" + 0.005*"7" + 0.005*"leaders"', '0.013*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"Shropshire" + 0.004*"making" + 0.004*"plans" + 0.004*"2022" + 0.004*"7" + 0.004*"February"']</t>
+    <t>['0.018*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.006*"progress" + 0.006*"making" + 0.005*"plans" + 0.005*"7" + 0.005*"practice" + 0.005*"2022"', '0.015*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"Shropshire" + 0.005*"plans" + 0.005*"progress" + 0.005*"2022" + 0.005*"making" + 0.004*"effective" + 0.004*"training"', '0.018*"’" + 0.008*"needs" + 0.007*"Shropshire" + 0.006*"progress" + 0.005*"well" + 0.005*"plans" + 0.005*"2022" + 0.005*"7" + 0.005*"leaders" + 0.004*"11"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3922,7 +3922,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"Slough" + 0.005*"3" + 0.004*"quality" + 0.004*"impact" + 0.004*"senior" + 0.004*"supported" + 0.004*"need"', '0.013*"’" + 0.007*"Slough" + 0.006*"plans" + 0.006*"practice" + 0.006*"quality" + 0.005*"However" + 0.005*"needs" + 0.005*"need" + 0.005*"supported" + 0.005*"leaders"', '0.021*"’" + 0.009*"Slough" + 0.007*"quality" + 0.006*"practice" + 0.006*"needs" + 0.006*"3" + 0.006*"plans" + 0.005*"impact" + 0.005*"leaders" + 0.005*"PAs"']</t>
+    <t>['0.021*"’" + 0.009*"Slough" + 0.007*"plans" + 0.006*"practice" + 0.006*"quality" + 0.006*"needs" + 0.005*"impact" + 0.005*"23" + 0.005*"senior" + 0.005*"leaders"', '0.008*"’" + 0.005*"quality" + 0.004*"Slough" + 0.004*"3" + 0.004*"needs" + 0.004*"plans" + 0.004*"leaders" + 0.004*"impact" + 0.003*"practice" + 0.003*"need"', '0.013*"’" + 0.008*"Slough" + 0.008*"needs" + 0.006*"plans" + 0.006*"quality" + 0.005*"practice" + 0.005*"need" + 0.005*"However" + 0.005*"leaders" + 0.005*"3"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3946,7 +3946,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.013*"lack" + 0.007*"2022" + 0.006*"risk" + 0.006*"need" + 0.006*"Solihull" + 0.005*"quality" + 0.005*"means" + 0.005*"significant" + 0.005*"oversight"', '0.013*"’" + 0.010*"lack" + 0.007*"2022" + 0.006*"Solihull" + 0.006*"need" + 0.005*"experiences" + 0.005*"quality" + 0.005*"risk" + 0.005*"significant" + 0.005*"practice"', '0.018*"’" + 0.010*"2022" + 0.009*"lack" + 0.006*"Solihull" + 0.006*"need" + 0.006*"practice" + 0.006*"risk" + 0.006*"quality" + 0.005*"experiences" + 0.005*"effective"']</t>
+    <t>['0.015*"’" + 0.010*"lack" + 0.010*"2022" + 0.007*"Solihull" + 0.007*"need" + 0.006*"quality" + 0.006*"risk" + 0.006*"experiences" + 0.005*"significant" + 0.005*"practice"', '0.016*"’" + 0.010*"lack" + 0.007*"2022" + 0.006*"effective" + 0.006*"need" + 0.006*"risk" + 0.006*"Solihull" + 0.005*"significant" + 0.005*"quality" + 0.005*"31"', '0.015*"’" + 0.011*"lack" + 0.008*"2022" + 0.005*"need" + 0.005*"practice" + 0.005*"Solihull" + 0.005*"risk" + 0.004*"means" + 0.004*"quality" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3970,7 +3970,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"Somerset" + 0.006*"good" + 0.006*"leaders" + 0.006*"supported" + 0.005*"number" + 0.005*"progress"', '0.020*"’" + 0.010*"well" + 0.008*"needs" + 0.007*"Somerset" + 0.006*"good" + 0.006*"plans" + 0.005*"practice" + 0.005*"supported" + 0.005*"family" + 0.005*"positive"', '0.012*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"including" + 0.005*"Somerset" + 0.005*"leaders" + 0.005*"need" + 0.005*"understand" + 0.004*"progress" + 0.004*"practice"']</t>
+    <t>['0.015*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"Somerset" + 0.005*"good" + 0.005*"need" + 0.005*"impact" + 0.004*"practice" + 0.004*"leaders" + 0.004*"plans"', '0.015*"’" + 0.010*"needs" + 0.007*"well" + 0.005*"number" + 0.005*"good" + 0.005*"Somerset" + 0.004*"plans" + 0.004*"regularly" + 0.004*"progress" + 0.004*"leaders"', '0.019*"’" + 0.009*"well" + 0.008*"Somerset" + 0.008*"plans" + 0.008*"needs" + 0.007*"supported" + 0.006*"good" + 0.006*"leaders" + 0.006*"including" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3994,7 +3994,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.013*"well" + 0.012*"quality" + 0.010*"leaders" + 0.007*"good" + 0.006*"timely" + 0.006*"’" + 0.006*"needs" + 0.006*"plans" + 0.006*"practice" + 0.005*"timeliness"', '0.011*"’" + 0.010*"plans" + 0.008*"quality" + 0.008*"leaders" + 0.007*"progress" + 0.007*"well" + 0.007*"good" + 0.006*"timely" + 0.005*"needs" + 0.005*"always"', '0.011*"well" + 0.011*"quality" + 0.009*"’" + 0.007*"plans" + 0.006*"leaders" + 0.006*"good" + 0.005*"needs" + 0.004*"timely" + 0.004*"always" + 0.004*"practice"']</t>
+    <t>['0.013*"well" + 0.012*"quality" + 0.010*"leaders" + 0.009*"’" + 0.008*"good" + 0.008*"plans" + 0.006*"progress" + 0.006*"timely" + 0.005*"needs" + 0.005*"arrangements"', '0.011*"quality" + 0.009*"well" + 0.009*"’" + 0.006*"leaders" + 0.006*"plans" + 0.006*"needs" + 0.006*"good" + 0.005*"timely" + 0.005*"always" + 0.004*"◼"', '0.009*"well" + 0.008*"plans" + 0.008*"’" + 0.007*"leaders" + 0.007*"quality" + 0.006*"timely" + 0.006*"needs" + 0.006*"good" + 0.005*"timeliness" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -4027,7 +4027,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.009*"needs" + 0.007*"South" + 0.007*"Tyneside" + 0.005*"oversight" + 0.005*"5" + 0.005*"carers" + 0.004*"management" + 0.004*"2023" + 0.004*"9"', '0.024*"’" + 0.009*"needs" + 0.008*"Tyneside" + 0.008*"South" + 0.005*"effective" + 0.005*"oversight" + 0.005*"9" + 0.005*"2022" + 0.005*"practice" + 0.005*"carers"', '0.025*"’" + 0.009*"needs" + 0.007*"South" + 0.006*"Tyneside" + 0.006*"However" + 0.006*"management" + 0.005*"carers" + 0.005*"effective" + 0.004*"progress" + 0.004*"5"']</t>
+    <t>['0.017*"’" + 0.008*"needs" + 0.007*"Tyneside" + 0.006*"South" + 0.005*"2022" + 0.005*"well" + 0.005*"leaders" + 0.005*"However" + 0.004*"9" + 0.004*"carers"', '0.020*"’" + 0.009*"needs" + 0.007*"South" + 0.007*"Tyneside" + 0.005*"However" + 0.005*"9" + 0.005*"carers" + 0.005*"management" + 0.005*"effective" + 0.005*"plans"', '0.031*"’" + 0.009*"needs" + 0.008*"South" + 0.008*"Tyneside" + 0.007*"oversight" + 0.005*"5" + 0.005*"management" + 0.005*"15" + 0.005*"practice" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -4057,7 +4057,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"Southampton" + 0.006*"plans" + 0.005*"improve" + 0.005*"needs" + 0.005*"5" + 0.004*"timely" + 0.004*"including" + 0.004*"experiences" + 0.004*"progress"', '0.020*"’" + 0.006*"plans" + 0.006*"Southampton" + 0.005*"progress" + 0.005*"improve" + 0.005*"needs" + 0.004*"make" + 0.004*"5" + 0.004*"experiences" + 0.004*"provide"', '0.012*"’" + 0.005*"plans" + 0.005*"including" + 0.004*"16" + 0.004*"progress" + 0.004*"Southampton" + 0.004*"5" + 0.004*"well" + 0.004*"good" + 0.003*"improve"']</t>
+    <t>['0.012*"’" + 0.004*"Southampton" + 0.004*"timely" + 0.004*"improve" + 0.004*"including" + 0.004*"16" + 0.003*"provide" + 0.003*"needs" + 0.003*"progress" + 0.003*"5"', '0.015*"’" + 0.007*"plans" + 0.006*"Southampton" + 0.005*"needs" + 0.005*"experiences" + 0.005*"progress" + 0.005*"2023" + 0.004*"June" + 0.004*"well" + 0.004*"improve"', '0.019*"’" + 0.006*"plans" + 0.005*"improve" + 0.005*"Southampton" + 0.005*"5" + 0.005*"including" + 0.005*"progress" + 0.005*"16" + 0.004*"timely" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -4093,7 +4093,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"practice" + 0.006*"quality" + 0.006*"leaders" + 0.006*"within" + 0.006*"planning" + 0.005*"number" + 0.005*"protection" + 0.004*"However" + 0.004*"good"', '0.014*"’" + 0.008*"practice" + 0.007*"planning" + 0.007*"quality" + 0.006*"protection" + 0.006*"leaders" + 0.005*"plans" + 0.005*"always" + 0.005*"needs" + 0.005*"effective"', '0.016*"’" + 0.010*"planning" + 0.006*"quality" + 0.006*"leaders" + 0.006*"number" + 0.006*"practice" + 0.006*"always" + 0.005*"within" + 0.005*"effective" + 0.005*"need"']</t>
+    <t>['0.012*"’" + 0.009*"quality" + 0.008*"planning" + 0.007*"practice" + 0.006*"leaders" + 0.006*"always" + 0.006*"number" + 0.005*"protection" + 0.005*"well" + 0.005*"effective"', '0.014*"’" + 0.009*"planning" + 0.007*"practice" + 0.005*"protection" + 0.005*"leaders" + 0.005*"within" + 0.005*"risk" + 0.005*"effective" + 0.005*"number" + 0.005*"quality"', '0.014*"’" + 0.007*"practice" + 0.007*"planning" + 0.006*"leaders" + 0.005*"needs" + 0.005*"carers" + 0.005*"number" + 0.005*"protection" + 0.005*"within" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -4114,7 +4114,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.008*"Helens" + 0.008*"well" + 0.007*"St" + 0.006*"progress" + 0.006*"needs" + 0.005*"risk" + 0.005*"need" + 0.005*"10" + 0.005*"21"', '0.015*"’" + 0.010*"St" + 0.008*"needs" + 0.008*"Helens" + 0.006*"progress" + 0.006*"well" + 0.006*"21" + 0.006*"need" + 0.006*"receive" + 0.006*"good"', '0.011*"’" + 0.006*"Helens" + 0.006*"needs" + 0.006*"10" + 0.005*"receive" + 0.005*"good" + 0.005*"well" + 0.005*"progress" + 0.005*"St" + 0.004*"21"']</t>
+    <t>['0.011*"’" + 0.006*"St" + 0.005*"progress" + 0.005*"Helens" + 0.005*"needs" + 0.005*"10" + 0.005*"need" + 0.005*"21" + 0.004*"July" + 0.004*"good"', '0.015*"’" + 0.008*"Helens" + 0.008*"needs" + 0.007*"St" + 0.006*"receive" + 0.006*"well" + 0.006*"need" + 0.006*"10" + 0.005*"progress" + 0.005*"good"', '0.019*"’" + 0.009*"St" + 0.008*"Helens" + 0.008*"well" + 0.007*"needs" + 0.006*"21" + 0.006*"progress" + 0.006*"good" + 0.006*"risk" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -4138,7 +4138,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.013*"needs" + 0.006*"progress" + 0.006*"quality" + 0.006*"practice" + 0.006*"oversight" + 0.005*"ensure" + 0.005*"plans" + 0.005*"health" + 0.005*"6"', '0.018*"’" + 0.013*"needs" + 0.007*"quality" + 0.007*"Staffordshire" + 0.006*"health" + 0.006*"ensure" + 0.006*"practice" + 0.006*"oversight" + 0.005*"progress" + 0.005*"10"', '0.013*"’" + 0.006*"needs" + 0.006*"progress" + 0.005*"Staffordshire" + 0.005*"oversight" + 0.004*"quality" + 0.004*"health" + 0.004*"plans" + 0.004*"practice" + 0.004*"risk"']</t>
+    <t>['0.013*"needs" + 0.012*"’" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.006*"plans" + 0.005*"ensure" + 0.005*"health" + 0.005*"practice" + 0.005*"progress" + 0.005*"quality"', '0.017*"’" + 0.008*"needs" + 0.007*"quality" + 0.006*"practice" + 0.005*"ensure" + 0.005*"progress" + 0.005*"health" + 0.005*"oversight" + 0.004*"6" + 0.004*"plans"', '0.021*"’" + 0.013*"needs" + 0.006*"progress" + 0.006*"practice" + 0.006*"quality" + 0.006*"health" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.006*"ensure" + 0.005*"10"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -4165,7 +4165,7 @@
     <t>18/05/22</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"practice" + 0.007*"well" + 0.006*"Stockport" + 0.006*"strong" + 0.006*"needs" + 0.005*"plans" + 0.005*"risk" + 0.005*"28" + 0.004*"ensure"', '0.011*"’" + 0.009*"well" + 0.007*"Stockport" + 0.006*"practice" + 0.006*"needs" + 0.005*"plans" + 0.005*"leaders" + 0.005*"risk" + 0.005*"quality" + 0.005*"strong"', '0.011*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"Stockport" + 0.006*"needs" + 0.005*"strong" + 0.005*"ensure" + 0.005*"risk" + 0.004*"plans" + 0.004*"range"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.007*"Stockport" + 0.006*"practice" + 0.006*"needs" + 0.005*"strong" + 0.005*"plans" + 0.004*"1" + 0.004*"risk" + 0.004*"April"', '0.008*"’" + 0.007*"practice" + 0.006*"well" + 0.006*"needs" + 0.005*"28" + 0.004*"strong" + 0.004*"team" + 0.004*"plans" + 0.004*"1" + 0.004*"Stockport"', '0.013*"’" + 0.008*"well" + 0.008*"Stockport" + 0.008*"practice" + 0.006*"needs" + 0.006*"strong" + 0.006*"risk" + 0.006*"ensure" + 0.006*"plans" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -4201,7 +4201,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"leaders" + 0.008*"plans" + 0.007*"needs" + 0.006*"well" + 0.006*"Stockton" + 0.006*"quality" + 0.005*"senior" + 0.005*"6" + 0.005*"good"', '0.015*"’" + 0.007*"well" + 0.007*"plans" + 0.007*"leaders" + 0.006*"good" + 0.006*"quality" + 0.006*"Stockton" + 0.006*"on-Tees" + 0.005*"needs" + 0.004*"17"', '0.022*"’" + 0.010*"plans" + 0.009*"leaders" + 0.007*"needs" + 0.007*"on-Tees" + 0.006*"well" + 0.006*"quality" + 0.005*"good" + 0.005*"senior" + 0.005*"Stockton"']</t>
+    <t>['0.019*"’" + 0.009*"leaders" + 0.009*"plans" + 0.008*"well" + 0.007*"on-Tees" + 0.007*"good" + 0.006*"quality" + 0.006*"needs" + 0.005*"6" + 0.005*"senior"', '0.024*"’" + 0.009*"leaders" + 0.008*"plans" + 0.007*"needs" + 0.007*"Stockton" + 0.006*"well" + 0.006*"quality" + 0.006*"senior" + 0.006*"on-Tees" + 0.005*"good"', '0.013*"’" + 0.008*"plans" + 0.007*"leaders" + 0.006*"Stockton" + 0.006*"needs" + 0.005*"carers" + 0.005*"well" + 0.005*"quality" + 0.005*"good" + 0.005*"on-Tees"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -4225,7 +4225,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.006*"ensure" + 0.006*"well" + 0.006*"needs" + 0.006*"protection" + 0.006*"However" + 0.005*"on-Trent" + 0.005*"need" + 0.005*"plans" + 0.005*"Stoke"', '0.016*"’" + 0.010*"needs" + 0.008*"Stoke" + 0.007*"on-Trent" + 0.006*"well" + 0.006*"However" + 0.006*"quality" + 0.005*"progress" + 0.005*"plans" + 0.005*"ensure"', '0.019*"’" + 0.008*"plans" + 0.008*"needs" + 0.008*"well" + 0.007*"on-Trent" + 0.007*"Stoke" + 0.007*"However" + 0.006*"protection" + 0.005*"3" + 0.005*"ensure"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.008*"on-Trent" + 0.007*"However" + 0.007*"Stoke" + 0.007*"well" + 0.006*"ensure" + 0.005*"protection" + 0.005*"plans" + 0.005*"quality"', '0.018*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"plans" + 0.007*"Stoke" + 0.007*"on-Trent" + 0.007*"However" + 0.006*"protection" + 0.005*"progress" + 0.005*"quality"', '0.014*"’" + 0.008*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.006*"Stoke" + 0.006*"well" + 0.005*"However" + 0.005*"on-Trent" + 0.005*"protection" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -4255,7 +4255,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.006*"progress" + 0.006*"effective" + 0.005*"leaders" + 0.004*"ensure" + 0.004*"practice" + 0.004*"need" + 0.004*"carers" + 0.004*"needs"', '0.014*"’" + 0.006*"well" + 0.005*"good" + 0.005*"progress" + 0.004*"effective" + 0.004*"ensure" + 0.004*"needs" + 0.004*"practice" + 0.004*"leaders" + 0.004*"need"', '0.011*"’" + 0.008*"progress" + 0.005*"well" + 0.005*"good" + 0.005*"effective" + 0.005*"leaders" + 0.004*"ensure" + 0.004*"high" + 0.004*"new" + 0.004*"practice"']</t>
+    <t>['0.010*"’" + 0.006*"effective" + 0.006*"well" + 0.006*"leaders" + 0.006*"progress" + 0.005*"good" + 0.005*"practice" + 0.004*"ensure" + 0.004*"needs" + 0.004*"experiences"', '0.019*"’" + 0.008*"well" + 0.007*"progress" + 0.005*"need" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"good" + 0.004*"Suffolk" + 0.004*"effective" + 0.004*"carers"', '0.009*"’" + 0.006*"progress" + 0.005*"well" + 0.005*"effective" + 0.004*"ensure" + 0.004*"good" + 0.004*"high" + 0.004*"protection" + 0.004*"leaders" + 0.003*"practice"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -4288,7 +4288,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"good" + 0.006*"quality" + 0.006*"Sunderland" + 0.005*"experienced" + 0.005*"practice" + 0.004*"training" + 0.004*"high"', '0.016*"’" + 0.008*"quality" + 0.007*"well" + 0.005*"needs" + 0.005*"experienced" + 0.005*"Sunderland" + 0.005*"robust" + 0.005*"council" + 0.004*"parents" + 0.004*"TfC"', '0.016*"’" + 0.008*"well" + 0.006*"Sunderland" + 0.006*"needs" + 0.006*"quality" + 0.005*"protection" + 0.005*"practice" + 0.005*"need" + 0.004*"experienced" + 0.004*"parents"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.006*"quality" + 0.005*"Sunderland" + 0.005*"well" + 0.005*"result" + 0.005*"training" + 0.005*"good" + 0.004*"experienced" + 0.004*"protection"', '0.020*"’" + 0.008*"well" + 0.007*"quality" + 0.006*"needs" + 0.006*"Sunderland" + 0.005*"parents" + 0.005*"TfC" + 0.005*"practice" + 0.005*"experienced" + 0.005*"council"', '0.013*"’" + 0.007*"well" + 0.007*"quality" + 0.007*"needs" + 0.006*"Sunderland" + 0.005*"experienced" + 0.005*"practice" + 0.004*"highly" + 0.004*"good" + 0.004*"council"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -4318,7 +4318,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"practice" + 0.008*"progress" + 0.006*"plans" + 0.005*"carers" + 0.005*"effective" + 0.005*"good" + 0.005*"Surrey"', '0.013*"’" + 0.011*"needs" + 0.010*"well" + 0.007*"practice" + 0.006*"progress" + 0.006*"quality" + 0.005*"good" + 0.005*"effective" + 0.005*"17" + 0.005*"However"', '0.011*"’" + 0.010*"well" + 0.010*"needs" + 0.006*"practice" + 0.005*"carers" + 0.005*"progress" + 0.005*"17" + 0.005*"plans" + 0.005*"However" + 0.004*"effective"']</t>
+    <t>['0.012*"needs" + 0.011*"well" + 0.010*"’" + 0.005*"However" + 0.005*"17" + 0.005*"progress" + 0.005*"practice" + 0.005*"carers" + 0.005*"Surrey" + 0.005*"effective"', '0.017*"’" + 0.011*"well" + 0.009*"practice" + 0.009*"needs" + 0.007*"progress" + 0.007*"plans" + 0.006*"quality" + 0.006*"good" + 0.005*"carers" + 0.005*"17"', '0.013*"’" + 0.008*"needs" + 0.006*"progress" + 0.006*"practice" + 0.006*"well" + 0.005*"effective" + 0.004*"quality" + 0.004*"carers" + 0.004*"However" + 0.004*"17"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -4342,7 +4342,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.014*"needs" + 0.011*"Swindon" + 0.010*"need" + 0.009*"well" + 0.007*"plans" + 0.006*"Council" + 0.006*"health" + 0.006*"home" + 0.006*"impact"', '0.024*"’" + 0.014*"needs" + 0.009*"well" + 0.008*"need" + 0.008*"always" + 0.006*"plans" + 0.006*"Swindon" + 0.005*"many" + 0.005*"effective" + 0.005*"Borough"', '0.017*"’" + 0.010*"needs" + 0.009*"Swindon" + 0.006*"well" + 0.006*"always" + 0.006*"need" + 0.005*"impact" + 0.005*"plans" + 0.005*"effective" + 0.004*"17"']</t>
+    <t>['0.017*"’" + 0.012*"needs" + 0.009*"Swindon" + 0.007*"need" + 0.007*"well" + 0.006*"plans" + 0.006*"health" + 0.006*"always" + 0.005*"home" + 0.005*"education"', '0.018*"’" + 0.012*"needs" + 0.010*"Swindon" + 0.009*"need" + 0.009*"well" + 0.007*"always" + 0.006*"impact" + 0.005*"effective" + 0.005*"health" + 0.005*"home"', '0.029*"’" + 0.015*"needs" + 0.009*"need" + 0.008*"well" + 0.008*"Swindon" + 0.008*"plans" + 0.006*"always" + 0.005*"impact" + 0.005*"effective" + 0.005*"Borough"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -4369,7 +4369,7 @@
     <t>0.1495</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.006*"experiences" + 0.005*"risk" + 0.005*"practice" + 0.005*"Tameside" + 0.005*"impact" + 0.005*"protection" + 0.005*"15" + 0.004*"response"', '0.017*"’" + 0.009*"needs" + 0.008*"quality" + 0.005*"experienced" + 0.005*"response" + 0.005*"2023" + 0.005*"impact" + 0.005*"understand" + 0.005*"risk" + 0.005*"protection"', '0.018*"’" + 0.009*"needs" + 0.007*"impact" + 0.007*"risk" + 0.006*"experienced" + 0.006*"4" + 0.005*"practice" + 0.005*"planning" + 0.005*"Tameside" + 0.005*"15"']</t>
+    <t>['0.019*"’" + 0.011*"needs" + 0.007*"risk" + 0.006*"experienced" + 0.006*"impact" + 0.006*"practice" + 0.005*"quality" + 0.005*"15" + 0.005*"2023" + 0.005*"response"', '0.017*"’" + 0.008*"needs" + 0.005*"risk" + 0.005*"4" + 0.005*"Tameside" + 0.005*"quality" + 0.005*"practice" + 0.005*"impact" + 0.005*"understand" + 0.005*"response"', '0.011*"’" + 0.007*"needs" + 0.007*"impact" + 0.006*"risk" + 0.005*"quality" + 0.005*"2023" + 0.005*"response" + 0.004*"practice" + 0.004*"4" + 0.004*"◼"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -4393,7 +4393,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"well" + 0.007*"effective" + 0.006*"need" + 0.006*"strong" + 0.006*"needs" + 0.005*"planning" + 0.005*"practice" + 0.004*"ensure" + 0.004*"benefit"', '0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"ensure" + 0.006*"effective" + 0.005*"plans" + 0.005*"leaders" + 0.005*"practice" + 0.004*"planning" + 0.004*"strong"', '0.020*"’" + 0.013*"well" + 0.008*"needs" + 0.007*"effective" + 0.007*"plans" + 0.006*"improve" + 0.005*"practice" + 0.005*"need" + 0.004*"timely" + 0.004*"strong"']</t>
+    <t>['0.013*"’" + 0.008*"well" + 0.006*"effective" + 0.004*"practice" + 0.004*"needs" + 0.004*"planning" + 0.004*"understand" + 0.004*"strong" + 0.004*"improve" + 0.004*"plans"', '0.016*"’" + 0.013*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"ensure" + 0.006*"plans" + 0.006*"need" + 0.005*"improve" + 0.005*"practice" + 0.005*"clear"', '0.017*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"strong" + 0.006*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"leaders" + 0.005*"practice" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -4417,7 +4417,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"well" + 0.006*"carers" + 0.005*"need" + 0.004*"effective" + 0.004*"leaders" + 0.004*"needs" + 0.004*"vulnerable" + 0.004*"Thurrock" + 0.003*"impact"', '0.008*"’" + 0.006*"well" + 0.004*"carers" + 0.004*"practice" + 0.004*"need" + 0.003*"needs" + 0.003*"ensure" + 0.003*"parents" + 0.003*"protection" + 0.003*"good"', '0.015*"’" + 0.011*"well" + 0.006*"carers" + 0.006*"need" + 0.005*"needs" + 0.005*"ensure" + 0.004*"practice" + 0.004*"leaders" + 0.004*"Thurrock" + 0.004*"effective"']</t>
+    <t>['0.012*"’" + 0.008*"well" + 0.005*"carers" + 0.005*"needs" + 0.004*"Thurrock" + 0.004*"need" + 0.004*"impact" + 0.004*"practice" + 0.004*"ensure" + 0.004*"leaders"', '0.012*"’" + 0.008*"well" + 0.005*"need" + 0.005*"carers" + 0.005*"ensure" + 0.005*"needs" + 0.004*"leaders" + 0.004*"protection" + 0.004*"Thurrock" + 0.004*"practice"', '0.015*"’" + 0.009*"well" + 0.007*"carers" + 0.005*"need" + 0.004*"effective" + 0.004*"practice" + 0.003*"protect" + 0.003*"needs" + 0.003*"quality" + 0.003*"ensure"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -4441,7 +4441,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"well" + 0.009*"Torbay" + 0.006*"needs" + 0.006*"good" + 0.005*"21" + 0.005*"effective" + 0.004*"2022" + 0.004*"April" + 0.004*"team"', '0.015*"’" + 0.009*"well" + 0.007*"good" + 0.007*"needs" + 0.007*"Torbay" + 0.005*"effective" + 0.004*"agencies" + 0.004*"timely" + 0.004*"1" + 0.004*"ensure"', '0.010*"’" + 0.007*"well" + 0.005*"Torbay" + 0.004*"good" + 0.004*"April" + 0.004*"effective" + 0.004*"progress" + 0.004*"needs" + 0.004*"timely" + 0.004*"agencies"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.007*"Torbay" + 0.007*"good" + 0.006*"needs" + 0.005*"effective" + 0.005*"progress" + 0.005*"timely" + 0.005*"1" + 0.004*"April"', '0.016*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"Torbay" + 0.004*"good" + 0.004*"team" + 0.004*"progress" + 0.004*"effective" + 0.004*"timely" + 0.004*"plans"', '0.018*"’" + 0.010*"well" + 0.009*"Torbay" + 0.006*"good" + 0.005*"effective" + 0.005*"21" + 0.005*"needs" + 0.005*"2022" + 0.005*"team" + 0.004*"agencies"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4465,7 +4465,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.010*"needs" + 0.009*"Trafford" + 0.008*"well" + 0.007*"plans" + 0.007*"quality" + 0.006*"leaders" + 0.006*"ensure" + 0.005*"2" + 0.005*"impact"', '0.011*"’" + 0.008*"needs" + 0.007*"Trafford" + 0.006*"plans" + 0.005*"leaders" + 0.005*"practice" + 0.005*"well" + 0.005*"placed" + 0.004*"quality" + 0.004*"21"', '0.016*"’" + 0.009*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"quality" + 0.006*"Trafford" + 0.006*"practice" + 0.006*"team" + 0.005*"placed" + 0.005*"leaders"']</t>
+    <t>['0.017*"’" + 0.010*"needs" + 0.009*"Trafford" + 0.008*"plans" + 0.007*"well" + 0.006*"quality" + 0.005*"leaders" + 0.005*"team" + 0.005*"practice" + 0.005*"2"', '0.014*"’" + 0.008*"Trafford" + 0.007*"needs" + 0.006*"quality" + 0.006*"leaders" + 0.006*"plans" + 0.005*"well" + 0.004*"practice" + 0.004*"December" + 0.004*"impact"', '0.017*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"quality" + 0.007*"plans" + 0.007*"Trafford" + 0.006*"practice" + 0.006*"leaders" + 0.006*"placed" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4486,7 +4486,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50172854</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"Walsall" + 0.005*"needs" + 0.005*"leaders" + 0.004*"4" + 0.004*"well" + 0.004*"positive" + 0.004*"plans" + 0.004*"appropriately" + 0.004*"good"', '0.024*"’" + 0.008*"leaders" + 0.007*"needs" + 0.006*"well" + 0.005*"oversight" + 0.005*"information" + 0.004*"progress" + 0.004*"need" + 0.004*"positive" + 0.004*"October"', '0.020*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"well" + 0.006*"Walsall" + 0.006*"Senior" + 0.006*"4" + 0.005*"information" + 0.005*"good" + 0.005*"2021"']</t>
+    <t>['0.024*"’" + 0.007*"needs" + 0.007*"leaders" + 0.005*"Senior" + 0.005*"information" + 0.005*"well" + 0.005*"4" + 0.005*"risk" + 0.004*"15" + 0.004*"Walsall"', '0.019*"’" + 0.010*"leaders" + 0.007*"needs" + 0.006*"Walsall" + 0.005*"well" + 0.005*"2021" + 0.005*"information" + 0.005*"oversight" + 0.005*"good" + 0.004*"receive"', '0.020*"’" + 0.007*"well" + 0.005*"4" + 0.005*"needs" + 0.005*"Walsall" + 0.005*"oversight" + 0.004*"leaders" + 0.004*"good" + 0.004*"Senior" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4516,7 +4516,7 @@
     <t>19/08/19</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"practice" + 0.005*"Senior" + 0.005*"number" + 0.004*"need" + 0.004*"plans" + 0.004*"carers" + 0.004*"home" + 0.004*"good"', '0.016*"’" + 0.006*"well" + 0.006*"practice" + 0.004*"plans" + 0.004*"good" + 0.004*"home" + 0.004*"Senior" + 0.004*"progress" + 0.003*"parents" + 0.003*"number"', '0.013*"’" + 0.006*"practice" + 0.005*"well" + 0.005*"progress" + 0.005*"plans" + 0.004*"number" + 0.004*"small" + 0.004*"information" + 0.004*"carers" + 0.004*"provided"']</t>
+    <t>['0.011*"’" + 0.007*"well" + 0.005*"practice" + 0.004*"number" + 0.003*"Senior" + 0.003*"progress" + 0.003*"carers" + 0.003*"plans" + 0.003*"live" + 0.003*"small"', '0.018*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"Senior" + 0.005*"plans" + 0.004*"home" + 0.004*"good" + 0.004*"progress" + 0.004*"need" + 0.004*"needs"', '0.011*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"number" + 0.004*"provided" + 0.004*"information" + 0.004*"progress" + 0.004*"plans" + 0.004*"carers" + 0.004*"parents"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4546,7 +4546,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"Warwickshire" + 0.005*"practice" + 0.005*"carers" + 0.005*"clear" + 0.005*"progress" + 0.005*"quality"', '0.011*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"well" + 0.005*"Warwickshire" + 0.005*"supported" + 0.005*"carers" + 0.004*"effective" + 0.004*"information" + 0.004*"good"', '0.010*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"Warwickshire" + 0.006*"plans" + 0.005*"practice" + 0.005*"good" + 0.004*"3" + 0.004*"Senior" + 0.004*"clear"']</t>
+    <t>['0.013*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"Warwickshire" + 0.005*"plans" + 0.005*"December" + 0.004*"progress" + 0.004*"carers" + 0.004*"3"', '0.012*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"Warwickshire" + 0.006*"practice" + 0.005*"carers" + 0.005*"Senior" + 0.005*"clear" + 0.005*"November"', '0.010*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Warwickshire" + 0.005*"3" + 0.005*"practice" + 0.004*"improve" + 0.004*"clear" + 0.004*"benefit"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4576,7 +4576,7 @@
     <t>0.1667</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"West" + 0.006*"well" + 0.005*"Berkshire" + 0.005*"18" + 0.004*"need" + 0.004*"14" + 0.004*"March" + 0.004*"needs" + 0.004*"working"', '0.016*"’" + 0.007*"West" + 0.007*"well" + 0.006*"Berkshire" + 0.004*"plans" + 0.004*"agency" + 0.004*"progress" + 0.004*"need" + 0.003*"needs" + 0.003*"2022"', '0.014*"’" + 0.007*"Berkshire" + 0.006*"West" + 0.005*"well" + 0.005*"early" + 0.005*"needs" + 0.004*"plans" + 0.004*"working" + 0.004*"need" + 0.004*"March"']</t>
+    <t>['0.017*"’" + 0.008*"West" + 0.008*"Berkshire" + 0.006*"well" + 0.005*"14" + 0.004*"agency" + 0.004*"plans" + 0.004*"practice" + 0.004*"need" + 0.004*"2022"', '0.015*"’" + 0.006*"well" + 0.005*"Berkshire" + 0.005*"West" + 0.004*"early" + 0.004*"working" + 0.004*"18" + 0.004*"needs" + 0.004*"plans" + 0.004*"need"', '0.010*"’" + 0.006*"West" + 0.006*"well" + 0.005*"Berkshire" + 0.004*"need" + 0.004*"needs" + 0.004*"agency" + 0.004*"education" + 0.004*"plans" + 0.004*"information"']</t>
   </si>
   <si>
     <t>2637548</t>
@@ -4600,7 +4600,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"Northamptonshire" + 0.007*"quality" + 0.006*"well" + 0.005*"West" + 0.005*"needs" + 0.005*"NCT" + 0.005*"practice" + 0.004*"experiences" + 0.004*"plans"', '0.018*"’" + 0.008*"Northamptonshire" + 0.007*"West" + 0.007*"quality" + 0.006*"well" + 0.005*"impact" + 0.005*"practice" + 0.005*"NCT" + 0.004*"needs" + 0.004*"3"', '0.017*"’" + 0.008*"Northamptonshire" + 0.007*"West" + 0.006*"well" + 0.006*"practice" + 0.005*"quality" + 0.005*"needs" + 0.004*"need" + 0.004*"plans" + 0.004*"NCT"']</t>
+    <t>['0.017*"’" + 0.008*"Northamptonshire" + 0.007*"well" + 0.006*"quality" + 0.005*"needs" + 0.005*"West" + 0.005*"However" + 0.005*"impact" + 0.005*"need" + 0.004*"plans"', '0.021*"’" + 0.008*"Northamptonshire" + 0.007*"West" + 0.007*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"NCT" + 0.004*"needs" + 0.004*"impact" + 0.004*"experiences"', '0.013*"’" + 0.008*"Northamptonshire" + 0.006*"West" + 0.006*"quality" + 0.006*"well" + 0.006*"practice" + 0.005*"3" + 0.005*"needs" + 0.004*"NCT" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4624,7 +4624,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"13" + 0.004*"well" + 0.004*"March" + 0.004*"West" + 0.004*"health" + 0.004*"number" + 0.004*"Sussex"', '0.017*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"Sussex" + 0.004*"number" + 0.004*"supported" + 0.004*"quality" + 0.004*"13" + 0.004*"March"', '0.013*"’" + 0.007*"well" + 0.006*"West" + 0.006*"plans" + 0.005*"Sussex" + 0.005*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"number" + 0.005*"13"']</t>
+    <t>['0.016*"’" + 0.008*"plans" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"well" + 0.005*"13" + 0.005*"health" + 0.004*"West" + 0.004*"March" + 0.004*"good"', '0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"practice" + 0.005*"number" + 0.004*"West" + 0.004*"plans" + 0.004*"health" + 0.004*"supported"', '0.011*"’" + 0.007*"well" + 0.006*"West" + 0.006*"plans" + 0.005*"quality" + 0.005*"needs" + 0.005*"13" + 0.005*"number" + 0.004*"Sussex" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4645,7 +4645,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"May" + 0.007*"practice" + 0.006*"needs" + 0.006*"appropriate" + 0.006*"plans" + 0.006*"Wigan" + 0.005*"quality" + 0.005*"leaders" + 0.005*"increased"', '0.013*"’" + 0.007*"May" + 0.007*"plans" + 0.007*"quality" + 0.007*"practice" + 0.006*"Wigan" + 0.006*"needs" + 0.005*"leaders" + 0.005*"timely" + 0.005*"appropriate"', '0.010*"’" + 0.006*"May" + 0.005*"plans" + 0.005*"Wigan" + 0.004*"practice" + 0.004*"needs" + 0.004*"quality" + 0.004*"9" + 0.004*"leaders" + 0.003*"management"']</t>
+    <t>['0.011*"’" + 0.006*"quality" + 0.006*"practice" + 0.006*"needs" + 0.005*"May" + 0.005*"well" + 0.005*"Wigan" + 0.004*"plans" + 0.004*"identified" + 0.004*"2022"', '0.009*"May" + 0.009*"’" + 0.007*"plans" + 0.007*"practice" + 0.006*"needs" + 0.006*"appropriate" + 0.006*"Wigan" + 0.006*"leaders" + 0.005*"quality" + 0.005*"9"', '0.017*"’" + 0.007*"plans" + 0.007*"May" + 0.007*"Wigan" + 0.007*"practice" + 0.006*"needs" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"increased" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4678,7 +4678,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"quality" + 0.006*"progress" + 0.006*"plans" + 0.005*"need" + 0.005*"including" + 0.005*"ensure" + 0.004*"supported"', '0.014*"’" + 0.011*"well" + 0.008*"need" + 0.007*"parents" + 0.007*"risk" + 0.007*"Wiltshire" + 0.007*"supported" + 0.006*"needs" + 0.006*"progress" + 0.006*"including"', '0.016*"’" + 0.011*"well" + 0.006*"needs" + 0.006*"Wiltshire" + 0.005*"need" + 0.005*"including" + 0.005*"progress" + 0.004*"parents" + 0.004*"ensure" + 0.004*"new"']</t>
+    <t>['0.016*"’" + 0.009*"well" + 0.008*"progress" + 0.007*"needs" + 0.006*"parents" + 0.006*"risk" + 0.006*"Wiltshire" + 0.006*"supported" + 0.006*"quality" + 0.006*"need"', '0.014*"’" + 0.012*"well" + 0.007*"needs" + 0.006*"risk" + 0.005*"including" + 0.005*"ensure" + 0.005*"need" + 0.005*"Wiltshire" + 0.005*"progress" + 0.005*"parents"', '0.015*"’" + 0.013*"well" + 0.008*"need" + 0.007*"needs" + 0.006*"plans" + 0.006*"Wiltshire" + 0.005*"parents" + 0.005*"supported" + 0.005*"including" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4711,7 +4711,7 @@
     <t>0.1655</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"needs" + 0.008*"ensure" + 0.007*"well" + 0.007*"Wirral" + 0.006*"practice" + 0.006*"plans" + 0.006*"number" + 0.005*"response" + 0.005*"18"', '0.008*"’" + 0.008*"needs" + 0.006*"Wirral" + 0.005*"ensure" + 0.005*"plans" + 0.005*"practice" + 0.005*"good" + 0.004*"small" + 0.004*"2023" + 0.004*"appropriate"', '0.011*"’" + 0.010*"needs" + 0.009*"Wirral" + 0.008*"ensure" + 0.007*"plans" + 0.006*"practice" + 0.006*"number" + 0.005*"18" + 0.005*"appropriate" + 0.005*"risk"']</t>
+    <t>['0.011*"’" + 0.009*"needs" + 0.008*"Wirral" + 0.007*"plans" + 0.007*"ensure" + 0.006*"practice" + 0.005*"number" + 0.005*"well" + 0.005*"risk" + 0.005*"appropriate"', '0.011*"needs" + 0.010*"’" + 0.007*"ensure" + 0.006*"18" + 0.005*"plans" + 0.005*"number" + 0.005*"good" + 0.005*"appropriate" + 0.005*"2023" + 0.005*"well"', '0.012*"’" + 0.009*"Wirral" + 0.008*"needs" + 0.007*"practice" + 0.007*"ensure" + 0.007*"plans" + 0.006*"response" + 0.006*"well" + 0.005*"small" + 0.005*"29"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4735,7 +4735,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"effective" + 0.005*"17" + 0.005*"needs" + 0.005*"quality" + 0.005*"plans" + 0.004*"Wokingham" + 0.004*"well" + 0.004*"March" + 0.004*"good"', '0.011*"’" + 0.008*"plans" + 0.007*"needs" + 0.006*"effective" + 0.006*"well" + 0.005*"progress" + 0.005*"appropriate" + 0.005*"6" + 0.005*"experiences" + 0.005*"provided"', '0.014*"’" + 0.007*"plans" + 0.007*"progress" + 0.007*"effective" + 0.006*"provided" + 0.006*"impact" + 0.005*"well" + 0.005*"experiences" + 0.005*"needs" + 0.005*"17"']</t>
+    <t>['0.012*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"effective" + 0.005*"experiences" + 0.005*"6" + 0.005*"provided" + 0.005*"quality"', '0.012*"’" + 0.007*"effective" + 0.007*"plans" + 0.006*"progress" + 0.005*"well" + 0.005*"needs" + 0.005*"17" + 0.005*"provided" + 0.004*"impact" + 0.004*"appropriate"', '0.013*"’" + 0.006*"needs" + 0.006*"plans" + 0.006*"effective" + 0.005*"experiences" + 0.005*"progress" + 0.004*"provided" + 0.004*"17" + 0.004*"Wokingham" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4759,7 +4759,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.005*"risks" + 0.005*"Wolverhampton" + 0.005*"practice" + 0.005*"supported" + 0.005*"strong" + 0.004*"education" + 0.004*"well" + 0.004*"plans"', '0.016*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"risks" + 0.005*"City" + 0.005*"quality" + 0.005*"practice" + 0.005*"plans" + 0.005*"28" + 0.004*"risk"', '0.013*"’" + 0.008*"Wolverhampton" + 0.007*"needs" + 0.007*"effective" + 0.006*"leaders" + 0.005*"plans" + 0.005*"receive" + 0.005*"quality" + 0.005*"risk" + 0.004*"well"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.004*"effective" + 0.004*"strong" + 0.004*"quality" + 0.004*"risks" + 0.004*"Wolverhampton" + 0.003*"plans" + 0.003*"well" + 0.003*"2022"', '0.013*"’" + 0.009*"needs" + 0.007*"effective" + 0.006*"plans" + 0.006*"Wolverhampton" + 0.006*"leaders" + 0.005*"receive" + 0.005*"supported" + 0.005*"risks" + 0.005*"education"', '0.017*"’" + 0.007*"needs" + 0.006*"Wolverhampton" + 0.005*"effective" + 0.005*"risks" + 0.005*"quality" + 0.005*"education" + 0.005*"receive" + 0.004*"risk" + 0.004*"well"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4789,7 +4789,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"plans" + 0.005*"needs" + 0.005*"well" + 0.005*"ensure" + 0.005*"Worcestershire" + 0.005*"appropriate" + 0.005*"15" + 0.005*"leaders" + 0.004*"experiences"', '0.019*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"Worcestershire" + 0.007*"plans" + 0.007*"leaders" + 0.007*"progress" + 0.006*"appropriate" + 0.006*"ensure" + 0.005*"making"', '0.023*"’" + 0.009*"plans" + 0.008*"well" + 0.008*"progress" + 0.007*"needs" + 0.007*"leaders" + 0.006*"Worcestershire" + 0.006*"ensure" + 0.005*"living" + 0.005*"appropriate"']</t>
+    <t>['0.015*"’" + 0.006*"Worcestershire" + 0.006*"needs" + 0.005*"well" + 0.005*"leaders" + 0.005*"plans" + 0.004*"appropriate" + 0.004*"progress" + 0.004*"ensure" + 0.004*"26"', '0.019*"’" + 0.009*"well" + 0.007*"plans" + 0.007*"Worcestershire" + 0.006*"appropriate" + 0.006*"ensure" + 0.006*"needs" + 0.005*"progress" + 0.005*"15" + 0.005*"improve"', '0.021*"’" + 0.009*"well" + 0.009*"plans" + 0.009*"needs" + 0.009*"leaders" + 0.008*"progress" + 0.007*"Worcestershire" + 0.006*"ensure" + 0.005*"appropriate" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>urn</t>

</xml_diff>

<commit_message>
publish last updated LA reports list on web
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -70,7 +70,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.008*"needs" + 0.008*"leaders" + 0.008*"within" + 0.006*"Barnsley" + 0.005*"plans" + 0.005*"practice" + 0.005*"11" + 0.005*"understand" + 0.004*"response"', '0.013*"’" + 0.008*"needs" + 0.007*"leaders" + 0.006*"Barnsley" + 0.005*"senior" + 0.005*"practice" + 0.004*"response" + 0.004*"2023" + 0.004*"September" + 0.004*"plans"', '0.016*"’" + 0.007*"practice" + 0.007*"needs" + 0.007*"leaders" + 0.006*"within" + 0.005*"Barnsley" + 0.004*"senior" + 0.004*"appropriate" + 0.004*"partners" + 0.004*"quality"']</t>
+    <t>['0.022*"’" + 0.008*"needs" + 0.007*"Barnsley" + 0.007*"leaders" + 0.006*"practice" + 0.006*"within" + 0.005*"plans" + 0.004*"understand" + 0.004*"11" + 0.004*"2023"', '0.013*"’" + 0.007*"needs" + 0.006*"within" + 0.006*"leaders" + 0.005*"practice" + 0.004*"Barnsley" + 0.004*"response" + 0.004*"2023" + 0.004*"quality" + 0.004*"appropriate"', '0.020*"’" + 0.009*"leaders" + 0.008*"needs" + 0.007*"within" + 0.006*"practice" + 0.006*"Barnsley" + 0.005*"plans" + 0.005*"senior" + 0.005*"11" + 0.005*"response"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -115,7 +115,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"well" + 0.006*"practice" + 0.006*"needs" + 0.005*"plans" + 0.005*"East" + 0.005*"28" + 0.005*"clear" + 0.004*"leaders" + 0.004*"Somerset"', '0.014*"’" + 0.009*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"receive" + 0.005*"practice" + 0.005*"North" + 0.005*"Somerset" + 0.005*"plans" + 0.004*"leaders"', '0.024*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"leaders" + 0.005*"practice" + 0.005*"effective" + 0.005*"2022" + 0.005*"Bath" + 0.005*"impact"']</t>
+    <t>['0.020*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"receive" + 0.005*"plans" + 0.005*"impact" + 0.005*"practice" + 0.005*"Bath" + 0.004*"protection"', '0.017*"’" + 0.009*"well" + 0.006*"practice" + 0.005*"needs" + 0.005*"leaders" + 0.005*"4" + 0.005*"plans" + 0.005*"Somerset" + 0.004*"East" + 0.004*"2022"', '0.016*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"plans" + 0.005*"leaders" + 0.005*"East" + 0.005*"February" + 0.004*"North" + 0.004*"clear"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -163,7 +163,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"ensure" + 0.006*"well" + 0.005*"needs" + 0.005*"plans" + 0.005*"good" + 0.005*"Bedford" + 0.005*"education" + 0.005*"progress" + 0.004*"supported"', '0.019*"’" + 0.007*"needs" + 0.005*"ensure" + 0.005*"supported" + 0.005*"Bedford" + 0.005*"plans" + 0.004*"good" + 0.004*"15" + 0.004*"need" + 0.004*"progress"', '0.022*"’" + 0.008*"needs" + 0.007*"ensure" + 0.007*"well" + 0.005*"Bedford" + 0.005*"plans" + 0.005*"family" + 0.005*"good" + 0.005*"supported" + 0.005*"progress"']</t>
+    <t>['0.015*"’" + 0.006*"ensure" + 0.005*"needs" + 0.005*"plans" + 0.005*"Borough" + 0.005*"Bedford" + 0.004*"well" + 0.004*"supported" + 0.004*"progress" + 0.004*"15"', '0.024*"’" + 0.007*"needs" + 0.006*"good" + 0.006*"ensure" + 0.006*"well" + 0.006*"Bedford" + 0.005*"supported" + 0.005*"need" + 0.005*"plans" + 0.004*"education"', '0.017*"’" + 0.007*"needs" + 0.006*"ensure" + 0.006*"well" + 0.006*"plans" + 0.005*"supported" + 0.005*"progress" + 0.005*"education" + 0.005*"Bedford" + 0.005*"relationships"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -208,7 +208,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.012*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"effective" + 0.006*"Birmingham" + 0.006*"trust" + 0.005*"progress" + 0.005*"appropriate" + 0.004*"2023"', '0.017*"’" + 0.009*"needs" + 0.008*"effective" + 0.007*"well" + 0.006*"plans" + 0.006*"progress" + 0.006*"Birmingham" + 0.005*"3" + 0.005*"appropriate" + 0.005*"risk"', '0.012*"’" + 0.009*"needs" + 0.006*"trust" + 0.005*"well" + 0.005*"effective" + 0.005*"plans" + 0.004*"Birmingham" + 0.004*"response" + 0.004*"20" + 0.004*"risk"']</t>
+    <t>['0.010*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"trust" + 0.006*"progress" + 0.006*"effective" + 0.005*"3" + 0.004*"appropriate" + 0.004*"well" + 0.004*"Birmingham"', '0.014*"’" + 0.010*"needs" + 0.007*"well" + 0.006*"trust" + 0.006*"Birmingham" + 0.006*"effective" + 0.005*"appropriate" + 0.005*"progress" + 0.005*"leaders" + 0.004*"plans"', '0.020*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"effective" + 0.007*"plans" + 0.006*"Birmingham" + 0.005*"progress" + 0.005*"risk" + 0.005*"timely" + 0.005*"3"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -250,7 +250,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"practice" + 0.007*"needs" + 0.007*"quality" + 0.006*"Darwen" + 0.006*"impact" + 0.005*"well" + 0.005*"plans" + 0.005*"effective" + 0.005*"Blackburn"', '0.012*"’" + 0.007*"needs" + 0.006*"Blackburn" + 0.006*"practice" + 0.006*"quality" + 0.005*"well" + 0.005*"receive" + 0.005*"effective" + 0.005*"means" + 0.005*"impact"', '0.015*"’" + 0.008*"Blackburn" + 0.008*"Darwen" + 0.008*"quality" + 0.007*"needs" + 0.007*"practice" + 0.007*"well" + 0.007*"impact" + 0.006*"planning" + 0.005*"leaders"']</t>
+    <t>['0.015*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"practice" + 0.007*"Darwen" + 0.006*"impact" + 0.006*"Blackburn" + 0.005*"well" + 0.005*"4" + 0.005*"plans"', '0.015*"’" + 0.008*"Blackburn" + 0.008*"quality" + 0.008*"needs" + 0.007*"practice" + 0.007*"well" + 0.007*"Darwen" + 0.006*"impact" + 0.005*"effective" + 0.005*"result"', '0.011*"’" + 0.007*"practice" + 0.006*"needs" + 0.005*"Blackburn" + 0.005*"Darwen" + 0.005*"impact" + 0.005*"quality" + 0.005*"well" + 0.005*"planning" + 0.004*"February"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -289,7 +289,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"Blackpool" + 0.006*"effective" + 0.005*"practice" + 0.005*"plans" + 0.005*"understand" + 0.004*"supported" + 0.004*"carers"', '0.016*"’" + 0.011*"needs" + 0.008*"well" + 0.006*"Blackpool" + 0.006*"16" + 0.005*"plans" + 0.005*"5" + 0.005*"practice" + 0.005*"good" + 0.005*"supported"', '0.017*"’" + 0.011*"needs" + 0.010*"well" + 0.009*"Blackpool" + 0.006*"effective" + 0.005*"quality" + 0.005*"plans" + 0.005*"practice" + 0.005*"progress" + 0.005*"supported"']</t>
+    <t>['0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.005*"plans" + 0.005*"Blackpool" + 0.005*"effective" + 0.005*"experiences" + 0.005*"practice" + 0.004*"supported" + 0.004*"December"', '0.019*"’" + 0.013*"needs" + 0.010*"well" + 0.008*"Blackpool" + 0.006*"practice" + 0.006*"supported" + 0.005*"effective" + 0.005*"quality" + 0.005*"16" + 0.005*"plans"', '0.014*"’" + 0.009*"well" + 0.009*"Blackpool" + 0.008*"needs" + 0.007*"effective" + 0.005*"experiences" + 0.005*"16" + 0.004*"progress" + 0.004*"quality" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80432</t>
@@ -322,7 +322,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.008*"needs" + 0.006*"supported" + 0.006*"plans" + 0.006*"Bolton" + 0.006*"planning" + 0.005*"11" + 0.005*"need" + 0.005*"strong"', '0.021*"’" + 0.010*"needs" + 0.010*"Bolton" + 0.008*"plans" + 0.008*"well" + 0.006*"need" + 0.006*"effective" + 0.006*"supported" + 0.005*"11" + 0.005*"2023"', '0.017*"’" + 0.009*"needs" + 0.008*"Bolton" + 0.007*"well" + 0.007*"plans" + 0.004*"experiences" + 0.004*"15" + 0.004*"good" + 0.004*"strong" + 0.004*"planning"']</t>
+    <t>['0.018*"’" + 0.010*"well" + 0.010*"Bolton" + 0.009*"needs" + 0.007*"plans" + 0.006*"supported" + 0.006*"strong" + 0.005*"need" + 0.005*"11" + 0.005*"timely"', '0.023*"’" + 0.010*"needs" + 0.008*"Bolton" + 0.008*"plans" + 0.007*"well" + 0.006*"planning" + 0.006*"response" + 0.005*"effective" + 0.005*"need" + 0.005*"appropriate"', '0.016*"’" + 0.009*"needs" + 0.007*"plans" + 0.007*"well" + 0.007*"supported" + 0.006*"Bolton" + 0.005*"11" + 0.005*"need" + 0.005*"effective" + 0.004*"15"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -358,7 +358,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"quality" + 0.006*"practice" + 0.005*"time" + 0.005*"risk" + 0.004*"progress" + 0.004*"Bournemouth" + 0.004*"impact" + 0.004*"Poole" + 0.004*"needs"', '0.016*"’" + 0.006*"practice" + 0.006*"quality" + 0.005*"progress" + 0.005*"Bournemouth" + 0.004*"risk" + 0.004*"6" + 0.004*"17" + 0.004*"Christchurch" + 0.004*"impact"', '0.021*"’" + 0.006*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"progress" + 0.005*"6" + 0.005*"Poole" + 0.005*"Christchurch" + 0.004*"17" + 0.004*"impact"']</t>
+    <t>['0.016*"’" + 0.005*"quality" + 0.005*"practice" + 0.005*"time" + 0.005*"2021" + 0.004*"Bournemouth" + 0.004*"progress" + 0.004*"Christchurch" + 0.004*"well" + 0.004*"However"', '0.014*"’" + 0.005*"progress" + 0.005*"quality" + 0.004*"practice" + 0.004*"impact" + 0.004*"Bournemouth" + 0.004*"However" + 0.004*"Poole" + 0.004*"6" + 0.004*"17"', '0.021*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"progress" + 0.005*"risk" + 0.005*"Christchurch" + 0.005*"17" + 0.005*"Poole" + 0.005*"6" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -403,7 +403,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"Bracknell" + 0.005*"provided" + 0.005*"needs" + 0.005*"Forest" + 0.005*"progress" + 0.005*"quality" + 0.005*"effective" + 0.005*"risk" + 0.004*"positive"', '0.020*"’" + 0.008*"needs" + 0.007*"risk" + 0.006*"Bracknell" + 0.006*"effective" + 0.006*"Forest" + 0.006*"provided" + 0.006*"progress" + 0.005*"need" + 0.005*"quality"', '0.016*"’" + 0.008*"Forest" + 0.008*"good" + 0.007*"quality" + 0.007*"Bracknell" + 0.007*"needs" + 0.007*"well" + 0.006*"risk" + 0.006*"plans" + 0.005*"effective"']</t>
+    <t>['0.018*"’" + 0.007*"Bracknell" + 0.007*"risk" + 0.007*"needs" + 0.007*"effective" + 0.006*"provided" + 0.006*"Forest" + 0.006*"progress" + 0.006*"good" + 0.005*"quality"', '0.017*"’" + 0.007*"Forest" + 0.007*"quality" + 0.006*"Bracknell" + 0.006*"good" + 0.006*"effective" + 0.006*"plans" + 0.005*"positive" + 0.005*"well" + 0.005*"needs"', '0.014*"’" + 0.007*"needs" + 0.006*"Forest" + 0.006*"risk" + 0.006*"Bracknell" + 0.006*"quality" + 0.006*"good" + 0.005*"plans" + 0.005*"well" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80438</t>
@@ -439,7 +439,7 @@
     <t>0.1856</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"Brighton" + 0.006*"Hove" + 0.006*"relationships" + 0.006*"practice" + 0.005*"experiences" + 0.005*"progress" + 0.005*"2024"', '0.017*"’" + 0.007*"well" + 0.006*"Hove" + 0.006*"needs" + 0.006*"Brighton" + 0.005*"practice" + 0.005*"relationships" + 0.005*"experiences" + 0.005*"progress" + 0.005*"receive"', '0.015*"’" + 0.008*"well" + 0.007*"Hove" + 0.007*"practice" + 0.007*"Brighton" + 0.005*"needs" + 0.005*"progress" + 0.005*"experiences" + 0.004*"relationships" + 0.004*"receive"']</t>
+    <t>['0.020*"’" + 0.009*"well" + 0.008*"Brighton" + 0.008*"Hove" + 0.007*"needs" + 0.007*"relationships" + 0.006*"practice" + 0.006*"progress" + 0.006*"experiences" + 0.005*"family"', '0.015*"’" + 0.006*"practice" + 0.006*"well" + 0.006*"needs" + 0.004*"relationships" + 0.004*"15" + 0.004*"experiences" + 0.004*"progress" + 0.004*"Brighton" + 0.004*"11"', '0.011*"’" + 0.007*"Hove" + 0.006*"needs" + 0.006*"well" + 0.005*"experiences" + 0.005*"practice" + 0.004*"Brighton" + 0.004*"11" + 0.004*"receive" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -475,7 +475,7 @@
     <t>0.1875</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"good" + 0.005*"Bristol" + 0.005*"plans" + 0.005*"health" + 0.005*"need" + 0.004*"timely" + 0.004*"always"', '0.016*"’" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"Bristol" + 0.005*"health" + 0.005*"progress" + 0.005*"plans" + 0.004*"need" + 0.004*"risk"', '0.023*"’" + 0.010*"well" + 0.009*"Bristol" + 0.009*"good" + 0.008*"needs" + 0.006*"progress" + 0.005*"health" + 0.005*"leaders" + 0.005*"receive" + 0.005*"27"']</t>
+    <t>['0.022*"’" + 0.010*"well" + 0.008*"Bristol" + 0.008*"needs" + 0.007*"good" + 0.006*"health" + 0.006*"plans" + 0.006*"progress" + 0.005*"leaders" + 0.005*"need"', '0.015*"’" + 0.008*"well" + 0.007*"Bristol" + 0.007*"good" + 0.007*"needs" + 0.004*"16" + 0.004*"leaders" + 0.004*"27" + 0.004*"receive" + 0.004*"ensure"', '0.018*"’" + 0.010*"good" + 0.007*"needs" + 0.007*"well" + 0.007*"Bristol" + 0.005*"always" + 0.005*"progress" + 0.005*"ensure" + 0.005*"need" + 0.004*"January"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -505,7 +505,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.005*"Buckinghamshire" + 0.004*"number" + 0.004*"17" + 0.003*"protection" + 0.003*"plans" + 0.003*"6" + 0.003*"needs" + 0.003*"December" + 0.003*"many"', '0.017*"’" + 0.005*"plans" + 0.005*"Buckinghamshire" + 0.005*"number" + 0.005*"6" + 0.005*"practice" + 0.004*"many" + 0.004*"17" + 0.004*"December" + 0.004*"needs"', '0.013*"’" + 0.005*"plans" + 0.005*"number" + 0.005*"17" + 0.004*"protection" + 0.004*"teams" + 0.004*"2021" + 0.004*"many" + 0.004*"well" + 0.004*"Buckinghamshire"']</t>
+    <t>['0.014*"’" + 0.005*"plans" + 0.005*"17" + 0.004*"6" + 0.004*"December" + 0.004*"needs" + 0.004*"practice" + 0.004*"2021" + 0.004*"number" + 0.004*"small"', '0.014*"’" + 0.006*"number" + 0.005*"Buckinghamshire" + 0.005*"plans" + 0.004*"many" + 0.004*"17" + 0.003*"6" + 0.003*"protection" + 0.003*"progress" + 0.003*"2021"', '0.012*"’" + 0.005*"plans" + 0.005*"Buckinghamshire" + 0.004*"protection" + 0.004*"number" + 0.004*"17" + 0.004*"many" + 0.004*"6" + 0.004*"well" + 0.004*"teams"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -544,7 +544,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.008*"protection" + 0.007*"needs" + 0.006*"team" + 0.005*"2021" + 0.005*"impact" + 0.005*"Bury" + 0.005*"quality" + 0.005*"practice" + 0.005*"need"', '0.013*"’" + 0.006*"2021" + 0.006*"practice" + 0.006*"needs" + 0.005*"need" + 0.005*"team" + 0.005*"protection" + 0.005*"risk" + 0.005*"Bury" + 0.004*"quality"', '0.012*"’" + 0.007*"2021" + 0.006*"needs" + 0.006*"protection" + 0.005*"practice" + 0.005*"team" + 0.005*"impact" + 0.005*"risk" + 0.005*"need" + 0.005*"plans"']</t>
+    <t>['0.012*"’" + 0.007*"protection" + 0.007*"needs" + 0.007*"team" + 0.006*"2021" + 0.006*"practice" + 0.006*"quality" + 0.005*"need" + 0.004*"impact" + 0.004*"e"', '0.011*"’" + 0.006*"2021" + 0.006*"needs" + 0.006*"protection" + 0.005*"team" + 0.004*"new" + 0.004*"practice" + 0.004*"risk" + 0.004*"25" + 0.004*"impact"', '0.011*"’" + 0.007*"2021" + 0.006*"needs" + 0.006*"practice" + 0.006*"impact" + 0.006*"Bury" + 0.006*"need" + 0.006*"protection" + 0.006*"risk" + 0.005*"5"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -583,7 +583,7 @@
     <t>0.194</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"needs" + 0.009*"Calderdale" + 0.006*"progress" + 0.006*"plans" + 0.005*"well" + 0.005*"ensure" + 0.005*"risk" + 0.005*"parents" + 0.004*"19"', '0.027*"’" + 0.010*"needs" + 0.009*"Calderdale" + 0.007*"well" + 0.006*"plans" + 0.006*"ensure" + 0.006*"risk" + 0.005*"information" + 0.005*"progress" + 0.005*"parents"', '0.014*"’" + 0.009*"needs" + 0.006*"Calderdale" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.004*"ensure" + 0.004*"risk" + 0.004*"19" + 0.004*"experiences"']</t>
+    <t>['0.021*"’" + 0.009*"needs" + 0.008*"Calderdale" + 0.007*"well" + 0.007*"plans" + 0.007*"ensure" + 0.006*"parents" + 0.005*"progress" + 0.005*"risk" + 0.005*"need"', '0.021*"’" + 0.011*"needs" + 0.010*"Calderdale" + 0.006*"progress" + 0.006*"plans" + 0.005*"risk" + 0.005*"well" + 0.005*"experiences" + 0.005*"ensure" + 0.004*"parents"', '0.017*"’" + 0.008*"needs" + 0.006*"Calderdale" + 0.006*"well" + 0.005*"ensure" + 0.004*"progress" + 0.004*"plans" + 0.004*"information" + 0.004*"risk" + 0.004*"PAs"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -613,7 +613,7 @@
     <t>0.2052</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"Cambridgeshire" + 0.007*"needs" + 0.007*"good" + 0.005*"effective" + 0.005*"4" + 0.005*"response" + 0.005*"well" + 0.005*"quality" + 0.004*"leaders"', '0.016*"’" + 0.008*"leaders" + 0.007*"needs" + 0.005*"Cambridgeshire" + 0.005*"effective" + 0.005*"2024" + 0.005*"experiences" + 0.005*"good" + 0.005*"well" + 0.004*"4"', '0.014*"’" + 0.006*"leaders" + 0.006*"needs" + 0.006*"Cambridgeshire" + 0.005*"well" + 0.004*"quality" + 0.004*"15" + 0.004*"practice" + 0.004*"effective" + 0.004*"response"']</t>
+    <t>['0.012*"’" + 0.006*"needs" + 0.006*"quality" + 0.005*"well" + 0.005*"leaders" + 0.005*"However" + 0.004*"4" + 0.004*"good" + 0.004*"effective" + 0.004*"Cambridgeshire"', '0.016*"’" + 0.009*"Cambridgeshire" + 0.007*"needs" + 0.007*"leaders" + 0.006*"good" + 0.005*"effective" + 0.005*"15" + 0.005*"response" + 0.005*"4" + 0.005*"carers"', '0.021*"’" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.005*"good" + 0.005*"Cambridgeshire" + 0.005*"well" + 0.004*"2024" + 0.004*"strong" + 0.004*"15"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -646,7 +646,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"carers" + 0.006*"need" + 0.006*"good" + 0.006*"Bedfordshire" + 0.005*"plans" + 0.005*"Central" + 0.005*"supported"', '0.016*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"need" + 0.007*"good" + 0.006*"plans" + 0.006*"carers" + 0.005*"progress" + 0.005*"number" + 0.005*"Central"', '0.015*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"plans" + 0.005*"need" + 0.005*"carers" + 0.004*"Central" + 0.004*"ensure" + 0.004*"Leaders"']</t>
+    <t>['0.018*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"carers" + 0.007*"need" + 0.007*"good" + 0.006*"Bedfordshire" + 0.006*"plans" + 0.005*"progress" + 0.005*"effective"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"carers" + 0.005*"need" + 0.005*"good" + 0.005*"plans" + 0.004*"progress" + 0.004*"Central" + 0.004*"Bedfordshire"', '0.017*"’" + 0.009*"well" + 0.007*"need" + 0.006*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"good" + 0.005*"carers" + 0.005*"supported" + 0.004*"Central"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -682,7 +682,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"2024" + 0.007*"needs" + 0.006*"plans" + 0.006*"practice" + 0.006*"well" + 0.006*"Cheshire" + 0.005*"protection" + 0.005*"East" + 0.005*"effective"', '0.013*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"2024" + 0.006*"practice" + 0.006*"plans" + 0.006*"quality" + 0.005*"East" + 0.005*"leaders" + 0.005*"Cheshire"', '0.012*"’" + 0.008*"2024" + 0.007*"plans" + 0.007*"needs" + 0.007*"quality" + 0.006*"practice" + 0.006*"leaders" + 0.006*"well" + 0.006*"East" + 0.005*"means"']</t>
+    <t>['0.012*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"practice" + 0.007*"well" + 0.006*"Cheshire" + 0.006*"2024" + 0.006*"quality" + 0.005*"East" + 0.005*"means"', '0.016*"’" + 0.008*"2024" + 0.007*"practice" + 0.007*"needs" + 0.007*"plans" + 0.006*"quality" + 0.006*"East" + 0.006*"effective" + 0.006*"well" + 0.006*"Cheshire"', '0.009*"’" + 0.008*"2024" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"quality" + 0.005*"East" + 0.005*"need" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -721,7 +721,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.006*"needs" + 0.004*"always" + 0.004*"order" + 0.004*"learning" + 0.004*"effective" + 0.004*"information" + 0.004*"practice" + 0.004*"plans"', '0.025*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"impact" + 0.005*"timely" + 0.005*"effective" + 0.004*"effectively" + 0.004*"use" + 0.004*"plans"', '0.020*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.004*"always" + 0.004*"effectively" + 0.004*"progress" + 0.004*"plans" + 0.004*"order" + 0.004*"timely"']</t>
+    <t>['0.020*"’" + 0.007*"needs" + 0.005*"well" + 0.004*"always" + 0.004*"including" + 0.004*"practice" + 0.004*"early" + 0.004*"order" + 0.004*"impact" + 0.004*"However"', '0.016*"’" + 0.009*"well" + 0.006*"needs" + 0.005*"effective" + 0.004*"plans" + 0.004*"practice" + 0.004*"effectively" + 0.004*"timely" + 0.004*"information" + 0.004*"order"', '0.027*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"impact" + 0.005*"effectively" + 0.004*"always" + 0.004*"good" + 0.004*"receive" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -760,7 +760,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.006*"plans" + 0.005*"Bradford" + 0.005*"2" + 0.005*"◼" + 0.005*"needs" + 0.004*"risk" + 0.004*"changes" + 0.004*"need" + 0.004*"2022"', '0.021*"’" + 0.007*"plans" + 0.005*"City" + 0.005*"Bradford" + 0.005*"quality" + 0.005*"impact" + 0.005*"many" + 0.004*"2" + 0.004*"needs" + 0.004*"lack"', '0.020*"’" + 0.006*"plans" + 0.005*"needs" + 0.004*"November" + 0.004*"impact" + 0.004*"However" + 0.004*"practice" + 0.004*"Metropolitan" + 0.004*"need" + 0.004*"2"']</t>
+    <t>['0.024*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"need" + 0.004*"quality" + 0.004*"2022" + 0.004*"◼" + 0.004*"Council" + 0.004*"risk" + 0.004*"Metropolitan"', '0.021*"’" + 0.008*"plans" + 0.005*"2" + 0.005*"impact" + 0.004*"need" + 0.004*"needs" + 0.004*"senior" + 0.004*"21" + 0.004*"November" + 0.004*"risk"', '0.017*"’" + 0.006*"Bradford" + 0.006*"plans" + 0.005*"many" + 0.005*"quality" + 0.005*"needs" + 0.005*"December" + 0.005*"2" + 0.005*"◼" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -796,7 +796,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.010*"needs" + 0.010*"’" + 0.010*"well" + 0.007*"ensure" + 0.006*"effective" + 0.006*"progress" + 0.005*"practice" + 0.005*"clear" + 0.004*"good" + 0.004*"plans"', '0.014*"needs" + 0.013*"’" + 0.010*"well" + 0.008*"clear" + 0.008*"ensure" + 0.006*"effective" + 0.006*"progress" + 0.006*"supported" + 0.005*"plans" + 0.005*"good"', '0.012*"’" + 0.010*"ensure" + 0.009*"well" + 0.009*"needs" + 0.007*"effective" + 0.006*"good" + 0.006*"plans" + 0.005*"progress" + 0.005*"within" + 0.005*"experiences"']</t>
+    <t>['0.009*"well" + 0.008*"’" + 0.008*"ensure" + 0.008*"clear" + 0.008*"needs" + 0.006*"progress" + 0.005*"effective" + 0.005*"timely" + 0.005*"understanding" + 0.005*"plans"', '0.015*"needs" + 0.014*"’" + 0.010*"well" + 0.009*"ensure" + 0.007*"effective" + 0.006*"good" + 0.006*"progress" + 0.005*"plans" + 0.005*"supported" + 0.005*"clearly"', '0.011*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"ensure" + 0.006*"effective" + 0.006*"plans" + 0.006*"clear" + 0.005*"good" + 0.005*"progress" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -835,7 +835,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"quality" + 0.007*"Wakefield" + 0.007*"plans" + 0.007*"well" + 0.006*"leaders" + 0.005*"effective" + 0.005*"November" + 0.005*"good" + 0.005*"progress"', '0.013*"’" + 0.009*"well" + 0.007*"November" + 0.007*"Wakefield" + 0.006*"good" + 0.006*"plans" + 0.005*"quality" + 0.005*"effective" + 0.005*"practice" + 0.005*"receive"', '0.020*"’" + 0.009*"leaders" + 0.008*"Wakefield" + 0.008*"quality" + 0.008*"November" + 0.008*"effective" + 0.007*"good" + 0.007*"well" + 0.006*"19" + 0.006*"progress"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.007*"November" + 0.007*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"Wakefield" + 0.006*"19" + 0.006*"leaders" + 0.005*"practice"', '0.017*"’" + 0.009*"well" + 0.008*"leaders" + 0.007*"Wakefield" + 0.007*"plans" + 0.006*"quality" + 0.006*"good" + 0.006*"November" + 0.006*"effective" + 0.005*"practice"', '0.018*"’" + 0.010*"Wakefield" + 0.009*"quality" + 0.008*"November" + 0.007*"leaders" + 0.007*"plans" + 0.007*"effective" + 0.006*"good" + 0.006*"progress" + 0.006*"well"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -868,7 +868,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"March" + 0.007*"needs" + 0.007*"well" + 0.006*"effective" + 0.006*"quality" + 0.006*"York" + 0.005*"need" + 0.005*"However" + 0.005*"ensure"', '0.015*"’" + 0.006*"March" + 0.006*"effective" + 0.005*"However" + 0.005*"plans" + 0.005*"ensure" + 0.004*"well" + 0.004*"needs" + 0.004*"good" + 0.004*"practice"', '0.016*"’" + 0.009*"needs" + 0.009*"quality" + 0.007*"March" + 0.006*"York" + 0.006*"effective" + 0.005*"ensure" + 0.005*"supported" + 0.005*"plans" + 0.005*"However"']</t>
+    <t>['0.015*"’" + 0.010*"quality" + 0.009*"needs" + 0.007*"March" + 0.006*"ensure" + 0.006*"York" + 0.005*"need" + 0.005*"training" + 0.005*"However" + 0.005*"plans"', '0.010*"’" + 0.006*"needs" + 0.005*"quality" + 0.005*"effective" + 0.005*"7" + 0.005*"good" + 0.005*"well" + 0.004*"March" + 0.004*"York" + 0.004*"ensure"', '0.017*"’" + 0.008*"March" + 0.008*"effective" + 0.006*"needs" + 0.006*"However" + 0.006*"plans" + 0.005*"supported" + 0.005*"York" + 0.005*"ensure" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -907,7 +907,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.013*"well" + 0.012*"’" + 0.010*"leaders" + 0.009*"quality" + 0.008*"effective" + 0.006*"arrangements" + 0.005*"good" + 0.005*"Senior" + 0.005*"plans" + 0.005*"timely"', '0.017*"well" + 0.012*"’" + 0.010*"quality" + 0.008*"effective" + 0.008*"leaders" + 0.007*"plans" + 0.006*"timely" + 0.006*"good" + 0.005*"arrangements" + 0.005*"highly"', '0.013*"well" + 0.012*"’" + 0.009*"quality" + 0.009*"effective" + 0.007*"leaders" + 0.005*"good" + 0.005*"highly" + 0.005*"plans" + 0.005*"arrangements" + 0.005*"timely"']</t>
+    <t>['0.016*"well" + 0.012*"’" + 0.011*"quality" + 0.010*"effective" + 0.009*"leaders" + 0.006*"timely" + 0.006*"good" + 0.006*"plans" + 0.006*"arrangements" + 0.006*"highly"', '0.012*"well" + 0.011*"’" + 0.008*"quality" + 0.006*"effective" + 0.005*"arrangements" + 0.005*"leaders" + 0.005*"plans" + 0.005*"timely" + 0.005*"good" + 0.004*"ensure"', '0.014*"well" + 0.013*"’" + 0.009*"effective" + 0.009*"leaders" + 0.009*"quality" + 0.006*"good" + 0.006*"plans" + 0.005*"highly" + 0.005*"arrangements" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -940,7 +940,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"Isles" + 0.010*"Scilly" + 0.007*"practice" + 0.007*"information" + 0.007*"needs" + 0.006*"place" + 0.006*"need" + 0.005*"protection" + 0.005*"risks"', '0.018*"’" + 0.012*"Scilly" + 0.012*"Isles" + 0.009*"information" + 0.007*"need" + 0.007*"practice" + 0.007*"needs" + 0.007*"protection" + 0.006*"quality" + 0.006*"place"', '0.024*"’" + 0.013*"Scilly" + 0.013*"Isles" + 0.010*"practice" + 0.010*"need" + 0.009*"information" + 0.007*"protection" + 0.006*"needs" + 0.006*"quality" + 0.006*"risks"']</t>
+    <t>['0.023*"’" + 0.012*"Isles" + 0.011*"Scilly" + 0.010*"information" + 0.008*"needs" + 0.008*"practice" + 0.008*"protection" + 0.007*"need" + 0.006*"place" + 0.005*"13"', '0.018*"’" + 0.013*"Isles" + 0.012*"Scilly" + 0.008*"need" + 0.008*"practice" + 0.006*"information" + 0.006*"needs" + 0.005*"quality" + 0.005*"protection" + 0.005*"risks"', '0.019*"’" + 0.012*"Scilly" + 0.011*"Isles" + 0.009*"information" + 0.009*"practice" + 0.009*"need" + 0.007*"quality" + 0.006*"protection" + 0.006*"place" + 0.006*"needs"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -976,7 +976,7 @@
     <t>0.1733</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.010*"Coventry" + 0.009*"well" + 0.009*"needs" + 0.008*"supported" + 0.008*"plans" + 0.007*"strong" + 0.006*"need" + 0.006*"family" + 0.005*"training"', '0.014*"’" + 0.007*"Coventry" + 0.005*"family" + 0.005*"supported" + 0.005*"well" + 0.005*"needs" + 0.004*"need" + 0.004*"strong" + 0.004*"plans" + 0.004*"20"', '0.016*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"family" + 0.006*"supported" + 0.005*"Coventry" + 0.005*"1" + 0.005*"plans" + 0.004*"PAs" + 0.004*"2022"']</t>
+    <t>['0.017*"’" + 0.009*"Coventry" + 0.007*"needs" + 0.007*"plans" + 0.006*"supported" + 0.006*"well" + 0.006*"strong" + 0.005*"need" + 0.005*"July" + 0.004*"20"', '0.021*"’" + 0.008*"needs" + 0.007*"supported" + 0.007*"Coventry" + 0.006*"well" + 0.006*"family" + 0.006*"plans" + 0.005*"PAs" + 0.004*"strong" + 0.004*"need"', '0.019*"’" + 0.011*"well" + 0.008*"Coventry" + 0.007*"supported" + 0.007*"family" + 0.006*"needs" + 0.006*"strong" + 0.006*"plans" + 0.005*"need" + 0.004*"understand"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -1018,7 +1018,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"needs" + 0.005*"October" + 0.004*"practice" + 0.004*"quality" + 0.004*"Darlington" + 0.004*"effective" + 0.004*"21"', '0.022*"’" + 0.008*"well" + 0.007*"October" + 0.007*"practice" + 0.007*"needs" + 0.006*"leaders" + 0.006*"effective" + 0.005*"Darlington" + 0.005*"supported" + 0.004*"family"', '0.019*"’" + 0.008*"well" + 0.008*"leaders" + 0.007*"needs" + 0.007*"October" + 0.007*"Darlington" + 0.006*"practice" + 0.005*"quality" + 0.005*"education" + 0.005*"supported"']</t>
+    <t>['0.022*"’" + 0.009*"well" + 0.007*"leaders" + 0.006*"practice" + 0.006*"needs" + 0.006*"October" + 0.005*"quality" + 0.005*"Darlington" + 0.005*"effective" + 0.005*"21"', '0.020*"’" + 0.007*"needs" + 0.007*"October" + 0.006*"Darlington" + 0.006*"well" + 0.006*"leaders" + 0.006*"practice" + 0.005*"education" + 0.005*"supported" + 0.005*"quality"', '0.013*"’" + 0.008*"well" + 0.007*"October" + 0.007*"needs" + 0.007*"leaders" + 0.006*"Darlington" + 0.006*"practice" + 0.004*"effective" + 0.004*"need" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -1060,7 +1060,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.012*"needs" + 0.007*"quality" + 0.006*"leaders" + 0.006*"receive" + 0.005*"appropriate" + 0.005*"good" + 0.005*"need" + 0.005*"views" + 0.005*"Derby"', '0.013*"’" + 0.008*"needs" + 0.005*"Derby" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"progress" + 0.005*"receive" + 0.004*"good" + 0.004*"plans" + 0.004*"leaders"', '0.025*"’" + 0.010*"Derby" + 0.008*"needs" + 0.007*"receive" + 0.007*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"progress" + 0.006*"need" + 0.005*"good"']</t>
+    <t>['0.024*"’" + 0.011*"needs" + 0.010*"Derby" + 0.007*"plans" + 0.007*"quality" + 0.007*"progress" + 0.006*"need" + 0.006*"receive" + 0.006*"appropriate" + 0.006*"good"', '0.019*"’" + 0.009*"needs" + 0.006*"quality" + 0.006*"receive" + 0.006*"well" + 0.005*"good" + 0.005*"Derby" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"progress"', '0.018*"’" + 0.007*"needs" + 0.006*"receive" + 0.006*"Derby" + 0.006*"quality" + 0.005*"leaders" + 0.005*"plans" + 0.005*"need" + 0.005*"carers" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80460</t>
@@ -1093,7 +1093,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"well" + 0.006*"Derbyshire" + 0.006*"needs" + 0.005*"plans" + 0.004*"positive" + 0.004*"need" + 0.004*"practice" + 0.004*"number" + 0.004*"10"', '0.012*"’" + 0.007*"well" + 0.007*"Derbyshire" + 0.005*"effective" + 0.005*"positive" + 0.005*"leaders" + 0.005*"10" + 0.005*"need" + 0.004*"progress" + 0.004*"needs"', '0.015*"’" + 0.009*"well" + 0.007*"Derbyshire" + 0.006*"plans" + 0.005*"health" + 0.005*"good" + 0.005*"education" + 0.005*"30" + 0.004*"positive" + 0.004*"leaders"']</t>
+    <t>['0.012*"’" + 0.006*"well" + 0.006*"Derbyshire" + 0.005*"positive" + 0.005*"good" + 0.005*"needs" + 0.005*"plans" + 0.004*"education" + 0.004*"effective" + 0.004*"need"', '0.008*"’" + 0.006*"well" + 0.005*"Derbyshire" + 0.005*"education" + 0.004*"leaders" + 0.004*"health" + 0.004*"November" + 0.004*"2023" + 0.004*"practice" + 0.004*"positive"', '0.019*"’" + 0.010*"well" + 0.007*"Derbyshire" + 0.006*"plans" + 0.005*"effective" + 0.005*"leaders" + 0.005*"needs" + 0.005*"need" + 0.005*"10" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1126,7 +1126,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.005*"leaders" + 0.005*"well" + 0.005*"risk" + 0.004*"health" + 0.004*"Devon" + 0.004*"need" + 0.004*"risks" + 0.004*"protection" + 0.004*"progress"', '0.012*"’" + 0.006*"well" + 0.005*"health" + 0.005*"progress" + 0.005*"leaders" + 0.004*"case" + 0.004*"risk" + 0.004*"protection" + 0.004*"needs" + 0.004*"risks"', '0.008*"’" + 0.006*"well" + 0.004*"risk" + 0.004*"leaders" + 0.004*"Devon" + 0.004*"progress" + 0.004*"health" + 0.004*"key" + 0.003*"time" + 0.003*"case"']</t>
+    <t>['0.010*"’" + 0.006*"leaders" + 0.005*"progress" + 0.005*"case" + 0.005*"risk" + 0.005*"health" + 0.005*"well" + 0.004*"time" + 0.004*"Devon" + 0.004*"practice"', '0.008*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"health" + 0.005*"areas" + 0.004*"risk" + 0.004*"leaders" + 0.004*"need" + 0.004*"including" + 0.004*"quality"', '0.009*"’" + 0.007*"well" + 0.005*"risk" + 0.005*"health" + 0.004*"plans" + 0.004*"early" + 0.004*"protection" + 0.004*"Devon" + 0.003*"leaders" + 0.003*"case"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1168,7 +1168,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.009*"well" + 0.007*"Doncaster" + 0.006*"leaders" + 0.006*"February" + 0.005*"information" + 0.005*"plans" + 0.005*"quality" + 0.005*"records" + 0.005*"progress"', '0.012*"’" + 0.005*"Doncaster" + 0.005*"records" + 0.004*"Trust" + 0.004*"well" + 0.004*"receive" + 0.004*"many" + 0.004*"arrangements" + 0.004*"leaders" + 0.003*"progress"', '0.017*"’" + 0.006*"many" + 0.005*"progress" + 0.005*"Doncaster" + 0.005*"oversight" + 0.005*"well" + 0.005*"arrangements" + 0.005*"quality" + 0.005*"records" + 0.004*"plans"']</t>
+    <t>['0.018*"’" + 0.006*"records" + 0.005*"well" + 0.005*"leaders" + 0.005*"Doncaster" + 0.005*"plans" + 0.004*"receive" + 0.004*"quality" + 0.004*"oversight" + 0.004*"information"', '0.019*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"Doncaster" + 0.005*"arrangements" + 0.005*"many" + 0.005*"14" + 0.005*"plans" + 0.005*"experiences" + 0.005*"quality"', '0.023*"’" + 0.007*"Doncaster" + 0.006*"progress" + 0.006*"well" + 0.005*"many" + 0.005*"records" + 0.005*"Trust" + 0.005*"quality" + 0.004*"protection" + 0.004*"oversight"']</t>
   </si>
   <si>
     <t>2532283</t>
@@ -1201,7 +1201,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"Dorset" + 0.006*"good" + 0.005*"well" + 0.004*"October" + 0.004*"needs" + 0.004*"arrangements" + 0.004*"2021" + 0.004*"home" + 0.004*"leaders"', '0.014*"’" + 0.006*"good" + 0.006*"Dorset" + 0.005*"well" + 0.005*"arrangements" + 0.004*"8" + 0.004*"needs" + 0.004*"including" + 0.004*"pandemic" + 0.004*"leaders"', '0.015*"’" + 0.008*"Dorset" + 0.006*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"8" + 0.004*"arrangements" + 0.004*"quality" + 0.004*"27" + 0.004*"supported"']</t>
+    <t>['0.014*"’" + 0.008*"Dorset" + 0.007*"good" + 0.007*"well" + 0.005*"arrangements" + 0.005*"27" + 0.005*"needs" + 0.005*"Senior" + 0.005*"8" + 0.004*"October"', '0.014*"’" + 0.008*"Dorset" + 0.005*"well" + 0.005*"good" + 0.004*"needs" + 0.004*"impact" + 0.004*"supported" + 0.004*"arrangements" + 0.004*"September" + 0.004*"need"', '0.013*"’" + 0.006*"Dorset" + 0.006*"good" + 0.005*"well" + 0.004*"including" + 0.004*"needs" + 0.004*"arrangements" + 0.004*"quality" + 0.004*"8" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1234,7 +1234,7 @@
     <t>0.1605</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.013*"needs" + 0.009*"Dudley" + 0.006*"plans" + 0.006*"well" + 0.006*"quality" + 0.005*"arrangements" + 0.005*"oversight" + 0.004*"management" + 0.004*"31"', '0.017*"’" + 0.011*"needs" + 0.006*"Dudley" + 0.005*"arrangements" + 0.005*"ensure" + 0.005*"well" + 0.005*"always" + 0.005*"oversight" + 0.004*"progress" + 0.004*"31"', '0.012*"’" + 0.008*"needs" + 0.007*"Dudley" + 0.006*"always" + 0.005*"plans" + 0.005*"home" + 0.005*"October" + 0.005*"ensure" + 0.004*"well" + 0.004*"enough"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.008*"Dudley" + 0.005*"well" + 0.004*"always" + 0.004*"However" + 0.004*"oversight" + 0.004*"arrangements" + 0.004*"plans" + 0.004*"2022"', '0.016*"’" + 0.014*"needs" + 0.009*"Dudley" + 0.006*"always" + 0.006*"well" + 0.006*"plans" + 0.006*"arrangements" + 0.005*"quality" + 0.005*"oversight" + 0.005*"ensure"', '0.016*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.005*"arrangements" + 0.005*"plans" + 0.005*"well" + 0.005*"ensure" + 0.004*"However" + 0.004*"always" + 0.004*"oversight"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1273,7 +1273,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.013*"needs" + 0.008*"plans" + 0.007*"May" + 0.006*"Durham" + 0.006*"well" + 0.005*"progress" + 0.005*"ensure" + 0.004*"risks" + 0.004*"leaders"', '0.011*"needs" + 0.010*"’" + 0.007*"Durham" + 0.006*"practice" + 0.006*"well" + 0.006*"May" + 0.006*"ensure" + 0.005*"plans" + 0.005*"10" + 0.004*"leaders"', '0.016*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"May" + 0.007*"Durham" + 0.007*"ensure" + 0.006*"practice" + 0.006*"plans" + 0.005*"supported" + 0.005*"family"']</t>
+    <t>['0.011*"’" + 0.010*"needs" + 0.006*"May" + 0.006*"well" + 0.005*"plans" + 0.005*"Durham" + 0.005*"practice" + 0.004*"10" + 0.004*"ensure" + 0.004*"family"', '0.013*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"May" + 0.005*"Durham" + 0.005*"leaders" + 0.005*"ensure" + 0.005*"practice" + 0.004*"carers" + 0.004*"20"', '0.017*"’" + 0.012*"needs" + 0.009*"Durham" + 0.008*"May" + 0.008*"plans" + 0.007*"well" + 0.007*"ensure" + 0.006*"practice" + 0.005*"risks" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1309,7 +1309,7 @@
     <t>0.1742</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"plans" + 0.009*"needs" + 0.008*"well" + 0.008*"progress" + 0.006*"East" + 0.006*"Riding" + 0.005*"education" + 0.005*"supported" + 0.005*"partners"', '0.010*"’" + 0.006*"progress" + 0.006*"Riding" + 0.005*"plans" + 0.005*"well" + 0.005*"needs" + 0.005*"East" + 0.004*"January" + 0.004*"partners" + 0.003*"development"', '0.020*"’" + 0.011*"needs" + 0.009*"well" + 0.009*"plans" + 0.007*"East" + 0.006*"Riding" + 0.006*"progress" + 0.006*"10" + 0.006*"good" + 0.005*"30"']</t>
+    <t>['0.019*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"plans" + 0.006*"East" + 0.006*"Riding" + 0.006*"progress" + 0.005*"good" + 0.005*"partners" + 0.005*"education"', '0.012*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"Riding" + 0.005*"progress" + 0.005*"2023" + 0.005*"partners" + 0.004*"East" + 0.004*"30"', '0.016*"’" + 0.009*"plans" + 0.008*"progress" + 0.008*"needs" + 0.008*"well" + 0.007*"East" + 0.006*"Riding" + 0.005*"10" + 0.005*"information" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1342,7 +1342,7 @@
     <t>0.1738</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"progress" + 0.005*"Sussex" + 0.005*"plans" + 0.005*"provide" + 0.004*"effective" + 0.004*"including" + 0.004*"impact"', '0.016*"’" + 0.009*"needs" + 0.009*"East" + 0.009*"well" + 0.009*"plans" + 0.006*"progress" + 0.006*"impact" + 0.006*"including" + 0.005*"Sussex" + 0.005*"relationships"', '0.020*"’" + 0.011*"well" + 0.008*"plans" + 0.008*"Sussex" + 0.006*"progress" + 0.006*"including" + 0.006*"needs" + 0.005*"impact" + 0.005*"effective" + 0.005*"provide"']</t>
+    <t>['0.018*"’" + 0.011*"well" + 0.008*"plans" + 0.008*"Sussex" + 0.007*"progress" + 0.007*"needs" + 0.007*"including" + 0.007*"East" + 0.006*"impact" + 0.005*"experiences"', '0.019*"’" + 0.010*"needs" + 0.010*"well" + 0.008*"plans" + 0.007*"East" + 0.006*"progress" + 0.005*"11" + 0.005*"effective" + 0.005*"impact" + 0.005*"including"', '0.007*"’" + 0.006*"well" + 0.005*"plans" + 0.005*"Sussex" + 0.005*"needs" + 0.004*"East" + 0.003*"progress" + 0.003*"including" + 0.003*"provide" + 0.003*"education"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1381,7 +1381,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"progress" + 0.006*"plans" + 0.006*"Essex" + 0.006*"well" + 0.005*"needs" + 0.005*"understand" + 0.005*"risk" + 0.005*"family" + 0.005*"leaders"', '0.018*"’" + 0.008*"well" + 0.007*"progress" + 0.007*"needs" + 0.006*"plans" + 0.006*"family" + 0.005*"‘" + 0.005*"need" + 0.005*"advisers" + 0.005*"new"', '0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.006*"experiences" + 0.005*"progress" + 0.005*"helped" + 0.004*"risk" + 0.004*"parents" + 0.004*"quality"']</t>
+    <t>['0.017*"’" + 0.007*"plans" + 0.007*"well" + 0.007*"progress" + 0.007*"needs" + 0.005*"practice" + 0.005*"understand" + 0.005*"risk" + 0.005*"need" + 0.005*"new"', '0.023*"’" + 0.007*"well" + 0.006*"progress" + 0.006*"Essex" + 0.006*"family" + 0.005*"needs" + 0.005*"plans" + 0.005*"experiences" + 0.005*"supported" + 0.005*"leaders"', '0.009*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"family" + 0.005*"parents" + 0.005*"experiences" + 0.005*"plans" + 0.004*"helped" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1420,7 +1420,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"practice" + 0.007*"effective" + 0.007*"good" + 0.006*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"timely" + 0.005*"ensure" + 0.004*"plans"', '0.011*"’" + 0.007*"effective" + 0.007*"well" + 0.007*"practice" + 0.006*"quality" + 0.006*"good" + 0.005*"needs" + 0.005*"need" + 0.005*"timely" + 0.004*"improve"', '0.014*"’" + 0.010*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"needs" + 0.005*"timely" + 0.005*"practice" + 0.005*"plans" + 0.005*"early" + 0.005*"progress"']</t>
+    <t>['0.015*"’" + 0.009*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"timely" + 0.004*"improve" + 0.004*"home"', '0.010*"’" + 0.007*"effective" + 0.007*"practice" + 0.007*"timely" + 0.006*"quality" + 0.006*"good" + 0.005*"well" + 0.005*"need" + 0.005*"plans" + 0.005*"improve"', '0.015*"’" + 0.009*"effective" + 0.007*"needs" + 0.007*"good" + 0.007*"practice" + 0.006*"well" + 0.005*"quality" + 0.004*"early" + 0.004*"home" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80470</t>
@@ -1456,7 +1456,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"needs" + 0.008*"February" + 0.007*"2022" + 0.006*"well" + 0.006*"experienced" + 0.005*"plans" + 0.005*"Gloucestershire" + 0.005*"protection" + 0.005*"need"', '0.012*"’" + 0.007*"plans" + 0.006*"February" + 0.006*"2022" + 0.006*"needs" + 0.005*"progress" + 0.005*"well" + 0.005*"Gloucestershire" + 0.005*"7" + 0.004*"family"', '0.019*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"2022" + 0.005*"February" + 0.005*"progress" + 0.005*"good" + 0.005*"appropriate" + 0.005*"well" + 0.004*"experienced"']</t>
+    <t>['0.017*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"February" + 0.006*"2022" + 0.005*"well" + 0.005*"timely" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"Gloucestershire"', '0.016*"’" + 0.008*"needs" + 0.008*"February" + 0.006*"2022" + 0.005*"protection" + 0.005*"progress" + 0.005*"need" + 0.005*"Gloucestershire" + 0.004*"plans" + 0.004*"experienced"', '0.018*"’" + 0.009*"needs" + 0.008*"2022" + 0.007*"plans" + 0.006*"well" + 0.006*"February" + 0.005*"18" + 0.005*"experienced" + 0.005*"Gloucestershire" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1489,7 +1489,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"well" + 0.007*"plans" + 0.007*"needs" + 0.007*"practice" + 0.007*"risk" + 0.007*"good" + 0.006*"effective" + 0.005*"always" + 0.005*"need"', '0.013*"’" + 0.011*"well" + 0.009*"practice" + 0.008*"needs" + 0.008*"planning" + 0.007*"plans" + 0.007*"quality" + 0.006*"risk" + 0.005*"good" + 0.005*"always"', '0.011*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"need" + 0.007*"practice" + 0.007*"plans" + 0.006*"risk" + 0.006*"good" + 0.006*"always" + 0.006*"effective"']</t>
+    <t>['0.011*"well" + 0.010*"practice" + 0.010*"’" + 0.008*"needs" + 0.008*"risk" + 0.007*"plans" + 0.007*"need" + 0.007*"planning" + 0.006*"good" + 0.006*"always"', '0.016*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"plans" + 0.006*"practice" + 0.006*"effective" + 0.006*"need" + 0.005*"oversight" + 0.005*"always"', '0.011*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"risk" + 0.006*"practice" + 0.006*"quality" + 0.006*"planning" + 0.006*"need" + 0.006*"always"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1516,7 +1516,7 @@
     <t>0.1893</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"quality" + 0.005*"well" + 0.005*"leaders" + 0.005*"Hampshire" + 0.004*"highly" + 0.004*"home" + 0.004*"progress"', '0.015*"’" + 0.006*"needs" + 0.005*"plans" + 0.005*"strong" + 0.004*"well" + 0.003*"leaders" + 0.003*"quality" + 0.003*"oversight" + 0.003*"improve" + 0.003*"progress"', '0.013*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"strong" + 0.005*"home" + 0.004*"quality" + 0.004*"leaders" + 0.004*"risk" + 0.004*"improve"']</t>
+    <t>['0.024*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.004*"leaders" + 0.004*"home" + 0.004*"highly" + 0.004*"Hampshire" + 0.004*"strong"', '0.015*"’" + 0.008*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"plans" + 0.004*"Hampshire" + 0.004*"strong" + 0.004*"home" + 0.004*"health" + 0.004*"progress"', '0.014*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"quality" + 0.005*"strong" + 0.004*"leaders" + 0.004*"decisions" + 0.004*"carers" + 0.004*"highly"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1546,7 +1546,7 @@
     <t>0.2009</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.008*"Hartlepool" + 0.007*"March" + 0.007*"well" + 0.007*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.005*"effective" + 0.005*"supported" + 0.005*"18"', '0.020*"’" + 0.007*"Hartlepool" + 0.007*"needs" + 0.006*"well" + 0.006*"leaders" + 0.005*"March" + 0.005*"ensure" + 0.005*"18" + 0.005*"clear" + 0.004*"supported"', '0.016*"’" + 0.010*"March" + 0.007*"needs" + 0.005*"Hartlepool" + 0.005*"well" + 0.004*"family" + 0.004*"plans" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"experiences"']</t>
+    <t>['0.019*"’" + 0.007*"Hartlepool" + 0.007*"needs" + 0.006*"March" + 0.006*"well" + 0.005*"strong" + 0.005*"practice" + 0.004*"need" + 0.004*"leaders" + 0.004*"clear"', '0.023*"’" + 0.008*"March" + 0.008*"Hartlepool" + 0.007*"needs" + 0.007*"leaders" + 0.006*"well" + 0.005*"supported" + 0.005*"plans" + 0.005*"ensure" + 0.005*"18"', '0.015*"’" + 0.007*"March" + 0.006*"needs" + 0.006*"well" + 0.006*"Hartlepool" + 0.004*"18" + 0.004*"leaders" + 0.004*"plans" + 0.004*"22" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80474</t>
@@ -1579,7 +1579,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"lack" + 0.005*"Herefordshire" + 0.005*"impact" + 0.005*"practice" + 0.005*"18" + 0.005*"needs" + 0.004*"plans" + 0.004*"need" + 0.004*"many"', '0.019*"’" + 0.006*"practice" + 0.005*"many" + 0.005*"Herefordshire" + 0.005*"lack" + 0.004*"2022" + 0.004*"impact" + 0.004*"29" + 0.004*"risk" + 0.004*"18"', '0.019*"’" + 0.006*"Herefordshire" + 0.006*"needs" + 0.005*"practice" + 0.005*"lack" + 0.005*"impact" + 0.005*"carers" + 0.005*"plans" + 0.004*"many" + 0.004*"agency"']</t>
+    <t>['0.021*"’" + 0.007*"practice" + 0.006*"Herefordshire" + 0.006*"plans" + 0.005*"lack" + 0.005*"needs" + 0.005*"impact" + 0.005*"many" + 0.005*"carers" + 0.004*"29"', '0.016*"’" + 0.005*"Herefordshire" + 0.005*"impact" + 0.005*"needs" + 0.004*"lack" + 0.004*"many" + 0.004*"practice" + 0.004*"progress" + 0.004*"July" + 0.004*"risk"', '0.013*"’" + 0.005*"lack" + 0.005*"practice" + 0.004*"Herefordshire" + 0.004*"impact" + 0.004*"quality" + 0.004*"many" + 0.004*"2022" + 0.004*"18" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80475</t>
@@ -1612,7 +1612,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.007*"well" + 0.006*"Hertfordshire" + 0.006*"receive" + 0.006*"needs" + 0.005*"need" + 0.005*"risk" + 0.004*"plans" + 0.004*"2023" + 0.004*"27"', '0.026*"’" + 0.007*"Hertfordshire" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"receive" + 0.005*"leaders" + 0.004*"2023" + 0.004*"positive" + 0.004*"relationships"', '0.014*"’" + 0.006*"needs" + 0.006*"well" + 0.005*"Hertfordshire" + 0.005*"‘" + 0.004*"23" + 0.003*"plans" + 0.003*"27" + 0.003*"family" + 0.003*"need"']</t>
+    <t>['0.022*"’" + 0.007*"well" + 0.007*"Hertfordshire" + 0.006*"needs" + 0.006*"receive" + 0.005*"plans" + 0.004*"positive" + 0.004*"23" + 0.004*"‘" + 0.004*"risk"', '0.019*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"receive" + 0.005*"Hertfordshire" + 0.004*"leaders" + 0.004*"family" + 0.004*"2023" + 0.004*"effective" + 0.004*"23"', '0.027*"’" + 0.007*"Hertfordshire" + 0.006*"needs" + 0.005*"well" + 0.005*"need" + 0.004*"January" + 0.004*"27" + 0.004*"plans" + 0.004*"Leaders" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1642,7 +1642,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"leaders" + 0.006*"Wight" + 0.006*"Senior" + 0.006*"needs" + 0.006*"3" + 0.006*"practice" + 0.005*"well" + 0.005*"quality" + 0.005*"progress"', '0.017*"’" + 0.009*"leaders" + 0.006*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"Isle" + 0.005*"supported" + 0.005*"time" + 0.005*"good" + 0.005*"progress"', '0.016*"’" + 0.007*"leaders" + 0.005*"well" + 0.005*"needs" + 0.005*"improve" + 0.005*"supported" + 0.005*"Isle" + 0.005*"progress" + 0.004*"Senior" + 0.004*"PAs"']</t>
+    <t>['0.015*"’" + 0.007*"leaders" + 0.005*"needs" + 0.005*"Wight" + 0.005*"supported" + 0.004*"plans" + 0.004*"30" + 0.004*"improve" + 0.004*"3" + 0.004*"practice"', '0.013*"’" + 0.006*"leaders" + 0.005*"Isle" + 0.005*"well" + 0.005*"supported" + 0.005*"3" + 0.005*"needs" + 0.005*"plans" + 0.004*"30" + 0.004*"Wight"', '0.022*"’" + 0.011*"leaders" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"Senior" + 0.005*"Isle" + 0.005*"PAs" + 0.005*"plans" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1666,7 +1666,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"Kent" + 0.007*"well" + 0.007*"needs" + 0.007*"Council" + 0.006*"progress" + 0.006*"County" + 0.005*"supported" + 0.005*"leaders" + 0.005*"practice"', '0.022*"’" + 0.009*"Kent" + 0.008*"needs" + 0.005*"supported" + 0.005*"well" + 0.005*"progress" + 0.004*"Council" + 0.004*"practice" + 0.004*"County" + 0.004*"2022"', '0.018*"’" + 0.011*"Kent" + 0.007*"needs" + 0.006*"supported" + 0.006*"Council" + 0.005*"well" + 0.005*"County" + 0.004*"need" + 0.004*"including" + 0.004*"plans"']</t>
+    <t>['0.011*"’" + 0.007*"Kent" + 0.006*"supported" + 0.005*"well" + 0.004*"progress" + 0.004*"leaders" + 0.004*"Council" + 0.004*"County" + 0.004*"needs" + 0.004*"including"', '0.018*"’" + 0.010*"Kent" + 0.007*"needs" + 0.007*"Council" + 0.006*"well" + 0.006*"County" + 0.005*"supported" + 0.004*"leaders" + 0.004*"progress" + 0.004*"including"', '0.022*"’" + 0.012*"Kent" + 0.009*"needs" + 0.006*"well" + 0.006*"Council" + 0.006*"supported" + 0.005*"practice" + 0.005*"County" + 0.005*"progress" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1696,7 +1696,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"number" + 0.005*"Hull" + 0.005*"planning" + 0.005*"need" + 0.005*"management" + 0.005*"agency" + 0.005*"protection" + 0.004*"practice" + 0.004*"experiences"', '0.017*"’" + 0.007*"number" + 0.006*"planning" + 0.006*"protection" + 0.006*"Hull" + 0.006*"well" + 0.005*"practice" + 0.005*"right" + 0.005*"impact" + 0.005*"need"', '0.016*"’" + 0.007*"well" + 0.007*"planning" + 0.007*"risks" + 0.007*"practice" + 0.006*"number" + 0.006*"protection" + 0.006*"need" + 0.006*"management" + 0.006*"small"']</t>
+    <t>['0.014*"’" + 0.006*"practice" + 0.006*"planning" + 0.006*"number" + 0.006*"risks" + 0.006*"well" + 0.006*"need" + 0.005*"protection" + 0.005*"needs" + 0.005*"team"', '0.020*"’" + 0.009*"number" + 0.007*"planning" + 0.007*"well" + 0.007*"Hull" + 0.006*"management" + 0.006*"practice" + 0.006*"protection" + 0.006*"need" + 0.006*"risks"', '0.012*"’" + 0.006*"protection" + 0.006*"planning" + 0.005*"impact" + 0.005*"need" + 0.005*"management" + 0.005*"small" + 0.004*"teams" + 0.004*"progress" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1729,7 +1729,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"practice" + 0.006*"quality" + 0.006*"good" + 0.005*"Senior" + 0.005*"needs" + 0.005*"protection" + 0.005*"senior" + 0.005*"plans" + 0.005*"well"', '0.012*"’" + 0.006*"plans" + 0.006*"good" + 0.006*"quality" + 0.005*"permanence" + 0.005*"protection" + 0.005*"well" + 0.005*"training" + 0.004*"needs" + 0.004*"senior"', '0.012*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"training" + 0.006*"well" + 0.005*"good" + 0.005*"permanence" + 0.005*"Senior" + 0.005*"need" + 0.004*"team"']</t>
+    <t>['0.011*"’" + 0.008*"good" + 0.007*"practice" + 0.006*"quality" + 0.006*"permanence" + 0.006*"protection" + 0.006*"plans" + 0.005*"Senior" + 0.005*"senior" + 0.005*"needs"', '0.013*"’" + 0.006*"quality" + 0.006*"practice" + 0.005*"needs" + 0.005*"protection" + 0.005*"well" + 0.004*"good" + 0.004*"plans" + 0.004*"Senior" + 0.004*"training"', '0.011*"’" + 0.006*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"permanence" + 0.005*"plans" + 0.005*"good" + 0.004*"senior" + 0.004*"training" + 0.004*"routinely"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1768,7 +1768,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"plans" + 0.006*"progress" + 0.006*"needs" + 0.006*"Knowsley" + 0.005*"2021" + 0.005*"quality" + 0.005*"need" + 0.005*"experiences" + 0.005*"good"', '0.013*"’" + 0.008*"progress" + 0.006*"quality" + 0.006*"Knowsley" + 0.006*"needs" + 0.005*"2021" + 0.005*"plans" + 0.005*"abuse" + 0.004*"education" + 0.004*"risk"', '0.015*"’" + 0.009*"progress" + 0.009*"needs" + 0.008*"quality" + 0.007*"plans" + 0.006*"2021" + 0.006*"Knowsley" + 0.005*"good" + 0.005*"need" + 0.005*"experiences"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"quality" + 0.005*"impact" + 0.005*"Knowsley" + 0.005*"experiences" + 0.005*"good" + 0.005*"need"', '0.011*"’" + 0.009*"progress" + 0.008*"plans" + 0.007*"quality" + 0.007*"Knowsley" + 0.006*"2021" + 0.006*"needs" + 0.005*"need" + 0.005*"domestic" + 0.005*"experiences"', '0.014*"’" + 0.009*"progress" + 0.007*"needs" + 0.007*"quality" + 0.007*"plans" + 0.006*"2021" + 0.006*"Knowsley" + 0.005*"abuse" + 0.005*"11" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1801,7 +1801,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"Lancashire" + 0.006*"plans" + 0.006*"need" + 0.006*"supported" + 0.006*"practice" + 0.005*"parents" + 0.005*"health"', '0.011*"’" + 0.005*"needs" + 0.005*"need" + 0.005*"well" + 0.005*"Lancashire" + 0.004*"supported" + 0.004*"positive" + 0.004*"live" + 0.004*"homes" + 0.004*"practice"', '0.019*"’" + 0.010*"well" + 0.009*"need" + 0.007*"needs" + 0.006*"Lancashire" + 0.006*"positive" + 0.005*"progress" + 0.005*"plans" + 0.005*"supported" + 0.005*"9"']</t>
+    <t>['0.016*"’" + 0.008*"needs" + 0.007*"Lancashire" + 0.007*"need" + 0.007*"well" + 0.005*"positive" + 0.005*"plans" + 0.005*"28" + 0.005*"good" + 0.005*"supported"', '0.017*"’" + 0.010*"well" + 0.008*"need" + 0.007*"needs" + 0.006*"Lancashire" + 0.006*"supported" + 0.006*"progress" + 0.006*"health" + 0.005*"live" + 0.005*"parents"', '0.016*"’" + 0.010*"well" + 0.007*"needs" + 0.006*"need" + 0.005*"supported" + 0.005*"practice" + 0.005*"progress" + 0.005*"9" + 0.005*"Lancashire" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80481</t>
@@ -1831,7 +1831,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"needs" + 0.008*"Leeds" + 0.007*"well" + 0.006*"practice" + 0.005*"risk" + 0.005*"plans" + 0.005*"supported" + 0.005*"4" + 0.005*"ensure"', '0.014*"’" + 0.006*"Leeds" + 0.005*"needs" + 0.005*"21" + 0.005*"risk" + 0.005*"well" + 0.004*"4" + 0.004*"relationships" + 0.004*"protection" + 0.004*"ensure"', '0.013*"’" + 0.007*"Leeds" + 0.007*"needs" + 0.006*"well" + 0.005*"risk" + 0.004*"2022" + 0.004*"education" + 0.004*"protection" + 0.004*"practice" + 0.004*"ensure"']</t>
+    <t>['0.013*"’" + 0.007*"Leeds" + 0.006*"practice" + 0.005*"well" + 0.005*"risk" + 0.004*"needs" + 0.004*"plans" + 0.004*"2022" + 0.004*"4" + 0.004*"relationships"', '0.017*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.006*"risk" + 0.005*"well" + 0.005*"plans" + 0.004*"protection" + 0.004*"practice" + 0.004*"including" + 0.004*"21"', '0.017*"’" + 0.008*"needs" + 0.008*"Leeds" + 0.006*"well" + 0.005*"making" + 0.005*"ensure" + 0.005*"4" + 0.005*"protection" + 0.004*"benefit" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1867,7 +1867,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"well" + 0.010*"2021" + 0.008*"Leicester" + 0.006*"good" + 0.005*"needs" + 0.005*"September" + 0.005*"ensure" + 0.005*"number" + 0.005*"including"', '0.020*"’" + 0.008*"2021" + 0.008*"well" + 0.006*"needs" + 0.006*"Leicester" + 0.005*"20" + 0.005*"good" + 0.005*"1" + 0.005*"ensure" + 0.005*"improve"', '0.023*"’" + 0.009*"Leicester" + 0.008*"needs" + 0.008*"well" + 0.007*"2021" + 0.007*"ensure" + 0.007*"good" + 0.006*"number" + 0.006*"1" + 0.006*"20"']</t>
+    <t>['0.017*"’" + 0.010*"2021" + 0.009*"Leicester" + 0.007*"well" + 0.006*"needs" + 0.006*"number" + 0.005*"20" + 0.005*"ensure" + 0.005*"1" + 0.005*"September"', '0.021*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"Leicester" + 0.008*"2021" + 0.007*"good" + 0.006*"number" + 0.005*"ensure" + 0.005*"including" + 0.005*"1"', '0.020*"’" + 0.009*"well" + 0.008*"2021" + 0.007*"good" + 0.006*"ensure" + 0.006*"Leicester" + 0.005*"needs" + 0.005*"improve" + 0.005*"circumstances" + 0.004*"1"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1903,7 +1903,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"good" + 0.008*"needs" + 0.008*"effective" + 0.007*"quality" + 0.007*"well" + 0.005*"impact" + 0.005*"risk" + 0.005*"practice" + 0.005*"need"', '0.011*"’" + 0.008*"well" + 0.007*"good" + 0.006*"effective" + 0.006*"needs" + 0.005*"practice" + 0.005*"quality" + 0.005*"education" + 0.005*"impact" + 0.004*"need"', '0.010*"’" + 0.008*"well" + 0.008*"good" + 0.006*"needs" + 0.005*"practice" + 0.005*"effective" + 0.005*"need" + 0.005*"quality" + 0.004*"education" + 0.004*"leaders"']</t>
+    <t>['0.010*"’" + 0.008*"good" + 0.007*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"effective" + 0.005*"impact" + 0.005*"education" + 0.005*"need" + 0.005*"quality"', '0.013*"’" + 0.008*"well" + 0.008*"good" + 0.008*"quality" + 0.008*"effective" + 0.007*"needs" + 0.005*"risk" + 0.005*"impact" + 0.005*"practice" + 0.005*"need"', '0.009*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.006*"effective" + 0.005*"practice" + 0.004*"quality" + 0.004*"progress" + 0.004*"need" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1936,7 +1936,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.007*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.004*"family" + 0.004*"need" + 0.004*"24" + 0.004*"2023"', '0.024*"’" + 0.007*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"24" + 0.004*"plans" + 0.004*"28" + 0.004*"family" + 0.004*"education" + 0.004*"progress"', '0.015*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"progress" + 0.004*"well" + 0.004*"family" + 0.004*"plans" + 0.004*"need" + 0.003*"effective" + 0.003*"number"']</t>
+    <t>['0.015*"’" + 0.007*"Lincolnshire" + 0.005*"well" + 0.004*"needs" + 0.004*"progress" + 0.004*"education" + 0.003*"plans" + 0.003*"working" + 0.003*"2023" + 0.003*"provide"', '0.020*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"family" + 0.004*"well" + 0.004*"24" + 0.004*"effective" + 0.004*"need"', '0.026*"’" + 0.008*"needs" + 0.008*"Lincolnshire" + 0.007*"well" + 0.005*"plans" + 0.005*"family" + 0.005*"April" + 0.004*"28" + 0.004*"progress" + 0.004*"24"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1966,7 +1966,7 @@
     <t>25/05/23</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"needs" + 0.007*"need" + 0.007*"always" + 0.006*"Liverpool" + 0.006*"practice" + 0.006*"quality" + 0.006*"24" + 0.005*"protection" + 0.005*"timely"', '0.019*"’" + 0.007*"practice" + 0.006*"always" + 0.006*"quality" + 0.005*"Liverpool" + 0.005*"needs" + 0.005*"protection" + 0.005*"need" + 0.004*"13" + 0.004*"including"', '0.017*"’" + 0.006*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"quality" + 0.004*"Liverpool" + 0.004*"PAs" + 0.004*"including" + 0.004*"last" + 0.003*"response"']</t>
+    <t>['0.017*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"timely" + 0.004*"PAs" + 0.004*"protection" + 0.004*"senior" + 0.004*"Liverpool"', '0.019*"’" + 0.007*"always" + 0.007*"practice" + 0.005*"need" + 0.005*"protection" + 0.005*"Liverpool" + 0.004*"2023" + 0.004*"needs" + 0.004*"harm" + 0.004*"met"', '0.020*"’" + 0.009*"needs" + 0.008*"need" + 0.007*"Liverpool" + 0.007*"quality" + 0.007*"always" + 0.007*"practice" + 0.005*"13" + 0.005*"protection" + 0.005*"24"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1999,7 +1999,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.028*"’" + 0.008*"needs" + 0.007*"good" + 0.007*"plans" + 0.005*"carers" + 0.005*"well" + 0.005*"progress" + 0.005*"Barking" + 0.005*"e" + 0.005*"information"', '0.017*"’" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"well" + 0.005*"practice" + 0.005*"London" + 0.005*"information" + 0.004*"10" + 0.004*"timely"', '0.019*"’" + 0.009*"needs" + 0.005*"carers" + 0.005*"practice" + 0.004*"progress" + 0.004*"ensure" + 0.004*"well" + 0.004*"21" + 0.004*"information" + 0.004*"plans"']</t>
+    <t>['0.019*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"good" + 0.005*"well" + 0.005*"practice" + 0.004*"progress" + 0.004*"information" + 0.004*"Barking" + 0.004*"ensure"', '0.023*"’" + 0.007*"needs" + 0.005*"practice" + 0.005*"progress" + 0.005*"carers" + 0.005*"planning" + 0.005*"good" + 0.005*"10" + 0.004*"information" + 0.004*"ensure"', '0.024*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"good" + 0.006*"carers" + 0.006*"well" + 0.005*"information" + 0.005*"Dagenham" + 0.004*"effective" + 0.004*"London"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -2038,7 +2038,7 @@
     <t>0.2188</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"needs" + 0.008*"good" + 0.006*"well" + 0.006*"clear" + 0.005*"progress" + 0.005*"need" + 0.005*"risk" + 0.005*"appropriate" + 0.005*"plans"', '0.015*"’" + 0.011*"well" + 0.011*"good" + 0.010*"need" + 0.010*"needs" + 0.008*"plans" + 0.007*"ensure" + 0.007*"progress" + 0.006*"clear" + 0.005*"quality"', '0.014*"’" + 0.009*"needs" + 0.008*"good" + 0.007*"well" + 0.007*"need" + 0.006*"progress" + 0.005*"quality" + 0.005*"effective" + 0.005*"plans" + 0.005*"ensure"']</t>
+    <t>['0.014*"’" + 0.011*"good" + 0.010*"needs" + 0.009*"need" + 0.008*"well" + 0.008*"progress" + 0.006*"risk" + 0.006*"plans" + 0.006*"ensure" + 0.006*"clear"', '0.012*"’" + 0.008*"needs" + 0.008*"need" + 0.008*"well" + 0.007*"good" + 0.005*"ensure" + 0.005*"clear" + 0.005*"plans" + 0.005*"progress" + 0.004*"receive"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.009*"good" + 0.006*"plans" + 0.006*"need" + 0.005*"clear" + 0.005*"progress" + 0.005*"quality" + 0.005*"appropriate"']</t>
   </si>
   <si>
     <t>80488</t>
@@ -2065,7 +2065,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Bexley" + 0.006*"need" + 0.005*"plans" + 0.005*"6" + 0.005*"effective" + 0.005*"10" + 0.005*"make"', '0.020*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"effective" + 0.005*"plans" + 0.005*"need" + 0.005*"Bexley" + 0.005*"practice" + 0.005*"including" + 0.004*"10"', '0.016*"’" + 0.006*"effective" + 0.005*"well" + 0.005*"need" + 0.005*"needs" + 0.005*"plans" + 0.004*"10" + 0.004*"make" + 0.004*"oversight" + 0.004*"Bexley"']</t>
+    <t>['0.024*"’" + 0.006*"effective" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.004*"needs" + 0.004*"Bexley" + 0.004*"6" + 0.004*"make" + 0.004*"protection"', '0.013*"’" + 0.005*"well" + 0.005*"needs" + 0.004*"Bexley" + 0.004*"2023" + 0.004*"effective" + 0.004*"10" + 0.004*"oversight" + 0.004*"make" + 0.004*"practice"', '0.020*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"need" + 0.006*"Bexley" + 0.006*"plans" + 0.006*"effective" + 0.005*"10" + 0.005*"including" + 0.005*"clear"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -2095,7 +2095,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"progress" + 0.007*"leaders" + 0.006*"well" + 0.006*"plans" + 0.005*"Brent" + 0.005*"quality" + 0.005*"information" + 0.005*"number" + 0.005*"However"', '0.016*"’" + 0.009*"well" + 0.007*"plans" + 0.007*"good" + 0.007*"number" + 0.006*"leaders" + 0.006*"quality" + 0.005*"Brent" + 0.005*"needs" + 0.005*"senior"', '0.019*"’" + 0.010*"well" + 0.008*"leaders" + 0.007*"progress" + 0.006*"plans" + 0.005*"Brent" + 0.005*"senior" + 0.005*"practice" + 0.005*"quality" + 0.005*"good"']</t>
+    <t>['0.021*"’" + 0.009*"well" + 0.008*"leaders" + 0.008*"plans" + 0.007*"progress" + 0.007*"Brent" + 0.006*"quality" + 0.006*"practice" + 0.006*"number" + 0.005*"good"', '0.014*"’" + 0.007*"well" + 0.006*"leaders" + 0.006*"number" + 0.005*"timely" + 0.005*"progress" + 0.005*"practice" + 0.005*"plans" + 0.005*"good" + 0.004*"Brent"', '0.015*"’" + 0.009*"well" + 0.007*"good" + 0.006*"progress" + 0.006*"leaders" + 0.006*"plans" + 0.005*"small" + 0.005*"senior" + 0.005*"quality" + 0.004*"number"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -2131,7 +2131,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.011*"Bromley" + 0.008*"well" + 0.006*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.005*"education" + 0.005*"health" + 0.004*"strong" + 0.004*"13"', '0.015*"’" + 0.008*"Bromley" + 0.006*"needs" + 0.006*"well" + 0.006*"plans" + 0.005*"practice" + 0.005*"17" + 0.005*"leaders" + 0.004*"health" + 0.004*"access"', '0.014*"’" + 0.008*"Bromley" + 0.007*"needs" + 0.005*"practice" + 0.005*"plans" + 0.004*"well" + 0.004*"leaders" + 0.004*"education" + 0.004*"progress" + 0.003*"health"']</t>
+    <t>['0.023*"’" + 0.011*"Bromley" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"health" + 0.005*"practice" + 0.005*"YPAs" + 0.004*"experiences"', '0.016*"’" + 0.008*"Bromley" + 0.007*"well" + 0.006*"needs" + 0.005*"leaders" + 0.005*"plans" + 0.005*"education" + 0.004*"quality" + 0.004*"practice" + 0.004*"progress"', '0.018*"’" + 0.007*"Bromley" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"plans" + 0.005*"education" + 0.004*"leaders" + 0.004*"17" + 0.004*"access"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -2164,7 +2164,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"Camden" + 0.005*"needs" + 0.005*"leaders" + 0.005*"practice" + 0.004*"response" + 0.004*"protection" + 0.004*"well" + 0.004*"meetings" + 0.004*"appropriate"', '0.011*"’" + 0.007*"leaders" + 0.006*"Camden" + 0.006*"practice" + 0.005*"well" + 0.005*"protection" + 0.004*"response" + 0.004*"meetings" + 0.004*"needs" + 0.004*"April"', '0.011*"’" + 0.008*"Camden" + 0.007*"leaders" + 0.006*"practice" + 0.006*"well" + 0.006*"protection" + 0.005*"25" + 0.005*"needs" + 0.005*"29" + 0.005*"appropriate"']</t>
+    <t>['0.007*"’" + 0.006*"needs" + 0.006*"leaders" + 0.005*"practice" + 0.005*"well" + 0.005*"Camden" + 0.004*"protection" + 0.004*"progress" + 0.004*"29" + 0.003*"2022"', '0.011*"’" + 0.007*"Camden" + 0.007*"leaders" + 0.005*"protection" + 0.005*"practice" + 0.005*"needs" + 0.004*"appropriate" + 0.004*"progress" + 0.004*"25" + 0.004*"April"', '0.013*"’" + 0.008*"Camden" + 0.007*"practice" + 0.006*"well" + 0.006*"response" + 0.006*"leaders" + 0.005*"protection" + 0.005*"29" + 0.005*"meetings" + 0.005*"25"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -2197,7 +2197,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"Croydon" + 0.005*"quality" + 0.005*"Senior" + 0.005*"education" + 0.004*"need" + 0.004*"risk" + 0.004*"plans"', '0.014*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"quality" + 0.006*"health" + 0.006*"plans" + 0.006*"effective" + 0.005*"Croydon" + 0.005*"need" + 0.005*"Senior"', '0.010*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"Croydon" + 0.006*"need" + 0.005*"Senior" + 0.005*"ensure" + 0.005*"However" + 0.005*"quality"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"ensure" + 0.006*"Croydon" + 0.006*"Senior" + 0.006*"need" + 0.005*"quality" + 0.005*"effective" + 0.005*"good"', '0.011*"’" + 0.007*"needs" + 0.006*"need" + 0.006*"well" + 0.006*"quality" + 0.005*"health" + 0.005*"Senior" + 0.005*"effective" + 0.004*"good" + 0.004*"Croydon"', '0.009*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Croydon" + 0.005*"good" + 0.005*"plans" + 0.005*"education" + 0.005*"Senior" + 0.005*"quality" + 0.005*"improved"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2233,7 +2233,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.010*"quality" + 0.008*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"good" + 0.005*"progress" + 0.004*"oversight" + 0.004*"Ealing" + 0.004*"experiences" + 0.004*"family"', '0.012*"’" + 0.012*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"progress" + 0.006*"risk" + 0.005*"plans" + 0.005*"experiences" + 0.004*"provide" + 0.004*"family"', '0.012*"’" + 0.007*"quality" + 0.006*"good" + 0.005*"well" + 0.005*"needs" + 0.004*"leaders" + 0.004*"fully" + 0.004*"risk" + 0.004*"provide" + 0.004*"management"']</t>
+    <t>['0.011*"’" + 0.011*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"progress" + 0.005*"risk" + 0.004*"well" + 0.004*"oversight" + 0.004*"experiences" + 0.004*"family"', '0.012*"’" + 0.009*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.006*"progress" + 0.005*"risk" + 0.005*"experiences" + 0.004*"leaders" + 0.004*"family"', '0.009*"’" + 0.008*"quality" + 0.005*"needs" + 0.004*"good" + 0.004*"plans" + 0.004*"well" + 0.004*"management" + 0.004*"risk" + 0.004*"progress" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80494</t>
@@ -2266,7 +2266,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.010*"needs" + 0.008*"practice" + 0.006*"good" + 0.006*"timely" + 0.006*"ensure" + 0.006*"Enfield" + 0.006*"effective" + 0.005*"clear" + 0.005*"need"', '0.012*"’" + 0.008*"good" + 0.008*"ensure" + 0.007*"Enfield" + 0.007*"needs" + 0.006*"quality" + 0.006*"clear" + 0.006*"effective" + 0.006*"practice" + 0.005*"progress"', '0.015*"’" + 0.009*"practice" + 0.008*"needs" + 0.008*"ensure" + 0.007*"effective" + 0.007*"leaders" + 0.007*"quality" + 0.007*"clear" + 0.007*"good" + 0.006*"Enfield"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.009*"practice" + 0.009*"ensure" + 0.008*"clear" + 0.007*"effective" + 0.007*"quality" + 0.006*"good" + 0.006*"Enfield" + 0.006*"timely"', '0.012*"’" + 0.008*"needs" + 0.008*"practice" + 0.008*"good" + 0.008*"ensure" + 0.006*"leaders" + 0.006*"timely" + 0.006*"quality" + 0.005*"Enfield" + 0.005*"effective"', '0.014*"’" + 0.007*"needs" + 0.007*"effective" + 0.007*"good" + 0.007*"Enfield" + 0.006*"ensure" + 0.006*"clear" + 0.006*"range" + 0.006*"improve" + 0.005*"arrangements"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2299,7 +2299,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.012*"well" + 0.009*"good" + 0.008*"needs" + 0.007*"range" + 0.006*"need" + 0.006*"plans" + 0.005*"consistently" + 0.005*"ensure" + 0.005*"progress"', '0.010*"’" + 0.008*"well" + 0.008*"plans" + 0.007*"needs" + 0.006*"need" + 0.006*"good" + 0.006*"ensure" + 0.005*"progress" + 0.005*"timely" + 0.005*"range"', '0.013*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"good" + 0.007*"needs" + 0.006*"need" + 0.005*"risk" + 0.005*"range" + 0.005*"quality" + 0.005*"progress"']</t>
+    <t>['0.010*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"ensure" + 0.005*"progress" + 0.005*"need" + 0.005*"range" + 0.004*"effective"', '0.014*"’" + 0.011*"well" + 0.009*"good" + 0.008*"needs" + 0.006*"need" + 0.006*"range" + 0.006*"plans" + 0.006*"risk" + 0.006*"ensure" + 0.006*"consistently"', '0.011*"’" + 0.009*"well" + 0.009*"plans" + 0.007*"good" + 0.007*"needs" + 0.006*"need" + 0.005*"range" + 0.005*"effective" + 0.005*"progress" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2338,7 +2338,7 @@
     <t>0.1417</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"practice" + 0.007*"planning" + 0.006*"number" + 0.006*"quality" + 0.006*"including" + 0.006*"effective" + 0.005*"need" + 0.005*"needs" + 0.005*"small"', '0.012*"’" + 0.011*"practice" + 0.007*"number" + 0.006*"needs" + 0.006*"within" + 0.005*"plans" + 0.005*"planning" + 0.005*"effective" + 0.005*"including" + 0.005*"cases"', '0.012*"’" + 0.010*"practice" + 0.006*"plans" + 0.006*"effective" + 0.006*"planning" + 0.006*"carers" + 0.006*"small" + 0.006*"protection" + 0.006*"within" + 0.005*"quality"']</t>
+    <t>['0.015*"’" + 0.009*"practice" + 0.007*"number" + 0.006*"planning" + 0.006*"need" + 0.006*"needs" + 0.006*"effective" + 0.005*"within" + 0.005*"cases" + 0.005*"leaders"', '0.014*"’" + 0.010*"practice" + 0.007*"plans" + 0.006*"needs" + 0.006*"effective" + 0.006*"within" + 0.006*"quality" + 0.006*"including" + 0.006*"However" + 0.006*"small"', '0.010*"’" + 0.009*"practice" + 0.006*"number" + 0.006*"planning" + 0.005*"including" + 0.005*"effective" + 0.005*"quality" + 0.005*"within" + 0.005*"plans" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2371,7 +2371,7 @@
     <t>0.1986</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"well" + 0.006*"receive" + 0.005*"needs" + 0.005*"Hammersmith" + 0.004*"11" + 0.004*"effective" + 0.004*"plans" + 0.004*"protection" + 0.003*"2024"', '0.020*"’" + 0.008*"well" + 0.006*"receive" + 0.005*"plans" + 0.005*"Fulham" + 0.005*"needs" + 0.004*"Leaders" + 0.004*"leaders" + 0.004*"effective" + 0.004*"2024"', '0.010*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"supported" + 0.005*"receive" + 0.005*"Hammersmith" + 0.004*"protection" + 0.004*"understand" + 0.004*"Fulham" + 0.004*"timely"']</t>
+    <t>['0.016*"’" + 0.008*"well" + 0.006*"receive" + 0.005*"Hammersmith" + 0.005*"understand" + 0.004*"effective" + 0.004*"supported" + 0.004*"needs" + 0.004*"Fulham" + 0.004*"leaders"', '0.014*"’" + 0.006*"well" + 0.005*"needs" + 0.004*"receive" + 0.004*"practice" + 0.004*"plans" + 0.004*"need" + 0.004*"Hammersmith" + 0.004*"Fulham" + 0.004*"Leaders"', '0.014*"’" + 0.007*"well" + 0.006*"receive" + 0.006*"needs" + 0.005*"plans" + 0.005*"leaders" + 0.005*"15" + 0.005*"Fulham" + 0.004*"protection" + 0.004*"2024"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2395,7 +2395,7 @@
     <t>13/02/2023</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"plans" + 0.009*"Haringey" + 0.006*"needs" + 0.006*"need" + 0.006*"well" + 0.005*"education" + 0.005*"good" + 0.005*"risk" + 0.004*"24"', '0.017*"’" + 0.008*"needs" + 0.008*"Haringey" + 0.006*"plans" + 0.005*"well" + 0.005*"good" + 0.005*"need" + 0.004*"progress" + 0.004*"education" + 0.004*"supported"', '0.013*"’" + 0.008*"needs" + 0.008*"Haringey" + 0.006*"well" + 0.006*"good" + 0.005*"progress" + 0.005*"plans" + 0.005*"training" + 0.005*"impact" + 0.004*"need"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Haringey" + 0.005*"plans" + 0.004*"well" + 0.004*"need" + 0.004*"practice" + 0.004*"risk" + 0.003*"improve" + 0.003*"supported"', '0.017*"’" + 0.010*"needs" + 0.009*"Haringey" + 0.008*"plans" + 0.007*"well" + 0.005*"good" + 0.005*"progress" + 0.005*"risk" + 0.005*"timely" + 0.005*"supported"', '0.016*"’" + 0.009*"Haringey" + 0.007*"plans" + 0.006*"good" + 0.006*"need" + 0.006*"needs" + 0.006*"well" + 0.005*"progress" + 0.005*"education" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2428,7 +2428,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.010*"well" + 0.010*"good" + 0.008*"needs" + 0.006*"plans" + 0.006*"experiences" + 0.006*"impact" + 0.005*"early" + 0.005*"practice" + 0.004*"school"', '0.010*"’" + 0.010*"good" + 0.006*"needs" + 0.006*"well" + 0.006*"protection" + 0.004*"need" + 0.004*"early" + 0.004*"impact" + 0.004*"practice" + 0.004*"plans"', '0.012*"’" + 0.011*"good" + 0.009*"needs" + 0.008*"well" + 0.006*"need" + 0.005*"practice" + 0.005*"protection" + 0.005*"impact" + 0.005*"plans" + 0.004*"quality"']</t>
+    <t>['0.011*"’" + 0.010*"good" + 0.009*"well" + 0.008*"needs" + 0.005*"practice" + 0.005*"team" + 0.005*"plans" + 0.005*"impact" + 0.005*"experiences" + 0.005*"need"', '0.011*"’" + 0.010*"good" + 0.008*"needs" + 0.008*"well" + 0.006*"need" + 0.005*"early" + 0.004*"experiences" + 0.004*"protection" + 0.004*"impact" + 0.004*"school"', '0.013*"’" + 0.012*"good" + 0.008*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"impact" + 0.006*"protection" + 0.005*"practice" + 0.005*"planning" + 0.004*"early"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2455,7 +2455,7 @@
     <t>16/02/24</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.014*"Havering" + 0.007*"plans" + 0.007*"quality" + 0.006*"effective" + 0.005*"oversight" + 0.005*"11" + 0.005*"needs" + 0.004*"2023" + 0.004*"December"', '0.017*"’" + 0.012*"Havering" + 0.009*"quality" + 0.008*"plans" + 0.005*"oversight" + 0.005*"22" + 0.005*"needs" + 0.004*"practice" + 0.004*"effective" + 0.004*"many"', '0.017*"’" + 0.009*"quality" + 0.007*"Havering" + 0.006*"plans" + 0.006*"oversight" + 0.005*"effective" + 0.004*"11" + 0.004*"practice" + 0.004*"needs" + 0.004*"2023"']</t>
+    <t>['0.020*"’" + 0.011*"Havering" + 0.007*"plans" + 0.007*"quality" + 0.006*"effective" + 0.006*"oversight" + 0.005*"many" + 0.004*"22" + 0.004*"experiences" + 0.004*"needs"', '0.018*"’" + 0.013*"Havering" + 0.010*"quality" + 0.008*"plans" + 0.005*"oversight" + 0.005*"needs" + 0.005*"practice" + 0.004*"11" + 0.004*"22" + 0.004*"2023"', '0.014*"’" + 0.009*"Havering" + 0.008*"quality" + 0.006*"effective" + 0.006*"plans" + 0.005*"practice" + 0.005*"needs" + 0.004*"oversight" + 0.004*"11" + 0.004*"December"']</t>
   </si>
   <si>
     <t>80501</t>
@@ -2488,7 +2488,7 @@
     <t>0.2119</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"Hillingdon" + 0.007*"needs" + 0.007*"plans" + 0.007*"well" + 0.004*"2023" + 0.004*"supported" + 0.004*"need" + 0.004*"timely" + 0.004*"2"', '0.019*"’" + 0.011*"needs" + 0.009*"plans" + 0.008*"Hillingdon" + 0.007*"well" + 0.006*"team" + 0.005*"2" + 0.004*"need" + 0.004*"PAs" + 0.004*"6"', '0.017*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Hillingdon" + 0.007*"plans" + 0.005*"need" + 0.005*"carers" + 0.004*"family" + 0.004*"6" + 0.004*"leaders"']</t>
+    <t>['0.017*"’" + 0.009*"needs" + 0.009*"Hillingdon" + 0.008*"plans" + 0.006*"well" + 0.005*"2" + 0.004*"leaders" + 0.004*"team" + 0.004*"improve" + 0.004*"need"', '0.019*"’" + 0.010*"needs" + 0.009*"plans" + 0.009*"well" + 0.008*"Hillingdon" + 0.005*"need" + 0.005*"team" + 0.004*"6" + 0.004*"family" + 0.004*"senior"', '0.015*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Hillingdon" + 0.005*"plans" + 0.005*"team" + 0.004*"6" + 0.004*"need" + 0.003*"2023" + 0.003*"2"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2521,7 +2521,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"effective" + 0.006*"Hounslow" + 0.006*"plans" + 0.006*"timely" + 0.004*"strong" + 0.004*"16" + 0.004*"practice"', '0.017*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"effective" + 0.007*"Hounslow" + 0.005*"plans" + 0.005*"timely" + 0.005*"education" + 0.004*"protection" + 0.004*"training"', '0.022*"’" + 0.012*"needs" + 0.011*"well" + 0.008*"Hounslow" + 0.007*"effective" + 0.007*"timely" + 0.005*"progress" + 0.005*"experiences" + 0.005*"oversight" + 0.005*"16"']</t>
+    <t>['0.025*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"Hounslow" + 0.008*"effective" + 0.006*"timely" + 0.006*"plans" + 0.005*"strong" + 0.005*"16" + 0.005*"progress"', '0.020*"’" + 0.012*"well" + 0.012*"needs" + 0.007*"timely" + 0.007*"effective" + 0.006*"Hounslow" + 0.005*"oversight" + 0.005*"plans" + 0.005*"experiences" + 0.004*"education"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"Hounslow" + 0.005*"plans" + 0.005*"timely" + 0.004*"20" + 0.004*"oversight" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2551,7 +2551,7 @@
     <t>0.209</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"well" + 0.011*"needs" + 0.007*"highly" + 0.007*"plans" + 0.006*"good" + 0.006*"quality" + 0.006*"practice" + 0.005*"effective" + 0.005*"leaders"', '0.010*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"plans" + 0.006*"good" + 0.006*"highly" + 0.005*"effective" + 0.005*"leaders" + 0.005*"risk" + 0.005*"Islington"', '0.013*"’" + 0.012*"needs" + 0.009*"well" + 0.006*"plans" + 0.005*"quality" + 0.005*"leaders" + 0.005*"Islington" + 0.005*"effective" + 0.004*"good" + 0.004*"practice"']</t>
+    <t>['0.011*"’" + 0.010*"well" + 0.006*"plans" + 0.005*"highly" + 0.005*"needs" + 0.005*"good" + 0.005*"quality" + 0.005*"risk" + 0.004*"effective" + 0.004*"practice"', '0.015*"needs" + 0.014*"’" + 0.012*"well" + 0.007*"plans" + 0.007*"highly" + 0.007*"good" + 0.006*"quality" + 0.006*"leaders" + 0.006*"effective" + 0.006*"Islington"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"plans" + 0.005*"leaders" + 0.005*"effective" + 0.005*"Islington" + 0.004*"quality" + 0.004*"good" + 0.004*"highly"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2587,7 +2587,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"need" + 0.007*"good" + 0.006*"Lambeth" + 0.006*"impact" + 0.006*"progress" + 0.005*"leaders"', '0.014*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Lambeth" + 0.006*"progress" + 0.006*"good" + 0.005*"impact" + 0.005*"need" + 0.005*"4"', '0.015*"’" + 0.008*"needs" + 0.008*"plans" + 0.008*"well" + 0.007*"good" + 0.007*"Lambeth" + 0.005*"number" + 0.005*"progress" + 0.005*"leaders" + 0.005*"need"']</t>
+    <t>['0.009*"’" + 0.008*"well" + 0.008*"good" + 0.007*"plans" + 0.007*"needs" + 0.005*"Lambeth" + 0.005*"need" + 0.005*"impact" + 0.005*"leaders" + 0.004*"4"', '0.019*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"Lambeth" + 0.006*"progress" + 0.006*"impact" + 0.006*"need" + 0.005*"24" + 0.005*"good"', '0.016*"’" + 0.011*"needs" + 0.008*"plans" + 0.007*"good" + 0.007*"well" + 0.007*"Lambeth" + 0.006*"progress" + 0.006*"need" + 0.005*"4" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2623,7 +2623,7 @@
     <t>0.1803</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Lewisham" + 0.006*"effective" + 0.005*"4" + 0.005*"15" + 0.005*"leaders" + 0.005*"progress"', '0.017*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"effective" + 0.005*"arrangements" + 0.005*"Lewisham" + 0.005*"2023" + 0.005*"good" + 0.005*"appropriate"', '0.020*"’" + 0.010*"well" + 0.007*"plans" + 0.007*"effective" + 0.006*"Lewisham" + 0.006*"progress" + 0.005*"good" + 0.005*"needs" + 0.004*"4" + 0.004*"December"']</t>
+    <t>['0.018*"’" + 0.007*"well" + 0.007*"plans" + 0.006*"effective" + 0.006*"needs" + 0.005*"good" + 0.005*"4" + 0.005*"arrangements" + 0.005*"leaders" + 0.005*"progress"', '0.015*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"effective" + 0.007*"plans" + 0.005*"supported" + 0.005*"benefit" + 0.005*"Lewisham" + 0.004*"leaders" + 0.004*"progress"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"Lewisham" + 0.006*"plans" + 0.006*"progress" + 0.005*"15" + 0.005*"effective" + 0.005*"4" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2647,7 +2647,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"leaders" + 0.005*"plans" + 0.004*"28" + 0.004*"progress" + 0.004*"family" + 0.004*"information" + 0.004*"good"', '0.018*"’" + 0.009*"well" + 0.008*"Merton" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"early" + 0.005*"family" + 0.005*"2022" + 0.004*"risk"', '0.011*"’" + 0.006*"Merton" + 0.006*"well" + 0.005*"needs" + 0.004*"information" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"family" + 0.004*"risk" + 0.004*"good"']</t>
+    <t>['0.016*"’" + 0.010*"well" + 0.006*"Merton" + 0.006*"needs" + 0.005*"family" + 0.005*"plans" + 0.005*"helping" + 0.005*"progress" + 0.004*"ensure" + 0.004*"education"', '0.016*"’" + 0.007*"Merton" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"4" + 0.004*"risk" + 0.004*"access" + 0.004*"family" + 0.004*"progress"', '0.013*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"needs" + 0.004*"progress" + 0.004*"across" + 0.004*"2022" + 0.004*"ensure" + 0.004*"practice" + 0.004*"early"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2671,7 +2671,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"need" + 0.007*"Newham" + 0.007*"needs" + 0.007*"plans" + 0.007*"progress" + 0.006*"practice" + 0.005*"effective" + 0.005*"good" + 0.004*"well"', '0.023*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"need" + 0.006*"plans" + 0.005*"progress" + 0.004*"Leaders" + 0.004*"effective" + 0.004*"good"', '0.017*"’" + 0.009*"needs" + 0.007*"effective" + 0.007*"progress" + 0.006*"practice" + 0.006*"Newham" + 0.006*"plans" + 0.005*"good" + 0.005*"18" + 0.005*"risks"']</t>
+    <t>['0.015*"’" + 0.007*"plans" + 0.006*"progress" + 0.006*"needs" + 0.006*"need" + 0.006*"Newham" + 0.006*"practice" + 0.005*"effective" + 0.005*"good" + 0.005*"Leaders"', '0.020*"’" + 0.010*"needs" + 0.007*"Newham" + 0.007*"practice" + 0.006*"progress" + 0.006*"effective" + 0.006*"plans" + 0.006*"need" + 0.005*"good" + 0.004*"well"', '0.021*"’" + 0.008*"Newham" + 0.007*"needs" + 0.006*"effective" + 0.005*"practice" + 0.005*"progress" + 0.005*"plans" + 0.005*"need" + 0.004*"good" + 0.004*"risks"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2701,7 +2701,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"practice" + 0.006*"needs" + 0.005*"need" + 0.005*"well" + 0.005*"strong" + 0.005*"Redbridge" + 0.005*"risk" + 0.005*"progress" + 0.004*"ensure"', '0.007*"well" + 0.007*"’" + 0.006*"practice" + 0.005*"need" + 0.005*"including" + 0.005*"effective" + 0.004*"good" + 0.004*"strong" + 0.004*"risk" + 0.004*"Redbridge"', '0.008*"practice" + 0.007*"needs" + 0.006*"well" + 0.006*"need" + 0.006*"effective" + 0.006*"Redbridge" + 0.005*"strong" + 0.005*"’" + 0.005*"risk" + 0.005*"team"']</t>
+    <t>['0.008*"practice" + 0.008*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"Redbridge" + 0.005*"strong" + 0.005*"risk" + 0.004*"effective" + 0.004*"need" + 0.004*"progress"', '0.007*"’" + 0.006*"need" + 0.006*"well" + 0.006*"effective" + 0.006*"strong" + 0.006*"needs" + 0.006*"practice" + 0.005*"Redbridge" + 0.005*"risk" + 0.005*"progress"', '0.008*"’" + 0.007*"practice" + 0.006*"well" + 0.006*"need" + 0.005*"including" + 0.005*"needs" + 0.005*"ensure" + 0.005*"Redbridge" + 0.004*"highly" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2728,7 +2728,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.013*"well" + 0.010*"Richmond" + 0.008*"needs" + 0.007*"good" + 0.007*"need" + 0.006*"supported" + 0.006*"team" + 0.006*"strong" + 0.005*"additional"', '0.015*"’" + 0.010*"well" + 0.007*"needs" + 0.006*"Richmond" + 0.005*"supported" + 0.005*"31" + 0.005*"team" + 0.004*"need" + 0.004*"good" + 0.004*"ensure"', '0.010*"’" + 0.008*"well" + 0.006*"Richmond" + 0.006*"needs" + 0.005*"team" + 0.005*"supported" + 0.004*"need" + 0.004*"good" + 0.004*"4" + 0.004*"2022"']</t>
+    <t>['0.012*"’" + 0.010*"well" + 0.010*"Richmond" + 0.007*"needs" + 0.006*"need" + 0.005*"team" + 0.005*"ensure" + 0.005*"Thames" + 0.004*"supported" + 0.004*"good"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"supported" + 0.006*"Richmond" + 0.006*"team" + 0.005*"need" + 0.005*"4" + 0.005*"additional" + 0.005*"31"', '0.016*"’" + 0.013*"well" + 0.008*"Richmond" + 0.007*"good" + 0.006*"needs" + 0.006*"supported" + 0.005*"team" + 0.005*"strong" + 0.005*"need" + 0.005*"4"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2758,7 +2758,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"Southwark" + 0.008*"good" + 0.007*"needs" + 0.007*"well" + 0.007*"progress" + 0.005*"leaders" + 0.005*"improve" + 0.005*"Leaders" + 0.005*"need"', '0.014*"’" + 0.010*"Southwark" + 0.007*"good" + 0.007*"well" + 0.006*"needs" + 0.005*"receive" + 0.005*"plans" + 0.005*"progress" + 0.005*"Leaders" + 0.005*"ensure"', '0.020*"’" + 0.009*"good" + 0.009*"well" + 0.008*"Southwark" + 0.008*"needs" + 0.007*"need" + 0.007*"effective" + 0.006*"plans" + 0.006*"strong" + 0.005*"progress"']</t>
+    <t>['0.015*"’" + 0.008*"Southwark" + 0.007*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"needs" + 0.005*"need" + 0.004*"progress" + 0.004*"strong" + 0.004*"30"', '0.020*"’" + 0.009*"good" + 0.008*"Southwark" + 0.008*"needs" + 0.007*"well" + 0.006*"Leaders" + 0.006*"strong" + 0.006*"need" + 0.005*"receive" + 0.005*"leaders"', '0.018*"’" + 0.011*"Southwark" + 0.008*"good" + 0.008*"well" + 0.007*"needs" + 0.007*"progress" + 0.007*"plans" + 0.006*"effective" + 0.005*"need" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2788,7 +2788,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sutton" + 0.005*"progress" + 0.005*"good" + 0.005*"receive" + 0.005*"effective" + 0.005*"supported" + 0.005*"leaders"', '0.013*"’" + 0.007*"well" + 0.006*"Sutton" + 0.005*"needs" + 0.005*"effective" + 0.004*"receive" + 0.004*"good" + 0.004*"progress" + 0.004*"10" + 0.004*"positive"', '0.018*"’" + 0.006*"well" + 0.006*"progress" + 0.006*"needs" + 0.005*"good" + 0.005*"receive" + 0.005*"6" + 0.005*"Sutton" + 0.004*"2021" + 0.004*"effective"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"Sutton" + 0.004*"supported" + 0.004*"10" + 0.004*"protection" + 0.004*"progress" + 0.004*"6"', '0.021*"’" + 0.008*"well" + 0.006*"Sutton" + 0.006*"effective" + 0.005*"progress" + 0.005*"needs" + 0.005*"6" + 0.005*"receive" + 0.005*"leaders" + 0.005*"good"', '0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sutton" + 0.006*"progress" + 0.005*"receive" + 0.005*"effective" + 0.005*"good" + 0.004*"10" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2818,7 +2818,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"good" + 0.006*"practice" + 0.006*"‘" + 0.005*"needs" + 0.005*"need" + 0.005*"well" + 0.005*"risk"', '0.017*"’" + 0.008*"good" + 0.007*"effective" + 0.006*"‘" + 0.006*"well" + 0.006*"progress" + 0.006*"plans" + 0.005*"need" + 0.005*"practice" + 0.005*"carers"', '0.011*"’" + 0.006*"good" + 0.005*"well" + 0.005*"plans" + 0.005*"early" + 0.005*"effective" + 0.004*"risk" + 0.004*"practice" + 0.004*"need" + 0.004*"‘"']</t>
+    <t>['0.018*"’" + 0.007*"plans" + 0.007*"good" + 0.007*"effective" + 0.007*"well" + 0.006*"need" + 0.006*"‘" + 0.005*"practice" + 0.005*"needs" + 0.005*"early"', '0.012*"’" + 0.006*"practice" + 0.006*"good" + 0.005*"plans" + 0.005*"‘" + 0.005*"need" + 0.005*"well" + 0.005*"early" + 0.005*"effective" + 0.004*"including"', '0.012*"’" + 0.007*"good" + 0.006*"effective" + 0.006*"‘" + 0.005*"needs" + 0.005*"plans" + 0.005*"progress" + 0.004*"practice" + 0.004*"early" + 0.004*"well"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2851,7 +2851,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.014*"well" + 0.010*"good" + 0.010*"needs" + 0.007*"effective" + 0.007*"need" + 0.005*"plans" + 0.005*"risk" + 0.005*"timely" + 0.004*"education"', '0.011*"’" + 0.009*"well" + 0.009*"needs" + 0.006*"good" + 0.006*"effective" + 0.005*"need" + 0.005*"plans" + 0.005*"timely" + 0.004*"protection" + 0.004*"risk"', '0.018*"’" + 0.011*"well" + 0.008*"effective" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"need" + 0.004*"timely" + 0.004*"ensure" + 0.004*"risk"']</t>
+    <t>['0.013*"well" + 0.011*"’" + 0.008*"needs" + 0.008*"good" + 0.006*"plans" + 0.006*"effective" + 0.006*"need" + 0.004*"appropriately" + 0.004*"progress" + 0.004*"planning"', '0.019*"’" + 0.012*"well" + 0.010*"needs" + 0.008*"good" + 0.008*"effective" + 0.006*"need" + 0.006*"risk" + 0.005*"plans" + 0.005*"timely" + 0.004*"protection"', '0.012*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"good" + 0.007*"effective" + 0.006*"need" + 0.005*"timely" + 0.005*"plans" + 0.004*"clear" + 0.004*"information"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2878,7 +2878,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"well" + 0.006*"ensure" + 0.006*"Senior" + 0.006*"effective" + 0.006*"practice" + 0.005*"progress" + 0.005*"team" + 0.005*"needs" + 0.005*"7"', '0.012*"’" + 0.005*"Senior" + 0.005*"receive" + 0.005*"practice" + 0.005*"supported" + 0.005*"progress" + 0.004*"7" + 0.004*"well" + 0.004*"effective" + 0.004*"Wandsworth"', '0.010*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"protection" + 0.006*"Wandsworth" + 0.006*"progress" + 0.005*"quality" + 0.005*"N" + 0.004*"7" + 0.004*"appropriate"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"7" + 0.006*"protection" + 0.005*"Senior" + 0.005*"ensure" + 0.005*"progress" + 0.005*"good" + 0.004*"Wandsworth"', '0.014*"’" + 0.007*"well" + 0.006*"practice" + 0.006*"progress" + 0.006*"Wandsworth" + 0.005*"needs" + 0.005*"team" + 0.005*"supported" + 0.005*"Senior" + 0.005*"effective"', '0.011*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"effective" + 0.005*"Senior" + 0.005*"quality" + 0.005*"ensure" + 0.005*"needs" + 0.005*"protection" + 0.005*"Wandsworth"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2911,7 +2911,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"highly" + 0.005*"needs" + 0.005*"practice" + 0.004*"across" + 0.004*"well" + 0.003*"quality" + 0.003*"high" + 0.003*"skilled" + 0.003*"Westminster"', '0.012*"’" + 0.006*"highly" + 0.005*"needs" + 0.005*"well" + 0.005*"practice" + 0.004*"many" + 0.004*"across" + 0.003*"skilled" + 0.003*"shared" + 0.003*"high"', '0.013*"’" + 0.009*"practice" + 0.007*"needs" + 0.006*"well" + 0.005*"highly" + 0.004*"many" + 0.004*"family" + 0.004*"across" + 0.004*"shared" + 0.003*"direct"']</t>
+    <t>['0.012*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"highly" + 0.005*"well" + 0.003*"high" + 0.003*"direct" + 0.003*"plans" + 0.003*"many" + 0.003*"supported"', '0.011*"’" + 0.007*"practice" + 0.006*"highly" + 0.006*"needs" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.004*"family" + 0.003*"shared" + 0.003*"high"', '0.015*"’" + 0.006*"practice" + 0.005*"highly" + 0.005*"needs" + 0.005*"well" + 0.004*"across" + 0.004*"family" + 0.004*"many" + 0.004*"skilled" + 0.003*"direct"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2944,7 +2944,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"need" + 0.006*"needs" + 0.005*"effective" + 0.005*"quality" + 0.005*"impact" + 0.005*"Luton" + 0.005*"good" + 0.004*"ensure" + 0.004*"plans"', '0.015*"’" + 0.006*"Luton" + 0.006*"effective" + 0.006*"plans" + 0.005*"good" + 0.005*"well" + 0.005*"progress" + 0.004*"needs" + 0.004*"need" + 0.004*"impact"', '0.019*"’" + 0.008*"need" + 0.008*"needs" + 0.007*"plans" + 0.006*"receive" + 0.006*"Luton" + 0.005*"progress" + 0.005*"impact" + 0.005*"ensure" + 0.005*"good"']</t>
+    <t>['0.019*"’" + 0.006*"plans" + 0.006*"needs" + 0.006*"need" + 0.005*"good" + 0.005*"Luton" + 0.005*"leaders" + 0.005*"effective" + 0.004*"impact" + 0.004*"ensure"', '0.017*"’" + 0.007*"need" + 0.007*"needs" + 0.006*"Luton" + 0.006*"good" + 0.005*"effective" + 0.005*"ensure" + 0.005*"progress" + 0.005*"plans" + 0.005*"impact"', '0.015*"’" + 0.006*"plans" + 0.006*"need" + 0.006*"effective" + 0.005*"Luton" + 0.005*"needs" + 0.005*"quality" + 0.005*"impact" + 0.005*"progress" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2971,7 +2971,7 @@
     <t>19/05/22</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.010*"needs" + 0.008*"Manchester" + 0.007*"supported" + 0.007*"well" + 0.006*"education" + 0.005*"plans" + 0.005*"always" + 0.005*"disabled" + 0.005*"21"', '0.020*"’" + 0.012*"Manchester" + 0.009*"needs" + 0.008*"always" + 0.006*"well" + 0.006*"supported" + 0.006*"protection" + 0.006*"education" + 0.005*"plans" + 0.005*"21"', '0.017*"’" + 0.011*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.006*"always" + 0.006*"effective" + 0.006*"supported" + 0.005*"plans" + 0.005*"family" + 0.005*"quality"']</t>
+    <t>['0.025*"’" + 0.013*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.006*"supported" + 0.006*"always" + 0.006*"education" + 0.006*"effective" + 0.006*"plans" + 0.005*"quality"', '0.016*"’" + 0.010*"needs" + 0.008*"Manchester" + 0.008*"supported" + 0.007*"well" + 0.006*"always" + 0.005*"21" + 0.005*"family" + 0.005*"education" + 0.005*"plans"', '0.020*"’" + 0.009*"needs" + 0.009*"Manchester" + 0.007*"always" + 0.006*"well" + 0.006*"protection" + 0.006*"effective" + 0.006*"plans" + 0.005*"supported" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -3001,7 +3001,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"practice" + 0.008*"Medway" + 0.007*"quality" + 0.007*"well" + 0.007*"needs" + 0.006*"leaders" + 0.006*"oversight" + 0.006*"impact" + 0.005*"good"', '0.018*"’" + 0.010*"Medway" + 0.008*"quality" + 0.008*"well" + 0.008*"practice" + 0.007*"oversight" + 0.007*"leaders" + 0.006*"needs" + 0.006*"impact" + 0.005*"experiences"', '0.012*"’" + 0.009*"Medway" + 0.008*"practice" + 0.008*"well" + 0.007*"quality" + 0.006*"leaders" + 0.005*"needs" + 0.005*"good" + 0.005*"risk" + 0.005*"impact"']</t>
+    <t>['0.020*"’" + 0.009*"Medway" + 0.009*"well" + 0.008*"practice" + 0.008*"quality" + 0.007*"leaders" + 0.006*"oversight" + 0.006*"needs" + 0.005*"28" + 0.005*"experiences"', '0.013*"’" + 0.010*"Medway" + 0.009*"practice" + 0.008*"quality" + 0.008*"well" + 0.008*"needs" + 0.006*"oversight" + 0.006*"experiences" + 0.006*"impact" + 0.005*"17"', '0.012*"’" + 0.008*"Medway" + 0.006*"quality" + 0.006*"impact" + 0.005*"practice" + 0.005*"well" + 0.005*"leaders" + 0.005*"17" + 0.005*"needs" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -3025,7 +3025,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"effective" + 0.007*"needs" + 0.007*"Middlesbrough" + 0.006*"well" + 0.006*"24" + 0.006*"practice" + 0.005*"plans" + 0.004*"impact" + 0.004*"2023"', '0.016*"’" + 0.009*"plans" + 0.008*"effective" + 0.007*"Middlesbrough" + 0.007*"needs" + 0.006*"practice" + 0.006*"progress" + 0.006*"well" + 0.005*"good" + 0.005*"place"', '0.012*"’" + 0.006*"well" + 0.006*"plans" + 0.006*"Middlesbrough" + 0.005*"place" + 0.004*"effective" + 0.004*"progress" + 0.004*"means" + 0.004*"needs" + 0.004*"13"']</t>
+    <t>['0.014*"’" + 0.008*"effective" + 0.008*"plans" + 0.007*"Middlesbrough" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"place" + 0.005*"impact" + 0.005*"progress"', '0.013*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"effective" + 0.005*"needs" + 0.005*"Middlesbrough" + 0.005*"24" + 0.005*"progress" + 0.005*"practice" + 0.004*"place"', '0.014*"’" + 0.007*"well" + 0.007*"Middlesbrough" + 0.007*"needs" + 0.007*"effective" + 0.006*"plans" + 0.006*"practice" + 0.006*"progress" + 0.005*"13" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -3052,7 +3052,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"Keynes" + 0.006*"Milton" + 0.005*"well" + 0.005*"need" + 0.005*"leaders" + 0.005*"October" + 0.005*"good" + 0.004*"plans" + 0.004*"practice"', '0.016*"’" + 0.007*"well" + 0.006*"Milton" + 0.006*"Keynes" + 0.006*"practice" + 0.005*"need" + 0.005*"5" + 0.005*"effective" + 0.004*"quality" + 0.004*"October"', '0.014*"’" + 0.006*"Milton" + 0.005*"need" + 0.005*"25" + 0.005*"plans" + 0.005*"Keynes" + 0.005*"needs" + 0.005*"good" + 0.004*"well" + 0.004*"education"']</t>
+    <t>['0.015*"’" + 0.006*"need" + 0.006*"Milton" + 0.005*"well" + 0.005*"leaders" + 0.005*"practice" + 0.005*"plans" + 0.005*"also" + 0.004*"education" + 0.004*"good"', '0.016*"’" + 0.007*"Keynes" + 0.005*"well" + 0.005*"practice" + 0.005*"need" + 0.005*"25" + 0.005*"Milton" + 0.005*"plans" + 0.004*"2021" + 0.004*"5"', '0.014*"’" + 0.007*"Milton" + 0.007*"Keynes" + 0.006*"well" + 0.005*"leaders" + 0.005*"good" + 0.005*"need" + 0.005*"5" + 0.005*"impact" + 0.004*"25"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -3079,7 +3079,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.011*"plans" + 0.007*"Newcastle" + 0.007*"needs" + 0.007*"protection" + 0.006*"good" + 0.006*"management" + 0.006*"well" + 0.006*"ensure" + 0.005*"making"', '0.013*"’" + 0.009*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"protection" + 0.006*"Newcastle" + 0.005*"response" + 0.005*"29" + 0.005*"making"', '0.020*"’" + 0.011*"plans" + 0.008*"needs" + 0.008*"Newcastle" + 0.007*"good" + 0.007*"progress" + 0.007*"protection" + 0.006*"well" + 0.006*"ensure" + 0.006*"need"']</t>
+    <t>['0.015*"’" + 0.010*"plans" + 0.008*"needs" + 0.008*"well" + 0.007*"Newcastle" + 0.007*"good" + 0.006*"protection" + 0.006*"making" + 0.006*"response" + 0.006*"progress"', '0.012*"’" + 0.010*"plans" + 0.008*"Newcastle" + 0.007*"protection" + 0.007*"good" + 0.006*"needs" + 0.005*"progress" + 0.005*"need" + 0.005*"ensure" + 0.005*"10"', '0.019*"’" + 0.011*"plans" + 0.008*"needs" + 0.007*"protection" + 0.006*"good" + 0.006*"Newcastle" + 0.006*"ensure" + 0.006*"well" + 0.006*"management" + 0.005*"making"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -3103,7 +3103,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"Norfolk" + 0.005*"practice" + 0.005*"carers" + 0.005*"needs" + 0.005*"supported" + 0.004*"18" + 0.004*"including" + 0.004*"leaders"', '0.014*"’" + 0.008*"Norfolk" + 0.007*"well" + 0.006*"carers" + 0.005*"practice" + 0.005*"supported" + 0.005*"needs" + 0.005*"including" + 0.005*"plans" + 0.005*"leaders"', '0.020*"’" + 0.009*"Norfolk" + 0.009*"well" + 0.007*"needs" + 0.007*"carers" + 0.006*"practice" + 0.006*"supported" + 0.004*"information" + 0.004*"effective" + 0.004*"plans"']</t>
+    <t>['0.011*"’" + 0.006*"Norfolk" + 0.006*"well" + 0.005*"supported" + 0.005*"leaders" + 0.004*"carers" + 0.004*"needs" + 0.004*"range" + 0.004*"practice" + 0.003*"information"', '0.016*"’" + 0.008*"Norfolk" + 0.007*"carers" + 0.007*"well" + 0.006*"needs" + 0.005*"leaders" + 0.004*"7" + 0.004*"18" + 0.004*"range" + 0.004*"family"', '0.020*"’" + 0.010*"well" + 0.008*"Norfolk" + 0.008*"practice" + 0.006*"needs" + 0.006*"supported" + 0.006*"plans" + 0.006*"carers" + 0.005*"effective" + 0.005*"including"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -3136,7 +3136,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.006*"risk" + 0.005*"practice" + 0.005*"many" + 0.005*"planning" + 0.004*"leaders" + 0.004*"need" + 0.004*"needs" + 0.004*"North" + 0.004*"harm"', '0.011*"’" + 0.006*"risk" + 0.006*"practice" + 0.006*"leaders" + 0.005*"needs" + 0.005*"planning" + 0.005*"plans" + 0.005*"Lincolnshire" + 0.005*"quality" + 0.004*"many"', '0.018*"’" + 0.009*"practice" + 0.007*"leaders" + 0.007*"planning" + 0.007*"needs" + 0.007*"risk" + 0.006*"need" + 0.005*"East" + 0.005*"oversight" + 0.005*"Lincolnshire"']</t>
+    <t>['0.014*"’" + 0.009*"practice" + 0.006*"risk" + 0.006*"leaders" + 0.006*"needs" + 0.006*"planning" + 0.005*"need" + 0.005*"East" + 0.004*"October" + 0.004*"quality"', '0.014*"’" + 0.007*"practice" + 0.007*"risk" + 0.006*"planning" + 0.005*"needs" + 0.005*"leaders" + 0.005*"Lincolnshire" + 0.005*"experiences" + 0.005*"2021" + 0.005*"North"', '0.014*"’" + 0.007*"practice" + 0.007*"leaders" + 0.007*"risk" + 0.006*"needs" + 0.006*"many" + 0.006*"planning" + 0.005*"need" + 0.005*"October" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -3166,7 +3166,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"‘" + 0.006*"family" + 0.005*"need" + 0.005*"well" + 0.005*"approach" + 0.005*"Lincolnshire" + 0.005*"10" + 0.005*"council" + 0.005*"team"', '0.020*"’" + 0.007*"‘" + 0.006*"family" + 0.006*"Lincolnshire" + 0.006*"leaders" + 0.006*"North" + 0.005*"well" + 0.005*"approach" + 0.005*"need" + 0.004*"10"', '0.022*"’" + 0.007*"‘" + 0.006*"North" + 0.005*"approach" + 0.005*"family" + 0.005*"10" + 0.005*"Lincolnshire" + 0.004*"14" + 0.004*"well" + 0.004*"protection"']</t>
+    <t>['0.028*"’" + 0.007*"‘" + 0.007*"family" + 0.007*"North" + 0.005*"10" + 0.005*"approach" + 0.005*"well" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"team"', '0.014*"’" + 0.007*"‘" + 0.006*"Lincolnshire" + 0.006*"family" + 0.005*"leaders" + 0.005*"approach" + 0.005*"protection" + 0.005*"well" + 0.004*"2022" + 0.004*"team"', '0.013*"’" + 0.007*"‘" + 0.006*"leaders" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"North" + 0.005*"well" + 0.004*"10" + 0.004*"family" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>2637539</t>
@@ -3202,7 +3202,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"Northamptonshire" + 0.006*"well" + 0.005*"North" + 0.004*"quality" + 0.004*"needs" + 0.004*"Leaders" + 0.004*"14" + 0.004*"2022" + 0.004*"need"', '0.017*"’" + 0.007*"Northamptonshire" + 0.007*"North" + 0.007*"well" + 0.006*"quality" + 0.006*"plans" + 0.005*"practice" + 0.005*"impact" + 0.005*"NCT" + 0.005*"3"', '0.019*"’" + 0.009*"Northamptonshire" + 0.007*"North" + 0.005*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"Leaders" + 0.005*"NCT" + 0.005*"experiences" + 0.005*"e"']</t>
+    <t>['0.019*"’" + 0.009*"Northamptonshire" + 0.006*"well" + 0.006*"North" + 0.006*"needs" + 0.005*"quality" + 0.005*"Leaders" + 0.005*"3" + 0.005*"practice" + 0.005*"2022"', '0.015*"’" + 0.006*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.006*"quality" + 0.005*"NCT" + 0.005*"impact" + 0.005*"practice" + 0.004*"e" + 0.004*"14"', '0.015*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.005*"quality" + 0.005*"impact" + 0.005*"need" + 0.005*"plans" + 0.005*"practice" + 0.005*"Leaders"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -3229,7 +3229,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"always" + 0.006*"Somerset" + 0.006*"needs" + 0.006*"quality" + 0.006*"number" + 0.006*"practice" + 0.005*"progress" + 0.005*"need" + 0.005*"North"', '0.010*"’" + 0.007*"needs" + 0.007*"quality" + 0.005*"North" + 0.005*"always" + 0.005*"need" + 0.004*"experienced" + 0.004*"number" + 0.004*"plans" + 0.004*"progress"', '0.021*"’" + 0.009*"quality" + 0.007*"needs" + 0.006*"North" + 0.006*"Somerset" + 0.006*"practice" + 0.006*"always" + 0.006*"risk" + 0.006*"number" + 0.005*"well"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.007*"quality" + 0.006*"North" + 0.006*"practice" + 0.006*"need" + 0.006*"always" + 0.006*"number" + 0.005*"Somerset" + 0.005*"well"', '0.016*"’" + 0.007*"quality" + 0.006*"progress" + 0.006*"needs" + 0.006*"always" + 0.005*"North" + 0.005*"number" + 0.005*"Somerset" + 0.005*"practice" + 0.005*"effective"', '0.017*"’" + 0.008*"quality" + 0.006*"Somerset" + 0.006*"always" + 0.005*"needs" + 0.005*"North" + 0.005*"risk" + 0.005*"practice" + 0.005*"number" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -3256,7 +3256,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.006*"leaders" + 0.005*"needs" + 0.005*"make" + 0.005*"need" + 0.004*"quality" + 0.004*"impact" + 0.004*"early" + 0.004*"way"', '0.016*"’" + 0.005*"quality" + 0.005*"leaders" + 0.005*"well" + 0.004*"make" + 0.004*"impact" + 0.004*"need" + 0.004*"good" + 0.004*"protection" + 0.004*"progress"', '0.014*"’" + 0.007*"well" + 0.006*"need" + 0.005*"leaders" + 0.004*"progress" + 0.004*"make" + 0.004*"quality" + 0.004*"early" + 0.004*"foster" + 0.004*"needs"']</t>
+    <t>['0.019*"’" + 0.006*"well" + 0.005*"leaders" + 0.005*"needs" + 0.005*"quality" + 0.004*"need" + 0.004*"make" + 0.004*"impact" + 0.003*"clear" + 0.003*"early"', '0.014*"’" + 0.007*"well" + 0.006*"need" + 0.005*"quality" + 0.005*"leaders" + 0.005*"needs" + 0.004*"make" + 0.004*"early" + 0.004*"foster" + 0.004*"family"', '0.015*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"make" + 0.005*"impact" + 0.004*"need" + 0.004*"understand" + 0.004*"early" + 0.004*"protection" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80530</t>
@@ -3286,7 +3286,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"practice" + 0.005*"Yorkshire" + 0.005*"North" + 0.005*"family" + 0.004*"3" + 0.004*"‘" + 0.004*"carers"', '0.022*"’" + 0.008*"North" + 0.007*"well" + 0.007*"needs" + 0.007*"Yorkshire" + 0.006*"practice" + 0.006*"family" + 0.005*"2023" + 0.005*"7" + 0.005*"‘"', '0.024*"’" + 0.009*"well" + 0.006*"practice" + 0.006*"family" + 0.006*"Yorkshire" + 0.005*"North" + 0.005*"‘" + 0.005*"need" + 0.004*"needs" + 0.004*"make"']</t>
+    <t>['0.020*"’" + 0.006*"practice" + 0.006*"well" + 0.006*"North" + 0.006*"needs" + 0.005*"family" + 0.005*"‘" + 0.004*"Yorkshire" + 0.004*"7" + 0.004*"ensure"', '0.019*"’" + 0.008*"Yorkshire" + 0.008*"well" + 0.007*"North" + 0.006*"practice" + 0.006*"family" + 0.005*"needs" + 0.005*"2023" + 0.005*"‘" + 0.004*"3"', '0.022*"’" + 0.010*"well" + 0.006*"North" + 0.006*"practice" + 0.006*"Yorkshire" + 0.005*"family" + 0.005*"needs" + 0.005*"3" + 0.004*"‘" + 0.004*"July"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -3313,7 +3313,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.012*"needs" + 0.011*"well" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.005*"impact" + 0.005*"experiences" + 0.005*"quality" + 0.004*"education"', '0.014*"’" + 0.006*"needs" + 0.006*"good" + 0.005*"quality" + 0.005*"need" + 0.005*"well" + 0.004*"impact" + 0.004*"education" + 0.004*"experiences" + 0.004*"progress"', '0.026*"’" + 0.010*"needs" + 0.010*"well" + 0.007*"good" + 0.007*"experiences" + 0.006*"need" + 0.005*"practice" + 0.005*"education" + 0.005*"impact" + 0.005*"leaders"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"good" + 0.005*"practice" + 0.004*"need" + 0.004*"impact" + 0.004*"experiences" + 0.004*"always" + 0.004*"education"', '0.025*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"good" + 0.007*"need" + 0.006*"experiences" + 0.005*"quality" + 0.005*"impact" + 0.005*"leaders" + 0.004*"education"', '0.024*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.006*"impact" + 0.005*"education" + 0.005*"experiences" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3343,7 +3343,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.006*"Nottingham" + 0.005*"oversight" + 0.005*"impact" + 0.005*"effective" + 0.005*"practice" + 0.005*"City" + 0.005*"July" + 0.005*"2022"', '0.013*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"Nottingham" + 0.005*"protection" + 0.005*"City" + 0.004*"impact" + 0.004*"11" + 0.004*"2022" + 0.004*"consistently"', '0.012*"’" + 0.008*"needs" + 0.007*"effective" + 0.006*"Nottingham" + 0.006*"plans" + 0.005*"11" + 0.005*"risk" + 0.005*"oversight" + 0.005*"consistently" + 0.004*"However"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"impact" + 0.005*"effective" + 0.005*"risk" + 0.005*"oversight" + 0.005*"2022" + 0.005*"protection" + 0.005*"However"', '0.016*"’" + 0.009*"needs" + 0.008*"Nottingham" + 0.005*"effective" + 0.005*"11" + 0.005*"oversight" + 0.005*"City" + 0.004*"significant" + 0.004*"practice" + 0.004*"impact"', '0.012*"’" + 0.007*"needs" + 0.005*"effective" + 0.005*"City" + 0.005*"However" + 0.005*"plans" + 0.005*"Nottingham" + 0.004*"impact" + 0.004*"information" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80534</t>
@@ -3367,7 +3367,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"well" + 0.008*"practice" + 0.005*"e" + 0.005*"needs" + 0.005*"areas" + 0.005*"quality" + 0.005*"ensure" + 0.005*"made" + 0.005*"plans"', '0.009*"’" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"receive" + 0.005*"ensure" + 0.005*"carers" + 0.005*"progress" + 0.004*"meetings"', '0.014*"’" + 0.008*"well" + 0.008*"practice" + 0.006*"receive" + 0.006*"needs" + 0.005*"made" + 0.005*"ensure" + 0.005*"progress" + 0.005*"quality" + 0.005*"placements"']</t>
+    <t>['0.013*"’" + 0.010*"well" + 0.008*"practice" + 0.006*"receive" + 0.006*"needs" + 0.005*"ensure" + 0.005*"progress" + 0.005*"placements" + 0.005*"quality" + 0.005*"number"', '0.012*"’" + 0.009*"practice" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"ensure" + 0.005*"made" + 0.004*"carers" + 0.004*"receive"', '0.012*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"e" + 0.005*"quality" + 0.005*"receive" + 0.005*"areas" + 0.005*"needs" + 0.005*"plans" + 0.005*"made"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3400,7 +3400,7 @@
     <t>04/03/19</t>
   </si>
   <si>
-    <t>['0.010*"good" + 0.009*"effective" + 0.008*"’" + 0.008*"practice" + 0.007*"well" + 0.007*"needs" + 0.006*"planning" + 0.005*"quality" + 0.005*"risk" + 0.005*"plans"', '0.013*"’" + 0.010*"good" + 0.010*"needs" + 0.009*"practice" + 0.007*"effective" + 0.007*"progress" + 0.007*"plans" + 0.006*"planning" + 0.006*"quality" + 0.005*"well"', '0.010*"’" + 0.010*"needs" + 0.009*"practice" + 0.007*"quality" + 0.007*"good" + 0.007*"effective" + 0.007*"progress" + 0.006*"well" + 0.005*"planning" + 0.005*"plans"']</t>
+    <t>['0.012*"’" + 0.012*"needs" + 0.010*"good" + 0.009*"practice" + 0.007*"well" + 0.007*"planning" + 0.006*"effective" + 0.006*"quality" + 0.006*"risk" + 0.006*"progress"', '0.009*"’" + 0.009*"good" + 0.009*"effective" + 0.008*"practice" + 0.007*"progress" + 0.007*"needs" + 0.007*"plans" + 0.006*"quality" + 0.005*"well" + 0.005*"information"', '0.010*"’" + 0.008*"effective" + 0.008*"practice" + 0.008*"good" + 0.007*"quality" + 0.007*"needs" + 0.006*"progress" + 0.006*"planning" + 0.006*"well" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3430,7 +3430,7 @@
     <t>0.1755</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.011*"needs" + 0.007*"Oxfordshire" + 0.006*"good" + 0.006*"supported" + 0.005*"progress" + 0.005*"well" + 0.005*"12" + 0.005*"quality" + 0.005*"receive"', '0.016*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"risk" + 0.006*"Oxfordshire" + 0.005*"practice" + 0.005*"supported" + 0.005*"good" + 0.004*"education" + 0.004*"arrangements"', '0.016*"’" + 0.011*"needs" + 0.007*"Oxfordshire" + 0.006*"risk" + 0.006*"well" + 0.005*"quality" + 0.005*"receive" + 0.005*"supported" + 0.005*"good" + 0.004*"arrangements"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.007*"well" + 0.007*"Oxfordshire" + 0.005*"receive" + 0.005*"risk" + 0.005*"quality" + 0.005*"supported" + 0.005*"good" + 0.005*"education"', '0.020*"’" + 0.011*"needs" + 0.007*"Oxfordshire" + 0.007*"well" + 0.006*"risk" + 0.006*"leaders" + 0.005*"good" + 0.005*"12" + 0.005*"education" + 0.005*"supported"', '0.023*"’" + 0.008*"needs" + 0.007*"Oxfordshire" + 0.006*"supported" + 0.006*"good" + 0.006*"well" + 0.005*"risk" + 0.005*"arrangements" + 0.005*"practice" + 0.005*"12"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3460,7 +3460,7 @@
     <t>30/01/24</t>
   </si>
   <si>
-    <t>['0.016*"needs" + 0.012*"’" + 0.007*"Peterborough" + 0.007*"need" + 0.006*"well" + 0.005*"good" + 0.005*"progress" + 0.005*"plans" + 0.005*"2023" + 0.005*"receive"', '0.013*"’" + 0.011*"needs" + 0.006*"2023" + 0.006*"well" + 0.006*"Peterborough" + 0.006*"education" + 0.006*"need" + 0.005*"supported" + 0.005*"progress" + 0.004*"27"', '0.017*"’" + 0.013*"needs" + 0.008*"need" + 0.007*"Peterborough" + 0.007*"2023" + 0.007*"progress" + 0.006*"8" + 0.006*"well" + 0.006*"supported" + 0.006*"plans"']</t>
+    <t>['0.015*"’" + 0.013*"needs" + 0.007*"Peterborough" + 0.007*"need" + 0.007*"2023" + 0.007*"progress" + 0.006*"well" + 0.006*"supported" + 0.005*"plans" + 0.005*"27"', '0.016*"’" + 0.014*"needs" + 0.007*"need" + 0.007*"Peterborough" + 0.006*"well" + 0.006*"progress" + 0.006*"2023" + 0.006*"8" + 0.005*"good" + 0.005*"supported"', '0.012*"needs" + 0.011*"’" + 0.006*"need" + 0.006*"Peterborough" + 0.006*"2023" + 0.005*"plans" + 0.005*"well" + 0.005*"8" + 0.005*"receive" + 0.004*"27"']</t>
   </si>
   <si>
     <t>80538</t>
@@ -3490,7 +3490,7 @@
     <t>15/03/24</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.006*"needs" + 0.005*"Plymouth" + 0.004*"well" + 0.004*"practice" + 0.004*"2024" + 0.004*"good" + 0.003*"plans" + 0.003*"Council" + 0.003*"2"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"Plymouth" + 0.005*"February" + 0.005*"plans" + 0.005*"timely" + 0.005*"22" + 0.005*"2024" + 0.004*"January"', '0.015*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Plymouth" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"2" + 0.005*"education" + 0.005*"City" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.009*"well" + 0.008*"Plymouth" + 0.007*"needs" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"risks" + 0.005*"Council" + 0.005*"education" + 0.005*"plans"', '0.013*"’" + 0.009*"needs" + 0.005*"Plymouth" + 0.005*"well" + 0.005*"practice" + 0.004*"education" + 0.004*"plans" + 0.004*"2024" + 0.004*"22" + 0.004*"January"', '0.010*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"Plymouth" + 0.005*"2" + 0.005*"practice" + 0.005*"appropriate" + 0.004*"quality" + 0.004*"January" + 0.004*"arrangements"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3523,7 +3523,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"care-experienced" + 0.008*"well" + 0.008*"needs" + 0.006*"plans" + 0.005*"health" + 0.005*"family" + 0.005*"Portsmouth" + 0.005*"risk" + 0.004*"need"', '0.013*"’" + 0.007*"care-experienced" + 0.006*"well" + 0.005*"family" + 0.005*"Portsmouth" + 0.005*"practice" + 0.004*"needs" + 0.004*"need" + 0.004*"plans" + 0.004*"health"', '0.020*"’" + 0.009*"Portsmouth" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"well" + 0.006*"health" + 0.005*"family" + 0.005*"19" + 0.005*"leaders" + 0.005*"progress"']</t>
+    <t>['0.014*"’" + 0.009*"well" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"family" + 0.005*"leaders" + 0.005*"health" + 0.005*"plans" + 0.004*"19"', '0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Portsmouth" + 0.007*"care-experienced" + 0.006*"family" + 0.005*"health" + 0.005*"plans" + 0.004*"practice" + 0.004*"need"', '0.020*"’" + 0.009*"care-experienced" + 0.006*"Portsmouth" + 0.006*"needs" + 0.006*"plans" + 0.005*"health" + 0.005*"progress" + 0.005*"well" + 0.005*"need" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3559,7 +3559,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"quality" + 0.006*"number" + 0.006*"well" + 0.006*"good" + 0.005*"arrangements" + 0.005*"need" + 0.005*"practice" + 0.005*"plans" + 0.004*"timely"', '0.019*"’" + 0.007*"plans" + 0.007*"number" + 0.006*"well" + 0.006*"effective" + 0.006*"quality" + 0.005*"carers" + 0.005*"need" + 0.005*"good" + 0.005*"timely"', '0.011*"’" + 0.007*"number" + 0.007*"quality" + 0.006*"well" + 0.006*"good" + 0.006*"However" + 0.006*"plans" + 0.005*"need" + 0.005*"effective" + 0.004*"ensure"']</t>
+    <t>['0.013*"’" + 0.007*"well" + 0.007*"number" + 0.007*"need" + 0.006*"quality" + 0.006*"plans" + 0.006*"good" + 0.005*"practice" + 0.005*"carers" + 0.004*"always"', '0.016*"’" + 0.008*"number" + 0.007*"plans" + 0.006*"well" + 0.005*"effective" + 0.005*"quality" + 0.005*"practice" + 0.005*"need" + 0.005*"good" + 0.004*"always"', '0.018*"’" + 0.008*"quality" + 0.006*"number" + 0.006*"timely" + 0.006*"well" + 0.006*"good" + 0.006*"However" + 0.006*"effective" + 0.005*"plans" + 0.005*"needs"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3583,7 +3583,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"plans" + 0.005*"Redcar" + 0.005*"Cleveland" + 0.005*"leaders" + 0.005*"needs" + 0.005*"20" + 0.005*"consistently" + 0.005*"2022" + 0.004*"1"', '0.015*"’" + 0.006*"However" + 0.006*"needs" + 0.005*"plans" + 0.005*"leaders" + 0.005*"consistently" + 0.005*"July" + 0.004*"2022" + 0.004*"risk" + 0.004*"areas"', '0.022*"’" + 0.008*"leaders" + 0.006*"However" + 0.006*"practice" + 0.006*"consistently" + 0.006*"20" + 0.005*"needs" + 0.005*"risk" + 0.005*"2022" + 0.005*"plans"']</t>
+    <t>['0.014*"’" + 0.005*"needs" + 0.005*"However" + 0.005*"consistently" + 0.005*"Redcar" + 0.004*"2022" + 0.004*"risk" + 0.004*"carers" + 0.004*"plans" + 0.004*"Cleveland"', '0.023*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"needs" + 0.006*"20" + 0.006*"However" + 0.005*"practice" + 0.005*"consistently" + 0.004*"oversight" + 0.004*"timely"', '0.015*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"consistently" + 0.006*"risk" + 0.005*"However" + 0.005*"practice" + 0.005*"2022" + 0.005*"needs" + 0.005*"Cleveland"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3610,7 +3610,7 @@
     <t>17/03/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"experienced" + 0.009*"practice" + 0.007*"needs" + 0.006*"response" + 0.006*"plans" + 0.006*"good" + 0.006*"Rochdale" + 0.006*"quality" + 0.005*"consistently"', '0.024*"’" + 0.009*"experienced" + 0.008*"needs" + 0.007*"practice" + 0.006*"plans" + 0.006*"response" + 0.005*"consistently" + 0.005*"well" + 0.005*"quality" + 0.004*"Rochdale"', '0.015*"’" + 0.010*"experienced" + 0.008*"needs" + 0.008*"practice" + 0.005*"consistently" + 0.005*"plans" + 0.005*"good" + 0.005*"leaders" + 0.005*"quality" + 0.004*"response"']</t>
+    <t>['0.015*"’" + 0.009*"experienced" + 0.007*"practice" + 0.007*"needs" + 0.005*"good" + 0.005*"consistently" + 0.005*"response" + 0.005*"plans" + 0.005*"quality" + 0.004*"well"', '0.015*"’" + 0.007*"experienced" + 0.007*"needs" + 0.006*"practice" + 0.006*"consistently" + 0.005*"quality" + 0.005*"well" + 0.005*"3" + 0.004*"Rochdale" + 0.004*"response"', '0.025*"’" + 0.011*"experienced" + 0.009*"practice" + 0.009*"needs" + 0.007*"plans" + 0.007*"response" + 0.006*"good" + 0.005*"Rochdale" + 0.005*"3" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3637,7 +3637,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"Rotherham" + 0.007*"needs" + 0.005*"However" + 0.005*"plans" + 0.004*"Council" + 0.004*"Metropolitan" + 0.004*"well" + 0.004*"clear" + 0.004*"ensure"', '0.020*"’" + 0.007*"needs" + 0.007*"Rotherham" + 0.006*"ensure" + 0.005*"plans" + 0.005*"Borough" + 0.005*"Council" + 0.005*"well" + 0.004*"1" + 0.004*"good"', '0.014*"’" + 0.010*"Rotherham" + 0.006*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"However" + 0.005*"Council" + 0.004*"June" + 0.004*"ensure" + 0.004*"clear"']</t>
+    <t>['0.013*"’" + 0.008*"Rotherham" + 0.007*"needs" + 0.006*"well" + 0.004*"Metropolitan" + 0.004*"good" + 0.004*"plans" + 0.004*"Council" + 0.004*"Borough" + 0.004*"However"', '0.012*"’" + 0.006*"Rotherham" + 0.005*"well" + 0.005*"good" + 0.005*"Council" + 0.004*"needs" + 0.004*"ensure" + 0.004*"However" + 0.004*"June" + 0.004*"improve"', '0.018*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"ensure" + 0.005*"good" + 0.005*"Council" + 0.005*"plans" + 0.005*"However" + 0.005*"well" + 0.004*"1"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3664,7 +3664,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.014*"well" + 0.011*"practice" + 0.008*"’" + 0.008*"highly" + 0.005*"needs" + 0.005*"need" + 0.004*"strong" + 0.004*"high" + 0.004*"effective" + 0.004*"leaders"', '0.013*"well" + 0.011*"’" + 0.007*"practice" + 0.006*"strong" + 0.005*"highly" + 0.005*"effective" + 0.004*"high" + 0.004*"leaders" + 0.004*"needs" + 0.004*"progress"', '0.014*"’" + 0.014*"well" + 0.012*"practice" + 0.008*"highly" + 0.008*"strong" + 0.006*"needs" + 0.006*"effective" + 0.006*"leaders" + 0.005*"professionals" + 0.004*"high"']</t>
+    <t>['0.016*"well" + 0.013*"practice" + 0.012*"’" + 0.009*"highly" + 0.007*"strong" + 0.006*"effective" + 0.006*"leaders" + 0.006*"needs" + 0.005*"need" + 0.005*"range"', '0.013*"well" + 0.009*"’" + 0.008*"practice" + 0.006*"needs" + 0.006*"highly" + 0.005*"strong" + 0.004*"effective" + 0.004*"high" + 0.004*"leaders" + 0.004*"risk"', '0.012*"’" + 0.010*"well" + 0.008*"practice" + 0.005*"highly" + 0.005*"strong" + 0.005*"needs" + 0.005*"high" + 0.004*"effective" + 0.004*"leaders" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3694,7 +3694,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"needs" + 0.005*"good" + 0.005*"practice" + 0.005*"need" + 0.005*"clear" + 0.004*"effective" + 0.004*"parents"', '0.012*"’" + 0.008*"plans" + 0.008*"well" + 0.008*"needs" + 0.005*"good" + 0.005*"effective" + 0.004*"supported" + 0.004*"Kingston" + 0.004*"range" + 0.004*"need"', '0.012*"well" + 0.011*"’" + 0.008*"plans" + 0.007*"needs" + 0.004*"good" + 0.004*"risk" + 0.004*"progress" + 0.004*"clear" + 0.004*"effective" + 0.004*"parents"']</t>
+    <t>['0.010*"’" + 0.007*"plans" + 0.007*"well" + 0.007*"needs" + 0.005*"supported" + 0.004*"good" + 0.004*"information" + 0.004*"understand" + 0.004*"appropriate" + 0.004*"effective"', '0.015*"’" + 0.011*"well" + 0.009*"plans" + 0.008*"needs" + 0.006*"good" + 0.005*"clear" + 0.005*"effective" + 0.005*"need" + 0.004*"practice" + 0.004*"progress"', '0.014*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"needs" + 0.005*"risk" + 0.004*"good" + 0.004*"practice" + 0.004*"effective" + 0.004*"need" + 0.004*"Kingston"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3724,7 +3724,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"plans" + 0.004*"needs" + 0.004*"use" + 0.004*"quality" + 0.004*"case" + 0.004*"well" + 0.004*"early" + 0.004*"health" + 0.004*"good"', '0.014*"’" + 0.006*"needs" + 0.006*"well" + 0.005*"quality" + 0.005*"plans" + 0.005*"benefit" + 0.004*"information" + 0.004*"always" + 0.004*"However" + 0.004*"informed"', '0.010*"’" + 0.007*"well" + 0.005*"quality" + 0.004*"effective" + 0.004*"plans" + 0.003*"need" + 0.003*"information" + 0.003*"actions" + 0.003*"However" + 0.003*"use"']</t>
+    <t>['0.008*"’" + 0.005*"quality" + 0.004*"well" + 0.004*"benefit" + 0.004*"use" + 0.004*"good" + 0.003*"needs" + 0.003*"plans" + 0.003*"actions" + 0.003*"information"', '0.008*"’" + 0.006*"well" + 0.004*"needs" + 0.004*"informed" + 0.004*"plans" + 0.004*"information" + 0.004*"timely" + 0.004*"quality" + 0.004*"effective" + 0.004*"risk"', '0.016*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"quality" + 0.005*"effective" + 0.004*"always" + 0.004*"actions" + 0.004*"benefit" + 0.004*"However"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3748,7 +3748,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"well" + 0.009*"good" + 0.009*"needs" + 0.008*"team" + 0.006*"practice" + 0.006*"need" + 0.006*"enough" + 0.005*"effective" + 0.005*"protection"', '0.012*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"good" + 0.007*"need" + 0.006*"effective" + 0.006*"ensure" + 0.006*"practice" + 0.006*"plans" + 0.005*"team"', '0.014*"’" + 0.012*"needs" + 0.010*"well" + 0.006*"protection" + 0.006*"practice" + 0.006*"need" + 0.006*"enough" + 0.006*"team" + 0.006*"ensure" + 0.006*"good"']</t>
+    <t>['0.010*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"protection" + 0.006*"team" + 0.005*"plans" + 0.005*"practice" + 0.005*"ensure"', '0.011*"’" + 0.009*"well" + 0.009*"needs" + 0.008*"good" + 0.007*"need" + 0.006*"protection" + 0.006*"practice" + 0.006*"effective" + 0.006*"team" + 0.005*"plans"', '0.016*"’" + 0.011*"well" + 0.010*"needs" + 0.007*"team" + 0.007*"practice" + 0.007*"good" + 0.006*"need" + 0.006*"ensure" + 0.006*"enough" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3775,7 +3775,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"effective" + 0.006*"plans" + 0.006*"needs" + 0.005*"well" + 0.005*"Salford" + 0.005*"progress" + 0.005*"planning" + 0.004*"2023" + 0.004*"quality"', '0.015*"’" + 0.009*"plans" + 0.008*"needs" + 0.008*"well" + 0.006*"Salford" + 0.006*"practice" + 0.006*"planning" + 0.006*"leaders" + 0.005*"effective" + 0.005*"ensure"', '0.012*"’" + 0.008*"effective" + 0.007*"needs" + 0.007*"well" + 0.007*"plans" + 0.005*"Salford" + 0.005*"6" + 0.004*"appropriate" + 0.004*"quality" + 0.004*"practice"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"effective" + 0.006*"plans" + 0.006*"practice" + 0.005*"leaders" + 0.005*"Salford" + 0.005*"experiences" + 0.004*"Council"', '0.013*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"effective" + 0.007*"needs" + 0.005*"planning" + 0.005*"10" + 0.005*"quality" + 0.005*"Salford" + 0.004*"6"', '0.014*"’" + 0.009*"plans" + 0.007*"Salford" + 0.007*"needs" + 0.006*"well" + 0.006*"effective" + 0.005*"planning" + 0.005*"practice" + 0.005*"appropriate" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3799,7 +3799,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"plans" + 0.007*"Sandwell" + 0.006*"quality" + 0.005*"number" + 0.005*"education" + 0.005*"effective" + 0.005*"many"', '0.014*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"Sandwell" + 0.006*"well" + 0.005*"Trust" + 0.005*"quality" + 0.004*"20" + 0.004*"progress" + 0.004*"many"', '0.012*"’" + 0.008*"Sandwell" + 0.007*"needs" + 0.006*"quality" + 0.006*"plans" + 0.005*"Trust" + 0.005*"well" + 0.004*"progress" + 0.004*"9" + 0.004*"education"']</t>
+    <t>['0.014*"’" + 0.010*"needs" + 0.008*"Sandwell" + 0.008*"plans" + 0.007*"well" + 0.005*"quality" + 0.005*"progress" + 0.005*"effective" + 0.005*"many" + 0.005*"Trust"', '0.015*"’" + 0.007*"plans" + 0.007*"Sandwell" + 0.007*"needs" + 0.006*"quality" + 0.005*"well" + 0.005*"20" + 0.005*"changes" + 0.005*"Trust" + 0.004*"progress"', '0.013*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sandwell" + 0.005*"plans" + 0.005*"education" + 0.005*"quality" + 0.005*"good" + 0.004*"Trust" + 0.004*"9"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3823,7 +3823,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"needs" + 0.006*"practice" + 0.006*"including" + 0.006*"oversight" + 0.005*"lack" + 0.005*"protection" + 0.005*"◼" + 0.005*"always" + 0.005*"plans"', '0.013*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"oversight" + 0.005*"Sefton" + 0.005*"protection" + 0.005*"including" + 0.004*"March" + 0.004*"response" + 0.004*"need"', '0.016*"’" + 0.008*"needs" + 0.006*"practice" + 0.005*"oversight" + 0.005*"many" + 0.005*"4" + 0.005*"management" + 0.005*"lack" + 0.004*"March" + 0.004*"planning"']</t>
+    <t>['0.014*"’" + 0.007*"needs" + 0.007*"oversight" + 0.004*"practice" + 0.004*"including" + 0.004*"protection" + 0.004*"plans" + 0.004*"lack" + 0.004*"many" + 0.004*"identified"', '0.016*"’" + 0.008*"needs" + 0.006*"practice" + 0.005*"protection" + 0.005*"lack" + 0.005*"many" + 0.005*"always" + 0.005*"timely" + 0.005*"oversight" + 0.005*"Sefton"', '0.017*"’" + 0.012*"needs" + 0.007*"practice" + 0.006*"◼" + 0.005*"4" + 0.005*"management" + 0.005*"oversight" + 0.005*"including" + 0.005*"March" + 0.005*"lack"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3856,7 +3856,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"Sheffield" + 0.008*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"leaders" + 0.005*"health" + 0.005*"11" + 0.005*"quality" + 0.005*"good"', '0.016*"’" + 0.010*"Sheffield" + 0.008*"needs" + 0.006*"health" + 0.006*"well" + 0.005*"practice" + 0.005*"22" + 0.005*"leaders" + 0.004*"experiences" + 0.004*"adviser"', '0.023*"’" + 0.012*"Sheffield" + 0.011*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"practice" + 0.005*"health" + 0.004*"quality" + 0.004*"effective"']</t>
+    <t>['0.022*"’" + 0.013*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.007*"leaders" + 0.006*"health" + 0.006*"practice" + 0.005*"quality" + 0.005*"plans" + 0.005*"effective"', '0.022*"’" + 0.009*"Sheffield" + 0.007*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"leaders" + 0.005*"quality" + 0.004*"good" + 0.004*"adviser" + 0.004*"health"', '0.016*"’" + 0.009*"Sheffield" + 0.007*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"health" + 0.004*"leaders" + 0.004*"22" + 0.004*"experiences" + 0.004*"11"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3886,7 +3886,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Shropshire" + 0.005*"plans" + 0.005*"progress" + 0.005*"making" + 0.005*"2022" + 0.005*"7" + 0.005*"11"', '0.014*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"plans" + 0.005*"Shropshire" + 0.005*"2022" + 0.005*"making" + 0.004*"need" + 0.004*"effective"', '0.017*"’" + 0.011*"needs" + 0.009*"Shropshire" + 0.007*"well" + 0.006*"progress" + 0.005*"plans" + 0.005*"practice" + 0.005*"making" + 0.005*"training" + 0.005*"2022"']</t>
+    <t>['0.015*"’" + 0.007*"needs" + 0.005*"well" + 0.004*"progress" + 0.004*"Shropshire" + 0.004*"plans" + 0.004*"making" + 0.004*"leaders" + 0.004*"2022" + 0.004*"make"', '0.015*"’" + 0.009*"needs" + 0.008*"Shropshire" + 0.006*"well" + 0.005*"plans" + 0.005*"2022" + 0.005*"making" + 0.004*"leaders" + 0.004*"progress" + 0.004*"7"', '0.019*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.007*"progress" + 0.006*"plans" + 0.005*"making" + 0.005*"7" + 0.005*"2022" + 0.005*"training"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3910,7 +3910,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"plans" + 0.007*"Slough" + 0.006*"needs" + 0.005*"practice" + 0.005*"impact" + 0.004*"leaders" + 0.004*"However" + 0.004*"need" + 0.004*"23"', '0.017*"’" + 0.009*"Slough" + 0.006*"quality" + 0.005*"practice" + 0.005*"23" + 0.005*"needs" + 0.005*"3" + 0.005*"impact" + 0.005*"leaders" + 0.004*"plans"', '0.017*"’" + 0.007*"needs" + 0.007*"Slough" + 0.007*"quality" + 0.007*"plans" + 0.006*"practice" + 0.005*"3" + 0.005*"progress" + 0.005*"However" + 0.005*"leaders"']</t>
+    <t>['0.014*"’" + 0.008*"Slough" + 0.007*"quality" + 0.007*"plans" + 0.006*"needs" + 0.006*"3" + 0.006*"practice" + 0.005*"leaders" + 0.005*"impact" + 0.005*"However"', '0.021*"’" + 0.008*"Slough" + 0.006*"practice" + 0.006*"quality" + 0.006*"plans" + 0.006*"needs" + 0.006*"leaders" + 0.005*"supported" + 0.005*"planning" + 0.004*"However"', '0.012*"’" + 0.007*"Slough" + 0.007*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"impact" + 0.005*"quality" + 0.005*"practice" + 0.004*"time" + 0.004*"January"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3934,7 +3934,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"lack" + 0.010*"2022" + 0.006*"Solihull" + 0.006*"risk" + 0.005*"practice" + 0.005*"effective" + 0.004*"need" + 0.004*"quality" + 0.004*"plans"', '0.012*"’" + 0.010*"lack" + 0.006*"need" + 0.006*"2022" + 0.006*"practice" + 0.006*"Solihull" + 0.006*"risk" + 0.005*"quality" + 0.005*"means" + 0.005*"significant"', '0.015*"’" + 0.010*"lack" + 0.008*"2022" + 0.007*"need" + 0.006*"Solihull" + 0.006*"quality" + 0.006*"risk" + 0.006*"experiences" + 0.005*"delay" + 0.005*"significant"']</t>
+    <t>['0.015*"’" + 0.012*"lack" + 0.011*"2022" + 0.008*"quality" + 0.007*"risk" + 0.007*"Solihull" + 0.006*"need" + 0.005*"practice" + 0.005*"experiences" + 0.005*"effective"', '0.017*"’" + 0.009*"lack" + 0.007*"2022" + 0.006*"need" + 0.006*"Solihull" + 0.005*"means" + 0.005*"experiences" + 0.005*"progress" + 0.005*"risk" + 0.005*"practice"', '0.013*"’" + 0.009*"lack" + 0.006*"2022" + 0.006*"significant" + 0.005*"Solihull" + 0.005*"risk" + 0.005*"effective" + 0.005*"practice" + 0.005*"need" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3958,7 +3958,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"well" + 0.009*"needs" + 0.006*"good" + 0.006*"Somerset" + 0.006*"plans" + 0.006*"supported" + 0.006*"including" + 0.005*"leaders" + 0.005*"number"', '0.019*"’" + 0.009*"Somerset" + 0.009*"needs" + 0.009*"well" + 0.006*"plans" + 0.005*"progress" + 0.005*"practice" + 0.005*"leaders" + 0.005*"need" + 0.005*"number"', '0.012*"’" + 0.007*"well" + 0.006*"good" + 0.006*"plans" + 0.006*"needs" + 0.005*"supported" + 0.005*"leaders" + 0.004*"Somerset" + 0.004*"regularly" + 0.004*"family"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"plans" + 0.006*"good" + 0.006*"Somerset" + 0.006*"supported" + 0.005*"family" + 0.005*"progress" + 0.005*"including"', '0.022*"’" + 0.009*"well" + 0.007*"Somerset" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"leaders" + 0.005*"including" + 0.005*"number" + 0.005*"practice"', '0.013*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Somerset" + 0.006*"plans" + 0.006*"supported" + 0.005*"number" + 0.005*"good" + 0.005*"need" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3982,7 +3982,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.011*"well" + 0.010*"’" + 0.009*"leaders" + 0.009*"quality" + 0.008*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"timely" + 0.005*"good" + 0.005*"South"', '0.013*"quality" + 0.013*"well" + 0.009*"leaders" + 0.009*"’" + 0.008*"good" + 0.008*"plans" + 0.007*"timely" + 0.006*"Senior" + 0.006*"needs" + 0.005*"always"', '0.008*"quality" + 0.007*"well" + 0.007*"’" + 0.006*"plans" + 0.006*"good" + 0.005*"leaders" + 0.004*"range" + 0.004*"needs" + 0.004*"timely" + 0.004*"progress"']</t>
+    <t>['0.009*"quality" + 0.008*"well" + 0.007*"’" + 0.007*"plans" + 0.005*"leaders" + 0.005*"progress" + 0.005*"good" + 0.004*"timely" + 0.004*"arrangements" + 0.004*"always"', '0.010*"well" + 0.010*"quality" + 0.009*"’" + 0.008*"good" + 0.007*"leaders" + 0.007*"plans" + 0.007*"needs" + 0.005*"progress" + 0.005*"timely" + 0.005*"arrangements"', '0.013*"well" + 0.011*"quality" + 0.010*"leaders" + 0.009*"’" + 0.008*"plans" + 0.007*"timely" + 0.007*"good" + 0.006*"needs" + 0.005*"progress" + 0.005*"timeliness"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -4015,7 +4015,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.007*"needs" + 0.007*"South" + 0.006*"Tyneside" + 0.005*"oversight" + 0.005*"management" + 0.005*"However" + 0.005*"practice" + 0.004*"carers" + 0.004*"effective"', '0.024*"’" + 0.008*"Tyneside" + 0.007*"South" + 0.006*"needs" + 0.006*"management" + 0.005*"oversight" + 0.005*"15" + 0.005*"9" + 0.005*"effective" + 0.005*"risk"', '0.023*"’" + 0.013*"needs" + 0.008*"South" + 0.008*"Tyneside" + 0.006*"However" + 0.005*"carers" + 0.005*"effective" + 0.005*"progress" + 0.005*"2023" + 0.005*"5"']</t>
+    <t>['0.021*"’" + 0.010*"needs" + 0.008*"Tyneside" + 0.007*"South" + 0.005*"carers" + 0.005*"2022" + 0.005*"effective" + 0.005*"2023" + 0.005*"5" + 0.004*"However"', '0.021*"’" + 0.008*"needs" + 0.007*"South" + 0.007*"Tyneside" + 0.006*"oversight" + 0.005*"practice" + 0.005*"management" + 0.005*"effective" + 0.005*"carers" + 0.004*"2022"', '0.029*"’" + 0.009*"needs" + 0.008*"South" + 0.008*"Tyneside" + 0.005*"However" + 0.005*"14" + 0.005*"risk" + 0.005*"oversight" + 0.005*"management" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -4045,7 +4045,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"plans" + 0.005*"Southampton" + 0.005*"improve" + 0.005*"progress" + 0.005*"needs" + 0.005*"experiences" + 0.004*"16" + 0.004*"good" + 0.004*"including"', '0.017*"’" + 0.005*"Southampton" + 0.005*"plans" + 0.004*"improve" + 0.004*"provide" + 0.004*"5" + 0.004*"needs" + 0.004*"need" + 0.004*"including" + 0.004*"well"', '0.017*"’" + 0.006*"Southampton" + 0.005*"progress" + 0.005*"plans" + 0.005*"including" + 0.005*"5" + 0.005*"2023" + 0.004*"timely" + 0.004*"experiences" + 0.004*"improve"']</t>
+    <t>['0.015*"’" + 0.005*"plans" + 0.005*"improve" + 0.005*"Southampton" + 0.005*"5" + 0.005*"experiences" + 0.005*"progress" + 0.004*"including" + 0.004*"provide" + 0.004*"needs"', '0.017*"’" + 0.006*"Southampton" + 0.005*"plans" + 0.005*"improve" + 0.005*"including" + 0.005*"needs" + 0.005*"progress" + 0.004*"make" + 0.004*"timely" + 0.004*"5"', '0.016*"’" + 0.007*"plans" + 0.006*"Southampton" + 0.005*"June" + 0.004*"progress" + 0.004*"16" + 0.004*"experiences" + 0.004*"well" + 0.004*"effective" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -4081,7 +4081,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"planning" + 0.007*"practice" + 0.007*"quality" + 0.006*"protection" + 0.006*"leaders" + 0.006*"number" + 0.005*"always" + 0.005*"within" + 0.005*"effective"', '0.011*"’" + 0.009*"planning" + 0.007*"practice" + 0.006*"quality" + 0.006*"need" + 0.006*"needs" + 0.006*"Southend" + 0.005*"good" + 0.005*"leaders" + 0.005*"always"', '0.016*"’" + 0.007*"practice" + 0.006*"quality" + 0.006*"leaders" + 0.006*"planning" + 0.005*"effective" + 0.005*"number" + 0.005*"within" + 0.005*"protection" + 0.004*"always"']</t>
+    <t>['0.013*"’" + 0.007*"planning" + 0.007*"quality" + 0.007*"practice" + 0.006*"leaders" + 0.006*"protection" + 0.005*"number" + 0.005*"always" + 0.005*"effective" + 0.005*"needs"', '0.015*"’" + 0.009*"planning" + 0.006*"quality" + 0.006*"practice" + 0.006*"leaders" + 0.005*"carers" + 0.005*"number" + 0.005*"effective" + 0.005*"need" + 0.005*"within"', '0.012*"’" + 0.008*"practice" + 0.007*"planning" + 0.007*"quality" + 0.006*"protection" + 0.005*"leaders" + 0.005*"always" + 0.005*"need" + 0.005*"risk" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -4102,7 +4102,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.008*"Helens" + 0.007*"St" + 0.007*"good" + 0.006*"well" + 0.006*"10" + 0.005*"progress" + 0.005*"risk" + 0.005*"21"', '0.019*"’" + 0.008*"St" + 0.007*"well" + 0.007*"Helens" + 0.007*"need" + 0.006*"receive" + 0.006*"progress" + 0.006*"needs" + 0.006*"21" + 0.005*"risk"', '0.010*"’" + 0.008*"Helens" + 0.007*"St" + 0.007*"needs" + 0.006*"progress" + 0.005*"well" + 0.005*"receive" + 0.004*"10" + 0.004*"21" + 0.004*"make"']</t>
+    <t>['0.018*"’" + 0.009*"Helens" + 0.009*"needs" + 0.008*"St" + 0.008*"well" + 0.006*"good" + 0.006*"progress" + 0.006*"risk" + 0.006*"need" + 0.006*"receive"', '0.017*"’" + 0.008*"St" + 0.007*"Helens" + 0.006*"progress" + 0.006*"21" + 0.006*"needs" + 0.005*"well" + 0.005*"10" + 0.005*"receive" + 0.005*"need"', '0.010*"’" + 0.006*"Helens" + 0.005*"St" + 0.005*"well" + 0.005*"10" + 0.005*"needs" + 0.004*"receive" + 0.004*"need" + 0.004*"risk" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -4126,7 +4126,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"needs" + 0.006*"progress" + 0.005*"quality" + 0.005*"plans" + 0.005*"practice" + 0.005*"oversight" + 0.005*"10" + 0.004*"health" + 0.004*"Staffordshire"', '0.021*"’" + 0.012*"needs" + 0.007*"quality" + 0.007*"oversight" + 0.007*"health" + 0.006*"practice" + 0.006*"Staffordshire" + 0.006*"ensure" + 0.006*"progress" + 0.005*"plans"', '0.014*"’" + 0.011*"needs" + 0.005*"ensure" + 0.005*"practice" + 0.005*"progress" + 0.005*"Staffordshire" + 0.005*"10" + 0.005*"oversight" + 0.005*"quality" + 0.005*"health"']</t>
+    <t>['0.018*"’" + 0.010*"needs" + 0.006*"quality" + 0.005*"oversight" + 0.005*"ensure" + 0.005*"plans" + 0.005*"practice" + 0.004*"health" + 0.004*"progress" + 0.004*"good"', '0.019*"’" + 0.013*"needs" + 0.007*"progress" + 0.006*"Staffordshire" + 0.006*"oversight" + 0.006*"quality" + 0.005*"practice" + 0.005*"ensure" + 0.005*"health" + 0.005*"impact"', '0.015*"’" + 0.011*"needs" + 0.006*"practice" + 0.006*"health" + 0.006*"quality" + 0.006*"progress" + 0.005*"Staffordshire" + 0.005*"10" + 0.005*"ensure" + 0.005*"oversight"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -4156,7 +4156,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"practice" + 0.007*"Stockport" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.006*"risk" + 0.005*"leaders" + 0.005*"1" + 0.005*"March"', '0.011*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"strong" + 0.006*"needs" + 0.006*"Stockport" + 0.006*"plans" + 0.005*"quality" + 0.004*"ensure" + 0.004*"range"', '0.010*"’" + 0.008*"well" + 0.006*"Stockport" + 0.006*"practice" + 0.006*"strong" + 0.005*"needs" + 0.005*"ensure" + 0.005*"risk" + 0.005*"team" + 0.005*"quality"']</t>
+    <t>['0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"Stockport" + 0.006*"ensure" + 0.005*"strong" + 0.005*"risk" + 0.005*"need" + 0.005*"plans"', '0.012*"’" + 0.008*"Stockport" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.006*"risk" + 0.005*"strong" + 0.005*"plans" + 0.005*"leaders" + 0.005*"March"', '0.011*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"Stockport" + 0.006*"plans" + 0.005*"strong" + 0.005*"needs" + 0.004*"quality" + 0.004*"28" + 0.004*"range"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -4192,7 +4192,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.011*"plans" + 0.008*"leaders" + 0.006*"quality" + 0.006*"needs" + 0.006*"6" + 0.006*"Stockton" + 0.006*"well" + 0.005*"good" + 0.005*"on-Tees"', '0.023*"’" + 0.010*"leaders" + 0.008*"well" + 0.008*"needs" + 0.007*"on-Tees" + 0.007*"plans" + 0.006*"Stockton" + 0.006*"good" + 0.005*"quality" + 0.005*"senior"', '0.008*"’" + 0.006*"plans" + 0.006*"senior" + 0.006*"quality" + 0.006*"leaders" + 0.005*"good" + 0.005*"Stockton" + 0.004*"well" + 0.004*"needs" + 0.004*"on-Tees"']</t>
+    <t>['0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"leaders" + 0.006*"good" + 0.006*"needs" + 0.006*"on-Tees" + 0.005*"quality" + 0.005*"Stockton" + 0.005*"carers"', '0.018*"’" + 0.012*"leaders" + 0.011*"plans" + 0.007*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"Stockton" + 0.005*"on-Tees" + 0.005*"good" + 0.005*"senior"', '0.024*"’" + 0.006*"leaders" + 0.006*"needs" + 0.006*"plans" + 0.006*"on-Tees" + 0.006*"Stockton" + 0.006*"well" + 0.005*"quality" + 0.005*"senior" + 0.005*"17"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -4216,7 +4216,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"needs" + 0.008*"Stoke" + 0.007*"well" + 0.007*"However" + 0.006*"ensure" + 0.006*"plans" + 0.006*"progress" + 0.006*"on-Trent" + 0.006*"protection"', '0.015*"’" + 0.009*"needs" + 0.008*"on-Trent" + 0.007*"well" + 0.006*"plans" + 0.006*"However" + 0.006*"quality" + 0.005*"protection" + 0.005*"Stoke" + 0.005*"leaders"', '0.012*"’" + 0.007*"plans" + 0.007*"on-Trent" + 0.006*"However" + 0.006*"needs" + 0.005*"well" + 0.005*"ensure" + 0.005*"Stoke" + 0.005*"effectively" + 0.005*"progress"']</t>
+    <t>['0.017*"’" + 0.008*"However" + 0.007*"needs" + 0.006*"on-Trent" + 0.006*"well" + 0.006*"plans" + 0.005*"Stoke" + 0.005*"protection" + 0.005*"3" + 0.005*"ensure"', '0.018*"’" + 0.009*"needs" + 0.007*"on-Trent" + 0.007*"Stoke" + 0.007*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"ensure" + 0.005*"However" + 0.005*"protection"', '0.017*"’" + 0.009*"needs" + 0.008*"Stoke" + 0.007*"well" + 0.007*"on-Trent" + 0.007*"plans" + 0.006*"However" + 0.006*"protection" + 0.006*"ensure" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -4246,7 +4246,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"well" + 0.006*"progress" + 0.006*"effective" + 0.005*"practice" + 0.005*"good" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"experiences" + 0.004*"high"', '0.015*"’" + 0.007*"well" + 0.005*"leaders" + 0.005*"progress" + 0.005*"effective" + 0.005*"good" + 0.004*"ensure" + 0.004*"carers" + 0.004*"need" + 0.004*"practice"', '0.011*"’" + 0.007*"progress" + 0.006*"well" + 0.005*"leaders" + 0.005*"good" + 0.004*"needs" + 0.004*"ensure" + 0.004*"effective" + 0.004*"Suffolk" + 0.003*"practice"']</t>
+    <t>['0.010*"’" + 0.005*"good" + 0.005*"well" + 0.004*"progress" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"effective" + 0.004*"high" + 0.004*"needs" + 0.003*"experiences"', '0.013*"’" + 0.006*"well" + 0.006*"effective" + 0.005*"progress" + 0.005*"practice" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"carers" + 0.004*"needs" + 0.004*"good"', '0.015*"’" + 0.008*"progress" + 0.007*"well" + 0.005*"leaders" + 0.005*"good" + 0.005*"effective" + 0.004*"ensure" + 0.004*"Suffolk" + 0.004*"needs" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -4279,7 +4279,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"quality" + 0.005*"experienced" + 0.005*"Sunderland" + 0.005*"good" + 0.005*"highly" + 0.004*"robust" + 0.004*"practice"', '0.020*"’" + 0.008*"quality" + 0.007*"well" + 0.007*"needs" + 0.007*"Sunderland" + 0.005*"protection" + 0.005*"parents" + 0.005*"experienced" + 0.005*"practice" + 0.005*"council"', '0.012*"’" + 0.007*"well" + 0.006*"quality" + 0.005*"needs" + 0.005*"Sunderland" + 0.004*"training" + 0.004*"good" + 0.004*"council" + 0.004*"TfC" + 0.004*"practice"']</t>
+    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Sunderland" + 0.005*"well" + 0.005*"quality" + 0.005*"experienced" + 0.004*"TfC" + 0.004*"risk" + 0.004*"parents" + 0.004*"protection"', '0.010*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"experienced" + 0.004*"quality" + 0.004*"council" + 0.004*"parents" + 0.004*"Sunderland" + 0.004*"protection"', '0.021*"’" + 0.008*"well" + 0.008*"quality" + 0.007*"needs" + 0.007*"Sunderland" + 0.005*"practice" + 0.005*"good" + 0.005*"training" + 0.005*"experienced" + 0.005*"TfC"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -4309,7 +4309,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"well" + 0.008*"needs" + 0.008*"practice" + 0.007*"progress" + 0.006*"good" + 0.005*"plans" + 0.005*"effective" + 0.005*"carers" + 0.005*"quality"', '0.014*"’" + 0.009*"needs" + 0.009*"well" + 0.007*"progress" + 0.007*"practice" + 0.006*"plans" + 0.005*"17" + 0.005*"quality" + 0.005*"carers" + 0.005*"effective"', '0.012*"’" + 0.012*"needs" + 0.007*"practice" + 0.006*"well" + 0.006*"progress" + 0.005*"17" + 0.004*"effective" + 0.004*"plans" + 0.004*"However" + 0.004*"quality"']</t>
+    <t>['0.012*"’" + 0.010*"needs" + 0.009*"well" + 0.006*"practice" + 0.006*"effective" + 0.006*"progress" + 0.006*"plans" + 0.005*"good" + 0.005*"carers" + 0.004*"However"', '0.012*"’" + 0.009*"well" + 0.009*"needs" + 0.006*"progress" + 0.006*"quality" + 0.006*"practice" + 0.006*"17" + 0.005*"carers" + 0.005*"good" + 0.004*"28"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.009*"practice" + 0.007*"progress" + 0.006*"plans" + 0.005*"However" + 0.005*"carers" + 0.005*"effective" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -4333,7 +4333,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.013*"needs" + 0.008*"Swindon" + 0.008*"well" + 0.007*"impact" + 0.007*"need" + 0.006*"plans" + 0.005*"always" + 0.005*"17" + 0.005*"means"', '0.014*"’" + 0.009*"needs" + 0.007*"need" + 0.007*"well" + 0.005*"plans" + 0.005*"always" + 0.005*"Swindon" + 0.005*"Council" + 0.005*"health" + 0.004*"risk"', '0.026*"’" + 0.015*"needs" + 0.011*"Swindon" + 0.010*"need" + 0.008*"well" + 0.008*"always" + 0.007*"plans" + 0.006*"effective" + 0.006*"health" + 0.006*"Borough"']</t>
+    <t>['0.017*"’" + 0.011*"needs" + 0.008*"well" + 0.007*"Swindon" + 0.007*"always" + 0.005*"need" + 0.005*"plans" + 0.005*"education" + 0.005*"impact" + 0.005*"However"', '0.019*"’" + 0.011*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"Swindon" + 0.005*"always" + 0.005*"need" + 0.005*"Council" + 0.004*"worker" + 0.004*"impact"', '0.026*"’" + 0.015*"needs" + 0.011*"need" + 0.011*"Swindon" + 0.009*"well" + 0.007*"plans" + 0.007*"always" + 0.007*"effective" + 0.006*"impact" + 0.006*"health"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -4360,7 +4360,7 @@
     <t>0.1495</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"impact" + 0.006*"needs" + 0.005*"2023" + 0.005*"risk" + 0.004*"experienced" + 0.004*"quality" + 0.004*"need" + 0.004*"practice" + 0.004*"plans"', '0.016*"’" + 0.010*"needs" + 0.007*"risk" + 0.007*"impact" + 0.006*"4" + 0.006*"practice" + 0.006*"Tameside" + 0.005*"quality" + 0.005*"progress" + 0.005*"2023"', '0.018*"’" + 0.009*"needs" + 0.006*"experienced" + 0.006*"response" + 0.006*"quality" + 0.005*"15" + 0.005*"risk" + 0.005*"impact" + 0.005*"experiences" + 0.005*"understand"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.006*"2023" + 0.006*"4" + 0.006*"impact" + 0.005*"practice" + 0.005*"risk" + 0.005*"quality" + 0.005*"experiences" + 0.005*"effective"', '0.016*"’" + 0.008*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"risk" + 0.005*"impact" + 0.005*"planning" + 0.004*"progress" + 0.004*"understand" + 0.004*"15"', '0.018*"’" + 0.010*"needs" + 0.007*"risk" + 0.007*"impact" + 0.007*"experienced" + 0.006*"response" + 0.006*"quality" + 0.005*"Tameside" + 0.005*"need" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -4384,7 +4384,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"well" + 0.007*"needs" + 0.005*"effective" + 0.004*"plans" + 0.004*"strong" + 0.003*"leaders" + 0.003*"family" + 0.003*"need" + 0.003*"planning"', '0.017*"’" + 0.012*"well" + 0.006*"effective" + 0.006*"needs" + 0.006*"strong" + 0.006*"plans" + 0.006*"practice" + 0.006*"ensure" + 0.005*"improve" + 0.005*"timely"', '0.017*"’" + 0.011*"well" + 0.009*"needs" + 0.008*"effective" + 0.007*"need" + 0.006*"plans" + 0.005*"planning" + 0.005*"strong" + 0.005*"practice" + 0.005*"ensure"']</t>
+    <t>['0.015*"’" + 0.012*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"ensure" + 0.005*"strong" + 0.005*"practice" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders"', '0.016*"’" + 0.009*"well" + 0.008*"effective" + 0.006*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"ensure" + 0.005*"practice" + 0.004*"strong" + 0.004*"planning"', '0.017*"’" + 0.012*"well" + 0.009*"needs" + 0.006*"effective" + 0.005*"strong" + 0.005*"improve" + 0.005*"plans" + 0.005*"need" + 0.005*"planning" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -4408,7 +4408,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"well" + 0.005*"carers" + 0.004*"needs" + 0.004*"Thurrock" + 0.004*"ensure" + 0.004*"need" + 0.004*"protection" + 0.004*"practice" + 0.004*"effective"', '0.013*"’" + 0.010*"well" + 0.005*"need" + 0.005*"carers" + 0.004*"ensure" + 0.004*"practice" + 0.004*"effective" + 0.004*"leaders" + 0.003*"quality" + 0.003*"needs"', '0.014*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"need" + 0.005*"needs" + 0.004*"practice" + 0.004*"good" + 0.004*"leaders" + 0.004*"parents" + 0.004*"Thurrock"']</t>
+    <t>['0.011*"’" + 0.006*"well" + 0.004*"carers" + 0.003*"leaders" + 0.003*"ensure" + 0.003*"need" + 0.003*"vulnerable" + 0.003*"practice" + 0.003*"needs" + 0.003*"protection"', '0.013*"’" + 0.007*"well" + 0.006*"carers" + 0.005*"needs" + 0.005*"need" + 0.004*"ensure" + 0.004*"Thurrock" + 0.003*"effective" + 0.003*"practice" + 0.003*"vulnerable"', '0.014*"’" + 0.010*"well" + 0.006*"carers" + 0.006*"need" + 0.005*"practice" + 0.004*"effective" + 0.004*"leaders" + 0.004*"protection" + 0.004*"needs" + 0.004*"Thurrock"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -4432,7 +4432,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"good" + 0.005*"Torbay" + 0.005*"needs" + 0.005*"progress" + 0.005*"effective" + 0.004*"1" + 0.004*"March" + 0.004*"April"', '0.018*"’" + 0.008*"Torbay" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"21" + 0.005*"plans" + 0.005*"timely" + 0.005*"effective" + 0.005*"team"', '0.014*"’" + 0.011*"well" + 0.008*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.005*"effective" + 0.005*"2022" + 0.004*"timely" + 0.004*"21" + 0.004*"team"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.006*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.005*"team" + 0.004*"21" + 0.004*"progress" + 0.004*"2022" + 0.004*"effective"', '0.017*"’" + 0.010*"well" + 0.009*"Torbay" + 0.006*"effective" + 0.005*"good" + 0.005*"progress" + 0.005*"1" + 0.005*"plans" + 0.005*"needs" + 0.004*"quality"', '0.015*"’" + 0.008*"well" + 0.007*"Torbay" + 0.007*"needs" + 0.006*"good" + 0.005*"timely" + 0.005*"effective" + 0.005*"agencies" + 0.004*"21" + 0.004*"1"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4456,7 +4456,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"needs" + 0.009*"Trafford" + 0.007*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"practice" + 0.005*"placed" + 0.005*"impact" + 0.005*"leaders"', '0.015*"’" + 0.008*"needs" + 0.008*"plans" + 0.007*"well" + 0.007*"Trafford" + 0.007*"leaders" + 0.007*"quality" + 0.006*"team" + 0.005*"practice" + 0.005*"placed"', '0.016*"’" + 0.008*"needs" + 0.006*"Trafford" + 0.006*"well" + 0.006*"quality" + 0.006*"plans" + 0.005*"leaders" + 0.004*"impact" + 0.004*"practice" + 0.004*"ensure"']</t>
+    <t>['0.018*"’" + 0.011*"needs" + 0.009*"Trafford" + 0.008*"well" + 0.006*"plans" + 0.006*"team" + 0.005*"quality" + 0.005*"practice" + 0.005*"placed" + 0.004*"impact"', '0.013*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"Trafford" + 0.006*"well" + 0.006*"quality" + 0.006*"practice" + 0.006*"2" + 0.005*"leaders" + 0.005*"impact"', '0.018*"’" + 0.009*"needs" + 0.007*"quality" + 0.007*"Trafford" + 0.007*"leaders" + 0.007*"plans" + 0.006*"well" + 0.005*"ensure" + 0.005*"placed" + 0.005*"December"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4480,7 +4480,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"leaders" + 0.006*"needs" + 0.005*"well" + 0.005*"Walsall" + 0.005*"information" + 0.005*"oversight" + 0.004*"Senior" + 0.004*"positive" + 0.004*"need"', '0.023*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"well" + 0.006*"Walsall" + 0.005*"4" + 0.005*"supported" + 0.005*"good" + 0.004*"oversight" + 0.004*"information"', '0.021*"’" + 0.007*"needs" + 0.007*"leaders" + 0.005*"Walsall" + 0.005*"4" + 0.005*"well" + 0.005*"Senior" + 0.004*"information" + 0.004*"progress" + 0.004*"2021"']</t>
+    <t>['0.021*"’" + 0.007*"needs" + 0.006*"Walsall" + 0.005*"leaders" + 0.005*"well" + 0.005*"Senior" + 0.005*"information" + 0.004*"oversight" + 0.004*"4" + 0.004*"15"', '0.022*"’" + 0.008*"leaders" + 0.006*"well" + 0.006*"4" + 0.006*"needs" + 0.004*"Walsall" + 0.004*"Senior" + 0.004*"information" + 0.004*"oversight" + 0.004*"carers"', '0.021*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"Walsall" + 0.005*"well" + 0.004*"information" + 0.004*"oversight" + 0.004*"2021" + 0.004*"good" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4510,7 +4510,7 @@
     <t>19/08/19</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"well" + 0.006*"practice" + 0.005*"good" + 0.004*"plans" + 0.004*"progress" + 0.004*"number" + 0.004*"carers" + 0.004*"Senior" + 0.004*"need"', '0.011*"’" + 0.006*"practice" + 0.005*"number" + 0.005*"Senior" + 0.004*"well" + 0.004*"needs" + 0.004*"plans" + 0.004*"carers" + 0.004*"good" + 0.004*"home"', '0.012*"’" + 0.007*"practice" + 0.005*"well" + 0.004*"plans" + 0.004*"progress" + 0.004*"Senior" + 0.004*"need" + 0.003*"home" + 0.003*"range" + 0.003*"provided"']</t>
+    <t>['0.012*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"Senior" + 0.004*"plans" + 0.004*"progress" + 0.004*"information" + 0.004*"carers" + 0.003*"number" + 0.003*"good"', '0.010*"’" + 0.006*"well" + 0.006*"practice" + 0.005*"number" + 0.004*"progress" + 0.004*"need" + 0.004*"information" + 0.004*"Senior" + 0.004*"needs" + 0.003*"good"', '0.018*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"plans" + 0.005*"home" + 0.004*"number" + 0.004*"good" + 0.004*"need" + 0.004*"Senior" + 0.004*"senior"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4540,7 +4540,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Warwickshire" + 0.006*"plans" + 0.005*"3" + 0.004*"information" + 0.004*"practice" + 0.004*"carers" + 0.004*"clear"', '0.011*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Warwickshire" + 0.006*"plans" + 0.005*"progress" + 0.005*"clear" + 0.005*"good" + 0.005*"carers" + 0.005*"practice"', '0.013*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"practice" + 0.005*"Warwickshire" + 0.005*"good" + 0.005*"22" + 0.004*"supported" + 0.004*"December"']</t>
+    <t>['0.011*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Warwickshire" + 0.005*"practice" + 0.005*"22" + 0.004*"December" + 0.004*"clear" + 0.004*"progress"', '0.014*"’" + 0.007*"well" + 0.006*"Warwickshire" + 0.006*"needs" + 0.006*"plans" + 0.005*"carers" + 0.005*"3" + 0.005*"practice" + 0.004*"Senior" + 0.004*"effective"', '0.009*"’" + 0.006*"good" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"clear" + 0.004*"information" + 0.004*"Warwickshire" + 0.004*"supported" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4564,7 +4564,7 @@
     <t>14/03/2022</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"West" + 0.006*"well" + 0.005*"Berkshire" + 0.005*"14" + 0.004*"needs" + 0.004*"need" + 0.004*"plans" + 0.004*"18" + 0.004*"working"', '0.017*"’" + 0.007*"West" + 0.006*"Berkshire" + 0.006*"well" + 0.004*"plans" + 0.004*"2022" + 0.004*"18" + 0.004*"early" + 0.004*"needs" + 0.004*"agency"', '0.012*"’" + 0.007*"Berkshire" + 0.006*"well" + 0.005*"West" + 0.004*"need" + 0.004*"agency" + 0.004*"working" + 0.004*"practice" + 0.003*"education" + 0.003*"plans"']</t>
+    <t>['0.018*"’" + 0.009*"West" + 0.007*"well" + 0.007*"Berkshire" + 0.005*"early" + 0.005*"working" + 0.004*"14" + 0.004*"March" + 0.004*"plans" + 0.004*"needs"', '0.011*"’" + 0.005*"well" + 0.004*"West" + 0.004*"Berkshire" + 0.004*"need" + 0.004*"progress" + 0.003*"plans" + 0.003*"18" + 0.003*"needs" + 0.003*"agency"', '0.011*"’" + 0.006*"Berkshire" + 0.005*"West" + 0.005*"need" + 0.004*"needs" + 0.004*"plans" + 0.004*"well" + 0.004*"agency" + 0.004*"18" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>2637548</t>
@@ -4588,7 +4588,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"West" + 0.007*"well" + 0.006*"Northamptonshire" + 0.005*"NCT" + 0.004*"quality" + 0.004*"practice" + 0.004*"impact" + 0.004*"plans" + 0.004*"14"', '0.020*"’" + 0.010*"Northamptonshire" + 0.007*"West" + 0.006*"well" + 0.006*"NCT" + 0.006*"quality" + 0.006*"practice" + 0.005*"3" + 0.005*"impact" + 0.005*"need"', '0.018*"’" + 0.009*"quality" + 0.006*"needs" + 0.006*"Northamptonshire" + 0.005*"practice" + 0.005*"West" + 0.005*"well" + 0.004*"plans" + 0.004*"Leaders" + 0.004*"need"']</t>
+    <t>['0.014*"’" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"West" + 0.006*"well" + 0.005*"impact" + 0.005*"3" + 0.005*"needs" + 0.005*"plans" + 0.004*"practice"', '0.019*"’" + 0.009*"Northamptonshire" + 0.007*"quality" + 0.006*"West" + 0.006*"well" + 0.005*"NCT" + 0.005*"need" + 0.004*"needs" + 0.004*"health" + 0.004*"place"', '0.018*"’" + 0.007*"Northamptonshire" + 0.007*"West" + 0.007*"practice" + 0.006*"well" + 0.005*"quality" + 0.005*"needs" + 0.005*"NCT" + 0.005*"3" + 0.004*"14"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4612,7 +4612,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"West" + 0.005*"health" + 0.005*"13" + 0.005*"Sussex" + 0.005*"quality" + 0.005*"practice"', '0.013*"’" + 0.007*"well" + 0.006*"plans" + 0.005*"Sussex" + 0.005*"needs" + 0.005*"West" + 0.005*"13" + 0.005*"number" + 0.005*"quality" + 0.004*"health"', '0.012*"’" + 0.005*"plans" + 0.005*"well" + 0.004*"needs" + 0.004*"number" + 0.004*"Sussex" + 0.004*"13" + 0.004*"2023" + 0.003*"quality" + 0.003*"supported"']</t>
+    <t>['0.011*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"quality" + 0.004*"clear" + 0.004*"Sussex" + 0.004*"West" + 0.004*"number" + 0.004*"practice"', '0.014*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"Sussex" + 0.006*"well" + 0.006*"13" + 0.005*"supported" + 0.005*"West" + 0.005*"number" + 0.004*"24"', '0.016*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"West" + 0.005*"needs" + 0.005*"practice" + 0.005*"health" + 0.005*"quality" + 0.004*"13" + 0.004*"number"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4633,7 +4633,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"May" + 0.006*"plans" + 0.006*"quality" + 0.006*"Wigan" + 0.006*"practice" + 0.005*"needs" + 0.005*"leaders" + 0.005*"9" + 0.004*"identified"', '0.013*"’" + 0.007*"May" + 0.006*"plans" + 0.006*"practice" + 0.006*"appropriate" + 0.005*"Wigan" + 0.005*"needs" + 0.005*"quality" + 0.004*"good" + 0.004*"timely"', '0.012*"’" + 0.007*"May" + 0.007*"needs" + 0.007*"appropriate" + 0.006*"practice" + 0.006*"plans" + 0.006*"Wigan" + 0.005*"quality" + 0.005*"leaders" + 0.005*"20"']</t>
+    <t>['0.012*"’" + 0.006*"May" + 0.006*"needs" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"Wigan" + 0.005*"plans" + 0.005*"leaders" + 0.004*"quality" + 0.004*"oversight"', '0.015*"’" + 0.007*"plans" + 0.007*"Wigan" + 0.007*"quality" + 0.007*"May" + 0.006*"timely" + 0.006*"appropriate" + 0.006*"needs" + 0.005*"practice" + 0.005*"9"', '0.009*"’" + 0.009*"May" + 0.009*"practice" + 0.006*"plans" + 0.006*"needs" + 0.005*"well" + 0.004*"appropriate" + 0.004*"leaders" + 0.004*"Wigan" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4666,7 +4666,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"well" + 0.007*"plans" + 0.006*"needs" + 0.006*"need" + 0.006*"parents" + 0.006*"Wiltshire" + 0.005*"including" + 0.005*"risk" + 0.005*"supported"', '0.014*"’" + 0.013*"well" + 0.008*"needs" + 0.006*"progress" + 0.006*"quality" + 0.006*"supported" + 0.006*"Wiltshire" + 0.005*"including" + 0.005*"parents" + 0.005*"ensure"', '0.018*"’" + 0.010*"well" + 0.008*"need" + 0.007*"needs" + 0.006*"risk" + 0.006*"ensure" + 0.006*"Wiltshire" + 0.006*"progress" + 0.006*"including" + 0.005*"parents"']</t>
+    <t>['0.014*"’" + 0.012*"well" + 0.007*"need" + 0.007*"Wiltshire" + 0.006*"parents" + 0.006*"quality" + 0.006*"needs" + 0.006*"plans" + 0.005*"progress" + 0.005*"including"', '0.013*"well" + 0.012*"’" + 0.008*"needs" + 0.006*"need" + 0.006*"progress" + 0.005*"plans" + 0.005*"parents" + 0.005*"including" + 0.005*"quality" + 0.005*"ensure"', '0.019*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"risk" + 0.006*"need" + 0.006*"progress" + 0.006*"Wiltshire" + 0.006*"supported" + 0.006*"including" + 0.005*"parents"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4696,7 +4696,7 @@
     <t>0.1655</t>
   </si>
   <si>
-    <t>['0.010*"needs" + 0.009*"’" + 0.007*"Wirral" + 0.006*"practice" + 0.006*"plans" + 0.006*"number" + 0.005*"ensure" + 0.005*"well" + 0.005*"18" + 0.005*"small"', '0.009*"’" + 0.008*"Wirral" + 0.008*"plans" + 0.007*"ensure" + 0.007*"needs" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"well" + 0.005*"family" + 0.005*"18"', '0.014*"’" + 0.011*"needs" + 0.008*"ensure" + 0.007*"Wirral" + 0.005*"well" + 0.005*"response" + 0.005*"practice" + 0.005*"risk" + 0.005*"plans" + 0.005*"29"']</t>
+    <t>['0.010*"needs" + 0.010*"’" + 0.007*"ensure" + 0.007*"Wirral" + 0.006*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"number" + 0.004*"practice" + 0.004*"September"', '0.009*"’" + 0.006*"18" + 0.006*"Wirral" + 0.006*"needs" + 0.006*"practice" + 0.006*"ensure" + 0.006*"plans" + 0.005*"family" + 0.005*"good" + 0.005*"number"', '0.013*"’" + 0.011*"needs" + 0.008*"Wirral" + 0.008*"ensure" + 0.007*"plans" + 0.007*"practice" + 0.006*"risk" + 0.005*"29" + 0.005*"response" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4720,7 +4720,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"effective" + 0.006*"plans" + 0.006*"6" + 0.005*"needs" + 0.005*"17" + 0.005*"provided" + 0.005*"Council" + 0.004*"quality" + 0.004*"well"', '0.012*"’" + 0.007*"effective" + 0.007*"plans" + 0.007*"progress" + 0.006*"needs" + 0.005*"well" + 0.005*"impact" + 0.004*"appropriate" + 0.004*"Borough" + 0.004*"good"', '0.015*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"well" + 0.006*"provided" + 0.005*"experiences" + 0.005*"quality" + 0.005*"effective" + 0.005*"17"']</t>
+    <t>['0.013*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"17" + 0.006*"well" + 0.005*"experiences" + 0.005*"needs" + 0.005*"appropriate" + 0.004*"progress" + 0.004*"provided"', '0.012*"’" + 0.006*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"provided" + 0.006*"effective" + 0.005*"progress" + 0.005*"impact" + 0.004*"protection" + 0.004*"Wokingham"', '0.012*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"effective" + 0.005*"provided" + 0.005*"experiences" + 0.004*"6" + 0.004*"parents" + 0.004*"clear"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4744,7 +4744,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"effective" + 0.006*"Wolverhampton" + 0.006*"receive" + 0.006*"quality" + 0.005*"risks" + 0.005*"risk" + 0.005*"strong"', '0.015*"’" + 0.007*"needs" + 0.005*"Wolverhampton" + 0.005*"effective" + 0.005*"leaders" + 0.004*"risks" + 0.004*"plans" + 0.004*"receive" + 0.004*"supported" + 0.004*"well"', '0.015*"’" + 0.007*"needs" + 0.006*"effective" + 0.005*"Wolverhampton" + 0.005*"risks" + 0.005*"education" + 0.005*"strong" + 0.004*"supported" + 0.004*"quality" + 0.004*"leaders"']</t>
+    <t>['0.018*"’" + 0.009*"needs" + 0.007*"effective" + 0.007*"Wolverhampton" + 0.005*"plans" + 0.005*"receive" + 0.005*"leaders" + 0.005*"education" + 0.005*"well" + 0.005*"risks"', '0.012*"’" + 0.006*"needs" + 0.005*"risks" + 0.005*"effective" + 0.005*"Wolverhampton" + 0.005*"quality" + 0.005*"plans" + 0.005*"supported" + 0.004*"1" + 0.004*"leaders"', '0.010*"’" + 0.007*"needs" + 0.004*"quality" + 0.004*"City" + 0.004*"risk" + 0.004*"strong" + 0.004*"effective" + 0.004*"practice" + 0.004*"supported" + 0.004*"risks"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4774,7 +4774,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"needs" + 0.007*"leaders" + 0.006*"Worcestershire" + 0.006*"progress" + 0.005*"ensure" + 0.005*"appropriate" + 0.004*"education"', '0.015*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"Worcestershire" + 0.007*"leaders" + 0.006*"progress" + 0.005*"ensure" + 0.005*"making" + 0.005*"15" + 0.005*"appropriate"', '0.019*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"progress" + 0.007*"Worcestershire" + 0.007*"needs" + 0.007*"ensure" + 0.006*"leaders" + 0.006*"appropriate" + 0.005*"26"']</t>
+    <t>['0.009*"’" + 0.007*"plans" + 0.007*"Worcestershire" + 0.006*"needs" + 0.006*"progress" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"well" + 0.004*"15" + 0.004*"ensure"', '0.025*"’" + 0.010*"well" + 0.008*"Worcestershire" + 0.008*"plans" + 0.008*"needs" + 0.008*"leaders" + 0.007*"ensure" + 0.007*"progress" + 0.006*"appropriate" + 0.005*"PAs"', '0.015*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"needs" + 0.006*"progress" + 0.006*"leaders" + 0.005*"Worcestershire" + 0.004*"May" + 0.004*"appropriate" + 0.004*"15"']</t>
   </si>
   <si>
     <t>urn</t>

</xml_diff>

<commit_message>
New inspections list added to web front
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -70,7 +70,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"needs" + 0.007*"Barnsley" + 0.007*"leaders" + 0.006*"practice" + 0.006*"within" + 0.005*"plans" + 0.004*"understand" + 0.004*"11" + 0.004*"2023"', '0.013*"’" + 0.007*"needs" + 0.006*"within" + 0.006*"leaders" + 0.005*"practice" + 0.004*"Barnsley" + 0.004*"response" + 0.004*"2023" + 0.004*"quality" + 0.004*"appropriate"', '0.020*"’" + 0.009*"leaders" + 0.008*"needs" + 0.007*"within" + 0.006*"practice" + 0.006*"Barnsley" + 0.005*"plans" + 0.005*"senior" + 0.005*"11" + 0.005*"response"']</t>
+    <t>['0.023*"’" + 0.009*"needs" + 0.007*"within" + 0.007*"leaders" + 0.006*"practice" + 0.005*"Barnsley" + 0.004*"response" + 0.004*"family" + 0.004*"senior" + 0.004*"11"', '0.018*"’" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.006*"Barnsley" + 0.005*"within" + 0.005*"plans" + 0.004*"senior" + 0.004*"11" + 0.004*"2023"', '0.016*"’" + 0.008*"needs" + 0.008*"leaders" + 0.006*"within" + 0.006*"Barnsley" + 0.005*"practice" + 0.005*"plans" + 0.004*"understand" + 0.004*"response" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -115,7 +115,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"receive" + 0.005*"plans" + 0.005*"impact" + 0.005*"practice" + 0.005*"Bath" + 0.004*"protection"', '0.017*"’" + 0.009*"well" + 0.006*"practice" + 0.005*"needs" + 0.005*"leaders" + 0.005*"4" + 0.005*"plans" + 0.005*"Somerset" + 0.004*"East" + 0.004*"2022"', '0.016*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"plans" + 0.005*"leaders" + 0.005*"East" + 0.005*"February" + 0.004*"North" + 0.004*"clear"']</t>
+    <t>['0.012*"’" + 0.008*"well" + 0.005*"needs" + 0.005*"plans" + 0.005*"effective" + 0.004*"East" + 0.004*"4" + 0.004*"‘" + 0.004*"practice" + 0.004*"February"', '0.020*"’" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.005*"receive" + 0.005*"leaders" + 0.005*"2022" + 0.005*"impact" + 0.005*"effective" + 0.005*"Bath"', '0.020*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"leaders" + 0.005*"practice" + 0.005*"4" + 0.005*"clear" + 0.004*"Somerset" + 0.004*"North"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -163,7 +163,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"ensure" + 0.005*"needs" + 0.005*"plans" + 0.005*"Borough" + 0.005*"Bedford" + 0.004*"well" + 0.004*"supported" + 0.004*"progress" + 0.004*"15"', '0.024*"’" + 0.007*"needs" + 0.006*"good" + 0.006*"ensure" + 0.006*"well" + 0.006*"Bedford" + 0.005*"supported" + 0.005*"need" + 0.005*"plans" + 0.004*"education"', '0.017*"’" + 0.007*"needs" + 0.006*"ensure" + 0.006*"well" + 0.006*"plans" + 0.005*"supported" + 0.005*"progress" + 0.005*"education" + 0.005*"Bedford" + 0.005*"relationships"']</t>
+    <t>['0.015*"’" + 0.005*"plans" + 0.005*"needs" + 0.005*"family" + 0.004*"ensure" + 0.004*"education" + 0.004*"Bedford" + 0.004*"relationships" + 0.004*"26" + 0.003*"practitioners"', '0.020*"’" + 0.008*"needs" + 0.006*"ensure" + 0.005*"supported" + 0.005*"Bedford" + 0.005*"Borough" + 0.005*"plans" + 0.005*"well" + 0.005*"progress" + 0.004*"15"', '0.020*"’" + 0.008*"well" + 0.007*"good" + 0.007*"ensure" + 0.007*"needs" + 0.005*"Bedford" + 0.005*"plans" + 0.005*"progress" + 0.005*"supported" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -208,7 +208,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"trust" + 0.006*"progress" + 0.006*"effective" + 0.005*"3" + 0.004*"appropriate" + 0.004*"well" + 0.004*"Birmingham"', '0.014*"’" + 0.010*"needs" + 0.007*"well" + 0.006*"trust" + 0.006*"Birmingham" + 0.006*"effective" + 0.005*"appropriate" + 0.005*"progress" + 0.005*"leaders" + 0.004*"plans"', '0.020*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"effective" + 0.007*"plans" + 0.006*"Birmingham" + 0.005*"progress" + 0.005*"risk" + 0.005*"timely" + 0.005*"3"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.007*"effective" + 0.007*"plans" + 0.006*"Birmingham" + 0.006*"well" + 0.006*"trust" + 0.005*"3" + 0.005*"progress" + 0.005*"appropriate"', '0.017*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"effective" + 0.005*"progress" + 0.005*"plans" + 0.005*"Birmingham" + 0.005*"leaders" + 0.004*"March" + 0.004*"trust"', '0.014*"’" + 0.011*"needs" + 0.007*"effective" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"Birmingham" + 0.005*"trust" + 0.004*"leaders" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -250,7 +250,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"practice" + 0.007*"Darwen" + 0.006*"impact" + 0.006*"Blackburn" + 0.005*"well" + 0.005*"4" + 0.005*"plans"', '0.015*"’" + 0.008*"Blackburn" + 0.008*"quality" + 0.008*"needs" + 0.007*"practice" + 0.007*"well" + 0.007*"Darwen" + 0.006*"impact" + 0.005*"effective" + 0.005*"result"', '0.011*"’" + 0.007*"practice" + 0.006*"needs" + 0.005*"Blackburn" + 0.005*"Darwen" + 0.005*"impact" + 0.005*"quality" + 0.005*"well" + 0.005*"planning" + 0.004*"February"']</t>
+    <t>['0.010*"’" + 0.007*"practice" + 0.007*"needs" + 0.007*"impact" + 0.007*"well" + 0.006*"Blackburn" + 0.006*"Darwen" + 0.005*"quality" + 0.005*"plans" + 0.005*"planning"', '0.014*"’" + 0.007*"needs" + 0.006*"practice" + 0.006*"impact" + 0.006*"quality" + 0.005*"strategy" + 0.005*"well" + 0.005*"Darwen" + 0.005*"means" + 0.005*"planning"', '0.016*"’" + 0.008*"quality" + 0.008*"Blackburn" + 0.008*"needs" + 0.007*"practice" + 0.007*"Darwen" + 0.006*"well" + 0.006*"effective" + 0.005*"result" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -289,7 +289,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.005*"plans" + 0.005*"Blackpool" + 0.005*"effective" + 0.005*"experiences" + 0.005*"practice" + 0.004*"supported" + 0.004*"December"', '0.019*"’" + 0.013*"needs" + 0.010*"well" + 0.008*"Blackpool" + 0.006*"practice" + 0.006*"supported" + 0.005*"effective" + 0.005*"quality" + 0.005*"16" + 0.005*"plans"', '0.014*"’" + 0.009*"well" + 0.009*"Blackpool" + 0.008*"needs" + 0.007*"effective" + 0.005*"experiences" + 0.005*"16" + 0.004*"progress" + 0.004*"quality" + 0.004*"plans"']</t>
+    <t>['0.014*"’" + 0.012*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.006*"effective" + 0.006*"practice" + 0.005*"supported" + 0.005*"5" + 0.005*"good" + 0.005*"16"', '0.019*"’" + 0.009*"needs" + 0.009*"well" + 0.008*"Blackpool" + 0.006*"effective" + 0.005*"plans" + 0.005*"including" + 0.005*"experiences" + 0.005*"practice" + 0.005*"timely"', '0.017*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"Blackpool" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective" + 0.004*"quality" + 0.004*"team" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80432</t>
@@ -322,7 +322,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"well" + 0.010*"Bolton" + 0.009*"needs" + 0.007*"plans" + 0.006*"supported" + 0.006*"strong" + 0.005*"need" + 0.005*"11" + 0.005*"timely"', '0.023*"’" + 0.010*"needs" + 0.008*"Bolton" + 0.008*"plans" + 0.007*"well" + 0.006*"planning" + 0.006*"response" + 0.005*"effective" + 0.005*"need" + 0.005*"appropriate"', '0.016*"’" + 0.009*"needs" + 0.007*"plans" + 0.007*"well" + 0.007*"supported" + 0.006*"Bolton" + 0.005*"11" + 0.005*"need" + 0.005*"effective" + 0.004*"15"']</t>
+    <t>['0.017*"’" + 0.007*"Bolton" + 0.007*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"need" + 0.005*"supported" + 0.005*"progress" + 0.005*"planning" + 0.005*"effective"', '0.015*"’" + 0.010*"needs" + 0.008*"Bolton" + 0.008*"well" + 0.007*"plans" + 0.006*"supported" + 0.006*"11" + 0.005*"need" + 0.004*"2023" + 0.004*"planning"', '0.024*"’" + 0.010*"needs" + 0.010*"well" + 0.009*"Bolton" + 0.008*"plans" + 0.006*"planning" + 0.005*"effective" + 0.005*"strong" + 0.005*"supported" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -358,7 +358,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.005*"quality" + 0.005*"practice" + 0.005*"time" + 0.005*"2021" + 0.004*"Bournemouth" + 0.004*"progress" + 0.004*"Christchurch" + 0.004*"well" + 0.004*"However"', '0.014*"’" + 0.005*"progress" + 0.005*"quality" + 0.004*"practice" + 0.004*"impact" + 0.004*"Bournemouth" + 0.004*"However" + 0.004*"Poole" + 0.004*"6" + 0.004*"17"', '0.021*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"progress" + 0.005*"risk" + 0.005*"Christchurch" + 0.005*"17" + 0.005*"Poole" + 0.005*"6" + 0.005*"impact"']</t>
+    <t>['0.018*"’" + 0.006*"progress" + 0.005*"practice" + 0.005*"17" + 0.005*"quality" + 0.005*"Christchurch" + 0.005*"well" + 0.004*"Poole" + 0.004*"time" + 0.004*"impact"', '0.010*"’" + 0.005*"practice" + 0.005*"quality" + 0.004*"progress" + 0.004*"well" + 0.004*"Poole" + 0.004*"risk" + 0.004*"17" + 0.004*"right" + 0.004*"impact"', '0.022*"’" + 0.007*"quality" + 0.006*"practice" + 0.005*"Bournemouth" + 0.005*"6" + 0.005*"However" + 0.005*"impact" + 0.005*"time" + 0.005*"risk" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -403,7 +403,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"Bracknell" + 0.007*"risk" + 0.007*"needs" + 0.007*"effective" + 0.006*"provided" + 0.006*"Forest" + 0.006*"progress" + 0.006*"good" + 0.005*"quality"', '0.017*"’" + 0.007*"Forest" + 0.007*"quality" + 0.006*"Bracknell" + 0.006*"good" + 0.006*"effective" + 0.006*"plans" + 0.005*"positive" + 0.005*"well" + 0.005*"needs"', '0.014*"’" + 0.007*"needs" + 0.006*"Forest" + 0.006*"risk" + 0.006*"Bracknell" + 0.006*"quality" + 0.006*"good" + 0.005*"plans" + 0.005*"well" + 0.005*"need"']</t>
+    <t>['0.017*"’" + 0.008*"Bracknell" + 0.007*"Forest" + 0.007*"progress" + 0.007*"needs" + 0.006*"good" + 0.006*"effective" + 0.006*"plans" + 0.006*"quality" + 0.005*"well"', '0.014*"’" + 0.006*"Forest" + 0.006*"needs" + 0.005*"good" + 0.005*"plans" + 0.005*"risk" + 0.005*"provided" + 0.004*"impact" + 0.004*"effective" + 0.004*"well"', '0.018*"’" + 0.008*"risk" + 0.007*"quality" + 0.007*"needs" + 0.007*"Bracknell" + 0.007*"Forest" + 0.006*"provided" + 0.006*"good" + 0.005*"effective" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80438</t>
@@ -439,7 +439,7 @@
     <t>0.1856</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"well" + 0.008*"Brighton" + 0.008*"Hove" + 0.007*"needs" + 0.007*"relationships" + 0.006*"practice" + 0.006*"progress" + 0.006*"experiences" + 0.005*"family"', '0.015*"’" + 0.006*"practice" + 0.006*"well" + 0.006*"needs" + 0.004*"relationships" + 0.004*"15" + 0.004*"experiences" + 0.004*"progress" + 0.004*"Brighton" + 0.004*"11"', '0.011*"’" + 0.007*"Hove" + 0.006*"needs" + 0.006*"well" + 0.005*"experiences" + 0.005*"practice" + 0.004*"Brighton" + 0.004*"11" + 0.004*"receive" + 0.004*"family"']</t>
+    <t>['0.018*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"practice" + 0.006*"Hove" + 0.006*"Brighton" + 0.005*"progress" + 0.005*"experiences" + 0.005*"receive" + 0.005*"relationships"', '0.016*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"Brighton" + 0.006*"practice" + 0.006*"Hove" + 0.005*"progress" + 0.005*"relationships" + 0.005*"experiences" + 0.004*"15"', '0.016*"’" + 0.008*"Hove" + 0.008*"well" + 0.007*"needs" + 0.007*"Brighton" + 0.006*"practice" + 0.005*"relationships" + 0.005*"experiences" + 0.005*"PAs" + 0.004*"11"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -475,7 +475,7 @@
     <t>0.1875</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"well" + 0.008*"Bristol" + 0.008*"needs" + 0.007*"good" + 0.006*"health" + 0.006*"plans" + 0.006*"progress" + 0.005*"leaders" + 0.005*"need"', '0.015*"’" + 0.008*"well" + 0.007*"Bristol" + 0.007*"good" + 0.007*"needs" + 0.004*"16" + 0.004*"leaders" + 0.004*"27" + 0.004*"receive" + 0.004*"ensure"', '0.018*"’" + 0.010*"good" + 0.007*"needs" + 0.007*"well" + 0.007*"Bristol" + 0.005*"always" + 0.005*"progress" + 0.005*"ensure" + 0.005*"need" + 0.004*"January"']</t>
+    <t>['0.020*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"good" + 0.006*"Bristol" + 0.005*"receive" + 0.004*"2023" + 0.004*"progress" + 0.004*"27" + 0.004*"including"', '0.017*"’" + 0.009*"Bristol" + 0.007*"good" + 0.006*"well" + 0.006*"needs" + 0.005*"need" + 0.004*"always" + 0.004*"leaders" + 0.004*"meetings" + 0.004*"health"', '0.020*"’" + 0.011*"well" + 0.008*"good" + 0.008*"needs" + 0.007*"Bristol" + 0.007*"health" + 0.006*"progress" + 0.006*"plans" + 0.005*"16" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -505,7 +505,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.005*"plans" + 0.005*"17" + 0.004*"6" + 0.004*"December" + 0.004*"needs" + 0.004*"practice" + 0.004*"2021" + 0.004*"number" + 0.004*"small"', '0.014*"’" + 0.006*"number" + 0.005*"Buckinghamshire" + 0.005*"plans" + 0.004*"many" + 0.004*"17" + 0.003*"6" + 0.003*"protection" + 0.003*"progress" + 0.003*"2021"', '0.012*"’" + 0.005*"plans" + 0.005*"Buckinghamshire" + 0.004*"protection" + 0.004*"number" + 0.004*"17" + 0.004*"many" + 0.004*"6" + 0.004*"well" + 0.004*"teams"']</t>
+    <t>['0.012*"’" + 0.005*"number" + 0.004*"17" + 0.004*"Buckinghamshire" + 0.004*"6" + 0.003*"many" + 0.003*"plans" + 0.003*"teams" + 0.003*"2021" + 0.003*"December"', '0.011*"’" + 0.006*"plans" + 0.005*"Buckinghamshire" + 0.005*"number" + 0.004*"many" + 0.004*"practice" + 0.004*"protection" + 0.004*"17" + 0.004*"December" + 0.004*"teams"', '0.016*"’" + 0.005*"plans" + 0.005*"17" + 0.004*"number" + 0.004*"Buckinghamshire" + 0.004*"protection" + 0.004*"6" + 0.004*"2021" + 0.004*"many" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -544,7 +544,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"protection" + 0.007*"needs" + 0.007*"team" + 0.006*"2021" + 0.006*"practice" + 0.006*"quality" + 0.005*"need" + 0.004*"impact" + 0.004*"e"', '0.011*"’" + 0.006*"2021" + 0.006*"needs" + 0.006*"protection" + 0.005*"team" + 0.004*"new" + 0.004*"practice" + 0.004*"risk" + 0.004*"25" + 0.004*"impact"', '0.011*"’" + 0.007*"2021" + 0.006*"needs" + 0.006*"practice" + 0.006*"impact" + 0.006*"Bury" + 0.006*"need" + 0.006*"protection" + 0.006*"risk" + 0.005*"5"']</t>
+    <t>['0.011*"’" + 0.007*"team" + 0.007*"protection" + 0.007*"2021" + 0.006*"needs" + 0.006*"practice" + 0.006*"need" + 0.005*"impact" + 0.005*"quality" + 0.005*"new"', '0.011*"’" + 0.006*"needs" + 0.006*"protection" + 0.005*"2021" + 0.005*"practice" + 0.005*"Bury" + 0.005*"risk" + 0.005*"team" + 0.004*"25" + 0.004*"always"', '0.011*"’" + 0.007*"2021" + 0.006*"protection" + 0.006*"needs" + 0.005*"impact" + 0.005*"quality" + 0.005*"Bury" + 0.005*"need" + 0.005*"practice" + 0.005*"response"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -583,7 +583,7 @@
     <t>0.194</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"needs" + 0.008*"Calderdale" + 0.007*"well" + 0.007*"plans" + 0.007*"ensure" + 0.006*"parents" + 0.005*"progress" + 0.005*"risk" + 0.005*"need"', '0.021*"’" + 0.011*"needs" + 0.010*"Calderdale" + 0.006*"progress" + 0.006*"plans" + 0.005*"risk" + 0.005*"well" + 0.005*"experiences" + 0.005*"ensure" + 0.004*"parents"', '0.017*"’" + 0.008*"needs" + 0.006*"Calderdale" + 0.006*"well" + 0.005*"ensure" + 0.004*"progress" + 0.004*"plans" + 0.004*"information" + 0.004*"risk" + 0.004*"PAs"']</t>
+    <t>['0.024*"’" + 0.009*"needs" + 0.008*"Calderdale" + 0.007*"well" + 0.007*"ensure" + 0.006*"progress" + 0.006*"plans" + 0.005*"parents" + 0.005*"supported" + 0.004*"risk"', '0.020*"’" + 0.010*"needs" + 0.009*"Calderdale" + 0.006*"plans" + 0.006*"risk" + 0.006*"progress" + 0.005*"ensure" + 0.005*"well" + 0.005*"experiences" + 0.004*"parents"', '0.015*"’" + 0.011*"needs" + 0.008*"Calderdale" + 0.006*"well" + 0.006*"plans" + 0.005*"progress" + 0.005*"experiences" + 0.005*"information" + 0.004*"parents" + 0.004*"19"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -613,7 +613,7 @@
     <t>0.2052</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"needs" + 0.006*"quality" + 0.005*"well" + 0.005*"leaders" + 0.005*"However" + 0.004*"4" + 0.004*"good" + 0.004*"effective" + 0.004*"Cambridgeshire"', '0.016*"’" + 0.009*"Cambridgeshire" + 0.007*"needs" + 0.007*"leaders" + 0.006*"good" + 0.005*"effective" + 0.005*"15" + 0.005*"response" + 0.005*"4" + 0.005*"carers"', '0.021*"’" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.005*"good" + 0.005*"Cambridgeshire" + 0.005*"well" + 0.004*"2024" + 0.004*"strong" + 0.004*"15"']</t>
+    <t>['0.014*"’" + 0.005*"needs" + 0.005*"Cambridgeshire" + 0.005*"good" + 0.004*"response" + 0.004*"4" + 0.004*"leaders" + 0.004*"quality" + 0.004*"March" + 0.004*"practice"', '0.015*"’" + 0.008*"needs" + 0.007*"Cambridgeshire" + 0.007*"leaders" + 0.005*"effective" + 0.005*"good" + 0.005*"However" + 0.005*"clear" + 0.005*"access" + 0.005*"practice"', '0.020*"’" + 0.007*"needs" + 0.006*"leaders" + 0.006*"Cambridgeshire" + 0.006*"good" + 0.005*"well" + 0.005*"4" + 0.005*"quality" + 0.005*"effective" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -646,7 +646,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"carers" + 0.007*"need" + 0.007*"good" + 0.006*"Bedfordshire" + 0.006*"plans" + 0.005*"progress" + 0.005*"effective"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"carers" + 0.005*"need" + 0.005*"good" + 0.005*"plans" + 0.004*"progress" + 0.004*"Central" + 0.004*"Bedfordshire"', '0.017*"’" + 0.009*"well" + 0.007*"need" + 0.006*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"good" + 0.005*"carers" + 0.005*"supported" + 0.004*"Central"']</t>
+    <t>['0.013*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"good" + 0.005*"progress" + 0.005*"carers" + 0.004*"information" + 0.004*"plans" + 0.004*"2022"', '0.019*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"need" + 0.006*"carers" + 0.006*"good" + 0.006*"progress" + 0.006*"Central" + 0.005*"Bedfordshire"', '0.014*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"need" + 0.006*"carers" + 0.005*"plans" + 0.005*"good" + 0.004*"effective" + 0.004*"Leaders" + 0.004*"Bedfordshire"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -682,7 +682,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"practice" + 0.007*"well" + 0.006*"Cheshire" + 0.006*"2024" + 0.006*"quality" + 0.005*"East" + 0.005*"means"', '0.016*"’" + 0.008*"2024" + 0.007*"practice" + 0.007*"needs" + 0.007*"plans" + 0.006*"quality" + 0.006*"East" + 0.006*"effective" + 0.006*"well" + 0.006*"Cheshire"', '0.009*"’" + 0.008*"2024" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"quality" + 0.005*"East" + 0.005*"need" + 0.005*"effective"']</t>
+    <t>['0.013*"’" + 0.009*"2024" + 0.007*"practice" + 0.007*"Cheshire" + 0.007*"needs" + 0.006*"plans" + 0.006*"effective" + 0.006*"leaders" + 0.006*"East" + 0.006*"quality"', '0.009*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"East" + 0.006*"2024" + 0.006*"well" + 0.006*"leaders" + 0.006*"quality" + 0.005*"practice" + 0.004*"risk"', '0.015*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"2024" + 0.007*"practice" + 0.006*"plans" + 0.006*"quality" + 0.005*"always" + 0.005*"Cheshire" + 0.005*"East"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -721,7 +721,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"needs" + 0.005*"well" + 0.004*"always" + 0.004*"including" + 0.004*"practice" + 0.004*"early" + 0.004*"order" + 0.004*"impact" + 0.004*"However"', '0.016*"’" + 0.009*"well" + 0.006*"needs" + 0.005*"effective" + 0.004*"plans" + 0.004*"practice" + 0.004*"effectively" + 0.004*"timely" + 0.004*"information" + 0.004*"order"', '0.027*"’" + 0.007*"well" + 0.007*"needs" + 0.005*"practice" + 0.005*"impact" + 0.005*"effectively" + 0.004*"always" + 0.004*"good" + 0.004*"receive" + 0.004*"effective"']</t>
+    <t>['0.013*"’" + 0.006*"well" + 0.006*"needs" + 0.004*"effective" + 0.004*"order" + 0.004*"impact" + 0.004*"practice" + 0.004*"receive" + 0.003*"learning" + 0.003*"good"', '0.019*"’" + 0.008*"well" + 0.005*"needs" + 0.004*"practice" + 0.004*"effectively" + 0.004*"timely" + 0.004*"receive" + 0.004*"effective" + 0.004*"plans" + 0.004*"always"', '0.027*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"practice" + 0.005*"always" + 0.005*"plans" + 0.005*"early" + 0.004*"effectively" + 0.004*"order" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -760,7 +760,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"need" + 0.004*"quality" + 0.004*"2022" + 0.004*"◼" + 0.004*"Council" + 0.004*"risk" + 0.004*"Metropolitan"', '0.021*"’" + 0.008*"plans" + 0.005*"2" + 0.005*"impact" + 0.004*"need" + 0.004*"needs" + 0.004*"senior" + 0.004*"21" + 0.004*"November" + 0.004*"risk"', '0.017*"’" + 0.006*"Bradford" + 0.006*"plans" + 0.005*"many" + 0.005*"quality" + 0.005*"needs" + 0.005*"December" + 0.005*"2" + 0.005*"◼" + 0.005*"practice"']</t>
+    <t>['0.020*"’" + 0.006*"plans" + 0.005*"quality" + 0.005*"need" + 0.005*"risk" + 0.005*"needs" + 0.005*"December" + 0.005*"Bradford" + 0.004*"Council" + 0.004*"2"', '0.020*"’" + 0.006*"plans" + 0.005*"21" + 0.005*"Bradford" + 0.005*"needs" + 0.005*"impact" + 0.005*"2" + 0.004*"City" + 0.004*"Metropolitan" + 0.004*"practice"', '0.022*"’" + 0.007*"plans" + 0.005*"Bradford" + 0.005*"2" + 0.004*"impact" + 0.004*"needs" + 0.004*"worker" + 0.004*"2022" + 0.004*"lack" + 0.004*"Council"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -796,7 +796,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.009*"well" + 0.008*"’" + 0.008*"ensure" + 0.008*"clear" + 0.008*"needs" + 0.006*"progress" + 0.005*"effective" + 0.005*"timely" + 0.005*"understanding" + 0.005*"plans"', '0.015*"needs" + 0.014*"’" + 0.010*"well" + 0.009*"ensure" + 0.007*"effective" + 0.006*"good" + 0.006*"progress" + 0.005*"plans" + 0.005*"supported" + 0.005*"clearly"', '0.011*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"ensure" + 0.006*"effective" + 0.006*"plans" + 0.006*"clear" + 0.005*"good" + 0.005*"progress" + 0.005*"experiences"']</t>
+    <t>['0.015*"’" + 0.013*"needs" + 0.013*"well" + 0.011*"ensure" + 0.008*"effective" + 0.007*"clear" + 0.007*"plans" + 0.007*"progress" + 0.006*"good" + 0.006*"individual"', '0.009*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"ensure" + 0.005*"clear" + 0.005*"progress" + 0.004*"effective" + 0.004*"timely" + 0.004*"experiences" + 0.004*"understanding"', '0.011*"needs" + 0.008*"’" + 0.007*"well" + 0.006*"effective" + 0.006*"ensure" + 0.005*"good" + 0.005*"clear" + 0.005*"progress" + 0.004*"supported" + 0.004*"individual"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -835,7 +835,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.007*"November" + 0.007*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"Wakefield" + 0.006*"19" + 0.006*"leaders" + 0.005*"practice"', '0.017*"’" + 0.009*"well" + 0.008*"leaders" + 0.007*"Wakefield" + 0.007*"plans" + 0.006*"quality" + 0.006*"good" + 0.006*"November" + 0.006*"effective" + 0.005*"practice"', '0.018*"’" + 0.010*"Wakefield" + 0.009*"quality" + 0.008*"November" + 0.007*"leaders" + 0.007*"plans" + 0.007*"effective" + 0.006*"good" + 0.006*"progress" + 0.006*"well"']</t>
+    <t>['0.021*"’" + 0.009*"well" + 0.008*"quality" + 0.008*"November" + 0.008*"leaders" + 0.008*"Wakefield" + 0.007*"effective" + 0.007*"good" + 0.007*"progress" + 0.006*"plans"', '0.012*"’" + 0.008*"Wakefield" + 0.007*"leaders" + 0.006*"plans" + 0.006*"November" + 0.006*"quality" + 0.006*"effective" + 0.005*"19" + 0.005*"practice" + 0.005*"good"', '0.015*"’" + 0.007*"Wakefield" + 0.007*"quality" + 0.007*"good" + 0.006*"November" + 0.006*"well" + 0.006*"effective" + 0.005*"leaders" + 0.005*"practice" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -868,7 +868,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"quality" + 0.009*"needs" + 0.007*"March" + 0.006*"ensure" + 0.006*"York" + 0.005*"need" + 0.005*"training" + 0.005*"However" + 0.005*"plans"', '0.010*"’" + 0.006*"needs" + 0.005*"quality" + 0.005*"effective" + 0.005*"7" + 0.005*"good" + 0.005*"well" + 0.004*"March" + 0.004*"York" + 0.004*"ensure"', '0.017*"’" + 0.008*"March" + 0.008*"effective" + 0.006*"needs" + 0.006*"However" + 0.006*"plans" + 0.005*"supported" + 0.005*"York" + 0.005*"ensure" + 0.005*"well"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.007*"quality" + 0.007*"March" + 0.006*"effective" + 0.006*"However" + 0.005*"well" + 0.005*"ensure" + 0.005*"practice" + 0.005*"York"', '0.012*"’" + 0.007*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"March" + 0.005*"need" + 0.005*"ensure" + 0.005*"However" + 0.004*"effective" + 0.004*"plans"', '0.018*"’" + 0.008*"March" + 0.007*"effective" + 0.007*"quality" + 0.006*"York" + 0.006*"needs" + 0.005*"plans" + 0.005*"good" + 0.005*"7" + 0.005*"training"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -907,7 +907,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.016*"well" + 0.012*"’" + 0.011*"quality" + 0.010*"effective" + 0.009*"leaders" + 0.006*"timely" + 0.006*"good" + 0.006*"plans" + 0.006*"arrangements" + 0.006*"highly"', '0.012*"well" + 0.011*"’" + 0.008*"quality" + 0.006*"effective" + 0.005*"arrangements" + 0.005*"leaders" + 0.005*"plans" + 0.005*"timely" + 0.005*"good" + 0.004*"ensure"', '0.014*"well" + 0.013*"’" + 0.009*"effective" + 0.009*"leaders" + 0.009*"quality" + 0.006*"good" + 0.006*"plans" + 0.005*"highly" + 0.005*"arrangements" + 0.005*"timely"']</t>
+    <t>['0.015*"well" + 0.010*"’" + 0.008*"effective" + 0.008*"quality" + 0.006*"plans" + 0.006*"leaders" + 0.006*"good" + 0.005*"arrangements" + 0.005*"strong" + 0.005*"Senior"', '0.015*"well" + 0.011*"’" + 0.011*"quality" + 0.008*"effective" + 0.008*"leaders" + 0.006*"timely" + 0.006*"highly" + 0.005*"good" + 0.005*"plans" + 0.005*"arrangements"', '0.014*"well" + 0.014*"’" + 0.010*"leaders" + 0.010*"quality" + 0.009*"effective" + 0.006*"good" + 0.006*"arrangements" + 0.006*"plans" + 0.006*"timely" + 0.005*"high"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -940,7 +940,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.012*"Isles" + 0.011*"Scilly" + 0.010*"information" + 0.008*"needs" + 0.008*"practice" + 0.008*"protection" + 0.007*"need" + 0.006*"place" + 0.005*"13"', '0.018*"’" + 0.013*"Isles" + 0.012*"Scilly" + 0.008*"need" + 0.008*"practice" + 0.006*"information" + 0.006*"needs" + 0.005*"quality" + 0.005*"protection" + 0.005*"risks"', '0.019*"’" + 0.012*"Scilly" + 0.011*"Isles" + 0.009*"information" + 0.009*"practice" + 0.009*"need" + 0.007*"quality" + 0.006*"protection" + 0.006*"place" + 0.006*"needs"']</t>
+    <t>['0.022*"’" + 0.013*"Isles" + 0.011*"Scilly" + 0.010*"information" + 0.008*"practice" + 0.007*"need" + 0.006*"place" + 0.006*"needs" + 0.006*"protection" + 0.006*"risks"', '0.022*"’" + 0.016*"Scilly" + 0.009*"Isles" + 0.009*"need" + 0.009*"practice" + 0.008*"information" + 0.008*"needs" + 0.006*"place" + 0.006*"protection" + 0.005*"risks"', '0.017*"’" + 0.013*"Isles" + 0.009*"Scilly" + 0.008*"information" + 0.008*"protection" + 0.007*"practice" + 0.007*"need" + 0.007*"quality" + 0.006*"needs" + 0.005*"11"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -976,7 +976,7 @@
     <t>0.1733</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"Coventry" + 0.007*"needs" + 0.007*"plans" + 0.006*"supported" + 0.006*"well" + 0.006*"strong" + 0.005*"need" + 0.005*"July" + 0.004*"20"', '0.021*"’" + 0.008*"needs" + 0.007*"supported" + 0.007*"Coventry" + 0.006*"well" + 0.006*"family" + 0.006*"plans" + 0.005*"PAs" + 0.004*"strong" + 0.004*"need"', '0.019*"’" + 0.011*"well" + 0.008*"Coventry" + 0.007*"supported" + 0.007*"family" + 0.006*"needs" + 0.006*"strong" + 0.006*"plans" + 0.005*"need" + 0.004*"understand"']</t>
+    <t>['0.013*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Coventry" + 0.005*"supported" + 0.005*"strong" + 0.004*"family" + 0.004*"need" + 0.004*"range" + 0.004*"receive"', '0.024*"’" + 0.010*"Coventry" + 0.008*"well" + 0.008*"needs" + 0.008*"supported" + 0.007*"plans" + 0.006*"family" + 0.006*"strong" + 0.005*"need" + 0.005*"1"', '0.018*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"supported" + 0.006*"Coventry" + 0.006*"plans" + 0.006*"family" + 0.005*"need" + 0.005*"strong" + 0.004*"20"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -1018,7 +1018,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"well" + 0.007*"leaders" + 0.006*"practice" + 0.006*"needs" + 0.006*"October" + 0.005*"quality" + 0.005*"Darlington" + 0.005*"effective" + 0.005*"21"', '0.020*"’" + 0.007*"needs" + 0.007*"October" + 0.006*"Darlington" + 0.006*"well" + 0.006*"leaders" + 0.006*"practice" + 0.005*"education" + 0.005*"supported" + 0.005*"quality"', '0.013*"’" + 0.008*"well" + 0.007*"October" + 0.007*"needs" + 0.007*"leaders" + 0.006*"Darlington" + 0.006*"practice" + 0.004*"effective" + 0.004*"need" + 0.004*"family"']</t>
+    <t>['0.020*"’" + 0.008*"leaders" + 0.007*"well" + 0.006*"October" + 0.006*"practice" + 0.005*"Darlington" + 0.005*"supported" + 0.005*"needs" + 0.005*"effective" + 0.005*"understand"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"October" + 0.006*"practice" + 0.006*"leaders" + 0.006*"Darlington" + 0.006*"quality" + 0.005*"plans" + 0.004*"effective"', '0.017*"’" + 0.007*"well" + 0.006*"October" + 0.006*"Darlington" + 0.006*"needs" + 0.006*"practice" + 0.006*"leaders" + 0.005*"effective" + 0.004*"supported" + 0.004*"access"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -1060,7 +1060,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.011*"needs" + 0.010*"Derby" + 0.007*"plans" + 0.007*"quality" + 0.007*"progress" + 0.006*"need" + 0.006*"receive" + 0.006*"appropriate" + 0.006*"good"', '0.019*"’" + 0.009*"needs" + 0.006*"quality" + 0.006*"receive" + 0.006*"well" + 0.005*"good" + 0.005*"Derby" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"progress"', '0.018*"’" + 0.007*"needs" + 0.006*"receive" + 0.006*"Derby" + 0.006*"quality" + 0.005*"leaders" + 0.005*"plans" + 0.005*"need" + 0.005*"carers" + 0.005*"well"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.008*"Derby" + 0.007*"receive" + 0.006*"good" + 0.006*"plans" + 0.005*"quality" + 0.005*"progress" + 0.005*"need" + 0.005*"leaders"', '0.015*"’" + 0.007*"needs" + 0.006*"Derby" + 0.006*"quality" + 0.006*"appropriate" + 0.005*"leaders" + 0.005*"well" + 0.005*"receive" + 0.005*"progress" + 0.005*"good"', '0.028*"’" + 0.011*"needs" + 0.007*"quality" + 0.007*"Derby" + 0.006*"receive" + 0.006*"progress" + 0.006*"well" + 0.006*"plans" + 0.006*"need" + 0.005*"appropriate"']</t>
   </si>
   <si>
     <t>80460</t>
@@ -1093,7 +1093,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"well" + 0.006*"Derbyshire" + 0.005*"positive" + 0.005*"good" + 0.005*"needs" + 0.005*"plans" + 0.004*"education" + 0.004*"effective" + 0.004*"need"', '0.008*"’" + 0.006*"well" + 0.005*"Derbyshire" + 0.005*"education" + 0.004*"leaders" + 0.004*"health" + 0.004*"November" + 0.004*"2023" + 0.004*"practice" + 0.004*"positive"', '0.019*"’" + 0.010*"well" + 0.007*"Derbyshire" + 0.006*"plans" + 0.005*"effective" + 0.005*"leaders" + 0.005*"needs" + 0.005*"need" + 0.005*"10" + 0.005*"progress"']</t>
+    <t>['0.009*"’" + 0.007*"well" + 0.005*"Derbyshire" + 0.005*"positive" + 0.004*"2023" + 0.004*"plans" + 0.004*"30" + 0.004*"effective" + 0.003*"health" + 0.003*"needs"', '0.008*"’" + 0.007*"well" + 0.005*"Derbyshire" + 0.004*"positive" + 0.003*"10" + 0.003*"leaders" + 0.003*"good" + 0.003*"practice" + 0.003*"plans" + 0.003*"progress"', '0.019*"’" + 0.008*"well" + 0.008*"Derbyshire" + 0.006*"plans" + 0.006*"needs" + 0.005*"need" + 0.005*"health" + 0.005*"good" + 0.005*"education" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1126,7 +1126,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"leaders" + 0.005*"progress" + 0.005*"case" + 0.005*"risk" + 0.005*"health" + 0.005*"well" + 0.004*"time" + 0.004*"Devon" + 0.004*"practice"', '0.008*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"health" + 0.005*"areas" + 0.004*"risk" + 0.004*"leaders" + 0.004*"need" + 0.004*"including" + 0.004*"quality"', '0.009*"’" + 0.007*"well" + 0.005*"risk" + 0.005*"health" + 0.004*"plans" + 0.004*"early" + 0.004*"protection" + 0.004*"Devon" + 0.003*"leaders" + 0.003*"case"']</t>
+    <t>['0.009*"’" + 0.006*"well" + 0.006*"risk" + 0.005*"leaders" + 0.005*"health" + 0.005*"progress" + 0.004*"risks" + 0.004*"Devon" + 0.004*"need" + 0.004*"case"', '0.009*"’" + 0.005*"well" + 0.005*"health" + 0.004*"leaders" + 0.004*"risk" + 0.004*"Devon" + 0.004*"practice" + 0.004*"areas" + 0.004*"time" + 0.004*"protection"', '0.009*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"health" + 0.004*"leaders" + 0.004*"protection" + 0.004*"living" + 0.004*"case" + 0.004*"quality" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1168,7 +1168,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.006*"records" + 0.005*"well" + 0.005*"leaders" + 0.005*"Doncaster" + 0.005*"plans" + 0.004*"receive" + 0.004*"quality" + 0.004*"oversight" + 0.004*"information"', '0.019*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"Doncaster" + 0.005*"arrangements" + 0.005*"many" + 0.005*"14" + 0.005*"plans" + 0.005*"experiences" + 0.005*"quality"', '0.023*"’" + 0.007*"Doncaster" + 0.006*"progress" + 0.006*"well" + 0.005*"many" + 0.005*"records" + 0.005*"Trust" + 0.005*"quality" + 0.004*"protection" + 0.004*"oversight"']</t>
+    <t>['0.020*"’" + 0.006*"Doncaster" + 0.005*"well" + 0.005*"many" + 0.005*"records" + 0.005*"2022" + 0.005*"plans" + 0.005*"arrangements" + 0.005*"leaders" + 0.005*"Trust"', '0.023*"’" + 0.008*"well" + 0.006*"Doncaster" + 0.006*"progress" + 0.005*"leaders" + 0.005*"plans" + 0.005*"quality" + 0.005*"many" + 0.005*"arrangements" + 0.005*"receive"', '0.016*"’" + 0.005*"well" + 0.005*"records" + 0.005*"information" + 0.005*"Doncaster" + 0.004*"leaders" + 0.004*"oversight" + 0.004*"effective" + 0.004*"progress" + 0.004*"time"']</t>
   </si>
   <si>
     <t>2532283</t>
@@ -1201,7 +1201,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Dorset" + 0.007*"good" + 0.007*"well" + 0.005*"arrangements" + 0.005*"27" + 0.005*"needs" + 0.005*"Senior" + 0.005*"8" + 0.004*"October"', '0.014*"’" + 0.008*"Dorset" + 0.005*"well" + 0.005*"good" + 0.004*"needs" + 0.004*"impact" + 0.004*"supported" + 0.004*"arrangements" + 0.004*"September" + 0.004*"need"', '0.013*"’" + 0.006*"Dorset" + 0.006*"good" + 0.005*"well" + 0.004*"including" + 0.004*"needs" + 0.004*"arrangements" + 0.004*"quality" + 0.004*"8" + 0.004*"supported"']</t>
+    <t>['0.012*"’" + 0.006*"good" + 0.006*"Dorset" + 0.005*"needs" + 0.004*"well" + 0.004*"arrangements" + 0.004*"8" + 0.004*"October" + 0.004*"quality" + 0.004*"Senior"', '0.015*"’" + 0.008*"Dorset" + 0.007*"well" + 0.005*"good" + 0.005*"needs" + 0.004*"protection" + 0.004*"need" + 0.004*"arrangements" + 0.004*"2021" + 0.004*"leaders"', '0.014*"’" + 0.009*"Dorset" + 0.007*"good" + 0.006*"well" + 0.005*"impact" + 0.005*"arrangements" + 0.004*"change" + 0.004*"8" + 0.004*"practice" + 0.004*"27"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1234,7 +1234,7 @@
     <t>0.1605</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.008*"Dudley" + 0.005*"well" + 0.004*"always" + 0.004*"However" + 0.004*"oversight" + 0.004*"arrangements" + 0.004*"plans" + 0.004*"2022"', '0.016*"’" + 0.014*"needs" + 0.009*"Dudley" + 0.006*"always" + 0.006*"well" + 0.006*"plans" + 0.006*"arrangements" + 0.005*"quality" + 0.005*"oversight" + 0.005*"ensure"', '0.016*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.005*"arrangements" + 0.005*"plans" + 0.005*"well" + 0.005*"ensure" + 0.004*"However" + 0.004*"always" + 0.004*"oversight"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.010*"Dudley" + 0.006*"arrangements" + 0.006*"always" + 0.005*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"oversight" + 0.004*"October"', '0.015*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.005*"plans" + 0.004*"ensure" + 0.004*"31" + 0.004*"However" + 0.004*"arrangements" + 0.004*"management"', '0.017*"’" + 0.011*"needs" + 0.006*"Dudley" + 0.005*"oversight" + 0.005*"well" + 0.005*"always" + 0.005*"However" + 0.005*"plans" + 0.005*"arrangements" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1273,7 +1273,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"needs" + 0.006*"May" + 0.006*"well" + 0.005*"plans" + 0.005*"Durham" + 0.005*"practice" + 0.004*"10" + 0.004*"ensure" + 0.004*"family"', '0.013*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"May" + 0.005*"Durham" + 0.005*"leaders" + 0.005*"ensure" + 0.005*"practice" + 0.004*"carers" + 0.004*"20"', '0.017*"’" + 0.012*"needs" + 0.009*"Durham" + 0.008*"May" + 0.008*"plans" + 0.007*"well" + 0.007*"ensure" + 0.006*"practice" + 0.005*"risks" + 0.005*"family"']</t>
+    <t>['0.009*"needs" + 0.008*"’" + 0.007*"well" + 0.005*"Durham" + 0.005*"May" + 0.005*"plans" + 0.005*"family" + 0.004*"ensure" + 0.004*"practice" + 0.004*"effective"', '0.016*"’" + 0.010*"needs" + 0.008*"plans" + 0.007*"well" + 0.007*"Durham" + 0.005*"ensure" + 0.005*"May" + 0.005*"risks" + 0.005*"10" + 0.005*"making"', '0.017*"’" + 0.012*"needs" + 0.009*"May" + 0.007*"Durham" + 0.007*"ensure" + 0.007*"practice" + 0.006*"plans" + 0.006*"well" + 0.005*"20" + 0.005*"risks"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1309,7 +1309,7 @@
     <t>0.1742</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"plans" + 0.006*"East" + 0.006*"Riding" + 0.006*"progress" + 0.005*"good" + 0.005*"partners" + 0.005*"education"', '0.012*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"Riding" + 0.005*"progress" + 0.005*"2023" + 0.005*"partners" + 0.004*"East" + 0.004*"30"', '0.016*"’" + 0.009*"plans" + 0.008*"progress" + 0.008*"needs" + 0.008*"well" + 0.007*"East" + 0.006*"Riding" + 0.005*"10" + 0.005*"information" + 0.005*"education"']</t>
+    <t>['0.015*"’" + 0.009*"plans" + 0.008*"needs" + 0.008*"well" + 0.007*"Riding" + 0.006*"progress" + 0.006*"10" + 0.005*"2023" + 0.005*"place" + 0.005*"education"', '0.016*"’" + 0.010*"needs" + 0.008*"plans" + 0.008*"progress" + 0.007*"East" + 0.007*"well" + 0.006*"Riding" + 0.005*"good" + 0.005*"partners" + 0.005*"education"', '0.018*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"needs" + 0.006*"progress" + 0.006*"East" + 0.005*"February" + 0.005*"Riding" + 0.005*"10" + 0.005*"30"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1342,7 +1342,7 @@
     <t>0.1738</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"well" + 0.008*"plans" + 0.008*"Sussex" + 0.007*"progress" + 0.007*"needs" + 0.007*"including" + 0.007*"East" + 0.006*"impact" + 0.005*"experiences"', '0.019*"’" + 0.010*"needs" + 0.010*"well" + 0.008*"plans" + 0.007*"East" + 0.006*"progress" + 0.005*"11" + 0.005*"effective" + 0.005*"impact" + 0.005*"including"', '0.007*"’" + 0.006*"well" + 0.005*"plans" + 0.005*"Sussex" + 0.005*"needs" + 0.004*"East" + 0.003*"progress" + 0.003*"including" + 0.003*"provide" + 0.003*"education"']</t>
+    <t>['0.015*"’" + 0.009*"well" + 0.006*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"East" + 0.005*"including" + 0.005*"impact" + 0.005*"11" + 0.004*"15"', '0.017*"’" + 0.010*"plans" + 0.010*"well" + 0.008*"East" + 0.007*"needs" + 0.006*"Sussex" + 0.006*"progress" + 0.006*"impact" + 0.005*"provide" + 0.005*"including"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"Sussex" + 0.007*"plans" + 0.006*"including" + 0.006*"progress" + 0.005*"East" + 0.005*"11" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1381,7 +1381,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"plans" + 0.007*"well" + 0.007*"progress" + 0.007*"needs" + 0.005*"practice" + 0.005*"understand" + 0.005*"risk" + 0.005*"need" + 0.005*"new"', '0.023*"’" + 0.007*"well" + 0.006*"progress" + 0.006*"Essex" + 0.006*"family" + 0.005*"needs" + 0.005*"plans" + 0.005*"experiences" + 0.005*"supported" + 0.005*"leaders"', '0.009*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"family" + 0.005*"parents" + 0.005*"experiences" + 0.005*"plans" + 0.004*"helped" + 0.004*"need"']</t>
+    <t>['0.024*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"progress" + 0.006*"family" + 0.006*"Essex" + 0.005*"experiences" + 0.005*"plans" + 0.005*"need" + 0.005*"practice"', '0.015*"’" + 0.008*"well" + 0.006*"progress" + 0.005*"parents" + 0.005*"plans" + 0.005*"helped" + 0.005*"risk" + 0.004*"‘" + 0.004*"needs" + 0.004*"understand"', '0.013*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"well" + 0.007*"progress" + 0.005*"advisers" + 0.005*"understand" + 0.005*"experiences" + 0.005*"supported" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1420,7 +1420,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"timely" + 0.004*"improve" + 0.004*"home"', '0.010*"’" + 0.007*"effective" + 0.007*"practice" + 0.007*"timely" + 0.006*"quality" + 0.006*"good" + 0.005*"well" + 0.005*"need" + 0.005*"plans" + 0.005*"improve"', '0.015*"’" + 0.009*"effective" + 0.007*"needs" + 0.007*"good" + 0.007*"practice" + 0.006*"well" + 0.005*"quality" + 0.004*"early" + 0.004*"home" + 0.004*"plans"']</t>
+    <t>['0.015*"’" + 0.009*"effective" + 0.007*"good" + 0.007*"needs" + 0.007*"well" + 0.006*"practice" + 0.006*"quality" + 0.006*"timely" + 0.005*"improve" + 0.005*"need"', '0.010*"’" + 0.007*"effective" + 0.005*"good" + 0.005*"practice" + 0.005*"needs" + 0.004*"plans" + 0.004*"timely" + 0.004*"quality" + 0.004*"early" + 0.004*"progress"', '0.014*"’" + 0.009*"effective" + 0.007*"quality" + 0.007*"practice" + 0.007*"good" + 0.005*"well" + 0.005*"early" + 0.005*"timely" + 0.005*"needs" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80470</t>
@@ -1456,7 +1456,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"February" + 0.006*"2022" + 0.005*"well" + 0.005*"timely" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"Gloucestershire"', '0.016*"’" + 0.008*"needs" + 0.008*"February" + 0.006*"2022" + 0.005*"protection" + 0.005*"progress" + 0.005*"need" + 0.005*"Gloucestershire" + 0.004*"plans" + 0.004*"experienced"', '0.018*"’" + 0.009*"needs" + 0.008*"2022" + 0.007*"plans" + 0.006*"well" + 0.006*"February" + 0.005*"18" + 0.005*"experienced" + 0.005*"Gloucestershire" + 0.005*"family"']</t>
+    <t>['0.018*"’" + 0.010*"needs" + 0.008*"plans" + 0.007*"2022" + 0.007*"February" + 0.006*"well" + 0.006*"experienced" + 0.005*"Gloucestershire" + 0.005*"timely" + 0.005*"progress"', '0.017*"’" + 0.008*"needs" + 0.006*"February" + 0.005*"plans" + 0.005*"2022" + 0.005*"well" + 0.005*"protection" + 0.004*"Gloucestershire" + 0.004*"appropriate" + 0.004*"timely"', '0.016*"’" + 0.008*"2022" + 0.007*"February" + 0.007*"needs" + 0.006*"progress" + 0.005*"plans" + 0.005*"well" + 0.005*"family" + 0.005*"leaders" + 0.004*"18"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1489,7 +1489,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.011*"well" + 0.010*"practice" + 0.010*"’" + 0.008*"needs" + 0.008*"risk" + 0.007*"plans" + 0.007*"need" + 0.007*"planning" + 0.006*"good" + 0.006*"always"', '0.016*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"good" + 0.006*"plans" + 0.006*"practice" + 0.006*"effective" + 0.006*"need" + 0.005*"oversight" + 0.005*"always"', '0.011*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"risk" + 0.006*"practice" + 0.006*"quality" + 0.006*"planning" + 0.006*"need" + 0.006*"always"']</t>
+    <t>['0.009*"well" + 0.008*"’" + 0.007*"needs" + 0.007*"practice" + 0.006*"plans" + 0.006*"good" + 0.006*"planning" + 0.005*"means" + 0.005*"risk" + 0.005*"response"', '0.012*"’" + 0.009*"well" + 0.007*"risk" + 0.007*"needs" + 0.007*"plans" + 0.007*"planning" + 0.006*"need" + 0.006*"good" + 0.006*"quality" + 0.006*"effective"', '0.014*"’" + 0.012*"well" + 0.011*"practice" + 0.009*"needs" + 0.008*"plans" + 0.008*"need" + 0.007*"always" + 0.006*"risk" + 0.006*"effective" + 0.006*"cases"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1516,7 +1516,7 @@
     <t>0.1893</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.004*"leaders" + 0.004*"home" + 0.004*"highly" + 0.004*"Hampshire" + 0.004*"strong"', '0.015*"’" + 0.008*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"plans" + 0.004*"Hampshire" + 0.004*"strong" + 0.004*"home" + 0.004*"health" + 0.004*"progress"', '0.014*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"quality" + 0.005*"strong" + 0.004*"leaders" + 0.004*"decisions" + 0.004*"carers" + 0.004*"highly"']</t>
+    <t>['0.024*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"quality" + 0.005*"Hampshire" + 0.004*"home" + 0.004*"strong" + 0.004*"improve" + 0.004*"leaders"', '0.012*"’" + 0.007*"plans" + 0.006*"needs" + 0.005*"well" + 0.004*"strong" + 0.004*"quality" + 0.004*"leaders" + 0.004*"highly" + 0.003*"health" + 0.003*"education"', '0.014*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"well" + 0.005*"leaders" + 0.004*"quality" + 0.004*"strong" + 0.004*"home" + 0.004*"need" + 0.004*"highly"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1546,7 +1546,7 @@
     <t>0.2009</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"Hartlepool" + 0.007*"needs" + 0.006*"March" + 0.006*"well" + 0.005*"strong" + 0.005*"practice" + 0.004*"need" + 0.004*"leaders" + 0.004*"clear"', '0.023*"’" + 0.008*"March" + 0.008*"Hartlepool" + 0.007*"needs" + 0.007*"leaders" + 0.006*"well" + 0.005*"supported" + 0.005*"plans" + 0.005*"ensure" + 0.005*"18"', '0.015*"’" + 0.007*"March" + 0.006*"needs" + 0.006*"well" + 0.006*"Hartlepool" + 0.004*"18" + 0.004*"leaders" + 0.004*"plans" + 0.004*"22" + 0.004*"progress"']</t>
+    <t>['0.016*"’" + 0.008*"needs" + 0.007*"Hartlepool" + 0.006*"March" + 0.006*"leaders" + 0.005*"well" + 0.005*"plans" + 0.004*"family" + 0.004*"clear" + 0.004*"18"', '0.019*"’" + 0.006*"March" + 0.005*"needs" + 0.005*"Hartlepool" + 0.005*"leaders" + 0.004*"well" + 0.004*"plans" + 0.004*"family" + 0.004*"supported" + 0.004*"senior"', '0.022*"’" + 0.009*"March" + 0.008*"Hartlepool" + 0.007*"well" + 0.007*"needs" + 0.006*"18" + 0.005*"leaders" + 0.005*"effective" + 0.005*"clear" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80474</t>
@@ -1579,7 +1579,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.007*"practice" + 0.006*"Herefordshire" + 0.006*"plans" + 0.005*"lack" + 0.005*"needs" + 0.005*"impact" + 0.005*"many" + 0.005*"carers" + 0.004*"29"', '0.016*"’" + 0.005*"Herefordshire" + 0.005*"impact" + 0.005*"needs" + 0.004*"lack" + 0.004*"many" + 0.004*"practice" + 0.004*"progress" + 0.004*"July" + 0.004*"risk"', '0.013*"’" + 0.005*"lack" + 0.005*"practice" + 0.004*"Herefordshire" + 0.004*"impact" + 0.004*"quality" + 0.004*"many" + 0.004*"2022" + 0.004*"18" + 0.004*"progress"']</t>
+    <t>['0.018*"’" + 0.005*"lack" + 0.005*"practice" + 0.005*"Herefordshire" + 0.005*"carers" + 0.005*"needs" + 0.004*"29" + 0.004*"risk" + 0.004*"identified" + 0.004*"ensure"', '0.016*"’" + 0.006*"impact" + 0.005*"practice" + 0.005*"Herefordshire" + 0.005*"plans" + 0.005*"needs" + 0.004*"quality" + 0.004*"agency" + 0.004*"progress" + 0.004*"including"', '0.017*"’" + 0.006*"practice" + 0.006*"lack" + 0.005*"Herefordshire" + 0.005*"many" + 0.004*"needs" + 0.004*"management" + 0.004*"2022" + 0.004*"impact" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80475</t>
@@ -1612,7 +1612,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.007*"well" + 0.007*"Hertfordshire" + 0.006*"needs" + 0.006*"receive" + 0.005*"plans" + 0.004*"positive" + 0.004*"23" + 0.004*"‘" + 0.004*"risk"', '0.019*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"receive" + 0.005*"Hertfordshire" + 0.004*"leaders" + 0.004*"family" + 0.004*"2023" + 0.004*"effective" + 0.004*"23"', '0.027*"’" + 0.007*"Hertfordshire" + 0.006*"needs" + 0.005*"well" + 0.005*"need" + 0.004*"January" + 0.004*"27" + 0.004*"plans" + 0.004*"Leaders" + 0.004*"risk"']</t>
+    <t>['0.016*"’" + 0.007*"Hertfordshire" + 0.006*"well" + 0.005*"plans" + 0.004*"needs" + 0.004*"27" + 0.004*"need" + 0.004*"education" + 0.004*"training" + 0.004*"working"', '0.029*"’" + 0.007*"Hertfordshire" + 0.007*"well" + 0.007*"receive" + 0.006*"needs" + 0.004*"risk" + 0.004*"leaders" + 0.004*"Leaders" + 0.004*"need" + 0.004*"27"', '0.021*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Hertfordshire" + 0.005*"positive" + 0.005*"plans" + 0.004*"2023" + 0.004*"receive" + 0.004*"risk" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1642,7 +1642,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"leaders" + 0.005*"needs" + 0.005*"Wight" + 0.005*"supported" + 0.004*"plans" + 0.004*"30" + 0.004*"improve" + 0.004*"3" + 0.004*"practice"', '0.013*"’" + 0.006*"leaders" + 0.005*"Isle" + 0.005*"well" + 0.005*"supported" + 0.005*"3" + 0.005*"needs" + 0.005*"plans" + 0.004*"30" + 0.004*"Wight"', '0.022*"’" + 0.011*"leaders" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"Senior" + 0.005*"Isle" + 0.005*"PAs" + 0.005*"plans" + 0.005*"good"']</t>
+    <t>['0.020*"’" + 0.007*"leaders" + 0.005*"practice" + 0.005*"PAs" + 0.005*"needs" + 0.005*"Wight" + 0.005*"November" + 0.005*"good" + 0.005*"plans" + 0.004*"3"', '0.018*"’" + 0.010*"leaders" + 0.007*"supported" + 0.006*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"30" + 0.005*"time" + 0.005*"3" + 0.005*"Isle"', '0.014*"’" + 0.008*"leaders" + 0.006*"Senior" + 0.006*"well" + 0.005*"Isle" + 0.005*"plans" + 0.005*"Wight" + 0.005*"needs" + 0.005*"3" + 0.005*"October"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1666,7 +1666,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"Kent" + 0.006*"supported" + 0.005*"well" + 0.004*"progress" + 0.004*"leaders" + 0.004*"Council" + 0.004*"County" + 0.004*"needs" + 0.004*"including"', '0.018*"’" + 0.010*"Kent" + 0.007*"needs" + 0.007*"Council" + 0.006*"well" + 0.006*"County" + 0.005*"supported" + 0.004*"leaders" + 0.004*"progress" + 0.004*"including"', '0.022*"’" + 0.012*"Kent" + 0.009*"needs" + 0.006*"well" + 0.006*"Council" + 0.006*"supported" + 0.005*"practice" + 0.005*"County" + 0.005*"progress" + 0.005*"ensure"']</t>
+    <t>['0.017*"’" + 0.009*"Kent" + 0.007*"well" + 0.006*"needs" + 0.005*"supported" + 0.004*"2022" + 0.004*"Council" + 0.004*"County" + 0.004*"practice" + 0.004*"progress"', '0.020*"’" + 0.010*"Kent" + 0.009*"needs" + 0.007*"supported" + 0.006*"Council" + 0.006*"County" + 0.005*"well" + 0.005*"progress" + 0.004*"need" + 0.004*"impact"', '0.016*"’" + 0.011*"Kent" + 0.006*"Council" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"supported" + 0.005*"progress" + 0.005*"County" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1696,7 +1696,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"practice" + 0.006*"planning" + 0.006*"number" + 0.006*"risks" + 0.006*"well" + 0.006*"need" + 0.005*"protection" + 0.005*"needs" + 0.005*"team"', '0.020*"’" + 0.009*"number" + 0.007*"planning" + 0.007*"well" + 0.007*"Hull" + 0.006*"management" + 0.006*"practice" + 0.006*"protection" + 0.006*"need" + 0.006*"risks"', '0.012*"’" + 0.006*"protection" + 0.006*"planning" + 0.005*"impact" + 0.005*"need" + 0.005*"management" + 0.005*"small" + 0.004*"teams" + 0.004*"progress" + 0.004*"practice"']</t>
+    <t>['0.019*"’" + 0.009*"number" + 0.008*"planning" + 0.006*"need" + 0.006*"risks" + 0.005*"right" + 0.005*"management" + 0.005*"practice" + 0.005*"well" + 0.005*"needs"', '0.013*"’" + 0.008*"protection" + 0.006*"well" + 0.006*"planning" + 0.006*"number" + 0.006*"practice" + 0.006*"Hull" + 0.006*"25" + 0.005*"risks" + 0.005*"need"', '0.015*"’" + 0.006*"Hull" + 0.006*"practice" + 0.006*"well" + 0.005*"teams" + 0.005*"number" + 0.005*"progress" + 0.005*"need" + 0.005*"planning" + 0.005*"14"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1729,7 +1729,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"good" + 0.007*"practice" + 0.006*"quality" + 0.006*"permanence" + 0.006*"protection" + 0.006*"plans" + 0.005*"Senior" + 0.005*"senior" + 0.005*"needs"', '0.013*"’" + 0.006*"quality" + 0.006*"practice" + 0.005*"needs" + 0.005*"protection" + 0.005*"well" + 0.004*"good" + 0.004*"plans" + 0.004*"Senior" + 0.004*"training"', '0.011*"’" + 0.006*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"permanence" + 0.005*"plans" + 0.005*"good" + 0.004*"senior" + 0.004*"training" + 0.004*"routinely"']</t>
+    <t>['0.009*"’" + 0.005*"quality" + 0.005*"plans" + 0.005*"good" + 0.004*"practice" + 0.004*"training" + 0.004*"well" + 0.004*"needs" + 0.004*"Senior" + 0.004*"last"', '0.012*"’" + 0.007*"quality" + 0.006*"practice" + 0.006*"needs" + 0.006*"training" + 0.006*"plans" + 0.005*"good" + 0.005*"protection" + 0.005*"permanence" + 0.005*"well"', '0.013*"’" + 0.007*"practice" + 0.007*"quality" + 0.007*"good" + 0.006*"permanence" + 0.005*"well" + 0.005*"Senior" + 0.005*"senior" + 0.005*"protection" + 0.005*"response"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1768,7 +1768,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"progress" + 0.006*"quality" + 0.005*"impact" + 0.005*"Knowsley" + 0.005*"experiences" + 0.005*"good" + 0.005*"need"', '0.011*"’" + 0.009*"progress" + 0.008*"plans" + 0.007*"quality" + 0.007*"Knowsley" + 0.006*"2021" + 0.006*"needs" + 0.005*"need" + 0.005*"domestic" + 0.005*"experiences"', '0.014*"’" + 0.009*"progress" + 0.007*"needs" + 0.007*"quality" + 0.007*"plans" + 0.006*"2021" + 0.006*"Knowsley" + 0.005*"abuse" + 0.005*"11" + 0.005*"good"']</t>
+    <t>['0.014*"’" + 0.007*"progress" + 0.006*"quality" + 0.006*"plans" + 0.005*"2021" + 0.005*"needs" + 0.005*"October" + 0.005*"place" + 0.005*"good" + 0.005*"domestic"', '0.014*"’" + 0.010*"progress" + 0.008*"needs" + 0.006*"Knowsley" + 0.005*"quality" + 0.005*"plans" + 0.005*"2021" + 0.005*"place" + 0.005*"abuse" + 0.005*"leaders"', '0.015*"’" + 0.009*"plans" + 0.008*"progress" + 0.008*"needs" + 0.008*"quality" + 0.007*"Knowsley" + 0.006*"impact" + 0.006*"2021" + 0.006*"experiences" + 0.006*"11"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1801,7 +1801,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.007*"Lancashire" + 0.007*"need" + 0.007*"well" + 0.005*"positive" + 0.005*"plans" + 0.005*"28" + 0.005*"good" + 0.005*"supported"', '0.017*"’" + 0.010*"well" + 0.008*"need" + 0.007*"needs" + 0.006*"Lancashire" + 0.006*"supported" + 0.006*"progress" + 0.006*"health" + 0.005*"live" + 0.005*"parents"', '0.016*"’" + 0.010*"well" + 0.007*"needs" + 0.006*"need" + 0.005*"supported" + 0.005*"practice" + 0.005*"progress" + 0.005*"9" + 0.005*"Lancashire" + 0.005*"plans"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.009*"well" + 0.008*"need" + 0.006*"Lancashire" + 0.006*"positive" + 0.006*"supported" + 0.006*"number" + 0.006*"homes" + 0.005*"parents"', '0.015*"’" + 0.007*"well" + 0.006*"Lancashire" + 0.006*"needs" + 0.005*"practice" + 0.005*"supported" + 0.005*"need" + 0.005*"good" + 0.005*"plans" + 0.005*"information"', '0.018*"’" + 0.010*"well" + 0.007*"need" + 0.006*"needs" + 0.006*"Lancashire" + 0.006*"plans" + 0.005*"practice" + 0.005*"health" + 0.004*"9" + 0.004*"positive"']</t>
   </si>
   <si>
     <t>80481</t>
@@ -1831,7 +1831,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"Leeds" + 0.006*"practice" + 0.005*"well" + 0.005*"risk" + 0.004*"needs" + 0.004*"plans" + 0.004*"2022" + 0.004*"4" + 0.004*"relationships"', '0.017*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.006*"risk" + 0.005*"well" + 0.005*"plans" + 0.004*"protection" + 0.004*"practice" + 0.004*"including" + 0.004*"21"', '0.017*"’" + 0.008*"needs" + 0.008*"Leeds" + 0.006*"well" + 0.005*"making" + 0.005*"ensure" + 0.005*"4" + 0.005*"protection" + 0.004*"benefit" + 0.004*"supported"']</t>
+    <t>['0.018*"’" + 0.008*"Leeds" + 0.008*"needs" + 0.006*"well" + 0.005*"protection" + 0.005*"practice" + 0.005*"risk" + 0.005*"4" + 0.004*"supported" + 0.004*"21"', '0.016*"’" + 0.007*"Leeds" + 0.006*"needs" + 0.006*"well" + 0.006*"risk" + 0.005*"plans" + 0.005*"ensure" + 0.005*"practice" + 0.004*"2022" + 0.004*"4"', '0.013*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"risk" + 0.004*"protection" + 0.004*"supported" + 0.004*"ensure" + 0.004*"including" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1867,7 +1867,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.010*"2021" + 0.009*"Leicester" + 0.007*"well" + 0.006*"needs" + 0.006*"number" + 0.005*"20" + 0.005*"ensure" + 0.005*"1" + 0.005*"September"', '0.021*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"Leicester" + 0.008*"2021" + 0.007*"good" + 0.006*"number" + 0.005*"ensure" + 0.005*"including" + 0.005*"1"', '0.020*"’" + 0.009*"well" + 0.008*"2021" + 0.007*"good" + 0.006*"ensure" + 0.006*"Leicester" + 0.005*"needs" + 0.005*"improve" + 0.005*"circumstances" + 0.004*"1"']</t>
+    <t>['0.026*"’" + 0.011*"well" + 0.010*"2021" + 0.009*"Leicester" + 0.008*"needs" + 0.007*"good" + 0.006*"number" + 0.006*"ensure" + 0.005*"1" + 0.005*"September"', '0.017*"’" + 0.007*"2021" + 0.007*"Leicester" + 0.006*"well" + 0.006*"needs" + 0.006*"good" + 0.006*"ensure" + 0.006*"20" + 0.005*"including" + 0.005*"1"', '0.009*"’" + 0.005*"well" + 0.005*"Leicester" + 0.004*"good" + 0.004*"2021" + 0.004*"ensure" + 0.004*"20" + 0.003*"1" + 0.003*"City" + 0.003*"including"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1903,7 +1903,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"good" + 0.007*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"effective" + 0.005*"impact" + 0.005*"education" + 0.005*"need" + 0.005*"quality"', '0.013*"’" + 0.008*"well" + 0.008*"good" + 0.008*"quality" + 0.008*"effective" + 0.007*"needs" + 0.005*"risk" + 0.005*"impact" + 0.005*"practice" + 0.005*"need"', '0.009*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.006*"effective" + 0.005*"practice" + 0.004*"quality" + 0.004*"progress" + 0.004*"need" + 0.004*"education"']</t>
+    <t>['0.010*"’" + 0.008*"good" + 0.006*"well" + 0.006*"effective" + 0.005*"need" + 0.005*"needs" + 0.004*"impact" + 0.004*"plans" + 0.004*"practice" + 0.004*"leaders"', '0.008*"’" + 0.008*"good" + 0.007*"practice" + 0.007*"effective" + 0.007*"well" + 0.006*"needs" + 0.006*"quality" + 0.005*"impact" + 0.004*"protection" + 0.004*"risk"', '0.014*"’" + 0.010*"well" + 0.008*"needs" + 0.007*"quality" + 0.007*"good" + 0.006*"effective" + 0.006*"education" + 0.005*"impact" + 0.005*"risk" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1936,7 +1936,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"Lincolnshire" + 0.005*"well" + 0.004*"needs" + 0.004*"progress" + 0.004*"education" + 0.003*"plans" + 0.003*"working" + 0.003*"2023" + 0.003*"provide"', '0.020*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"family" + 0.004*"well" + 0.004*"24" + 0.004*"effective" + 0.004*"need"', '0.026*"’" + 0.008*"needs" + 0.008*"Lincolnshire" + 0.007*"well" + 0.005*"plans" + 0.005*"family" + 0.005*"April" + 0.004*"28" + 0.004*"progress" + 0.004*"24"']</t>
+    <t>['0.017*"’" + 0.006*"Lincolnshire" + 0.005*"needs" + 0.005*"family" + 0.005*"effective" + 0.004*"well" + 0.004*"plans" + 0.004*"number" + 0.004*"24" + 0.004*"progress"', '0.027*"’" + 0.007*"needs" + 0.007*"Lincolnshire" + 0.006*"well" + 0.005*"need" + 0.004*"progress" + 0.004*"plans" + 0.004*"family" + 0.004*"2023" + 0.004*"April"', '0.019*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"24" + 0.004*"education" + 0.004*"28" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1966,7 +1966,7 @@
     <t>25/05/23</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"timely" + 0.004*"PAs" + 0.004*"protection" + 0.004*"senior" + 0.004*"Liverpool"', '0.019*"’" + 0.007*"always" + 0.007*"practice" + 0.005*"need" + 0.005*"protection" + 0.005*"Liverpool" + 0.004*"2023" + 0.004*"needs" + 0.004*"harm" + 0.004*"met"', '0.020*"’" + 0.009*"needs" + 0.008*"need" + 0.007*"Liverpool" + 0.007*"quality" + 0.007*"always" + 0.007*"practice" + 0.005*"13" + 0.005*"protection" + 0.005*"24"']</t>
+    <t>['0.020*"’" + 0.008*"need" + 0.007*"practice" + 0.007*"needs" + 0.006*"Liverpool" + 0.006*"always" + 0.005*"quality" + 0.005*"protection" + 0.004*"planning" + 0.004*"13"', '0.022*"’" + 0.007*"always" + 0.007*"practice" + 0.007*"needs" + 0.006*"Liverpool" + 0.005*"quality" + 0.005*"need" + 0.004*"timely" + 0.004*"response" + 0.004*"met"', '0.015*"’" + 0.008*"needs" + 0.006*"protection" + 0.005*"practice" + 0.005*"need" + 0.005*"quality" + 0.005*"always" + 0.005*"Liverpool" + 0.004*"PAs" + 0.004*"13"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1999,7 +1999,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"good" + 0.005*"well" + 0.005*"practice" + 0.004*"progress" + 0.004*"information" + 0.004*"Barking" + 0.004*"ensure"', '0.023*"’" + 0.007*"needs" + 0.005*"practice" + 0.005*"progress" + 0.005*"carers" + 0.005*"planning" + 0.005*"good" + 0.005*"10" + 0.004*"information" + 0.004*"ensure"', '0.024*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"good" + 0.006*"carers" + 0.006*"well" + 0.005*"information" + 0.005*"Dagenham" + 0.004*"effective" + 0.004*"London"']</t>
+    <t>['0.023*"’" + 0.009*"needs" + 0.006*"good" + 0.005*"carers" + 0.005*"plans" + 0.005*"ensure" + 0.005*"practice" + 0.005*"progress" + 0.005*"information" + 0.004*"10"', '0.020*"’" + 0.009*"needs" + 0.006*"plans" + 0.006*"good" + 0.005*"information" + 0.005*"practice" + 0.005*"well" + 0.005*"progress" + 0.004*"ensure" + 0.004*"timely"', '0.023*"’" + 0.006*"well" + 0.006*"carers" + 0.005*"plans" + 0.005*"needs" + 0.005*"e" + 0.005*"good" + 0.005*"London" + 0.004*"practice" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -2038,7 +2038,7 @@
     <t>0.2188</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"good" + 0.010*"needs" + 0.009*"need" + 0.008*"well" + 0.008*"progress" + 0.006*"risk" + 0.006*"plans" + 0.006*"ensure" + 0.006*"clear"', '0.012*"’" + 0.008*"needs" + 0.008*"need" + 0.008*"well" + 0.007*"good" + 0.005*"ensure" + 0.005*"clear" + 0.005*"plans" + 0.005*"progress" + 0.004*"receive"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.009*"good" + 0.006*"plans" + 0.006*"need" + 0.005*"clear" + 0.005*"progress" + 0.005*"quality" + 0.005*"appropriate"']</t>
+    <t>['0.016*"’" + 0.012*"needs" + 0.011*"good" + 0.009*"well" + 0.008*"need" + 0.008*"progress" + 0.007*"plans" + 0.007*"ensure" + 0.007*"clear" + 0.006*"risk"', '0.013*"’" + 0.009*"well" + 0.008*"need" + 0.007*"good" + 0.007*"needs" + 0.005*"quality" + 0.005*"plans" + 0.005*"progress" + 0.005*"clear" + 0.005*"appropriate"', '0.012*"’" + 0.008*"good" + 0.007*"well" + 0.007*"need" + 0.007*"needs" + 0.005*"progress" + 0.005*"supported" + 0.005*"plans" + 0.004*"risks" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80488</t>
@@ -2065,7 +2065,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.006*"effective" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.004*"needs" + 0.004*"Bexley" + 0.004*"6" + 0.004*"make" + 0.004*"protection"', '0.013*"’" + 0.005*"well" + 0.005*"needs" + 0.004*"Bexley" + 0.004*"2023" + 0.004*"effective" + 0.004*"10" + 0.004*"oversight" + 0.004*"make" + 0.004*"practice"', '0.020*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"need" + 0.006*"Bexley" + 0.006*"plans" + 0.006*"effective" + 0.005*"10" + 0.005*"including" + 0.005*"clear"']</t>
+    <t>['0.018*"’" + 0.006*"well" + 0.005*"Bexley" + 0.005*"need" + 0.005*"oversight" + 0.004*"make" + 0.004*"needs" + 0.004*"10" + 0.004*"effective" + 0.004*"progress"', '0.019*"’" + 0.006*"effective" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"need" + 0.005*"Bexley" + 0.004*"10" + 0.004*"6" + 0.004*"February"', '0.021*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"need" + 0.006*"Bexley" + 0.006*"effective" + 0.005*"including" + 0.005*"2023" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -2095,7 +2095,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"well" + 0.008*"leaders" + 0.008*"plans" + 0.007*"progress" + 0.007*"Brent" + 0.006*"quality" + 0.006*"practice" + 0.006*"number" + 0.005*"good"', '0.014*"’" + 0.007*"well" + 0.006*"leaders" + 0.006*"number" + 0.005*"timely" + 0.005*"progress" + 0.005*"practice" + 0.005*"plans" + 0.005*"good" + 0.004*"Brent"', '0.015*"’" + 0.009*"well" + 0.007*"good" + 0.006*"progress" + 0.006*"leaders" + 0.006*"plans" + 0.005*"small" + 0.005*"senior" + 0.005*"quality" + 0.004*"number"']</t>
+    <t>['0.012*"’" + 0.007*"leaders" + 0.006*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"practice" + 0.005*"number" + 0.005*"family" + 0.005*"Brent" + 0.004*"20"', '0.015*"’" + 0.007*"progress" + 0.007*"well" + 0.006*"leaders" + 0.005*"senior" + 0.005*"good" + 0.005*"plans" + 0.005*"Brent" + 0.005*"number" + 0.005*"However"', '0.022*"’" + 0.011*"well" + 0.008*"leaders" + 0.008*"plans" + 0.007*"progress" + 0.007*"quality" + 0.006*"Brent" + 0.006*"good" + 0.005*"number" + 0.005*"senior"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -2131,7 +2131,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.011*"Bromley" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"leaders" + 0.005*"health" + 0.005*"practice" + 0.005*"YPAs" + 0.004*"experiences"', '0.016*"’" + 0.008*"Bromley" + 0.007*"well" + 0.006*"needs" + 0.005*"leaders" + 0.005*"plans" + 0.005*"education" + 0.004*"quality" + 0.004*"practice" + 0.004*"progress"', '0.018*"’" + 0.007*"Bromley" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"plans" + 0.005*"education" + 0.004*"leaders" + 0.004*"17" + 0.004*"access"']</t>
+    <t>['0.023*"’" + 0.011*"Bromley" + 0.008*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"practice" + 0.005*"leaders" + 0.005*"education" + 0.005*"17" + 0.004*"progress"', '0.020*"’" + 0.008*"Bromley" + 0.006*"needs" + 0.006*"leaders" + 0.006*"plans" + 0.005*"well" + 0.005*"experiences" + 0.004*"education" + 0.004*"health" + 0.004*"practice"', '0.015*"’" + 0.008*"Bromley" + 0.006*"well" + 0.006*"needs" + 0.005*"leaders" + 0.005*"health" + 0.005*"practice" + 0.004*"plans" + 0.004*"YPAs" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -2164,7 +2164,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.006*"needs" + 0.006*"leaders" + 0.005*"practice" + 0.005*"well" + 0.005*"Camden" + 0.004*"protection" + 0.004*"progress" + 0.004*"29" + 0.003*"2022"', '0.011*"’" + 0.007*"Camden" + 0.007*"leaders" + 0.005*"protection" + 0.005*"practice" + 0.005*"needs" + 0.004*"appropriate" + 0.004*"progress" + 0.004*"25" + 0.004*"April"', '0.013*"’" + 0.008*"Camden" + 0.007*"practice" + 0.006*"well" + 0.006*"response" + 0.006*"leaders" + 0.005*"protection" + 0.005*"29" + 0.005*"meetings" + 0.005*"25"']</t>
+    <t>['0.014*"’" + 0.007*"practice" + 0.007*"Camden" + 0.007*"leaders" + 0.006*"well" + 0.006*"needs" + 0.005*"response" + 0.005*"29" + 0.005*"protection" + 0.004*"appropriate"', '0.008*"’" + 0.006*"Camden" + 0.006*"protection" + 0.005*"leaders" + 0.005*"response" + 0.004*"well" + 0.004*"practice" + 0.004*"appropriate" + 0.004*"25" + 0.004*"needs"', '0.008*"’" + 0.008*"Camden" + 0.006*"leaders" + 0.005*"practice" + 0.005*"well" + 0.004*"25" + 0.004*"needs" + 0.004*"protection" + 0.004*"29" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -2197,7 +2197,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"ensure" + 0.006*"Croydon" + 0.006*"Senior" + 0.006*"need" + 0.005*"quality" + 0.005*"effective" + 0.005*"good"', '0.011*"’" + 0.007*"needs" + 0.006*"need" + 0.006*"well" + 0.006*"quality" + 0.005*"health" + 0.005*"Senior" + 0.005*"effective" + 0.004*"good" + 0.004*"Croydon"', '0.009*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Croydon" + 0.005*"good" + 0.005*"plans" + 0.005*"education" + 0.005*"Senior" + 0.005*"quality" + 0.005*"improved"']</t>
+    <t>['0.009*"’" + 0.008*"needs" + 0.006*"Croydon" + 0.006*"well" + 0.005*"health" + 0.005*"need" + 0.005*"Senior" + 0.004*"ensure" + 0.004*"quality" + 0.004*"improved"', '0.011*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"Senior" + 0.006*"Croydon" + 0.006*"quality" + 0.006*"ensure" + 0.005*"need" + 0.005*"effective" + 0.005*"good"', '0.015*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"good" + 0.006*"quality" + 0.005*"need" + 0.005*"effective" + 0.005*"Croydon" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2233,7 +2233,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.011*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"progress" + 0.005*"risk" + 0.004*"well" + 0.004*"oversight" + 0.004*"experiences" + 0.004*"family"', '0.012*"’" + 0.009*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.006*"progress" + 0.005*"risk" + 0.005*"experiences" + 0.004*"leaders" + 0.004*"family"', '0.009*"’" + 0.008*"quality" + 0.005*"needs" + 0.004*"good" + 0.004*"plans" + 0.004*"well" + 0.004*"management" + 0.004*"risk" + 0.004*"progress" + 0.004*"experiences"']</t>
+    <t>['0.011*"’" + 0.010*"quality" + 0.009*"needs" + 0.006*"good" + 0.005*"risk" + 0.005*"plans" + 0.004*"progress" + 0.004*"family" + 0.004*"oversight" + 0.004*"experiences"', '0.013*"’" + 0.010*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"experiences" + 0.005*"plans" + 0.005*"progress" + 0.005*"Ealing" + 0.005*"risk" + 0.005*"well"', '0.008*"quality" + 0.008*"’" + 0.007*"good" + 0.005*"progress" + 0.004*"management" + 0.004*"plans" + 0.004*"appropriately" + 0.004*"needs" + 0.004*"well" + 0.004*"provide"']</t>
   </si>
   <si>
     <t>80494</t>
@@ -2266,7 +2266,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.009*"practice" + 0.009*"ensure" + 0.008*"clear" + 0.007*"effective" + 0.007*"quality" + 0.006*"good" + 0.006*"Enfield" + 0.006*"timely"', '0.012*"’" + 0.008*"needs" + 0.008*"practice" + 0.008*"good" + 0.008*"ensure" + 0.006*"leaders" + 0.006*"timely" + 0.006*"quality" + 0.005*"Enfield" + 0.005*"effective"', '0.014*"’" + 0.007*"needs" + 0.007*"effective" + 0.007*"good" + 0.007*"Enfield" + 0.006*"ensure" + 0.006*"clear" + 0.006*"range" + 0.006*"improve" + 0.005*"arrangements"']</t>
+    <t>['0.014*"’" + 0.009*"good" + 0.008*"practice" + 0.007*"effective" + 0.007*"needs" + 0.006*"Enfield" + 0.006*"ensure" + 0.005*"clear" + 0.005*"leaders" + 0.005*"timely"', '0.014*"’" + 0.010*"needs" + 0.007*"clear" + 0.006*"good" + 0.006*"timely" + 0.006*"ensure" + 0.006*"Enfield" + 0.006*"quality" + 0.006*"well" + 0.006*"practice"', '0.013*"’" + 0.010*"ensure" + 0.009*"needs" + 0.008*"practice" + 0.007*"effective" + 0.006*"good" + 0.006*"quality" + 0.006*"clear" + 0.006*"Enfield" + 0.006*"leaders"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2299,7 +2299,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"ensure" + 0.005*"progress" + 0.005*"need" + 0.005*"range" + 0.004*"effective"', '0.014*"’" + 0.011*"well" + 0.009*"good" + 0.008*"needs" + 0.006*"need" + 0.006*"range" + 0.006*"plans" + 0.006*"risk" + 0.006*"ensure" + 0.006*"consistently"', '0.011*"’" + 0.009*"well" + 0.009*"plans" + 0.007*"good" + 0.007*"needs" + 0.006*"need" + 0.005*"range" + 0.005*"effective" + 0.005*"progress" + 0.004*"quality"']</t>
+    <t>['0.016*"’" + 0.009*"good" + 0.009*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"range" + 0.007*"need" + 0.005*"information" + 0.005*"risk" + 0.005*"risks"', '0.009*"well" + 0.009*"’" + 0.008*"needs" + 0.006*"good" + 0.006*"range" + 0.005*"need" + 0.005*"effective" + 0.005*"progress" + 0.005*"plans" + 0.004*"effectively"', '0.011*"well" + 0.011*"’" + 0.009*"plans" + 0.007*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"ensure" + 0.005*"progress" + 0.005*"quality" + 0.005*"consistently"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2338,7 +2338,7 @@
     <t>0.1417</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"practice" + 0.007*"number" + 0.006*"planning" + 0.006*"need" + 0.006*"needs" + 0.006*"effective" + 0.005*"within" + 0.005*"cases" + 0.005*"leaders"', '0.014*"’" + 0.010*"practice" + 0.007*"plans" + 0.006*"needs" + 0.006*"effective" + 0.006*"within" + 0.006*"quality" + 0.006*"including" + 0.006*"However" + 0.006*"small"', '0.010*"’" + 0.009*"practice" + 0.006*"number" + 0.006*"planning" + 0.005*"including" + 0.005*"effective" + 0.005*"quality" + 0.005*"within" + 0.005*"plans" + 0.005*"progress"']</t>
+    <t>['0.017*"’" + 0.009*"practice" + 0.007*"number" + 0.007*"within" + 0.006*"planning" + 0.006*"needs" + 0.006*"including" + 0.006*"effective" + 0.006*"need" + 0.005*"plans"', '0.011*"’" + 0.008*"practice" + 0.006*"plans" + 0.005*"number" + 0.004*"effective" + 0.004*"needs" + 0.004*"planning" + 0.004*"quality" + 0.004*"leaders" + 0.004*"However"', '0.012*"practice" + 0.010*"’" + 0.007*"planning" + 0.006*"effective" + 0.006*"number" + 0.006*"small" + 0.006*"quality" + 0.005*"including" + 0.005*"needs" + 0.005*"within"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2371,7 +2371,7 @@
     <t>0.1986</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"receive" + 0.005*"Hammersmith" + 0.005*"understand" + 0.004*"effective" + 0.004*"supported" + 0.004*"needs" + 0.004*"Fulham" + 0.004*"leaders"', '0.014*"’" + 0.006*"well" + 0.005*"needs" + 0.004*"receive" + 0.004*"practice" + 0.004*"plans" + 0.004*"need" + 0.004*"Hammersmith" + 0.004*"Fulham" + 0.004*"Leaders"', '0.014*"’" + 0.007*"well" + 0.006*"receive" + 0.006*"needs" + 0.005*"plans" + 0.005*"leaders" + 0.005*"15" + 0.005*"Fulham" + 0.004*"protection" + 0.004*"2024"']</t>
+    <t>['0.014*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"leaders" + 0.004*"Fulham" + 0.004*"receive" + 0.004*"Leaders" + 0.004*"15" + 0.004*"protection" + 0.004*"progress"', '0.015*"’" + 0.006*"Hammersmith" + 0.006*"well" + 0.005*"needs" + 0.005*"receive" + 0.005*"plans" + 0.004*"protection" + 0.004*"Fulham" + 0.004*"leaders" + 0.004*"2024"', '0.016*"’" + 0.009*"well" + 0.007*"receive" + 0.005*"needs" + 0.004*"plans" + 0.004*"supported" + 0.004*"effective" + 0.004*"2024" + 0.004*"Fulham" + 0.004*"Hammersmith"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2395,7 +2395,7 @@
     <t>13/02/2023</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Haringey" + 0.005*"plans" + 0.004*"well" + 0.004*"need" + 0.004*"practice" + 0.004*"risk" + 0.003*"improve" + 0.003*"supported"', '0.017*"’" + 0.010*"needs" + 0.009*"Haringey" + 0.008*"plans" + 0.007*"well" + 0.005*"good" + 0.005*"progress" + 0.005*"risk" + 0.005*"timely" + 0.005*"supported"', '0.016*"’" + 0.009*"Haringey" + 0.007*"plans" + 0.006*"good" + 0.006*"need" + 0.006*"needs" + 0.006*"well" + 0.005*"progress" + 0.005*"education" + 0.004*"impact"']</t>
+    <t>['0.012*"’" + 0.009*"needs" + 0.008*"Haringey" + 0.006*"plans" + 0.005*"well" + 0.005*"impact" + 0.005*"progress" + 0.004*"supported" + 0.004*"good" + 0.004*"need"', '0.015*"’" + 0.007*"plans" + 0.007*"needs" + 0.007*"well" + 0.007*"Haringey" + 0.005*"good" + 0.005*"risk" + 0.004*"need" + 0.004*"supported" + 0.004*"leaders"', '0.018*"’" + 0.010*"Haringey" + 0.007*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"good" + 0.006*"need" + 0.005*"well" + 0.005*"24" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2428,7 +2428,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"good" + 0.009*"well" + 0.008*"needs" + 0.005*"practice" + 0.005*"team" + 0.005*"plans" + 0.005*"impact" + 0.005*"experiences" + 0.005*"need"', '0.011*"’" + 0.010*"good" + 0.008*"needs" + 0.008*"well" + 0.006*"need" + 0.005*"early" + 0.004*"experiences" + 0.004*"protection" + 0.004*"impact" + 0.004*"school"', '0.013*"’" + 0.012*"good" + 0.008*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"impact" + 0.006*"protection" + 0.005*"practice" + 0.005*"planning" + 0.004*"early"']</t>
+    <t>['0.012*"’" + 0.012*"good" + 0.008*"needs" + 0.008*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"impact" + 0.005*"experiences" + 0.005*"need" + 0.005*"protection"', '0.012*"good" + 0.010*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"impact" + 0.006*"plans" + 0.005*"need" + 0.005*"planning" + 0.005*"experiences" + 0.005*"protection"', '0.013*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"good" + 0.005*"practice" + 0.005*"early" + 0.005*"protection" + 0.005*"need" + 0.004*"school" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2455,7 +2455,7 @@
     <t>16/02/24</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"Havering" + 0.007*"plans" + 0.007*"quality" + 0.006*"effective" + 0.006*"oversight" + 0.005*"many" + 0.004*"22" + 0.004*"experiences" + 0.004*"needs"', '0.018*"’" + 0.013*"Havering" + 0.010*"quality" + 0.008*"plans" + 0.005*"oversight" + 0.005*"needs" + 0.005*"practice" + 0.004*"11" + 0.004*"22" + 0.004*"2023"', '0.014*"’" + 0.009*"Havering" + 0.008*"quality" + 0.006*"effective" + 0.006*"plans" + 0.005*"practice" + 0.005*"needs" + 0.004*"oversight" + 0.004*"11" + 0.004*"December"']</t>
+    <t>['0.010*"’" + 0.008*"Havering" + 0.006*"plans" + 0.005*"quality" + 0.004*"oversight" + 0.004*"22" + 0.003*"effective" + 0.003*"well" + 0.003*"protection" + 0.003*"2023"', '0.022*"’" + 0.012*"Havering" + 0.011*"quality" + 0.008*"plans" + 0.006*"effective" + 0.006*"oversight" + 0.005*"11" + 0.005*"needs" + 0.005*"practice" + 0.004*"22"', '0.013*"’" + 0.011*"Havering" + 0.006*"quality" + 0.005*"plans" + 0.005*"2023" + 0.005*"many" + 0.004*"needs" + 0.004*"well" + 0.003*"effective" + 0.003*"supported"']</t>
   </si>
   <si>
     <t>80501</t>
@@ -2488,7 +2488,7 @@
     <t>0.2119</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"needs" + 0.009*"Hillingdon" + 0.008*"plans" + 0.006*"well" + 0.005*"2" + 0.004*"leaders" + 0.004*"team" + 0.004*"improve" + 0.004*"need"', '0.019*"’" + 0.010*"needs" + 0.009*"plans" + 0.009*"well" + 0.008*"Hillingdon" + 0.005*"need" + 0.005*"team" + 0.004*"6" + 0.004*"family" + 0.004*"senior"', '0.015*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Hillingdon" + 0.005*"plans" + 0.005*"team" + 0.004*"6" + 0.004*"need" + 0.003*"2023" + 0.003*"2"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"Hillingdon" + 0.006*"plans" + 0.005*"team" + 0.005*"need" + 0.004*"6" + 0.004*"leaders" + 0.004*"PAs"', '0.016*"’" + 0.009*"needs" + 0.009*"plans" + 0.008*"Hillingdon" + 0.006*"well" + 0.004*"team" + 0.004*"October" + 0.004*"6" + 0.004*"2" + 0.004*"carers"', '0.020*"’" + 0.010*"needs" + 0.008*"plans" + 0.008*"well" + 0.007*"Hillingdon" + 0.005*"need" + 0.005*"2" + 0.004*"experiences" + 0.004*"team" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2521,7 +2521,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"Hounslow" + 0.008*"effective" + 0.006*"timely" + 0.006*"plans" + 0.005*"strong" + 0.005*"16" + 0.005*"progress"', '0.020*"’" + 0.012*"well" + 0.012*"needs" + 0.007*"timely" + 0.007*"effective" + 0.006*"Hounslow" + 0.005*"oversight" + 0.005*"plans" + 0.005*"experiences" + 0.004*"education"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"Hounslow" + 0.005*"plans" + 0.005*"timely" + 0.004*"20" + 0.004*"oversight" + 0.004*"leaders"']</t>
+    <t>['0.015*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"Hounslow" + 0.007*"well" + 0.005*"timely" + 0.005*"strong" + 0.005*"oversight" + 0.004*"plans" + 0.004*"training"', '0.023*"’" + 0.012*"needs" + 0.011*"well" + 0.008*"effective" + 0.007*"timely" + 0.007*"plans" + 0.007*"Hounslow" + 0.005*"experiences" + 0.005*"20" + 0.005*"16"', '0.020*"’" + 0.012*"needs" + 0.011*"well" + 0.007*"Hounslow" + 0.006*"effective" + 0.006*"timely" + 0.004*"plans" + 0.004*"progress" + 0.004*"16" + 0.004*"oversight"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2551,7 +2551,7 @@
     <t>0.209</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"well" + 0.006*"plans" + 0.005*"highly" + 0.005*"needs" + 0.005*"good" + 0.005*"quality" + 0.005*"risk" + 0.004*"effective" + 0.004*"practice"', '0.015*"needs" + 0.014*"’" + 0.012*"well" + 0.007*"plans" + 0.007*"highly" + 0.007*"good" + 0.006*"quality" + 0.006*"leaders" + 0.006*"effective" + 0.006*"Islington"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"plans" + 0.005*"leaders" + 0.005*"effective" + 0.005*"Islington" + 0.004*"quality" + 0.004*"good" + 0.004*"highly"']</t>
+    <t>['0.011*"needs" + 0.010*"’" + 0.010*"well" + 0.007*"highly" + 0.006*"quality" + 0.005*"practice" + 0.005*"effective" + 0.005*"good" + 0.005*"risk" + 0.005*"plans"', '0.009*"well" + 0.009*"’" + 0.009*"needs" + 0.007*"good" + 0.007*"plans" + 0.006*"leaders" + 0.006*"quality" + 0.005*"highly" + 0.005*"effective" + 0.005*"risk"', '0.017*"’" + 0.012*"needs" + 0.011*"well" + 0.008*"plans" + 0.005*"good" + 0.005*"effective" + 0.005*"Islington" + 0.005*"quality" + 0.005*"highly" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2587,7 +2587,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.008*"well" + 0.008*"good" + 0.007*"plans" + 0.007*"needs" + 0.005*"Lambeth" + 0.005*"need" + 0.005*"impact" + 0.005*"leaders" + 0.004*"4"', '0.019*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"Lambeth" + 0.006*"progress" + 0.006*"impact" + 0.006*"need" + 0.005*"24" + 0.005*"good"', '0.016*"’" + 0.011*"needs" + 0.008*"plans" + 0.007*"good" + 0.007*"well" + 0.007*"Lambeth" + 0.006*"progress" + 0.006*"need" + 0.005*"4" + 0.005*"leaders"']</t>
+    <t>['0.013*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.005*"need" + 0.005*"Lambeth" + 0.004*"24" + 0.004*"supported" + 0.004*"progress"', '0.018*"’" + 0.010*"needs" + 0.009*"plans" + 0.008*"well" + 0.007*"impact" + 0.007*"leaders" + 0.006*"Lambeth" + 0.006*"good" + 0.005*"need" + 0.005*"24"', '0.013*"’" + 0.008*"well" + 0.008*"needs" + 0.008*"progress" + 0.007*"Lambeth" + 0.007*"good" + 0.006*"need" + 0.006*"plans" + 0.005*"4" + 0.005*"number"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2623,7 +2623,7 @@
     <t>0.1803</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.007*"plans" + 0.006*"effective" + 0.006*"needs" + 0.005*"good" + 0.005*"4" + 0.005*"arrangements" + 0.005*"leaders" + 0.005*"progress"', '0.015*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"effective" + 0.007*"plans" + 0.005*"supported" + 0.005*"benefit" + 0.005*"Lewisham" + 0.004*"leaders" + 0.004*"progress"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.008*"Lewisham" + 0.006*"plans" + 0.006*"progress" + 0.005*"15" + 0.005*"effective" + 0.005*"4" + 0.005*"good"']</t>
+    <t>['0.019*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"effective" + 0.005*"Lewisham" + 0.004*"progress" + 0.004*"receive" + 0.004*"2023" + 0.004*"appropriate"', '0.019*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"plans" + 0.006*"Lewisham" + 0.006*"effective" + 0.005*"progress" + 0.005*"4" + 0.005*"15" + 0.005*"leaders"', '0.014*"’" + 0.007*"well" + 0.007*"effective" + 0.007*"needs" + 0.006*"Lewisham" + 0.005*"good" + 0.005*"arrangements" + 0.005*"progress" + 0.005*"4" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2647,7 +2647,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"well" + 0.006*"Merton" + 0.006*"needs" + 0.005*"family" + 0.005*"plans" + 0.005*"helping" + 0.005*"progress" + 0.004*"ensure" + 0.004*"education"', '0.016*"’" + 0.007*"Merton" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"4" + 0.004*"risk" + 0.004*"access" + 0.004*"family" + 0.004*"progress"', '0.013*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"needs" + 0.004*"progress" + 0.004*"across" + 0.004*"2022" + 0.004*"ensure" + 0.004*"practice" + 0.004*"early"']</t>
+    <t>['0.016*"’" + 0.009*"well" + 0.007*"Merton" + 0.005*"ensure" + 0.005*"plans" + 0.005*"needs" + 0.005*"4" + 0.004*"progress" + 0.004*"28" + 0.004*"good"', '0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Merton" + 0.005*"family" + 0.004*"4" + 0.004*"education" + 0.004*"plans" + 0.004*"impact" + 0.004*"2022"', '0.011*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Merton" + 0.005*"plans" + 0.005*"progress" + 0.004*"good" + 0.004*"family" + 0.004*"information" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2671,7 +2671,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"plans" + 0.006*"progress" + 0.006*"needs" + 0.006*"need" + 0.006*"Newham" + 0.006*"practice" + 0.005*"effective" + 0.005*"good" + 0.005*"Leaders"', '0.020*"’" + 0.010*"needs" + 0.007*"Newham" + 0.007*"practice" + 0.006*"progress" + 0.006*"effective" + 0.006*"plans" + 0.006*"need" + 0.005*"good" + 0.004*"well"', '0.021*"’" + 0.008*"Newham" + 0.007*"needs" + 0.006*"effective" + 0.005*"practice" + 0.005*"progress" + 0.005*"plans" + 0.005*"need" + 0.004*"good" + 0.004*"risks"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.008*"Newham" + 0.008*"plans" + 0.006*"practice" + 0.006*"progress" + 0.006*"need" + 0.005*"effective" + 0.005*"good" + 0.005*"Leaders"', '0.022*"’" + 0.008*"needs" + 0.007*"practice" + 0.006*"effective" + 0.006*"progress" + 0.005*"need" + 0.005*"plans" + 0.005*"good" + 0.005*"Newham" + 0.004*"ensure"', '0.020*"’" + 0.008*"Newham" + 0.007*"needs" + 0.006*"progress" + 0.006*"need" + 0.006*"effective" + 0.005*"plans" + 0.005*"good" + 0.005*"practice" + 0.005*"risks"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2701,7 +2701,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.008*"practice" + 0.008*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"Redbridge" + 0.005*"strong" + 0.005*"risk" + 0.004*"effective" + 0.004*"need" + 0.004*"progress"', '0.007*"’" + 0.006*"need" + 0.006*"well" + 0.006*"effective" + 0.006*"strong" + 0.006*"needs" + 0.006*"practice" + 0.005*"Redbridge" + 0.005*"risk" + 0.005*"progress"', '0.008*"’" + 0.007*"practice" + 0.006*"well" + 0.006*"need" + 0.005*"including" + 0.005*"needs" + 0.005*"ensure" + 0.005*"Redbridge" + 0.004*"highly" + 0.004*"risk"']</t>
+    <t>['0.009*"’" + 0.007*"practice" + 0.006*"well" + 0.006*"needs" + 0.005*"need" + 0.005*"Redbridge" + 0.005*"effective" + 0.005*"ensure" + 0.005*"including" + 0.005*"risk"', '0.007*"well" + 0.007*"’" + 0.006*"practice" + 0.006*"need" + 0.006*"effective" + 0.006*"strong" + 0.005*"needs" + 0.005*"risk" + 0.005*"including" + 0.005*"Redbridge"', '0.007*"’" + 0.007*"practice" + 0.006*"needs" + 0.006*"well" + 0.005*"team" + 0.005*"Redbridge" + 0.005*"progress" + 0.005*"strong" + 0.005*"need" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2728,7 +2728,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.010*"well" + 0.010*"Richmond" + 0.007*"needs" + 0.006*"need" + 0.005*"team" + 0.005*"ensure" + 0.005*"Thames" + 0.004*"supported" + 0.004*"good"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"supported" + 0.006*"Richmond" + 0.006*"team" + 0.005*"need" + 0.005*"4" + 0.005*"additional" + 0.005*"31"', '0.016*"’" + 0.013*"well" + 0.008*"Richmond" + 0.007*"good" + 0.006*"needs" + 0.006*"supported" + 0.005*"team" + 0.005*"strong" + 0.005*"need" + 0.005*"4"']</t>
+    <t>['0.016*"’" + 0.011*"well" + 0.008*"Richmond" + 0.006*"need" + 0.006*"needs" + 0.006*"supported" + 0.006*"good" + 0.005*"team" + 0.005*"additional" + 0.005*"31"', '0.018*"’" + 0.013*"well" + 0.009*"needs" + 0.008*"Richmond" + 0.007*"team" + 0.006*"supported" + 0.006*"need" + 0.005*"ensure" + 0.005*"good" + 0.005*"strong"', '0.011*"’" + 0.007*"well" + 0.007*"Richmond" + 0.006*"supported" + 0.006*"needs" + 0.006*"good" + 0.004*"4" + 0.004*"team" + 0.004*"need" + 0.004*"Thames"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2758,7 +2758,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"Southwark" + 0.007*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"needs" + 0.005*"need" + 0.004*"progress" + 0.004*"strong" + 0.004*"30"', '0.020*"’" + 0.009*"good" + 0.008*"Southwark" + 0.008*"needs" + 0.007*"well" + 0.006*"Leaders" + 0.006*"strong" + 0.006*"need" + 0.005*"receive" + 0.005*"leaders"', '0.018*"’" + 0.011*"Southwark" + 0.008*"good" + 0.008*"well" + 0.007*"needs" + 0.007*"progress" + 0.007*"plans" + 0.006*"effective" + 0.005*"need" + 0.005*"leaders"']</t>
+    <t>['0.016*"’" + 0.007*"Southwark" + 0.006*"good" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"Leaders" + 0.005*"needs" + 0.005*"need" + 0.004*"strong"', '0.015*"’" + 0.009*"Southwark" + 0.007*"needs" + 0.007*"well" + 0.006*"good" + 0.005*"progress" + 0.005*"Leaders" + 0.005*"strong" + 0.005*"plans" + 0.005*"experiences"', '0.021*"’" + 0.010*"Southwark" + 0.009*"good" + 0.009*"well" + 0.008*"needs" + 0.007*"need" + 0.006*"progress" + 0.006*"receive" + 0.006*"plans" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2788,7 +2788,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"Sutton" + 0.004*"supported" + 0.004*"10" + 0.004*"protection" + 0.004*"progress" + 0.004*"6"', '0.021*"’" + 0.008*"well" + 0.006*"Sutton" + 0.006*"effective" + 0.005*"progress" + 0.005*"needs" + 0.005*"6" + 0.005*"receive" + 0.005*"leaders" + 0.005*"good"', '0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sutton" + 0.006*"progress" + 0.005*"receive" + 0.005*"effective" + 0.005*"good" + 0.004*"10" + 0.004*"supported"']</t>
+    <t>['0.017*"’" + 0.006*"Sutton" + 0.005*"well" + 0.005*"good" + 0.005*"needs" + 0.005*"progress" + 0.004*"10" + 0.004*"supported" + 0.004*"receive" + 0.004*"practice"', '0.018*"’" + 0.009*"well" + 0.006*"Sutton" + 0.006*"needs" + 0.005*"leaders" + 0.005*"6" + 0.005*"receive" + 0.005*"effective" + 0.005*"10" + 0.005*"need"', '0.014*"’" + 0.007*"needs" + 0.007*"progress" + 0.005*"well" + 0.005*"effective" + 0.005*"receive" + 0.005*"good" + 0.004*"Sutton" + 0.004*"supported" + 0.004*"‘"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2818,7 +2818,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"plans" + 0.007*"good" + 0.007*"effective" + 0.007*"well" + 0.006*"need" + 0.006*"‘" + 0.005*"practice" + 0.005*"needs" + 0.005*"early"', '0.012*"’" + 0.006*"practice" + 0.006*"good" + 0.005*"plans" + 0.005*"‘" + 0.005*"need" + 0.005*"well" + 0.005*"early" + 0.005*"effective" + 0.004*"including"', '0.012*"’" + 0.007*"good" + 0.006*"effective" + 0.006*"‘" + 0.005*"needs" + 0.005*"plans" + 0.005*"progress" + 0.004*"practice" + 0.004*"early" + 0.004*"well"']</t>
+    <t>['0.020*"’" + 0.007*"effective" + 0.007*"good" + 0.006*"well" + 0.006*"early" + 0.006*"plans" + 0.005*"‘" + 0.005*"progress" + 0.005*"carers" + 0.005*"risk"', '0.011*"’" + 0.007*"plans" + 0.007*"good" + 0.006*"practice" + 0.006*"‘" + 0.005*"effective" + 0.005*"need" + 0.005*"well" + 0.005*"progress" + 0.004*"needs"', '0.011*"’" + 0.006*"good" + 0.005*"plans" + 0.005*"‘" + 0.005*"need" + 0.005*"well" + 0.005*"effective" + 0.005*"practice" + 0.005*"including" + 0.004*"early"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2851,7 +2851,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.013*"well" + 0.011*"’" + 0.008*"needs" + 0.008*"good" + 0.006*"plans" + 0.006*"effective" + 0.006*"need" + 0.004*"appropriately" + 0.004*"progress" + 0.004*"planning"', '0.019*"’" + 0.012*"well" + 0.010*"needs" + 0.008*"good" + 0.008*"effective" + 0.006*"need" + 0.006*"risk" + 0.005*"plans" + 0.005*"timely" + 0.004*"protection"', '0.012*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"good" + 0.007*"effective" + 0.006*"need" + 0.005*"timely" + 0.005*"plans" + 0.004*"clear" + 0.004*"information"']</t>
+    <t>['0.016*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"effective" + 0.005*"plans" + 0.005*"good" + 0.005*"need" + 0.004*"timely" + 0.004*"risk" + 0.004*"clear"', '0.015*"’" + 0.013*"well" + 0.009*"needs" + 0.008*"good" + 0.008*"effective" + 0.005*"need" + 0.005*"timely" + 0.005*"plans" + 0.004*"practice" + 0.004*"protection"', '0.012*"’" + 0.011*"well" + 0.011*"good" + 0.008*"needs" + 0.007*"need" + 0.007*"effective" + 0.005*"plans" + 0.005*"risk" + 0.005*"timely" + 0.004*"information"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2878,7 +2878,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"7" + 0.006*"protection" + 0.005*"Senior" + 0.005*"ensure" + 0.005*"progress" + 0.005*"good" + 0.004*"Wandsworth"', '0.014*"’" + 0.007*"well" + 0.006*"practice" + 0.006*"progress" + 0.006*"Wandsworth" + 0.005*"needs" + 0.005*"team" + 0.005*"supported" + 0.005*"Senior" + 0.005*"effective"', '0.011*"’" + 0.006*"well" + 0.005*"progress" + 0.005*"effective" + 0.005*"Senior" + 0.005*"quality" + 0.005*"ensure" + 0.005*"needs" + 0.005*"protection" + 0.005*"Wandsworth"']</t>
+    <t>['0.009*"’" + 0.007*"well" + 0.006*"effective" + 0.006*"7" + 0.005*"supported" + 0.005*"needs" + 0.005*"ensure" + 0.005*"progress" + 0.005*"protection" + 0.005*"18"', '0.011*"’" + 0.006*"well" + 0.006*"progress" + 0.006*"needs" + 0.005*"protection" + 0.005*"practice" + 0.005*"However" + 0.005*"Wandsworth" + 0.005*"Senior" + 0.005*"team"', '0.014*"’" + 0.006*"Senior" + 0.006*"well" + 0.005*"Wandsworth" + 0.005*"quality" + 0.005*"progress" + 0.005*"practice" + 0.005*"needs" + 0.004*"receive" + 0.004*"improve"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2911,7 +2911,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"highly" + 0.005*"well" + 0.003*"high" + 0.003*"direct" + 0.003*"plans" + 0.003*"many" + 0.003*"supported"', '0.011*"’" + 0.007*"practice" + 0.006*"highly" + 0.006*"needs" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.004*"family" + 0.003*"shared" + 0.003*"high"', '0.015*"’" + 0.006*"practice" + 0.005*"highly" + 0.005*"needs" + 0.005*"well" + 0.004*"across" + 0.004*"family" + 0.004*"many" + 0.004*"skilled" + 0.003*"direct"']</t>
+    <t>['0.013*"’" + 0.007*"practice" + 0.005*"highly" + 0.005*"well" + 0.005*"needs" + 0.004*"many" + 0.004*"high" + 0.004*"across" + 0.004*"shared" + 0.003*"experiences"', '0.010*"’" + 0.007*"needs" + 0.006*"practice" + 0.006*"highly" + 0.005*"well" + 0.004*"family" + 0.004*"across" + 0.004*"many" + 0.003*"informed" + 0.003*"plans"', '0.014*"’" + 0.006*"practice" + 0.006*"highly" + 0.006*"needs" + 0.005*"well" + 0.004*"across" + 0.004*"plans" + 0.003*"Westminster" + 0.003*"interventions" + 0.003*"shared"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2944,7 +2944,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.006*"plans" + 0.006*"needs" + 0.006*"need" + 0.005*"good" + 0.005*"Luton" + 0.005*"leaders" + 0.005*"effective" + 0.004*"impact" + 0.004*"ensure"', '0.017*"’" + 0.007*"need" + 0.007*"needs" + 0.006*"Luton" + 0.006*"good" + 0.005*"effective" + 0.005*"ensure" + 0.005*"progress" + 0.005*"plans" + 0.005*"impact"', '0.015*"’" + 0.006*"plans" + 0.006*"need" + 0.006*"effective" + 0.005*"Luton" + 0.005*"needs" + 0.005*"quality" + 0.005*"impact" + 0.005*"progress" + 0.004*"receive"']</t>
+    <t>['0.012*"’" + 0.007*"need" + 0.006*"needs" + 0.005*"plans" + 0.005*"effective" + 0.005*"Luton" + 0.005*"quality" + 0.005*"receive" + 0.005*"ensure" + 0.004*"impact"', '0.022*"’" + 0.007*"plans" + 0.006*"need" + 0.006*"Luton" + 0.006*"good" + 0.006*"progress" + 0.005*"impact" + 0.005*"needs" + 0.005*"effective" + 0.005*"Leaders"', '0.016*"’" + 0.007*"needs" + 0.006*"need" + 0.006*"effective" + 0.005*"Luton" + 0.005*"well" + 0.005*"plans" + 0.005*"take" + 0.005*"quality" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2971,7 +2971,7 @@
     <t>19/05/22</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.013*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.006*"supported" + 0.006*"always" + 0.006*"education" + 0.006*"effective" + 0.006*"plans" + 0.005*"quality"', '0.016*"’" + 0.010*"needs" + 0.008*"Manchester" + 0.008*"supported" + 0.007*"well" + 0.006*"always" + 0.005*"21" + 0.005*"family" + 0.005*"education" + 0.005*"plans"', '0.020*"’" + 0.009*"needs" + 0.009*"Manchester" + 0.007*"always" + 0.006*"well" + 0.006*"protection" + 0.006*"effective" + 0.006*"plans" + 0.005*"supported" + 0.005*"progress"']</t>
+    <t>['0.024*"’" + 0.012*"Manchester" + 0.010*"needs" + 0.007*"well" + 0.007*"supported" + 0.006*"always" + 0.006*"plans" + 0.005*"disabled" + 0.005*"family" + 0.005*"protection"', '0.010*"’" + 0.008*"Manchester" + 0.006*"needs" + 0.005*"supported" + 0.004*"always" + 0.004*"well" + 0.004*"education" + 0.004*"1" + 0.004*"protection" + 0.004*"effective"', '0.024*"’" + 0.010*"Manchester" + 0.010*"needs" + 0.008*"always" + 0.007*"well" + 0.007*"supported" + 0.006*"quality" + 0.006*"plans" + 0.006*"education" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -3001,7 +3001,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"Medway" + 0.009*"well" + 0.008*"practice" + 0.008*"quality" + 0.007*"leaders" + 0.006*"oversight" + 0.006*"needs" + 0.005*"28" + 0.005*"experiences"', '0.013*"’" + 0.010*"Medway" + 0.009*"practice" + 0.008*"quality" + 0.008*"well" + 0.008*"needs" + 0.006*"oversight" + 0.006*"experiences" + 0.006*"impact" + 0.005*"17"', '0.012*"’" + 0.008*"Medway" + 0.006*"quality" + 0.006*"impact" + 0.005*"practice" + 0.005*"well" + 0.005*"leaders" + 0.005*"17" + 0.005*"needs" + 0.005*"risk"']</t>
+    <t>['0.016*"’" + 0.011*"Medway" + 0.008*"quality" + 0.008*"well" + 0.007*"oversight" + 0.007*"practice" + 0.006*"leaders" + 0.006*"needs" + 0.005*"progress" + 0.005*"experiences"', '0.017*"’" + 0.010*"practice" + 0.008*"well" + 0.008*"Medway" + 0.007*"leaders" + 0.006*"quality" + 0.006*"needs" + 0.006*"oversight" + 0.005*"good" + 0.005*"improve"', '0.014*"’" + 0.009*"quality" + 0.009*"Medway" + 0.007*"needs" + 0.007*"well" + 0.007*"impact" + 0.006*"practice" + 0.005*"leaders" + 0.005*"good" + 0.005*"clear"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -3025,7 +3025,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"effective" + 0.008*"plans" + 0.007*"Middlesbrough" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"place" + 0.005*"impact" + 0.005*"progress"', '0.013*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"effective" + 0.005*"needs" + 0.005*"Middlesbrough" + 0.005*"24" + 0.005*"progress" + 0.005*"practice" + 0.004*"place"', '0.014*"’" + 0.007*"well" + 0.007*"Middlesbrough" + 0.007*"needs" + 0.007*"effective" + 0.006*"plans" + 0.006*"practice" + 0.006*"progress" + 0.005*"13" + 0.005*"good"']</t>
+    <t>['0.013*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"Middlesbrough" + 0.007*"practice" + 0.006*"needs" + 0.005*"progress" + 0.005*"24" + 0.005*"effective" + 0.005*"means"', '0.015*"’" + 0.009*"effective" + 0.007*"Middlesbrough" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"progress" + 0.005*"13" + 0.005*"practice" + 0.005*"24"', '0.012*"’" + 0.007*"effective" + 0.006*"plans" + 0.006*"Middlesbrough" + 0.005*"needs" + 0.005*"practice" + 0.005*"progress" + 0.005*"place" + 0.004*"well" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -3052,7 +3052,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"need" + 0.006*"Milton" + 0.005*"well" + 0.005*"leaders" + 0.005*"practice" + 0.005*"plans" + 0.005*"also" + 0.004*"education" + 0.004*"good"', '0.016*"’" + 0.007*"Keynes" + 0.005*"well" + 0.005*"practice" + 0.005*"need" + 0.005*"25" + 0.005*"Milton" + 0.005*"plans" + 0.004*"2021" + 0.004*"5"', '0.014*"’" + 0.007*"Milton" + 0.007*"Keynes" + 0.006*"well" + 0.005*"leaders" + 0.005*"good" + 0.005*"need" + 0.005*"5" + 0.005*"impact" + 0.004*"25"']</t>
+    <t>['0.019*"’" + 0.007*"Milton" + 0.006*"Keynes" + 0.006*"need" + 0.006*"well" + 0.006*"practice" + 0.005*"25" + 0.005*"plans" + 0.005*"October" + 0.005*"family"', '0.012*"’" + 0.006*"well" + 0.005*"Milton" + 0.005*"needs" + 0.004*"need" + 0.004*"Keynes" + 0.004*"25" + 0.004*"leaders" + 0.004*"practice" + 0.004*"education"', '0.011*"’" + 0.006*"Keynes" + 0.005*"leaders" + 0.005*"well" + 0.005*"need" + 0.005*"good" + 0.005*"Milton" + 0.004*"plans" + 0.004*"practice" + 0.004*"carers"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -3079,7 +3079,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"plans" + 0.008*"needs" + 0.008*"well" + 0.007*"Newcastle" + 0.007*"good" + 0.006*"protection" + 0.006*"making" + 0.006*"response" + 0.006*"progress"', '0.012*"’" + 0.010*"plans" + 0.008*"Newcastle" + 0.007*"protection" + 0.007*"good" + 0.006*"needs" + 0.005*"progress" + 0.005*"need" + 0.005*"ensure" + 0.005*"10"', '0.019*"’" + 0.011*"plans" + 0.008*"needs" + 0.007*"protection" + 0.006*"good" + 0.006*"Newcastle" + 0.006*"ensure" + 0.006*"well" + 0.006*"management" + 0.005*"making"']</t>
+    <t>['0.012*"’" + 0.010*"plans" + 0.008*"good" + 0.008*"needs" + 0.007*"Newcastle" + 0.007*"making" + 0.006*"protection" + 0.005*"well" + 0.005*"management" + 0.005*"ensure"', '0.020*"’" + 0.010*"plans" + 0.008*"needs" + 0.007*"protection" + 0.007*"well" + 0.006*"good" + 0.006*"Newcastle" + 0.006*"ensure" + 0.006*"response" + 0.006*"right"', '0.014*"’" + 0.011*"plans" + 0.007*"progress" + 0.007*"Newcastle" + 0.007*"needs" + 0.007*"protection" + 0.007*"well" + 0.006*"good" + 0.005*"need" + 0.005*"management"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -3103,7 +3103,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"Norfolk" + 0.006*"well" + 0.005*"supported" + 0.005*"leaders" + 0.004*"carers" + 0.004*"needs" + 0.004*"range" + 0.004*"practice" + 0.003*"information"', '0.016*"’" + 0.008*"Norfolk" + 0.007*"carers" + 0.007*"well" + 0.006*"needs" + 0.005*"leaders" + 0.004*"7" + 0.004*"18" + 0.004*"range" + 0.004*"family"', '0.020*"’" + 0.010*"well" + 0.008*"Norfolk" + 0.008*"practice" + 0.006*"needs" + 0.006*"supported" + 0.006*"plans" + 0.006*"carers" + 0.005*"effective" + 0.005*"including"']</t>
+    <t>['0.008*"’" + 0.005*"Norfolk" + 0.005*"well" + 0.005*"supported" + 0.004*"practice" + 0.004*"needs" + 0.003*"18" + 0.003*"leaders" + 0.003*"carers" + 0.003*"including"', '0.017*"’" + 0.010*"well" + 0.008*"Norfolk" + 0.007*"carers" + 0.006*"supported" + 0.005*"needs" + 0.005*"practice" + 0.004*"18" + 0.004*"including" + 0.004*"leaders"', '0.020*"’" + 0.009*"Norfolk" + 0.008*"well" + 0.007*"needs" + 0.007*"practice" + 0.006*"carers" + 0.005*"plans" + 0.005*"information" + 0.005*"range" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -3136,7 +3136,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"practice" + 0.006*"risk" + 0.006*"leaders" + 0.006*"needs" + 0.006*"planning" + 0.005*"need" + 0.005*"East" + 0.004*"October" + 0.004*"quality"', '0.014*"’" + 0.007*"practice" + 0.007*"risk" + 0.006*"planning" + 0.005*"needs" + 0.005*"leaders" + 0.005*"Lincolnshire" + 0.005*"experiences" + 0.005*"2021" + 0.005*"North"', '0.014*"’" + 0.007*"practice" + 0.007*"leaders" + 0.007*"risk" + 0.006*"needs" + 0.006*"many" + 0.006*"planning" + 0.005*"need" + 0.005*"October" + 0.005*"plans"']</t>
+    <t>['0.018*"’" + 0.009*"practice" + 0.008*"risk" + 0.008*"leaders" + 0.007*"needs" + 0.006*"many" + 0.006*"planning" + 0.006*"Lincolnshire" + 0.005*"North" + 0.005*"plans"', '0.011*"’" + 0.007*"practice" + 0.005*"planning" + 0.005*"need" + 0.005*"needs" + 0.005*"leaders" + 0.005*"2021" + 0.005*"risk" + 0.004*"senior" + 0.004*"North"', '0.011*"’" + 0.007*"planning" + 0.007*"practice" + 0.006*"risk" + 0.006*"needs" + 0.006*"leaders" + 0.005*"need" + 0.005*"oversight" + 0.005*"quality" + 0.004*"Council"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -3166,7 +3166,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.028*"’" + 0.007*"‘" + 0.007*"family" + 0.007*"North" + 0.005*"10" + 0.005*"approach" + 0.005*"well" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"team"', '0.014*"’" + 0.007*"‘" + 0.006*"Lincolnshire" + 0.006*"family" + 0.005*"leaders" + 0.005*"approach" + 0.005*"protection" + 0.005*"well" + 0.004*"2022" + 0.004*"team"', '0.013*"’" + 0.007*"‘" + 0.006*"leaders" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"North" + 0.005*"well" + 0.004*"10" + 0.004*"family" + 0.004*"practice"']</t>
+    <t>['0.022*"’" + 0.009*"‘" + 0.006*"approach" + 0.006*"Lincolnshire" + 0.006*"family" + 0.006*"North" + 0.005*"well" + 0.005*"leaders" + 0.005*"10" + 0.005*"practice"', '0.016*"’" + 0.006*"family" + 0.006*"‘" + 0.005*"Lincolnshire" + 0.005*"need" + 0.005*"approach" + 0.005*"10" + 0.005*"14" + 0.004*"team" + 0.004*"needs"', '0.022*"’" + 0.006*"‘" + 0.006*"leaders" + 0.006*"North" + 0.006*"family" + 0.005*"well" + 0.005*"protection" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"14"']</t>
   </si>
   <si>
     <t>2637539</t>
@@ -3202,7 +3202,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"Northamptonshire" + 0.006*"well" + 0.006*"North" + 0.006*"needs" + 0.005*"quality" + 0.005*"Leaders" + 0.005*"3" + 0.005*"practice" + 0.005*"2022"', '0.015*"’" + 0.006*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.006*"quality" + 0.005*"NCT" + 0.005*"impact" + 0.005*"practice" + 0.004*"e" + 0.004*"14"', '0.015*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.005*"quality" + 0.005*"impact" + 0.005*"need" + 0.005*"plans" + 0.005*"practice" + 0.005*"Leaders"']</t>
+    <t>['0.016*"’" + 0.009*"Northamptonshire" + 0.006*"well" + 0.005*"impact" + 0.005*"NCT" + 0.005*"quality" + 0.005*"Leaders" + 0.004*"North" + 0.004*"need" + 0.004*"needs"', '0.018*"’" + 0.008*"North" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"well" + 0.005*"needs" + 0.005*"practice" + 0.005*"impact" + 0.005*"e" + 0.005*"home"', '0.016*"’" + 0.008*"Northamptonshire" + 0.006*"North" + 0.006*"well" + 0.005*"NCT" + 0.005*"practice" + 0.005*"quality" + 0.005*"need" + 0.005*"Leaders" + 0.005*"3"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -3229,7 +3229,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"needs" + 0.007*"quality" + 0.006*"North" + 0.006*"practice" + 0.006*"need" + 0.006*"always" + 0.006*"number" + 0.005*"Somerset" + 0.005*"well"', '0.016*"’" + 0.007*"quality" + 0.006*"progress" + 0.006*"needs" + 0.006*"always" + 0.005*"North" + 0.005*"number" + 0.005*"Somerset" + 0.005*"practice" + 0.005*"effective"', '0.017*"’" + 0.008*"quality" + 0.006*"Somerset" + 0.006*"always" + 0.005*"needs" + 0.005*"North" + 0.005*"risk" + 0.005*"practice" + 0.005*"number" + 0.005*"progress"']</t>
+    <t>['0.017*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"North" + 0.006*"well" + 0.006*"Somerset" + 0.005*"practice" + 0.005*"need" + 0.005*"always" + 0.005*"number"', '0.017*"’" + 0.009*"quality" + 0.008*"needs" + 0.006*"always" + 0.006*"number" + 0.006*"risk" + 0.006*"Somerset" + 0.006*"practice" + 0.005*"progress" + 0.005*"effective"', '0.015*"’" + 0.006*"quality" + 0.006*"always" + 0.006*"North" + 0.005*"needs" + 0.005*"Somerset" + 0.005*"need" + 0.005*"progress" + 0.005*"practice" + 0.005*"number"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -3256,7 +3256,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.006*"well" + 0.005*"leaders" + 0.005*"needs" + 0.005*"quality" + 0.004*"need" + 0.004*"make" + 0.004*"impact" + 0.003*"clear" + 0.003*"early"', '0.014*"’" + 0.007*"well" + 0.006*"need" + 0.005*"quality" + 0.005*"leaders" + 0.005*"needs" + 0.004*"make" + 0.004*"early" + 0.004*"foster" + 0.004*"family"', '0.015*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"make" + 0.005*"impact" + 0.004*"need" + 0.004*"understand" + 0.004*"early" + 0.004*"protection" + 0.004*"progress"']</t>
+    <t>['0.010*"’" + 0.007*"well" + 0.005*"leaders" + 0.005*"need" + 0.005*"make" + 0.004*"needs" + 0.004*"quality" + 0.004*"impact" + 0.004*"family" + 0.004*"understand"', '0.020*"’" + 0.006*"need" + 0.005*"make" + 0.005*"impact" + 0.004*"quality" + 0.004*"well" + 0.004*"clear" + 0.004*"protection" + 0.004*"needs" + 0.004*"good"', '0.016*"’" + 0.008*"well" + 0.007*"leaders" + 0.005*"quality" + 0.005*"need" + 0.004*"needs" + 0.004*"early" + 0.004*"make" + 0.004*"foster" + 0.003*"understand"']</t>
   </si>
   <si>
     <t>80530</t>
@@ -3286,7 +3286,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.006*"practice" + 0.006*"well" + 0.006*"North" + 0.006*"needs" + 0.005*"family" + 0.005*"‘" + 0.004*"Yorkshire" + 0.004*"7" + 0.004*"ensure"', '0.019*"’" + 0.008*"Yorkshire" + 0.008*"well" + 0.007*"North" + 0.006*"practice" + 0.006*"family" + 0.005*"needs" + 0.005*"2023" + 0.005*"‘" + 0.004*"3"', '0.022*"’" + 0.010*"well" + 0.006*"North" + 0.006*"practice" + 0.006*"Yorkshire" + 0.005*"family" + 0.005*"needs" + 0.005*"3" + 0.004*"‘" + 0.004*"July"']</t>
+    <t>['0.025*"’" + 0.010*"well" + 0.008*"Yorkshire" + 0.008*"practice" + 0.007*"North" + 0.006*"family" + 0.006*"needs" + 0.006*"‘" + 0.005*"3" + 0.005*"supported"', '0.019*"’" + 0.006*"North" + 0.006*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"Yorkshire" + 0.005*"family" + 0.005*"‘" + 0.004*"7" + 0.004*"need"', '0.012*"’" + 0.005*"well" + 0.005*"North" + 0.004*"family" + 0.004*"needs" + 0.004*"Yorkshire" + 0.004*"practice" + 0.003*"2023" + 0.003*"July" + 0.003*"effective"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -3313,7 +3313,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"good" + 0.005*"practice" + 0.004*"need" + 0.004*"impact" + 0.004*"experiences" + 0.004*"always" + 0.004*"education"', '0.025*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"good" + 0.007*"need" + 0.006*"experiences" + 0.005*"quality" + 0.005*"impact" + 0.005*"leaders" + 0.004*"education"', '0.024*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"good" + 0.007*"need" + 0.006*"practice" + 0.006*"impact" + 0.005*"education" + 0.005*"experiences" + 0.005*"quality"']</t>
+    <t>['0.024*"’" + 0.012*"needs" + 0.010*"well" + 0.009*"good" + 0.007*"need" + 0.006*"experiences" + 0.006*"practice" + 0.005*"impact" + 0.005*"education" + 0.005*"quality"', '0.020*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"need" + 0.005*"impact" + 0.005*"experiences" + 0.005*"good" + 0.005*"practice" + 0.004*"quality" + 0.004*"leaders"', '0.021*"’" + 0.011*"needs" + 0.009*"well" + 0.007*"good" + 0.005*"experiences" + 0.005*"need" + 0.005*"effective" + 0.005*"practice" + 0.005*"impact" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3343,7 +3343,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"impact" + 0.005*"effective" + 0.005*"risk" + 0.005*"oversight" + 0.005*"2022" + 0.005*"protection" + 0.005*"However"', '0.016*"’" + 0.009*"needs" + 0.008*"Nottingham" + 0.005*"effective" + 0.005*"11" + 0.005*"oversight" + 0.005*"City" + 0.004*"significant" + 0.004*"practice" + 0.004*"impact"', '0.012*"’" + 0.007*"needs" + 0.005*"effective" + 0.005*"City" + 0.005*"However" + 0.005*"plans" + 0.005*"Nottingham" + 0.004*"impact" + 0.004*"information" + 0.004*"good"']</t>
+    <t>['0.010*"’" + 0.008*"needs" + 0.007*"Nottingham" + 0.006*"effective" + 0.005*"11" + 0.005*"City" + 0.005*"impact" + 0.004*"2022" + 0.004*"plans" + 0.004*"practice"', '0.016*"’" + 0.010*"needs" + 0.006*"plans" + 0.006*"oversight" + 0.005*"effective" + 0.005*"Nottingham" + 0.005*"impact" + 0.004*"11" + 0.004*"However" + 0.004*"risk"', '0.015*"’" + 0.006*"plans" + 0.005*"needs" + 0.005*"Nottingham" + 0.005*"impact" + 0.005*"July" + 0.004*"practice" + 0.004*"City" + 0.004*"effective" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80534</t>
@@ -3367,7 +3367,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.010*"well" + 0.008*"practice" + 0.006*"receive" + 0.006*"needs" + 0.005*"ensure" + 0.005*"progress" + 0.005*"placements" + 0.005*"quality" + 0.005*"number"', '0.012*"’" + 0.009*"practice" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"progress" + 0.005*"ensure" + 0.005*"made" + 0.004*"carers" + 0.004*"receive"', '0.012*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"e" + 0.005*"quality" + 0.005*"receive" + 0.005*"areas" + 0.005*"needs" + 0.005*"plans" + 0.005*"made"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"needs" + 0.006*"e" + 0.005*"made" + 0.005*"progress" + 0.005*"receive" + 0.005*"number" + 0.005*"ensure"', '0.014*"’" + 0.008*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"plans" + 0.006*"receive" + 0.005*"ensure" + 0.005*"made" + 0.004*"e" + 0.004*"quality"', '0.012*"’" + 0.008*"practice" + 0.006*"quality" + 0.005*"well" + 0.005*"areas" + 0.005*"progress" + 0.005*"receive" + 0.005*"ensure" + 0.005*"carers" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3400,7 +3400,7 @@
     <t>04/03/19</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.012*"needs" + 0.010*"good" + 0.009*"practice" + 0.007*"well" + 0.007*"planning" + 0.006*"effective" + 0.006*"quality" + 0.006*"risk" + 0.006*"progress"', '0.009*"’" + 0.009*"good" + 0.009*"effective" + 0.008*"practice" + 0.007*"progress" + 0.007*"needs" + 0.007*"plans" + 0.006*"quality" + 0.005*"well" + 0.005*"information"', '0.010*"’" + 0.008*"effective" + 0.008*"practice" + 0.008*"good" + 0.007*"quality" + 0.007*"needs" + 0.006*"progress" + 0.006*"planning" + 0.006*"well" + 0.005*"plans"']</t>
+    <t>['0.011*"good" + 0.011*"needs" + 0.010*"’" + 0.008*"effective" + 0.008*"practice" + 0.007*"well" + 0.007*"quality" + 0.007*"plans" + 0.006*"planning" + 0.006*"progress"', '0.010*"’" + 0.009*"practice" + 0.007*"effective" + 0.007*"needs" + 0.007*"good" + 0.006*"well" + 0.006*"progress" + 0.005*"information" + 0.005*"quality" + 0.005*"risk"', '0.012*"’" + 0.009*"good" + 0.009*"practice" + 0.008*"needs" + 0.007*"progress" + 0.007*"effective" + 0.006*"planning" + 0.006*"quality" + 0.006*"plans" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3430,7 +3430,7 @@
     <t>0.1755</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"needs" + 0.007*"well" + 0.007*"Oxfordshire" + 0.005*"receive" + 0.005*"risk" + 0.005*"quality" + 0.005*"supported" + 0.005*"good" + 0.005*"education"', '0.020*"’" + 0.011*"needs" + 0.007*"Oxfordshire" + 0.007*"well" + 0.006*"risk" + 0.006*"leaders" + 0.005*"good" + 0.005*"12" + 0.005*"education" + 0.005*"supported"', '0.023*"’" + 0.008*"needs" + 0.007*"Oxfordshire" + 0.006*"supported" + 0.006*"good" + 0.006*"well" + 0.005*"risk" + 0.005*"arrangements" + 0.005*"practice" + 0.005*"12"']</t>
+    <t>['0.020*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"risk" + 0.006*"good" + 0.006*"supported" + 0.005*"progress" + 0.005*"12" + 0.005*"quality" + 0.005*"Oxfordshire"', '0.015*"’" + 0.009*"Oxfordshire" + 0.008*"needs" + 0.005*"23" + 0.005*"risk" + 0.005*"practice" + 0.005*"well" + 0.005*"receive" + 0.004*"good" + 0.004*"supported"', '0.022*"’" + 0.012*"needs" + 0.008*"Oxfordshire" + 0.007*"well" + 0.006*"supported" + 0.005*"risk" + 0.005*"good" + 0.005*"education" + 0.005*"receive" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3460,7 +3460,7 @@
     <t>30/01/24</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.013*"needs" + 0.007*"Peterborough" + 0.007*"need" + 0.007*"2023" + 0.007*"progress" + 0.006*"well" + 0.006*"supported" + 0.005*"plans" + 0.005*"27"', '0.016*"’" + 0.014*"needs" + 0.007*"need" + 0.007*"Peterborough" + 0.006*"well" + 0.006*"progress" + 0.006*"2023" + 0.006*"8" + 0.005*"good" + 0.005*"supported"', '0.012*"needs" + 0.011*"’" + 0.006*"need" + 0.006*"Peterborough" + 0.006*"2023" + 0.005*"plans" + 0.005*"well" + 0.005*"8" + 0.005*"receive" + 0.004*"27"']</t>
+    <t>['0.018*"’" + 0.013*"needs" + 0.008*"well" + 0.007*"need" + 0.007*"progress" + 0.007*"2023" + 0.007*"Peterborough" + 0.006*"8" + 0.005*"plans" + 0.005*"receive"', '0.014*"needs" + 0.013*"’" + 0.009*"Peterborough" + 0.008*"need" + 0.006*"2023" + 0.005*"supported" + 0.005*"27" + 0.005*"progress" + 0.005*"good" + 0.005*"well"', '0.012*"needs" + 0.011*"’" + 0.005*"2023" + 0.005*"well" + 0.005*"Peterborough" + 0.004*"December" + 0.004*"8" + 0.004*"plans" + 0.004*"supported" + 0.004*"27"']</t>
   </si>
   <si>
     <t>80538</t>
@@ -3490,7 +3490,7 @@
     <t>15/03/24</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.008*"Plymouth" + 0.007*"needs" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"risks" + 0.005*"Council" + 0.005*"education" + 0.005*"plans"', '0.013*"’" + 0.009*"needs" + 0.005*"Plymouth" + 0.005*"well" + 0.005*"practice" + 0.004*"education" + 0.004*"plans" + 0.004*"2024" + 0.004*"22" + 0.004*"January"', '0.010*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"Plymouth" + 0.005*"2" + 0.005*"practice" + 0.005*"appropriate" + 0.004*"quality" + 0.004*"January" + 0.004*"arrangements"']</t>
+    <t>['0.011*"’" + 0.009*"needs" + 0.006*"well" + 0.005*"Plymouth" + 0.005*"practice" + 0.004*"January" + 0.004*"February" + 0.004*"good" + 0.004*"plans" + 0.004*"leaders"', '0.011*"’" + 0.008*"needs" + 0.007*"Plymouth" + 0.007*"well" + 0.005*"22" + 0.005*"education" + 0.005*"2024" + 0.004*"appropriate" + 0.004*"plans" + 0.004*"City"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Plymouth" + 0.006*"practice" + 0.005*"2" + 0.005*"timely" + 0.005*"appropriate" + 0.005*"risks" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3523,7 +3523,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"well" + 0.008*"care-experienced" + 0.007*"needs" + 0.007*"Portsmouth" + 0.006*"family" + 0.005*"leaders" + 0.005*"health" + 0.005*"plans" + 0.004*"19"', '0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Portsmouth" + 0.007*"care-experienced" + 0.006*"family" + 0.005*"health" + 0.005*"plans" + 0.004*"practice" + 0.004*"need"', '0.020*"’" + 0.009*"care-experienced" + 0.006*"Portsmouth" + 0.006*"needs" + 0.006*"plans" + 0.005*"health" + 0.005*"progress" + 0.005*"well" + 0.005*"need" + 0.005*"risk"']</t>
+    <t>['0.017*"’" + 0.010*"care-experienced" + 0.008*"Portsmouth" + 0.007*"needs" + 0.006*"health" + 0.005*"family" + 0.005*"plans" + 0.005*"risk" + 0.005*"practice" + 0.005*"need"', '0.017*"’" + 0.010*"well" + 0.007*"care-experienced" + 0.006*"family" + 0.005*"needs" + 0.005*"Portsmouth" + 0.005*"practice" + 0.004*"health" + 0.004*"carers" + 0.004*"leaders"', '0.016*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"care-experienced" + 0.006*"plans" + 0.006*"Portsmouth" + 0.005*"family" + 0.004*"progress" + 0.004*"leaders" + 0.004*"May"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3559,7 +3559,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"number" + 0.007*"need" + 0.006*"quality" + 0.006*"plans" + 0.006*"good" + 0.005*"practice" + 0.005*"carers" + 0.004*"always"', '0.016*"’" + 0.008*"number" + 0.007*"plans" + 0.006*"well" + 0.005*"effective" + 0.005*"quality" + 0.005*"practice" + 0.005*"need" + 0.005*"good" + 0.004*"always"', '0.018*"’" + 0.008*"quality" + 0.006*"number" + 0.006*"timely" + 0.006*"well" + 0.006*"good" + 0.006*"However" + 0.006*"effective" + 0.005*"plans" + 0.005*"needs"']</t>
+    <t>['0.014*"’" + 0.009*"number" + 0.007*"plans" + 0.006*"well" + 0.006*"quality" + 0.005*"good" + 0.005*"need" + 0.004*"needs" + 0.004*"always" + 0.004*"timely"', '0.015*"’" + 0.006*"quality" + 0.005*"plans" + 0.005*"carers" + 0.005*"practice" + 0.005*"number" + 0.005*"need" + 0.005*"well" + 0.004*"needs" + 0.004*"ensure"', '0.017*"’" + 0.008*"quality" + 0.007*"well" + 0.007*"effective" + 0.007*"number" + 0.006*"good" + 0.005*"plans" + 0.005*"need" + 0.005*"However" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3583,7 +3583,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.005*"needs" + 0.005*"However" + 0.005*"consistently" + 0.005*"Redcar" + 0.004*"2022" + 0.004*"risk" + 0.004*"carers" + 0.004*"plans" + 0.004*"Cleveland"', '0.023*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"needs" + 0.006*"20" + 0.006*"However" + 0.005*"practice" + 0.005*"consistently" + 0.004*"oversight" + 0.004*"timely"', '0.015*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"consistently" + 0.006*"risk" + 0.005*"However" + 0.005*"practice" + 0.005*"2022" + 0.005*"needs" + 0.005*"Cleveland"']</t>
+    <t>['0.020*"’" + 0.006*"needs" + 0.006*"leaders" + 0.006*"consistently" + 0.005*"carers" + 0.005*"However" + 0.005*"plans" + 0.005*"Redcar" + 0.005*"20" + 0.004*"Cleveland"', '0.015*"’" + 0.006*"plans" + 0.006*"leaders" + 0.006*"needs" + 0.006*"However" + 0.005*"Redcar" + 0.005*"consistently" + 0.005*"2022" + 0.005*"20" + 0.005*"appropriate"', '0.017*"’" + 0.006*"leaders" + 0.006*"plans" + 0.006*"risk" + 0.006*"However" + 0.006*"practice" + 0.005*"consistently" + 0.005*"2022" + 0.005*"needs" + 0.005*"Cleveland"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3610,7 +3610,7 @@
     <t>17/03/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"experienced" + 0.007*"practice" + 0.007*"needs" + 0.005*"good" + 0.005*"consistently" + 0.005*"response" + 0.005*"plans" + 0.005*"quality" + 0.004*"well"', '0.015*"’" + 0.007*"experienced" + 0.007*"needs" + 0.006*"practice" + 0.006*"consistently" + 0.005*"quality" + 0.005*"well" + 0.005*"3" + 0.004*"Rochdale" + 0.004*"response"', '0.025*"’" + 0.011*"experienced" + 0.009*"practice" + 0.009*"needs" + 0.007*"plans" + 0.007*"response" + 0.006*"good" + 0.005*"Rochdale" + 0.005*"3" + 0.005*"quality"']</t>
+    <t>['0.020*"’" + 0.008*"needs" + 0.008*"practice" + 0.007*"experienced" + 0.006*"good" + 0.006*"plans" + 0.005*"quality" + 0.005*"response" + 0.005*"consistently" + 0.005*"well"', '0.019*"’" + 0.010*"experienced" + 0.008*"practice" + 0.007*"needs" + 0.006*"plans" + 0.006*"consistently" + 0.006*"Rochdale" + 0.005*"response" + 0.005*"well" + 0.005*"quality"', '0.022*"’" + 0.011*"experienced" + 0.008*"practice" + 0.007*"needs" + 0.007*"response" + 0.006*"3" + 0.005*"23" + 0.005*"plans" + 0.005*"quality" + 0.005*"consistently"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3637,7 +3637,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"Rotherham" + 0.007*"needs" + 0.006*"well" + 0.004*"Metropolitan" + 0.004*"good" + 0.004*"plans" + 0.004*"Council" + 0.004*"Borough" + 0.004*"However"', '0.012*"’" + 0.006*"Rotherham" + 0.005*"well" + 0.005*"good" + 0.005*"Council" + 0.004*"needs" + 0.004*"ensure" + 0.004*"However" + 0.004*"June" + 0.004*"improve"', '0.018*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"ensure" + 0.005*"good" + 0.005*"Council" + 0.005*"plans" + 0.005*"However" + 0.005*"well" + 0.004*"1"']</t>
+    <t>['0.015*"’" + 0.011*"Rotherham" + 0.007*"needs" + 0.006*"Council" + 0.005*"good" + 0.005*"However" + 0.005*"well" + 0.004*"ensure" + 0.004*"plans" + 0.004*"Borough"', '0.016*"’" + 0.007*"needs" + 0.006*"Rotherham" + 0.005*"ensure" + 0.005*"plans" + 0.004*"Metropolitan" + 0.004*"July" + 0.004*"Council" + 0.004*"well" + 0.004*"27"', '0.014*"’" + 0.008*"Rotherham" + 0.007*"well" + 0.006*"good" + 0.005*"However" + 0.004*"needs" + 0.004*"plans" + 0.004*"ensure" + 0.004*"Council" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3664,7 +3664,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.016*"well" + 0.013*"practice" + 0.012*"’" + 0.009*"highly" + 0.007*"strong" + 0.006*"effective" + 0.006*"leaders" + 0.006*"needs" + 0.005*"need" + 0.005*"range"', '0.013*"well" + 0.009*"’" + 0.008*"practice" + 0.006*"needs" + 0.006*"highly" + 0.005*"strong" + 0.004*"effective" + 0.004*"high" + 0.004*"leaders" + 0.004*"risk"', '0.012*"’" + 0.010*"well" + 0.008*"practice" + 0.005*"highly" + 0.005*"strong" + 0.005*"needs" + 0.005*"high" + 0.004*"effective" + 0.004*"leaders" + 0.004*"progress"']</t>
+    <t>['0.015*"well" + 0.012*"’" + 0.011*"practice" + 0.008*"highly" + 0.006*"needs" + 0.005*"strong" + 0.004*"range" + 0.004*"effective" + 0.004*"professionals" + 0.004*"high"', '0.012*"well" + 0.011*"’" + 0.009*"practice" + 0.008*"strong" + 0.006*"highly" + 0.006*"leaders" + 0.006*"needs" + 0.005*"effective" + 0.004*"professionals" + 0.004*"improve"', '0.014*"well" + 0.011*"’" + 0.011*"practice" + 0.007*"highly" + 0.006*"strong" + 0.006*"effective" + 0.005*"high" + 0.005*"needs" + 0.005*"leaders" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3694,7 +3694,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"plans" + 0.007*"well" + 0.007*"needs" + 0.005*"supported" + 0.004*"good" + 0.004*"information" + 0.004*"understand" + 0.004*"appropriate" + 0.004*"effective"', '0.015*"’" + 0.011*"well" + 0.009*"plans" + 0.008*"needs" + 0.006*"good" + 0.005*"clear" + 0.005*"effective" + 0.005*"need" + 0.004*"practice" + 0.004*"progress"', '0.014*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"needs" + 0.005*"risk" + 0.004*"good" + 0.004*"practice" + 0.004*"effective" + 0.004*"need" + 0.004*"Kingston"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.005*"good" + 0.005*"effective" + 0.005*"clear" + 0.005*"risk" + 0.004*"progress" + 0.004*"Kingston"', '0.011*"’" + 0.009*"plans" + 0.008*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"practice" + 0.005*"good" + 0.004*"appropriate" + 0.004*"supported" + 0.004*"need"', '0.012*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.005*"good" + 0.005*"need" + 0.005*"parents" + 0.004*"clear" + 0.004*"practice" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3724,7 +3724,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.005*"quality" + 0.004*"well" + 0.004*"benefit" + 0.004*"use" + 0.004*"good" + 0.003*"needs" + 0.003*"plans" + 0.003*"actions" + 0.003*"information"', '0.008*"’" + 0.006*"well" + 0.004*"needs" + 0.004*"informed" + 0.004*"plans" + 0.004*"information" + 0.004*"timely" + 0.004*"quality" + 0.004*"effective" + 0.004*"risk"', '0.016*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"quality" + 0.005*"effective" + 0.004*"always" + 0.004*"actions" + 0.004*"benefit" + 0.004*"However"']</t>
+    <t>['0.008*"’" + 0.005*"well" + 0.004*"plans" + 0.004*"quality" + 0.004*"actions" + 0.004*"always" + 0.004*"management" + 0.003*"needs" + 0.003*"need" + 0.003*"timely"', '0.011*"’" + 0.006*"quality" + 0.005*"needs" + 0.005*"well" + 0.004*"plans" + 0.004*"effective" + 0.004*"information" + 0.004*"However" + 0.004*"benefit" + 0.004*"early"', '0.014*"’" + 0.006*"well" + 0.005*"needs" + 0.005*"use" + 0.004*"plans" + 0.004*"benefit" + 0.004*"health" + 0.004*"quality" + 0.004*"information" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3748,7 +3748,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"protection" + 0.006*"team" + 0.005*"plans" + 0.005*"practice" + 0.005*"ensure"', '0.011*"’" + 0.009*"well" + 0.009*"needs" + 0.008*"good" + 0.007*"need" + 0.006*"protection" + 0.006*"practice" + 0.006*"effective" + 0.006*"team" + 0.005*"plans"', '0.016*"’" + 0.011*"well" + 0.010*"needs" + 0.007*"team" + 0.007*"practice" + 0.007*"good" + 0.006*"need" + 0.006*"ensure" + 0.006*"enough" + 0.006*"effective"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.007*"good" + 0.007*"need" + 0.007*"plans" + 0.007*"team" + 0.006*"needs" + 0.005*"effective" + 0.005*"enough" + 0.005*"ensure"', '0.013*"’" + 0.012*"well" + 0.011*"needs" + 0.007*"practice" + 0.007*"team" + 0.007*"good" + 0.006*"need" + 0.006*"enough" + 0.006*"effective" + 0.005*"protection"', '0.013*"’" + 0.009*"needs" + 0.008*"good" + 0.008*"well" + 0.006*"protection" + 0.006*"need" + 0.006*"ensure" + 0.006*"practice" + 0.005*"team" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3775,7 +3775,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"effective" + 0.006*"plans" + 0.006*"practice" + 0.005*"leaders" + 0.005*"Salford" + 0.005*"experiences" + 0.004*"Council"', '0.013*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"effective" + 0.007*"needs" + 0.005*"planning" + 0.005*"10" + 0.005*"quality" + 0.005*"Salford" + 0.004*"6"', '0.014*"’" + 0.009*"plans" + 0.007*"Salford" + 0.007*"needs" + 0.006*"well" + 0.006*"effective" + 0.005*"planning" + 0.005*"practice" + 0.005*"appropriate" + 0.005*"leaders"']</t>
+    <t>['0.011*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"plans" + 0.007*"effective" + 0.005*"Salford" + 0.004*"leaders" + 0.004*"means" + 0.004*"Council" + 0.004*"planning"', '0.014*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"effective" + 0.005*"Salford" + 0.005*"2023" + 0.005*"leaders" + 0.004*"quality"', '0.015*"’" + 0.008*"plans" + 0.008*"needs" + 0.008*"well" + 0.007*"effective" + 0.006*"Salford" + 0.006*"planning" + 0.005*"practice" + 0.005*"10" + 0.005*"6"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3799,7 +3799,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.010*"needs" + 0.008*"Sandwell" + 0.008*"plans" + 0.007*"well" + 0.005*"quality" + 0.005*"progress" + 0.005*"effective" + 0.005*"many" + 0.005*"Trust"', '0.015*"’" + 0.007*"plans" + 0.007*"Sandwell" + 0.007*"needs" + 0.006*"quality" + 0.005*"well" + 0.005*"20" + 0.005*"changes" + 0.005*"Trust" + 0.004*"progress"', '0.013*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sandwell" + 0.005*"plans" + 0.005*"education" + 0.005*"quality" + 0.005*"good" + 0.004*"Trust" + 0.004*"9"']</t>
+    <t>['0.008*"’" + 0.007*"plans" + 0.007*"Sandwell" + 0.007*"needs" + 0.006*"quality" + 0.005*"well" + 0.005*"education" + 0.004*"number" + 0.004*"progress" + 0.004*"Trust"', '0.007*"’" + 0.006*"Sandwell" + 0.006*"needs" + 0.005*"well" + 0.004*"quality" + 0.004*"education" + 0.004*"practice" + 0.004*"9" + 0.004*"many" + 0.004*"changes"', '0.020*"’" + 0.009*"needs" + 0.008*"plans" + 0.008*"well" + 0.008*"Sandwell" + 0.006*"quality" + 0.005*"Trust" + 0.005*"20" + 0.005*"number" + 0.005*"9"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3823,7 +3823,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"needs" + 0.007*"oversight" + 0.004*"practice" + 0.004*"including" + 0.004*"protection" + 0.004*"plans" + 0.004*"lack" + 0.004*"many" + 0.004*"identified"', '0.016*"’" + 0.008*"needs" + 0.006*"practice" + 0.005*"protection" + 0.005*"lack" + 0.005*"many" + 0.005*"always" + 0.005*"timely" + 0.005*"oversight" + 0.005*"Sefton"', '0.017*"’" + 0.012*"needs" + 0.007*"practice" + 0.006*"◼" + 0.005*"4" + 0.005*"management" + 0.005*"oversight" + 0.005*"including" + 0.005*"March" + 0.005*"lack"']</t>
+    <t>['0.018*"’" + 0.011*"needs" + 0.008*"practice" + 0.006*"oversight" + 0.005*"management" + 0.005*"including" + 0.005*"protection" + 0.005*"◼" + 0.005*"timely" + 0.005*"many"', '0.014*"’" + 0.008*"needs" + 0.005*"including" + 0.005*"lack" + 0.005*"practice" + 0.005*"management" + 0.005*"oversight" + 0.004*"protection" + 0.004*"result" + 0.004*"always"', '0.015*"’" + 0.009*"needs" + 0.006*"oversight" + 0.005*"lack" + 0.005*"Sefton" + 0.005*"21" + 0.005*"practice" + 0.005*"many" + 0.005*"protection" + 0.005*"March"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3856,7 +3856,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.013*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.007*"leaders" + 0.006*"health" + 0.006*"practice" + 0.005*"quality" + 0.005*"plans" + 0.005*"effective"', '0.022*"’" + 0.009*"Sheffield" + 0.007*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"leaders" + 0.005*"quality" + 0.004*"good" + 0.004*"adviser" + 0.004*"health"', '0.016*"’" + 0.009*"Sheffield" + 0.007*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"health" + 0.004*"leaders" + 0.004*"22" + 0.004*"experiences" + 0.004*"11"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.008*"Sheffield" + 0.008*"well" + 0.006*"practice" + 0.006*"leaders" + 0.005*"health" + 0.004*"quality" + 0.004*"plans" + 0.004*"adviser"', '0.025*"’" + 0.013*"Sheffield" + 0.008*"needs" + 0.006*"leaders" + 0.005*"practice" + 0.005*"quality" + 0.005*"well" + 0.005*"health" + 0.004*"effective" + 0.004*"ensure"', '0.021*"’" + 0.011*"Sheffield" + 0.009*"needs" + 0.007*"well" + 0.006*"health" + 0.006*"practice" + 0.005*"11" + 0.005*"experiences" + 0.005*"receive" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3886,7 +3886,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.005*"well" + 0.004*"progress" + 0.004*"Shropshire" + 0.004*"plans" + 0.004*"making" + 0.004*"leaders" + 0.004*"2022" + 0.004*"make"', '0.015*"’" + 0.009*"needs" + 0.008*"Shropshire" + 0.006*"well" + 0.005*"plans" + 0.005*"2022" + 0.005*"making" + 0.004*"leaders" + 0.004*"progress" + 0.004*"7"', '0.019*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.007*"progress" + 0.006*"plans" + 0.005*"making" + 0.005*"7" + 0.005*"2022" + 0.005*"training"']</t>
+    <t>['0.019*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Shropshire" + 0.006*"progress" + 0.005*"2022" + 0.005*"plans" + 0.005*"11" + 0.005*"training" + 0.005*"7"', '0.017*"’" + 0.008*"needs" + 0.008*"Shropshire" + 0.006*"well" + 0.005*"plans" + 0.005*"making" + 0.005*"practice" + 0.005*"progress" + 0.005*"7" + 0.005*"leaders"', '0.015*"’" + 0.009*"needs" + 0.006*"progress" + 0.006*"well" + 0.006*"Shropshire" + 0.005*"plans" + 0.005*"2022" + 0.005*"making" + 0.004*"effectively" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3910,7 +3910,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Slough" + 0.007*"quality" + 0.007*"plans" + 0.006*"needs" + 0.006*"3" + 0.006*"practice" + 0.005*"leaders" + 0.005*"impact" + 0.005*"However"', '0.021*"’" + 0.008*"Slough" + 0.006*"practice" + 0.006*"quality" + 0.006*"plans" + 0.006*"needs" + 0.006*"leaders" + 0.005*"supported" + 0.005*"planning" + 0.004*"However"', '0.012*"’" + 0.007*"Slough" + 0.007*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"impact" + 0.005*"quality" + 0.005*"practice" + 0.004*"time" + 0.004*"January"']</t>
+    <t>['0.011*"’" + 0.007*"Slough" + 0.005*"practice" + 0.005*"needs" + 0.005*"quality" + 0.004*"3" + 0.004*"plans" + 0.004*"23" + 0.004*"impact" + 0.004*"senior"', '0.020*"’" + 0.007*"Slough" + 0.007*"plans" + 0.007*"needs" + 0.007*"quality" + 0.006*"3" + 0.005*"leaders" + 0.005*"However" + 0.005*"supported" + 0.005*"impact"', '0.013*"’" + 0.009*"Slough" + 0.007*"practice" + 0.006*"plans" + 0.006*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"impact" + 0.004*"leaders" + 0.004*"planning"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3934,7 +3934,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"lack" + 0.011*"2022" + 0.008*"quality" + 0.007*"risk" + 0.007*"Solihull" + 0.006*"need" + 0.005*"practice" + 0.005*"experiences" + 0.005*"effective"', '0.017*"’" + 0.009*"lack" + 0.007*"2022" + 0.006*"need" + 0.006*"Solihull" + 0.005*"means" + 0.005*"experiences" + 0.005*"progress" + 0.005*"risk" + 0.005*"practice"', '0.013*"’" + 0.009*"lack" + 0.006*"2022" + 0.006*"significant" + 0.005*"Solihull" + 0.005*"risk" + 0.005*"effective" + 0.005*"practice" + 0.005*"need" + 0.005*"plans"']</t>
+    <t>['0.017*"’" + 0.012*"lack" + 0.008*"2022" + 0.006*"risk" + 0.006*"need" + 0.006*"Solihull" + 0.005*"experiences" + 0.005*"quality" + 0.005*"significant" + 0.005*"timely"', '0.012*"’" + 0.009*"lack" + 0.008*"2022" + 0.006*"need" + 0.005*"practice" + 0.005*"quality" + 0.005*"significant" + 0.005*"means" + 0.004*"delay" + 0.004*"effective"', '0.016*"’" + 0.010*"lack" + 0.009*"2022" + 0.007*"Solihull" + 0.006*"need" + 0.006*"risk" + 0.006*"quality" + 0.005*"practice" + 0.005*"effective" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3958,7 +3958,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.006*"plans" + 0.006*"good" + 0.006*"Somerset" + 0.006*"supported" + 0.005*"family" + 0.005*"progress" + 0.005*"including"', '0.022*"’" + 0.009*"well" + 0.007*"Somerset" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.005*"leaders" + 0.005*"including" + 0.005*"number" + 0.005*"practice"', '0.013*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Somerset" + 0.006*"plans" + 0.006*"supported" + 0.005*"number" + 0.005*"good" + 0.005*"need" + 0.005*"leaders"']</t>
+    <t>['0.019*"’" + 0.012*"well" + 0.010*"needs" + 0.008*"plans" + 0.007*"Somerset" + 0.006*"leaders" + 0.006*"practice" + 0.006*"good" + 0.006*"supported" + 0.006*"need"', '0.015*"’" + 0.007*"Somerset" + 0.005*"good" + 0.005*"well" + 0.005*"needs" + 0.005*"including" + 0.004*"need" + 0.004*"plans" + 0.004*"29" + 0.004*"July"', '0.016*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"Somerset" + 0.005*"progress" + 0.005*"good" + 0.005*"supported" + 0.005*"leaders" + 0.004*"plans" + 0.004*"including"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3982,7 +3982,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.009*"quality" + 0.008*"well" + 0.007*"’" + 0.007*"plans" + 0.005*"leaders" + 0.005*"progress" + 0.005*"good" + 0.004*"timely" + 0.004*"arrangements" + 0.004*"always"', '0.010*"well" + 0.010*"quality" + 0.009*"’" + 0.008*"good" + 0.007*"leaders" + 0.007*"plans" + 0.007*"needs" + 0.005*"progress" + 0.005*"timely" + 0.005*"arrangements"', '0.013*"well" + 0.011*"quality" + 0.010*"leaders" + 0.009*"’" + 0.008*"plans" + 0.007*"timely" + 0.007*"good" + 0.006*"needs" + 0.005*"progress" + 0.005*"timeliness"']</t>
+    <t>['0.009*"quality" + 0.009*"well" + 0.008*"leaders" + 0.008*"’" + 0.007*"plans" + 0.007*"good" + 0.006*"timely" + 0.005*"progress" + 0.005*"practice" + 0.005*"needs"', '0.011*"well" + 0.010*"quality" + 0.009*"’" + 0.008*"leaders" + 0.007*"plans" + 0.006*"good" + 0.006*"timely" + 0.006*"◼" + 0.005*"needs" + 0.005*"progress"', '0.012*"well" + 0.011*"quality" + 0.009*"’" + 0.008*"leaders" + 0.008*"plans" + 0.007*"good" + 0.006*"needs" + 0.006*"timely" + 0.005*"progress" + 0.005*"South"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -4015,7 +4015,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"needs" + 0.008*"Tyneside" + 0.007*"South" + 0.005*"carers" + 0.005*"2022" + 0.005*"effective" + 0.005*"2023" + 0.005*"5" + 0.004*"However"', '0.021*"’" + 0.008*"needs" + 0.007*"South" + 0.007*"Tyneside" + 0.006*"oversight" + 0.005*"practice" + 0.005*"management" + 0.005*"effective" + 0.005*"carers" + 0.004*"2022"', '0.029*"’" + 0.009*"needs" + 0.008*"South" + 0.008*"Tyneside" + 0.005*"However" + 0.005*"14" + 0.005*"risk" + 0.005*"oversight" + 0.005*"management" + 0.005*"effective"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.009*"South" + 0.007*"Tyneside" + 0.005*"management" + 0.005*"9" + 0.005*"However" + 0.005*"oversight" + 0.005*"risk" + 0.005*"living"', '0.024*"’" + 0.010*"needs" + 0.007*"South" + 0.006*"Tyneside" + 0.005*"carers" + 0.005*"15" + 0.005*"practice" + 0.005*"effective" + 0.005*"However" + 0.004*"oversight"', '0.029*"’" + 0.008*"Tyneside" + 0.008*"needs" + 0.006*"oversight" + 0.006*"effective" + 0.006*"South" + 0.005*"management" + 0.005*"However" + 0.005*"9" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -4045,7 +4045,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.005*"plans" + 0.005*"improve" + 0.005*"Southampton" + 0.005*"5" + 0.005*"experiences" + 0.005*"progress" + 0.004*"including" + 0.004*"provide" + 0.004*"needs"', '0.017*"’" + 0.006*"Southampton" + 0.005*"plans" + 0.005*"improve" + 0.005*"including" + 0.005*"needs" + 0.005*"progress" + 0.004*"make" + 0.004*"timely" + 0.004*"5"', '0.016*"’" + 0.007*"plans" + 0.006*"Southampton" + 0.005*"June" + 0.004*"progress" + 0.004*"16" + 0.004*"experiences" + 0.004*"well" + 0.004*"effective" + 0.004*"needs"']</t>
+    <t>['0.015*"’" + 0.006*"Southampton" + 0.005*"improve" + 0.005*"plans" + 0.005*"including" + 0.004*"5" + 0.004*"experiences" + 0.004*"provide" + 0.004*"progress" + 0.003*"June"', '0.017*"’" + 0.006*"Southampton" + 0.006*"plans" + 0.005*"needs" + 0.005*"16" + 0.005*"including" + 0.005*"provide" + 0.004*"well" + 0.004*"5" + 0.004*"progress"', '0.016*"’" + 0.007*"plans" + 0.006*"progress" + 0.005*"improve" + 0.005*"Southampton" + 0.004*"needs" + 0.004*"2023" + 0.004*"5" + 0.004*"timely" + 0.004*"16"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -4081,7 +4081,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"planning" + 0.007*"quality" + 0.007*"practice" + 0.006*"leaders" + 0.006*"protection" + 0.005*"number" + 0.005*"always" + 0.005*"effective" + 0.005*"needs"', '0.015*"’" + 0.009*"planning" + 0.006*"quality" + 0.006*"practice" + 0.006*"leaders" + 0.005*"carers" + 0.005*"number" + 0.005*"effective" + 0.005*"need" + 0.005*"within"', '0.012*"’" + 0.008*"practice" + 0.007*"planning" + 0.007*"quality" + 0.006*"protection" + 0.005*"leaders" + 0.005*"always" + 0.005*"need" + 0.005*"risk" + 0.005*"plans"']</t>
+    <t>['0.013*"’" + 0.010*"planning" + 0.007*"leaders" + 0.007*"quality" + 0.006*"practice" + 0.006*"always" + 0.006*"number" + 0.005*"protection" + 0.005*"needs" + 0.005*"good"', '0.016*"’" + 0.008*"practice" + 0.006*"quality" + 0.006*"within" + 0.006*"leaders" + 0.006*"planning" + 0.006*"number" + 0.006*"effective" + 0.006*"need" + 0.005*"carers"', '0.009*"’" + 0.007*"planning" + 0.006*"quality" + 0.006*"practice" + 0.005*"protection" + 0.004*"effective" + 0.004*"within" + 0.004*"risk" + 0.004*"However" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -4102,7 +4102,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"Helens" + 0.009*"needs" + 0.008*"St" + 0.008*"well" + 0.006*"good" + 0.006*"progress" + 0.006*"risk" + 0.006*"need" + 0.006*"receive"', '0.017*"’" + 0.008*"St" + 0.007*"Helens" + 0.006*"progress" + 0.006*"21" + 0.006*"needs" + 0.005*"well" + 0.005*"10" + 0.005*"receive" + 0.005*"need"', '0.010*"’" + 0.006*"Helens" + 0.005*"St" + 0.005*"well" + 0.005*"10" + 0.005*"needs" + 0.004*"receive" + 0.004*"need" + 0.004*"risk" + 0.004*"effective"']</t>
+    <t>['0.017*"’" + 0.008*"Helens" + 0.007*"St" + 0.007*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"need" + 0.005*"21" + 0.005*"good" + 0.005*"risk"', '0.016*"’" + 0.009*"Helens" + 0.008*"needs" + 0.008*"St" + 0.007*"receive" + 0.006*"well" + 0.006*"risk" + 0.006*"10" + 0.006*"progress" + 0.006*"21"', '0.014*"’" + 0.008*"St" + 0.007*"needs" + 0.006*"well" + 0.006*"Helens" + 0.006*"10" + 0.006*"need" + 0.006*"progress" + 0.005*"good" + 0.005*"21"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -4126,7 +4126,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"needs" + 0.006*"quality" + 0.005*"oversight" + 0.005*"ensure" + 0.005*"plans" + 0.005*"practice" + 0.004*"health" + 0.004*"progress" + 0.004*"good"', '0.019*"’" + 0.013*"needs" + 0.007*"progress" + 0.006*"Staffordshire" + 0.006*"oversight" + 0.006*"quality" + 0.005*"practice" + 0.005*"ensure" + 0.005*"health" + 0.005*"impact"', '0.015*"’" + 0.011*"needs" + 0.006*"practice" + 0.006*"health" + 0.006*"quality" + 0.006*"progress" + 0.005*"Staffordshire" + 0.005*"10" + 0.005*"ensure" + 0.005*"oversight"']</t>
+    <t>['0.016*"’" + 0.010*"needs" + 0.006*"progress" + 0.006*"quality" + 0.005*"ensure" + 0.005*"health" + 0.005*"plans" + 0.005*"practice" + 0.005*"oversight" + 0.004*"Staffordshire"', '0.017*"’" + 0.011*"needs" + 0.007*"practice" + 0.007*"progress" + 0.006*"quality" + 0.006*"oversight" + 0.005*"Staffordshire" + 0.005*"ensure" + 0.005*"health" + 0.004*"risk"', '0.018*"’" + 0.013*"needs" + 0.006*"oversight" + 0.006*"Staffordshire" + 0.006*"health" + 0.006*"quality" + 0.005*"ensure" + 0.005*"plans" + 0.005*"practice" + 0.005*"10"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -4156,7 +4156,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"Stockport" + 0.006*"ensure" + 0.005*"strong" + 0.005*"risk" + 0.005*"need" + 0.005*"plans"', '0.012*"’" + 0.008*"Stockport" + 0.007*"practice" + 0.007*"well" + 0.006*"needs" + 0.006*"risk" + 0.005*"strong" + 0.005*"plans" + 0.005*"leaders" + 0.005*"March"', '0.011*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"Stockport" + 0.006*"plans" + 0.005*"strong" + 0.005*"needs" + 0.004*"quality" + 0.004*"28" + 0.004*"range"']</t>
+    <t>['0.010*"’" + 0.008*"practice" + 0.008*"well" + 0.007*"needs" + 0.006*"Stockport" + 0.005*"strong" + 0.005*"plans" + 0.005*"risk" + 0.005*"28" + 0.004*"quality"', '0.010*"’" + 0.009*"well" + 0.007*"practice" + 0.007*"Stockport" + 0.006*"plans" + 0.006*"strong" + 0.005*"risk" + 0.005*"ensure" + 0.005*"needs" + 0.005*"leaders"', '0.014*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Stockport" + 0.005*"practice" + 0.005*"strong" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"April" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -4192,7 +4192,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"leaders" + 0.006*"good" + 0.006*"needs" + 0.006*"on-Tees" + 0.005*"quality" + 0.005*"Stockton" + 0.005*"carers"', '0.018*"’" + 0.012*"leaders" + 0.011*"plans" + 0.007*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"Stockton" + 0.005*"on-Tees" + 0.005*"good" + 0.005*"senior"', '0.024*"’" + 0.006*"leaders" + 0.006*"needs" + 0.006*"plans" + 0.006*"on-Tees" + 0.006*"Stockton" + 0.006*"well" + 0.005*"quality" + 0.005*"senior" + 0.005*"17"']</t>
+    <t>['0.022*"’" + 0.010*"leaders" + 0.008*"plans" + 0.007*"well" + 0.006*"on-Tees" + 0.006*"needs" + 0.006*"quality" + 0.005*"senior" + 0.005*"Stockton" + 0.005*"March"', '0.020*"’" + 0.009*"plans" + 0.008*"leaders" + 0.008*"needs" + 0.007*"well" + 0.007*"good" + 0.007*"Stockton" + 0.006*"quality" + 0.006*"on-Tees" + 0.006*"carers"', '0.013*"’" + 0.007*"leaders" + 0.006*"plans" + 0.005*"quality" + 0.005*"Stockton" + 0.005*"well" + 0.004*"on-Tees" + 0.004*"good" + 0.004*"needs" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -4216,7 +4216,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"However" + 0.007*"needs" + 0.006*"on-Trent" + 0.006*"well" + 0.006*"plans" + 0.005*"Stoke" + 0.005*"protection" + 0.005*"3" + 0.005*"ensure"', '0.018*"’" + 0.009*"needs" + 0.007*"on-Trent" + 0.007*"Stoke" + 0.007*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"ensure" + 0.005*"However" + 0.005*"protection"', '0.017*"’" + 0.009*"needs" + 0.008*"Stoke" + 0.007*"well" + 0.007*"on-Trent" + 0.007*"plans" + 0.006*"However" + 0.006*"protection" + 0.006*"ensure" + 0.005*"progress"']</t>
+    <t>['0.016*"’" + 0.010*"needs" + 0.009*"on-Trent" + 0.007*"Stoke" + 0.007*"However" + 0.007*"ensure" + 0.006*"well" + 0.006*"plans" + 0.005*"protection" + 0.005*"progress"', '0.021*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"needs" + 0.007*"Stoke" + 0.006*"However" + 0.006*"protection" + 0.006*"ensure" + 0.005*"on-Trent" + 0.005*"progress"', '0.013*"’" + 0.008*"needs" + 0.006*"However" + 0.006*"Stoke" + 0.006*"plans" + 0.006*"well" + 0.006*"on-Trent" + 0.006*"protection" + 0.005*"need" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -4246,7 +4246,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"good" + 0.005*"well" + 0.004*"progress" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"effective" + 0.004*"high" + 0.004*"needs" + 0.003*"experiences"', '0.013*"’" + 0.006*"well" + 0.006*"effective" + 0.005*"progress" + 0.005*"practice" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"carers" + 0.004*"needs" + 0.004*"good"', '0.015*"’" + 0.008*"progress" + 0.007*"well" + 0.005*"leaders" + 0.005*"good" + 0.005*"effective" + 0.004*"ensure" + 0.004*"Suffolk" + 0.004*"needs" + 0.004*"practice"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.006*"progress" + 0.004*"good" + 0.004*"practice" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"high" + 0.004*"effective" + 0.003*"need"', '0.015*"’" + 0.007*"progress" + 0.007*"well" + 0.005*"good" + 0.005*"leaders" + 0.005*"ensure" + 0.005*"effective" + 0.004*"practice" + 0.004*"needs" + 0.004*"carers"', '0.014*"’" + 0.006*"effective" + 0.005*"well" + 0.005*"leaders" + 0.005*"progress" + 0.004*"ensure" + 0.004*"Suffolk" + 0.004*"good" + 0.004*"practice" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -4279,7 +4279,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"needs" + 0.006*"Sunderland" + 0.005*"well" + 0.005*"quality" + 0.005*"experienced" + 0.004*"TfC" + 0.004*"risk" + 0.004*"parents" + 0.004*"protection"', '0.010*"’" + 0.006*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"experienced" + 0.004*"quality" + 0.004*"council" + 0.004*"parents" + 0.004*"Sunderland" + 0.004*"protection"', '0.021*"’" + 0.008*"well" + 0.008*"quality" + 0.007*"needs" + 0.007*"Sunderland" + 0.005*"practice" + 0.005*"good" + 0.005*"training" + 0.005*"experienced" + 0.005*"TfC"']</t>
+    <t>['0.018*"’" + 0.008*"Sunderland" + 0.008*"well" + 0.006*"quality" + 0.006*"needs" + 0.005*"experienced" + 0.005*"good" + 0.005*"practice" + 0.004*"result" + 0.004*"training"', '0.013*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"quality" + 0.006*"practice" + 0.005*"protection" + 0.005*"experienced" + 0.005*"Sunderland" + 0.004*"parents" + 0.004*"highly"', '0.016*"’" + 0.007*"quality" + 0.007*"well" + 0.007*"needs" + 0.006*"council" + 0.005*"protection" + 0.005*"TfC" + 0.004*"Sunderland" + 0.004*"parents" + 0.004*"experienced"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -4309,7 +4309,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.010*"needs" + 0.009*"well" + 0.006*"practice" + 0.006*"effective" + 0.006*"progress" + 0.006*"plans" + 0.005*"good" + 0.005*"carers" + 0.004*"However"', '0.012*"’" + 0.009*"well" + 0.009*"needs" + 0.006*"progress" + 0.006*"quality" + 0.006*"practice" + 0.006*"17" + 0.005*"carers" + 0.005*"good" + 0.004*"28"', '0.016*"’" + 0.009*"well" + 0.009*"needs" + 0.009*"practice" + 0.007*"progress" + 0.006*"plans" + 0.005*"However" + 0.005*"carers" + 0.005*"effective" + 0.005*"good"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.009*"well" + 0.006*"practice" + 0.005*"plans" + 0.005*"progress" + 0.005*"good" + 0.005*"carers" + 0.005*"17" + 0.004*"However"', '0.011*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"practice" + 0.006*"progress" + 0.005*"carers" + 0.005*"receive" + 0.005*"effective" + 0.005*"good" + 0.005*"plans"', '0.015*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"practice" + 0.007*"progress" + 0.006*"quality" + 0.005*"effective" + 0.005*"plans" + 0.005*"17" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -4333,7 +4333,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"needs" + 0.008*"well" + 0.007*"Swindon" + 0.007*"always" + 0.005*"need" + 0.005*"plans" + 0.005*"education" + 0.005*"impact" + 0.005*"However"', '0.019*"’" + 0.011*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"Swindon" + 0.005*"always" + 0.005*"need" + 0.005*"Council" + 0.004*"worker" + 0.004*"impact"', '0.026*"’" + 0.015*"needs" + 0.011*"need" + 0.011*"Swindon" + 0.009*"well" + 0.007*"plans" + 0.007*"always" + 0.007*"effective" + 0.006*"impact" + 0.006*"health"']</t>
+    <t>['0.020*"’" + 0.013*"needs" + 0.009*"Swindon" + 0.009*"need" + 0.007*"plans" + 0.007*"well" + 0.006*"always" + 0.006*"effective" + 0.006*"impact" + 0.005*"home"', '0.024*"’" + 0.015*"needs" + 0.009*"well" + 0.009*"Swindon" + 0.007*"always" + 0.007*"need" + 0.005*"plans" + 0.005*"health" + 0.005*"impact" + 0.005*"education"', '0.021*"’" + 0.010*"needs" + 0.009*"need" + 0.008*"Swindon" + 0.007*"well" + 0.006*"plans" + 0.006*"impact" + 0.005*"always" + 0.005*"health" + 0.005*"Borough"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -4360,7 +4360,7 @@
     <t>0.1495</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.006*"2023" + 0.006*"4" + 0.006*"impact" + 0.005*"practice" + 0.005*"risk" + 0.005*"quality" + 0.005*"experiences" + 0.005*"effective"', '0.016*"’" + 0.008*"needs" + 0.005*"quality" + 0.005*"practice" + 0.005*"risk" + 0.005*"impact" + 0.005*"planning" + 0.004*"progress" + 0.004*"understand" + 0.004*"15"', '0.018*"’" + 0.010*"needs" + 0.007*"risk" + 0.007*"impact" + 0.007*"experienced" + 0.006*"response" + 0.006*"quality" + 0.005*"Tameside" + 0.005*"need" + 0.005*"protection"']</t>
+    <t>['0.017*"’" + 0.009*"needs" + 0.007*"risk" + 0.006*"response" + 0.006*"impact" + 0.006*"2023" + 0.005*"4" + 0.005*"experienced" + 0.005*"effective" + 0.005*"quality"', '0.015*"’" + 0.009*"needs" + 0.006*"impact" + 0.006*"quality" + 0.006*"risk" + 0.005*"practice" + 0.005*"progress" + 0.005*"Tameside" + 0.005*"2023" + 0.005*"planning"', '0.016*"’" + 0.009*"needs" + 0.006*"impact" + 0.006*"experienced" + 0.005*"quality" + 0.005*"risk" + 0.005*"experiences" + 0.005*"practice" + 0.005*"understand" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -4384,7 +4384,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"ensure" + 0.005*"strong" + 0.005*"practice" + 0.005*"need" + 0.005*"plans" + 0.005*"leaders"', '0.016*"’" + 0.009*"well" + 0.008*"effective" + 0.006*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"ensure" + 0.005*"practice" + 0.004*"strong" + 0.004*"planning"', '0.017*"’" + 0.012*"well" + 0.009*"needs" + 0.006*"effective" + 0.005*"strong" + 0.005*"improve" + 0.005*"plans" + 0.005*"need" + 0.005*"planning" + 0.005*"timely"']</t>
+    <t>['0.021*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"ensure" + 0.005*"strong" + 0.005*"practice" + 0.005*"leaders"', '0.014*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"ensure" + 0.006*"strong" + 0.005*"need" + 0.005*"practice" + 0.005*"improve" + 0.004*"planning"', '0.011*"well" + 0.010*"’" + 0.006*"effective" + 0.006*"needs" + 0.005*"plans" + 0.004*"need" + 0.004*"highly" + 0.004*"benefit" + 0.004*"strong" + 0.004*"carers"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -4408,7 +4408,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.004*"carers" + 0.003*"leaders" + 0.003*"ensure" + 0.003*"need" + 0.003*"vulnerable" + 0.003*"practice" + 0.003*"needs" + 0.003*"protection"', '0.013*"’" + 0.007*"well" + 0.006*"carers" + 0.005*"needs" + 0.005*"need" + 0.004*"ensure" + 0.004*"Thurrock" + 0.003*"effective" + 0.003*"practice" + 0.003*"vulnerable"', '0.014*"’" + 0.010*"well" + 0.006*"carers" + 0.006*"need" + 0.005*"practice" + 0.004*"effective" + 0.004*"leaders" + 0.004*"protection" + 0.004*"needs" + 0.004*"Thurrock"']</t>
+    <t>['0.013*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"need" + 0.005*"ensure" + 0.004*"needs" + 0.004*"effective" + 0.004*"practice" + 0.004*"impact" + 0.003*"good"', '0.011*"’" + 0.007*"well" + 0.005*"need" + 0.005*"carers" + 0.004*"Thurrock" + 0.004*"leaders" + 0.004*"needs" + 0.004*"practice" + 0.004*"effective" + 0.003*"protection"', '0.014*"’" + 0.010*"well" + 0.006*"carers" + 0.005*"need" + 0.004*"needs" + 0.004*"practice" + 0.004*"ensure" + 0.004*"protection" + 0.004*"leaders" + 0.004*"Thurrock"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -4432,7 +4432,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.006*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.005*"team" + 0.004*"21" + 0.004*"progress" + 0.004*"2022" + 0.004*"effective"', '0.017*"’" + 0.010*"well" + 0.009*"Torbay" + 0.006*"effective" + 0.005*"good" + 0.005*"progress" + 0.005*"1" + 0.005*"plans" + 0.005*"needs" + 0.004*"quality"', '0.015*"’" + 0.008*"well" + 0.007*"Torbay" + 0.007*"needs" + 0.006*"good" + 0.005*"timely" + 0.005*"effective" + 0.005*"agencies" + 0.004*"21" + 0.004*"1"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.006*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.005*"progress" + 0.005*"effective" + 0.004*"team" + 0.004*"2022" + 0.004*"March"', '0.011*"’" + 0.009*"well" + 0.006*"Torbay" + 0.005*"good" + 0.004*"supported" + 0.004*"effective" + 0.004*"timely" + 0.004*"focus" + 0.004*"plans" + 0.004*"April"', '0.019*"’" + 0.009*"well" + 0.009*"Torbay" + 0.007*"needs" + 0.007*"good" + 0.005*"21" + 0.005*"effective" + 0.005*"team" + 0.005*"1" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4456,7 +4456,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"needs" + 0.009*"Trafford" + 0.008*"well" + 0.006*"plans" + 0.006*"team" + 0.005*"quality" + 0.005*"practice" + 0.005*"placed" + 0.004*"impact"', '0.013*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"Trafford" + 0.006*"well" + 0.006*"quality" + 0.006*"practice" + 0.006*"2" + 0.005*"leaders" + 0.005*"impact"', '0.018*"’" + 0.009*"needs" + 0.007*"quality" + 0.007*"Trafford" + 0.007*"leaders" + 0.007*"plans" + 0.006*"well" + 0.005*"ensure" + 0.005*"placed" + 0.005*"December"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"quality" + 0.006*"Trafford" + 0.006*"well" + 0.005*"practice" + 0.004*"2" + 0.004*"ensure" + 0.004*"leaders"', '0.018*"’" + 0.012*"needs" + 0.008*"well" + 0.008*"Trafford" + 0.007*"quality" + 0.006*"leaders" + 0.006*"plans" + 0.005*"practice" + 0.005*"placed" + 0.005*"ensure"', '0.017*"’" + 0.009*"Trafford" + 0.008*"plans" + 0.007*"needs" + 0.007*"well" + 0.006*"quality" + 0.005*"team" + 0.005*"leaders" + 0.005*"impact" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4480,7 +4480,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.007*"needs" + 0.006*"Walsall" + 0.005*"leaders" + 0.005*"well" + 0.005*"Senior" + 0.005*"information" + 0.004*"oversight" + 0.004*"4" + 0.004*"15"', '0.022*"’" + 0.008*"leaders" + 0.006*"well" + 0.006*"4" + 0.006*"needs" + 0.004*"Walsall" + 0.004*"Senior" + 0.004*"information" + 0.004*"oversight" + 0.004*"carers"', '0.021*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"Walsall" + 0.005*"well" + 0.004*"information" + 0.004*"oversight" + 0.004*"2021" + 0.004*"good" + 0.004*"need"']</t>
+    <t>['0.022*"’" + 0.008*"leaders" + 0.007*"needs" + 0.006*"Walsall" + 0.006*"information" + 0.005*"well" + 0.005*"Senior" + 0.005*"4" + 0.005*"oversight" + 0.005*"15"', '0.020*"’" + 0.006*"leaders" + 0.006*"needs" + 0.005*"well" + 0.005*"4" + 0.005*"Walsall" + 0.005*"oversight" + 0.004*"receive" + 0.004*"information" + 0.004*"15"', '0.021*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"well" + 0.005*"Walsall" + 0.004*"good" + 0.004*"early" + 0.004*"Senior" + 0.004*"risks" + 0.004*"2021"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4510,7 +4510,7 @@
     <t>19/08/19</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"Senior" + 0.004*"plans" + 0.004*"progress" + 0.004*"information" + 0.004*"carers" + 0.003*"number" + 0.003*"good"', '0.010*"’" + 0.006*"well" + 0.006*"practice" + 0.005*"number" + 0.004*"progress" + 0.004*"need" + 0.004*"information" + 0.004*"Senior" + 0.004*"needs" + 0.003*"good"', '0.018*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"plans" + 0.005*"home" + 0.004*"number" + 0.004*"good" + 0.004*"need" + 0.004*"Senior" + 0.004*"senior"']</t>
+    <t>['0.015*"’" + 0.008*"practice" + 0.005*"well" + 0.005*"Senior" + 0.004*"progress" + 0.004*"plans" + 0.004*"number" + 0.003*"good" + 0.003*"protection" + 0.003*"needs"', '0.009*"’" + 0.007*"well" + 0.005*"Senior" + 0.005*"practice" + 0.004*"carers" + 0.004*"good" + 0.004*"need" + 0.004*"information" + 0.004*"number" + 0.004*"small"', '0.017*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"number" + 0.005*"plans" + 0.004*"home" + 0.004*"provided" + 0.004*"progress" + 0.004*"need" + 0.004*"carers"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4540,7 +4540,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"Warwickshire" + 0.005*"practice" + 0.005*"22" + 0.004*"December" + 0.004*"clear" + 0.004*"progress"', '0.014*"’" + 0.007*"well" + 0.006*"Warwickshire" + 0.006*"needs" + 0.006*"plans" + 0.005*"carers" + 0.005*"3" + 0.005*"practice" + 0.004*"Senior" + 0.004*"effective"', '0.009*"’" + 0.006*"good" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"clear" + 0.004*"information" + 0.004*"Warwickshire" + 0.004*"supported" + 0.004*"practice"']</t>
+    <t>['0.013*"’" + 0.006*"Warwickshire" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.004*"carers" + 0.004*"3" + 0.004*"2021" + 0.004*"effective" + 0.004*"November"', '0.010*"’" + 0.007*"needs" + 0.006*"practice" + 0.006*"well" + 0.005*"carers" + 0.005*"Warwickshire" + 0.005*"good" + 0.005*"Senior" + 0.004*"information" + 0.004*"plans"', '0.012*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"Warwickshire" + 0.006*"clear" + 0.005*"progress" + 0.005*"practice" + 0.005*"good" + 0.004*"3"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4564,7 +4564,7 @@
     <t>14/03/2022</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"West" + 0.007*"well" + 0.007*"Berkshire" + 0.005*"early" + 0.005*"working" + 0.004*"14" + 0.004*"March" + 0.004*"plans" + 0.004*"needs"', '0.011*"’" + 0.005*"well" + 0.004*"West" + 0.004*"Berkshire" + 0.004*"need" + 0.004*"progress" + 0.003*"plans" + 0.003*"18" + 0.003*"needs" + 0.003*"agency"', '0.011*"’" + 0.006*"Berkshire" + 0.005*"West" + 0.005*"need" + 0.004*"needs" + 0.004*"plans" + 0.004*"well" + 0.004*"agency" + 0.004*"18" + 0.004*"2022"']</t>
+    <t>['0.017*"’" + 0.007*"well" + 0.006*"Berkshire" + 0.005*"West" + 0.005*"plans" + 0.004*"14" + 0.004*"agency" + 0.004*"18" + 0.004*"early" + 0.004*"working"', '0.011*"’" + 0.008*"West" + 0.005*"well" + 0.005*"Berkshire" + 0.005*"need" + 0.005*"progress" + 0.004*"working" + 0.004*"needs" + 0.004*"18" + 0.004*"March"', '0.014*"’" + 0.007*"Berkshire" + 0.007*"West" + 0.005*"well" + 0.005*"needs" + 0.004*"early" + 0.004*"agency" + 0.004*"2022" + 0.004*"need" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>2637548</t>
@@ -4588,7 +4588,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"West" + 0.006*"well" + 0.005*"impact" + 0.005*"3" + 0.005*"needs" + 0.005*"plans" + 0.004*"practice"', '0.019*"’" + 0.009*"Northamptonshire" + 0.007*"quality" + 0.006*"West" + 0.006*"well" + 0.005*"NCT" + 0.005*"need" + 0.004*"needs" + 0.004*"health" + 0.004*"place"', '0.018*"’" + 0.007*"Northamptonshire" + 0.007*"West" + 0.007*"practice" + 0.006*"well" + 0.005*"quality" + 0.005*"needs" + 0.005*"NCT" + 0.005*"3" + 0.004*"14"']</t>
+    <t>['0.013*"’" + 0.009*"Northamptonshire" + 0.007*"quality" + 0.006*"well" + 0.006*"West" + 0.005*"practice" + 0.005*"needs" + 0.005*"NCT" + 0.004*"plans" + 0.004*"Leaders"', '0.018*"’" + 0.007*"Northamptonshire" + 0.007*"well" + 0.007*"West" + 0.006*"quality" + 0.006*"practice" + 0.005*"needs" + 0.005*"3" + 0.005*"impact" + 0.004*"plans"', '0.020*"’" + 0.007*"Northamptonshire" + 0.006*"West" + 0.006*"quality" + 0.005*"well" + 0.005*"14" + 0.005*"NCT" + 0.005*"3" + 0.005*"needs" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4612,7 +4612,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"quality" + 0.004*"clear" + 0.004*"Sussex" + 0.004*"West" + 0.004*"number" + 0.004*"practice"', '0.014*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"Sussex" + 0.006*"well" + 0.006*"13" + 0.005*"supported" + 0.005*"West" + 0.005*"number" + 0.004*"24"', '0.016*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"West" + 0.005*"needs" + 0.005*"practice" + 0.005*"health" + 0.005*"quality" + 0.004*"13" + 0.004*"number"']</t>
+    <t>['0.014*"’" + 0.006*"plans" + 0.006*"well" + 0.006*"needs" + 0.005*"West" + 0.005*"13" + 0.005*"Sussex" + 0.004*"number" + 0.004*"24" + 0.004*"quality"', '0.016*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"West" + 0.005*"Sussex" + 0.005*"13" + 0.004*"practice" + 0.004*"clear" + 0.004*"number"', '0.011*"’" + 0.006*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"Sussex" + 0.005*"quality" + 0.005*"good" + 0.005*"supported" + 0.004*"health" + 0.004*"13"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4633,7 +4633,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"May" + 0.006*"needs" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"Wigan" + 0.005*"plans" + 0.005*"leaders" + 0.004*"quality" + 0.004*"oversight"', '0.015*"’" + 0.007*"plans" + 0.007*"Wigan" + 0.007*"quality" + 0.007*"May" + 0.006*"timely" + 0.006*"appropriate" + 0.006*"needs" + 0.005*"practice" + 0.005*"9"', '0.009*"’" + 0.009*"May" + 0.009*"practice" + 0.006*"plans" + 0.006*"needs" + 0.005*"well" + 0.004*"appropriate" + 0.004*"leaders" + 0.004*"Wigan" + 0.004*"quality"']</t>
+    <t>['0.011*"’" + 0.006*"plans" + 0.006*"appropriate" + 0.006*"May" + 0.006*"practice" + 0.005*"Wigan" + 0.005*"quality" + 0.005*"increased" + 0.004*"leaders" + 0.004*"needs"', '0.012*"’" + 0.007*"May" + 0.005*"practice" + 0.005*"quality" + 0.005*"20" + 0.005*"plans" + 0.004*"well" + 0.004*"needs" + 0.004*"Wigan" + 0.004*"leaders"', '0.013*"’" + 0.008*"May" + 0.008*"needs" + 0.007*"practice" + 0.007*"plans" + 0.007*"Wigan" + 0.006*"quality" + 0.006*"9" + 0.005*"timely" + 0.005*"appropriate"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4666,7 +4666,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"well" + 0.007*"need" + 0.007*"Wiltshire" + 0.006*"parents" + 0.006*"quality" + 0.006*"needs" + 0.006*"plans" + 0.005*"progress" + 0.005*"including"', '0.013*"well" + 0.012*"’" + 0.008*"needs" + 0.006*"need" + 0.006*"progress" + 0.005*"plans" + 0.005*"parents" + 0.005*"including" + 0.005*"quality" + 0.005*"ensure"', '0.019*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"risk" + 0.006*"need" + 0.006*"progress" + 0.006*"Wiltshire" + 0.006*"supported" + 0.006*"including" + 0.005*"parents"']</t>
+    <t>['0.013*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"progress" + 0.005*"ensure" + 0.005*"Wiltshire" + 0.005*"parents" + 0.005*"risk" + 0.005*"quality" + 0.004*"need"', '0.018*"’" + 0.013*"well" + 0.007*"needs" + 0.007*"Wiltshire" + 0.006*"including" + 0.006*"need" + 0.006*"plans" + 0.006*"progress" + 0.006*"risk" + 0.005*"parents"', '0.014*"’" + 0.010*"well" + 0.007*"need" + 0.007*"needs" + 0.007*"supported" + 0.006*"parents" + 0.006*"including" + 0.006*"risk" + 0.005*"progress" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4696,7 +4696,7 @@
     <t>0.1655</t>
   </si>
   <si>
-    <t>['0.010*"needs" + 0.010*"’" + 0.007*"ensure" + 0.007*"Wirral" + 0.006*"well" + 0.006*"plans" + 0.006*"good" + 0.005*"number" + 0.004*"practice" + 0.004*"September"', '0.009*"’" + 0.006*"18" + 0.006*"Wirral" + 0.006*"needs" + 0.006*"practice" + 0.006*"ensure" + 0.006*"plans" + 0.005*"family" + 0.005*"good" + 0.005*"number"', '0.013*"’" + 0.011*"needs" + 0.008*"Wirral" + 0.008*"ensure" + 0.007*"plans" + 0.007*"practice" + 0.006*"risk" + 0.005*"29" + 0.005*"response" + 0.005*"well"']</t>
+    <t>['0.013*"’" + 0.010*"needs" + 0.009*"Wirral" + 0.007*"ensure" + 0.006*"well" + 0.006*"plans" + 0.006*"good" + 0.006*"practice" + 0.006*"response" + 0.005*"appropriate"', '0.009*"needs" + 0.008*"plans" + 0.007*"’" + 0.007*"ensure" + 0.007*"practice" + 0.005*"Wirral" + 0.005*"18" + 0.005*"number" + 0.005*"29" + 0.005*"effective"', '0.012*"’" + 0.009*"needs" + 0.006*"ensure" + 0.006*"Wirral" + 0.005*"plans" + 0.005*"practice" + 0.005*"number" + 0.004*"well" + 0.004*"September" + 0.004*"response"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4720,7 +4720,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"17" + 0.006*"well" + 0.005*"experiences" + 0.005*"needs" + 0.005*"appropriate" + 0.004*"progress" + 0.004*"provided"', '0.012*"’" + 0.006*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"provided" + 0.006*"effective" + 0.005*"progress" + 0.005*"impact" + 0.004*"protection" + 0.004*"Wokingham"', '0.012*"’" + 0.007*"plans" + 0.006*"needs" + 0.006*"progress" + 0.006*"effective" + 0.005*"provided" + 0.005*"experiences" + 0.004*"6" + 0.004*"parents" + 0.004*"clear"']</t>
+    <t>['0.012*"’" + 0.006*"effective" + 0.005*"plans" + 0.005*"progress" + 0.005*"impact" + 0.005*"well" + 0.004*"needs" + 0.004*"protection" + 0.004*"experiences" + 0.004*"6"', '0.014*"’" + 0.007*"plans" + 0.006*"effective" + 0.006*"needs" + 0.006*"progress" + 0.005*"well" + 0.005*"provided" + 0.005*"17" + 0.005*"Wokingham" + 0.005*"March"', '0.011*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"effective" + 0.005*"provided" + 0.005*"progress" + 0.005*"well" + 0.005*"appropriate" + 0.004*"quality" + 0.004*"clear"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4744,7 +4744,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"needs" + 0.007*"effective" + 0.007*"Wolverhampton" + 0.005*"plans" + 0.005*"receive" + 0.005*"leaders" + 0.005*"education" + 0.005*"well" + 0.005*"risks"', '0.012*"’" + 0.006*"needs" + 0.005*"risks" + 0.005*"effective" + 0.005*"Wolverhampton" + 0.005*"quality" + 0.005*"plans" + 0.005*"supported" + 0.004*"1" + 0.004*"leaders"', '0.010*"’" + 0.007*"needs" + 0.004*"quality" + 0.004*"City" + 0.004*"risk" + 0.004*"strong" + 0.004*"effective" + 0.004*"practice" + 0.004*"supported" + 0.004*"risks"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.006*"effective" + 0.006*"quality" + 0.006*"supported" + 0.005*"risks" + 0.005*"leaders" + 0.005*"strong" + 0.005*"Wolverhampton" + 0.004*"risk"', '0.016*"’" + 0.008*"needs" + 0.008*"Wolverhampton" + 0.007*"plans" + 0.006*"effective" + 0.006*"receive" + 0.005*"28" + 0.005*"risks" + 0.004*"risk" + 0.004*"education"', '0.013*"’" + 0.005*"needs" + 0.005*"effective" + 0.005*"leaders" + 0.005*"quality" + 0.004*"risks" + 0.004*"education" + 0.004*"receive" + 0.004*"practice" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4774,7 +4774,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.007*"plans" + 0.007*"Worcestershire" + 0.006*"needs" + 0.006*"progress" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"well" + 0.004*"15" + 0.004*"ensure"', '0.025*"’" + 0.010*"well" + 0.008*"Worcestershire" + 0.008*"plans" + 0.008*"needs" + 0.008*"leaders" + 0.007*"ensure" + 0.007*"progress" + 0.006*"appropriate" + 0.005*"PAs"', '0.015*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"needs" + 0.006*"progress" + 0.006*"leaders" + 0.005*"Worcestershire" + 0.004*"May" + 0.004*"appropriate" + 0.004*"15"']</t>
+    <t>['0.020*"’" + 0.009*"well" + 0.007*"Worcestershire" + 0.007*"progress" + 0.006*"ensure" + 0.006*"plans" + 0.006*"needs" + 0.005*"leaders" + 0.005*"appropriate" + 0.004*"good"', '0.014*"’" + 0.009*"needs" + 0.009*"well" + 0.008*"plans" + 0.008*"leaders" + 0.007*"progress" + 0.006*"Worcestershire" + 0.005*"appropriate" + 0.005*"improve" + 0.005*"Senior"', '0.022*"’" + 0.009*"plans" + 0.008*"Worcestershire" + 0.007*"needs" + 0.007*"well" + 0.007*"ensure" + 0.006*"leaders" + 0.006*"progress" + 0.005*"appropriate" + 0.005*"education"']</t>
   </si>
   <si>
     <t>urn</t>

</xml_diff>

<commit_message>
server timestamp correction +1h fix
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -70,7 +70,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"Barnsley" + 0.006*"leaders" + 0.006*"needs" + 0.005*"practice" + 0.005*"within" + 0.004*"need" + 0.004*"plans" + 0.004*"quality" + 0.004*"11"', '0.017*"’" + 0.009*"needs" + 0.007*"leaders" + 0.006*"within" + 0.005*"practice" + 0.005*"plans" + 0.005*"Barnsley" + 0.005*"11" + 0.004*"2023" + 0.004*"September"', '0.026*"’" + 0.008*"needs" + 0.008*"leaders" + 0.007*"within" + 0.006*"practice" + 0.006*"Barnsley" + 0.005*"15" + 0.005*"senior" + 0.005*"response" + 0.004*"plans"']</t>
+    <t>['0.016*"’" + 0.007*"needs" + 0.007*"leaders" + 0.006*"practice" + 0.005*"within" + 0.004*"Barnsley" + 0.004*"understand" + 0.004*"September" + 0.004*"11" + 0.004*"plans"', '0.021*"’" + 0.008*"needs" + 0.007*"within" + 0.007*"Barnsley" + 0.006*"leaders" + 0.006*"practice" + 0.005*"response" + 0.005*"senior" + 0.005*"15" + 0.005*"plans"', '0.019*"’" + 0.009*"leaders" + 0.008*"needs" + 0.005*"Barnsley" + 0.005*"within" + 0.004*"senior" + 0.004*"plans" + 0.004*"practice" + 0.004*"quality" + 0.004*"Senior"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -115,7 +115,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"well" + 0.005*"plans" + 0.005*"practice" + 0.005*"needs" + 0.005*"North" + 0.004*"impact" + 0.004*"28" + 0.004*"effective" + 0.004*"Bath"', '0.016*"’" + 0.008*"well" + 0.006*"leaders" + 0.006*"needs" + 0.005*"North" + 0.005*"practice" + 0.005*"plans" + 0.005*"4" + 0.005*"28" + 0.005*"effective"', '0.021*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"plans" + 0.005*"4" + 0.005*"clear" + 0.005*"effective" + 0.005*"Bath" + 0.005*"receive"']</t>
+    <t>['0.018*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"leaders" + 0.005*"4" + 0.005*"Bath" + 0.005*"North" + 0.005*"effective" + 0.005*"impact"', '0.017*"’" + 0.010*"well" + 0.007*"plans" + 0.006*"needs" + 0.005*"leaders" + 0.005*"practice" + 0.005*"East" + 0.005*"effective" + 0.004*"clear" + 0.004*"receive"', '0.018*"’" + 0.007*"well" + 0.005*"practice" + 0.005*"receive" + 0.004*"needs" + 0.004*"Somerset" + 0.004*"plans" + 0.004*"impact" + 0.004*"protection" + 0.004*"clear"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -163,7 +163,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"ensure" + 0.006*"plans" + 0.005*"Bedford" + 0.005*"progress" + 0.005*"supported" + 0.005*"26" + 0.005*"family"', '0.016*"’" + 0.007*"ensure" + 0.006*"needs" + 0.005*"plans" + 0.005*"Bedford" + 0.005*"good" + 0.004*"family" + 0.004*"progress" + 0.004*"education" + 0.004*"relationships"', '0.021*"’" + 0.006*"needs" + 0.005*"supported" + 0.005*"good" + 0.005*"well" + 0.005*"ensure" + 0.005*"Borough" + 0.005*"Bedford" + 0.004*"education" + 0.004*"15"']</t>
+    <t>['0.013*"’" + 0.007*"needs" + 0.005*"Bedford" + 0.005*"ensure" + 0.004*"progress" + 0.004*"supported" + 0.004*"well" + 0.004*"relationships" + 0.004*"Borough" + 0.004*"good"', '0.022*"’" + 0.008*"needs" + 0.007*"ensure" + 0.006*"plans" + 0.006*"well" + 0.006*"good" + 0.005*"Bedford" + 0.005*"progress" + 0.005*"education" + 0.005*"family"', '0.018*"’" + 0.006*"ensure" + 0.006*"supported" + 0.006*"well" + 0.005*"family" + 0.005*"needs" + 0.005*"education" + 0.005*"plans" + 0.005*"Bedford" + 0.004*"Borough"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -208,7 +208,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"trust" + 0.005*"well" + 0.005*"progress" + 0.005*"Birmingham" + 0.005*"plans" + 0.005*"risk" + 0.005*"arrangements"', '0.017*"’" + 0.011*"needs" + 0.007*"well" + 0.007*"Birmingham" + 0.006*"effective" + 0.006*"plans" + 0.005*"progress" + 0.005*"timely" + 0.005*"3" + 0.005*"risk"', '0.015*"’" + 0.009*"needs" + 0.007*"effective" + 0.006*"well" + 0.006*"plans" + 0.006*"trust" + 0.006*"appropriate" + 0.005*"progress" + 0.005*"3" + 0.005*"Birmingham"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"Birmingham" + 0.006*"effective" + 0.005*"progress" + 0.005*"appropriate" + 0.005*"plans" + 0.004*"response" + 0.004*"3"', '0.012*"’" + 0.006*"needs" + 0.005*"plans" + 0.005*"well" + 0.005*"progress" + 0.004*"3" + 0.004*"risk" + 0.004*"20" + 0.004*"effective" + 0.004*"appropriate"', '0.019*"’" + 0.012*"needs" + 0.008*"effective" + 0.007*"trust" + 0.007*"plans" + 0.006*"well" + 0.006*"Birmingham" + 0.006*"progress" + 0.005*"risk" + 0.005*"3"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -250,7 +250,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"needs" + 0.008*"Darwen" + 0.006*"practice" + 0.006*"Blackburn" + 0.006*"quality" + 0.006*"impact" + 0.005*"result" + 0.005*"well" + 0.005*"leaders"', '0.012*"’" + 0.008*"needs" + 0.008*"quality" + 0.007*"practice" + 0.007*"Blackburn" + 0.007*"well" + 0.006*"need" + 0.005*"impact" + 0.005*"Darwen" + 0.005*"effective"', '0.014*"’" + 0.007*"practice" + 0.007*"impact" + 0.006*"quality" + 0.006*"Blackburn" + 0.006*"well" + 0.006*"Darwen" + 0.006*"needs" + 0.005*"means" + 0.005*"planning"']</t>
+    <t>['0.014*"’" + 0.010*"needs" + 0.007*"practice" + 0.006*"Blackburn" + 0.006*"quality" + 0.006*"Darwen" + 0.006*"impact" + 0.006*"effective" + 0.006*"planning" + 0.006*"well"', '0.013*"’" + 0.007*"practice" + 0.006*"needs" + 0.006*"Darwen" + 0.006*"Blackburn" + 0.005*"quality" + 0.005*"impact" + 0.005*"means" + 0.005*"progress" + 0.005*"plans"', '0.014*"’" + 0.008*"quality" + 0.007*"practice" + 0.007*"well" + 0.007*"Blackburn" + 0.007*"Darwen" + 0.006*"impact" + 0.006*"needs" + 0.005*"result" + 0.005*"planning"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -289,7 +289,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.005*"effective" + 0.005*"plans" + 0.004*"quality" + 0.004*"experiences" + 0.004*"supported" + 0.004*"good"', '0.017*"’" + 0.008*"well" + 0.008*"needs" + 0.006*"Blackpool" + 0.005*"supported" + 0.005*"effective" + 0.004*"progress" + 0.004*"plans" + 0.004*"quality" + 0.004*"experiences"', '0.018*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"Blackpool" + 0.006*"effective" + 0.006*"practice" + 0.006*"16" + 0.006*"plans" + 0.005*"5" + 0.005*"need"']</t>
+    <t>['0.016*"’" + 0.009*"needs" + 0.008*"Blackpool" + 0.008*"well" + 0.005*"effective" + 0.005*"16" + 0.005*"5" + 0.005*"good" + 0.005*"supported" + 0.005*"plans"', '0.017*"’" + 0.014*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.007*"effective" + 0.006*"practice" + 0.005*"supported" + 0.005*"experiences" + 0.005*"16" + 0.005*"carers"', '0.016*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"Blackpool" + 0.006*"practice" + 0.006*"plans" + 0.006*"quality" + 0.005*"progress" + 0.005*"response" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80432</t>
@@ -322,7 +322,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"needs" + 0.008*"Bolton" + 0.008*"well" + 0.008*"plans" + 0.006*"need" + 0.006*"September" + 0.005*"11" + 0.005*"supported" + 0.005*"strong"', '0.022*"’" + 0.009*"needs" + 0.008*"Bolton" + 0.008*"well" + 0.008*"plans" + 0.006*"supported" + 0.006*"timely" + 0.005*"effective" + 0.005*"planning" + 0.005*"need"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Bolton" + 0.006*"plans" + 0.005*"planning" + 0.005*"supported" + 0.005*"effective" + 0.004*"strong" + 0.004*"experiences"']</t>
+    <t>['0.013*"’" + 0.011*"needs" + 0.007*"Bolton" + 0.006*"well" + 0.005*"supported" + 0.005*"plans" + 0.004*"planning" + 0.004*"timely" + 0.004*"2023" + 0.004*"11"', '0.020*"’" + 0.008*"well" + 0.008*"Bolton" + 0.008*"plans" + 0.008*"needs" + 0.006*"need" + 0.006*"supported" + 0.005*"planning" + 0.005*"effective" + 0.005*"strong"', '0.021*"’" + 0.010*"needs" + 0.009*"well" + 0.009*"Bolton" + 0.008*"plans" + 0.006*"15" + 0.005*"11" + 0.005*"strong" + 0.005*"supported" + 0.005*"need"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -358,7 +358,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.005*"impact" + 0.005*"Christchurch" + 0.005*"many" + 0.005*"time" + 0.004*"progress" + 0.004*"quality" + 0.004*"practice" + 0.004*"17" + 0.004*"risk"', '0.016*"’" + 0.007*"quality" + 0.007*"practice" + 0.006*"6" + 0.005*"progress" + 0.005*"17" + 0.005*"However" + 0.004*"Poole" + 0.004*"well" + 0.004*"risk"', '0.019*"’" + 0.006*"quality" + 0.006*"practice" + 0.005*"progress" + 0.005*"Poole" + 0.005*"Bournemouth" + 0.004*"risk" + 0.004*"Christchurch" + 0.004*"2021" + 0.004*"right"']</t>
+    <t>['0.016*"’" + 0.007*"quality" + 0.006*"6" + 0.005*"Poole" + 0.005*"practice" + 0.004*"progress" + 0.004*"risk" + 0.004*"Christchurch" + 0.004*"17" + 0.004*"impact"', '0.021*"’" + 0.006*"progress" + 0.006*"practice" + 0.006*"quality" + 0.005*"time" + 0.005*"risk" + 0.005*"17" + 0.005*"impact" + 0.005*"Bournemouth" + 0.004*"December"', '0.016*"’" + 0.006*"practice" + 0.005*"quality" + 0.005*"well" + 0.005*"Bournemouth" + 0.004*"many" + 0.004*"However" + 0.004*"Christchurch" + 0.004*"Poole" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -403,7 +403,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"risk" + 0.006*"positive" + 0.006*"needs" + 0.006*"Bracknell" + 0.006*"effective" + 0.006*"quality" + 0.005*"Forest" + 0.005*"need" + 0.005*"good"', '0.012*"’" + 0.007*"risk" + 0.005*"Bracknell" + 0.005*"quality" + 0.005*"good" + 0.005*"provided" + 0.004*"plans" + 0.004*"effective" + 0.004*"Forest" + 0.004*"progress"', '0.019*"’" + 0.009*"Forest" + 0.008*"needs" + 0.008*"Bracknell" + 0.007*"good" + 0.006*"quality" + 0.006*"plans" + 0.006*"well" + 0.006*"effective" + 0.006*"progress"']</t>
+    <t>['0.017*"’" + 0.007*"Bracknell" + 0.006*"needs" + 0.006*"quality" + 0.006*"leaders" + 0.005*"progress" + 0.005*"Forest" + 0.005*"plans" + 0.005*"risk" + 0.005*"positive"', '0.017*"’" + 0.009*"Forest" + 0.008*"risk" + 0.007*"Bracknell" + 0.007*"needs" + 0.007*"good" + 0.006*"quality" + 0.006*"well" + 0.005*"2022" + 0.005*"need"', '0.015*"’" + 0.006*"effective" + 0.006*"needs" + 0.006*"progress" + 0.006*"provided" + 0.006*"impact" + 0.006*"risk" + 0.005*"good" + 0.005*"quality" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80438</t>
@@ -439,7 +439,7 @@
     <t>0.1856</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"practice" + 0.005*"progress" + 0.005*"Brighton" + 0.005*"Hove" + 0.005*"PAs" + 0.005*"11" + 0.005*"experiences"', '0.019*"’" + 0.009*"well" + 0.007*"Brighton" + 0.007*"Hove" + 0.006*"practice" + 0.006*"needs" + 0.006*"relationships" + 0.005*"carers" + 0.005*"experiences" + 0.005*"March"', '0.016*"’" + 0.007*"Hove" + 0.007*"needs" + 0.006*"well" + 0.006*"Brighton" + 0.006*"progress" + 0.006*"experiences" + 0.005*"practice" + 0.005*"relationships" + 0.004*"15"']</t>
+    <t>['0.017*"’" + 0.007*"needs" + 0.007*"Hove" + 0.006*"well" + 0.006*"practice" + 0.006*"Brighton" + 0.005*"progress" + 0.005*"experiences" + 0.005*"relationships" + 0.004*"carers"', '0.012*"’" + 0.007*"well" + 0.007*"Brighton" + 0.006*"experiences" + 0.006*"relationships" + 0.006*"needs" + 0.005*"practice" + 0.005*"progress" + 0.005*"Hove" + 0.005*"11"', '0.019*"’" + 0.009*"well" + 0.007*"Hove" + 0.006*"needs" + 0.006*"practice" + 0.006*"Brighton" + 0.005*"receive" + 0.005*"PAs" + 0.005*"family" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -475,7 +475,7 @@
     <t>0.1875</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"well" + 0.008*"good" + 0.008*"needs" + 0.008*"Bristol" + 0.005*"progress" + 0.005*"2023" + 0.005*"leaders" + 0.005*"health" + 0.004*"16"', '0.022*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"good" + 0.006*"Bristol" + 0.006*"progress" + 0.005*"need" + 0.005*"health" + 0.005*"receive" + 0.004*"16"', '0.018*"’" + 0.008*"Bristol" + 0.008*"good" + 0.007*"well" + 0.006*"needs" + 0.005*"health" + 0.005*"ensure" + 0.005*"plans" + 0.005*"leaders" + 0.004*"need"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.009*"well" + 0.006*"good" + 0.006*"Bristol" + 0.006*"receive" + 0.005*"progress" + 0.005*"health" + 0.004*"leaders" + 0.004*"arrangements"', '0.017*"’" + 0.009*"well" + 0.008*"good" + 0.007*"needs" + 0.006*"Bristol" + 0.005*"health" + 0.005*"leaders" + 0.005*"plans" + 0.004*"always" + 0.004*"need"', '0.021*"’" + 0.010*"Bristol" + 0.008*"well" + 0.008*"good" + 0.006*"needs" + 0.006*"progress" + 0.005*"need" + 0.005*"health" + 0.005*"16" + 0.005*"always"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -505,7 +505,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"plans" + 0.004*"December" + 0.004*"Buckinghamshire" + 0.004*"many" + 0.004*"17" + 0.003*"teams" + 0.003*"6" + 0.003*"2021" + 0.003*"well"', '0.014*"’" + 0.007*"number" + 0.005*"17" + 0.005*"protection" + 0.005*"Buckinghamshire" + 0.005*"practice" + 0.004*"plans" + 0.004*"many" + 0.004*"needs" + 0.004*"small"', '0.012*"’" + 0.006*"plans" + 0.005*"6" + 0.004*"Buckinghamshire" + 0.004*"2021" + 0.004*"17" + 0.004*"number" + 0.004*"many" + 0.004*"protection" + 0.004*"December"']</t>
+    <t>['0.011*"’" + 0.006*"many" + 0.005*"plans" + 0.004*"practice" + 0.004*"December" + 0.004*"number" + 0.004*"protection" + 0.004*"Buckinghamshire" + 0.004*"6" + 0.004*"needs"', '0.014*"’" + 0.006*"number" + 0.006*"plans" + 0.005*"17" + 0.005*"Buckinghamshire" + 0.004*"protection" + 0.004*"teams" + 0.004*"2021" + 0.004*"practice" + 0.004*"well"', '0.014*"’" + 0.004*"Buckinghamshire" + 0.004*"6" + 0.004*"17" + 0.004*"number" + 0.004*"plans" + 0.004*"December" + 0.003*"small" + 0.003*"2021" + 0.003*"many"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -544,7 +544,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"protection" + 0.005*"2021" + 0.005*"needs" + 0.005*"team" + 0.005*"Bury" + 0.005*"risk" + 0.004*"practice" + 0.004*"need" + 0.004*"impact"', '0.009*"’" + 0.008*"needs" + 0.007*"2021" + 0.007*"protection" + 0.006*"team" + 0.005*"practice" + 0.005*"impact" + 0.005*"quality" + 0.005*"need" + 0.005*"risk"', '0.015*"’" + 0.007*"protection" + 0.006*"2021" + 0.006*"practice" + 0.006*"team" + 0.006*"needs" + 0.005*"need" + 0.005*"Bury" + 0.005*"impact" + 0.005*"new"']</t>
+    <t>['0.009*"’" + 0.006*"needs" + 0.005*"team" + 0.005*"practice" + 0.004*"need" + 0.004*"impact" + 0.004*"2021" + 0.004*"protection" + 0.004*"delay" + 0.004*"timely"', '0.012*"’" + 0.008*"protection" + 0.007*"2021" + 0.006*"needs" + 0.006*"Bury" + 0.006*"need" + 0.006*"risk" + 0.006*"practice" + 0.005*"new" + 0.005*"5"', '0.011*"’" + 0.007*"2021" + 0.007*"needs" + 0.006*"team" + 0.006*"practice" + 0.006*"protection" + 0.006*"impact" + 0.005*"quality" + 0.005*"progress" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -583,7 +583,7 @@
     <t>0.194</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.011*"needs" + 0.010*"Calderdale" + 0.007*"well" + 0.007*"plans" + 0.007*"ensure" + 0.006*"progress" + 0.005*"parents" + 0.005*"risk" + 0.005*"PAs"', '0.011*"’" + 0.007*"Calderdale" + 0.006*"needs" + 0.004*"plans" + 0.004*"progress" + 0.004*"ensure" + 0.004*"parents" + 0.004*"well" + 0.004*"information" + 0.004*"experiences"', '0.017*"’" + 0.011*"needs" + 0.007*"Calderdale" + 0.006*"risk" + 0.005*"well" + 0.005*"progress" + 0.004*"experiences" + 0.004*"plans" + 0.004*"2024" + 0.004*"information"']</t>
+    <t>['0.022*"’" + 0.010*"needs" + 0.009*"Calderdale" + 0.006*"well" + 0.006*"plans" + 0.006*"ensure" + 0.005*"information" + 0.005*"progress" + 0.004*"risk" + 0.004*"19"', '0.016*"’" + 0.008*"needs" + 0.007*"Calderdale" + 0.006*"parents" + 0.006*"progress" + 0.005*"well" + 0.005*"experiences" + 0.005*"23" + 0.005*"risk" + 0.005*"ensure"', '0.022*"’" + 0.011*"needs" + 0.009*"Calderdale" + 0.007*"plans" + 0.006*"well" + 0.006*"ensure" + 0.005*"risk" + 0.005*"progress" + 0.005*"need" + 0.004*"19"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -613,7 +613,7 @@
     <t>0.2052</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.006*"leaders" + 0.006*"Cambridgeshire" + 0.006*"effective" + 0.005*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"However" + 0.004*"quality" + 0.004*"leadership"', '0.015*"’" + 0.008*"needs" + 0.007*"leaders" + 0.006*"Cambridgeshire" + 0.005*"well" + 0.005*"good" + 0.005*"response" + 0.004*"clear" + 0.004*"effective" + 0.004*"15"', '0.021*"’" + 0.007*"Cambridgeshire" + 0.007*"needs" + 0.006*"good" + 0.006*"leaders" + 0.005*"4" + 0.005*"practice" + 0.005*"quality" + 0.004*"March" + 0.004*"15"']</t>
+    <t>['0.013*"’" + 0.007*"Cambridgeshire" + 0.006*"needs" + 0.005*"quality" + 0.005*"well" + 0.005*"leadership" + 0.005*"leaders" + 0.005*"good" + 0.004*"effective" + 0.004*"However"', '0.019*"’" + 0.007*"needs" + 0.007*"leaders" + 0.006*"good" + 0.006*"4" + 0.005*"well" + 0.004*"Cambridgeshire" + 0.004*"effective" + 0.004*"response" + 0.004*"supported"', '0.017*"’" + 0.007*"needs" + 0.007*"Cambridgeshire" + 0.007*"leaders" + 0.005*"effective" + 0.005*"practice" + 0.005*"good" + 0.005*"2024" + 0.004*"well" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -646,7 +646,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"well" + 0.007*"need" + 0.007*"plans" + 0.007*"needs" + 0.006*"good" + 0.006*"carers" + 0.005*"progress" + 0.005*"effective" + 0.004*"Bedfordshire"', '0.018*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"carers" + 0.006*"need" + 0.006*"progress" + 0.006*"good" + 0.006*"supported" + 0.005*"Bedfordshire" + 0.005*"Central"', '0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"plans" + 0.006*"good" + 0.005*"need" + 0.005*"Central" + 0.005*"carers" + 0.004*"number" + 0.004*"Leaders"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.006*"progress" + 0.006*"needs" + 0.006*"need" + 0.006*"good" + 0.006*"plans" + 0.006*"carers" + 0.005*"17" + 0.005*"effective"', '0.014*"’" + 0.009*"well" + 0.007*"carers" + 0.007*"need" + 0.006*"needs" + 0.006*"Central" + 0.005*"plans" + 0.005*"good" + 0.005*"2022" + 0.005*"Bedfordshire"', '0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"plans" + 0.005*"progress" + 0.005*"carers" + 0.005*"Bedfordshire" + 0.005*"education"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -682,7 +682,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"2024" + 0.006*"well" + 0.006*"practice" + 0.006*"plans" + 0.005*"quality" + 0.005*"leaders" + 0.005*"access" + 0.005*"effective" + 0.005*"means"', '0.014*"’" + 0.010*"needs" + 0.008*"2024" + 0.008*"plans" + 0.008*"practice" + 0.007*"quality" + 0.007*"East" + 0.007*"well" + 0.006*"Cheshire" + 0.005*"effective"', '0.010*"’" + 0.007*"2024" + 0.006*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"leaders" + 0.005*"always" + 0.005*"Cheshire" + 0.005*"practice" + 0.005*"need"']</t>
+    <t>['0.014*"’" + 0.008*"2024" + 0.008*"needs" + 0.008*"well" + 0.007*"practice" + 0.007*"quality" + 0.006*"plans" + 0.006*"leaders" + 0.006*"East" + 0.006*"Cheshire"', '0.010*"’" + 0.007*"2024" + 0.007*"plans" + 0.006*"practice" + 0.006*"Cheshire" + 0.005*"leaders" + 0.005*"well" + 0.005*"East" + 0.005*"effective" + 0.005*"needs"', '0.013*"’" + 0.009*"needs" + 0.007*"2024" + 0.007*"plans" + 0.006*"practice" + 0.006*"quality" + 0.006*"well" + 0.005*"East" + 0.005*"Cheshire" + 0.005*"always"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -721,7 +721,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"needs" + 0.007*"well" + 0.004*"learning" + 0.004*"receive" + 0.004*"impact" + 0.004*"order" + 0.003*"practice" + 0.003*"plans" + 0.003*"use"', '0.026*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"practice" + 0.005*"effectively" + 0.005*"order" + 0.005*"effective" + 0.005*"always" + 0.004*"plans" + 0.004*"impact"', '0.016*"’" + 0.008*"well" + 0.006*"needs" + 0.004*"plans" + 0.004*"practice" + 0.004*"impact" + 0.003*"timely" + 0.003*"use" + 0.003*"risks" + 0.003*"always"']</t>
+    <t>['0.023*"’" + 0.008*"needs" + 0.007*"well" + 0.005*"practice" + 0.005*"plans" + 0.005*"always" + 0.005*"impact" + 0.004*"receive" + 0.004*"learning" + 0.004*"effectively"', '0.022*"’" + 0.007*"well" + 0.007*"needs" + 0.004*"order" + 0.004*"practice" + 0.004*"good" + 0.004*"effectively" + 0.004*"information" + 0.004*"timely" + 0.004*"effective"', '0.019*"’" + 0.007*"well" + 0.006*"needs" + 0.004*"progress" + 0.004*"practice" + 0.004*"order" + 0.004*"effective" + 0.004*"early" + 0.004*"impact" + 0.004*"always"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -760,7 +760,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.027*"’" + 0.007*"plans" + 0.005*"risk" + 0.005*"2022" + 0.005*"Bradford" + 0.005*"impact" + 0.005*"need" + 0.005*"changes" + 0.004*"progress" + 0.004*"quality"', '0.018*"’" + 0.007*"plans" + 0.005*"needs" + 0.005*"2" + 0.005*"Bradford" + 0.005*"quality" + 0.004*"◼" + 0.004*"City" + 0.004*"Council" + 0.004*"need"', '0.011*"’" + 0.005*"needs" + 0.005*"plans" + 0.004*"worker" + 0.004*"impact" + 0.004*"Bradford" + 0.004*"2" + 0.004*"practice" + 0.004*"many" + 0.004*"November"']</t>
+    <t>['0.022*"’" + 0.006*"plans" + 0.006*"Bradford" + 0.006*"risk" + 0.005*"need" + 0.005*"2" + 0.005*"needs" + 0.005*"quality" + 0.005*"21" + 0.004*"impact"', '0.023*"’" + 0.007*"plans" + 0.005*"needs" + 0.005*"impact" + 0.005*"quality" + 0.005*"many" + 0.004*"lack" + 0.004*"Council" + 0.004*"Bradford" + 0.004*"senior"', '0.015*"’" + 0.007*"plans" + 0.004*"worker" + 0.004*"many" + 0.004*"2" + 0.004*"Bradford" + 0.004*"needs" + 0.004*"Council" + 0.004*"practice" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -796,7 +796,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"ensure" + 0.009*"needs" + 0.009*"well" + 0.007*"clear" + 0.006*"progress" + 0.006*"effective" + 0.006*"plans" + 0.006*"practice" + 0.005*"good"', '0.013*"needs" + 0.011*"’" + 0.010*"well" + 0.009*"ensure" + 0.007*"effective" + 0.006*"clear" + 0.005*"good" + 0.005*"within" + 0.005*"plans" + 0.005*"timely"', '0.012*"needs" + 0.012*"’" + 0.010*"well" + 0.008*"ensure" + 0.006*"progress" + 0.006*"effective" + 0.006*"plans" + 0.005*"good" + 0.005*"clear" + 0.005*"clearly"']</t>
+    <t>['0.013*"needs" + 0.012*"’" + 0.010*"well" + 0.010*"ensure" + 0.008*"effective" + 0.007*"clear" + 0.006*"progress" + 0.005*"supported" + 0.005*"plans" + 0.005*"good"', '0.014*"’" + 0.011*"needs" + 0.009*"well" + 0.008*"ensure" + 0.006*"progress" + 0.006*"effective" + 0.006*"good" + 0.006*"experiences" + 0.005*"plans" + 0.005*"within"', '0.010*"well" + 0.010*"needs" + 0.009*"’" + 0.007*"ensure" + 0.006*"clear" + 0.006*"practice" + 0.006*"plans" + 0.005*"good" + 0.005*"supported" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -835,7 +835,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.007*"quality" + 0.007*"leaders" + 0.007*"Wakefield" + 0.006*"good" + 0.006*"November" + 0.006*"effective" + 0.005*"needs" + 0.005*"timely"', '0.019*"’" + 0.009*"Wakefield" + 0.009*"quality" + 0.008*"leaders" + 0.008*"November" + 0.008*"well" + 0.008*"effective" + 0.007*"plans" + 0.007*"good" + 0.007*"practice"', '0.013*"’" + 0.006*"November" + 0.006*"good" + 0.005*"well" + 0.005*"quality" + 0.005*"plans" + 0.005*"leaders" + 0.005*"Wakefield" + 0.004*"progress" + 0.004*"effective"']</t>
+    <t>['0.018*"’" + 0.008*"Wakefield" + 0.008*"well" + 0.007*"good" + 0.007*"plans" + 0.007*"quality" + 0.006*"November" + 0.006*"leaders" + 0.006*"effective" + 0.006*"practice"', '0.016*"’" + 0.008*"leaders" + 0.008*"quality" + 0.007*"well" + 0.007*"Wakefield" + 0.007*"good" + 0.006*"November" + 0.005*"19" + 0.005*"effective" + 0.005*"8"', '0.016*"’" + 0.008*"November" + 0.008*"effective" + 0.008*"Wakefield" + 0.007*"quality" + 0.007*"well" + 0.007*"leaders" + 0.006*"progress" + 0.006*"plans" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -868,7 +868,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"needs" + 0.008*"March" + 0.006*"effective" + 0.006*"York" + 0.006*"quality" + 0.006*"training" + 0.005*"need" + 0.005*"good" + 0.005*"However"', '0.014*"’" + 0.007*"March" + 0.007*"quality" + 0.007*"needs" + 0.006*"effective" + 0.006*"plans" + 0.006*"However" + 0.005*"York" + 0.005*"supported" + 0.005*"well"', '0.012*"’" + 0.006*"quality" + 0.006*"ensure" + 0.005*"needs" + 0.005*"effective" + 0.005*"well" + 0.004*"March" + 0.004*"meet" + 0.004*"However" + 0.004*"need"']</t>
+    <t>['0.014*"’" + 0.007*"March" + 0.006*"quality" + 0.006*"needs" + 0.005*"well" + 0.005*"York" + 0.005*"However" + 0.005*"effective" + 0.005*"appropriate" + 0.005*"training"', '0.013*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"March" + 0.007*"effective" + 0.006*"plans" + 0.005*"However" + 0.005*"good" + 0.005*"7" + 0.005*"ensure"', '0.018*"’" + 0.008*"needs" + 0.007*"March" + 0.006*"quality" + 0.006*"effective" + 0.006*"ensure" + 0.005*"York" + 0.005*"However" + 0.004*"well" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -907,7 +907,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.015*"well" + 0.010*"’" + 0.008*"leaders" + 0.008*"effective" + 0.008*"quality" + 0.006*"good" + 0.005*"plans" + 0.004*"Senior" + 0.004*"timely" + 0.004*"arrangements"', '0.014*"’" + 0.014*"well" + 0.010*"quality" + 0.010*"leaders" + 0.009*"effective" + 0.006*"arrangements" + 0.006*"plans" + 0.006*"highly" + 0.005*"timely" + 0.005*"strong"', '0.015*"well" + 0.012*"’" + 0.010*"quality" + 0.009*"effective" + 0.008*"good" + 0.006*"leaders" + 0.006*"plans" + 0.006*"timely" + 0.006*"arrangements" + 0.005*"high"']</t>
+    <t>['0.019*"well" + 0.012*"’" + 0.010*"quality" + 0.009*"effective" + 0.008*"leaders" + 0.007*"good" + 0.006*"timely" + 0.006*"plans" + 0.005*"arrangements" + 0.005*"highly"', '0.011*"’" + 0.011*"well" + 0.010*"leaders" + 0.009*"quality" + 0.009*"effective" + 0.007*"plans" + 0.006*"arrangements" + 0.005*"good" + 0.005*"timely" + 0.005*"needs"', '0.013*"’" + 0.012*"well" + 0.009*"quality" + 0.007*"leaders" + 0.007*"effective" + 0.005*"ensure" + 0.005*"timely" + 0.005*"arrangements" + 0.005*"Senior" + 0.005*"targeted"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -940,7 +940,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"Isles" + 0.010*"Scilly" + 0.010*"need" + 0.009*"practice" + 0.007*"information" + 0.006*"protection" + 0.006*"needs" + 0.005*"place" + 0.005*"risks"', '0.027*"’" + 0.015*"Scilly" + 0.013*"Isles" + 0.010*"information" + 0.008*"practice" + 0.008*"need" + 0.007*"needs" + 0.007*"protection" + 0.007*"quality" + 0.007*"place"', '0.015*"’" + 0.011*"Isles" + 0.010*"Scilly" + 0.009*"practice" + 0.008*"information" + 0.006*"needs" + 0.006*"need" + 0.006*"protection" + 0.005*"risks" + 0.005*"ensure"']</t>
+    <t>['0.021*"’" + 0.012*"Scilly" + 0.011*"Isles" + 0.010*"practice" + 0.008*"information" + 0.008*"need" + 0.007*"protection" + 0.007*"quality" + 0.006*"needs" + 0.006*"place"', '0.017*"’" + 0.013*"Isles" + 0.010*"Scilly" + 0.009*"need" + 0.007*"information" + 0.007*"practice" + 0.006*"place" + 0.006*"protection" + 0.006*"needs" + 0.005*"risks"', '0.024*"’" + 0.013*"Scilly" + 0.012*"Isles" + 0.010*"information" + 0.008*"practice" + 0.008*"needs" + 0.008*"need" + 0.006*"protection" + 0.005*"place" + 0.005*"Leaders"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -976,7 +976,7 @@
     <t>0.1733</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"Coventry" + 0.007*"family" + 0.006*"needs" + 0.005*"supported" + 0.005*"plans" + 0.005*"strong" + 0.005*"well" + 0.004*"arrangements" + 0.004*"need"', '0.023*"’" + 0.009*"Coventry" + 0.009*"needs" + 0.008*"well" + 0.007*"supported" + 0.006*"plans" + 0.005*"family" + 0.005*"strong" + 0.005*"need" + 0.005*"1"', '0.016*"’" + 0.011*"well" + 0.007*"plans" + 0.007*"Coventry" + 0.007*"needs" + 0.007*"supported" + 0.006*"need" + 0.006*"strong" + 0.005*"family" + 0.005*"PAs"']</t>
+    <t>['0.028*"’" + 0.010*"Coventry" + 0.008*"well" + 0.008*"supported" + 0.007*"plans" + 0.007*"strong" + 0.007*"needs" + 0.007*"family" + 0.006*"need" + 0.005*"2022"', '0.009*"’" + 0.007*"Coventry" + 0.007*"well" + 0.007*"needs" + 0.006*"supported" + 0.006*"family" + 0.005*"need" + 0.004*"training" + 0.004*"plans" + 0.004*"However"', '0.012*"’" + 0.009*"well" + 0.009*"needs" + 0.005*"plans" + 0.005*"supported" + 0.005*"Coventry" + 0.004*"strong" + 0.004*"PAs" + 0.004*"use" + 0.003*"training"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -1018,7 +1018,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"leaders" + 0.006*"October" + 0.006*"Darlington" + 0.006*"practice" + 0.005*"family" + 0.005*"effective" + 0.005*"plans"', '0.014*"’" + 0.009*"well" + 0.007*"October" + 0.006*"leaders" + 0.006*"practice" + 0.006*"needs" + 0.006*"Darlington" + 0.005*"quality" + 0.005*"effective" + 0.004*"education"', '0.022*"’" + 0.008*"well" + 0.007*"leaders" + 0.006*"October" + 0.006*"needs" + 0.006*"practice" + 0.005*"Darlington" + 0.005*"supported" + 0.005*"quality" + 0.005*"effective"']</t>
+    <t>['0.022*"’" + 0.009*"well" + 0.007*"October" + 0.007*"practice" + 0.007*"leaders" + 0.006*"needs" + 0.005*"supported" + 0.005*"quality" + 0.005*"Darlington" + 0.005*"family"', '0.017*"’" + 0.008*"needs" + 0.007*"October" + 0.006*"well" + 0.006*"leaders" + 0.005*"practice" + 0.004*"21" + 0.004*"Darlington" + 0.004*"quality" + 0.004*"effective"', '0.015*"’" + 0.008*"well" + 0.008*"Darlington" + 0.007*"leaders" + 0.006*"practice" + 0.006*"needs" + 0.006*"effective" + 0.005*"October" + 0.005*"plans" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -1060,7 +1060,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.011*"needs" + 0.008*"Derby" + 0.008*"quality" + 0.007*"receive" + 0.006*"plans" + 0.006*"progress" + 0.005*"appropriate" + 0.005*"leaders" + 0.005*"need"', '0.013*"’" + 0.006*"needs" + 0.006*"Derby" + 0.005*"progress" + 0.005*"receive" + 0.004*"leaders" + 0.004*"well" + 0.004*"quality" + 0.004*"need" + 0.004*"good"', '0.024*"’" + 0.010*"needs" + 0.007*"Derby" + 0.006*"well" + 0.006*"appropriate" + 0.006*"good" + 0.006*"quality" + 0.006*"plans" + 0.006*"need" + 0.005*"leaders"']</t>
+    <t>['0.023*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"Derby" + 0.007*"receive" + 0.006*"progress" + 0.006*"need" + 0.006*"well" + 0.005*"plans" + 0.005*"leaders"', '0.020*"’" + 0.013*"needs" + 0.008*"Derby" + 0.007*"quality" + 0.006*"plans" + 0.006*"progress" + 0.006*"good" + 0.006*"receive" + 0.005*"leaders" + 0.005*"appropriate"', '0.019*"’" + 0.006*"needs" + 0.006*"Derby" + 0.005*"receive" + 0.005*"well" + 0.005*"appropriate" + 0.005*"need" + 0.005*"good" + 0.004*"plans" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80460</t>
@@ -1093,7 +1093,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"well" + 0.005*"Derbyshire" + 0.005*"effective" + 0.005*"plans" + 0.004*"positive" + 0.004*"10" + 0.004*"health" + 0.004*"need" + 0.004*"good"', '0.015*"’" + 0.009*"well" + 0.006*"Derbyshire" + 0.005*"need" + 0.005*"needs" + 0.005*"leaders" + 0.005*"good" + 0.004*"progress" + 0.004*"positive" + 0.004*"plans"', '0.014*"’" + 0.008*"Derbyshire" + 0.006*"well" + 0.005*"plans" + 0.005*"education" + 0.005*"positive" + 0.005*"needs" + 0.005*"effective" + 0.004*"number" + 0.004*"health"']</t>
+    <t>['0.011*"’" + 0.008*"well" + 0.007*"Derbyshire" + 0.005*"positive" + 0.005*"10" + 0.005*"health" + 0.005*"leaders" + 0.005*"practice" + 0.005*"good" + 0.004*"number"', '0.016*"’" + 0.008*"well" + 0.008*"Derbyshire" + 0.005*"positive" + 0.005*"plans" + 0.005*"need" + 0.005*"needs" + 0.005*"education" + 0.004*"2023" + 0.004*"leaders"', '0.015*"’" + 0.008*"well" + 0.005*"effective" + 0.005*"plans" + 0.005*"needs" + 0.005*"Derbyshire" + 0.004*"10" + 0.004*"30" + 0.004*"progress" + 0.004*"October"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1126,7 +1126,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.006*"’" + 0.005*"progress" + 0.004*"case" + 0.004*"well" + 0.004*"risk" + 0.004*"health" + 0.004*"quality" + 0.004*"practice" + 0.004*"information" + 0.004*"leaders"', '0.010*"’" + 0.007*"well" + 0.006*"risk" + 0.005*"progress" + 0.004*"leaders" + 0.004*"health" + 0.004*"key" + 0.004*"practice" + 0.004*"Devon" + 0.004*"protection"', '0.011*"’" + 0.006*"leaders" + 0.006*"well" + 0.005*"health" + 0.004*"time" + 0.004*"areas" + 0.004*"including" + 0.004*"Devon" + 0.004*"risk" + 0.004*"protection"']</t>
+    <t>['0.007*"’" + 0.005*"risk" + 0.005*"well" + 0.004*"health" + 0.004*"leaders" + 0.004*"protection" + 0.004*"risks" + 0.003*"including" + 0.003*"areas" + 0.003*"Devon"', '0.012*"’" + 0.007*"well" + 0.005*"progress" + 0.005*"leaders" + 0.004*"case" + 0.004*"risk" + 0.004*"living" + 0.004*"Devon" + 0.004*"protection" + 0.004*"health"', '0.008*"’" + 0.006*"well" + 0.005*"health" + 0.004*"practice" + 0.004*"quality" + 0.004*"progress" + 0.004*"leaders" + 0.004*"key" + 0.004*"risk" + 0.004*"risks"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1168,7 +1168,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"Doncaster" + 0.005*"well" + 0.004*"oversight" + 0.004*"progress" + 0.004*"many" + 0.004*"information" + 0.004*"arrangements" + 0.004*"plans" + 0.004*"records"', '0.024*"’" + 0.007*"well" + 0.007*"Doncaster" + 0.005*"progress" + 0.005*"records" + 0.005*"protection" + 0.005*"many" + 0.005*"leaders" + 0.005*"plans" + 0.005*"effective"', '0.018*"’" + 0.006*"well" + 0.006*"quality" + 0.005*"leaders" + 0.005*"Doncaster" + 0.005*"records" + 0.005*"many" + 0.005*"arrangements" + 0.005*"plans" + 0.004*"progress"']</t>
+    <t>['0.016*"’" + 0.006*"well" + 0.005*"many" + 0.005*"information" + 0.005*"Doncaster" + 0.005*"quality" + 0.005*"arrangements" + 0.005*"February" + 0.005*"plans" + 0.004*"progress"', '0.021*"’" + 0.006*"Doncaster" + 0.006*"progress" + 0.006*"well" + 0.005*"leaders" + 0.005*"many" + 0.005*"records" + 0.004*"effective" + 0.004*"protection" + 0.004*"oversight"', '0.023*"’" + 0.007*"well" + 0.006*"Doncaster" + 0.005*"quality" + 0.005*"records" + 0.005*"leaders" + 0.005*"plans" + 0.005*"oversight" + 0.005*"Trust" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>2532283</t>
@@ -1201,7 +1201,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"Dorset" + 0.007*"good" + 0.005*"well" + 0.005*"needs" + 0.004*"change" + 0.004*"quality" + 0.004*"including" + 0.004*"need" + 0.004*"arrangements"', '0.012*"’" + 0.008*"Dorset" + 0.005*"arrangements" + 0.005*"well" + 0.005*"2021" + 0.004*"good" + 0.004*"practice" + 0.004*"8" + 0.004*"including" + 0.004*"27"', '0.017*"’" + 0.007*"well" + 0.007*"good" + 0.006*"Dorset" + 0.005*"leaders" + 0.005*"needs" + 0.005*"impact" + 0.004*"8" + 0.004*"pandemic" + 0.004*"October"']</t>
+    <t>['0.007*"’" + 0.004*"Dorset" + 0.004*"good" + 0.004*"well" + 0.003*"27" + 0.003*"needs" + 0.003*"leaders" + 0.003*"impact" + 0.003*"quality" + 0.003*"Senior"', '0.018*"’" + 0.011*"Dorset" + 0.008*"good" + 0.006*"well" + 0.006*"arrangements" + 0.005*"needs" + 0.005*"need" + 0.004*"September" + 0.004*"pandemic" + 0.004*"2021"', '0.011*"’" + 0.006*"well" + 0.005*"Dorset" + 0.005*"impact" + 0.004*"including" + 0.004*"8" + 0.004*"good" + 0.004*"change" + 0.004*"quality" + 0.004*"October"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1234,7 +1234,7 @@
     <t>0.1605</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.013*"needs" + 0.009*"Dudley" + 0.006*"plans" + 0.005*"always" + 0.005*"arrangements" + 0.005*"enough" + 0.005*"oversight" + 0.005*"October" + 0.005*"quality"', '0.017*"’" + 0.013*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.005*"always" + 0.005*"ensure" + 0.005*"arrangements" + 0.004*"31" + 0.004*"However" + 0.004*"plans"', '0.014*"’" + 0.007*"Dudley" + 0.007*"needs" + 0.005*"well" + 0.005*"arrangements" + 0.005*"quality" + 0.005*"oversight" + 0.004*"plans" + 0.004*"always" + 0.004*"management"']</t>
+    <t>['0.015*"’" + 0.008*"Dudley" + 0.008*"needs" + 0.006*"plans" + 0.005*"arrangements" + 0.005*"well" + 0.005*"always" + 0.004*"October" + 0.004*"11" + 0.004*"2022"', '0.014*"’" + 0.008*"needs" + 0.006*"Dudley" + 0.006*"plans" + 0.005*"oversight" + 0.005*"well" + 0.005*"arrangements" + 0.004*"However" + 0.004*"quality" + 0.004*"ensure"', '0.015*"’" + 0.015*"needs" + 0.009*"Dudley" + 0.006*"always" + 0.006*"well" + 0.005*"ensure" + 0.005*"arrangements" + 0.005*"quality" + 0.004*"enough" + 0.004*"31"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1273,7 +1273,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.005*"May" + 0.005*"Durham" + 0.005*"well" + 0.004*"plans" + 0.004*"ensure" + 0.004*"needs" + 0.003*"20" + 0.003*"supported" + 0.003*"leaders"', '0.016*"’" + 0.014*"needs" + 0.008*"Durham" + 0.007*"May" + 0.007*"plans" + 0.007*"ensure" + 0.006*"well" + 0.005*"practice" + 0.005*"leaders" + 0.005*"risks"', '0.016*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"May" + 0.007*"plans" + 0.007*"Durham" + 0.006*"practice" + 0.005*"ensure" + 0.005*"family" + 0.005*"making"']</t>
+    <t>['0.016*"’" + 0.011*"needs" + 0.008*"Durham" + 0.007*"plans" + 0.006*"May" + 0.006*"well" + 0.005*"ensure" + 0.005*"leaders" + 0.005*"number" + 0.005*"risks"', '0.011*"’" + 0.008*"needs" + 0.007*"May" + 0.007*"plans" + 0.006*"well" + 0.006*"family" + 0.005*"ensure" + 0.004*"Durham" + 0.004*"practice" + 0.004*"risks"', '0.015*"’" + 0.012*"needs" + 0.008*"Durham" + 0.007*"well" + 0.007*"May" + 0.007*"practice" + 0.007*"ensure" + 0.005*"plans" + 0.005*"progress" + 0.005*"20"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1309,7 +1309,7 @@
     <t>0.1742</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.011*"plans" + 0.010*"needs" + 0.009*"well" + 0.006*"Riding" + 0.006*"progress" + 0.006*"East" + 0.006*"10" + 0.006*"education" + 0.005*"30"', '0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"progress" + 0.006*"plans" + 0.005*"Riding" + 0.005*"partners" + 0.004*"place" + 0.004*"good" + 0.004*"February"', '0.019*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"progress" + 0.008*"East" + 0.006*"Riding" + 0.006*"plans" + 0.005*"January" + 0.004*"good" + 0.004*"30"']</t>
+    <t>['0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"East" + 0.006*"plans" + 0.006*"progress" + 0.005*"Riding" + 0.004*"2023" + 0.004*"February" + 0.004*"partners"', '0.014*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"Riding" + 0.006*"East" + 0.006*"needs" + 0.006*"progress" + 0.005*"development" + 0.005*"10" + 0.005*"practice"', '0.018*"’" + 0.011*"needs" + 0.009*"plans" + 0.008*"well" + 0.008*"progress" + 0.006*"Riding" + 0.006*"good" + 0.006*"education" + 0.005*"10" + 0.005*"East"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1342,7 +1342,7 @@
     <t>0.1738</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"well" + 0.009*"plans" + 0.007*"progress" + 0.007*"East" + 0.006*"needs" + 0.006*"11" + 0.006*"Sussex" + 0.005*"impact" + 0.005*"including"', '0.015*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.006*"East" + 0.005*"progress" + 0.005*"relationships" + 0.005*"experiences" + 0.005*"including" + 0.005*"11"', '0.018*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"Sussex" + 0.007*"plans" + 0.007*"East" + 0.006*"including" + 0.005*"progress" + 0.005*"impact" + 0.005*"provide"']</t>
+    <t>['0.014*"’" + 0.007*"plans" + 0.006*"well" + 0.005*"Sussex" + 0.005*"needs" + 0.005*"including" + 0.005*"progress" + 0.005*"provide" + 0.004*"relationships" + 0.004*"East"', '0.016*"’" + 0.006*"well" + 0.006*"East" + 0.005*"progress" + 0.005*"needs" + 0.005*"plans" + 0.005*"including" + 0.005*"impact" + 0.004*"education" + 0.004*"Sussex"', '0.018*"’" + 0.013*"well" + 0.010*"needs" + 0.009*"plans" + 0.007*"East" + 0.007*"Sussex" + 0.007*"progress" + 0.006*"including" + 0.006*"impact" + 0.006*"11"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1381,7 +1381,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"well" + 0.006*"progress" + 0.006*"needs" + 0.006*"plans" + 0.005*"advisers" + 0.005*"Essex" + 0.005*"experiences" + 0.004*"provide" + 0.004*"family"', '0.019*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"progress" + 0.006*"needs" + 0.005*"understand" + 0.005*"family" + 0.005*"practice" + 0.004*"Essex" + 0.004*"‘"', '0.020*"’" + 0.007*"progress" + 0.006*"needs" + 0.006*"risk" + 0.006*"well" + 0.006*"family" + 0.005*"plans" + 0.005*"leaders" + 0.005*"Essex" + 0.005*"new"']</t>
+    <t>['0.017*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"progress" + 0.006*"needs" + 0.005*"quality" + 0.005*"family" + 0.005*"supported" + 0.005*"risk" + 0.005*"new"', '0.018*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"progress" + 0.005*"parents" + 0.005*"plans" + 0.005*"Essex" + 0.005*"leaders" + 0.005*"family" + 0.005*"experiences"', '0.018*"’" + 0.007*"progress" + 0.006*"needs" + 0.006*"well" + 0.006*"plans" + 0.006*"understand" + 0.005*"need" + 0.005*"family" + 0.005*"advisers" + 0.005*"Essex"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1420,7 +1420,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"effective" + 0.007*"needs" + 0.007*"quality" + 0.006*"good" + 0.006*"practice" + 0.006*"timely" + 0.006*"well" + 0.006*"early" + 0.004*"improve"', '0.015*"’" + 0.009*"effective" + 0.007*"practice" + 0.007*"good" + 0.006*"quality" + 0.005*"timely" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"need"', '0.011*"’" + 0.009*"effective" + 0.007*"good" + 0.006*"needs" + 0.006*"practice" + 0.006*"well" + 0.005*"quality" + 0.004*"timely" + 0.004*"home" + 0.004*"improve"']</t>
+    <t>['0.013*"’" + 0.007*"practice" + 0.007*"effective" + 0.007*"good" + 0.006*"quality" + 0.006*"well" + 0.006*"needs" + 0.005*"team" + 0.004*"early" + 0.004*"plans"', '0.014*"’" + 0.009*"effective" + 0.007*"quality" + 0.006*"good" + 0.005*"practice" + 0.005*"well" + 0.005*"needs" + 0.005*"timely" + 0.005*"need" + 0.005*"plans"', '0.014*"’" + 0.009*"effective" + 0.008*"good" + 0.007*"needs" + 0.006*"timely" + 0.006*"practice" + 0.005*"well" + 0.005*"quality" + 0.005*"early" + 0.005*"improve"']</t>
   </si>
   <si>
     <t>80470</t>
@@ -1456,7 +1456,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.010*"needs" + 0.006*"2022" + 0.006*"plans" + 0.006*"February" + 0.005*"progress" + 0.005*"Gloucestershire" + 0.004*"experienced" + 0.004*"protection" + 0.004*"7"', '0.015*"’" + 0.008*"February" + 0.007*"2022" + 0.006*"needs" + 0.006*"plans" + 0.005*"Gloucestershire" + 0.005*"experienced" + 0.005*"well" + 0.005*"need" + 0.005*"progress"', '0.018*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"2022" + 0.006*"February" + 0.005*"18" + 0.005*"family" + 0.005*"timely" + 0.005*"7"']</t>
+    <t>['0.015*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"2022" + 0.007*"February" + 0.006*"progress" + 0.005*"well" + 0.005*"leaders" + 0.005*"family" + 0.005*"protection"', '0.020*"’" + 0.007*"February" + 0.007*"needs" + 0.007*"2022" + 0.006*"plans" + 0.006*"experienced" + 0.006*"well" + 0.005*"Gloucestershire" + 0.005*"7" + 0.005*"good"', '0.015*"’" + 0.010*"needs" + 0.006*"2022" + 0.006*"plans" + 0.006*"February" + 0.005*"well" + 0.005*"Gloucestershire" + 0.005*"timely" + 0.004*"appropriate" + 0.004*"18"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1489,7 +1489,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"well" + 0.010*"practice" + 0.009*"needs" + 0.008*"plans" + 0.008*"risk" + 0.007*"effective" + 0.007*"need" + 0.006*"planning" + 0.005*"always"', '0.015*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"practice" + 0.007*"need" + 0.007*"plans" + 0.007*"good" + 0.007*"risk" + 0.006*"always" + 0.006*"oversight"', '0.010*"well" + 0.009*"’" + 0.007*"planning" + 0.007*"good" + 0.007*"quality" + 0.006*"plans" + 0.006*"needs" + 0.006*"practice" + 0.006*"cases" + 0.005*"need"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.008*"practice" + 0.007*"needs" + 0.007*"plans" + 0.006*"planning" + 0.006*"need" + 0.005*"good" + 0.005*"effective" + 0.005*"cases"', '0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"risk" + 0.007*"effective" + 0.006*"plans" + 0.006*"need" + 0.006*"quality" + 0.006*"practice" + 0.006*"always"', '0.013*"’" + 0.011*"well" + 0.009*"practice" + 0.008*"needs" + 0.008*"plans" + 0.007*"planning" + 0.007*"good" + 0.007*"need" + 0.007*"risk" + 0.006*"always"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1516,7 +1516,7 @@
     <t>0.1893</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"improve" + 0.004*"quality" + 0.004*"plans" + 0.004*"Hampshire" + 0.004*"leaders" + 0.004*"practice" + 0.004*"health"', '0.016*"’" + 0.006*"plans" + 0.005*"well" + 0.005*"needs" + 0.004*"home" + 0.004*"health" + 0.004*"strong" + 0.004*"progress" + 0.004*"leaders" + 0.003*"need"', '0.020*"’" + 0.011*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"quality" + 0.005*"leaders" + 0.005*"strong" + 0.004*"highly" + 0.004*"decisions" + 0.004*"home"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.006*"well" + 0.005*"quality" + 0.005*"strong" + 0.004*"plans" + 0.004*"Hampshire" + 0.004*"oversight" + 0.003*"leaders" + 0.003*"education"', '0.023*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"well" + 0.005*"home" + 0.005*"leaders" + 0.004*"highly" + 0.004*"improve" + 0.004*"strong" + 0.004*"progress"', '0.018*"’" + 0.007*"needs" + 0.005*"quality" + 0.004*"well" + 0.004*"plans" + 0.004*"leaders" + 0.004*"need" + 0.004*"strong" + 0.004*"improve" + 0.004*"plan"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1546,7 +1546,7 @@
     <t>0.2009</t>
   </si>
   <si>
-    <t>['0.028*"’" + 0.008*"March" + 0.008*"Hartlepool" + 0.007*"well" + 0.007*"needs" + 0.006*"leaders" + 0.006*"effective" + 0.005*"strong" + 0.005*"18" + 0.005*"ensure"', '0.012*"’" + 0.008*"needs" + 0.008*"Hartlepool" + 0.006*"March" + 0.006*"plans" + 0.005*"leaders" + 0.005*"well" + 0.005*"18" + 0.005*"clear" + 0.004*"need"', '0.011*"’" + 0.005*"March" + 0.004*"needs" + 0.004*"well" + 0.004*"Hartlepool" + 0.004*"supported" + 0.004*"leaders" + 0.004*"22" + 0.003*"practice" + 0.003*"18"']</t>
+    <t>['0.023*"’" + 0.008*"March" + 0.007*"Hartlepool" + 0.007*"needs" + 0.007*"well" + 0.005*"leaders" + 0.005*"strong" + 0.005*"supported" + 0.005*"22" + 0.005*"18"', '0.020*"’" + 0.009*"March" + 0.007*"Hartlepool" + 0.006*"needs" + 0.005*"need" + 0.005*"well" + 0.005*"leaders" + 0.005*"18" + 0.005*"plans" + 0.005*"effective"', '0.015*"’" + 0.007*"needs" + 0.007*"Hartlepool" + 0.006*"leaders" + 0.006*"well" + 0.005*"clear" + 0.005*"ensure" + 0.005*"practice" + 0.005*"March" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80474</t>
@@ -1579,7 +1579,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.006*"practice" + 0.005*"needs" + 0.005*"Herefordshire" + 0.005*"impact" + 0.005*"2022" + 0.005*"quality" + 0.005*"lack" + 0.004*"plans" + 0.004*"risk"', '0.017*"’" + 0.005*"Herefordshire" + 0.005*"lack" + 0.005*"many" + 0.005*"practice" + 0.004*"needs" + 0.004*"progress" + 0.004*"impact" + 0.004*"plans" + 0.004*"18"', '0.015*"’" + 0.006*"practice" + 0.005*"many" + 0.005*"Herefordshire" + 0.005*"lack" + 0.005*"impact" + 0.004*"needs" + 0.004*"agency" + 0.004*"plans" + 0.004*"oversight"']</t>
+    <t>['0.020*"’" + 0.005*"lack" + 0.005*"needs" + 0.005*"practice" + 0.005*"many" + 0.005*"impact" + 0.005*"quality" + 0.005*"Herefordshire" + 0.005*"progress" + 0.004*"plans"', '0.019*"’" + 0.006*"Herefordshire" + 0.006*"practice" + 0.005*"needs" + 0.005*"carers" + 0.005*"many" + 0.005*"plans" + 0.005*"lack" + 0.005*"impact" + 0.005*"18"', '0.009*"’" + 0.005*"practice" + 0.005*"lack" + 0.004*"impact" + 0.003*"29" + 0.003*"Herefordshire" + 0.003*"July" + 0.003*"management" + 0.003*"carers" + 0.003*"need"']</t>
   </si>
   <si>
     <t>80475</t>
@@ -1612,7 +1612,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"Hertfordshire" + 0.005*"need" + 0.005*"plans" + 0.004*"receive" + 0.004*"family" + 0.004*"education" + 0.004*"effective"', '0.022*"’" + 0.007*"Hertfordshire" + 0.006*"well" + 0.005*"needs" + 0.005*"receive" + 0.005*"plans" + 0.005*"‘" + 0.004*"positive" + 0.004*"27" + 0.004*"January"', '0.020*"’" + 0.006*"receive" + 0.005*"Hertfordshire" + 0.005*"needs" + 0.005*"well" + 0.004*"leaders" + 0.004*"risk" + 0.004*"2023" + 0.004*"effective" + 0.004*"plans"']</t>
+    <t>['0.023*"’" + 0.007*"needs" + 0.007*"Hertfordshire" + 0.007*"well" + 0.005*"receive" + 0.005*"plans" + 0.005*"‘" + 0.004*"family" + 0.004*"leaders" + 0.004*"2023"', '0.027*"’" + 0.007*"Hertfordshire" + 0.006*"well" + 0.006*"receive" + 0.006*"needs" + 0.005*"plans" + 0.004*"27" + 0.004*"need" + 0.004*"23" + 0.004*"positive"', '0.012*"’" + 0.006*"well" + 0.005*"needs" + 0.004*"risk" + 0.004*"Hertfordshire" + 0.004*"know" + 0.003*"family" + 0.003*"‘" + 0.003*"effective" + 0.003*"January"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1642,7 +1642,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.009*"leaders" + 0.008*"needs" + 0.006*"well" + 0.006*"Wight" + 0.006*"Isle" + 0.005*"plans" + 0.005*"Senior" + 0.005*"practice" + 0.005*"supported"', '0.012*"’" + 0.008*"leaders" + 0.005*"well" + 0.005*"3" + 0.005*"improve" + 0.005*"Senior" + 0.005*"Wight" + 0.004*"PAs" + 0.004*"Isle" + 0.004*"protection"', '0.014*"’" + 0.008*"leaders" + 0.006*"progress" + 0.005*"supported" + 0.005*"November" + 0.005*"well" + 0.005*"3" + 0.004*"PAs" + 0.004*"plans" + 0.004*"needs"']</t>
+    <t>['0.014*"’" + 0.006*"leaders" + 0.005*"well" + 0.005*"needs" + 0.005*"Isle" + 0.004*"PAs" + 0.004*"progress" + 0.004*"plans" + 0.004*"practice" + 0.004*"supported"', '0.021*"’" + 0.010*"leaders" + 0.006*"Senior" + 0.006*"well" + 0.006*"progress" + 0.006*"Isle" + 0.005*"supported" + 0.005*"needs" + 0.005*"improve" + 0.005*"practice"', '0.016*"’" + 0.008*"leaders" + 0.006*"Wight" + 0.006*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"3" + 0.005*"well" + 0.005*"protection" + 0.005*"supported"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1666,7 +1666,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"Kent" + 0.008*"well" + 0.007*"needs" + 0.006*"supported" + 0.005*"Council" + 0.005*"County" + 0.004*"including" + 0.004*"leaders" + 0.004*"progress"', '0.016*"’" + 0.009*"Kent" + 0.008*"Council" + 0.007*"needs" + 0.006*"County" + 0.005*"supported" + 0.005*"well" + 0.005*"progress" + 0.005*"practice" + 0.004*"2022"', '0.015*"’" + 0.011*"Kent" + 0.007*"needs" + 0.005*"supported" + 0.004*"well" + 0.004*"leaders" + 0.004*"9" + 0.004*"practice" + 0.004*"progress" + 0.004*"Council"']</t>
+    <t>['0.009*"’" + 0.007*"well" + 0.007*"Kent" + 0.005*"needs" + 0.004*"Council" + 0.004*"supported" + 0.004*"leaders" + 0.004*"council" + 0.004*"provide" + 0.003*"County"', '0.024*"’" + 0.009*"Kent" + 0.008*"needs" + 0.006*"supported" + 0.005*"well" + 0.005*"practice" + 0.005*"Council" + 0.004*"County" + 0.004*"including" + 0.004*"progress"', '0.018*"’" + 0.012*"Kent" + 0.007*"needs" + 0.007*"Council" + 0.006*"County" + 0.006*"well" + 0.006*"supported" + 0.006*"progress" + 0.005*"ensure" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1696,7 +1696,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"planning" + 0.006*"well" + 0.006*"number" + 0.006*"risks" + 0.005*"protection" + 0.005*"progress" + 0.005*"Hull" + 0.005*"small" + 0.005*"agency"', '0.015*"’" + 0.007*"planning" + 0.007*"practice" + 0.006*"number" + 0.006*"Hull" + 0.006*"need" + 0.006*"protection" + 0.005*"teams" + 0.005*"management" + 0.005*"25"', '0.015*"’" + 0.008*"number" + 0.006*"well" + 0.006*"practice" + 0.006*"protection" + 0.006*"management" + 0.005*"need" + 0.005*"planning" + 0.005*"risks" + 0.005*"Hull"']</t>
+    <t>['0.017*"’" + 0.007*"number" + 0.007*"well" + 0.007*"protection" + 0.006*"practice" + 0.006*"planning" + 0.006*"need" + 0.005*"Hull" + 0.005*"impact" + 0.005*"oversight"', '0.016*"’" + 0.007*"planning" + 0.007*"well" + 0.007*"management" + 0.007*"risks" + 0.006*"number" + 0.006*"practice" + 0.005*"needs" + 0.005*"need" + 0.005*"Hull"', '0.013*"’" + 0.007*"number" + 0.006*"protection" + 0.006*"planning" + 0.006*"Hull" + 0.006*"oversight" + 0.005*"practice" + 0.005*"need" + 0.005*"small" + 0.005*"14"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1729,7 +1729,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"quality" + 0.007*"good" + 0.006*"practice" + 0.006*"well" + 0.006*"Senior" + 0.005*"permanence" + 0.005*"plans" + 0.005*"senior" + 0.005*"need"', '0.012*"’" + 0.006*"practice" + 0.005*"permanence" + 0.005*"plans" + 0.005*"quality" + 0.005*"well" + 0.005*"good" + 0.004*"training" + 0.004*"protection" + 0.004*"needs"', '0.010*"’" + 0.007*"quality" + 0.006*"practice" + 0.006*"good" + 0.006*"protection" + 0.005*"needs" + 0.005*"training" + 0.005*"Senior" + 0.005*"plans" + 0.005*"senior"']</t>
+    <t>['0.011*"’" + 0.008*"practice" + 0.007*"quality" + 0.006*"well" + 0.005*"good" + 0.005*"protection" + 0.005*"Senior" + 0.005*"plans" + 0.005*"needs" + 0.005*"senior"', '0.009*"’" + 0.005*"quality" + 0.005*"practice" + 0.005*"training" + 0.004*"plans" + 0.004*"good" + 0.004*"needs" + 0.004*"well" + 0.004*"senior" + 0.004*"risk"', '0.014*"’" + 0.007*"good" + 0.007*"permanence" + 0.007*"quality" + 0.005*"plans" + 0.005*"protection" + 0.005*"training" + 0.005*"Senior" + 0.005*"practice" + 0.005*"needs"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1768,7 +1768,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"plans" + 0.006*"2021" + 0.006*"Knowsley" + 0.006*"progress" + 0.005*"impact" + 0.005*"risk" + 0.004*"experiences"', '0.019*"’" + 0.010*"progress" + 0.008*"plans" + 0.007*"quality" + 0.007*"Knowsley" + 0.006*"needs" + 0.006*"need" + 0.006*"22" + 0.005*"11" + 0.005*"abuse"', '0.012*"’" + 0.008*"progress" + 0.007*"needs" + 0.006*"quality" + 0.006*"plans" + 0.006*"good" + 0.005*"2021" + 0.005*"experiences" + 0.005*"Knowsley" + 0.004*"risk"']</t>
+    <t>['0.015*"’" + 0.010*"progress" + 0.007*"plans" + 0.007*"2021" + 0.007*"needs" + 0.007*"quality" + 0.006*"Knowsley" + 0.006*"experiences" + 0.005*"need" + 0.005*"good"', '0.015*"’" + 0.008*"quality" + 0.007*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"Knowsley" + 0.006*"abuse" + 0.005*"2021" + 0.005*"education" + 0.005*"domestic"', '0.012*"’" + 0.007*"progress" + 0.007*"needs" + 0.007*"plans" + 0.006*"Knowsley" + 0.004*"quality" + 0.004*"abuse" + 0.004*"experiences" + 0.004*"2021" + 0.004*"place"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1801,7 +1801,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"need" + 0.006*"Lancashire" + 0.006*"practice" + 0.005*"plans" + 0.005*"supported" + 0.004*"health" + 0.004*"live"', '0.020*"’" + 0.009*"well" + 0.008*"need" + 0.007*"needs" + 0.006*"supported" + 0.006*"Lancashire" + 0.005*"28" + 0.005*"parents" + 0.005*"progress" + 0.005*"live"', '0.013*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"Lancashire" + 0.005*"positive" + 0.005*"need" + 0.005*"plans" + 0.005*"information" + 0.005*"supported" + 0.004*"homes"']</t>
+    <t>['0.011*"’" + 0.008*"need" + 0.008*"well" + 0.008*"needs" + 0.006*"Lancashire" + 0.006*"positive" + 0.005*"parents" + 0.005*"progress" + 0.005*"homes" + 0.004*"plans"', '0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"need" + 0.005*"practice" + 0.005*"Lancashire" + 0.004*"progress" + 0.004*"supported" + 0.004*"live" + 0.004*"health"', '0.021*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"need" + 0.007*"Lancashire" + 0.006*"supported" + 0.006*"plans" + 0.005*"practice" + 0.005*"live" + 0.005*"health"']</t>
   </si>
   <si>
     <t>80481</t>
@@ -1831,7 +1831,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.007*"Leeds" + 0.005*"4" + 0.005*"2022" + 0.005*"well" + 0.005*"ensure" + 0.005*"supported" + 0.004*"March" + 0.004*"plans"', '0.020*"’" + 0.008*"needs" + 0.008*"Leeds" + 0.007*"risk" + 0.007*"well" + 0.005*"practice" + 0.005*"21" + 0.005*"benefit" + 0.005*"protection" + 0.005*"ensure"', '0.011*"’" + 0.007*"Leeds" + 0.005*"well" + 0.004*"needs" + 0.004*"practice" + 0.004*"supported" + 0.004*"plans" + 0.004*"protection" + 0.004*"4" + 0.003*"making"']</t>
+    <t>['0.017*"’" + 0.009*"Leeds" + 0.008*"needs" + 0.006*"risk" + 0.006*"well" + 0.005*"practice" + 0.005*"including" + 0.005*"2022" + 0.005*"making" + 0.005*"plans"', '0.014*"’" + 0.007*"Leeds" + 0.006*"well" + 0.006*"needs" + 0.005*"ensure" + 0.004*"4" + 0.004*"21" + 0.004*"risk" + 0.004*"February" + 0.004*"supported"', '0.016*"’" + 0.006*"needs" + 0.006*"Leeds" + 0.005*"well" + 0.005*"4" + 0.004*"practice" + 0.004*"protection" + 0.004*"risk" + 0.004*"benefit" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1867,7 +1867,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"Leicester" + 0.006*"2021" + 0.006*"needs" + 0.005*"good" + 0.005*"ensure" + 0.005*"October" + 0.005*"well" + 0.005*"20" + 0.005*"number"', '0.022*"’" + 0.010*"Leicester" + 0.009*"well" + 0.007*"needs" + 0.007*"2021" + 0.006*"good" + 0.006*"1" + 0.006*"ensure" + 0.006*"number" + 0.006*"including"', '0.019*"’" + 0.011*"2021" + 0.011*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"ensure" + 0.005*"September" + 0.005*"Council" + 0.005*"number" + 0.005*"1"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"2021" + 0.007*"Leicester" + 0.006*"good" + 0.006*"ensure" + 0.005*"including" + 0.005*"number" + 0.005*"1"', '0.022*"’" + 0.011*"2021" + 0.009*"well" + 0.009*"Leicester" + 0.007*"needs" + 0.006*"good" + 0.006*"20" + 0.005*"number" + 0.005*"1" + 0.005*"ensure"', '0.020*"’" + 0.008*"well" + 0.007*"2021" + 0.007*"Leicester" + 0.006*"ensure" + 0.005*"needs" + 0.005*"number" + 0.005*"good" + 0.005*"1" + 0.005*"including"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1903,7 +1903,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.007*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"effective" + 0.005*"impact" + 0.004*"quality" + 0.004*"practice" + 0.004*"education" + 0.003*"leaders"', '0.013*"’" + 0.010*"good" + 0.008*"well" + 0.008*"needs" + 0.007*"effective" + 0.007*"practice" + 0.006*"quality" + 0.006*"risk" + 0.005*"need" + 0.005*"leaders"', '0.011*"’" + 0.007*"well" + 0.007*"effective" + 0.006*"quality" + 0.005*"impact" + 0.005*"needs" + 0.005*"education" + 0.004*"good" + 0.004*"need" + 0.004*"practice"']</t>
+    <t>['0.013*"’" + 0.009*"well" + 0.007*"good" + 0.007*"effective" + 0.006*"practice" + 0.005*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"risk" + 0.004*"impact"', '0.010*"’" + 0.008*"needs" + 0.008*"good" + 0.008*"well" + 0.008*"quality" + 0.006*"impact" + 0.006*"effective" + 0.005*"practice" + 0.004*"protection" + 0.004*"risk"', '0.010*"’" + 0.007*"good" + 0.007*"well" + 0.007*"needs" + 0.006*"effective" + 0.006*"education" + 0.005*"quality" + 0.005*"practice" + 0.005*"leaders" + 0.004*"permanence"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1936,7 +1936,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"family" + 0.005*"plans" + 0.004*"number" + 0.004*"24" + 0.004*"progress" + 0.004*"28"', '0.022*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.005*"well" + 0.005*"need" + 0.005*"plans" + 0.005*"progress" + 0.005*"24" + 0.004*"working" + 0.004*"effective"', '0.021*"’" + 0.006*"well" + 0.005*"Lincolnshire" + 0.005*"needs" + 0.004*"plans" + 0.004*"progress" + 0.004*"family" + 0.004*"offer" + 0.004*"April" + 0.004*"supported"']</t>
+    <t>['0.022*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"24" + 0.005*"28" + 0.004*"progress" + 0.004*"supported" + 0.004*"need"', '0.015*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"family" + 0.005*"progress" + 0.004*"effective" + 0.004*"need" + 0.004*"plans" + 0.004*"24"', '0.026*"’" + 0.007*"Lincolnshire" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.004*"family" + 0.004*"offer" + 0.004*"2023" + 0.004*"number"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1966,7 +1966,7 @@
     <t>25/05/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.007*"practice" + 0.007*"always" + 0.005*"Liverpool" + 0.005*"need" + 0.005*"met" + 0.005*"PAs" + 0.005*"13" + 0.005*"quality"', '0.015*"’" + 0.007*"needs" + 0.006*"always" + 0.006*"practice" + 0.006*"Liverpool" + 0.005*"need" + 0.005*"protection" + 0.004*"24" + 0.004*"receive" + 0.004*"quality"', '0.026*"’" + 0.008*"need" + 0.007*"needs" + 0.007*"quality" + 0.007*"practice" + 0.006*"Liverpool" + 0.006*"always" + 0.005*"harm" + 0.004*"protection" + 0.004*"timely"']</t>
+    <t>['0.011*"’" + 0.007*"practice" + 0.006*"need" + 0.006*"always" + 0.005*"needs" + 0.005*"Liverpool" + 0.004*"timely" + 0.004*"impact" + 0.004*"met" + 0.004*"24"', '0.025*"’" + 0.007*"needs" + 0.007*"Liverpool" + 0.007*"always" + 0.007*"need" + 0.007*"practice" + 0.006*"quality" + 0.006*"protection" + 0.005*"PAs" + 0.005*"2023"', '0.016*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"practice" + 0.006*"need" + 0.005*"always" + 0.004*"24" + 0.004*"13" + 0.004*"protection" + 0.004*"planning"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1999,7 +1999,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.007*"needs" + 0.005*"good" + 0.005*"well" + 0.005*"London" + 0.005*"carers" + 0.004*"planning" + 0.004*"plans" + 0.004*"2023" + 0.004*"information"', '0.023*"’" + 0.009*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"information" + 0.005*"good" + 0.005*"carers" + 0.005*"e" + 0.005*"progress" + 0.004*"10"', '0.021*"’" + 0.008*"needs" + 0.007*"practice" + 0.006*"good" + 0.005*"plans" + 0.005*"carers" + 0.005*"progress" + 0.004*"Dagenham" + 0.004*"ensure" + 0.004*"well"']</t>
+    <t>['0.028*"’" + 0.009*"needs" + 0.007*"good" + 0.006*"plans" + 0.006*"carers" + 0.006*"progress" + 0.006*"well" + 0.005*"information" + 0.005*"practice" + 0.005*"Dagenham"', '0.018*"’" + 0.008*"needs" + 0.006*"plans" + 0.005*"well" + 0.004*"practice" + 0.004*"London" + 0.004*"information" + 0.004*"e" + 0.004*"2023" + 0.004*"leaders"', '0.013*"’" + 0.005*"needs" + 0.004*"good" + 0.004*"practice" + 0.004*"well" + 0.004*"carers" + 0.004*"plans" + 0.003*"timely" + 0.003*"progress" + 0.003*"e"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -2038,7 +2038,7 @@
     <t>0.2188</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.011*"well" + 0.010*"good" + 0.008*"needs" + 0.008*"need" + 0.006*"plans" + 0.006*"ensure" + 0.006*"progress" + 0.005*"risk" + 0.005*"quality"', '0.011*"needs" + 0.010*"’" + 0.009*"progress" + 0.008*"need" + 0.007*"well" + 0.007*"good" + 0.006*"clear" + 0.006*"ensure" + 0.005*"plans" + 0.005*"appropriate"', '0.014*"’" + 0.010*"good" + 0.009*"needs" + 0.007*"need" + 0.007*"well" + 0.006*"quality" + 0.006*"plans" + 0.006*"clear" + 0.005*"effective" + 0.005*"ensure"']</t>
+    <t>['0.015*"’" + 0.011*"well" + 0.010*"good" + 0.009*"needs" + 0.007*"need" + 0.007*"progress" + 0.006*"plans" + 0.006*"clear" + 0.005*"ensure" + 0.005*"risk"', '0.015*"’" + 0.009*"needs" + 0.009*"good" + 0.008*"need" + 0.007*"well" + 0.006*"progress" + 0.005*"plans" + 0.005*"quality" + 0.005*"ensure" + 0.005*"clear"', '0.011*"’" + 0.009*"needs" + 0.009*"good" + 0.007*"well" + 0.007*"need" + 0.006*"plans" + 0.006*"ensure" + 0.006*"clear" + 0.005*"quality" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80488</t>
@@ -2065,7 +2065,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"well" + 0.005*"need" + 0.005*"plans" + 0.005*"Bexley" + 0.005*"effective" + 0.004*"needs" + 0.004*"February" + 0.004*"progress" + 0.004*"including"', '0.020*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"Bexley" + 0.006*"need" + 0.005*"10" + 0.005*"effective" + 0.005*"6" + 0.005*"practice"', '0.022*"’" + 0.007*"needs" + 0.006*"effective" + 0.005*"well" + 0.005*"including" + 0.005*"need" + 0.004*"6" + 0.004*"oversight" + 0.004*"2023" + 0.004*"make"']</t>
+    <t>['0.012*"’" + 0.005*"Bexley" + 0.004*"needs" + 0.004*"effective" + 0.004*"need" + 0.004*"well" + 0.004*"including" + 0.004*"education" + 0.004*"plans" + 0.004*"ensure"', '0.022*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"effective" + 0.005*"plans" + 0.004*"Bexley" + 0.004*"clear" + 0.004*"make" + 0.004*"6"', '0.021*"’" + 0.006*"needs" + 0.006*"Bexley" + 0.006*"well" + 0.006*"plans" + 0.005*"effective" + 0.005*"10" + 0.005*"need" + 0.005*"practice" + 0.005*"6"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -2095,7 +2095,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"well" + 0.008*"leaders" + 0.005*"progress" + 0.005*"practice" + 0.005*"plans" + 0.005*"quality" + 0.005*"number" + 0.005*"small" + 0.005*"good"', '0.020*"’" + 0.010*"well" + 0.008*"plans" + 0.008*"leaders" + 0.007*"good" + 0.006*"progress" + 0.006*"Brent" + 0.006*"quality" + 0.006*"senior" + 0.006*"number"', '0.012*"’" + 0.007*"progress" + 0.006*"well" + 0.005*"plans" + 0.005*"Brent" + 0.005*"leaders" + 0.005*"number" + 0.004*"small" + 0.004*"needs" + 0.004*"good"']</t>
+    <t>['0.018*"’" + 0.008*"well" + 0.008*"leaders" + 0.007*"number" + 0.007*"plans" + 0.006*"Brent" + 0.006*"progress" + 0.005*"good" + 0.005*"practice" + 0.005*"information"', '0.020*"’" + 0.009*"well" + 0.008*"leaders" + 0.006*"progress" + 0.006*"plans" + 0.006*"quality" + 0.006*"practice" + 0.005*"good" + 0.005*"senior" + 0.005*"However"', '0.013*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"progress" + 0.006*"good" + 0.006*"quality" + 0.006*"senior" + 0.006*"leaders" + 0.005*"Brent" + 0.005*"family"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -2131,7 +2131,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"Bromley" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.005*"17" + 0.004*"relationships" + 0.004*"education" + 0.004*"plans" + 0.004*"strong"', '0.022*"’" + 0.009*"Bromley" + 0.008*"well" + 0.007*"needs" + 0.005*"plans" + 0.005*"leaders" + 0.004*"education" + 0.004*"understand" + 0.004*"health" + 0.004*"13"', '0.016*"’" + 0.008*"Bromley" + 0.007*"practice" + 0.007*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"leaders" + 0.005*"health" + 0.004*"education" + 0.004*"helping"']</t>
+    <t>['0.023*"’" + 0.009*"Bromley" + 0.009*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"leaders" + 0.005*"education" + 0.005*"health" + 0.004*"progress" + 0.004*"practice"', '0.009*"’" + 0.005*"leaders" + 0.005*"well" + 0.005*"plans" + 0.004*"needs" + 0.004*"health" + 0.004*"17" + 0.003*"practice" + 0.003*"Bromley" + 0.003*"strong"', '0.021*"’" + 0.011*"Bromley" + 0.008*"needs" + 0.006*"practice" + 0.006*"well" + 0.005*"plans" + 0.005*"leaders" + 0.005*"education" + 0.005*"helping" + 0.004*"strong"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -2164,7 +2164,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"Camden" + 0.006*"well" + 0.006*"practice" + 0.006*"leaders" + 0.005*"needs" + 0.005*"29" + 0.005*"protection" + 0.004*"progress" + 0.004*"response"', '0.009*"’" + 0.007*"Camden" + 0.006*"practice" + 0.006*"response" + 0.005*"25" + 0.005*"protection" + 0.005*"leaders" + 0.005*"appropriate" + 0.005*"needs" + 0.004*"well"', '0.011*"’" + 0.008*"leaders" + 0.007*"Camden" + 0.005*"practice" + 0.005*"well" + 0.005*"protection" + 0.005*"needs" + 0.004*"April" + 0.004*"2022" + 0.004*"meetings"']</t>
+    <t>['0.009*"’" + 0.007*"Camden" + 0.006*"practice" + 0.006*"leaders" + 0.005*"protection" + 0.004*"well" + 0.004*"29" + 0.004*"response" + 0.004*"25" + 0.004*"progress"', '0.012*"’" + 0.007*"leaders" + 0.007*"Camden" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"protection" + 0.005*"29" + 0.005*"appropriate" + 0.005*"response"', '0.010*"’" + 0.007*"Camden" + 0.006*"practice" + 0.006*"leaders" + 0.005*"well" + 0.005*"response" + 0.004*"meetings" + 0.004*"needs" + 0.004*"25" + 0.004*"appropriate"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -2197,7 +2197,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.006*"well" + 0.006*"Croydon" + 0.005*"good" + 0.005*"quality" + 0.005*"health" + 0.005*"ensure" + 0.005*"Senior" + 0.005*"risk" + 0.005*"arrangements"', '0.008*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"Croydon" + 0.005*"plans" + 0.005*"ensure" + 0.005*"Senior" + 0.005*"need" + 0.004*"However" + 0.004*"quality"', '0.015*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"need" + 0.006*"quality" + 0.006*"Senior" + 0.005*"effective" + 0.005*"good" + 0.005*"Croydon" + 0.005*"education"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.007*"Senior" + 0.007*"needs" + 0.006*"Croydon" + 0.006*"plans" + 0.005*"ensure" + 0.005*"risk" + 0.005*"health" + 0.005*"quality"', '0.010*"’" + 0.007*"needs" + 0.005*"well" + 0.005*"Croydon" + 0.005*"good" + 0.005*"need" + 0.005*"ensure" + 0.005*"effective" + 0.004*"quality" + 0.004*"experiences"', '0.012*"’" + 0.008*"needs" + 0.006*"quality" + 0.006*"well" + 0.006*"need" + 0.006*"Croydon" + 0.005*"good" + 0.005*"health" + 0.005*"effective" + 0.005*"improved"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2233,7 +2233,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.012*"quality" + 0.010*"’" + 0.007*"needs" + 0.007*"good" + 0.005*"progress" + 0.005*"plans" + 0.005*"risk" + 0.005*"leaders" + 0.005*"family" + 0.004*"management"', '0.011*"’" + 0.008*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"plans" + 0.005*"Ealing" + 0.004*"experiences" + 0.004*"well" + 0.004*"family" + 0.004*"teams"', '0.012*"’" + 0.007*"quality" + 0.007*"needs" + 0.006*"good" + 0.005*"progress" + 0.005*"risk" + 0.005*"well" + 0.005*"plans" + 0.004*"experiences" + 0.004*"oversight"']</t>
+    <t>['0.013*"’" + 0.011*"quality" + 0.008*"needs" + 0.007*"good" + 0.005*"progress" + 0.005*"plans" + 0.005*"Ealing" + 0.004*"well" + 0.004*"appropriately" + 0.004*"fully"', '0.010*"’" + 0.009*"quality" + 0.006*"good" + 0.006*"needs" + 0.005*"well" + 0.005*"risk" + 0.004*"plans" + 0.004*"progress" + 0.004*"experiences" + 0.004*"family"', '0.009*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"risk" + 0.006*"good" + 0.005*"experiences" + 0.005*"plans" + 0.005*"progress" + 0.005*"management" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80494</t>
@@ -2266,7 +2266,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"ensure" + 0.006*"effective" + 0.006*"good" + 0.006*"clear" + 0.006*"Enfield" + 0.005*"appropriate" + 0.005*"practice" + 0.005*"needs" + 0.005*"quality"', '0.016*"’" + 0.010*"practice" + 0.009*"needs" + 0.008*"good" + 0.007*"ensure" + 0.007*"quality" + 0.007*"timely" + 0.006*"effective" + 0.006*"clear" + 0.006*"Enfield"', '0.012*"’" + 0.010*"needs" + 0.007*"ensure" + 0.007*"good" + 0.006*"effective" + 0.006*"Enfield" + 0.006*"leaders" + 0.006*"practice" + 0.006*"clear" + 0.005*"timely"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.008*"effective" + 0.007*"ensure" + 0.007*"quality" + 0.007*"good" + 0.007*"practice" + 0.006*"leaders" + 0.006*"Enfield" + 0.006*"clear"', '0.014*"’" + 0.009*"ensure" + 0.008*"practice" + 0.008*"good" + 0.008*"clear" + 0.007*"needs" + 0.006*"Enfield" + 0.006*"effective" + 0.006*"timely" + 0.006*"leaders"', '0.013*"’" + 0.010*"needs" + 0.007*"practice" + 0.007*"Enfield" + 0.006*"timely" + 0.006*"effective" + 0.006*"progress" + 0.006*"need" + 0.006*"good" + 0.006*"improve"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2299,7 +2299,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.009*"good" + 0.008*"plans" + 0.007*"needs" + 0.007*"need" + 0.006*"range" + 0.006*"consistently" + 0.005*"risks" + 0.005*"timely"', '0.012*"’" + 0.012*"well" + 0.008*"needs" + 0.008*"good" + 0.008*"plans" + 0.006*"need" + 0.006*"range" + 0.006*"progress" + 0.006*"ensure" + 0.005*"effective"', '0.007*"well" + 0.006*"’" + 0.006*"needs" + 0.006*"good" + 0.005*"plans" + 0.004*"arrangements" + 0.004*"need" + 0.004*"progress" + 0.004*"ensure" + 0.003*"range"']</t>
+    <t>['0.012*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"good" + 0.006*"range" + 0.006*"ensure" + 0.005*"risk" + 0.005*"need" + 0.005*"progress"', '0.010*"’" + 0.010*"well" + 0.007*"plans" + 0.007*"needs" + 0.006*"good" + 0.005*"range" + 0.004*"need" + 0.004*"progress" + 0.004*"consistently" + 0.004*"effective"', '0.013*"’" + 0.010*"well" + 0.010*"good" + 0.008*"plans" + 0.008*"need" + 0.007*"needs" + 0.006*"range" + 0.006*"progress" + 0.006*"information" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2338,7 +2338,7 @@
     <t>0.1417</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"practice" + 0.007*"plans" + 0.006*"number" + 0.006*"needs" + 0.006*"quality" + 0.005*"within" + 0.005*"planning" + 0.005*"carers" + 0.005*"effective"', '0.012*"’" + 0.009*"practice" + 0.005*"number" + 0.005*"However" + 0.005*"quality" + 0.005*"planning" + 0.005*"effective" + 0.005*"leaders" + 0.005*"plans" + 0.005*"within"', '0.016*"’" + 0.011*"practice" + 0.007*"planning" + 0.007*"number" + 0.007*"effective" + 0.006*"including" + 0.006*"needs" + 0.006*"within" + 0.005*"However" + 0.005*"need"']</t>
+    <t>['0.015*"’" + 0.012*"practice" + 0.008*"number" + 0.006*"planning" + 0.006*"However" + 0.006*"leaders" + 0.006*"carers" + 0.006*"including" + 0.005*"making" + 0.005*"plans"', '0.014*"’" + 0.009*"practice" + 0.007*"effective" + 0.006*"quality" + 0.006*"needs" + 0.006*"plans" + 0.005*"within" + 0.005*"planning" + 0.005*"including" + 0.005*"cases"', '0.010*"’" + 0.008*"practice" + 0.006*"planning" + 0.006*"within" + 0.006*"number" + 0.006*"small" + 0.005*"quality" + 0.005*"needs" + 0.005*"including" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2371,7 +2371,7 @@
     <t>0.1986</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"well" + 0.005*"receive" + 0.005*"needs" + 0.005*"11" + 0.004*"Fulham" + 0.004*"protection" + 0.004*"effective" + 0.004*"Hammersmith" + 0.004*"plans"', '0.013*"’" + 0.006*"well" + 0.005*"receive" + 0.005*"needs" + 0.004*"plans" + 0.004*"Fulham" + 0.004*"timely" + 0.004*"leaders" + 0.004*"Hammersmith" + 0.004*"effective"', '0.016*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"receive" + 0.005*"Leaders" + 0.005*"2024" + 0.005*"Hammersmith" + 0.004*"plans" + 0.004*"Fulham" + 0.004*"leaders"']</t>
+    <t>['0.012*"’" + 0.007*"well" + 0.006*"receive" + 0.005*"needs" + 0.005*"plans" + 0.004*"Hammersmith" + 0.004*"effective" + 0.004*"supported" + 0.004*"11" + 0.004*"need"', '0.015*"’" + 0.006*"well" + 0.005*"receive" + 0.005*"Hammersmith" + 0.005*"needs" + 0.004*"Fulham" + 0.004*"plans" + 0.004*"Leaders" + 0.004*"effective" + 0.004*"leaders"', '0.017*"’" + 0.010*"well" + 0.005*"receive" + 0.005*"needs" + 0.005*"Fulham" + 0.004*"2024" + 0.004*"understand" + 0.004*"leaders" + 0.004*"11" + 0.004*"15"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2395,7 +2395,7 @@
     <t>13/02/2023</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"Haringey" + 0.008*"needs" + 0.007*"plans" + 0.006*"well" + 0.005*"need" + 0.005*"progress" + 0.004*"education" + 0.004*"good" + 0.004*"timely"', '0.013*"’" + 0.007*"plans" + 0.007*"Haringey" + 0.006*"needs" + 0.006*"need" + 0.005*"well" + 0.005*"risk" + 0.004*"good" + 0.004*"supported" + 0.004*"24"', '0.017*"’" + 0.009*"Haringey" + 0.008*"needs" + 0.007*"good" + 0.006*"plans" + 0.006*"well" + 0.005*"progress" + 0.004*"impact" + 0.004*"education" + 0.004*"risk"']</t>
+    <t>['0.017*"’" + 0.010*"Haringey" + 0.010*"needs" + 0.007*"well" + 0.006*"plans" + 0.005*"supported" + 0.004*"training" + 0.004*"good" + 0.004*"risk" + 0.004*"education"', '0.016*"’" + 0.006*"Haringey" + 0.006*"needs" + 0.005*"plans" + 0.005*"need" + 0.005*"progress" + 0.004*"supported" + 0.004*"well" + 0.004*"24" + 0.004*"training"', '0.014*"’" + 0.008*"plans" + 0.008*"Haringey" + 0.007*"good" + 0.007*"needs" + 0.006*"need" + 0.006*"progress" + 0.006*"well" + 0.004*"risk" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2428,7 +2428,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"needs" + 0.009*"well" + 0.009*"good" + 0.006*"experiences" + 0.005*"need" + 0.005*"plans" + 0.005*"practice" + 0.005*"protection" + 0.005*"early"', '0.012*"good" + 0.010*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"impact" + 0.005*"protection" + 0.005*"plans" + 0.005*"need" + 0.005*"school" + 0.005*"practice"', '0.010*"good" + 0.010*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"impact" + 0.005*"plans" + 0.005*"early" + 0.005*"practice" + 0.005*"school" + 0.004*"protection"']</t>
+    <t>['0.012*"’" + 0.010*"good" + 0.008*"needs" + 0.008*"well" + 0.006*"protection" + 0.005*"plans" + 0.005*"early" + 0.005*"impact" + 0.005*"experiences" + 0.005*"practice"', '0.011*"’" + 0.010*"good" + 0.008*"needs" + 0.008*"well" + 0.006*"practice" + 0.005*"plans" + 0.005*"need" + 0.005*"protection" + 0.005*"impact" + 0.005*"planning"', '0.012*"good" + 0.011*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"impact" + 0.005*"need" + 0.005*"plans" + 0.005*"experiences" + 0.004*"practice" + 0.004*"early"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2455,7 +2455,7 @@
     <t>16/02/24</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.015*"Havering" + 0.006*"plans" + 0.006*"oversight" + 0.006*"quality" + 0.006*"effective" + 0.005*"needs" + 0.004*"22" + 0.004*"11" + 0.004*"well"', '0.016*"’" + 0.011*"quality" + 0.010*"Havering" + 0.008*"plans" + 0.006*"effective" + 0.005*"oversight" + 0.005*"11" + 0.004*"many" + 0.004*"needs" + 0.004*"practice"', '0.018*"’" + 0.008*"quality" + 0.008*"Havering" + 0.006*"plans" + 0.005*"needs" + 0.004*"practice" + 0.004*"oversight" + 0.004*"many" + 0.004*"2023" + 0.004*"effective"']</t>
+    <t>['0.017*"’" + 0.010*"Havering" + 0.008*"plans" + 0.006*"quality" + 0.005*"effective" + 0.005*"11" + 0.004*"December" + 0.004*"oversight" + 0.004*"supported" + 0.004*"22"', '0.019*"’" + 0.012*"Havering" + 0.009*"quality" + 0.006*"plans" + 0.005*"oversight" + 0.005*"effective" + 0.005*"needs" + 0.005*"11" + 0.004*"22" + 0.004*"well"', '0.017*"’" + 0.012*"Havering" + 0.010*"quality" + 0.007*"plans" + 0.006*"oversight" + 0.005*"effective" + 0.005*"needs" + 0.005*"practice" + 0.004*"2023" + 0.004*"variable"']</t>
   </si>
   <si>
     <t>80501</t>
@@ -2488,7 +2488,7 @@
     <t>0.2119</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"needs" + 0.008*"Hillingdon" + 0.007*"well" + 0.007*"plans" + 0.005*"need" + 0.004*"team" + 0.004*"senior" + 0.004*"6" + 0.004*"family"', '0.022*"’" + 0.010*"needs" + 0.007*"Hillingdon" + 0.007*"well" + 0.006*"plans" + 0.005*"team" + 0.005*"6" + 0.005*"2" + 0.004*"2023" + 0.004*"family"', '0.013*"’" + 0.010*"needs" + 0.010*"plans" + 0.008*"Hillingdon" + 0.008*"well" + 0.005*"team" + 0.005*"need" + 0.004*"carers" + 0.004*"understand" + 0.004*"leaders"']</t>
+    <t>['0.023*"’" + 0.011*"needs" + 0.009*"Hillingdon" + 0.009*"well" + 0.008*"plans" + 0.006*"team" + 0.005*"need" + 0.005*"leaders" + 0.005*"2" + 0.004*"6"', '0.011*"’" + 0.006*"needs" + 0.006*"plans" + 0.006*"Hillingdon" + 0.005*"well" + 0.004*"6" + 0.004*"team" + 0.004*"carers" + 0.004*"2" + 0.003*"PAs"', '0.015*"’" + 0.009*"plans" + 0.009*"needs" + 0.007*"well" + 0.006*"Hillingdon" + 0.005*"PAs" + 0.004*"need" + 0.004*"2023" + 0.004*"carers" + 0.004*"detailed"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2521,7 +2521,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.013*"well" + 0.010*"needs" + 0.008*"effective" + 0.007*"Hounslow" + 0.006*"16" + 0.005*"strong" + 0.005*"experiences" + 0.004*"20" + 0.004*"plans"', '0.025*"’" + 0.012*"needs" + 0.010*"well" + 0.008*"timely" + 0.008*"Hounslow" + 0.008*"effective" + 0.006*"plans" + 0.005*"oversight" + 0.004*"leaders" + 0.004*"progress"', '0.019*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Hounslow" + 0.006*"effective" + 0.005*"plans" + 0.005*"timely" + 0.005*"progress" + 0.004*"experiences" + 0.004*"education"']</t>
+    <t>['0.015*"’" + 0.011*"needs" + 0.011*"well" + 0.007*"plans" + 0.007*"Hounslow" + 0.007*"effective" + 0.007*"timely" + 0.005*"progress" + 0.004*"oversight" + 0.004*"strong"', '0.016*"’" + 0.010*"needs" + 0.010*"well" + 0.006*"Hounslow" + 0.005*"effective" + 0.005*"strong" + 0.005*"timely" + 0.005*"16" + 0.004*"20" + 0.004*"plans"', '0.027*"’" + 0.011*"needs" + 0.010*"well" + 0.009*"effective" + 0.007*"Hounslow" + 0.006*"timely" + 0.005*"oversight" + 0.005*"plans" + 0.004*"experiences" + 0.004*"16"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2551,7 +2551,7 @@
     <t>0.209</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.012*"needs" + 0.011*"well" + 0.006*"good" + 0.006*"effective" + 0.006*"leaders" + 0.006*"plans" + 0.005*"quality" + 0.005*"Islington" + 0.005*"highly"', '0.010*"’" + 0.010*"well" + 0.010*"needs" + 0.007*"highly" + 0.005*"effective" + 0.005*"good" + 0.005*"Islington" + 0.005*"leaders" + 0.005*"practice" + 0.005*"quality"', '0.014*"’" + 0.011*"needs" + 0.010*"well" + 0.009*"plans" + 0.006*"quality" + 0.006*"highly" + 0.006*"good" + 0.005*"risk" + 0.005*"school" + 0.004*"leaders"']</t>
+    <t>['0.009*"well" + 0.008*"needs" + 0.007*"’" + 0.007*"plans" + 0.006*"highly" + 0.005*"Islington" + 0.004*"practice" + 0.004*"leaders" + 0.004*"good" + 0.004*"effective"', '0.016*"’" + 0.014*"needs" + 0.010*"well" + 0.008*"plans" + 0.007*"quality" + 0.006*"leaders" + 0.006*"good" + 0.006*"effective" + 0.005*"highly" + 0.005*"early"', '0.012*"’" + 0.011*"well" + 0.009*"needs" + 0.006*"good" + 0.006*"highly" + 0.005*"Islington" + 0.005*"effective" + 0.005*"risk" + 0.005*"quality" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2587,7 +2587,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"need" + 0.007*"Lambeth" + 0.007*"good" + 0.006*"impact" + 0.006*"progress" + 0.006*"4"', '0.013*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"Lambeth" + 0.006*"good" + 0.006*"progress" + 0.005*"impact" + 0.004*"leaders" + 0.004*"arrangements"', '0.011*"’" + 0.008*"needs" + 0.007*"plans" + 0.007*"well" + 0.007*"good" + 0.005*"Lambeth" + 0.005*"proceedings" + 0.005*"arrangements" + 0.005*"need" + 0.004*"leaders"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.009*"well" + 0.007*"plans" + 0.007*"good" + 0.007*"Lambeth" + 0.006*"need" + 0.006*"progress" + 0.005*"4" + 0.005*"arrangements"', '0.018*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"good" + 0.006*"impact" + 0.006*"plans" + 0.006*"need" + 0.006*"progress" + 0.005*"4" + 0.005*"leaders"', '0.011*"’" + 0.009*"plans" + 0.008*"needs" + 0.007*"well" + 0.007*"Lambeth" + 0.006*"good" + 0.006*"number" + 0.005*"progress" + 0.005*"impact" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2623,7 +2623,7 @@
     <t>0.1803</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"well" + 0.006*"Lewisham" + 0.005*"effective" + 0.005*"4" + 0.005*"arrangements" + 0.004*"benefit" + 0.004*"progress"', '0.012*"’" + 0.009*"needs" + 0.006*"well" + 0.006*"plans" + 0.005*"effective" + 0.005*"Lewisham" + 0.005*"good" + 0.005*"leaders" + 0.005*"progress" + 0.004*"4"', '0.021*"’" + 0.011*"well" + 0.007*"plans" + 0.007*"effective" + 0.006*"Lewisham" + 0.006*"needs" + 0.005*"progress" + 0.005*"good" + 0.005*"15" + 0.005*"ensure"']</t>
+    <t>['0.020*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"Lewisham" + 0.006*"4" + 0.005*"effective" + 0.005*"good" + 0.005*"progress" + 0.005*"appropriate"', '0.011*"’" + 0.006*"effective" + 0.005*"well" + 0.005*"needs" + 0.004*"plans" + 0.004*"Lewisham" + 0.004*"progress" + 0.004*"education" + 0.004*"benefit" + 0.004*"supported"', '0.018*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.007*"effective" + 0.006*"Lewisham" + 0.006*"need" + 0.006*"progress" + 0.005*"15" + 0.005*"December"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2647,7 +2647,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.006*"Merton" + 0.006*"needs" + 0.005*"family" + 0.005*"plans" + 0.005*"progress" + 0.005*"4" + 0.004*"good" + 0.004*"information"', '0.015*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"needs" + 0.004*"plans" + 0.004*"helping" + 0.004*"impact" + 0.004*"progress" + 0.004*"across" + 0.004*"2022"', '0.015*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"needs" + 0.004*"across" + 0.004*"ensure" + 0.004*"plans" + 0.004*"family" + 0.004*"health" + 0.004*"good"']</t>
+    <t>['0.016*"’" + 0.009*"well" + 0.008*"Merton" + 0.006*"needs" + 0.006*"plans" + 0.005*"progress" + 0.005*"family" + 0.005*"28" + 0.005*"helping" + 0.004*"good"', '0.014*"’" + 0.006*"well" + 0.005*"needs" + 0.005*"Merton" + 0.004*"progress" + 0.004*"good" + 0.004*"family" + 0.004*"ensure" + 0.004*"helping" + 0.004*"access"', '0.016*"’" + 0.008*"well" + 0.005*"needs" + 0.005*"4" + 0.005*"Merton" + 0.004*"leaders" + 0.004*"family" + 0.004*"plans" + 0.004*"information" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2671,7 +2671,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"needs" + 0.007*"effective" + 0.007*"practice" + 0.006*"Newham" + 0.006*"plans" + 0.006*"need" + 0.006*"progress" + 0.005*"good" + 0.005*"18"', '0.024*"’" + 0.008*"needs" + 0.007*"Newham" + 0.006*"progress" + 0.006*"plans" + 0.006*"need" + 0.005*"good" + 0.005*"practice" + 0.005*"effective" + 0.005*"well"', '0.014*"’" + 0.008*"needs" + 0.006*"Newham" + 0.006*"practice" + 0.006*"progress" + 0.005*"need" + 0.005*"plans" + 0.005*"effective" + 0.004*"18" + 0.004*"Leaders"']</t>
+    <t>['0.022*"’" + 0.009*"needs" + 0.007*"Newham" + 0.007*"effective" + 0.006*"progress" + 0.006*"practice" + 0.006*"plans" + 0.006*"need" + 0.006*"good" + 0.005*"ensure"', '0.019*"’" + 0.007*"needs" + 0.007*"Newham" + 0.006*"practice" + 0.006*"plans" + 0.006*"need" + 0.006*"progress" + 0.005*"effective" + 0.005*"Leaders" + 0.005*"well"', '0.015*"’" + 0.007*"needs" + 0.006*"Newham" + 0.006*"progress" + 0.006*"plans" + 0.006*"need" + 0.005*"practice" + 0.005*"effective" + 0.005*"good" + 0.004*"risks"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2701,7 +2701,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.008*"needs" + 0.007*"’" + 0.006*"well" + 0.006*"practice" + 0.005*"need" + 0.005*"risk" + 0.004*"Redbridge" + 0.004*"effective" + 0.004*"team" + 0.004*"management"', '0.009*"’" + 0.008*"practice" + 0.008*"well" + 0.006*"strong" + 0.006*"need" + 0.006*"needs" + 0.005*"effective" + 0.005*"Redbridge" + 0.005*"good" + 0.005*"team"', '0.006*"’" + 0.005*"Redbridge" + 0.005*"practice" + 0.005*"including" + 0.005*"effective" + 0.005*"progress" + 0.005*"risk" + 0.005*"need" + 0.005*"ensure" + 0.004*"strong"']</t>
+    <t>['0.007*"need" + 0.006*"needs" + 0.006*"’" + 0.005*"well" + 0.005*"practice" + 0.005*"ensure" + 0.005*"effective" + 0.005*"strong" + 0.005*"risk" + 0.004*"progress"', '0.007*"well" + 0.007*"’" + 0.006*"needs" + 0.006*"practice" + 0.006*"strong" + 0.006*"Redbridge" + 0.005*"progress" + 0.005*"need" + 0.005*"effective" + 0.005*"including"', '0.010*"’" + 0.009*"practice" + 0.005*"effective" + 0.005*"well" + 0.005*"need" + 0.005*"good" + 0.005*"Redbridge" + 0.005*"risk" + 0.005*"needs" + 0.005*"team"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2728,7 +2728,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"well" + 0.009*"Richmond" + 0.008*"needs" + 0.006*"supported" + 0.005*"4" + 0.005*"need" + 0.005*"good" + 0.005*"team" + 0.005*"strong"', '0.014*"well" + 0.013*"’" + 0.007*"Richmond" + 0.006*"good" + 0.005*"supported" + 0.005*"team" + 0.005*"needs" + 0.005*"ensure" + 0.005*"additional" + 0.005*"need"', '0.015*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Richmond" + 0.007*"need" + 0.006*"team" + 0.006*"good" + 0.005*"supported" + 0.005*"additional" + 0.005*"2022"']</t>
+    <t>['0.017*"’" + 0.013*"well" + 0.007*"needs" + 0.007*"need" + 0.007*"Richmond" + 0.006*"team" + 0.006*"good" + 0.005*"2022" + 0.005*"strong" + 0.005*"supported"', '0.013*"’" + 0.010*"well" + 0.007*"Richmond" + 0.007*"needs" + 0.006*"supported" + 0.005*"good" + 0.005*"team" + 0.005*"additional" + 0.005*"need" + 0.004*"range"', '0.015*"’" + 0.009*"Richmond" + 0.009*"well" + 0.007*"needs" + 0.007*"supported" + 0.005*"good" + 0.005*"Thames" + 0.005*"ensure" + 0.005*"team" + 0.004*"4"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2758,7 +2758,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"good" + 0.007*"Southwark" + 0.006*"progress" + 0.005*"well" + 0.004*"needs" + 0.004*"need" + 0.004*"effective" + 0.004*"education" + 0.004*"receive"', '0.023*"’" + 0.011*"Southwark" + 0.009*"needs" + 0.009*"well" + 0.008*"good" + 0.007*"need" + 0.006*"strong" + 0.006*"effective" + 0.006*"Leaders" + 0.005*"leaders"', '0.014*"’" + 0.008*"Southwark" + 0.008*"good" + 0.007*"progress" + 0.007*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"Leaders" + 0.005*"strong" + 0.005*"education"']</t>
+    <t>['0.015*"’" + 0.008*"Southwark" + 0.008*"good" + 0.007*"needs" + 0.007*"well" + 0.006*"progress" + 0.006*"strong" + 0.005*"receive" + 0.005*"plans" + 0.005*"practice"', '0.021*"’" + 0.008*"Southwark" + 0.008*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"progress" + 0.006*"effective" + 0.006*"good" + 0.005*"leaders" + 0.005*"plans"', '0.018*"’" + 0.011*"Southwark" + 0.010*"good" + 0.008*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"Leaders" + 0.005*"need" + 0.005*"strong" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2788,7 +2788,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.006*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"progress" + 0.005*"Sutton" + 0.005*"leaders" + 0.004*"6" + 0.004*"receive" + 0.004*"10"', '0.016*"’" + 0.008*"well" + 0.007*"Sutton" + 0.006*"needs" + 0.006*"effective" + 0.005*"supported" + 0.005*"progress" + 0.005*"need" + 0.005*"receive" + 0.004*"good"', '0.016*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"Sutton" + 0.005*"receive" + 0.005*"effective" + 0.005*"progress" + 0.005*"10" + 0.005*"6" + 0.004*"protection"']</t>
+    <t>['0.017*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"Sutton" + 0.005*"receive" + 0.005*"good" + 0.005*"progress" + 0.005*"effective" + 0.005*"6" + 0.004*"need"', '0.016*"’" + 0.007*"well" + 0.006*"Sutton" + 0.005*"needs" + 0.005*"progress" + 0.005*"effective" + 0.005*"receive" + 0.005*"good" + 0.004*"6" + 0.004*"need"', '0.017*"’" + 0.006*"well" + 0.005*"needs" + 0.005*"Sutton" + 0.005*"progress" + 0.004*"leaders" + 0.004*"6" + 0.004*"supported" + 0.004*"effective" + 0.004*"10"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2818,7 +2818,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"good" + 0.005*"‘" + 0.005*"practice" + 0.005*"plans" + 0.005*"effective" + 0.005*"including" + 0.004*"progress" + 0.004*"well" + 0.004*"need"', '0.015*"’" + 0.007*"good" + 0.006*"plans" + 0.006*"need" + 0.006*"effective" + 0.005*"‘" + 0.005*"practice" + 0.005*"progress" + 0.005*"well" + 0.005*"risk"', '0.015*"’" + 0.007*"effective" + 0.007*"well" + 0.006*"plans" + 0.006*"early" + 0.006*"‘" + 0.005*"good" + 0.005*"practice" + 0.005*"needs" + 0.005*"carers"']</t>
+    <t>['0.011*"’" + 0.005*"effective" + 0.005*"good" + 0.005*"well" + 0.005*"need" + 0.005*"plans" + 0.005*"early" + 0.004*"‘" + 0.004*"needs" + 0.004*"progress"', '0.018*"’" + 0.008*"plans" + 0.007*"good" + 0.006*"practice" + 0.006*"effective" + 0.006*"‘" + 0.005*"well" + 0.005*"progress" + 0.005*"needs" + 0.005*"early"', '0.013*"’" + 0.007*"good" + 0.007*"effective" + 0.006*"‘" + 0.006*"well" + 0.005*"including" + 0.005*"plans" + 0.005*"practice" + 0.005*"need" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2851,7 +2851,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.011*"well" + 0.009*"good" + 0.008*"needs" + 0.006*"need" + 0.006*"effective" + 0.005*"plans" + 0.004*"protection" + 0.004*"ensure" + 0.004*"risk"', '0.014*"’" + 0.010*"well" + 0.010*"needs" + 0.008*"good" + 0.008*"effective" + 0.006*"risk" + 0.006*"need" + 0.005*"plans" + 0.005*"timely" + 0.005*"information"', '0.016*"’" + 0.014*"well" + 0.008*"effective" + 0.008*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"plans" + 0.005*"timely" + 0.004*"receive" + 0.004*"clear"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.009*"well" + 0.009*"good" + 0.007*"effective" + 0.006*"need" + 0.005*"plans" + 0.005*"protection" + 0.004*"risk" + 0.004*"timely"', '0.015*"well" + 0.014*"’" + 0.010*"needs" + 0.009*"good" + 0.007*"effective" + 0.006*"need" + 0.006*"timely" + 0.005*"plans" + 0.005*"risk" + 0.005*"progress"', '0.015*"’" + 0.011*"well" + 0.007*"effective" + 0.006*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"need" + 0.004*"ensure" + 0.004*"information" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2878,7 +2878,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"quality" + 0.006*"progress" + 0.006*"effective" + 0.006*"well" + 0.006*"needs" + 0.005*"Senior" + 0.005*"good" + 0.005*"protection" + 0.005*"Wandsworth"', '0.011*"’" + 0.006*"practice" + 0.006*"well" + 0.006*"protection" + 0.005*"progress" + 0.005*"needs" + 0.005*"Senior" + 0.005*"7" + 0.005*"supported" + 0.005*"ensure"', '0.012*"’" + 0.008*"well" + 0.006*"Wandsworth" + 0.005*"practice" + 0.005*"needs" + 0.005*"team" + 0.005*"progress" + 0.004*"supported" + 0.004*"good" + 0.004*"2022"']</t>
+    <t>['0.009*"’" + 0.006*"well" + 0.005*"ensure" + 0.004*"good" + 0.004*"timely" + 0.004*"needs" + 0.004*"effective" + 0.004*"18" + 0.004*"progress" + 0.004*"practice"', '0.015*"’" + 0.007*"progress" + 0.006*"needs" + 0.006*"Wandsworth" + 0.006*"well" + 0.005*"protection" + 0.005*"Senior" + 0.005*"7" + 0.005*"supported" + 0.005*"quality"', '0.010*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"Senior" + 0.005*"protection" + 0.005*"effective" + 0.005*"needs" + 0.005*"progress" + 0.005*"18" + 0.004*"Wandsworth"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2911,7 +2911,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"needs" + 0.005*"highly" + 0.005*"practice" + 0.004*"many" + 0.004*"well" + 0.003*"direct" + 0.003*"shared" + 0.003*"risk" + 0.003*"skilled"', '0.011*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"highly" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.004*"family" + 0.003*"high" + 0.003*"protection"', '0.015*"’" + 0.008*"practice" + 0.006*"highly" + 0.006*"well" + 0.005*"needs" + 0.004*"across" + 0.004*"plans" + 0.004*"family" + 0.003*"many" + 0.003*"skilled"']</t>
+    <t>['0.010*"’" + 0.005*"practice" + 0.005*"highly" + 0.005*"needs" + 0.004*"many" + 0.004*"well" + 0.003*"across" + 0.003*"plans" + 0.003*"shared" + 0.003*"supported"', '0.016*"’" + 0.008*"practice" + 0.007*"needs" + 0.006*"highly" + 0.005*"well" + 0.004*"skilled" + 0.004*"family" + 0.004*"across" + 0.004*"shared" + 0.004*"high"', '0.010*"’" + 0.005*"well" + 0.005*"highly" + 0.005*"practice" + 0.005*"needs" + 0.004*"many" + 0.004*"across" + 0.003*"direct" + 0.003*"family" + 0.003*"number"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2944,7 +2944,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"need" + 0.007*"plans" + 0.006*"needs" + 0.006*"Luton" + 0.006*"good" + 0.005*"quality" + 0.005*"effective" + 0.005*"ensure" + 0.005*"well"', '0.014*"’" + 0.006*"need" + 0.006*"needs" + 0.005*"Luton" + 0.005*"impact" + 0.005*"effective" + 0.005*"plans" + 0.005*"good" + 0.004*"progress" + 0.004*"take"', '0.018*"’" + 0.007*"needs" + 0.006*"need" + 0.006*"plans" + 0.006*"impact" + 0.006*"Luton" + 0.006*"effective" + 0.005*"progress" + 0.005*"good" + 0.005*"receive"']</t>
+    <t>['0.020*"’" + 0.006*"need" + 0.006*"Luton" + 0.006*"effective" + 0.006*"needs" + 0.005*"ensure" + 0.005*"good" + 0.005*"impact" + 0.005*"well" + 0.005*"plans"', '0.014*"’" + 0.005*"needs" + 0.004*"need" + 0.004*"plans" + 0.004*"impact" + 0.004*"Luton" + 0.004*"progress" + 0.003*"ensure" + 0.003*"quality" + 0.003*"Leaders"', '0.017*"’" + 0.008*"plans" + 0.008*"need" + 0.007*"needs" + 0.006*"Luton" + 0.006*"good" + 0.006*"effective" + 0.006*"progress" + 0.005*"quality" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2971,7 +2971,7 @@
     <t>19/05/22</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.012*"Manchester" + 0.011*"needs" + 0.008*"well" + 0.007*"supported" + 0.007*"always" + 0.006*"protection" + 0.006*"plans" + 0.005*"disabled" + 0.005*"progress"', '0.015*"’" + 0.007*"Manchester" + 0.007*"needs" + 0.006*"supported" + 0.005*"effective" + 0.005*"always" + 0.005*"quality" + 0.005*"plans" + 0.005*"protection" + 0.005*"family"', '0.023*"’" + 0.011*"Manchester" + 0.009*"needs" + 0.007*"well" + 0.007*"always" + 0.006*"education" + 0.006*"supported" + 0.005*"family" + 0.005*"plans" + 0.005*"effective"']</t>
+    <t>['0.016*"’" + 0.009*"Manchester" + 0.007*"needs" + 0.006*"supported" + 0.005*"progress" + 0.005*"well" + 0.004*"education" + 0.004*"plans" + 0.004*"effective" + 0.004*"family"', '0.026*"’" + 0.011*"Manchester" + 0.010*"needs" + 0.008*"well" + 0.007*"supported" + 0.007*"always" + 0.006*"education" + 0.006*"disabled" + 0.005*"21" + 0.005*"protection"', '0.019*"’" + 0.010*"needs" + 0.010*"Manchester" + 0.007*"always" + 0.006*"well" + 0.006*"plans" + 0.006*"supported" + 0.005*"effective" + 0.005*"protection" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -3001,7 +3001,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"leaders" + 0.008*"Medway" + 0.007*"well" + 0.007*"practice" + 0.007*"needs" + 0.006*"quality" + 0.006*"impact" + 0.005*"progress" + 0.005*"28"', '0.016*"’" + 0.012*"Medway" + 0.008*"well" + 0.007*"oversight" + 0.007*"quality" + 0.007*"practice" + 0.007*"leaders" + 0.006*"needs" + 0.006*"experiences" + 0.006*"impact"', '0.019*"’" + 0.010*"practice" + 0.009*"quality" + 0.007*"Medway" + 0.007*"well" + 0.006*"risk" + 0.006*"needs" + 0.005*"oversight" + 0.005*"clear" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.007*"quality" + 0.007*"Medway" + 0.007*"needs" + 0.007*"well" + 0.006*"leaders" + 0.006*"practice" + 0.005*"Senior" + 0.005*"impact" + 0.005*"oversight"', '0.014*"’" + 0.009*"Medway" + 0.007*"well" + 0.007*"quality" + 0.006*"practice" + 0.006*"leaders" + 0.006*"needs" + 0.005*"impact" + 0.005*"oversight" + 0.005*"risk"', '0.017*"’" + 0.010*"Medway" + 0.010*"practice" + 0.009*"well" + 0.008*"quality" + 0.007*"oversight" + 0.007*"leaders" + 0.006*"needs" + 0.006*"experiences" + 0.006*"17"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -3025,7 +3025,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"effective" + 0.006*"Middlesbrough" + 0.006*"plans" + 0.006*"progress" + 0.006*"well" + 0.005*"needs" + 0.005*"place" + 0.005*"practice" + 0.004*"means"', '0.012*"’" + 0.007*"plans" + 0.007*"effective" + 0.006*"Middlesbrough" + 0.006*"well" + 0.005*"needs" + 0.005*"impact" + 0.005*"practice" + 0.005*"good" + 0.005*"risk"', '0.014*"’" + 0.007*"Middlesbrough" + 0.007*"well" + 0.007*"plans" + 0.007*"effective" + 0.007*"needs" + 0.006*"practice" + 0.006*"24" + 0.005*"progress" + 0.005*"means"']</t>
+    <t>['0.011*"’" + 0.008*"effective" + 0.007*"plans" + 0.006*"well" + 0.006*"Middlesbrough" + 0.005*"good" + 0.005*"practice" + 0.005*"needs" + 0.005*"March" + 0.005*"progress"', '0.012*"’" + 0.007*"plans" + 0.006*"effective" + 0.006*"needs" + 0.005*"practice" + 0.005*"well" + 0.005*"Middlesbrough" + 0.005*"progress" + 0.004*"planning" + 0.004*"good"', '0.016*"’" + 0.008*"Middlesbrough" + 0.007*"well" + 0.007*"plans" + 0.007*"needs" + 0.007*"effective" + 0.006*"practice" + 0.006*"progress" + 0.005*"place" + 0.005*"24"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -3052,7 +3052,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"Milton" + 0.006*"well" + 0.006*"2021" + 0.005*"good" + 0.004*"Keynes" + 0.004*"team" + 0.004*"need" + 0.004*"25" + 0.004*"5"', '0.012*"’" + 0.006*"well" + 0.006*"Milton" + 0.006*"need" + 0.006*"practice" + 0.005*"leaders" + 0.005*"Keynes" + 0.005*"team" + 0.004*"October" + 0.004*"family"', '0.019*"’" + 0.007*"Keynes" + 0.006*"need" + 0.005*"plans" + 0.005*"well" + 0.005*"Milton" + 0.005*"needs" + 0.005*"25" + 0.005*"leaders" + 0.005*"practice"']</t>
+    <t>['0.017*"’" + 0.006*"Milton" + 0.005*"Keynes" + 0.005*"well" + 0.005*"need" + 0.005*"25" + 0.005*"plans" + 0.005*"October" + 0.004*"practice" + 0.004*"education"', '0.016*"’" + 0.007*"Keynes" + 0.006*"well" + 0.005*"leaders" + 0.005*"need" + 0.005*"5" + 0.005*"practice" + 0.005*"Milton" + 0.005*"team" + 0.004*"family"', '0.011*"’" + 0.006*"Milton" + 0.005*"need" + 0.005*"well" + 0.005*"good" + 0.005*"2021" + 0.005*"Keynes" + 0.005*"November" + 0.004*"practice" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -3079,7 +3079,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.012*"plans" + 0.008*"good" + 0.008*"needs" + 0.007*"progress" + 0.006*"Newcastle" + 0.006*"protection" + 0.006*"making" + 0.006*"ensure" + 0.006*"management"', '0.015*"’" + 0.009*"plans" + 0.007*"needs" + 0.007*"protection" + 0.007*"Newcastle" + 0.006*"well" + 0.006*"making" + 0.005*"good" + 0.005*"ensure" + 0.004*"right"', '0.017*"’" + 0.010*"plans" + 0.008*"Newcastle" + 0.008*"needs" + 0.007*"well" + 0.007*"protection" + 0.006*"good" + 0.006*"10" + 0.006*"response" + 0.006*"progress"']</t>
+    <t>['0.016*"’" + 0.008*"Newcastle" + 0.008*"plans" + 0.007*"needs" + 0.006*"protection" + 0.005*"good" + 0.005*"ensure" + 0.005*"making" + 0.005*"well" + 0.005*"progress"', '0.017*"’" + 0.012*"plans" + 0.009*"needs" + 0.007*"protection" + 0.007*"progress" + 0.007*"good" + 0.007*"Newcastle" + 0.007*"well" + 0.006*"ensure" + 0.006*"making"', '0.014*"’" + 0.010*"plans" + 0.007*"good" + 0.007*"needs" + 0.007*"well" + 0.006*"10" + 0.006*"protection" + 0.006*"Newcastle" + 0.005*"need" + 0.005*"planning"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -3103,7 +3103,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"well" + 0.007*"Norfolk" + 0.006*"carers" + 0.006*"practice" + 0.005*"needs" + 0.005*"supported" + 0.005*"progress" + 0.004*"effective" + 0.004*"7"', '0.014*"’" + 0.007*"Norfolk" + 0.007*"well" + 0.006*"carers" + 0.005*"supported" + 0.005*"practice" + 0.005*"needs" + 0.004*"range" + 0.004*"18" + 0.004*"information"', '0.018*"’" + 0.009*"Norfolk" + 0.008*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"carers" + 0.005*"supported" + 0.005*"plans" + 0.005*"18" + 0.005*"range"']</t>
+    <t>['0.014*"’" + 0.009*"Norfolk" + 0.006*"needs" + 0.006*"well" + 0.006*"carers" + 0.005*"practice" + 0.005*"supported" + 0.004*"7" + 0.004*"family" + 0.004*"plans"', '0.019*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"Norfolk" + 0.005*"progress" + 0.005*"needs" + 0.004*"including" + 0.004*"supported" + 0.004*"practice" + 0.004*"18"', '0.017*"’" + 0.009*"well" + 0.009*"Norfolk" + 0.007*"practice" + 0.006*"supported" + 0.006*"needs" + 0.006*"carers" + 0.005*"range" + 0.005*"plans" + 0.005*"information"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -3136,7 +3136,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"leaders" + 0.007*"practice" + 0.006*"planning" + 0.006*"needs" + 0.006*"risk" + 0.005*"North" + 0.005*"many" + 0.005*"plans" + 0.005*"East"', '0.015*"’" + 0.009*"practice" + 0.006*"risk" + 0.006*"needs" + 0.006*"need" + 0.006*"planning" + 0.006*"leaders" + 0.005*"oversight" + 0.005*"experiences" + 0.004*"quality"', '0.010*"’" + 0.008*"risk" + 0.007*"practice" + 0.006*"planning" + 0.006*"leaders" + 0.006*"needs" + 0.005*"plans" + 0.005*"need" + 0.005*"Council" + 0.005*"North"']</t>
+    <t>['0.011*"’" + 0.009*"practice" + 0.006*"needs" + 0.005*"risk" + 0.005*"planning" + 0.005*"East" + 0.005*"many" + 0.005*"leaders" + 0.005*"need" + 0.004*"2021"', '0.017*"’" + 0.008*"planning" + 0.008*"risk" + 0.007*"leaders" + 0.007*"practice" + 0.006*"needs" + 0.006*"need" + 0.005*"plans" + 0.005*"October" + 0.005*"North"', '0.012*"’" + 0.008*"practice" + 0.006*"needs" + 0.006*"leaders" + 0.006*"risk" + 0.005*"East" + 0.005*"2021" + 0.005*"North" + 0.004*"Council" + 0.004*"many"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -3166,7 +3166,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.007*"‘" + 0.007*"North" + 0.007*"family" + 0.006*"Lincolnshire" + 0.006*"approach" + 0.005*"10" + 0.005*"need" + 0.005*"team" + 0.005*"council"', '0.022*"’" + 0.007*"‘" + 0.006*"leaders" + 0.006*"well" + 0.005*"family" + 0.005*"North" + 0.005*"approach" + 0.004*"Lincolnshire" + 0.004*"protection" + 0.004*"need"', '0.016*"’" + 0.008*"‘" + 0.005*"well" + 0.005*"Lincolnshire" + 0.005*"family" + 0.005*"leaders" + 0.004*"need" + 0.004*"10" + 0.004*"October" + 0.004*"approach"']</t>
+    <t>['0.022*"’" + 0.008*"‘" + 0.006*"leaders" + 0.006*"family" + 0.006*"approach" + 0.006*"North" + 0.005*"well" + 0.005*"10" + 0.005*"14" + 0.005*"Lincolnshire"', '0.023*"’" + 0.007*"‘" + 0.006*"Lincolnshire" + 0.006*"family" + 0.005*"North" + 0.005*"well" + 0.005*"2022" + 0.005*"council" + 0.005*"approach" + 0.005*"need"', '0.014*"’" + 0.006*"‘" + 0.005*"family" + 0.005*"need" + 0.004*"10" + 0.004*"protection" + 0.004*"North" + 0.004*"leaders" + 0.004*"Lincolnshire" + 0.004*"well"']</t>
   </si>
   <si>
     <t>2637539</t>
@@ -3202,7 +3202,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"Northamptonshire" + 0.006*"quality" + 0.006*"North" + 0.005*"practice" + 0.005*"needs" + 0.005*"impact" + 0.004*"NCT" + 0.004*"well" + 0.004*"Leaders"', '0.016*"’" + 0.008*"Northamptonshire" + 0.007*"well" + 0.006*"North" + 0.006*"Leaders" + 0.005*"3" + 0.005*"practice" + 0.005*"needs" + 0.005*"e" + 0.005*"quality"', '0.020*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"well" + 0.006*"quality" + 0.005*"impact" + 0.005*"NCT" + 0.005*"need" + 0.004*"practice" + 0.004*"experiences"']</t>
+    <t>['0.017*"’" + 0.009*"Northamptonshire" + 0.008*"North" + 0.007*"well" + 0.006*"quality" + 0.006*"Leaders" + 0.006*"NCT" + 0.006*"plans" + 0.005*"needs" + 0.005*"impact"', '0.009*"’" + 0.007*"Northamptonshire" + 0.006*"North" + 0.005*"quality" + 0.004*"2022" + 0.004*"well" + 0.004*"practice" + 0.004*"3" + 0.004*"needs" + 0.004*"NCT"', '0.021*"’" + 0.008*"Northamptonshire" + 0.006*"well" + 0.006*"North" + 0.005*"practice" + 0.005*"quality" + 0.005*"impact" + 0.005*"October" + 0.004*"need" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -3229,7 +3229,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"quality" + 0.008*"needs" + 0.006*"North" + 0.006*"progress" + 0.006*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"plans" + 0.005*"risk"', '0.016*"’" + 0.007*"quality" + 0.006*"number" + 0.006*"needs" + 0.006*"always" + 0.006*"Somerset" + 0.005*"practice" + 0.005*"need" + 0.005*"North" + 0.005*"appropriate"', '0.019*"’" + 0.007*"Somerset" + 0.006*"always" + 0.006*"needs" + 0.006*"quality" + 0.006*"North" + 0.006*"number" + 0.005*"experienced" + 0.005*"risk" + 0.005*"well"']</t>
+    <t>['0.016*"’" + 0.009*"quality" + 0.007*"always" + 0.006*"practice" + 0.006*"needs" + 0.005*"experienced" + 0.005*"13" + 0.005*"North" + 0.005*"Somerset" + 0.005*"well"', '0.014*"’" + 0.007*"needs" + 0.007*"quality" + 0.006*"need" + 0.005*"North" + 0.005*"progress" + 0.005*"Somerset" + 0.005*"always" + 0.004*"practice" + 0.004*"well"', '0.020*"’" + 0.007*"number" + 0.007*"needs" + 0.006*"Somerset" + 0.006*"quality" + 0.006*"North" + 0.006*"risk" + 0.006*"always" + 0.006*"practice" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -3256,7 +3256,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.007*"well" + 0.006*"need" + 0.006*"leaders" + 0.005*"quality" + 0.004*"make" + 0.004*"impact" + 0.004*"needs" + 0.004*"protection" + 0.004*"family"', '0.013*"’" + 0.006*"well" + 0.006*"leaders" + 0.005*"need" + 0.004*"make" + 0.004*"progress" + 0.004*"impact" + 0.004*"foster" + 0.004*"quality" + 0.004*"needs"', '0.016*"’" + 0.006*"well" + 0.005*"quality" + 0.005*"early" + 0.005*"needs" + 0.005*"leaders" + 0.005*"make" + 0.004*"clear" + 0.004*"need" + 0.004*"impact"']</t>
+    <t>['0.016*"’" + 0.007*"well" + 0.005*"quality" + 0.005*"need" + 0.005*"leaders" + 0.004*"early" + 0.004*"make" + 0.004*"needs" + 0.004*"progress" + 0.004*"impact"', '0.016*"’" + 0.007*"well" + 0.005*"need" + 0.005*"leaders" + 0.005*"needs" + 0.005*"quality" + 0.004*"impact" + 0.004*"make" + 0.004*"protection" + 0.004*"clear"', '0.015*"’" + 0.006*"leaders" + 0.006*"make" + 0.005*"well" + 0.005*"need" + 0.004*"impact" + 0.004*"needs" + 0.004*"early" + 0.004*"quality" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80530</t>
@@ -3286,7 +3286,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"well" + 0.006*"practice" + 0.006*"North" + 0.006*"Yorkshire" + 0.006*"needs" + 0.005*"family" + 0.005*"‘" + 0.004*"carers" + 0.004*"2023"', '0.021*"’" + 0.007*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.005*"needs" + 0.004*"family" + 0.004*"North" + 0.004*"3" + 0.004*"‘" + 0.004*"supported"', '0.021*"’" + 0.009*"well" + 0.008*"North" + 0.006*"family" + 0.006*"Yorkshire" + 0.006*"needs" + 0.006*"practice" + 0.005*"‘" + 0.005*"3" + 0.005*"7"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"family" + 0.005*"needs" + 0.005*"North" + 0.005*"‘" + 0.004*"3" + 0.004*"2023" + 0.004*"Yorkshire"', '0.020*"’" + 0.007*"North" + 0.007*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.006*"family" + 0.005*"needs" + 0.005*"‘" + 0.005*"need" + 0.004*"supported"', '0.024*"’" + 0.008*"well" + 0.008*"Yorkshire" + 0.007*"North" + 0.006*"needs" + 0.005*"family" + 0.005*"practice" + 0.005*"‘" + 0.005*"3" + 0.004*"7"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -3313,7 +3313,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.012*"well" + 0.010*"needs" + 0.007*"good" + 0.006*"education" + 0.006*"need" + 0.005*"impact" + 0.005*"quality" + 0.005*"experiences" + 0.005*"practice"', '0.022*"’" + 0.011*"needs" + 0.008*"good" + 0.008*"well" + 0.007*"need" + 0.006*"experiences" + 0.006*"practice" + 0.005*"always" + 0.005*"impact" + 0.005*"quality"', '0.019*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"good" + 0.006*"need" + 0.005*"experiences" + 0.005*"impact" + 0.005*"plans" + 0.004*"practice" + 0.004*"senior"']</t>
+    <t>['0.026*"’" + 0.011*"well" + 0.008*"needs" + 0.007*"need" + 0.007*"good" + 0.006*"practice" + 0.006*"education" + 0.006*"impact" + 0.005*"quality" + 0.005*"experiences"', '0.017*"’" + 0.010*"needs" + 0.007*"well" + 0.005*"need" + 0.005*"good" + 0.005*"impact" + 0.004*"education" + 0.004*"leaders" + 0.004*"experiences" + 0.004*"plans"', '0.021*"’" + 0.012*"needs" + 0.009*"good" + 0.008*"well" + 0.007*"experiences" + 0.006*"need" + 0.005*"practice" + 0.005*"quality" + 0.004*"impact" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3343,7 +3343,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"needs" + 0.006*"plans" + 0.005*"City" + 0.005*"Nottingham" + 0.005*"effective" + 0.005*"impact" + 0.005*"11" + 0.004*"risk" + 0.004*"oversight"', '0.011*"’" + 0.008*"needs" + 0.005*"plans" + 0.005*"Nottingham" + 0.004*"impact" + 0.004*"effective" + 0.004*"practice" + 0.004*"July" + 0.004*"oversight" + 0.004*"2022"', '0.015*"’" + 0.009*"needs" + 0.006*"effective" + 0.006*"Nottingham" + 0.005*"oversight" + 0.005*"impact" + 0.005*"However" + 0.005*"11" + 0.005*"plans" + 0.004*"practice"']</t>
+    <t>['0.012*"’" + 0.007*"needs" + 0.006*"Nottingham" + 0.005*"effective" + 0.005*"plans" + 0.005*"11" + 0.004*"impact" + 0.004*"practice" + 0.004*"City" + 0.004*"protection"', '0.014*"’" + 0.008*"needs" + 0.005*"Nottingham" + 0.005*"plans" + 0.005*"2022" + 0.005*"oversight" + 0.005*"effective" + 0.005*"risk" + 0.004*"City" + 0.004*"consistently"', '0.015*"’" + 0.009*"needs" + 0.006*"impact" + 0.006*"plans" + 0.005*"effective" + 0.005*"Nottingham" + 0.005*"11" + 0.005*"However" + 0.005*"City" + 0.005*"oversight"']</t>
   </si>
   <si>
     <t>80534</t>
@@ -3367,7 +3367,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"practice" + 0.007*"well" + 0.007*"ensure" + 0.006*"plans" + 0.006*"receive" + 0.006*"made" + 0.006*"needs" + 0.005*"quality" + 0.005*"carers"', '0.009*"’" + 0.009*"well" + 0.006*"needs" + 0.006*"practice" + 0.006*"areas" + 0.006*"quality" + 0.005*"good" + 0.005*"receive" + 0.005*"e" + 0.004*"number"', '0.011*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"progress" + 0.006*"needs" + 0.005*"plans" + 0.005*"receive" + 0.005*"carers" + 0.005*"made" + 0.004*"meetings"']</t>
+    <t>['0.008*"well" + 0.008*"’" + 0.005*"practice" + 0.005*"e" + 0.005*"receive" + 0.005*"progress" + 0.005*"plans" + 0.004*"ensure" + 0.004*"meetings" + 0.004*"education"', '0.018*"’" + 0.009*"well" + 0.008*"practice" + 0.006*"needs" + 0.006*"made" + 0.006*"receive" + 0.006*"ensure" + 0.006*"plans" + 0.005*"areas" + 0.005*"carers"', '0.008*"practice" + 0.007*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"quality" + 0.005*"progress" + 0.005*"receive" + 0.005*"made" + 0.004*"ensure" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3400,7 +3400,7 @@
     <t>04/03/19</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.010*"needs" + 0.008*"good" + 0.008*"practice" + 0.006*"quality" + 0.006*"effective" + 0.005*"progress" + 0.005*"well" + 0.005*"plans" + 0.005*"planning"', '0.011*"’" + 0.010*"good" + 0.010*"effective" + 0.009*"practice" + 0.009*"needs" + 0.007*"quality" + 0.007*"well" + 0.007*"planning" + 0.006*"plans" + 0.006*"progress"', '0.010*"’" + 0.009*"good" + 0.009*"needs" + 0.008*"practice" + 0.007*"progress" + 0.007*"effective" + 0.007*"well" + 0.006*"planning" + 0.005*"quality" + 0.005*"plans"']</t>
+    <t>['0.009*"good" + 0.008*"’" + 0.008*"needs" + 0.008*"practice" + 0.007*"effective" + 0.007*"quality" + 0.006*"planning" + 0.006*"well" + 0.005*"progress" + 0.005*"many"', '0.014*"’" + 0.010*"good" + 0.010*"needs" + 0.009*"effective" + 0.009*"practice" + 0.008*"well" + 0.007*"progress" + 0.007*"quality" + 0.006*"plans" + 0.006*"planning"', '0.009*"practice" + 0.008*"needs" + 0.008*"’" + 0.008*"good" + 0.007*"planning" + 0.006*"effective" + 0.006*"plans" + 0.006*"progress" + 0.005*"quality" + 0.004*"well"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3430,7 +3430,7 @@
     <t>0.1755</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"needs" + 0.009*"Oxfordshire" + 0.007*"well" + 0.006*"12" + 0.005*"receive" + 0.005*"risk" + 0.005*"education" + 0.005*"leaders" + 0.005*"supported"', '0.025*"’" + 0.011*"needs" + 0.008*"good" + 0.006*"Oxfordshire" + 0.006*"risk" + 0.006*"supported" + 0.006*"well" + 0.005*"quality" + 0.005*"arrangements" + 0.005*"practice"', '0.015*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"progress" + 0.005*"risk" + 0.005*"Oxfordshire" + 0.005*"practice" + 0.005*"supported" + 0.005*"23" + 0.004*"quality"']</t>
+    <t>['0.023*"’" + 0.011*"needs" + 0.007*"Oxfordshire" + 0.006*"risk" + 0.005*"well" + 0.005*"progress" + 0.005*"good" + 0.005*"leaders" + 0.005*"quality" + 0.005*"practice"', '0.018*"’" + 0.009*"needs" + 0.008*"supported" + 0.007*"Oxfordshire" + 0.006*"well" + 0.006*"good" + 0.006*"risk" + 0.005*"quality" + 0.005*"arrangements" + 0.005*"12"', '0.016*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"Oxfordshire" + 0.005*"good" + 0.005*"supported" + 0.005*"risk" + 0.004*"receive" + 0.004*"23" + 0.004*"quality"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3460,7 +3460,7 @@
     <t>30/01/24</t>
   </si>
   <si>
-    <t>['0.016*"needs" + 0.015*"’" + 0.006*"progress" + 0.006*"well" + 0.006*"Peterborough" + 0.006*"27" + 0.005*"need" + 0.005*"2023" + 0.005*"receive" + 0.005*"supported"', '0.011*"’" + 0.010*"needs" + 0.008*"need" + 0.007*"Peterborough" + 0.006*"well" + 0.006*"2023" + 0.006*"November" + 0.005*"plans" + 0.005*"progress" + 0.005*"December"', '0.016*"’" + 0.013*"needs" + 0.008*"need" + 0.008*"Peterborough" + 0.007*"2023" + 0.006*"well" + 0.006*"8" + 0.006*"progress" + 0.006*"supported" + 0.006*"plans"']</t>
+    <t>['0.019*"needs" + 0.014*"’" + 0.008*"Peterborough" + 0.007*"progress" + 0.007*"need" + 0.006*"2023" + 0.006*"well" + 0.005*"27" + 0.005*"supported" + 0.005*"December"', '0.015*"’" + 0.009*"needs" + 0.007*"Peterborough" + 0.007*"need" + 0.007*"well" + 0.006*"2023" + 0.005*"receive" + 0.005*"good" + 0.005*"8" + 0.005*"progress"', '0.015*"’" + 0.010*"needs" + 0.007*"need" + 0.006*"2023" + 0.006*"well" + 0.006*"plans" + 0.005*"8" + 0.005*"supported" + 0.005*"progress" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80538</t>
@@ -3490,7 +3490,7 @@
     <t>15/03/24</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"Plymouth" + 0.005*"appropriate" + 0.005*"risks" + 0.004*"practice" + 0.004*"ensure" + 0.004*"always" + 0.004*"education"', '0.013*"’" + 0.005*"plans" + 0.005*"Plymouth" + 0.005*"needs" + 0.005*"practice" + 0.005*"well" + 0.004*"22" + 0.004*"2024" + 0.004*"January" + 0.004*"2"', '0.014*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Plymouth" + 0.006*"practice" + 0.005*"education" + 0.005*"2" + 0.005*"2024" + 0.005*"appropriate" + 0.005*"good"']</t>
+    <t>['0.012*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"Plymouth" + 0.005*"2" + 0.005*"education" + 0.005*"practice" + 0.005*"risks" + 0.005*"plans" + 0.004*"appropriate"', '0.011*"’" + 0.010*"needs" + 0.007*"well" + 0.007*"Plymouth" + 0.005*"practice" + 0.005*"appropriate" + 0.005*"timely" + 0.005*"February" + 0.004*"plans" + 0.004*"benefit"', '0.015*"’" + 0.007*"needs" + 0.007*"Plymouth" + 0.006*"well" + 0.005*"effective" + 0.005*"practice" + 0.004*"2024" + 0.004*"education" + 0.004*"City" + 0.004*"January"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3523,7 +3523,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"Portsmouth" + 0.009*"care-experienced" + 0.008*"well" + 0.007*"needs" + 0.006*"family" + 0.006*"plans" + 0.005*"health" + 0.005*"progress" + 0.005*"19"', '0.018*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"care-experienced" + 0.005*"Portsmouth" + 0.004*"health" + 0.004*"early" + 0.004*"family" + 0.004*"risk" + 0.004*"foster"', '0.013*"’" + 0.008*"care-experienced" + 0.006*"needs" + 0.006*"family" + 0.006*"well" + 0.005*"plans" + 0.005*"health" + 0.005*"risk" + 0.005*"Portsmouth" + 0.004*"May"']</t>
+    <t>['0.023*"’" + 0.007*"Portsmouth" + 0.007*"care-experienced" + 0.006*"needs" + 0.005*"plans" + 0.005*"health" + 0.005*"well" + 0.005*"good" + 0.005*"practice" + 0.005*"family"', '0.015*"’" + 0.009*"well" + 0.007*"care-experienced" + 0.006*"needs" + 0.006*"family" + 0.005*"plans" + 0.005*"Portsmouth" + 0.004*"leaders" + 0.004*"receive" + 0.004*"offer"', '0.012*"’" + 0.009*"care-experienced" + 0.008*"Portsmouth" + 0.008*"well" + 0.007*"needs" + 0.006*"health" + 0.006*"family" + 0.005*"leaders" + 0.005*"progress" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3559,7 +3559,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"number" + 0.006*"quality" + 0.006*"plans" + 0.006*"well" + 0.006*"practice" + 0.005*"timely" + 0.005*"needs" + 0.005*"good" + 0.004*"ensure"', '0.012*"’" + 0.009*"number" + 0.007*"quality" + 0.006*"well" + 0.006*"good" + 0.006*"effective" + 0.006*"plans" + 0.005*"need" + 0.005*"However" + 0.005*"carers"', '0.021*"’" + 0.007*"quality" + 0.007*"well" + 0.006*"plans" + 0.006*"need" + 0.005*"good" + 0.005*"effective" + 0.005*"number" + 0.004*"timely" + 0.004*"However"']</t>
+    <t>['0.017*"’" + 0.008*"good" + 0.008*"number" + 0.006*"need" + 0.006*"plans" + 0.006*"quality" + 0.006*"well" + 0.005*"needs" + 0.005*"effective" + 0.005*"However"', '0.014*"’" + 0.007*"well" + 0.006*"plans" + 0.006*"quality" + 0.006*"number" + 0.005*"effective" + 0.005*"carers" + 0.005*"However" + 0.004*"ensure" + 0.004*"always"', '0.016*"’" + 0.007*"quality" + 0.007*"number" + 0.006*"well" + 0.005*"timely" + 0.005*"practice" + 0.005*"plans" + 0.005*"effective" + 0.005*"need" + 0.004*"arrangements"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3583,7 +3583,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"However" + 0.005*"consistently" + 0.005*"needs" + 0.005*"Redcar" + 0.005*"carers" + 0.005*"1" + 0.005*"risk"', '0.019*"’" + 0.007*"practice" + 0.006*"leaders" + 0.006*"However" + 0.006*"2022" + 0.006*"plans" + 0.006*"consistently" + 0.006*"needs" + 0.005*"20" + 0.005*"Cleveland"', '0.012*"’" + 0.006*"needs" + 0.005*"20" + 0.005*"plans" + 0.004*"consistently" + 0.004*"timely" + 0.004*"leaders" + 0.004*"However" + 0.004*"Redcar" + 0.004*"2022"']</t>
+    <t>['0.021*"’" + 0.007*"However" + 0.006*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.005*"consistently" + 0.005*"Cleveland" + 0.005*"ensure" + 0.005*"practice" + 0.004*"20"', '0.011*"’" + 0.008*"leaders" + 0.006*"plans" + 0.006*"2022" + 0.005*"response" + 0.005*"20" + 0.005*"needs" + 0.005*"consistently" + 0.005*"carers" + 0.005*"However"', '0.020*"’" + 0.006*"consistently" + 0.005*"However" + 0.005*"needs" + 0.005*"risk" + 0.005*"plans" + 0.005*"practice" + 0.005*"Cleveland" + 0.005*"Redcar" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3610,7 +3610,7 @@
     <t>17/03/23</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.011*"experienced" + 0.010*"needs" + 0.010*"practice" + 0.007*"response" + 0.006*"plans" + 0.006*"consistently" + 0.005*"good" + 0.005*"Rochdale" + 0.005*"PAs"', '0.019*"’" + 0.008*"experienced" + 0.007*"practice" + 0.006*"quality" + 0.006*"response" + 0.005*"consistently" + 0.005*"plans" + 0.005*"needs" + 0.005*"good" + 0.005*"Rochdale"', '0.014*"’" + 0.008*"experienced" + 0.006*"needs" + 0.006*"practice" + 0.005*"plans" + 0.005*"well" + 0.005*"quality" + 0.004*"23" + 0.004*"good" + 0.004*"3"']</t>
+    <t>['0.017*"’" + 0.008*"needs" + 0.008*"experienced" + 0.006*"response" + 0.006*"practice" + 0.006*"plans" + 0.006*"consistently" + 0.005*"3" + 0.005*"progress" + 0.005*"quality"', '0.020*"’" + 0.009*"practice" + 0.008*"experienced" + 0.006*"needs" + 0.005*"plans" + 0.005*"response" + 0.005*"quality" + 0.004*"consistently" + 0.004*"well" + 0.004*"good"', '0.023*"’" + 0.012*"experienced" + 0.008*"practice" + 0.008*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"consistently" + 0.006*"quality" + 0.006*"response" + 0.005*"Rochdale"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3637,7 +3637,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"Rotherham" + 0.007*"needs" + 0.005*"However" + 0.005*"good" + 0.005*"Council" + 0.005*"well" + 0.005*"ensure" + 0.005*"plans" + 0.005*"27"', '0.012*"’" + 0.008*"Rotherham" + 0.006*"needs" + 0.005*"well" + 0.005*"ensure" + 0.005*"good" + 0.004*"plans" + 0.004*"Council" + 0.004*"June" + 0.004*"receive"', '0.011*"’" + 0.007*"Rotherham" + 0.006*"needs" + 0.005*"well" + 0.005*"good" + 0.004*"protection" + 0.004*"clear" + 0.004*"Council" + 0.004*"Metropolitan" + 0.004*"However"']</t>
+    <t>['0.013*"’" + 0.006*"Rotherham" + 0.005*"needs" + 0.005*"Council" + 0.005*"well" + 0.004*"However" + 0.004*"good" + 0.004*"ensure" + 0.004*"protection" + 0.004*"Borough"', '0.014*"’" + 0.009*"Rotherham" + 0.006*"needs" + 0.006*"good" + 0.005*"However" + 0.005*"well" + 0.005*"ensure" + 0.005*"Metropolitan" + 0.004*"1" + 0.004*"clear"', '0.017*"’" + 0.010*"Rotherham" + 0.008*"needs" + 0.006*"well" + 0.005*"Council" + 0.005*"plans" + 0.005*"ensure" + 0.005*"good" + 0.004*"progress" + 0.004*"Borough"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3664,7 +3664,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.012*"well" + 0.012*"’" + 0.011*"practice" + 0.007*"strong" + 0.006*"highly" + 0.006*"effective" + 0.005*"needs" + 0.005*"leaders" + 0.004*"high" + 0.004*"improve"', '0.015*"well" + 0.011*"’" + 0.010*"practice" + 0.008*"highly" + 0.006*"needs" + 0.006*"leaders" + 0.006*"effective" + 0.006*"strong" + 0.004*"professionals" + 0.004*"high"', '0.013*"well" + 0.011*"’" + 0.010*"practice" + 0.008*"highly" + 0.006*"strong" + 0.005*"needs" + 0.004*"high" + 0.004*"leaders" + 0.004*"effective" + 0.004*"range"']</t>
+    <t>['0.014*"well" + 0.010*"’" + 0.009*"practice" + 0.007*"highly" + 0.007*"strong" + 0.005*"effective" + 0.005*"needs" + 0.005*"high" + 0.004*"professionals" + 0.004*"progress"', '0.014*"’" + 0.010*"practice" + 0.010*"well" + 0.005*"strong" + 0.005*"leaders" + 0.005*"needs" + 0.005*"highly" + 0.005*"high" + 0.004*"effective" + 0.004*"excellent"', '0.016*"well" + 0.012*"practice" + 0.011*"’" + 0.009*"highly" + 0.007*"strong" + 0.006*"needs" + 0.006*"leaders" + 0.006*"effective" + 0.004*"range" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3694,7 +3694,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"good" + 0.004*"clear" + 0.004*"need" + 0.004*"range" + 0.004*"effective" + 0.004*"progress"', '0.015*"’" + 0.008*"plans" + 0.007*"well" + 0.007*"needs" + 0.005*"good" + 0.005*"supported" + 0.004*"practice" + 0.004*"need" + 0.004*"parents" + 0.004*"effective"', '0.013*"’" + 0.010*"well" + 0.010*"plans" + 0.008*"needs" + 0.005*"effective" + 0.005*"good" + 0.005*"practice" + 0.005*"clear" + 0.004*"risk" + 0.004*"need"']</t>
+    <t>['0.013*"’" + 0.008*"needs" + 0.008*"plans" + 0.007*"well" + 0.004*"practice" + 0.004*"need" + 0.004*"risk" + 0.004*"parents" + 0.004*"effective" + 0.004*"good"', '0.012*"’" + 0.008*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"good" + 0.005*"effective" + 0.004*"clear" + 0.004*"range" + 0.004*"progress" + 0.004*"need"', '0.015*"’" + 0.011*"well" + 0.009*"plans" + 0.008*"needs" + 0.005*"good" + 0.005*"effective" + 0.005*"clear" + 0.005*"practice" + 0.004*"need" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3724,7 +3724,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.008*"’" + 0.005*"quality" + 0.005*"plans" + 0.004*"well" + 0.004*"actions" + 0.004*"effective" + 0.004*"good" + 0.004*"information" + 0.004*"informed" + 0.003*"However"', '0.009*"’" + 0.005*"well" + 0.004*"needs" + 0.004*"actions" + 0.004*"plans" + 0.004*"quality" + 0.004*"always" + 0.004*"case" + 0.003*"use" + 0.003*"oversight"', '0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"quality" + 0.005*"benefit" + 0.004*"health" + 0.004*"plans" + 0.004*"information" + 0.004*"use" + 0.004*"effective"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"plans" + 0.004*"benefit" + 0.004*"quality" + 0.004*"effective" + 0.004*"information" + 0.004*"always" + 0.003*"early"', '0.011*"’" + 0.004*"quality" + 0.004*"plans" + 0.004*"well" + 0.004*"information" + 0.004*"use" + 0.004*"effective" + 0.004*"needs" + 0.004*"health" + 0.003*"early"', '0.013*"’" + 0.006*"well" + 0.005*"quality" + 0.005*"needs" + 0.005*"actions" + 0.004*"use" + 0.004*"However" + 0.004*"benefit" + 0.004*"plans" + 0.004*"information"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3748,7 +3748,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"good" + 0.006*"ensure" + 0.006*"need" + 0.006*"effective" + 0.006*"enough" + 0.005*"practice" + 0.005*"team"', '0.015*"’" + 0.011*"needs" + 0.010*"well" + 0.009*"good" + 0.008*"need" + 0.007*"team" + 0.007*"protection" + 0.007*"practice" + 0.006*"plans" + 0.006*"effective"', '0.011*"well" + 0.010*"’" + 0.009*"needs" + 0.006*"team" + 0.006*"good" + 0.005*"practice" + 0.005*"ensure" + 0.005*"plans" + 0.005*"enough" + 0.004*"quality"']</t>
+    <t>['0.013*"’" + 0.012*"well" + 0.009*"needs" + 0.008*"team" + 0.007*"need" + 0.007*"practice" + 0.006*"enough" + 0.006*"good" + 0.005*"protection" + 0.005*"ensure"', '0.012*"’" + 0.011*"needs" + 0.009*"well" + 0.009*"good" + 0.007*"plans" + 0.006*"protection" + 0.006*"practice" + 0.006*"need" + 0.006*"ensure" + 0.005*"team"', '0.013*"’" + 0.008*"well" + 0.008*"good" + 0.007*"needs" + 0.006*"effective" + 0.006*"need" + 0.005*"ensure" + 0.005*"practice" + 0.005*"team" + 0.005*"enough"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3775,7 +3775,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"well" + 0.007*"effective" + 0.007*"plans" + 0.007*"needs" + 0.006*"Salford" + 0.005*"planning" + 0.005*"leaders" + 0.005*"practice" + 0.004*"2023"', '0.011*"’" + 0.006*"plans" + 0.006*"effective" + 0.006*"needs" + 0.006*"well" + 0.005*"Salford" + 0.005*"practice" + 0.005*"planning" + 0.004*"appropriate" + 0.004*"quality"', '0.018*"’" + 0.009*"plans" + 0.008*"needs" + 0.007*"well" + 0.006*"Salford" + 0.006*"effective" + 0.005*"practice" + 0.005*"progress" + 0.005*"planning" + 0.005*"experiences"']</t>
+    <t>['0.013*"’" + 0.008*"Salford" + 0.008*"plans" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.005*"6" + 0.005*"planning" + 0.005*"progress" + 0.005*"experiences"', '0.016*"’" + 0.008*"plans" + 0.008*"effective" + 0.007*"well" + 0.007*"needs" + 0.006*"planning" + 0.005*"10" + 0.005*"2023" + 0.005*"practice" + 0.005*"quality"', '0.011*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"needs" + 0.006*"effective" + 0.006*"practice" + 0.005*"Salford" + 0.004*"ensures" + 0.004*"impact" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3799,7 +3799,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.008*"plans" + 0.008*"well" + 0.008*"Sandwell" + 0.006*"quality" + 0.005*"progress" + 0.004*"2022" + 0.004*"9" + 0.004*"Trust"', '0.015*"’" + 0.008*"Sandwell" + 0.007*"needs" + 0.006*"Trust" + 0.006*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"number" + 0.005*"20" + 0.005*"education"', '0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"quality" + 0.006*"Sandwell" + 0.005*"9" + 0.004*"20" + 0.004*"effective" + 0.004*"changes"']</t>
+    <t>['0.013*"’" + 0.007*"needs" + 0.006*"Sandwell" + 0.006*"plans" + 0.005*"number" + 0.005*"well" + 0.005*"quality" + 0.004*"20" + 0.004*"Trust" + 0.004*"progress"', '0.014*"’" + 0.008*"well" + 0.007*"Sandwell" + 0.007*"plans" + 0.007*"needs" + 0.006*"quality" + 0.006*"education" + 0.005*"progress" + 0.005*"Trust" + 0.005*"2022"', '0.015*"’" + 0.009*"needs" + 0.008*"Sandwell" + 0.007*"plans" + 0.007*"well" + 0.006*"quality" + 0.005*"9" + 0.005*"20" + 0.005*"Trust" + 0.004*"many"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3823,7 +3823,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.007*"practice" + 0.006*"oversight" + 0.005*"including" + 0.005*"timely" + 0.005*"protection" + 0.005*"◼" + 0.005*"management" + 0.005*"February"', '0.013*"’" + 0.008*"needs" + 0.006*"lack" + 0.005*"including" + 0.005*"oversight" + 0.005*"management" + 0.005*"plans" + 0.005*"protection" + 0.005*"practice" + 0.004*"21"', '0.021*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"many" + 0.005*"oversight" + 0.005*"◼" + 0.005*"protection" + 0.005*"need" + 0.005*"always" + 0.005*"March"']</t>
+    <t>['0.013*"’" + 0.006*"practice" + 0.006*"needs" + 0.005*"lack" + 0.005*"oversight" + 0.005*"many" + 0.005*"management" + 0.005*"protection" + 0.004*"4" + 0.004*"21"', '0.016*"’" + 0.011*"needs" + 0.006*"practice" + 0.006*"oversight" + 0.006*"protection" + 0.006*"lack" + 0.005*"including" + 0.005*"March" + 0.004*"4" + 0.004*"timely"', '0.018*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"◼" + 0.005*"including" + 0.005*"oversight" + 0.005*"timely" + 0.005*"Sefton" + 0.005*"management" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3856,7 +3856,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.009*"Sheffield" + 0.007*"needs" + 0.007*"practice" + 0.006*"leaders" + 0.005*"adviser" + 0.005*"well" + 0.004*"health" + 0.004*"experiences" + 0.004*"22"', '0.024*"’" + 0.012*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.005*"quality" + 0.005*"health" + 0.005*"leaders" + 0.005*"11" + 0.005*"practice" + 0.005*"ensure"', '0.014*"’" + 0.012*"Sheffield" + 0.008*"needs" + 0.007*"well" + 0.006*"health" + 0.005*"good" + 0.005*"practice" + 0.005*"leaders" + 0.005*"effective" + 0.004*"experiences"']</t>
+    <t>['0.022*"’" + 0.013*"Sheffield" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.006*"health" + 0.005*"well" + 0.005*"adviser" + 0.005*"experiences" + 0.005*"effective"', '0.023*"’" + 0.011*"Sheffield" + 0.011*"needs" + 0.007*"well" + 0.005*"leaders" + 0.005*"quality" + 0.005*"plans" + 0.005*"practice" + 0.005*"health" + 0.005*"good"', '0.012*"’" + 0.008*"Sheffield" + 0.008*"well" + 0.007*"needs" + 0.005*"practice" + 0.004*"leaders" + 0.004*"health" + 0.004*"mental" + 0.004*"11" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3886,7 +3886,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Shropshire" + 0.006*"progress" + 0.005*"plans" + 0.004*"2022" + 0.004*"practice" + 0.004*"February" + 0.004*"making"', '0.015*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Shropshire" + 0.006*"plans" + 0.005*"2022" + 0.005*"7" + 0.005*"progress" + 0.004*"effective" + 0.004*"making"', '0.020*"’" + 0.008*"needs" + 0.008*"Shropshire" + 0.006*"progress" + 0.006*"well" + 0.006*"making" + 0.005*"plans" + 0.005*"2022" + 0.005*"11" + 0.005*"leaders"']</t>
+    <t>['0.016*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Shropshire" + 0.005*"7" + 0.004*"2022" + 0.004*"plans" + 0.004*"effectively" + 0.004*"progress" + 0.004*"making"', '0.020*"’" + 0.011*"needs" + 0.008*"well" + 0.008*"Shropshire" + 0.007*"progress" + 0.006*"plans" + 0.006*"making" + 0.005*"2022" + 0.005*"11" + 0.005*"7"', '0.011*"’" + 0.006*"Shropshire" + 0.004*"needs" + 0.004*"progress" + 0.004*"2022" + 0.004*"plans" + 0.004*"well" + 0.004*"making" + 0.004*"leaders" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3910,7 +3910,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"plans" + 0.008*"Slough" + 0.007*"needs" + 0.006*"quality" + 0.005*"leaders" + 0.005*"3" + 0.005*"supported" + 0.005*"need" + 0.004*"planning"', '0.017*"’" + 0.009*"Slough" + 0.007*"practice" + 0.006*"quality" + 0.006*"needs" + 0.005*"plans" + 0.005*"supported" + 0.005*"senior" + 0.005*"3" + 0.005*"impact"', '0.011*"’" + 0.006*"Slough" + 0.006*"needs" + 0.005*"impact" + 0.005*"However" + 0.005*"plans" + 0.005*"quality" + 0.004*"practice" + 0.004*"leaders" + 0.004*"need"']</t>
+    <t>['0.019*"’" + 0.008*"Slough" + 0.006*"needs" + 0.006*"practice" + 0.005*"leaders" + 0.005*"quality" + 0.005*"23" + 0.004*"impact" + 0.004*"3" + 0.004*"senior"', '0.017*"’" + 0.009*"Slough" + 0.008*"plans" + 0.007*"quality" + 0.006*"needs" + 0.006*"3" + 0.006*"practice" + 0.005*"impact" + 0.005*"January" + 0.005*"supported"', '0.009*"’" + 0.005*"Slough" + 0.005*"quality" + 0.005*"needs" + 0.005*"plans" + 0.004*"need" + 0.004*"practice" + 0.004*"However" + 0.004*"senior" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3934,7 +3934,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"lack" + 0.009*"2022" + 0.006*"practice" + 0.006*"risk" + 0.006*"Solihull" + 0.006*"need" + 0.005*"November" + 0.005*"quality" + 0.005*"experiences"', '0.012*"’" + 0.008*"2022" + 0.007*"lack" + 0.006*"need" + 0.006*"Solihull" + 0.006*"risk" + 0.005*"effective" + 0.005*"significant" + 0.005*"quality" + 0.004*"experiences"', '0.016*"’" + 0.012*"lack" + 0.007*"2022" + 0.006*"Solihull" + 0.006*"need" + 0.006*"quality" + 0.005*"means" + 0.005*"risk" + 0.005*"practice" + 0.005*"experiences"']</t>
+    <t>['0.016*"’" + 0.009*"lack" + 0.007*"2022" + 0.007*"Solihull" + 0.006*"need" + 0.005*"quality" + 0.005*"experiences" + 0.005*"risk" + 0.005*"oversight" + 0.005*"significant"', '0.014*"’" + 0.013*"lack" + 0.008*"2022" + 0.006*"risk" + 0.006*"quality" + 0.006*"practice" + 0.006*"Solihull" + 0.006*"effective" + 0.005*"significant" + 0.005*"need"', '0.016*"’" + 0.010*"lack" + 0.009*"2022" + 0.008*"need" + 0.006*"risk" + 0.005*"Solihull" + 0.005*"practice" + 0.005*"effective" + 0.005*"quality" + 0.005*"means"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3958,7 +3958,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"plans" + 0.007*"Somerset" + 0.006*"good" + 0.006*"number" + 0.005*"progress" + 0.005*"supported" + 0.005*"range"', '0.019*"’" + 0.008*"well" + 0.007*"needs" + 0.005*"including" + 0.005*"plans" + 0.005*"supported" + 0.005*"Somerset" + 0.005*"good" + 0.005*"positive" + 0.004*"practice"', '0.017*"’" + 0.010*"well" + 0.010*"needs" + 0.007*"Somerset" + 0.006*"need" + 0.006*"good" + 0.006*"regularly" + 0.006*"leaders" + 0.005*"plans" + 0.005*"supported"']</t>
+    <t>['0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.007*"Somerset" + 0.006*"plans" + 0.006*"number" + 0.005*"good" + 0.005*"practice" + 0.005*"need" + 0.005*"leaders"', '0.020*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"Somerset" + 0.007*"supported" + 0.006*"good" + 0.006*"plans" + 0.006*"including" + 0.005*"leaders" + 0.005*"progress"', '0.014*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"good" + 0.006*"Somerset" + 0.006*"plans" + 0.005*"leaders" + 0.005*"progress" + 0.004*"practice" + 0.004*"including"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3982,7 +3982,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.014*"well" + 0.012*"quality" + 0.011*"’" + 0.009*"leaders" + 0.007*"good" + 0.007*"plans" + 0.007*"progress" + 0.007*"timely" + 0.006*"needs" + 0.005*"◼"', '0.010*"quality" + 0.008*"’" + 0.008*"well" + 0.007*"leaders" + 0.007*"plans" + 0.006*"good" + 0.006*"timely" + 0.006*"needs" + 0.005*"South" + 0.004*"practice"', '0.010*"well" + 0.009*"plans" + 0.008*"quality" + 0.008*"leaders" + 0.006*"good" + 0.006*"’" + 0.005*"always" + 0.005*"practice" + 0.005*"timely" + 0.005*"Senior"']</t>
+    <t>['0.012*"quality" + 0.010*"well" + 0.010*"’" + 0.008*"plans" + 0.008*"good" + 0.007*"leaders" + 0.006*"timely" + 0.006*"needs" + 0.005*"progress" + 0.005*"always"', '0.011*"well" + 0.009*"quality" + 0.009*"leaders" + 0.007*"plans" + 0.007*"’" + 0.006*"needs" + 0.006*"progress" + 0.005*"always" + 0.005*"good" + 0.005*"impact"', '0.011*"well" + 0.009*"leaders" + 0.009*"’" + 0.009*"quality" + 0.007*"plans" + 0.007*"timely" + 0.007*"good" + 0.005*"needs" + 0.005*"practice" + 0.005*"Senior"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -4015,7 +4015,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"Tyneside" + 0.006*"needs" + 0.005*"South" + 0.005*"9" + 0.005*"However" + 0.005*"oversight" + 0.004*"5" + 0.004*"carers" + 0.004*"management"', '0.030*"’" + 0.011*"needs" + 0.008*"South" + 0.007*"Tyneside" + 0.006*"oversight" + 0.006*"carers" + 0.005*"effective" + 0.005*"practice" + 0.005*"2023" + 0.005*"However"', '0.020*"’" + 0.008*"Tyneside" + 0.008*"South" + 0.007*"needs" + 0.006*"9" + 0.005*"management" + 0.005*"However" + 0.004*"effective" + 0.004*"14" + 0.004*"5"']</t>
+    <t>['0.017*"’" + 0.007*"needs" + 0.006*"Tyneside" + 0.006*"South" + 0.005*"carers" + 0.004*"5" + 0.004*"management" + 0.004*"However" + 0.004*"well" + 0.004*"effective"', '0.029*"’" + 0.009*"needs" + 0.008*"South" + 0.007*"Tyneside" + 0.006*"management" + 0.006*"oversight" + 0.006*"9" + 0.006*"15" + 0.005*"However" + 0.005*"effective"', '0.023*"’" + 0.010*"needs" + 0.008*"Tyneside" + 0.007*"South" + 0.005*"carers" + 0.005*"oversight" + 0.005*"practice" + 0.005*"effective" + 0.005*"progress" + 0.005*"5"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -4045,7 +4045,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"Southampton" + 0.006*"5" + 0.006*"plans" + 0.006*"improve" + 0.005*"including" + 0.005*"progress" + 0.005*"needs" + 0.004*"good" + 0.004*"16"', '0.013*"’" + 0.004*"2023" + 0.004*"plans" + 0.003*"information" + 0.003*"experiences" + 0.003*"progress" + 0.003*"16" + 0.003*"timely" + 0.003*"improve" + 0.003*"provide"', '0.019*"’" + 0.007*"plans" + 0.005*"needs" + 0.005*"Southampton" + 0.005*"progress" + 0.004*"experiences" + 0.004*"improve" + 0.004*"including" + 0.004*"timely" + 0.004*"16"']</t>
+    <t>['0.016*"’" + 0.006*"improve" + 0.006*"Southampton" + 0.005*"plans" + 0.005*"including" + 0.005*"progress" + 0.005*"good" + 0.004*"16" + 0.004*"needs" + 0.004*"June"', '0.012*"’" + 0.006*"plans" + 0.005*"Southampton" + 0.005*"5" + 0.005*"including" + 0.005*"needs" + 0.004*"provide" + 0.004*"progress" + 0.004*"experiences" + 0.004*"16"', '0.019*"’" + 0.006*"plans" + 0.005*"Southampton" + 0.005*"progress" + 0.004*"timely" + 0.004*"5" + 0.004*"2023" + 0.004*"experiences" + 0.004*"needs" + 0.004*"improve"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -4081,7 +4081,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"leaders" + 0.007*"planning" + 0.007*"quality" + 0.007*"practice" + 0.007*"protection" + 0.006*"always" + 0.006*"within" + 0.005*"good" + 0.005*"number"', '0.011*"’" + 0.007*"quality" + 0.007*"planning" + 0.007*"practice" + 0.005*"within" + 0.005*"plans" + 0.005*"number" + 0.005*"need" + 0.005*"effective" + 0.005*"leaders"', '0.013*"’" + 0.009*"planning" + 0.007*"practice" + 0.005*"number" + 0.005*"quality" + 0.005*"protection" + 0.005*"leaders" + 0.005*"needs" + 0.005*"effective" + 0.005*"need"']</t>
+    <t>['0.014*"’" + 0.008*"quality" + 0.006*"planning" + 0.006*"practice" + 0.006*"always" + 0.005*"However" + 0.005*"needs" + 0.005*"within" + 0.005*"Southend" + 0.005*"protection"', '0.015*"’" + 0.009*"planning" + 0.007*"practice" + 0.007*"leaders" + 0.006*"risk" + 0.006*"number" + 0.006*"quality" + 0.006*"within" + 0.005*"protection" + 0.005*"need"', '0.011*"’" + 0.007*"practice" + 0.007*"planning" + 0.006*"leaders" + 0.006*"effective" + 0.006*"quality" + 0.005*"protection" + 0.005*"number" + 0.005*"carers" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -4102,7 +4102,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Helens" + 0.007*"well" + 0.007*"St" + 0.007*"progress" + 0.007*"needs" + 0.006*"21" + 0.005*"need" + 0.005*"receive" + 0.005*"good"', '0.017*"’" + 0.008*"St" + 0.008*"needs" + 0.007*"Helens" + 0.006*"well" + 0.006*"10" + 0.006*"receive" + 0.006*"progress" + 0.005*"need" + 0.005*"good"', '0.013*"’" + 0.007*"St" + 0.007*"Helens" + 0.006*"needs" + 0.006*"well" + 0.005*"risk" + 0.005*"good" + 0.005*"10" + 0.005*"receive" + 0.005*"effective"']</t>
+    <t>['0.017*"’" + 0.009*"Helens" + 0.008*"needs" + 0.008*"St" + 0.006*"well" + 0.006*"progress" + 0.006*"risk" + 0.006*"good" + 0.006*"need" + 0.005*"effective"', '0.016*"’" + 0.008*"St" + 0.007*"well" + 0.007*"receive" + 0.007*"Helens" + 0.006*"needs" + 0.006*"21" + 0.006*"progress" + 0.005*"10" + 0.005*"need"', '0.015*"’" + 0.007*"St" + 0.007*"Helens" + 0.007*"needs" + 0.006*"10" + 0.006*"well" + 0.005*"21" + 0.005*"progress" + 0.005*"good" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -4126,7 +4126,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.013*"needs" + 0.006*"Staffordshire" + 0.006*"health" + 0.006*"quality" + 0.006*"progress" + 0.006*"oversight" + 0.006*"practice" + 0.006*"ensure" + 0.005*"plans"', '0.021*"’" + 0.011*"needs" + 0.007*"progress" + 0.006*"practice" + 0.006*"quality" + 0.006*"oversight" + 0.005*"health" + 0.005*"Staffordshire" + 0.005*"6" + 0.005*"10"', '0.013*"’" + 0.010*"needs" + 0.006*"ensure" + 0.006*"quality" + 0.005*"oversight" + 0.005*"practice" + 0.004*"plans" + 0.004*"good" + 0.004*"impact" + 0.004*"health"']</t>
+    <t>['0.018*"’" + 0.012*"needs" + 0.007*"quality" + 0.007*"progress" + 0.006*"practice" + 0.006*"ensure" + 0.006*"Staffordshire" + 0.006*"health" + 0.005*"plans" + 0.005*"oversight"', '0.018*"’" + 0.011*"needs" + 0.006*"practice" + 0.006*"quality" + 0.006*"oversight" + 0.005*"Staffordshire" + 0.005*"ensure" + 0.005*"plans" + 0.005*"progress" + 0.004*"10"', '0.015*"’" + 0.012*"needs" + 0.006*"health" + 0.006*"oversight" + 0.005*"progress" + 0.005*"quality" + 0.005*"ensure" + 0.005*"Staffordshire" + 0.004*"10" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -4156,7 +4156,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.008*"well" + 0.008*"practice" + 0.007*"Stockport" + 0.006*"strong" + 0.006*"needs" + 0.005*"risk" + 0.005*"leaders" + 0.005*"plans" + 0.005*"28"', '0.011*"’" + 0.007*"Stockport" + 0.007*"well" + 0.006*"practice" + 0.006*"needs" + 0.006*"plans" + 0.005*"strong" + 0.005*"need" + 0.005*"ensure" + 0.004*"response"', '0.012*"’" + 0.009*"well" + 0.007*"practice" + 0.006*"needs" + 0.006*"risk" + 0.005*"Stockport" + 0.005*"strong" + 0.005*"range" + 0.005*"plans" + 0.004*"April"']</t>
+    <t>['0.009*"’" + 0.008*"well" + 0.007*"Stockport" + 0.006*"needs" + 0.006*"practice" + 0.005*"risk" + 0.005*"plans" + 0.005*"team" + 0.005*"range" + 0.004*"appropriate"', '0.011*"’" + 0.009*"practice" + 0.008*"well" + 0.007*"Stockport" + 0.006*"strong" + 0.006*"plans" + 0.005*"needs" + 0.005*"ensure" + 0.005*"risk" + 0.004*"leaders"', '0.012*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"Stockport" + 0.005*"strong" + 0.005*"28" + 0.005*"plans" + 0.005*"quality" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -4192,7 +4192,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.009*"plans" + 0.009*"leaders" + 0.007*"well" + 0.007*"quality" + 0.007*"on-Tees" + 0.007*"needs" + 0.006*"good" + 0.006*"Stockton" + 0.005*"senior"', '0.021*"’" + 0.009*"leaders" + 0.008*"plans" + 0.006*"needs" + 0.006*"Stockton" + 0.005*"good" + 0.005*"on-Tees" + 0.005*"quality" + 0.005*"6" + 0.004*"education"', '0.018*"’" + 0.008*"leaders" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"Stockton" + 0.006*"quality" + 0.006*"on-Tees" + 0.005*"senior" + 0.005*"good"']</t>
+    <t>['0.019*"’" + 0.009*"leaders" + 0.009*"plans" + 0.007*"well" + 0.007*"Stockton" + 0.007*"needs" + 0.007*"on-Tees" + 0.006*"good" + 0.005*"quality" + 0.005*"senior"', '0.015*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"needs" + 0.005*"quality" + 0.005*"on-Tees" + 0.005*"2023" + 0.004*"carers" + 0.004*"senior" + 0.004*"well"', '0.023*"’" + 0.009*"plans" + 0.009*"leaders" + 0.007*"quality" + 0.007*"well" + 0.006*"good" + 0.006*"needs" + 0.005*"Stockton" + 0.005*"senior" + 0.005*"on-Tees"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -4216,7 +4216,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.007*"Stoke" + 0.006*"However" + 0.006*"plans" + 0.006*"on-Trent" + 0.005*"ensure" + 0.005*"protection" + 0.005*"well" + 0.005*"consistently"', '0.017*"’" + 0.010*"needs" + 0.009*"on-Trent" + 0.007*"Stoke" + 0.007*"well" + 0.006*"plans" + 0.006*"progress" + 0.006*"protection" + 0.006*"However" + 0.005*"information"', '0.019*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"However" + 0.007*"ensure" + 0.007*"plans" + 0.006*"Stoke" + 0.006*"quality" + 0.005*"on-Trent" + 0.005*"protection"']</t>
+    <t>['0.020*"’" + 0.009*"needs" + 0.008*"However" + 0.008*"on-Trent" + 0.008*"well" + 0.007*"Stoke" + 0.007*"ensure" + 0.007*"plans" + 0.006*"protection" + 0.006*"progress"', '0.016*"’" + 0.008*"needs" + 0.006*"Stoke" + 0.006*"plans" + 0.005*"on-Trent" + 0.005*"well" + 0.004*"protection" + 0.004*"14" + 0.004*"However" + 0.004*"ensure"', '0.014*"’" + 0.008*"needs" + 0.007*"Stoke" + 0.007*"well" + 0.006*"plans" + 0.006*"on-Trent" + 0.005*"protection" + 0.005*"However" + 0.005*"quality" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -4246,7 +4246,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.007*"’" + 0.005*"well" + 0.005*"effective" + 0.005*"leaders" + 0.004*"ensure" + 0.004*"good" + 0.004*"practice" + 0.004*"need" + 0.004*"Suffolk" + 0.004*"progress"', '0.018*"’" + 0.007*"progress" + 0.007*"well" + 0.005*"effective" + 0.005*"good" + 0.005*"ensure" + 0.005*"leaders" + 0.005*"practice" + 0.004*"needs" + 0.004*"carers"', '0.013*"’" + 0.007*"progress" + 0.006*"well" + 0.004*"leaders" + 0.004*"effective" + 0.004*"good" + 0.004*"high" + 0.004*"needs" + 0.004*"ensure" + 0.003*"carers"']</t>
+    <t>['0.016*"’" + 0.008*"well" + 0.007*"progress" + 0.006*"leaders" + 0.005*"good" + 0.005*"effective" + 0.004*"ensure" + 0.004*"Suffolk" + 0.004*"high" + 0.004*"practice"', '0.011*"’" + 0.006*"progress" + 0.006*"effective" + 0.005*"practice" + 0.005*"ensure" + 0.005*"well" + 0.005*"good" + 0.004*"leaders" + 0.004*"need" + 0.004*"needs"', '0.012*"’" + 0.006*"well" + 0.005*"progress" + 0.004*"needs" + 0.004*"effective" + 0.004*"good" + 0.004*"ensure" + 0.004*"carers" + 0.003*"impact" + 0.003*"leaders"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -4279,7 +4279,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"quality" + 0.007*"well" + 0.006*"Sunderland" + 0.006*"needs" + 0.005*"experienced" + 0.005*"protection" + 0.004*"TfC" + 0.004*"council" + 0.004*"high"', '0.019*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Sunderland" + 0.005*"practice" + 0.005*"quality" + 0.005*"experienced" + 0.005*"training" + 0.004*"cared" + 0.004*"protection"', '0.017*"’" + 0.008*"quality" + 0.007*"well" + 0.005*"needs" + 0.005*"Sunderland" + 0.005*"experienced" + 0.004*"practice" + 0.004*"parents" + 0.004*"good" + 0.004*"robust"']</t>
+    <t>['0.017*"’" + 0.007*"well" + 0.007*"quality" + 0.007*"needs" + 0.005*"experienced" + 0.005*"cared" + 0.005*"practice" + 0.004*"result" + 0.004*"council" + 0.004*"good"', '0.018*"’" + 0.007*"well" + 0.006*"quality" + 0.006*"Sunderland" + 0.005*"needs" + 0.005*"practice" + 0.005*"risk" + 0.005*"parents" + 0.005*"highly" + 0.005*"training"', '0.013*"’" + 0.007*"Sunderland" + 0.007*"needs" + 0.007*"quality" + 0.007*"well" + 0.005*"TfC" + 0.005*"experienced" + 0.004*"parents" + 0.004*"practice" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -4309,7 +4309,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.010*"needs" + 0.007*"well" + 0.005*"plans" + 0.005*"17" + 0.004*"However" + 0.004*"practice" + 0.004*"progress" + 0.004*"Surrey" + 0.004*"carers"', '0.015*"’" + 0.011*"needs" + 0.011*"well" + 0.008*"practice" + 0.007*"progress" + 0.006*"effective" + 0.005*"quality" + 0.005*"good" + 0.005*"carers" + 0.005*"17"', '0.013*"’" + 0.009*"well" + 0.008*"practice" + 0.007*"progress" + 0.007*"needs" + 0.006*"plans" + 0.005*"good" + 0.005*"quality" + 0.005*"However" + 0.005*"Surrey"']</t>
+    <t>['0.011*"well" + 0.010*"’" + 0.008*"needs" + 0.007*"practice" + 0.005*"plans" + 0.005*"progress" + 0.005*"ensure" + 0.005*"effective" + 0.005*"However" + 0.004*"carers"', '0.011*"’" + 0.010*"well" + 0.008*"needs" + 0.005*"practice" + 0.005*"progress" + 0.005*"carers" + 0.004*"17" + 0.004*"Surrey" + 0.004*"plans" + 0.004*"January"', '0.017*"’" + 0.011*"needs" + 0.008*"progress" + 0.008*"practice" + 0.008*"well" + 0.007*"good" + 0.006*"quality" + 0.006*"plans" + 0.006*"17" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -4333,7 +4333,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.028*"’" + 0.013*"needs" + 0.009*"need" + 0.008*"well" + 0.008*"plans" + 0.007*"Swindon" + 0.006*"effective" + 0.005*"always" + 0.005*"Borough" + 0.005*"lack"', '0.018*"’" + 0.014*"needs" + 0.011*"Swindon" + 0.010*"need" + 0.008*"always" + 0.008*"well" + 0.006*"plans" + 0.006*"impact" + 0.006*"health" + 0.006*"education"', '0.020*"’" + 0.012*"needs" + 0.008*"Swindon" + 0.008*"well" + 0.006*"impact" + 0.006*"need" + 0.006*"health" + 0.005*"always" + 0.005*"plans" + 0.005*"17"']</t>
+    <t>['0.019*"’" + 0.012*"needs" + 0.008*"Swindon" + 0.007*"need" + 0.006*"well" + 0.006*"effective" + 0.006*"plans" + 0.006*"always" + 0.005*"impact" + 0.004*"Council"', '0.017*"’" + 0.012*"needs" + 0.009*"Swindon" + 0.008*"well" + 0.008*"need" + 0.006*"home" + 0.005*"always" + 0.005*"impact" + 0.005*"risk" + 0.005*"plans"', '0.027*"’" + 0.014*"needs" + 0.009*"need" + 0.009*"Swindon" + 0.008*"well" + 0.007*"always" + 0.007*"plans" + 0.006*"impact" + 0.006*"health" + 0.005*"However"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -4360,7 +4360,7 @@
     <t>0.1495</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"needs" + 0.006*"risk" + 0.006*"practice" + 0.006*"quality" + 0.005*"experienced" + 0.005*"impact" + 0.005*"2023" + 0.005*"plans" + 0.005*"4"', '0.013*"’" + 0.008*"needs" + 0.007*"risk" + 0.006*"impact" + 0.006*"experienced" + 0.005*"quality" + 0.005*"December" + 0.005*"need" + 0.005*"4" + 0.005*"practice"', '0.016*"’" + 0.010*"needs" + 0.006*"impact" + 0.006*"experiences" + 0.006*"response" + 0.005*"quality" + 0.005*"risk" + 0.005*"protection" + 0.005*"understand" + 0.005*"practice"']</t>
+    <t>['0.017*"’" + 0.006*"experienced" + 0.006*"4" + 0.006*"risk" + 0.006*"impact" + 0.006*"needs" + 0.005*"quality" + 0.005*"understand" + 0.005*"response" + 0.005*"practice"', '0.015*"’" + 0.008*"needs" + 0.006*"risk" + 0.006*"quality" + 0.006*"experienced" + 0.006*"impact" + 0.005*"December" + 0.005*"practice" + 0.005*"progress" + 0.004*"planning"', '0.016*"’" + 0.012*"needs" + 0.006*"impact" + 0.006*"practice" + 0.006*"Tameside" + 0.006*"risk" + 0.006*"2023" + 0.005*"experiences" + 0.005*"response" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -4384,7 +4384,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.012*"well" + 0.008*"effective" + 0.007*"needs" + 0.007*"plans" + 0.006*"strong" + 0.005*"need" + 0.005*"ensure" + 0.005*"carers" + 0.005*"practice"', '0.017*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"effective" + 0.005*"need" + 0.005*"practice" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"strong" + 0.004*"improve"', '0.015*"’" + 0.011*"well" + 0.008*"needs" + 0.005*"effective" + 0.005*"strong" + 0.005*"plans" + 0.005*"planning" + 0.005*"clear" + 0.005*"need" + 0.004*"ensure"']</t>
+    <t>['0.019*"’" + 0.014*"well" + 0.009*"needs" + 0.007*"effective" + 0.006*"strong" + 0.006*"plans" + 0.005*"planning" + 0.005*"benefit" + 0.005*"improve" + 0.005*"leaders"', '0.013*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"effective" + 0.005*"ensure" + 0.005*"strong" + 0.005*"plans" + 0.005*"improve" + 0.005*"clear"', '0.015*"’" + 0.009*"well" + 0.008*"effective" + 0.007*"needs" + 0.006*"practice" + 0.006*"need" + 0.005*"plans" + 0.005*"ensure" + 0.005*"planning" + 0.004*"strong"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -4408,7 +4408,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"need" + 0.005*"needs" + 0.005*"practice" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"Thurrock" + 0.004*"protection"', '0.011*"’" + 0.009*"well" + 0.004*"carers" + 0.004*"Thurrock" + 0.004*"practice" + 0.004*"ensure" + 0.004*"protect" + 0.004*"needs" + 0.004*"effective" + 0.004*"impact"', '0.012*"’" + 0.007*"well" + 0.006*"need" + 0.006*"carers" + 0.004*"effective" + 0.004*"parents" + 0.004*"needs" + 0.004*"leaders" + 0.003*"quality" + 0.003*"ensure"']</t>
+    <t>['0.012*"’" + 0.007*"well" + 0.004*"practice" + 0.004*"carers" + 0.003*"need" + 0.003*"ensure" + 0.003*"Thurrock" + 0.003*"time" + 0.003*"effective" + 0.003*"needs"', '0.012*"’" + 0.005*"well" + 0.005*"needs" + 0.004*"carers" + 0.004*"quality" + 0.004*"need" + 0.004*"leaders" + 0.004*"effective" + 0.003*"practice" + 0.003*"Thurrock"', '0.015*"’" + 0.010*"well" + 0.007*"carers" + 0.006*"need" + 0.005*"ensure" + 0.005*"needs" + 0.004*"practice" + 0.004*"Thurrock" + 0.004*"leaders" + 0.004*"vulnerable"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -4432,7 +4432,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"21" + 0.004*"1" + 0.004*"Torbay" + 0.004*"effective" + 0.004*"team" + 0.004*"March"', '0.021*"’" + 0.011*"well" + 0.009*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.005*"effective" + 0.005*"team" + 0.005*"progress" + 0.005*"timely" + 0.004*"April"', '0.013*"’" + 0.008*"Torbay" + 0.008*"well" + 0.006*"needs" + 0.005*"good" + 0.005*"effective" + 0.004*"timely" + 0.004*"agencies" + 0.004*"21" + 0.004*"education"']</t>
+    <t>['0.022*"’" + 0.010*"well" + 0.007*"Torbay" + 0.007*"needs" + 0.006*"effective" + 0.005*"good" + 0.005*"2022" + 0.005*"21" + 0.004*"team" + 0.004*"timely"', '0.013*"’" + 0.009*"well" + 0.008*"Torbay" + 0.006*"good" + 0.005*"progress" + 0.005*"needs" + 0.005*"team" + 0.005*"21" + 0.004*"agencies" + 0.004*"April"', '0.012*"’" + 0.006*"well" + 0.006*"Torbay" + 0.006*"good" + 0.006*"needs" + 0.004*"plans" + 0.004*"effective" + 0.004*"1" + 0.004*"timely" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4456,7 +4456,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Trafford" + 0.008*"needs" + 0.008*"plans" + 0.007*"well" + 0.007*"quality" + 0.006*"placed" + 0.005*"practice" + 0.005*"impact" + 0.005*"21"', '0.019*"’" + 0.010*"needs" + 0.007*"Trafford" + 0.007*"plans" + 0.006*"well" + 0.006*"leaders" + 0.006*"team" + 0.006*"quality" + 0.005*"placed" + 0.005*"practice"', '0.014*"’" + 0.009*"needs" + 0.008*"Trafford" + 0.007*"well" + 0.007*"quality" + 0.007*"plans" + 0.005*"worker" + 0.005*"leaders" + 0.005*"practice" + 0.005*"2"']</t>
+    <t>['0.013*"’" + 0.009*"needs" + 0.009*"Trafford" + 0.007*"well" + 0.007*"quality" + 0.007*"plans" + 0.007*"leaders" + 0.006*"practice" + 0.005*"ensure" + 0.005*"impact"', '0.019*"’" + 0.010*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"Trafford" + 0.006*"practice" + 0.005*"quality" + 0.005*"leaders" + 0.005*"21" + 0.005*"team"', '0.018*"’" + 0.009*"needs" + 0.008*"Trafford" + 0.007*"plans" + 0.007*"well" + 0.006*"quality" + 0.005*"team" + 0.004*"leaders" + 0.004*"impact" + 0.004*"November"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4480,7 +4480,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"needs" + 0.009*"leaders" + 0.005*"Walsall" + 0.005*"information" + 0.005*"Senior" + 0.004*"2021" + 0.004*"well" + 0.004*"4" + 0.004*"risk"', '0.024*"’" + 0.006*"leaders" + 0.006*"Walsall" + 0.005*"oversight" + 0.005*"well" + 0.005*"good" + 0.004*"information" + 0.004*"needs" + 0.004*"Senior" + 0.004*"2021"', '0.023*"’" + 0.007*"well" + 0.007*"leaders" + 0.006*"needs" + 0.005*"Walsall" + 0.005*"4" + 0.005*"need" + 0.004*"information" + 0.004*"positive" + 0.004*"Senior"']</t>
+    <t>['0.024*"’" + 0.008*"leaders" + 0.007*"needs" + 0.006*"Walsall" + 0.005*"information" + 0.005*"well" + 0.005*"2021" + 0.005*"4" + 0.005*"good" + 0.004*"oversight"', '0.017*"’" + 0.006*"needs" + 0.006*"well" + 0.006*"leaders" + 0.004*"Walsall" + 0.004*"Senior" + 0.004*"4" + 0.004*"information" + 0.004*"15" + 0.004*"good"', '0.021*"’" + 0.007*"leaders" + 0.006*"needs" + 0.006*"well" + 0.005*"Walsall" + 0.005*"oversight" + 0.005*"Senior" + 0.005*"positive" + 0.004*"4" + 0.004*"October"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4510,7 +4510,7 @@
     <t>19/08/19</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"well" + 0.006*"practice" + 0.004*"plans" + 0.004*"information" + 0.004*"number" + 0.003*"placed" + 0.003*"Senior" + 0.003*"needs" + 0.003*"good"', '0.014*"’" + 0.007*"well" + 0.006*"practice" + 0.005*"number" + 0.004*"progress" + 0.004*"carers" + 0.004*"home" + 0.004*"plans" + 0.004*"protection" + 0.004*"improve"', '0.016*"’" + 0.007*"practice" + 0.006*"well" + 0.006*"Senior" + 0.005*"plans" + 0.004*"need" + 0.004*"good" + 0.004*"progress" + 0.004*"senior" + 0.004*"number"']</t>
+    <t>['0.015*"’" + 0.006*"well" + 0.006*"practice" + 0.004*"plans" + 0.004*"number" + 0.004*"Senior" + 0.004*"home" + 0.004*"information" + 0.004*"good" + 0.004*"needs"', '0.008*"’" + 0.006*"practice" + 0.006*"well" + 0.005*"progress" + 0.004*"plans" + 0.004*"good" + 0.004*"need" + 0.004*"Senior" + 0.004*"small" + 0.004*"carers"', '0.018*"’" + 0.007*"well" + 0.007*"practice" + 0.005*"number" + 0.005*"Senior" + 0.004*"progress" + 0.004*"carers" + 0.004*"plans" + 0.004*"need" + 0.004*"improve"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4540,7 +4540,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"Warwickshire" + 0.005*"plans" + 0.005*"Senior" + 0.005*"practice" + 0.005*"carers" + 0.004*"benefit" + 0.004*"progress"', '0.013*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.005*"Warwickshire" + 0.005*"good" + 0.005*"3" + 0.004*"carers" + 0.004*"effective" + 0.004*"information"', '0.011*"’" + 0.007*"needs" + 0.007*"Warwickshire" + 0.006*"well" + 0.005*"good" + 0.005*"practice" + 0.005*"plans" + 0.005*"clear" + 0.005*"progress" + 0.004*"3"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.005*"Warwickshire" + 0.004*"well" + 0.004*"plans" + 0.004*"22" + 0.004*"effective" + 0.004*"good" + 0.004*"November" + 0.003*"ensure"', '0.011*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"Warwickshire" + 0.006*"practice" + 0.005*"good" + 0.004*"clear" + 0.004*"carers" + 0.004*"3"', '0.014*"’" + 0.007*"well" + 0.007*"plans" + 0.005*"Warwickshire" + 0.005*"needs" + 0.005*"information" + 0.005*"carers" + 0.005*"progress" + 0.005*"practice" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4564,7 +4564,7 @@
     <t>14/03/2022</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"Berkshire" + 0.006*"West" + 0.005*"well" + 0.005*"needs" + 0.005*"agency" + 0.005*"plans" + 0.004*"early" + 0.004*"18" + 0.004*"14"', '0.017*"’" + 0.008*"well" + 0.007*"West" + 0.005*"Berkshire" + 0.005*"need" + 0.004*"March" + 0.004*"working" + 0.004*"plans" + 0.004*"practice" + 0.004*"needs"', '0.011*"’" + 0.006*"Berkshire" + 0.006*"West" + 0.004*"18" + 0.004*"working" + 0.004*"well" + 0.003*"14" + 0.003*"early" + 0.003*"practice" + 0.003*"plans"']</t>
+    <t>['0.018*"’" + 0.008*"West" + 0.007*"Berkshire" + 0.006*"well" + 0.005*"need" + 0.004*"early" + 0.004*"needs" + 0.004*"practice" + 0.004*"plans" + 0.004*"agency"', '0.011*"’" + 0.005*"West" + 0.004*"well" + 0.004*"needs" + 0.004*"Berkshire" + 0.003*"working" + 0.003*"2022" + 0.003*"March" + 0.003*"14" + 0.003*"agency"', '0.013*"’" + 0.006*"well" + 0.006*"Berkshire" + 0.006*"West" + 0.005*"plans" + 0.005*"14" + 0.004*"18" + 0.004*"agency" + 0.004*"education" + 0.004*"needs"']</t>
   </si>
   <si>
     <t>2637548</t>
@@ -4588,7 +4588,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"Northamptonshire" + 0.008*"quality" + 0.007*"West" + 0.007*"well" + 0.005*"practice" + 0.005*"plans" + 0.005*"14" + 0.005*"However" + 0.004*"needs"', '0.015*"’" + 0.006*"Northamptonshire" + 0.006*"practice" + 0.006*"needs" + 0.005*"West" + 0.005*"well" + 0.005*"quality" + 0.004*"impact" + 0.004*"need" + 0.004*"3"', '0.014*"’" + 0.008*"Northamptonshire" + 0.006*"West" + 0.006*"well" + 0.005*"NCT" + 0.005*"quality" + 0.005*"3" + 0.005*"needs" + 0.004*"impact" + 0.004*"practice"']</t>
+    <t>['0.016*"’" + 0.008*"Northamptonshire" + 0.006*"quality" + 0.005*"West" + 0.005*"needs" + 0.005*"well" + 0.005*"practice" + 0.005*"October" + 0.005*"2022" + 0.004*"3"', '0.017*"’" + 0.009*"Northamptonshire" + 0.006*"West" + 0.006*"quality" + 0.005*"well" + 0.005*"experiences" + 0.004*"14" + 0.004*"practice" + 0.004*"needs" + 0.004*"plans"', '0.019*"’" + 0.007*"well" + 0.007*"Northamptonshire" + 0.007*"West" + 0.007*"quality" + 0.006*"practice" + 0.006*"NCT" + 0.005*"impact" + 0.005*"needs" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4612,7 +4612,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"West" + 0.005*"quality" + 0.004*"number" + 0.004*"Sussex" + 0.004*"13" + 0.004*"supported"', '0.014*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"Sussex" + 0.005*"health" + 0.005*"plans" + 0.005*"2023" + 0.005*"quality" + 0.005*"number" + 0.005*"planning"', '0.013*"’" + 0.008*"plans" + 0.006*"well" + 0.006*"13" + 0.005*"West" + 0.005*"needs" + 0.005*"Sussex" + 0.004*"number" + 0.004*"good" + 0.004*"supported"']</t>
+    <t>['0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.006*"West" + 0.006*"Sussex" + 0.005*"supported" + 0.005*"quality" + 0.005*"13" + 0.004*"number"', '0.006*"’" + 0.005*"well" + 0.005*"needs" + 0.004*"Sussex" + 0.004*"plans" + 0.004*"number" + 0.004*"West" + 0.004*"health" + 0.004*"quality" + 0.004*"13"', '0.016*"’" + 0.006*"plans" + 0.006*"well" + 0.005*"13" + 0.005*"needs" + 0.005*"practice" + 0.004*"education" + 0.004*"quality" + 0.004*"number" + 0.004*"Sussex"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4633,7 +4633,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"needs" + 0.007*"May" + 0.006*"Wigan" + 0.006*"plans" + 0.006*"quality" + 0.005*"practice" + 0.005*"appropriate" + 0.005*"leaders" + 0.004*"20"', '0.012*"’" + 0.008*"May" + 0.007*"practice" + 0.007*"plans" + 0.006*"needs" + 0.005*"increased" + 0.005*"9" + 0.005*"appropriate" + 0.005*"Wigan" + 0.005*"quality"', '0.014*"’" + 0.007*"May" + 0.006*"practice" + 0.006*"plans" + 0.006*"Wigan" + 0.006*"quality" + 0.005*"appropriate" + 0.005*"2022" + 0.005*"timely" + 0.005*"well"']</t>
+    <t>['0.013*"’" + 0.007*"May" + 0.006*"plans" + 0.006*"practice" + 0.006*"quality" + 0.005*"9" + 0.005*"Wigan" + 0.005*"increased" + 0.005*"timely" + 0.005*"appropriate"', '0.014*"’" + 0.008*"plans" + 0.007*"May" + 0.007*"needs" + 0.006*"Wigan" + 0.006*"practice" + 0.006*"leaders" + 0.006*"quality" + 0.005*"appropriate" + 0.005*"2022"', '0.011*"’" + 0.008*"May" + 0.007*"practice" + 0.006*"needs" + 0.006*"Wigan" + 0.005*"appropriate" + 0.005*"quality" + 0.005*"plans" + 0.005*"well" + 0.005*"good"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4666,7 +4666,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.010*"well" + 0.010*"’" + 0.006*"progress" + 0.006*"needs" + 0.006*"Wiltshire" + 0.006*"need" + 0.005*"risk" + 0.005*"parents" + 0.005*"plans" + 0.004*"family"', '0.018*"’" + 0.012*"well" + 0.008*"needs" + 0.007*"including" + 0.007*"progress" + 0.006*"need" + 0.006*"Wiltshire" + 0.006*"quality" + 0.006*"supported" + 0.005*"plans"', '0.016*"’" + 0.010*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"risk" + 0.006*"parents" + 0.005*"supported" + 0.005*"Wiltshire" + 0.005*"plans" + 0.005*"ensure"']</t>
+    <t>['0.017*"’" + 0.014*"well" + 0.008*"needs" + 0.008*"Wiltshire" + 0.007*"need" + 0.007*"including" + 0.006*"supported" + 0.006*"parents" + 0.006*"quality" + 0.005*"progress"', '0.012*"’" + 0.010*"well" + 0.007*"needs" + 0.005*"risk" + 0.005*"plans" + 0.005*"progress" + 0.005*"quality" + 0.005*"supported" + 0.005*"parents" + 0.005*"including"', '0.015*"’" + 0.009*"well" + 0.007*"need" + 0.006*"progress" + 0.006*"needs" + 0.006*"ensure" + 0.006*"risk" + 0.005*"parents" + 0.005*"plans" + 0.005*"Wiltshire"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4696,7 +4696,7 @@
     <t>0.1655</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"needs" + 0.008*"Wirral" + 0.006*"plans" + 0.005*"well" + 0.005*"ensure" + 0.005*"18" + 0.005*"number" + 0.005*"appropriate" + 0.005*"small"', '0.013*"’" + 0.010*"needs" + 0.009*"ensure" + 0.008*"practice" + 0.007*"plans" + 0.007*"Wirral" + 0.006*"response" + 0.006*"well" + 0.005*"small" + 0.005*"good"', '0.009*"needs" + 0.008*"’" + 0.007*"Wirral" + 0.006*"ensure" + 0.006*"plans" + 0.006*"practice" + 0.005*"number" + 0.005*"well" + 0.005*"29" + 0.004*"good"']</t>
+    <t>['0.011*"’" + 0.009*"needs" + 0.008*"Wirral" + 0.007*"practice" + 0.006*"ensure" + 0.005*"plans" + 0.005*"well" + 0.005*"response" + 0.005*"effective" + 0.005*"good"', '0.010*"needs" + 0.009*"ensure" + 0.008*"’" + 0.007*"plans" + 0.006*"Wirral" + 0.005*"small" + 0.005*"practice" + 0.005*"well" + 0.005*"risk" + 0.004*"number"', '0.013*"’" + 0.009*"needs" + 0.007*"Wirral" + 0.007*"plans" + 0.006*"ensure" + 0.005*"well" + 0.005*"number" + 0.005*"practice" + 0.005*"18" + 0.005*"2023"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4720,7 +4720,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.006*"effective" + 0.005*"plans" + 0.005*"well" + 0.005*"provided" + 0.004*"progress" + 0.004*"protection" + 0.004*"2023" + 0.004*"experiences" + 0.004*"6"', '0.008*"’" + 0.006*"experiences" + 0.005*"needs" + 0.005*"17" + 0.005*"effective" + 0.005*"progress" + 0.005*"plans" + 0.005*"protection" + 0.004*"Council" + 0.004*"Borough"', '0.017*"’" + 0.008*"plans" + 0.007*"needs" + 0.007*"progress" + 0.007*"effective" + 0.006*"well" + 0.005*"provided" + 0.005*"parents" + 0.005*"appropriate" + 0.005*"quality"']</t>
+    <t>['0.016*"’" + 0.006*"needs" + 0.006*"effective" + 0.006*"plans" + 0.005*"well" + 0.005*"progress" + 0.005*"Borough" + 0.005*"provided" + 0.005*"quality" + 0.004*"experiences"', '0.008*"’" + 0.008*"plans" + 0.005*"progress" + 0.005*"provided" + 0.005*"effective" + 0.004*"needs" + 0.004*"protection" + 0.004*"Wokingham" + 0.004*"appropriate" + 0.004*"well"', '0.012*"’" + 0.007*"effective" + 0.007*"17" + 0.006*"plans" + 0.006*"needs" + 0.006*"well" + 0.006*"progress" + 0.005*"experiences" + 0.005*"parents" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4744,7 +4744,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.006*"Wolverhampton" + 0.006*"needs" + 0.005*"effective" + 0.005*"plans" + 0.005*"supported" + 0.004*"strong" + 0.004*"receive" + 0.004*"risk" + 0.004*"leaders"', '0.012*"’" + 0.008*"needs" + 0.006*"effective" + 0.006*"risks" + 0.005*"Wolverhampton" + 0.005*"quality" + 0.005*"receive" + 0.005*"education" + 0.005*"plans" + 0.004*"1"', '0.018*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"practice" + 0.005*"leaders" + 0.005*"plans" + 0.005*"Wolverhampton" + 0.005*"education" + 0.004*"risks" + 0.004*"quality"']</t>
+    <t>['0.008*"’" + 0.005*"needs" + 0.005*"effective" + 0.004*"28" + 0.004*"Wolverhampton" + 0.004*"supported" + 0.004*"plans" + 0.003*"receive" + 0.003*"risks" + 0.003*"1"', '0.015*"’" + 0.008*"needs" + 0.006*"Wolverhampton" + 0.006*"effective" + 0.005*"plans" + 0.005*"risks" + 0.005*"quality" + 0.005*"education" + 0.004*"strong" + 0.004*"receive"', '0.016*"’" + 0.008*"needs" + 0.006*"effective" + 0.005*"Wolverhampton" + 0.005*"leaders" + 0.005*"risks" + 0.005*"plans" + 0.005*"practice" + 0.005*"receive" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4774,7 +4774,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"Worcestershire" + 0.007*"plans" + 0.007*"progress" + 0.006*"leaders" + 0.006*"ensure" + 0.006*"appropriate" + 0.005*"Senior"', '0.020*"’" + 0.009*"plans" + 0.008*"well" + 0.007*"needs" + 0.007*"leaders" + 0.007*"ensure" + 0.006*"Worcestershire" + 0.006*"progress" + 0.005*"appropriate" + 0.005*"making"', '0.018*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"Worcestershire" + 0.007*"plans" + 0.007*"progress" + 0.007*"leaders" + 0.006*"appropriate" + 0.005*"26" + 0.005*"ensure"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.008*"Worcestershire" + 0.008*"well" + 0.007*"plans" + 0.007*"leaders" + 0.007*"progress" + 0.006*"ensure" + 0.005*"appropriate" + 0.005*"PAs"', '0.021*"’" + 0.009*"well" + 0.009*"plans" + 0.007*"needs" + 0.007*"Worcestershire" + 0.007*"progress" + 0.006*"leaders" + 0.006*"appropriate" + 0.006*"ensure" + 0.005*"26"', '0.016*"’" + 0.007*"well" + 0.007*"plans" + 0.006*"leaders" + 0.006*"needs" + 0.006*"progress" + 0.005*"Worcestershire" + 0.005*"Senior" + 0.005*"appropriate" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>urn</t>

</xml_diff>

<commit_message>
Somerset autority status update
</commit_message>
<xml_diff>
--- a/ofsted_childrens_services_overview.xlsx
+++ b/ofsted_childrens_services_overview.xlsx
@@ -70,7 +70,7 @@
     <t>Sentiment neutral</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"leaders" + 0.007*"needs" + 0.006*"practice" + 0.005*"Barnsley" + 0.005*"within" + 0.004*"senior" + 0.004*"response" + 0.004*"understand" + 0.004*"progress"', '0.016*"’" + 0.007*"needs" + 0.007*"within" + 0.007*"leaders" + 0.006*"Barnsley" + 0.005*"practice" + 0.005*"11" + 0.004*"understand" + 0.004*"response" + 0.004*"progress"', '0.022*"’" + 0.009*"needs" + 0.007*"leaders" + 0.007*"within" + 0.006*"plans" + 0.006*"practice" + 0.005*"Barnsley" + 0.004*"senior" + 0.004*"September" + 0.004*"15"']</t>
+    <t>['0.023*"’" + 0.010*"needs" + 0.009*"leaders" + 0.007*"within" + 0.007*"Barnsley" + 0.006*"practice" + 0.005*"11" + 0.005*"senior" + 0.005*"response" + 0.005*"plans"', '0.014*"’" + 0.006*"needs" + 0.006*"within" + 0.006*"leaders" + 0.005*"practice" + 0.004*"Barnsley" + 0.004*"plans" + 0.004*"senior" + 0.004*"quality" + 0.004*"15"', '0.016*"’" + 0.006*"leaders" + 0.006*"within" + 0.005*"needs" + 0.005*"practice" + 0.005*"Barnsley" + 0.004*"2023" + 0.004*"plans" + 0.004*"response" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80427</t>
@@ -115,7 +115,7 @@
     <t>5</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"practice" + 0.005*"Somerset" + 0.005*"leaders" + 0.005*"plans" + 0.005*"4" + 0.005*"effective" + 0.005*"receive"', '0.020*"’" + 0.010*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"practice" + 0.005*"leaders" + 0.005*"protection" + 0.004*"Bath" + 0.004*"effective" + 0.004*"including"', '0.014*"’" + 0.009*"well" + 0.005*"needs" + 0.005*"East" + 0.004*"receive" + 0.004*"effective" + 0.004*"practice" + 0.004*"plans" + 0.004*"North" + 0.004*"impact"']</t>
+    <t>['0.015*"’" + 0.010*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"practice" + 0.005*"Bath" + 0.005*"effective" + 0.004*"4" + 0.004*"leaders" + 0.004*"impact"', '0.014*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"practice" + 0.005*"Somerset" + 0.005*"plans" + 0.005*"February" + 0.004*"leaders" + 0.004*"North" + 0.004*"effective"', '0.023*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"leaders" + 0.006*"practice" + 0.005*"plans" + 0.005*"clear" + 0.005*"4" + 0.005*"28" + 0.004*"Somerset"']</t>
   </si>
   <si>
     <t>80428</t>
@@ -163,7 +163,7 @@
     <t>7</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.008*"needs" + 0.007*"ensure" + 0.005*"Bedford" + 0.005*"good" + 0.005*"supported" + 0.005*"plans" + 0.005*"well" + 0.005*"made" + 0.005*"education"', '0.013*"’" + 0.006*"well" + 0.005*"needs" + 0.005*"plans" + 0.005*"Bedford" + 0.005*"ensure" + 0.004*"need" + 0.004*"progress" + 0.004*"family" + 0.004*"good"', '0.015*"’" + 0.006*"well" + 0.006*"needs" + 0.006*"ensure" + 0.005*"progress" + 0.005*"supported" + 0.005*"plans" + 0.005*"good" + 0.005*"Bedford" + 0.004*"relationships"']</t>
+    <t>['0.022*"’" + 0.006*"ensure" + 0.006*"well" + 0.006*"needs" + 0.006*"education" + 0.005*"supported" + 0.005*"plans" + 0.005*"Bedford" + 0.005*"progress" + 0.005*"Borough"', '0.020*"’" + 0.008*"needs" + 0.006*"Bedford" + 0.006*"well" + 0.006*"good" + 0.006*"ensure" + 0.006*"plans" + 0.005*"progress" + 0.005*"family" + 0.004*"Borough"', '0.013*"’" + 0.007*"needs" + 0.006*"ensure" + 0.005*"supported" + 0.004*"well" + 0.004*"plans" + 0.004*"Bedford" + 0.004*"good" + 0.004*"relationships" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80429</t>
@@ -208,7 +208,7 @@
     <t>4</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"plans" + 0.004*"appropriate" + 0.004*"3" + 0.004*"progress" + 0.004*"trust" + 0.004*"Birmingham"', '0.017*"’" + 0.008*"needs" + 0.007*"Birmingham" + 0.006*"well" + 0.006*"effective" + 0.006*"progress" + 0.005*"plans" + 0.005*"leaders" + 0.005*"trust" + 0.005*"ensure"', '0.016*"’" + 0.012*"needs" + 0.008*"effective" + 0.007*"plans" + 0.007*"well" + 0.006*"trust" + 0.006*"Birmingham" + 0.005*"risk" + 0.005*"progress" + 0.005*"appropriate"']</t>
+    <t>['0.013*"’" + 0.011*"needs" + 0.007*"well" + 0.007*"effective" + 0.006*"plans" + 0.006*"progress" + 0.005*"3" + 0.005*"Birmingham" + 0.005*"trust" + 0.005*"risk"', '0.020*"’" + 0.009*"needs" + 0.007*"well" + 0.007*"effective" + 0.007*"plans" + 0.006*"Birmingham" + 0.006*"progress" + 0.005*"trust" + 0.005*"20" + 0.005*"appropriate"', '0.012*"’" + 0.008*"needs" + 0.005*"effective" + 0.005*"trust" + 0.005*"leaders" + 0.005*"well" + 0.005*"Birmingham" + 0.004*"plans" + 0.004*"progress" + 0.004*"ensure"']</t>
   </si>
   <si>
     <t>80430</t>
@@ -250,7 +250,7 @@
     <t>0.1834</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"quality" + 0.006*"Blackburn" + 0.006*"Darwen" + 0.005*"effective" + 0.005*"practice" + 0.005*"impact" + 0.005*"progress"', '0.013*"’" + 0.008*"needs" + 0.008*"practice" + 0.007*"Blackburn" + 0.007*"Darwen" + 0.007*"quality" + 0.006*"impact" + 0.005*"well" + 0.005*"leaders" + 0.005*"result"', '0.012*"’" + 0.008*"practice" + 0.007*"quality" + 0.007*"impact" + 0.007*"needs" + 0.006*"planning" + 0.006*"Blackburn" + 0.006*"well" + 0.005*"Darwen" + 0.005*"plans"']</t>
+    <t>['0.013*"’" + 0.007*"needs" + 0.007*"practice" + 0.006*"impact" + 0.006*"Blackburn" + 0.006*"well" + 0.006*"quality" + 0.005*"Darwen" + 0.005*"planning" + 0.005*"means"', '0.015*"’" + 0.009*"quality" + 0.007*"Darwen" + 0.007*"Blackburn" + 0.007*"needs" + 0.006*"practice" + 0.006*"planning" + 0.006*"result" + 0.005*"impact" + 0.005*"plans"', '0.014*"’" + 0.008*"needs" + 0.008*"practice" + 0.008*"well" + 0.007*"Blackburn" + 0.007*"Darwen" + 0.006*"impact" + 0.006*"quality" + 0.006*"effective" + 0.005*"leaders"']</t>
   </si>
   <si>
     <t>80431</t>
@@ -289,7 +289,7 @@
     <t>0.1202</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Blackpool" + 0.006*"plans" + 0.005*"effective" + 0.005*"16" + 0.004*"timely" + 0.004*"practice" + 0.004*"progress"', '0.018*"’" + 0.012*"needs" + 0.008*"well" + 0.008*"Blackpool" + 0.006*"effective" + 0.005*"practice" + 0.005*"experiences" + 0.005*"plans" + 0.005*"quality" + 0.005*"supported"', '0.016*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"Blackpool" + 0.005*"supported" + 0.005*"practice" + 0.004*"effective" + 0.004*"16" + 0.004*"leaders" + 0.004*"quality"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.006*"Blackpool" + 0.005*"effective" + 0.005*"practice" + 0.005*"16" + 0.004*"progress" + 0.004*"response" + 0.004*"understand"', '0.020*"’" + 0.012*"needs" + 0.009*"well" + 0.008*"Blackpool" + 0.006*"effective" + 0.006*"practice" + 0.006*"plans" + 0.005*"16" + 0.005*"experiences" + 0.005*"carers"', '0.014*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"Blackpool" + 0.005*"quality" + 0.005*"supported" + 0.005*"plans" + 0.004*"effective" + 0.004*"good" + 0.004*"homes"']</t>
   </si>
   <si>
     <t>80432</t>
@@ -322,7 +322,7 @@
     <t>3</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.010*"needs" + 0.009*"Bolton" + 0.008*"plans" + 0.006*"well" + 0.006*"planning" + 0.006*"supported" + 0.005*"timely" + 0.005*"need" + 0.005*"response"', '0.018*"’" + 0.010*"needs" + 0.010*"well" + 0.008*"Bolton" + 0.006*"plans" + 0.005*"supported" + 0.005*"11" + 0.005*"effective" + 0.005*"planning" + 0.005*"strong"', '0.019*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.007*"Bolton" + 0.006*"need" + 0.005*"strong" + 0.005*"11" + 0.005*"supported" + 0.004*"health"']</t>
+    <t>['0.012*"’" + 0.011*"needs" + 0.008*"well" + 0.008*"Bolton" + 0.007*"plans" + 0.006*"need" + 0.006*"strong" + 0.005*"planning" + 0.005*"supported" + 0.005*"effective"', '0.024*"’" + 0.008*"Bolton" + 0.008*"needs" + 0.007*"plans" + 0.007*"well" + 0.006*"supported" + 0.005*"11" + 0.005*"response" + 0.005*"planning" + 0.005*"effective"', '0.021*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"Bolton" + 0.008*"plans" + 0.005*"supported" + 0.005*"strong" + 0.005*"planning" + 0.004*"need" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>2532287</t>
@@ -358,7 +358,7 @@
     <t>0.153</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.006*"quality" + 0.005*"progress" + 0.005*"practice" + 0.005*"well" + 0.005*"6" + 0.004*"impact" + 0.004*"17" + 0.004*"time" + 0.004*"risk"', '0.016*"’" + 0.005*"progress" + 0.005*"practice" + 0.004*"17" + 0.004*"However" + 0.004*"Bournemouth" + 0.004*"impact" + 0.004*"many" + 0.004*"Christchurch" + 0.004*"2021"', '0.021*"’" + 0.008*"quality" + 0.007*"practice" + 0.005*"Poole" + 0.005*"Bournemouth" + 0.005*"risk" + 0.005*"Christchurch" + 0.005*"progress" + 0.005*"6" + 0.005*"time"']</t>
+    <t>['0.021*"’" + 0.007*"quality" + 0.007*"progress" + 0.006*"practice" + 0.005*"Bournemouth" + 0.005*"time" + 0.005*"Christchurch" + 0.005*"many" + 0.005*"However" + 0.005*"Poole"', '0.009*"’" + 0.005*"6" + 0.004*"quality" + 0.004*"time" + 0.004*"Bournemouth" + 0.004*"practice" + 0.004*"Poole" + 0.004*"progress" + 0.004*"However" + 0.003*"well"', '0.020*"’" + 0.006*"practice" + 0.006*"17" + 0.006*"quality" + 0.005*"6" + 0.005*"risk" + 0.005*"impact" + 0.004*"Christchurch" + 0.004*"Poole" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80436</t>
@@ -403,7 +403,7 @@
     <t>0.2035</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"Bracknell" + 0.006*"quality" + 0.006*"needs" + 0.006*"well" + 0.006*"good" + 0.006*"provided" + 0.006*"risk" + 0.006*"effective" + 0.005*"Forest"', '0.018*"’" + 0.008*"needs" + 0.007*"Forest" + 0.006*"effective" + 0.006*"Bracknell" + 0.006*"good" + 0.006*"risk" + 0.005*"17" + 0.005*"plans" + 0.005*"need"', '0.014*"’" + 0.007*"Forest" + 0.007*"Bracknell" + 0.007*"risk" + 0.007*"quality" + 0.006*"progress" + 0.006*"plans" + 0.006*"provided" + 0.006*"needs" + 0.006*"good"']</t>
+    <t>['0.016*"’" + 0.008*"Bracknell" + 0.007*"Forest" + 0.007*"needs" + 0.007*"good" + 0.006*"effective" + 0.006*"provided" + 0.006*"need" + 0.005*"risk" + 0.005*"quality"', '0.015*"’" + 0.008*"risk" + 0.007*"needs" + 0.007*"Forest" + 0.007*"Bracknell" + 0.006*"quality" + 0.006*"good" + 0.006*"effective" + 0.005*"progress" + 0.005*"provided"', '0.018*"’" + 0.006*"quality" + 0.006*"well" + 0.006*"risk" + 0.006*"needs" + 0.005*"Forest" + 0.005*"plans" + 0.005*"progress" + 0.005*"effective" + 0.005*"impact"']</t>
   </si>
   <si>
     <t>80438</t>
@@ -439,7 +439,7 @@
     <t>0.1856</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.007*"Hove" + 0.007*"well" + 0.006*"Brighton" + 0.006*"practice" + 0.005*"receive" + 0.005*"progress" + 0.005*"experiences" + 0.005*"15" + 0.005*"relationships"', '0.019*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"Brighton" + 0.006*"practice" + 0.006*"relationships" + 0.006*"Hove" + 0.006*"progress" + 0.005*"experiences" + 0.005*"carers"', '0.011*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"Hove" + 0.006*"Brighton" + 0.006*"practice" + 0.005*"relationships" + 0.005*"experiences" + 0.004*"family" + 0.004*"progress"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.006*"Brighton" + 0.005*"Hove" + 0.005*"needs" + 0.005*"experiences" + 0.005*"relationships" + 0.005*"family" + 0.005*"practice" + 0.005*"11"', '0.017*"’" + 0.008*"needs" + 0.007*"Hove" + 0.007*"practice" + 0.006*"well" + 0.006*"Brighton" + 0.006*"progress" + 0.006*"relationships" + 0.005*"experiences" + 0.005*"carers"', '0.015*"’" + 0.008*"well" + 0.007*"Hove" + 0.007*"Brighton" + 0.007*"practice" + 0.006*"needs" + 0.005*"progress" + 0.005*"PAs" + 0.005*"experiences" + 0.005*"receive"']</t>
   </si>
   <si>
     <t>80441</t>
@@ -475,7 +475,7 @@
     <t>0.1875</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.010*"well" + 0.009*"needs" + 0.009*"good" + 0.007*"Bristol" + 0.006*"health" + 0.006*"progress" + 0.005*"receive" + 0.005*"arrangements" + 0.005*"need"', '0.019*"’" + 0.008*"Bristol" + 0.007*"good" + 0.007*"well" + 0.006*"needs" + 0.006*"health" + 0.005*"leaders" + 0.005*"progress" + 0.005*"16" + 0.005*"27"', '0.015*"’" + 0.008*"well" + 0.006*"Bristol" + 0.006*"needs" + 0.006*"good" + 0.004*"need" + 0.004*"progress" + 0.004*"16" + 0.004*"leaders" + 0.004*"plans"']</t>
+    <t>['0.017*"’" + 0.011*"well" + 0.009*"good" + 0.008*"Bristol" + 0.007*"needs" + 0.005*"progress" + 0.005*"2023" + 0.005*"plans" + 0.004*"need" + 0.004*"health"', '0.021*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"good" + 0.006*"Bristol" + 0.006*"leaders" + 0.005*"progress" + 0.005*"receive" + 0.005*"plans" + 0.005*"16"', '0.019*"’" + 0.008*"Bristol" + 0.008*"needs" + 0.007*"good" + 0.007*"well" + 0.006*"health" + 0.005*"need" + 0.005*"risk" + 0.005*"always" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80442</t>
@@ -505,7 +505,7 @@
     <t>0.159</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.005*"plans" + 0.005*"many" + 0.005*"6" + 0.004*"Buckinghamshire" + 0.004*"number" + 0.004*"17" + 0.004*"practice" + 0.004*"2021" + 0.004*"protection"', '0.012*"’" + 0.005*"number" + 0.004*"Buckinghamshire" + 0.004*"6" + 0.004*"17" + 0.004*"practice" + 0.004*"December" + 0.004*"family" + 0.003*"plans" + 0.003*"protection"', '0.012*"’" + 0.006*"plans" + 0.005*"17" + 0.005*"number" + 0.004*"protection" + 0.004*"Buckinghamshire" + 0.004*"well" + 0.004*"many" + 0.004*"2021" + 0.004*"impact"']</t>
+    <t>['0.014*"’" + 0.005*"number" + 0.004*"Buckinghamshire" + 0.004*"December" + 0.004*"6" + 0.004*"17" + 0.004*"many" + 0.004*"plans" + 0.003*"needs" + 0.003*"small"', '0.013*"’" + 0.006*"plans" + 0.005*"17" + 0.005*"protection" + 0.005*"Buckinghamshire" + 0.004*"well" + 0.004*"2021" + 0.004*"practice" + 0.004*"teams" + 0.004*"6"', '0.013*"’" + 0.006*"number" + 0.005*"plans" + 0.004*"many" + 0.004*"practice" + 0.004*"6" + 0.004*"2021" + 0.003*"Buckinghamshire" + 0.003*"December" + 0.003*"protection"']</t>
   </si>
   <si>
     <t>80443</t>
@@ -544,7 +544,7 @@
     <t>0.1441</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"needs" + 0.007*"2021" + 0.006*"protection" + 0.006*"practice" + 0.005*"team" + 0.005*"impact" + 0.005*"need" + 0.005*"new" + 0.005*"October"', '0.010*"’" + 0.006*"2021" + 0.006*"needs" + 0.006*"team" + 0.005*"protection" + 0.005*"quality" + 0.005*"risk" + 0.004*"practice" + 0.004*"timely" + 0.004*"need"', '0.011*"’" + 0.007*"protection" + 0.006*"2021" + 0.006*"5" + 0.005*"needs" + 0.005*"team" + 0.005*"risk" + 0.005*"practice" + 0.005*"impact" + 0.005*"need"']</t>
+    <t>['0.008*"’" + 0.006*"practice" + 0.006*"needs" + 0.006*"protection" + 0.005*"team" + 0.004*"need" + 0.004*"senior" + 0.004*"impact" + 0.004*"5" + 0.004*"2021"', '0.013*"’" + 0.007*"needs" + 0.007*"2021" + 0.006*"team" + 0.006*"protection" + 0.005*"impact" + 0.005*"need" + 0.005*"practice" + 0.005*"new" + 0.005*"quality"', '0.012*"’" + 0.008*"2021" + 0.007*"protection" + 0.006*"needs" + 0.006*"practice" + 0.006*"risk" + 0.005*"Bury" + 0.005*"impact" + 0.005*"quality" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80444</t>
@@ -583,7 +583,7 @@
     <t>0.194</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.010*"Calderdale" + 0.009*"needs" + 0.006*"well" + 0.006*"ensure" + 0.006*"plans" + 0.005*"parents" + 0.005*"progress" + 0.005*"risk" + 0.005*"experiences"', '0.023*"’" + 0.010*"needs" + 0.008*"Calderdale" + 0.006*"progress" + 0.006*"well" + 0.006*"plans" + 0.005*"ensure" + 0.005*"information" + 0.005*"need" + 0.005*"parents"', '0.019*"’" + 0.010*"needs" + 0.007*"Calderdale" + 0.006*"well" + 0.005*"risk" + 0.005*"ensure" + 0.005*"plans" + 0.005*"progress" + 0.005*"experiences" + 0.005*"risks"']</t>
+    <t>['0.018*"’" + 0.010*"needs" + 0.010*"Calderdale" + 0.006*"well" + 0.006*"progress" + 0.005*"19" + 0.005*"risk" + 0.005*"information" + 0.005*"ensure" + 0.005*"plans"', '0.019*"’" + 0.011*"needs" + 0.007*"Calderdale" + 0.007*"well" + 0.006*"progress" + 0.006*"ensure" + 0.005*"risk" + 0.005*"parents" + 0.005*"information" + 0.005*"plans"', '0.024*"’" + 0.008*"needs" + 0.008*"Calderdale" + 0.008*"plans" + 0.005*"ensure" + 0.005*"well" + 0.005*"experiences" + 0.004*"risk" + 0.004*"PAs" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80445</t>
@@ -613,7 +613,7 @@
     <t>0.2052</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"needs" + 0.006*"Cambridgeshire" + 0.006*"leaders" + 0.005*"effective" + 0.005*"4" + 0.005*"good" + 0.005*"quality" + 0.005*"leadership" + 0.005*"response"', '0.014*"’" + 0.007*"Cambridgeshire" + 0.007*"needs" + 0.007*"leaders" + 0.006*"good" + 0.005*"well" + 0.005*"effective" + 0.005*"practice" + 0.004*"quality" + 0.004*"However"', '0.018*"’" + 0.006*"leaders" + 0.006*"Cambridgeshire" + 0.005*"needs" + 0.005*"well" + 0.005*"good" + 0.004*"15" + 0.004*"2024" + 0.004*"4" + 0.004*"timely"']</t>
+    <t>['0.010*"’" + 0.007*"Cambridgeshire" + 0.006*"needs" + 0.005*"leaders" + 0.005*"effective" + 0.004*"good" + 0.004*"leadership" + 0.004*"practice" + 0.004*"quality" + 0.004*"response"', '0.015*"’" + 0.005*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"leaders" + 0.005*"Cambridgeshire" + 0.005*"effective" + 0.004*"plans" + 0.004*"15" + 0.004*"practice"', '0.021*"’" + 0.008*"needs" + 0.007*"leaders" + 0.007*"Cambridgeshire" + 0.006*"good" + 0.005*"quality" + 0.005*"4" + 0.005*"However" + 0.005*"well" + 0.005*"effective"']</t>
   </si>
   <si>
     <t>80446</t>
@@ -646,7 +646,7 @@
     <t>0.196</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"well" + 0.008*"needs" + 0.006*"need" + 0.006*"good" + 0.006*"plans" + 0.006*"progress" + 0.005*"carers" + 0.005*"number" + 0.005*"information"', '0.015*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"carers" + 0.006*"good" + 0.006*"need" + 0.005*"plans" + 0.005*"Central" + 0.005*"education" + 0.004*"effective"', '0.018*"’" + 0.008*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"progress" + 0.006*"carers" + 0.006*"plans" + 0.005*"good" + 0.005*"Bedfordshire" + 0.004*"Leaders"']</t>
+    <t>['0.015*"’" + 0.008*"well" + 0.006*"needs" + 0.006*"carers" + 0.006*"plans" + 0.006*"need" + 0.005*"Bedfordshire" + 0.004*"effective" + 0.004*"information" + 0.004*"progress"', '0.015*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"need" + 0.007*"progress" + 0.006*"carers" + 0.006*"plans" + 0.006*"good" + 0.005*"Central" + 0.005*"Bedfordshire"', '0.018*"’" + 0.009*"well" + 0.008*"good" + 0.006*"needs" + 0.006*"need" + 0.006*"carers" + 0.005*"plans" + 0.005*"17" + 0.005*"progress" + 0.005*"Central"']</t>
   </si>
   <si>
     <t>80447</t>
@@ -682,7 +682,7 @@
     <t>0.1661</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"needs" + 0.008*"Cheshire" + 0.008*"2024" + 0.007*"practice" + 0.007*"plans" + 0.006*"well" + 0.006*"quality" + 0.006*"effective" + 0.006*"East"', '0.010*"’" + 0.007*"2024" + 0.006*"plans" + 0.005*"needs" + 0.005*"practice" + 0.005*"effective" + 0.004*"quality" + 0.004*"risk" + 0.004*"access" + 0.004*"East"', '0.014*"’" + 0.008*"well" + 0.008*"2024" + 0.007*"plans" + 0.007*"needs" + 0.007*"practice" + 0.006*"quality" + 0.006*"leaders" + 0.006*"East" + 0.005*"always"']</t>
+    <t>['0.014*"’" + 0.009*"2024" + 0.008*"needs" + 0.008*"well" + 0.007*"plans" + 0.006*"practice" + 0.006*"Cheshire" + 0.006*"quality" + 0.005*"effective" + 0.005*"East"', '0.013*"’" + 0.007*"needs" + 0.007*"plans" + 0.006*"2024" + 0.006*"East" + 0.006*"practice" + 0.006*"Cheshire" + 0.006*"leaders" + 0.006*"quality" + 0.006*"well"', '0.011*"’" + 0.007*"practice" + 0.007*"2024" + 0.006*"needs" + 0.006*"plans" + 0.006*"quality" + 0.006*"well" + 0.005*"effective" + 0.005*"leaders" + 0.005*"East"']</t>
   </si>
   <si>
     <t>80448</t>
@@ -721,7 +721,7 @@
     <t>0.1831</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.008*"well" + 0.008*"needs" + 0.005*"plans" + 0.005*"practice" + 0.005*"effective" + 0.005*"impact" + 0.004*"effectively" + 0.004*"early" + 0.004*"However"', '0.015*"’" + 0.007*"well" + 0.007*"needs" + 0.004*"always" + 0.004*"learning" + 0.004*"receive" + 0.004*"timely" + 0.004*"effective" + 0.004*"strong" + 0.004*"effectively"', '0.024*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"practice" + 0.005*"order" + 0.004*"intervention" + 0.004*"always" + 0.004*"effectively" + 0.004*"impact" + 0.004*"receive"']</t>
+    <t>['0.020*"’" + 0.009*"well" + 0.007*"needs" + 0.005*"effectively" + 0.005*"impact" + 0.005*"practice" + 0.005*"learning" + 0.004*"risk" + 0.004*"always" + 0.004*"use"', '0.022*"’" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"impact" + 0.005*"timely" + 0.004*"intervention" + 0.004*"always" + 0.004*"However" + 0.004*"progress"', '0.022*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"effective" + 0.005*"order" + 0.005*"plans" + 0.005*"receive" + 0.004*"always" + 0.004*"practice" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80449</t>
@@ -760,7 +760,7 @@
     <t>0.1327</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.005*"plans" + 0.004*"2022" + 0.004*"Council" + 0.004*"City" + 0.004*"senior" + 0.004*"lack" + 0.003*"risk" + 0.003*"2" + 0.003*"Bradford"', '0.022*"’" + 0.006*"plans" + 0.005*"impact" + 0.005*"practice" + 0.005*"2" + 0.005*"risk" + 0.004*"21" + 0.004*"Bradford" + 0.004*"Metropolitan" + 0.004*"need"', '0.024*"’" + 0.008*"plans" + 0.006*"needs" + 0.006*"Bradford" + 0.005*"quality" + 0.005*"changes" + 0.005*"2" + 0.005*"need" + 0.005*"◼" + 0.005*"progress"']</t>
+    <t>['0.021*"’" + 0.007*"plans" + 0.005*"need" + 0.005*"needs" + 0.005*"2" + 0.004*"Bradford" + 0.004*"◼" + 0.004*"2022" + 0.004*"progress" + 0.004*"City"', '0.020*"’" + 0.006*"plans" + 0.006*"Bradford" + 0.005*"risk" + 0.005*"2022" + 0.005*"impact" + 0.005*"practice" + 0.004*"quality" + 0.004*"need" + 0.004*"needs"', '0.021*"’" + 0.007*"plans" + 0.005*"needs" + 0.005*"impact" + 0.005*"2" + 0.005*"December" + 0.005*"However" + 0.005*"quality" + 0.004*"21" + 0.004*"worker"']</t>
   </si>
   <si>
     <t>80450</t>
@@ -796,7 +796,7 @@
     <t>0.2065</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.014*"needs" + 0.012*"well" + 0.010*"ensure" + 0.007*"clear" + 0.007*"effective" + 0.006*"plans" + 0.006*"good" + 0.006*"progress" + 0.005*"practice"', '0.011*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"ensure" + 0.005*"effective" + 0.005*"clear" + 0.005*"progress" + 0.005*"practice" + 0.004*"good" + 0.004*"within"', '0.010*"needs" + 0.009*"’" + 0.008*"well" + 0.008*"ensure" + 0.006*"effective" + 0.006*"progress" + 0.006*"plans" + 0.005*"supported" + 0.005*"clear" + 0.005*"individual"']</t>
+    <t>['0.011*"’" + 0.010*"well" + 0.009*"needs" + 0.008*"ensure" + 0.007*"clear" + 0.006*"effective" + 0.006*"good" + 0.005*"progress" + 0.005*"plans" + 0.005*"individual"', '0.013*"’" + 0.012*"needs" + 0.008*"well" + 0.007*"effective" + 0.007*"ensure" + 0.006*"clear" + 0.006*"progress" + 0.006*"good" + 0.005*"within" + 0.005*"plans"', '0.012*"needs" + 0.012*"’" + 0.011*"well" + 0.010*"ensure" + 0.006*"effective" + 0.005*"progress" + 0.005*"plans" + 0.005*"clear" + 0.005*"practice" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>80451</t>
@@ -835,7 +835,7 @@
     <t>0.1674</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"Wakefield" + 0.007*"leaders" + 0.007*"quality" + 0.007*"effective" + 0.007*"well" + 0.007*"November" + 0.007*"good" + 0.006*"plans" + 0.006*"progress"', '0.017*"’" + 0.009*"November" + 0.007*"well" + 0.007*"quality" + 0.006*"Wakefield" + 0.006*"good" + 0.006*"effective" + 0.006*"leaders" + 0.006*"plans" + 0.005*"practice"', '0.018*"’" + 0.008*"well" + 0.007*"leaders" + 0.007*"Wakefield" + 0.007*"quality" + 0.006*"good" + 0.006*"effective" + 0.006*"progress" + 0.005*"November" + 0.005*"plans"']</t>
+    <t>['0.015*"’" + 0.008*"Wakefield" + 0.007*"leaders" + 0.007*"effective" + 0.006*"well" + 0.006*"quality" + 0.006*"receive" + 0.005*"good" + 0.005*"November" + 0.005*"progress"', '0.020*"’" + 0.009*"quality" + 0.008*"Wakefield" + 0.008*"November" + 0.008*"well" + 0.007*"leaders" + 0.007*"effective" + 0.007*"good" + 0.006*"plans" + 0.005*"practice"', '0.015*"’" + 0.008*"well" + 0.008*"November" + 0.007*"plans" + 0.007*"good" + 0.007*"quality" + 0.007*"Wakefield" + 0.006*"leaders" + 0.006*"needs" + 0.006*"effective"']</t>
   </si>
   <si>
     <t>80453</t>
@@ -868,7 +868,7 @@
     <t>0.1621</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"However" + 0.006*"effective" + 0.005*"March" + 0.005*"York" + 0.005*"well" + 0.005*"need" + 0.005*"education"', '0.015*"’" + 0.008*"March" + 0.007*"needs" + 0.006*"quality" + 0.006*"effective" + 0.005*"practice" + 0.005*"7" + 0.005*"plans" + 0.005*"York" + 0.005*"However"', '0.015*"’" + 0.008*"needs" + 0.007*"March" + 0.007*"quality" + 0.006*"ensure" + 0.006*"effective" + 0.005*"York" + 0.005*"plans" + 0.005*"supported" + 0.005*"However"']</t>
+    <t>['0.011*"’" + 0.006*"needs" + 0.006*"March" + 0.005*"well" + 0.005*"York" + 0.005*"quality" + 0.004*"However" + 0.004*"ensure" + 0.004*"experiences" + 0.004*"practice"', '0.019*"’" + 0.009*"March" + 0.008*"quality" + 0.007*"needs" + 0.007*"effective" + 0.006*"plans" + 0.005*"practice" + 0.005*"ensure" + 0.005*"need" + 0.005*"York"', '0.013*"’" + 0.008*"needs" + 0.007*"effective" + 0.006*"quality" + 0.006*"However" + 0.006*"ensure" + 0.005*"York" + 0.005*"well" + 0.005*"March" + 0.005*"training"']</t>
   </si>
   <si>
     <t>80454</t>
@@ -907,7 +907,7 @@
     <t>0.1994</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.013*"well" + 0.007*"quality" + 0.007*"effective" + 0.005*"leaders" + 0.005*"timely" + 0.005*"plans" + 0.005*"Senior" + 0.005*"good" + 0.004*"arrangements"', '0.016*"well" + 0.012*"’" + 0.010*"leaders" + 0.009*"effective" + 0.008*"quality" + 0.006*"arrangements" + 0.006*"good" + 0.006*"highly" + 0.006*"plans" + 0.005*"Senior"', '0.014*"well" + 0.013*"quality" + 0.011*"’" + 0.009*"effective" + 0.008*"leaders" + 0.006*"timely" + 0.006*"plans" + 0.006*"good" + 0.005*"arrangements" + 0.005*"accommodation"']</t>
+    <t>['0.016*"well" + 0.009*"’" + 0.008*"effective" + 0.008*"quality" + 0.008*"leaders" + 0.006*"good" + 0.005*"arrangements" + 0.005*"highly" + 0.005*"timely" + 0.004*"accommodation"', '0.012*"well" + 0.012*"’" + 0.010*"effective" + 0.010*"quality" + 0.008*"leaders" + 0.007*"plans" + 0.006*"timely" + 0.006*"good" + 0.005*"arrangements" + 0.005*"highly"', '0.015*"well" + 0.015*"’" + 0.010*"quality" + 0.009*"leaders" + 0.008*"effective" + 0.006*"good" + 0.005*"arrangements" + 0.005*"timely" + 0.005*"plans" + 0.005*"high"']</t>
   </si>
   <si>
     <t>80455</t>
@@ -940,7 +940,7 @@
     <t>0.104</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.011*"Scilly" + 0.009*"practice" + 0.009*"Isles" + 0.008*"need" + 0.008*"needs" + 0.008*"information" + 0.007*"protection" + 0.006*"place" + 0.006*"risks"', '0.021*"’" + 0.014*"Isles" + 0.012*"Scilly" + 0.009*"information" + 0.007*"practice" + 0.007*"need" + 0.007*"protection" + 0.006*"13" + 0.006*"place" + 0.006*"quality"', '0.019*"’" + 0.013*"Scilly" + 0.013*"Isles" + 0.010*"information" + 0.008*"practice" + 0.008*"need" + 0.007*"quality" + 0.006*"needs" + 0.006*"protection" + 0.006*"risks"']</t>
+    <t>['0.026*"’" + 0.012*"Isles" + 0.012*"Scilly" + 0.009*"information" + 0.008*"need" + 0.008*"protection" + 0.008*"practice" + 0.007*"needs" + 0.006*"risks" + 0.006*"quality"', '0.017*"’" + 0.012*"Scilly" + 0.011*"Isles" + 0.008*"practice" + 0.008*"information" + 0.006*"need" + 0.006*"needs" + 0.006*"11" + 0.005*"place" + 0.005*"protection"', '0.018*"’" + 0.012*"Isles" + 0.012*"Scilly" + 0.009*"information" + 0.009*"practice" + 0.009*"need" + 0.007*"needs" + 0.007*"protection" + 0.006*"place" + 0.006*"quality"']</t>
   </si>
   <si>
     <t>80456</t>
@@ -976,7 +976,7 @@
     <t>0.1733</t>
   </si>
   <si>
-    <t>['0.024*"’" + 0.009*"well" + 0.008*"supported" + 0.008*"needs" + 0.008*"Coventry" + 0.007*"plans" + 0.006*"strong" + 0.005*"family" + 0.005*"need" + 0.005*"2022"', '0.015*"’" + 0.009*"Coventry" + 0.006*"well" + 0.006*"plans" + 0.005*"family" + 0.005*"needs" + 0.004*"supported" + 0.004*"training" + 0.004*"use" + 0.004*"education"', '0.016*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"Coventry" + 0.006*"strong" + 0.006*"supported" + 0.006*"family" + 0.006*"need" + 0.005*"plans" + 0.005*"PAs"']</t>
+    <t>['0.018*"’" + 0.008*"Coventry" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"family" + 0.006*"strong" + 0.005*"need" + 0.005*"supported" + 0.005*"1"', '0.020*"’" + 0.008*"well" + 0.008*"Coventry" + 0.007*"needs" + 0.006*"supported" + 0.005*"family" + 0.005*"strong" + 0.005*"plans" + 0.005*"need" + 0.004*"July"', '0.020*"’" + 0.008*"well" + 0.008*"Coventry" + 0.008*"supported" + 0.008*"needs" + 0.007*"plans" + 0.006*"family" + 0.005*"strong" + 0.005*"need" + 0.005*"20"']</t>
   </si>
   <si>
     <t>80458</t>
@@ -1018,7 +1018,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"leaders" + 0.006*"October" + 0.006*"Darlington" + 0.006*"effective" + 0.005*"practice" + 0.005*"supported" + 0.004*"quality"', '0.021*"’" + 0.008*"October" + 0.007*"practice" + 0.007*"needs" + 0.007*"well" + 0.006*"leaders" + 0.006*"Darlington" + 0.005*"need" + 0.005*"education" + 0.005*"quality"', '0.014*"’" + 0.009*"well" + 0.007*"leaders" + 0.006*"practice" + 0.006*"Darlington" + 0.005*"October" + 0.005*"quality" + 0.005*"needs" + 0.004*"effective" + 0.004*"plans"']</t>
+    <t>['0.020*"’" + 0.008*"leaders" + 0.008*"well" + 0.007*"needs" + 0.006*"practice" + 0.006*"Darlington" + 0.005*"quality" + 0.005*"October" + 0.005*"effective" + 0.004*"family"', '0.019*"’" + 0.008*"October" + 0.007*"well" + 0.007*"needs" + 0.007*"practice" + 0.006*"Darlington" + 0.006*"leaders" + 0.005*"supported" + 0.005*"effective" + 0.004*"education"', '0.014*"’" + 0.008*"well" + 0.006*"October" + 0.005*"Darlington" + 0.005*"practice" + 0.005*"leaders" + 0.005*"needs" + 0.004*"effective" + 0.004*"quality" + 0.004*"21"']</t>
   </si>
   <si>
     <t>80459</t>
@@ -1060,7 +1060,7 @@
     <t>0.1995</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.011*"needs" + 0.008*"Derby" + 0.006*"need" + 0.006*"good" + 0.006*"receive" + 0.006*"progress" + 0.006*"quality" + 0.005*"plans" + 0.005*"well"', '0.017*"’" + 0.009*"needs" + 0.007*"receive" + 0.006*"quality" + 0.006*"plans" + 0.006*"Derby" + 0.006*"well" + 0.005*"appropriate" + 0.005*"leaders" + 0.005*"progress"', '0.024*"’" + 0.008*"needs" + 0.007*"Derby" + 0.007*"quality" + 0.006*"leaders" + 0.006*"progress" + 0.005*"appropriate" + 0.005*"plans" + 0.005*"21" + 0.005*"views"']</t>
+    <t>['0.026*"’" + 0.011*"needs" + 0.009*"Derby" + 0.007*"quality" + 0.006*"plans" + 0.006*"good" + 0.006*"receive" + 0.006*"progress" + 0.006*"appropriate" + 0.006*"leaders"', '0.019*"’" + 0.010*"needs" + 0.006*"receive" + 0.006*"well" + 0.006*"Derby" + 0.006*"need" + 0.006*"appropriate" + 0.005*"progress" + 0.005*"quality" + 0.005*"oversight"', '0.013*"’" + 0.005*"receive" + 0.005*"quality" + 0.005*"leaders" + 0.004*"progress" + 0.004*"needs" + 0.004*"helps" + 0.004*"Derby" + 0.004*"oversight" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80460</t>
@@ -1093,7 +1093,7 @@
     <t>0.1913</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"Derbyshire" + 0.006*"well" + 0.005*"need" + 0.004*"plans" + 0.004*"good" + 0.004*"health" + 0.004*"30" + 0.004*"needs" + 0.004*"positive"', '0.015*"’" + 0.009*"well" + 0.007*"Derbyshire" + 0.005*"education" + 0.005*"plans" + 0.005*"leaders" + 0.005*"health" + 0.005*"10" + 0.004*"needs" + 0.004*"number"', '0.014*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.006*"positive" + 0.005*"needs" + 0.005*"plans" + 0.005*"30" + 0.005*"October" + 0.005*"effective" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.008*"Derbyshire" + 0.007*"well" + 0.005*"plans" + 0.004*"positive" + 0.004*"effective" + 0.004*"October" + 0.004*"health" + 0.004*"education" + 0.004*"experiences"', '0.011*"’" + 0.008*"well" + 0.006*"Derbyshire" + 0.006*"needs" + 0.005*"positive" + 0.005*"health" + 0.004*"plans" + 0.004*"good" + 0.004*"effective" + 0.004*"need"', '0.015*"’" + 0.009*"well" + 0.006*"Derbyshire" + 0.005*"need" + 0.005*"leaders" + 0.005*"10" + 0.005*"30" + 0.005*"needs" + 0.005*"good" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80461</t>
@@ -1126,7 +1126,7 @@
     <t>0.1234</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.006*"well" + 0.005*"risk" + 0.005*"health" + 0.005*"progress" + 0.005*"leaders" + 0.004*"areas" + 0.004*"practice" + 0.004*"needs" + 0.004*"protection"', '0.009*"’" + 0.006*"well" + 0.005*"progress" + 0.004*"health" + 0.004*"risk" + 0.004*"protection" + 0.004*"living" + 0.004*"quality" + 0.004*"leaders" + 0.003*"plans"', '0.009*"’" + 0.006*"leaders" + 0.005*"well" + 0.004*"case" + 0.004*"health" + 0.004*"Devon" + 0.004*"risk" + 0.004*"risks" + 0.004*"need" + 0.004*"time"']</t>
+    <t>['0.007*"’" + 0.005*"well" + 0.005*"health" + 0.005*"leaders" + 0.004*"progress" + 0.004*"protection" + 0.004*"practice" + 0.004*"risk" + 0.004*"areas" + 0.004*"risks"', '0.010*"’" + 0.007*"well" + 0.005*"health" + 0.005*"risk" + 0.005*"leaders" + 0.005*"progress" + 0.004*"practice" + 0.004*"case" + 0.004*"quality" + 0.004*"living"', '0.010*"’" + 0.005*"risk" + 0.005*"well" + 0.004*"leaders" + 0.004*"time" + 0.004*"progress" + 0.004*"Devon" + 0.004*"areas" + 0.004*"need" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80462</t>
@@ -1168,7 +1168,7 @@
     <t>6</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.005*"well" + 0.005*"effective" + 0.005*"February" + 0.004*"Doncaster" + 0.004*"records" + 0.004*"leaders" + 0.004*"protection" + 0.004*"arrangements" + 0.004*"25"', '0.017*"’" + 0.007*"Doncaster" + 0.006*"well" + 0.005*"many" + 0.005*"plans" + 0.005*"leaders" + 0.005*"Trust" + 0.005*"arrangements" + 0.005*"progress" + 0.005*"oversight"', '0.025*"’" + 0.007*"well" + 0.006*"Doncaster" + 0.006*"progress" + 0.005*"quality" + 0.005*"records" + 0.005*"many" + 0.005*"information" + 0.005*"plans" + 0.005*"leaders"']</t>
+    <t>['0.020*"’" + 0.006*"well" + 0.005*"records" + 0.005*"progress" + 0.005*"plans" + 0.005*"oversight" + 0.005*"leaders" + 0.004*"experiences" + 0.004*"quality" + 0.004*"time"', '0.023*"’" + 0.007*"well" + 0.007*"Doncaster" + 0.006*"many" + 0.005*"leaders" + 0.005*"progress" + 0.005*"quality" + 0.005*"protection" + 0.005*"14" + 0.005*"plans"', '0.015*"’" + 0.006*"well" + 0.006*"Doncaster" + 0.005*"information" + 0.005*"records" + 0.004*"arrangements" + 0.004*"many" + 0.004*"leaders" + 0.004*"25" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>2532283</t>
@@ -1201,7 +1201,7 @@
     <t>0.1922</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.009*"Dorset" + 0.006*"well" + 0.006*"good" + 0.005*"arrangements" + 0.005*"need" + 0.004*"needs" + 0.004*"Senior" + 0.004*"8" + 0.004*"October"', '0.017*"’" + 0.008*"Dorset" + 0.006*"good" + 0.006*"well" + 0.005*"27" + 0.005*"needs" + 0.005*"arrangements" + 0.005*"leaders" + 0.004*"8" + 0.004*"including"', '0.009*"’" + 0.006*"good" + 0.005*"Dorset" + 0.005*"well" + 0.004*"quality" + 0.004*"change" + 0.004*"needs" + 0.003*"leaders" + 0.003*"arrangements" + 0.003*"2021"']</t>
+    <t>['0.017*"’" + 0.008*"Dorset" + 0.007*"good" + 0.006*"well" + 0.005*"8" + 0.005*"arrangements" + 0.004*"needs" + 0.004*"including" + 0.004*"home" + 0.004*"need"', '0.012*"’" + 0.009*"Dorset" + 0.006*"well" + 0.005*"good" + 0.005*"arrangements" + 0.005*"needs" + 0.004*"2021" + 0.004*"8" + 0.004*"October" + 0.004*"leaders"', '0.010*"’" + 0.006*"good" + 0.006*"well" + 0.005*"Dorset" + 0.004*"October" + 0.004*"needs" + 0.004*"change" + 0.004*"27" + 0.004*"impact" + 0.003*"health"']</t>
   </si>
   <si>
     <t>80464</t>
@@ -1234,7 +1234,7 @@
     <t>0.1605</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"needs" + 0.010*"Dudley" + 0.006*"always" + 0.006*"arrangements" + 0.006*"well" + 0.005*"plans" + 0.005*"ensure" + 0.005*"However" + 0.005*"practice"', '0.016*"’" + 0.010*"needs" + 0.007*"Dudley" + 0.006*"well" + 0.004*"plans" + 0.004*"11" + 0.004*"ensure" + 0.004*"2022" + 0.004*"arrangements" + 0.004*"oversight"', '0.015*"’" + 0.010*"needs" + 0.006*"Dudley" + 0.006*"plans" + 0.005*"quality" + 0.005*"oversight" + 0.004*"management" + 0.004*"well" + 0.004*"always" + 0.004*"11"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.008*"Dudley" + 0.005*"well" + 0.005*"always" + 0.004*"However" + 0.004*"arrangements" + 0.004*"enough" + 0.004*"management" + 0.004*"31"', '0.016*"’" + 0.010*"Dudley" + 0.009*"needs" + 0.006*"always" + 0.005*"arrangements" + 0.005*"quality" + 0.005*"well" + 0.005*"oversight" + 0.005*"plans" + 0.004*"ensure"', '0.014*"needs" + 0.014*"’" + 0.006*"plans" + 0.006*"Dudley" + 0.006*"well" + 0.005*"arrangements" + 0.005*"always" + 0.005*"ensure" + 0.005*"oversight" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80465</t>
@@ -1273,7 +1273,7 @@
     <t>0.1734</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"needs" + 0.007*"May" + 0.006*"Durham" + 0.005*"progress" + 0.005*"practice" + 0.005*"well" + 0.005*"making" + 0.005*"supported" + 0.004*"plans"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"Durham" + 0.007*"plans" + 0.006*"ensure" + 0.005*"family" + 0.005*"number" + 0.005*"May" + 0.004*"practice"', '0.017*"’" + 0.012*"needs" + 0.008*"May" + 0.007*"Durham" + 0.007*"plans" + 0.007*"ensure" + 0.007*"well" + 0.006*"practice" + 0.006*"leaders" + 0.005*"risks"']</t>
+    <t>['0.013*"’" + 0.008*"Durham" + 0.008*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"practice" + 0.005*"leaders" + 0.005*"May" + 0.005*"risks" + 0.005*"20"', '0.017*"’" + 0.013*"needs" + 0.009*"May" + 0.008*"plans" + 0.008*"ensure" + 0.008*"well" + 0.007*"Durham" + 0.006*"practice" + 0.005*"progress" + 0.005*"number"', '0.010*"’" + 0.008*"needs" + 0.005*"May" + 0.005*"Durham" + 0.005*"well" + 0.004*"plans" + 0.004*"ensure" + 0.004*"leaders" + 0.004*"family" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80466</t>
@@ -1309,7 +1309,7 @@
     <t>0.1742</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.011*"needs" + 0.010*"plans" + 0.009*"well" + 0.006*"Riding" + 0.006*"East" + 0.006*"progress" + 0.005*"partners" + 0.004*"10" + 0.004*"information"', '0.013*"’" + 0.008*"progress" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.005*"Riding" + 0.005*"East" + 0.004*"10" + 0.004*"30" + 0.004*"education"', '0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"plans" + 0.007*"East" + 0.007*"progress" + 0.006*"Riding" + 0.005*"good" + 0.005*"10" + 0.005*"education"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.008*"plans" + 0.007*"well" + 0.006*"progress" + 0.005*"East" + 0.005*"Riding" + 0.004*"10" + 0.004*"education" + 0.004*"good"', '0.016*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"needs" + 0.007*"Riding" + 0.006*"progress" + 0.006*"East" + 0.006*"partners" + 0.005*"good" + 0.005*"10"', '0.017*"’" + 0.009*"plans" + 0.009*"needs" + 0.008*"well" + 0.008*"progress" + 0.006*"East" + 0.006*"Riding" + 0.005*"30" + 0.005*"place" + 0.005*"2023"']</t>
   </si>
   <si>
     <t>80467</t>
@@ -1342,7 +1342,7 @@
     <t>0.1738</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"plans" + 0.008*"well" + 0.007*"progress" + 0.006*"needs" + 0.006*"Sussex" + 0.006*"including" + 0.006*"East" + 0.005*"impact" + 0.005*"15"', '0.015*"’" + 0.009*"well" + 0.007*"needs" + 0.007*"plans" + 0.007*"East" + 0.005*"impact" + 0.005*"progress" + 0.005*"experiences" + 0.005*"including" + 0.005*"Sussex"', '0.019*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"plans" + 0.007*"Sussex" + 0.006*"East" + 0.006*"provide" + 0.006*"progress" + 0.005*"including" + 0.005*"11"']</t>
+    <t>['0.018*"’" + 0.011*"well" + 0.008*"plans" + 0.007*"needs" + 0.007*"progress" + 0.006*"East" + 0.006*"including" + 0.006*"provide" + 0.006*"impact" + 0.006*"Sussex"', '0.012*"’" + 0.007*"well" + 0.006*"Sussex" + 0.006*"progress" + 0.006*"needs" + 0.005*"including" + 0.005*"East" + 0.004*"plans" + 0.004*"11" + 0.004*"effective"', '0.017*"’" + 0.009*"plans" + 0.009*"needs" + 0.009*"well" + 0.007*"East" + 0.006*"Sussex" + 0.005*"progress" + 0.005*"experiences" + 0.005*"impact" + 0.005*"including"']</t>
   </si>
   <si>
     <t>80468</t>
@@ -1381,7 +1381,7 @@
     <t>0.1965</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.006*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"progress" + 0.005*"new" + 0.005*"need" + 0.005*"advisers" + 0.005*"Essex" + 0.004*"parents"', '0.013*"’" + 0.006*"well" + 0.005*"risk" + 0.004*"progress" + 0.004*"supported" + 0.004*"new" + 0.004*"quality" + 0.004*"need" + 0.004*"Essex" + 0.004*"experiences"', '0.019*"’" + 0.008*"progress" + 0.007*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"family" + 0.006*"understand" + 0.005*"‘" + 0.005*"Essex" + 0.005*"experiences"']</t>
+    <t>['0.021*"’" + 0.008*"well" + 0.007*"plans" + 0.006*"Essex" + 0.005*"understand" + 0.005*"family" + 0.005*"needs" + 0.005*"progress" + 0.005*"practice" + 0.005*"helped"', '0.016*"’" + 0.009*"progress" + 0.007*"well" + 0.007*"needs" + 0.005*"family" + 0.005*"risk" + 0.005*"plans" + 0.005*"advisers" + 0.004*"need" + 0.004*"helped"', '0.016*"’" + 0.007*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"new" + 0.005*"experiences" + 0.005*"well" + 0.005*"leaders" + 0.005*"supported" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80469</t>
@@ -1420,7 +1420,7 @@
     <t>0.1938</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"effective" + 0.008*"good" + 0.006*"quality" + 0.006*"practice" + 0.006*"well" + 0.006*"needs" + 0.006*"timely" + 0.005*"early" + 0.005*"plans"', '0.011*"’" + 0.008*"effective" + 0.007*"good" + 0.006*"practice" + 0.006*"needs" + 0.005*"well" + 0.005*"quality" + 0.004*"timely" + 0.004*"progress" + 0.004*"improve"', '0.013*"’" + 0.007*"effective" + 0.007*"quality" + 0.007*"practice" + 0.006*"needs" + 0.006*"timely" + 0.006*"well" + 0.005*"good" + 0.005*"plans" + 0.004*"improve"']</t>
+    <t>['0.012*"’" + 0.007*"effective" + 0.007*"practice" + 0.006*"quality" + 0.006*"good" + 0.005*"needs" + 0.005*"focus" + 0.005*"improve" + 0.004*"team" + 0.004*"timely"', '0.016*"’" + 0.008*"effective" + 0.007*"good" + 0.006*"quality" + 0.006*"needs" + 0.006*"practice" + 0.006*"well" + 0.005*"need" + 0.005*"timely" + 0.005*"improve"', '0.012*"’" + 0.009*"effective" + 0.007*"good" + 0.006*"well" + 0.006*"practice" + 0.006*"timely" + 0.006*"needs" + 0.006*"quality" + 0.005*"early" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80470</t>
@@ -1456,7 +1456,7 @@
     <t>0.1977</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"needs" + 0.007*"February" + 0.006*"2022" + 0.006*"well" + 0.006*"plans" + 0.005*"leaders" + 0.005*"7" + 0.005*"family" + 0.005*"good"', '0.015*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"2022" + 0.006*"Gloucestershire" + 0.006*"February" + 0.005*"protection" + 0.005*"progress" + 0.005*"well" + 0.004*"family"', '0.017*"’" + 0.008*"needs" + 0.008*"2022" + 0.007*"plans" + 0.007*"February" + 0.006*"progress" + 0.005*"well" + 0.005*"18" + 0.005*"quality" + 0.005*"need"']</t>
+    <t>['0.021*"’" + 0.009*"needs" + 0.008*"plans" + 0.008*"2022" + 0.007*"February" + 0.006*"well" + 0.005*"progress" + 0.005*"Gloucestershire" + 0.005*"experienced" + 0.005*"protection"', '0.017*"’" + 0.008*"needs" + 0.007*"2022" + 0.007*"February" + 0.006*"plans" + 0.005*"timely" + 0.005*"well" + 0.005*"progress" + 0.004*"18" + 0.004*"Gloucestershire"', '0.012*"’" + 0.007*"needs" + 0.006*"February" + 0.005*"well" + 0.005*"good" + 0.005*"2022" + 0.004*"plans" + 0.004*"experienced" + 0.004*"Gloucestershire" + 0.004*"family"']</t>
   </si>
   <si>
     <t>80471</t>
@@ -1489,7 +1489,7 @@
     <t>0.1822</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.013*"well" + 0.009*"needs" + 0.009*"plans" + 0.008*"need" + 0.007*"risk" + 0.007*"planning" + 0.007*"practice" + 0.006*"always" + 0.006*"good"', '0.011*"’" + 0.009*"practice" + 0.007*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"always" + 0.006*"quality" + 0.006*"risk" + 0.005*"planning"', '0.010*"’" + 0.009*"practice" + 0.009*"well" + 0.007*"needs" + 0.007*"risk" + 0.006*"plans" + 0.006*"effective" + 0.005*"planning" + 0.005*"need" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.012*"well" + 0.010*"needs" + 0.009*"plans" + 0.007*"practice" + 0.007*"need" + 0.007*"risk" + 0.006*"planning" + 0.006*"always" + 0.006*"good"', '0.010*"’" + 0.009*"well" + 0.008*"practice" + 0.007*"plans" + 0.007*"planning" + 0.007*"good" + 0.006*"needs" + 0.006*"effective" + 0.006*"risk" + 0.005*"quality"', '0.009*"practice" + 0.008*"’" + 0.008*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"risk" + 0.006*"effective" + 0.005*"always" + 0.005*"good" + 0.005*"plans"']</t>
   </si>
   <si>
     <t>80472</t>
@@ -1516,7 +1516,7 @@
     <t>0.1893</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"well" + 0.005*"strong" + 0.004*"carers" + 0.004*"leaders" + 0.004*"highly" + 0.004*"improve" + 0.004*"home"', '0.024*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"quality" + 0.005*"leaders" + 0.005*"plans" + 0.004*"home" + 0.004*"strong" + 0.004*"improve" + 0.004*"Hampshire"', '0.018*"’" + 0.007*"needs" + 0.006*"plans" + 0.005*"well" + 0.005*"quality" + 0.004*"health" + 0.004*"home" + 0.004*"progress" + 0.004*"strong" + 0.004*"Hampshire"']</t>
+    <t>['0.016*"’" + 0.007*"needs" + 0.006*"plans" + 0.006*"well" + 0.005*"quality" + 0.005*"leaders" + 0.004*"home" + 0.004*"Hampshire" + 0.004*"improve" + 0.004*"carers"', '0.018*"’" + 0.006*"needs" + 0.006*"plans" + 0.005*"quality" + 0.005*"well" + 0.004*"improve" + 0.004*"strong" + 0.004*"home" + 0.004*"leaders" + 0.004*"highly"', '0.022*"’" + 0.009*"needs" + 0.006*"well" + 0.005*"strong" + 0.005*"plans" + 0.004*"need" + 0.004*"quality" + 0.004*"Hampshire" + 0.004*"leaders" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80473</t>
@@ -1546,7 +1546,7 @@
     <t>0.2009</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"March" + 0.005*"Hartlepool" + 0.005*"well" + 0.005*"ensure" + 0.004*"need" + 0.004*"leaders" + 0.004*"plans" + 0.004*"needs" + 0.004*"22"', '0.018*"’" + 0.006*"Hartlepool" + 0.006*"March" + 0.006*"well" + 0.005*"needs" + 0.005*"18" + 0.005*"leaders" + 0.005*"supported" + 0.004*"practice" + 0.004*"strong"', '0.023*"’" + 0.009*"needs" + 0.008*"Hartlepool" + 0.008*"March" + 0.006*"leaders" + 0.006*"well" + 0.005*"plans" + 0.005*"clear" + 0.005*"effective" + 0.005*"18"']</t>
+    <t>['0.019*"’" + 0.007*"needs" + 0.007*"Hartlepool" + 0.005*"March" + 0.005*"well" + 0.005*"leaders" + 0.005*"practice" + 0.004*"18" + 0.004*"clear" + 0.004*"plans"', '0.019*"’" + 0.007*"March" + 0.007*"needs" + 0.006*"Hartlepool" + 0.006*"well" + 0.006*"leaders" + 0.005*"22" + 0.005*"effective" + 0.005*"strong" + 0.005*"family"', '0.021*"’" + 0.008*"March" + 0.008*"Hartlepool" + 0.006*"well" + 0.006*"needs" + 0.006*"leaders" + 0.005*"plans" + 0.005*"18" + 0.005*"strong" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80474</t>
@@ -1579,7 +1579,7 @@
     <t>0.1018</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.005*"lack" + 0.004*"many" + 0.004*"plans" + 0.004*"Herefordshire" + 0.004*"impact" + 0.004*"practice" + 0.004*"including" + 0.003*"needs" + 0.003*"oversight"', '0.022*"’" + 0.007*"practice" + 0.006*"Herefordshire" + 0.006*"lack" + 0.005*"impact" + 0.005*"needs" + 0.005*"many" + 0.005*"July" + 0.004*"quality" + 0.004*"18"', '0.012*"’" + 0.005*"Herefordshire" + 0.005*"needs" + 0.004*"harm" + 0.004*"practice" + 0.004*"plans" + 0.004*"impact" + 0.004*"29" + 0.004*"carers" + 0.004*"many"']</t>
+    <t>['0.016*"’" + 0.005*"practice" + 0.005*"impact" + 0.005*"lack" + 0.004*"Herefordshire" + 0.004*"needs" + 0.004*"many" + 0.004*"plans" + 0.004*"progress" + 0.004*"July"', '0.016*"’" + 0.006*"lack" + 0.005*"Herefordshire" + 0.005*"needs" + 0.005*"impact" + 0.004*"practice" + 0.004*"quality" + 0.004*"plans" + 0.004*"management" + 0.004*"oversight"', '0.019*"’" + 0.007*"practice" + 0.006*"Herefordshire" + 0.005*"many" + 0.005*"18" + 0.005*"impact" + 0.004*"needs" + 0.004*"lack" + 0.004*"plans" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80475</t>
@@ -1612,7 +1612,7 @@
     <t>0.1744</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.005*"needs" + 0.005*"Hertfordshire" + 0.004*"2023" + 0.004*"well" + 0.003*"receive" + 0.003*"positive" + 0.003*"27" + 0.003*"‘" + 0.003*"training"', '0.024*"’" + 0.007*"well" + 0.007*"Hertfordshire" + 0.006*"needs" + 0.005*"need" + 0.005*"23" + 0.004*"leaders" + 0.004*"plans" + 0.004*"risk" + 0.004*"receive"', '0.026*"’" + 0.007*"well" + 0.007*"Hertfordshire" + 0.007*"receive" + 0.006*"needs" + 0.005*"plans" + 0.004*"27" + 0.004*"effective" + 0.004*"risk" + 0.004*"January"']</t>
+    <t>['0.018*"’" + 0.006*"Hertfordshire" + 0.006*"well" + 0.005*"needs" + 0.005*"receive" + 0.004*"‘" + 0.004*"effective" + 0.004*"family" + 0.004*"January" + 0.004*"23"', '0.018*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"Hertfordshire" + 0.004*"risk" + 0.004*"receive" + 0.003*"training" + 0.003*"‘" + 0.003*"effective" + 0.003*"need"', '0.028*"’" + 0.007*"Hertfordshire" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"receive" + 0.005*"2023" + 0.005*"positive" + 0.005*"leaders" + 0.005*"23"']</t>
   </si>
   <si>
     <t>80419</t>
@@ -1642,7 +1642,7 @@
     <t>0.1908</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"leaders" + 0.006*"well" + 0.006*"3" + 0.006*"needs" + 0.005*"improve" + 0.005*"supported" + 0.005*"progress" + 0.005*"plans" + 0.005*"Wight"', '0.014*"’" + 0.008*"leaders" + 0.006*"Senior" + 0.006*"well" + 0.005*"plans" + 0.005*"information" + 0.005*"PAs" + 0.005*"Wight" + 0.005*"needs" + 0.005*"supported"', '0.016*"’" + 0.008*"leaders" + 0.006*"needs" + 0.006*"Isle" + 0.005*"practice" + 0.005*"good" + 0.005*"well" + 0.005*"3" + 0.005*"progress" + 0.005*"October"']</t>
+    <t>['0.018*"’" + 0.008*"leaders" + 0.005*"needs" + 0.005*"well" + 0.005*"PAs" + 0.005*"Isle" + 0.005*"Wight" + 0.005*"plans" + 0.005*"experiences" + 0.005*"progress"', '0.017*"’" + 0.010*"leaders" + 0.006*"needs" + 0.005*"supported" + 0.005*"Isle" + 0.005*"good" + 0.005*"well" + 0.005*"Senior" + 0.005*"3" + 0.005*"30"', '0.018*"’" + 0.007*"leaders" + 0.006*"Senior" + 0.006*"well" + 0.006*"plans" + 0.005*"progress" + 0.005*"3" + 0.005*"needs" + 0.005*"Wight" + 0.005*"improve"']</t>
   </si>
   <si>
     <t>80476</t>
@@ -1666,7 +1666,7 @@
     <t>0.2202</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"Kent" + 0.008*"needs" + 0.007*"supported" + 0.006*"County" + 0.006*"Council" + 0.005*"well" + 0.004*"practice" + 0.004*"need" + 0.004*"progress"', '0.021*"’" + 0.011*"Kent" + 0.007*"well" + 0.007*"Council" + 0.007*"needs" + 0.005*"supported" + 0.005*"County" + 0.005*"progress" + 0.005*"practice" + 0.004*"leaders"', '0.014*"’" + 0.008*"Kent" + 0.007*"needs" + 0.006*"well" + 0.004*"supported" + 0.004*"progress" + 0.004*"ensure" + 0.004*"Council" + 0.004*"leaders" + 0.004*"impact"']</t>
+    <t>['0.020*"’" + 0.008*"needs" + 0.008*"Kent" + 0.007*"well" + 0.005*"supported" + 0.005*"Council" + 0.004*"leaders" + 0.004*"progress" + 0.004*"County" + 0.004*"including"', '0.020*"’" + 0.011*"Kent" + 0.007*"needs" + 0.006*"supported" + 0.006*"Council" + 0.005*"well" + 0.005*"9" + 0.005*"County" + 0.005*"practice" + 0.005*"impact"', '0.014*"’" + 0.011*"Kent" + 0.007*"Council" + 0.006*"needs" + 0.006*"County" + 0.006*"well" + 0.005*"progress" + 0.005*"supported" + 0.005*"practice" + 0.004*"2022"']</t>
   </si>
   <si>
     <t>80477</t>
@@ -1696,7 +1696,7 @@
     <t>0.1534</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.006*"planning" + 0.006*"protection" + 0.006*"practice" + 0.006*"progress" + 0.006*"Hull" + 0.005*"well" + 0.005*"number" + 0.005*"risks" + 0.005*"impact"', '0.016*"’" + 0.008*"number" + 0.006*"Hull" + 0.006*"practice" + 0.006*"management" + 0.006*"planning" + 0.005*"well" + 0.005*"risks" + 0.005*"need" + 0.005*"November"', '0.017*"’" + 0.007*"number" + 0.007*"planning" + 0.007*"well" + 0.006*"need" + 0.006*"protection" + 0.006*"small" + 0.005*"management" + 0.005*"practice" + 0.005*"needs"']</t>
+    <t>['0.013*"’" + 0.007*"number" + 0.005*"well" + 0.005*"practice" + 0.005*"impact" + 0.005*"planning" + 0.005*"teams" + 0.005*"need" + 0.004*"25" + 0.004*"management"', '0.014*"’" + 0.007*"number" + 0.006*"risks" + 0.006*"protection" + 0.006*"well" + 0.006*"small" + 0.006*"need" + 0.006*"planning" + 0.006*"practice" + 0.006*"management"', '0.019*"’" + 0.008*"planning" + 0.007*"number" + 0.006*"Hull" + 0.006*"protection" + 0.006*"practice" + 0.006*"well" + 0.005*"oversight" + 0.005*"need" + 0.005*"agency"']</t>
   </si>
   <si>
     <t>80478</t>
@@ -1729,7 +1729,7 @@
     <t>0.1559</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"good" + 0.007*"practice" + 0.006*"quality" + 0.005*"Senior" + 0.005*"training" + 0.005*"protection" + 0.005*"needs" + 0.005*"need" + 0.005*"plans"', '0.012*"’" + 0.007*"quality" + 0.006*"good" + 0.005*"practice" + 0.005*"well" + 0.005*"needs" + 0.005*"training" + 0.005*"plans" + 0.004*"Senior" + 0.004*"senior"', '0.012*"’" + 0.006*"permanence" + 0.006*"practice" + 0.006*"quality" + 0.006*"plans" + 0.005*"well" + 0.005*"protection" + 0.005*"senior" + 0.004*"Senior" + 0.004*"needs"']</t>
+    <t>['0.012*"’" + 0.006*"practice" + 0.006*"quality" + 0.006*"good" + 0.006*"training" + 0.006*"permanence" + 0.005*"plans" + 0.005*"needs" + 0.005*"senior" + 0.005*"protection"', '0.012*"’" + 0.007*"good" + 0.007*"quality" + 0.006*"well" + 0.005*"practice" + 0.005*"needs" + 0.005*"Senior" + 0.005*"permanence" + 0.005*"protection" + 0.005*"training"', '0.010*"’" + 0.007*"practice" + 0.006*"quality" + 0.005*"well" + 0.005*"plans" + 0.005*"Senior" + 0.005*"protection" + 0.004*"permanence" + 0.004*"good" + 0.004*"senior"']</t>
   </si>
   <si>
     <t>80479</t>
@@ -1768,7 +1768,7 @@
     <t>0</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"progress" + 0.007*"needs" + 0.006*"quality" + 0.006*"plans" + 0.005*"2021" + 0.005*"Knowsley" + 0.005*"impact" + 0.005*"good" + 0.005*"22"', '0.014*"’" + 0.008*"plans" + 0.008*"progress" + 0.008*"needs" + 0.006*"experiences" + 0.006*"2021" + 0.005*"Knowsley" + 0.005*"quality" + 0.005*"need" + 0.005*"11"', '0.014*"’" + 0.009*"progress" + 0.008*"quality" + 0.007*"plans" + 0.007*"Knowsley" + 0.006*"needs" + 0.006*"2021" + 0.005*"experiences" + 0.005*"good" + 0.005*"domestic"']</t>
+    <t>['0.014*"’" + 0.008*"plans" + 0.007*"progress" + 0.007*"needs" + 0.006*"quality" + 0.005*"impact" + 0.005*"2021" + 0.005*"22" + 0.005*"experiences" + 0.005*"abuse"', '0.010*"’" + 0.007*"needs" + 0.006*"Knowsley" + 0.006*"progress" + 0.005*"2021" + 0.005*"plans" + 0.005*"quality" + 0.004*"need" + 0.004*"experiences" + 0.004*"education"', '0.017*"’" + 0.010*"progress" + 0.009*"quality" + 0.007*"plans" + 0.007*"needs" + 0.006*"Knowsley" + 0.006*"good" + 0.006*"2021" + 0.005*"need" + 0.005*"11"']</t>
   </si>
   <si>
     <t>80480</t>
@@ -1801,7 +1801,7 @@
     <t>0.1671</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"need" + 0.007*"well" + 0.006*"Lancashire" + 0.006*"needs" + 0.006*"plans" + 0.005*"9" + 0.005*"live" + 0.005*"parents" + 0.005*"supported"', '0.017*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"need" + 0.007*"Lancashire" + 0.006*"plans" + 0.006*"information" + 0.005*"practice" + 0.005*"progress" + 0.005*"live"', '0.015*"’" + 0.010*"well" + 0.007*"needs" + 0.006*"need" + 0.006*"supported" + 0.005*"practice" + 0.005*"number" + 0.005*"Lancashire" + 0.005*"positive" + 0.005*"health"']</t>
+    <t>['0.019*"’" + 0.009*"well" + 0.007*"need" + 0.007*"needs" + 0.006*"positive" + 0.005*"good" + 0.005*"supported" + 0.005*"Lancashire" + 0.005*"plans" + 0.005*"practice"', '0.014*"’" + 0.009*"well" + 0.008*"need" + 0.008*"needs" + 0.006*"Lancashire" + 0.006*"live" + 0.005*"supported" + 0.005*"plans" + 0.005*"9" + 0.005*"progress"', '0.015*"’" + 0.007*"Lancashire" + 0.007*"well" + 0.007*"needs" + 0.005*"plans" + 0.005*"need" + 0.005*"practice" + 0.005*"health" + 0.005*"supported" + 0.005*"9"']</t>
   </si>
   <si>
     <t>80481</t>
@@ -1831,7 +1831,7 @@
     <t>0.1792</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.006*"Leeds" + 0.006*"well" + 0.006*"risk" + 0.004*"March" + 0.004*"ensure" + 0.004*"practice" + 0.004*"2022" + 0.004*"4"', '0.016*"’" + 0.009*"Leeds" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.005*"21" + 0.004*"plans" + 0.004*"protection" + 0.004*"supported" + 0.004*"February"', '0.015*"’" + 0.008*"needs" + 0.006*"well" + 0.006*"Leeds" + 0.005*"risk" + 0.005*"protection" + 0.005*"4" + 0.005*"ensure" + 0.004*"plans" + 0.004*"leaders"']</t>
+    <t>['0.016*"’" + 0.007*"Leeds" + 0.006*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"risk" + 0.005*"4" + 0.004*"making" + 0.004*"ensure" + 0.004*"February"', '0.014*"’" + 0.007*"Leeds" + 0.007*"needs" + 0.006*"risk" + 0.005*"well" + 0.005*"ensure" + 0.004*"protection" + 0.004*"2022" + 0.004*"information" + 0.004*"4"', '0.018*"’" + 0.008*"needs" + 0.007*"Leeds" + 0.006*"well" + 0.005*"plans" + 0.005*"supported" + 0.005*"risk" + 0.005*"protection" + 0.004*"including" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80482</t>
@@ -1867,7 +1867,7 @@
     <t>0.2013</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.009*"well" + 0.009*"Leicester" + 0.007*"2021" + 0.007*"needs" + 0.006*"good" + 0.005*"number" + 0.005*"20" + 0.005*"ensure" + 0.004*"1"', '0.023*"’" + 0.009*"2021" + 0.007*"needs" + 0.007*"well" + 0.007*"Leicester" + 0.006*"ensure" + 0.006*"good" + 0.005*"1" + 0.005*"20" + 0.005*"including"', '0.016*"’" + 0.010*"well" + 0.009*"2021" + 0.007*"Leicester" + 0.006*"number" + 0.005*"good" + 0.005*"ensure" + 0.005*"needs" + 0.005*"1" + 0.004*"City"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.008*"needs" + 0.007*"2021" + 0.007*"ensure" + 0.006*"Leicester" + 0.005*"Council" + 0.005*"good" + 0.005*"including" + 0.005*"October"', '0.013*"’" + 0.007*"2021" + 0.006*"needs" + 0.006*"Leicester" + 0.006*"well" + 0.005*"good" + 0.005*"September" + 0.005*"number" + 0.005*"ensure" + 0.004*"including"', '0.025*"’" + 0.011*"well" + 0.010*"2021" + 0.009*"Leicester" + 0.007*"good" + 0.007*"number" + 0.006*"needs" + 0.006*"20" + 0.006*"1" + 0.005*"ensure"']</t>
   </si>
   <si>
     <t>80483</t>
@@ -1903,7 +1903,7 @@
     <t>0.1795</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.008*"needs" + 0.008*"well" + 0.008*"good" + 0.007*"quality" + 0.006*"effective" + 0.006*"practice" + 0.005*"need" + 0.005*"education" + 0.005*"impact"', '0.011*"’" + 0.009*"well" + 0.009*"good" + 0.006*"effective" + 0.006*"needs" + 0.005*"practice" + 0.005*"quality" + 0.005*"impact" + 0.004*"protection" + 0.004*"improved"', '0.009*"’" + 0.007*"effective" + 0.006*"well" + 0.006*"good" + 0.005*"needs" + 0.005*"quality" + 0.005*"education" + 0.004*"risk" + 0.004*"practice" + 0.004*"need"']</t>
+    <t>['0.010*"’" + 0.008*"good" + 0.008*"well" + 0.007*"needs" + 0.006*"quality" + 0.006*"effective" + 0.005*"practice" + 0.005*"impact" + 0.004*"need" + 0.004*"education"', '0.008*"’" + 0.007*"well" + 0.007*"good" + 0.006*"needs" + 0.006*"practice" + 0.005*"effective" + 0.005*"impact" + 0.004*"need" + 0.004*"quality" + 0.004*"protection"', '0.014*"’" + 0.008*"well" + 0.007*"effective" + 0.007*"good" + 0.007*"quality" + 0.006*"needs" + 0.005*"education" + 0.005*"practice" + 0.005*"risk" + 0.005*"need"']</t>
   </si>
   <si>
     <t>80484</t>
@@ -1936,7 +1936,7 @@
     <t>0.2164</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"needs" + 0.006*"Lincolnshire" + 0.006*"well" + 0.004*"family" + 0.004*"plans" + 0.004*"24" + 0.004*"28" + 0.004*"progress" + 0.004*"effective"', '0.026*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"Lincolnshire" + 0.005*"progress" + 0.004*"24" + 0.004*"plans" + 0.004*"offer" + 0.004*"working" + 0.004*"education"', '0.021*"’" + 0.010*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"family" + 0.004*"28" + 0.004*"number" + 0.004*"need"']</t>
+    <t>['0.026*"’" + 0.008*"Lincolnshire" + 0.007*"needs" + 0.006*"well" + 0.005*"need" + 0.005*"plans" + 0.004*"progress" + 0.004*"28" + 0.004*"offer" + 0.004*"family"', '0.021*"’" + 0.007*"needs" + 0.007*"Lincolnshire" + 0.006*"well" + 0.005*"progress" + 0.005*"plans" + 0.004*"24" + 0.004*"family" + 0.004*"2023" + 0.004*"April"', '0.016*"’" + 0.007*"Lincolnshire" + 0.005*"needs" + 0.005*"well" + 0.005*"family" + 0.005*"plans" + 0.004*"number" + 0.004*"24" + 0.004*"working" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80485</t>
@@ -1966,7 +1966,7 @@
     <t>25/05/23</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.007*"always" + 0.007*"needs" + 0.007*"practice" + 0.006*"need" + 0.006*"quality" + 0.005*"protection" + 0.005*"timely" + 0.004*"met" + 0.004*"24"', '0.018*"’" + 0.007*"needs" + 0.006*"quality" + 0.005*"always" + 0.005*"13" + 0.005*"practice" + 0.005*"need" + 0.005*"Liverpool" + 0.005*"PAs" + 0.004*"24"', '0.020*"’" + 0.008*"Liverpool" + 0.008*"needs" + 0.007*"need" + 0.007*"practice" + 0.006*"always" + 0.005*"quality" + 0.005*"timely" + 0.004*"plans" + 0.004*"met"']</t>
+    <t>['0.019*"’" + 0.009*"practice" + 0.006*"needs" + 0.006*"need" + 0.005*"quality" + 0.005*"always" + 0.005*"Liverpool" + 0.005*"timely" + 0.005*"protection" + 0.004*"receive"', '0.023*"’" + 0.008*"needs" + 0.007*"Liverpool" + 0.006*"practice" + 0.006*"always" + 0.006*"need" + 0.006*"quality" + 0.005*"13" + 0.005*"protection" + 0.004*"timely"', '0.014*"’" + 0.008*"always" + 0.007*"need" + 0.007*"needs" + 0.005*"quality" + 0.005*"Liverpool" + 0.005*"protection" + 0.005*"PAs" + 0.005*"practice" + 0.004*"met"']</t>
   </si>
   <si>
     <t>80486</t>
@@ -1999,7 +1999,7 @@
     <t>0.2002</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.006*"needs" + 0.006*"carers" + 0.005*"plans" + 0.005*"good" + 0.005*"practice" + 0.005*"well" + 0.005*"information" + 0.005*"London" + 0.005*"ensure"', '0.024*"’" + 0.011*"needs" + 0.006*"plans" + 0.006*"good" + 0.006*"carers" + 0.005*"well" + 0.005*"progress" + 0.005*"practice" + 0.005*"information" + 0.005*"Dagenham"', '0.021*"’" + 0.006*"needs" + 0.005*"good" + 0.004*"well" + 0.004*"practice" + 0.004*"plans" + 0.004*"impact" + 0.004*"planning" + 0.004*"progress" + 0.004*"e"']</t>
+    <t>['0.028*"’" + 0.009*"needs" + 0.006*"progress" + 0.005*"plans" + 0.005*"good" + 0.005*"practice" + 0.005*"carers" + 0.004*"well" + 0.004*"e" + 0.004*"2023"', '0.021*"’" + 0.008*"needs" + 0.006*"good" + 0.005*"plans" + 0.005*"practice" + 0.005*"health" + 0.005*"10" + 0.005*"e" + 0.004*"London" + 0.004*"carers"', '0.016*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"plans" + 0.006*"information" + 0.006*"good" + 0.006*"carers" + 0.005*"timely" + 0.004*"ensure" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80487</t>
@@ -2038,7 +2038,7 @@
     <t>0.2188</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.012*"good" + 0.011*"well" + 0.009*"needs" + 0.007*"progress" + 0.007*"need" + 0.007*"plans" + 0.006*"clear" + 0.005*"appropriate" + 0.005*"carers"', '0.013*"’" + 0.009*"good" + 0.009*"needs" + 0.009*"need" + 0.006*"ensure" + 0.006*"well" + 0.006*"clear" + 0.006*"plans" + 0.005*"risk" + 0.005*"effective"', '0.013*"’" + 0.009*"needs" + 0.008*"well" + 0.007*"need" + 0.006*"good" + 0.006*"ensure" + 0.006*"progress" + 0.005*"risk" + 0.005*"quality" + 0.005*"plans"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.009*"good" + 0.009*"well" + 0.007*"need" + 0.006*"progress" + 0.006*"clear" + 0.006*"plans" + 0.006*"risk" + 0.005*"receive"', '0.016*"’" + 0.010*"needs" + 0.009*"good" + 0.007*"need" + 0.007*"well" + 0.007*"progress" + 0.006*"ensure" + 0.005*"quality" + 0.005*"plans" + 0.005*"timely"', '0.012*"’" + 0.010*"well" + 0.009*"good" + 0.008*"needs" + 0.008*"need" + 0.006*"plans" + 0.006*"ensure" + 0.005*"progress" + 0.005*"clear" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80488</t>
@@ -2065,7 +2065,7 @@
     <t>0.1906</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.006*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"need" + 0.005*"plans" + 0.005*"Bexley" + 0.004*"practice" + 0.004*"progress" + 0.004*"clear"', '0.019*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"make" + 0.005*"need" + 0.005*"Bexley" + 0.005*"effective" + 0.005*"10" + 0.004*"practice" + 0.004*"plans"', '0.017*"’" + 0.006*"well" + 0.006*"effective" + 0.006*"plans" + 0.006*"need" + 0.005*"Bexley" + 0.005*"needs" + 0.004*"10" + 0.004*"6" + 0.004*"2023"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.005*"needs" + 0.005*"need" + 0.005*"effective" + 0.004*"plans" + 0.004*"including" + 0.004*"6" + 0.004*"practice" + 0.004*"10"', '0.024*"’" + 0.007*"well" + 0.007*"needs" + 0.006*"Bexley" + 0.006*"plans" + 0.006*"need" + 0.006*"effective" + 0.005*"6" + 0.005*"10" + 0.004*"make"', '0.016*"’" + 0.006*"needs" + 0.005*"effective" + 0.005*"need" + 0.005*"Bexley" + 0.004*"well" + 0.004*"plans" + 0.004*"make" + 0.004*"10" + 0.004*"including"']</t>
   </si>
   <si>
     <t>80489</t>
@@ -2095,7 +2095,7 @@
     <t>0.1959</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.008*"well" + 0.008*"leaders" + 0.007*"progress" + 0.005*"plans" + 0.005*"needs" + 0.005*"number" + 0.005*"quality" + 0.004*"family" + 0.004*"range"', '0.020*"’" + 0.009*"well" + 0.007*"plans" + 0.007*"Brent" + 0.006*"progress" + 0.006*"leaders" + 0.006*"good" + 0.006*"practice" + 0.006*"senior" + 0.006*"quality"', '0.014*"’" + 0.008*"well" + 0.007*"leaders" + 0.006*"good" + 0.006*"plans" + 0.005*"progress" + 0.005*"Brent" + 0.005*"small" + 0.005*"However" + 0.005*"number"']</t>
+    <t>['0.018*"’" + 0.008*"well" + 0.007*"number" + 0.007*"good" + 0.006*"plans" + 0.006*"progress" + 0.006*"quality" + 0.006*"leaders" + 0.005*"small" + 0.005*"practice"', '0.015*"’" + 0.011*"well" + 0.008*"leaders" + 0.007*"plans" + 0.006*"Brent" + 0.006*"progress" + 0.005*"timely" + 0.005*"good" + 0.005*"quality" + 0.005*"practice"', '0.019*"’" + 0.008*"leaders" + 0.007*"progress" + 0.007*"well" + 0.006*"senior" + 0.006*"plans" + 0.005*"quality" + 0.005*"needs" + 0.005*"Brent" + 0.005*"information"']</t>
   </si>
   <si>
     <t>80490</t>
@@ -2131,7 +2131,7 @@
     <t>0.1797</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"Bromley" + 0.006*"needs" + 0.005*"well" + 0.004*"health" + 0.004*"plans" + 0.004*"17" + 0.004*"leaders" + 0.004*"practice" + 0.004*"YPAs"', '0.025*"’" + 0.010*"Bromley" + 0.007*"needs" + 0.007*"plans" + 0.006*"well" + 0.006*"practice" + 0.006*"leaders" + 0.005*"education" + 0.004*"13" + 0.004*"strong"', '0.018*"’" + 0.009*"Bromley" + 0.008*"well" + 0.006*"needs" + 0.005*"leaders" + 0.005*"health" + 0.004*"practice" + 0.004*"education" + 0.004*"helping" + 0.004*"progress"']</t>
+    <t>['0.018*"’" + 0.009*"Bromley" + 0.007*"plans" + 0.006*"well" + 0.005*"leaders" + 0.005*"needs" + 0.005*"health" + 0.005*"practice" + 0.004*"education" + 0.004*"strong"', '0.014*"’" + 0.009*"Bromley" + 0.007*"needs" + 0.006*"well" + 0.005*"leaders" + 0.004*"progress" + 0.004*"plans" + 0.004*"November" + 0.004*"education" + 0.004*"practice"', '0.025*"’" + 0.009*"Bromley" + 0.008*"needs" + 0.008*"well" + 0.006*"practice" + 0.005*"plans" + 0.005*"leaders" + 0.005*"education" + 0.004*"17" + 0.004*"health"']</t>
   </si>
   <si>
     <t>80491</t>
@@ -2164,7 +2164,7 @@
     <t>0.1894</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"practice" + 0.006*"Camden" + 0.006*"leaders" + 0.006*"needs" + 0.005*"appropriate" + 0.005*"25" + 0.005*"progress" + 0.005*"well" + 0.004*"meetings"', '0.010*"’" + 0.008*"Camden" + 0.006*"well" + 0.005*"leaders" + 0.005*"practice" + 0.005*"protection" + 0.004*"needs" + 0.004*"29" + 0.004*"progress" + 0.004*"25"', '0.012*"’" + 0.007*"leaders" + 0.006*"Camden" + 0.006*"response" + 0.006*"practice" + 0.005*"protection" + 0.005*"well" + 0.004*"2022" + 0.004*"29" + 0.004*"needs"']</t>
+    <t>['0.013*"’" + 0.006*"leaders" + 0.006*"Camden" + 0.006*"practice" + 0.005*"appropriate" + 0.005*"progress" + 0.005*"response" + 0.005*"well" + 0.004*"25" + 0.004*"2022"', '0.010*"’" + 0.008*"Camden" + 0.007*"leaders" + 0.006*"practice" + 0.006*"protection" + 0.006*"needs" + 0.005*"well" + 0.004*"29" + 0.004*"25" + 0.004*"response"', '0.010*"’" + 0.007*"Camden" + 0.006*"well" + 0.006*"leaders" + 0.006*"practice" + 0.005*"protection" + 0.004*"response" + 0.004*"needs" + 0.004*"29" + 0.004*"meetings"']</t>
   </si>
   <si>
     <t>80492</t>
@@ -2197,7 +2197,7 @@
     <t>16/03/20</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.006*"well" + 0.005*"quality" + 0.005*"need" + 0.005*"experiences" + 0.005*"Croydon" + 0.005*"effective" + 0.005*"risk" + 0.004*"improved"', '0.007*"’" + 0.006*"need" + 0.006*"needs" + 0.006*"Senior" + 0.006*"well" + 0.005*"ensure" + 0.005*"risk" + 0.005*"Croydon" + 0.004*"health" + 0.004*"improved"', '0.012*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"Croydon" + 0.006*"good" + 0.006*"education" + 0.006*"Senior" + 0.006*"quality" + 0.006*"ensure" + 0.006*"plans"']</t>
+    <t>['0.012*"’" + 0.008*"needs" + 0.006*"effective" + 0.006*"well" + 0.006*"Senior" + 0.006*"need" + 0.005*"quality" + 0.005*"Croydon" + 0.005*"improved" + 0.005*"plans"', '0.012*"’" + 0.008*"well" + 0.007*"Croydon" + 0.007*"needs" + 0.006*"ensure" + 0.006*"quality" + 0.006*"health" + 0.006*"good" + 0.006*"Senior" + 0.005*"need"', '0.011*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.004*"need" + 0.004*"Croydon" + 0.004*"improved" + 0.004*"good" + 0.004*"education" + 0.004*"Senior"']</t>
   </si>
   <si>
     <t>80493</t>
@@ -2233,7 +2233,7 @@
     <t>0.1711</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.010*"quality" + 0.006*"needs" + 0.006*"good" + 0.005*"experiences" + 0.005*"progress" + 0.004*"leaders" + 0.004*"risk" + 0.004*"well" + 0.004*"plans"', '0.013*"’" + 0.010*"quality" + 0.006*"good" + 0.006*"needs" + 0.005*"risk" + 0.005*"plans" + 0.004*"well" + 0.004*"management" + 0.004*"progress" + 0.004*"fully"', '0.009*"’" + 0.008*"quality" + 0.008*"needs" + 0.007*"good" + 0.006*"progress" + 0.005*"plans" + 0.004*"Ealing" + 0.004*"experiences" + 0.004*"provide" + 0.004*"family"']</t>
+    <t>['0.014*"’" + 0.008*"good" + 0.008*"quality" + 0.006*"needs" + 0.006*"plans" + 0.005*"risk" + 0.005*"progress" + 0.005*"well" + 0.005*"always" + 0.005*"fully"', '0.013*"quality" + 0.011*"’" + 0.010*"needs" + 0.006*"good" + 0.006*"progress" + 0.005*"experiences" + 0.005*"oversight" + 0.005*"Ealing" + 0.004*"management" + 0.004*"improve"', '0.007*"quality" + 0.006*"’" + 0.005*"plans" + 0.005*"risk" + 0.004*"management" + 0.004*"needs" + 0.004*"improve" + 0.004*"good" + 0.003*"Ealing" + 0.003*"family"']</t>
   </si>
   <si>
     <t>80494</t>
@@ -2266,7 +2266,7 @@
     <t>0.2022</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"effective" + 0.008*"practice" + 0.008*"ensure" + 0.007*"good" + 0.007*"needs" + 0.007*"clear" + 0.006*"timely" + 0.006*"range" + 0.006*"leaders"', '0.014*"’" + 0.010*"needs" + 0.008*"good" + 0.007*"Enfield" + 0.007*"ensure" + 0.006*"quality" + 0.006*"leaders" + 0.006*"practice" + 0.006*"effective" + 0.006*"timely"', '0.014*"’" + 0.008*"needs" + 0.008*"practice" + 0.007*"ensure" + 0.007*"Enfield" + 0.006*"good" + 0.006*"clear" + 0.006*"quality" + 0.006*"improve" + 0.005*"effective"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.008*"clear" + 0.008*"practice" + 0.008*"effective" + 0.008*"good" + 0.007*"ensure" + 0.007*"Enfield" + 0.007*"quality" + 0.006*"timely"', '0.013*"’" + 0.008*"practice" + 0.007*"needs" + 0.007*"good" + 0.007*"effective" + 0.007*"ensure" + 0.005*"clear" + 0.005*"leaders" + 0.005*"progress" + 0.005*"need"', '0.012*"’" + 0.008*"ensure" + 0.007*"needs" + 0.007*"practice" + 0.006*"good" + 0.006*"Enfield" + 0.006*"timely" + 0.005*"quality" + 0.005*"leaders" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80495</t>
@@ -2299,7 +2299,7 @@
     <t>0.2109</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"good" + 0.007*"range" + 0.006*"plans" + 0.005*"risk" + 0.005*"ensure" + 0.005*"need" + 0.005*"timely"', '0.012*"well" + 0.011*"’" + 0.008*"plans" + 0.008*"needs" + 0.008*"need" + 0.007*"good" + 0.005*"progress" + 0.005*"range" + 0.005*"quality" + 0.005*"ensure"', '0.012*"’" + 0.009*"good" + 0.008*"well" + 0.008*"plans" + 0.006*"needs" + 0.005*"range" + 0.005*"progress" + 0.005*"information" + 0.005*"need" + 0.005*"consistently"']</t>
+    <t>['0.008*"good" + 0.008*"’" + 0.007*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"quality" + 0.005*"ensure" + 0.004*"range" + 0.004*"information"', '0.011*"’" + 0.009*"well" + 0.006*"plans" + 0.006*"range" + 0.006*"need" + 0.006*"needs" + 0.005*"good" + 0.005*"ensure" + 0.005*"risk" + 0.005*"progress"', '0.015*"’" + 0.011*"well" + 0.009*"needs" + 0.009*"good" + 0.009*"plans" + 0.007*"need" + 0.006*"range" + 0.006*"progress" + 0.005*"risks" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80496</t>
@@ -2338,7 +2338,7 @@
     <t>0.1417</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"practice" + 0.007*"number" + 0.007*"need" + 0.007*"effective" + 0.006*"quality" + 0.006*"protection" + 0.006*"needs" + 0.006*"including" + 0.005*"within"', '0.013*"’" + 0.008*"practice" + 0.006*"However" + 0.005*"planning" + 0.005*"plans" + 0.005*"effective" + 0.005*"within" + 0.005*"leaders" + 0.005*"small" + 0.005*"progress"', '0.014*"’" + 0.012*"practice" + 0.007*"planning" + 0.007*"number" + 0.006*"plans" + 0.006*"needs" + 0.006*"within" + 0.005*"making" + 0.005*"including" + 0.005*"However"']</t>
+    <t>['0.014*"’" + 0.010*"practice" + 0.007*"number" + 0.006*"effective" + 0.006*"planning" + 0.006*"leaders" + 0.006*"However" + 0.006*"small" + 0.005*"within" + 0.005*"plans"', '0.015*"’" + 0.011*"practice" + 0.006*"effective" + 0.006*"oversight" + 0.006*"plans" + 0.006*"needs" + 0.006*"including" + 0.006*"quality" + 0.005*"planning" + 0.005*"number"', '0.010*"’" + 0.008*"practice" + 0.007*"planning" + 0.006*"number" + 0.006*"within" + 0.005*"needs" + 0.005*"including" + 0.005*"However" + 0.005*"quality" + 0.005*"making"']</t>
   </si>
   <si>
     <t>80497</t>
@@ -2371,7 +2371,7 @@
     <t>0.1986</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.008*"well" + 0.005*"receive" + 0.005*"needs" + 0.005*"Fulham" + 0.004*"Leaders" + 0.004*"effective" + 0.004*"plans" + 0.004*"15" + 0.004*"11"', '0.016*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"Hammersmith" + 0.005*"2024" + 0.005*"receive" + 0.005*"supported" + 0.004*"plans" + 0.004*"leaders" + 0.004*"practice"', '0.013*"’" + 0.007*"receive" + 0.006*"well" + 0.004*"Fulham" + 0.004*"leaders" + 0.004*"needs" + 0.004*"place" + 0.004*"plans" + 0.004*"effective" + 0.004*"11"']</t>
+    <t>['0.017*"’" + 0.007*"well" + 0.004*"needs" + 0.004*"protection" + 0.004*"Hammersmith" + 0.004*"effective" + 0.004*"Fulham" + 0.004*"2024" + 0.004*"March" + 0.004*"11"', '0.013*"’" + 0.007*"well" + 0.006*"receive" + 0.005*"leaders" + 0.005*"Hammersmith" + 0.004*"supported" + 0.004*"needs" + 0.004*"effective" + 0.004*"11" + 0.004*"15"', '0.015*"’" + 0.008*"well" + 0.007*"receive" + 0.007*"needs" + 0.006*"plans" + 0.005*"Fulham" + 0.005*"practice" + 0.005*"Leaders" + 0.005*"understand" + 0.004*"2024"']</t>
   </si>
   <si>
     <t>80498</t>
@@ -2395,7 +2395,7 @@
     <t>13/02/2023</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.007*"plans" + 0.006*"Haringey" + 0.005*"needs" + 0.005*"well" + 0.005*"progress" + 0.004*"good" + 0.004*"need" + 0.004*"13" + 0.004*"2023"', '0.019*"’" + 0.010*"needs" + 0.008*"Haringey" + 0.007*"good" + 0.006*"plans" + 0.006*"well" + 0.005*"impact" + 0.005*"progress" + 0.005*"risk" + 0.005*"education"', '0.014*"’" + 0.011*"Haringey" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"need" + 0.005*"supported" + 0.004*"progress" + 0.004*"February" + 0.004*"good"']</t>
+    <t>['0.015*"’" + 0.010*"needs" + 0.007*"Haringey" + 0.006*"well" + 0.006*"good" + 0.005*"progress" + 0.005*"plans" + 0.004*"impact" + 0.004*"supported" + 0.004*"need"', '0.015*"’" + 0.008*"Haringey" + 0.006*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"need" + 0.004*"progress" + 0.004*"13" + 0.004*"good" + 0.004*"education"', '0.016*"’" + 0.009*"Haringey" + 0.009*"plans" + 0.007*"needs" + 0.006*"need" + 0.005*"good" + 0.005*"well" + 0.005*"24" + 0.005*"education" + 0.004*"risk"']</t>
   </si>
   <si>
     <t>80499</t>
@@ -2428,7 +2428,7 @@
     <t>0.2023</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.008*"well" + 0.008*"good" + 0.005*"needs" + 0.005*"impact" + 0.005*"plans" + 0.005*"practice" + 0.004*"planning" + 0.004*"experiences" + 0.004*"early"', '0.013*"’" + 0.010*"good" + 0.009*"well" + 0.009*"needs" + 0.006*"need" + 0.006*"practice" + 0.005*"early" + 0.005*"plans" + 0.005*"impact" + 0.005*"protection"', '0.013*"good" + 0.012*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"protection" + 0.006*"impact" + 0.006*"experiences" + 0.006*"plans" + 0.005*"Harrow" + 0.005*"need"']</t>
+    <t>['0.012*"’" + 0.010*"good" + 0.009*"well" + 0.009*"needs" + 0.005*"school" + 0.005*"early" + 0.005*"need" + 0.005*"experiences" + 0.004*"protection" + 0.004*"plans"', '0.010*"’" + 0.010*"good" + 0.009*"well" + 0.007*"needs" + 0.005*"impact" + 0.005*"need" + 0.005*"plans" + 0.005*"protection" + 0.005*"early" + 0.005*"experiences"', '0.012*"’" + 0.012*"good" + 0.008*"needs" + 0.007*"well" + 0.007*"impact" + 0.006*"practice" + 0.006*"plans" + 0.005*"protection" + 0.004*"need" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80500</t>
@@ -2455,7 +2455,7 @@
     <t>16/02/24</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.011*"Havering" + 0.009*"quality" + 0.007*"plans" + 0.006*"oversight" + 0.006*"effective" + 0.005*"22" + 0.005*"11" + 0.005*"needs" + 0.004*"December"', '0.020*"’" + 0.011*"Havering" + 0.009*"quality" + 0.008*"plans" + 0.005*"effective" + 0.005*"oversight" + 0.005*"11" + 0.004*"well" + 0.004*"22" + 0.004*"needs"', '0.012*"’" + 0.011*"Havering" + 0.008*"quality" + 0.006*"plans" + 0.005*"needs" + 0.005*"effective" + 0.005*"oversight" + 0.004*"practice" + 0.003*"many" + 0.003*"progress"']</t>
+    <t>['0.016*"’" + 0.013*"Havering" + 0.008*"quality" + 0.006*"plans" + 0.005*"oversight" + 0.004*"needs" + 0.004*"effective" + 0.004*"11" + 0.004*"many" + 0.004*"progress"', '0.020*"’" + 0.010*"quality" + 0.009*"Havering" + 0.008*"plans" + 0.005*"oversight" + 0.005*"effective" + 0.005*"needs" + 0.005*"11" + 0.005*"22" + 0.004*"practice"', '0.016*"’" + 0.011*"Havering" + 0.008*"quality" + 0.006*"plans" + 0.006*"effective" + 0.005*"oversight" + 0.004*"needs" + 0.004*"2023" + 0.004*"well" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80501</t>
@@ -2488,7 +2488,7 @@
     <t>0.2119</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"Hillingdon" + 0.008*"plans" + 0.008*"needs" + 0.007*"well" + 0.004*"team" + 0.004*"need" + 0.004*"senior" + 0.004*"leaders" + 0.004*"supported"', '0.021*"’" + 0.012*"needs" + 0.008*"plans" + 0.008*"Hillingdon" + 0.007*"well" + 0.005*"2" + 0.005*"6" + 0.005*"family" + 0.004*"need" + 0.004*"team"', '0.018*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"Hillingdon" + 0.006*"plans" + 0.005*"team" + 0.005*"need" + 0.004*"6" + 0.004*"carers" + 0.004*"understand"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.008*"plans" + 0.007*"Hillingdon" + 0.007*"well" + 0.004*"need" + 0.004*"6" + 0.004*"supported" + 0.004*"team" + 0.003*"practice"', '0.022*"’" + 0.010*"needs" + 0.008*"plans" + 0.008*"well" + 0.008*"Hillingdon" + 0.005*"team" + 0.004*"need" + 0.004*"2023" + 0.004*"2" + 0.004*"leaders"', '0.015*"’" + 0.009*"needs" + 0.008*"Hillingdon" + 0.007*"well" + 0.006*"plans" + 0.005*"team" + 0.004*"2" + 0.004*"need" + 0.004*"6" + 0.004*"leaders"']</t>
   </si>
   <si>
     <t>80503</t>
@@ -2521,7 +2521,7 @@
     <t>0.1948</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"well" + 0.006*"effective" + 0.006*"needs" + 0.005*"Hounslow" + 0.005*"oversight" + 0.005*"timely" + 0.005*"plans" + 0.004*"strong" + 0.004*"education"', '0.022*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"Hounslow" + 0.005*"effective" + 0.005*"timely" + 0.004*"20" + 0.004*"16" + 0.004*"oversight" + 0.004*"supported"', '0.020*"’" + 0.014*"needs" + 0.013*"well" + 0.009*"effective" + 0.008*"Hounslow" + 0.007*"timely" + 0.007*"plans" + 0.005*"experiences" + 0.005*"strong" + 0.005*"progress"']</t>
+    <t>['0.010*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"plans" + 0.004*"16" + 0.004*"timely" + 0.004*"Hounslow" + 0.003*"strong" + 0.003*"progress"', '0.025*"’" + 0.013*"needs" + 0.012*"well" + 0.009*"Hounslow" + 0.009*"effective" + 0.007*"timely" + 0.005*"oversight" + 0.005*"plans" + 0.005*"education" + 0.005*"16"', '0.018*"’" + 0.009*"needs" + 0.008*"well" + 0.006*"plans" + 0.006*"effective" + 0.005*"timely" + 0.005*"strong" + 0.005*"Hounslow" + 0.004*"experiences" + 0.004*"training"']</t>
   </si>
   <si>
     <t>80505</t>
@@ -2551,7 +2551,7 @@
     <t>0.209</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.012*"well" + 0.011*"needs" + 0.006*"highly" + 0.006*"plans" + 0.006*"good" + 0.006*"practice" + 0.005*"quality" + 0.005*"leaders" + 0.004*"effective"', '0.013*"needs" + 0.013*"’" + 0.009*"well" + 0.007*"plans" + 0.006*"highly" + 0.006*"good" + 0.006*"quality" + 0.006*"effective" + 0.005*"Islington" + 0.005*"risk"', '0.013*"’" + 0.010*"well" + 0.008*"needs" + 0.006*"plans" + 0.006*"leaders" + 0.005*"good" + 0.005*"quality" + 0.005*"effective" + 0.005*"Islington" + 0.005*"highly"']</t>
+    <t>['0.013*"’" + 0.012*"well" + 0.011*"needs" + 0.008*"plans" + 0.007*"quality" + 0.006*"highly" + 0.006*"good" + 0.006*"effective" + 0.006*"leaders" + 0.005*"practice"', '0.014*"’" + 0.011*"needs" + 0.009*"well" + 0.006*"highly" + 0.005*"plans" + 0.005*"good" + 0.005*"effective" + 0.005*"quality" + 0.005*"risk" + 0.004*"leaders"', '0.011*"needs" + 0.010*"’" + 0.010*"well" + 0.006*"good" + 0.006*"plans" + 0.005*"leaders" + 0.005*"Islington" + 0.005*"highly" + 0.005*"quality" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80506</t>
@@ -2587,7 +2587,7 @@
     <t>0.1718</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"well" + 0.010*"needs" + 0.008*"plans" + 0.007*"good" + 0.007*"Lambeth" + 0.006*"progress" + 0.006*"need" + 0.006*"impact" + 0.006*"4"', '0.013*"’" + 0.008*"needs" + 0.007*"Lambeth" + 0.007*"plans" + 0.006*"good" + 0.006*"well" + 0.005*"leaders" + 0.005*"impact" + 0.005*"need" + 0.004*"Leaders"', '0.014*"’" + 0.007*"needs" + 0.007*"plans" + 0.006*"good" + 0.006*"well" + 0.006*"progress" + 0.006*"leaders" + 0.005*"2022" + 0.005*"need" + 0.005*"information"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"need" + 0.007*"good" + 0.007*"Lambeth" + 0.006*"plans" + 0.006*"leaders" + 0.005*"progress" + 0.005*"impact"', '0.016*"’" + 0.009*"needs" + 0.008*"plans" + 0.007*"well" + 0.007*"good" + 0.006*"progress" + 0.006*"Lambeth" + 0.005*"need" + 0.005*"arrangements" + 0.005*"impact"', '0.018*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"plans" + 0.006*"good" + 0.006*"impact" + 0.006*"Lambeth" + 0.005*"progress" + 0.005*"4" + 0.005*"carers"']</t>
   </si>
   <si>
     <t>80508</t>
@@ -2623,7 +2623,7 @@
     <t>0.1803</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"well" + 0.009*"needs" + 0.007*"plans" + 0.006*"Lewisham" + 0.006*"effective" + 0.005*"leaders" + 0.005*"good" + 0.005*"4" + 0.005*"15"', '0.016*"’" + 0.007*"plans" + 0.007*"well" + 0.006*"needs" + 0.005*"effective" + 0.005*"leaders" + 0.005*"arrangements" + 0.005*"progress" + 0.004*"good" + 0.004*"Lewisham"', '0.016*"’" + 0.008*"well" + 0.007*"effective" + 0.007*"Lewisham" + 0.006*"needs" + 0.005*"progress" + 0.005*"plans" + 0.005*"4" + 0.004*"supported" + 0.004*"appropriate"']</t>
+    <t>['0.018*"’" + 0.008*"needs" + 0.006*"progress" + 0.006*"well" + 0.005*"4" + 0.005*"effective" + 0.005*"plans" + 0.005*"Lewisham" + 0.005*"good" + 0.004*"receive"', '0.019*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"plans" + 0.007*"effective" + 0.006*"Lewisham" + 0.005*"arrangements" + 0.005*"need" + 0.005*"15" + 0.005*"good"', '0.013*"’" + 0.008*"well" + 0.007*"plans" + 0.006*"Lewisham" + 0.005*"needs" + 0.005*"effective" + 0.005*"leaders" + 0.005*"4" + 0.004*"2023" + 0.004*"progress"']</t>
   </si>
   <si>
     <t>80510</t>
@@ -2647,7 +2647,7 @@
     <t>0.1982</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"Merton" + 0.006*"needs" + 0.005*"family" + 0.005*"plans" + 0.005*"2022" + 0.005*"progress" + 0.004*"28" + 0.004*"ensure"', '0.020*"’" + 0.009*"well" + 0.006*"Merton" + 0.006*"needs" + 0.005*"plans" + 0.004*"good" + 0.004*"risk" + 0.004*"progress" + 0.004*"ensure" + 0.004*"family"', '0.013*"’" + 0.008*"well" + 0.006*"Merton" + 0.005*"needs" + 0.004*"across" + 0.004*"progress" + 0.004*"good" + 0.004*"plans" + 0.004*"helping" + 0.004*"effective"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"Merton" + 0.005*"plans" + 0.004*"4" + 0.004*"progress" + 0.004*"helping" + 0.004*"2022" + 0.004*"ensure"', '0.018*"’" + 0.008*"well" + 0.008*"Merton" + 0.005*"good" + 0.005*"family" + 0.005*"needs" + 0.005*"ensure" + 0.004*"progress" + 0.004*"health" + 0.004*"information"', '0.012*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"plans" + 0.004*"Merton" + 0.004*"education" + 0.004*"across" + 0.004*"family" + 0.004*"leaders" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80511</t>
@@ -2671,7 +2671,7 @@
     <t>0.1861</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.009*"needs" + 0.008*"Newham" + 0.006*"practice" + 0.006*"plans" + 0.006*"effective" + 0.006*"need" + 0.005*"progress" + 0.005*"good" + 0.005*"receive"', '0.016*"’" + 0.008*"needs" + 0.006*"progress" + 0.006*"need" + 0.006*"Newham" + 0.006*"effective" + 0.005*"practice" + 0.005*"plans" + 0.005*"good" + 0.004*"early"', '0.018*"’" + 0.007*"needs" + 0.007*"plans" + 0.007*"Newham" + 0.007*"progress" + 0.006*"practice" + 0.006*"effective" + 0.005*"need" + 0.005*"good" + 0.005*"18"']</t>
+    <t>['0.014*"’" + 0.006*"needs" + 0.006*"need" + 0.006*"practice" + 0.005*"Newham" + 0.005*"effective" + 0.004*"risks" + 0.004*"progress" + 0.004*"planning" + 0.004*"plans"', '0.020*"’" + 0.010*"needs" + 0.007*"effective" + 0.007*"progress" + 0.007*"Newham" + 0.006*"plans" + 0.006*"good" + 0.006*"Leaders" + 0.006*"need" + 0.005*"practice"', '0.021*"’" + 0.008*"Newham" + 0.007*"practice" + 0.007*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"need" + 0.005*"good" + 0.005*"effective" + 0.004*"18"']</t>
   </si>
   <si>
     <t>80512</t>
@@ -2701,7 +2701,7 @@
     <t>0.2269</t>
   </si>
   <si>
-    <t>['0.008*"well" + 0.007*"’" + 0.006*"effective" + 0.006*"practice" + 0.005*"needs" + 0.005*"good" + 0.005*"risk" + 0.005*"protection" + 0.005*"Redbridge" + 0.005*"need"', '0.009*"’" + 0.008*"practice" + 0.006*"needs" + 0.006*"need" + 0.006*"including" + 0.006*"Redbridge" + 0.005*"well" + 0.005*"strong" + 0.004*"effective" + 0.004*"ensure"', '0.007*"’" + 0.006*"practice" + 0.006*"needs" + 0.006*"need" + 0.006*"strong" + 0.005*"risk" + 0.005*"well" + 0.005*"Redbridge" + 0.004*"effective" + 0.004*"including"']</t>
+    <t>['0.006*"needs" + 0.006*"well" + 0.006*"’" + 0.005*"Redbridge" + 0.005*"effective" + 0.005*"strong" + 0.005*"practice" + 0.005*"team" + 0.004*"need" + 0.004*"ensure"', '0.007*"’" + 0.006*"well" + 0.005*"strong" + 0.005*"practice" + 0.005*"effective" + 0.005*"need" + 0.004*"risk" + 0.004*"including" + 0.004*"good" + 0.004*"Redbridge"', '0.009*"’" + 0.009*"practice" + 0.007*"needs" + 0.007*"need" + 0.007*"well" + 0.005*"risk" + 0.005*"Redbridge" + 0.005*"effective" + 0.005*"strong" + 0.005*"including"']</t>
   </si>
   <si>
     <t>80513</t>
@@ -2728,7 +2728,7 @@
     <t>0.2056</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.013*"well" + 0.007*"needs" + 0.006*"team" + 0.006*"supported" + 0.006*"Richmond" + 0.005*"need" + 0.005*"good" + 0.005*"additional" + 0.004*"4"', '0.018*"’" + 0.010*"Richmond" + 0.008*"well" + 0.007*"needs" + 0.006*"supported" + 0.006*"good" + 0.005*"need" + 0.005*"team" + 0.005*"additional" + 0.005*"ensure"', '0.013*"’" + 0.011*"well" + 0.008*"Richmond" + 0.007*"needs" + 0.006*"need" + 0.006*"supported" + 0.006*"good" + 0.006*"Thames" + 0.005*"team" + 0.005*"strong"']</t>
+    <t>['0.015*"’" + 0.007*"Richmond" + 0.007*"needs" + 0.006*"supported" + 0.006*"well" + 0.005*"need" + 0.004*"good" + 0.004*"team" + 0.004*"strong" + 0.004*"January"', '0.015*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"Richmond" + 0.007*"team" + 0.005*"supported" + 0.005*"good" + 0.005*"ensure" + 0.005*"need" + 0.005*"4"', '0.016*"’" + 0.015*"well" + 0.009*"Richmond" + 0.008*"needs" + 0.006*"good" + 0.006*"need" + 0.006*"supported" + 0.005*"protection" + 0.005*"team" + 0.005*"2022"']</t>
   </si>
   <si>
     <t>80514</t>
@@ -2758,7 +2758,7 @@
     <t>11/11/22</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"Southwark" + 0.007*"well" + 0.007*"good" + 0.005*"needs" + 0.005*"progress" + 0.005*"Leaders" + 0.005*"strong" + 0.005*"ensure" + 0.004*"risks"', '0.022*"’" + 0.010*"Southwark" + 0.009*"good" + 0.009*"well" + 0.008*"needs" + 0.007*"plans" + 0.006*"progress" + 0.006*"need" + 0.006*"effective" + 0.005*"leaders"', '0.016*"’" + 0.009*"Southwark" + 0.007*"needs" + 0.006*"good" + 0.006*"progress" + 0.005*"well" + 0.005*"need" + 0.005*"Leaders" + 0.005*"strong" + 0.005*"effective"']</t>
+    <t>['0.022*"’" + 0.009*"Southwark" + 0.008*"well" + 0.008*"good" + 0.007*"need" + 0.007*"needs" + 0.006*"Leaders" + 0.006*"progress" + 0.006*"strong" + 0.006*"effective"', '0.014*"’" + 0.009*"good" + 0.008*"needs" + 0.008*"Southwark" + 0.007*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"leaders" + 0.005*"practice" + 0.005*"effective"', '0.017*"’" + 0.011*"Southwark" + 0.007*"well" + 0.007*"needs" + 0.006*"good" + 0.006*"plans" + 0.006*"progress" + 0.005*"receive" + 0.005*"quality" + 0.005*"2022"']</t>
   </si>
   <si>
     <t>80515</t>
@@ -2788,7 +2788,7 @@
     <t>0.2064</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.006*"well" + 0.006*"Sutton" + 0.005*"needs" + 0.004*"effective" + 0.004*"receive" + 0.004*"progress" + 0.003*"6" + 0.003*"supported" + 0.003*"leaders"', '0.014*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"progress" + 0.005*"Sutton" + 0.005*"receive" + 0.004*"good" + 0.004*"effective" + 0.004*"leaders" + 0.004*"6"', '0.020*"’" + 0.006*"well" + 0.006*"Sutton" + 0.006*"good" + 0.006*"progress" + 0.006*"needs" + 0.005*"effective" + 0.005*"6" + 0.005*"supported" + 0.005*"‘"']</t>
+    <t>['0.016*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"receive" + 0.005*"Sutton" + 0.005*"leaders" + 0.004*"progress" + 0.004*"good" + 0.004*"need" + 0.004*"supported"', '0.016*"’" + 0.005*"progress" + 0.005*"Sutton" + 0.005*"needs" + 0.005*"good" + 0.005*"receive" + 0.005*"well" + 0.004*"6" + 0.004*"effective" + 0.004*"10"', '0.018*"’" + 0.008*"well" + 0.007*"Sutton" + 0.006*"needs" + 0.006*"effective" + 0.005*"progress" + 0.005*"December" + 0.005*"good" + 0.005*"6" + 0.004*"receive"']</t>
   </si>
   <si>
     <t>80516</t>
@@ -2818,7 +2818,7 @@
     <t>0.2155</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"good" + 0.007*"plans" + 0.006*"need" + 0.006*"effective" + 0.006*"‘" + 0.006*"practice" + 0.006*"well" + 0.005*"early" + 0.005*"risk"', '0.015*"’" + 0.006*"effective" + 0.006*"well" + 0.006*"plans" + 0.006*"good" + 0.006*"‘" + 0.005*"early" + 0.005*"needs" + 0.005*"including" + 0.005*"progress"', '0.011*"’" + 0.006*"good" + 0.005*"practice" + 0.005*"plans" + 0.005*"effective" + 0.004*"progress" + 0.004*"‘" + 0.004*"well" + 0.004*"need" + 0.004*"early"']</t>
+    <t>['0.014*"’" + 0.006*"early" + 0.006*"plans" + 0.006*"practice" + 0.006*"good" + 0.005*"needs" + 0.005*"well" + 0.005*"effective" + 0.005*"‘" + 0.005*"need"', '0.013*"’" + 0.006*"plans" + 0.006*"effective" + 0.006*"‘" + 0.005*"need" + 0.005*"well" + 0.005*"risk" + 0.005*"practice" + 0.005*"progress" + 0.005*"good"', '0.017*"’" + 0.009*"good" + 0.007*"effective" + 0.006*"plans" + 0.006*"well" + 0.006*"‘" + 0.005*"practice" + 0.005*"need" + 0.005*"progress" + 0.005*"early"']</t>
   </si>
   <si>
     <t>80517</t>
@@ -2851,7 +2851,7 @@
     <t>0.2179</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.012*"well" + 0.011*"needs" + 0.009*"effective" + 0.008*"good" + 0.006*"need" + 0.005*"plans" + 0.005*"timely" + 0.005*"risk" + 0.004*"appropriately"', '0.007*"’" + 0.006*"well" + 0.006*"good" + 0.006*"effective" + 0.005*"needs" + 0.005*"plans" + 0.004*"need" + 0.003*"clear" + 0.003*"education" + 0.003*"protection"', '0.017*"’" + 0.014*"well" + 0.009*"good" + 0.008*"needs" + 0.006*"need" + 0.006*"effective" + 0.005*"plans" + 0.005*"timely" + 0.005*"actions" + 0.005*"risk"']</t>
+    <t>['0.012*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"good" + 0.006*"effective" + 0.006*"need" + 0.005*"plans" + 0.005*"timely" + 0.004*"ensure" + 0.004*"risk"', '0.018*"’" + 0.013*"well" + 0.009*"needs" + 0.009*"good" + 0.007*"effective" + 0.006*"need" + 0.005*"protection" + 0.005*"timely" + 0.005*"plans" + 0.004*"risk"', '0.012*"well" + 0.012*"’" + 0.008*"needs" + 0.008*"good" + 0.008*"effective" + 0.006*"need" + 0.006*"plans" + 0.005*"clear" + 0.004*"risk" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80518</t>
@@ -2878,7 +2878,7 @@
     <t>18/11/2022</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"well" + 0.007*"protection" + 0.006*"needs" + 0.006*"practice" + 0.005*"Wandsworth" + 0.005*"progress" + 0.005*"Senior" + 0.005*"receive" + 0.005*"ensure"', '0.010*"’" + 0.005*"well" + 0.005*"Senior" + 0.004*"supported" + 0.004*"effective" + 0.004*"good" + 0.004*"needs" + 0.004*"ensure" + 0.004*"7" + 0.004*"Wandsworth"', '0.011*"’" + 0.007*"progress" + 0.007*"well" + 0.005*"Wandsworth" + 0.005*"effective" + 0.005*"7" + 0.005*"supported" + 0.005*"quality" + 0.005*"needs" + 0.005*"practice"']</t>
+    <t>['0.012*"’" + 0.007*"well" + 0.006*"protection" + 0.005*"progress" + 0.005*"quality" + 0.005*"ensure" + 0.005*"7" + 0.005*"Senior" + 0.005*"receive" + 0.005*"needs"', '0.013*"’" + 0.006*"practice" + 0.006*"Wandsworth" + 0.006*"well" + 0.005*"progress" + 0.005*"Senior" + 0.005*"effective" + 0.005*"needs" + 0.004*"early" + 0.004*"quality"', '0.010*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"progress" + 0.005*"protection" + 0.005*"supported" + 0.005*"practice" + 0.005*"Senior" + 0.005*"18" + 0.005*"Wandsworth"']</t>
   </si>
   <si>
     <t>80519</t>
@@ -2911,7 +2911,7 @@
     <t>0.181</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.006*"needs" + 0.006*"practice" + 0.005*"well" + 0.004*"highly" + 0.004*"across" + 0.004*"skilled" + 0.003*"shared" + 0.003*"many" + 0.003*"e"', '0.013*"’" + 0.007*"highly" + 0.006*"practice" + 0.006*"needs" + 0.005*"well" + 0.004*"many" + 0.004*"across" + 0.003*"high" + 0.003*"family" + 0.003*"shared"', '0.013*"’" + 0.007*"practice" + 0.006*"needs" + 0.005*"highly" + 0.005*"well" + 0.004*"family" + 0.004*"many" + 0.003*"plans" + 0.003*"direct" + 0.003*"Westminster"']</t>
+    <t>['0.012*"’" + 0.007*"needs" + 0.006*"practice" + 0.005*"highly" + 0.005*"well" + 0.005*"many" + 0.004*"family" + 0.003*"across" + 0.003*"plans" + 0.003*"Westminster"', '0.012*"’" + 0.008*"practice" + 0.006*"well" + 0.006*"needs" + 0.005*"highly" + 0.004*"direct" + 0.004*"family" + 0.004*"skilled" + 0.003*"across" + 0.003*"interventions"', '0.015*"’" + 0.007*"highly" + 0.006*"practice" + 0.005*"needs" + 0.004*"across" + 0.004*"well" + 0.004*"shared" + 0.003*"many" + 0.003*"plans" + 0.003*"high"']</t>
   </si>
   <si>
     <t>80520</t>
@@ -2944,7 +2944,7 @@
     <t>0.2106</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.008*"needs" + 0.007*"Luton" + 0.006*"need" + 0.006*"plans" + 0.006*"good" + 0.005*"progress" + 0.005*"quality" + 0.005*"impact" + 0.005*"receive"', '0.013*"’" + 0.006*"plans" + 0.005*"effective" + 0.005*"needs" + 0.005*"well" + 0.005*"need" + 0.004*"Luton" + 0.004*"impact" + 0.004*"quality" + 0.004*"leaders"', '0.015*"’" + 0.007*"need" + 0.007*"effective" + 0.006*"ensure" + 0.006*"good" + 0.005*"plans" + 0.005*"needs" + 0.005*"Luton" + 0.005*"progress" + 0.005*"impact"']</t>
+    <t>['0.017*"’" + 0.006*"need" + 0.006*"effective" + 0.005*"11" + 0.005*"plans" + 0.005*"receive" + 0.005*"Luton" + 0.005*"progress" + 0.005*"well" + 0.005*"good"', '0.016*"’" + 0.007*"need" + 0.006*"Luton" + 0.006*"needs" + 0.006*"plans" + 0.005*"effective" + 0.004*"22" + 0.004*"provide" + 0.004*"ensure" + 0.004*"good"', '0.018*"’" + 0.007*"needs" + 0.007*"need" + 0.006*"plans" + 0.006*"impact" + 0.006*"good" + 0.005*"Luton" + 0.005*"effective" + 0.005*"progress" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80521</t>
@@ -2971,7 +2971,7 @@
     <t>19/05/22</t>
   </si>
   <si>
-    <t>['0.023*"’" + 0.011*"Manchester" + 0.008*"needs" + 0.007*"well" + 0.007*"supported" + 0.006*"education" + 0.005*"effective" + 0.005*"always" + 0.005*"protection" + 0.005*"family"', '0.015*"’" + 0.010*"Manchester" + 0.008*"needs" + 0.006*"always" + 0.006*"supported" + 0.005*"protection" + 0.005*"well" + 0.005*"plans" + 0.005*"progress" + 0.005*"education"', '0.024*"’" + 0.011*"needs" + 0.010*"Manchester" + 0.007*"well" + 0.007*"always" + 0.007*"plans" + 0.006*"supported" + 0.005*"quality" + 0.005*"disabled" + 0.005*"protection"']</t>
+    <t>['0.018*"’" + 0.010*"Manchester" + 0.007*"well" + 0.006*"needs" + 0.006*"always" + 0.006*"supported" + 0.006*"protection" + 0.005*"plans" + 0.005*"quality" + 0.004*"family"', '0.018*"’" + 0.010*"needs" + 0.008*"well" + 0.008*"Manchester" + 0.006*"education" + 0.006*"supported" + 0.005*"effective" + 0.005*"April" + 0.005*"always" + 0.005*"quality"', '0.026*"’" + 0.013*"Manchester" + 0.011*"needs" + 0.007*"always" + 0.007*"supported" + 0.006*"plans" + 0.006*"well" + 0.006*"1" + 0.005*"effective" + 0.005*"disabled"']</t>
   </si>
   <si>
     <t>80522</t>
@@ -3001,7 +3001,7 @@
     <t>11/09/23</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"Medway" + 0.009*"practice" + 0.008*"leaders" + 0.008*"quality" + 0.007*"well" + 0.006*"impact" + 0.006*"experiences" + 0.006*"oversight" + 0.005*"needs"', '0.016*"’" + 0.008*"Medway" + 0.008*"needs" + 0.008*"well" + 0.008*"quality" + 0.007*"oversight" + 0.006*"practice" + 0.005*"risk" + 0.005*"clear" + 0.005*"good"', '0.014*"’" + 0.009*"practice" + 0.007*"well" + 0.007*"quality" + 0.007*"Medway" + 0.006*"leaders" + 0.005*"17" + 0.005*"impact" + 0.005*"experiences" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.010*"Medway" + 0.008*"quality" + 0.008*"practice" + 0.007*"well" + 0.007*"needs" + 0.006*"impact" + 0.006*"oversight" + 0.005*"experiences" + 0.005*"good"', '0.019*"’" + 0.010*"Medway" + 0.008*"well" + 0.008*"practice" + 0.007*"quality" + 0.007*"leaders" + 0.006*"risk" + 0.006*"oversight" + 0.006*"needs" + 0.005*"clear"', '0.013*"’" + 0.008*"practice" + 0.008*"quality" + 0.007*"Medway" + 0.007*"well" + 0.006*"leaders" + 0.005*"oversight" + 0.005*"needs" + 0.005*"progress" + 0.005*"experiences"']</t>
   </si>
   <si>
     <t>80523</t>
@@ -3025,7 +3025,7 @@
     <t>0.1551</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"effective" + 0.007*"plans" + 0.006*"well" + 0.005*"needs" + 0.005*"Middlesbrough" + 0.005*"practice" + 0.004*"24" + 0.004*"progress" + 0.004*"13"', '0.014*"’" + 0.008*"plans" + 0.008*"effective" + 0.008*"Middlesbrough" + 0.006*"practice" + 0.006*"progress" + 0.005*"well" + 0.005*"place" + 0.005*"impact" + 0.005*"needs"', '0.015*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"Middlesbrough" + 0.006*"plans" + 0.005*"effective" + 0.005*"practice" + 0.005*"progress" + 0.005*"good" + 0.004*"24"']</t>
+    <t>['0.016*"’" + 0.008*"plans" + 0.008*"well" + 0.007*"effective" + 0.007*"needs" + 0.007*"Middlesbrough" + 0.006*"progress" + 0.006*"place" + 0.005*"practice" + 0.005*"good"', '0.010*"’" + 0.007*"plans" + 0.006*"effective" + 0.006*"Middlesbrough" + 0.005*"well" + 0.005*"practice" + 0.005*"means" + 0.005*"needs" + 0.004*"progress" + 0.004*"2023"', '0.014*"’" + 0.007*"Middlesbrough" + 0.007*"effective" + 0.006*"needs" + 0.006*"practice" + 0.006*"plans" + 0.005*"well" + 0.005*"24" + 0.005*"13" + 0.005*"March"']</t>
   </si>
   <si>
     <t>80524</t>
@@ -3052,7 +3052,7 @@
     <t>0.1723</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.006*"Milton" + 0.006*"Keynes" + 0.005*"well" + 0.005*"25" + 0.005*"5" + 0.005*"team" + 0.005*"leaders" + 0.005*"need" + 0.005*"practice"', '0.016*"’" + 0.006*"Keynes" + 0.006*"need" + 0.006*"well" + 0.005*"Milton" + 0.005*"practice" + 0.005*"good" + 0.004*"leaders" + 0.004*"carers" + 0.004*"quality"', '0.012*"’" + 0.006*"Milton" + 0.006*"well" + 0.006*"Keynes" + 0.005*"need" + 0.005*"25" + 0.005*"practice" + 0.005*"October" + 0.005*"plans" + 0.005*"good"']</t>
+    <t>['0.020*"’" + 0.006*"well" + 0.006*"Keynes" + 0.005*"plans" + 0.005*"Milton" + 0.005*"practice" + 0.005*"25" + 0.005*"October" + 0.005*"need" + 0.005*"education"', '0.012*"’" + 0.007*"Milton" + 0.007*"Keynes" + 0.007*"need" + 0.006*"well" + 0.005*"leaders" + 0.005*"good" + 0.005*"25" + 0.005*"practice" + 0.004*"2021"', '0.010*"’" + 0.005*"Keynes" + 0.004*"Milton" + 0.004*"need" + 0.004*"good" + 0.004*"practice" + 0.004*"effective" + 0.004*"impact" + 0.003*"5" + 0.003*"team"']</t>
   </si>
   <si>
     <t>80525</t>
@@ -3079,7 +3079,7 @@
     <t>0.1678</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.011*"plans" + 0.010*"needs" + 0.009*"Newcastle" + 0.007*"well" + 0.007*"good" + 0.006*"progress" + 0.006*"making" + 0.006*"protection" + 0.006*"management"', '0.015*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"protection" + 0.006*"good" + 0.006*"well" + 0.006*"progress" + 0.005*"ensure" + 0.005*"Newcastle" + 0.005*"need"', '0.016*"’" + 0.012*"plans" + 0.007*"protection" + 0.007*"good" + 0.007*"response" + 0.006*"Newcastle" + 0.006*"needs" + 0.006*"well" + 0.006*"10" + 0.005*"making"']</t>
+    <t>['0.012*"’" + 0.008*"Newcastle" + 0.008*"plans" + 0.008*"needs" + 0.007*"progress" + 0.007*"good" + 0.006*"protection" + 0.006*"ensure" + 0.005*"well" + 0.005*"making"', '0.016*"’" + 0.011*"plans" + 0.007*"protection" + 0.007*"Newcastle" + 0.007*"good" + 0.006*"needs" + 0.006*"well" + 0.006*"need" + 0.005*"management" + 0.005*"response"', '0.019*"’" + 0.011*"plans" + 0.009*"needs" + 0.007*"well" + 0.007*"good" + 0.006*"protection" + 0.006*"ensure" + 0.006*"making" + 0.005*"Newcastle" + 0.005*"response"']</t>
   </si>
   <si>
     <t>80418</t>
@@ -3103,7 +3103,7 @@
     <t>0.1799</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"carers" + 0.007*"Norfolk" + 0.006*"well" + 0.005*"needs" + 0.005*"practice" + 0.004*"supported" + 0.004*"leaders" + 0.004*"progress" + 0.004*"7"', '0.016*"’" + 0.009*"well" + 0.007*"Norfolk" + 0.006*"carers" + 0.006*"practice" + 0.006*"plans" + 0.005*"needs" + 0.005*"leaders" + 0.005*"range" + 0.005*"7"', '0.018*"’" + 0.009*"Norfolk" + 0.008*"well" + 0.006*"needs" + 0.006*"supported" + 0.006*"practice" + 0.005*"carers" + 0.005*"including" + 0.005*"information" + 0.004*"progress"']</t>
+    <t>['0.017*"’" + 0.008*"Norfolk" + 0.007*"well" + 0.006*"needs" + 0.006*"carers" + 0.005*"practice" + 0.005*"including" + 0.005*"plans" + 0.004*"leaders" + 0.004*"supported"', '0.017*"’" + 0.008*"Norfolk" + 0.007*"well" + 0.006*"practice" + 0.005*"carers" + 0.005*"supported" + 0.005*"needs" + 0.004*"including" + 0.004*"strong" + 0.004*"range"', '0.017*"’" + 0.009*"well" + 0.008*"Norfolk" + 0.007*"carers" + 0.006*"supported" + 0.006*"needs" + 0.005*"practice" + 0.005*"18" + 0.005*"7" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80526</t>
@@ -3136,7 +3136,7 @@
     <t>0.0968</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"risk" + 0.007*"practice" + 0.006*"planning" + 0.006*"leaders" + 0.005*"oversight" + 0.005*"East" + 0.005*"need" + 0.005*"needs" + 0.004*"Lincolnshire"', '0.012*"’" + 0.007*"risk" + 0.006*"practice" + 0.006*"leaders" + 0.006*"planning" + 0.005*"2021" + 0.005*"needs" + 0.005*"need" + 0.005*"many" + 0.005*"October"', '0.015*"’" + 0.009*"practice" + 0.008*"needs" + 0.007*"leaders" + 0.006*"planning" + 0.006*"risk" + 0.006*"North" + 0.006*"quality" + 0.005*"need" + 0.005*"many"']</t>
+    <t>['0.013*"’" + 0.008*"leaders" + 0.006*"risk" + 0.006*"planning" + 0.006*"needs" + 0.006*"practice" + 0.005*"need" + 0.005*"many" + 0.005*"Lincolnshire" + 0.004*"North"', '0.013*"’" + 0.007*"practice" + 0.006*"risk" + 0.005*"East" + 0.005*"Lincolnshire" + 0.005*"quality" + 0.005*"planning" + 0.005*"needs" + 0.005*"need" + 0.004*"harm"', '0.015*"’" + 0.009*"practice" + 0.008*"risk" + 0.007*"needs" + 0.007*"planning" + 0.007*"leaders" + 0.005*"2021" + 0.005*"many" + 0.005*"need" + 0.005*"senior"']</t>
   </si>
   <si>
     <t>80527</t>
@@ -3166,7 +3166,7 @@
     <t>0.2145</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.007*"‘" + 0.006*"approach" + 0.006*"North" + 0.005*"well" + 0.005*"leaders" + 0.005*"need" + 0.004*"council" + 0.004*"2022" + 0.004*"10"', '0.022*"’" + 0.007*"family" + 0.007*"‘" + 0.007*"Lincolnshire" + 0.006*"10" + 0.005*"need" + 0.005*"North" + 0.005*"leaders" + 0.005*"well" + 0.005*"protection"', '0.010*"’" + 0.008*"‘" + 0.006*"family" + 0.005*"Lincolnshire" + 0.005*"team" + 0.005*"North" + 0.004*"leaders" + 0.004*"approach" + 0.004*"well" + 0.004*"October"']</t>
+    <t>['0.021*"’" + 0.007*"‘" + 0.006*"leaders" + 0.006*"family" + 0.006*"well" + 0.005*"approach" + 0.005*"Lincolnshire" + 0.005*"10" + 0.005*"North" + 0.004*"practice"', '0.022*"’" + 0.007*"‘" + 0.006*"family" + 0.005*"need" + 0.005*"Lincolnshire" + 0.005*"North" + 0.005*"approach" + 0.005*"well" + 0.005*"2022" + 0.004*"protection"', '0.018*"’" + 0.007*"‘" + 0.006*"North" + 0.006*"family" + 0.005*"leaders" + 0.005*"Lincolnshire" + 0.005*"home" + 0.004*"need" + 0.004*"October" + 0.004*"10"']</t>
   </si>
   <si>
     <t>2637539</t>
@@ -3202,7 +3202,7 @@
     <t>8</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.007*"Northamptonshire" + 0.006*"well" + 0.005*"North" + 0.005*"needs" + 0.005*"practice" + 0.004*"plans" + 0.004*"need" + 0.004*"3" + 0.004*"Leaders"', '0.020*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.007*"well" + 0.006*"quality" + 0.005*"Leaders" + 0.005*"impact" + 0.005*"NCT" + 0.005*"needs" + 0.005*"e"', '0.017*"’" + 0.008*"Northamptonshire" + 0.007*"North" + 0.006*"quality" + 0.006*"well" + 0.005*"experiences" + 0.005*"practice" + 0.005*"NCT" + 0.005*"14" + 0.005*"need"']</t>
+    <t>['0.013*"’" + 0.006*"Northamptonshire" + 0.005*"NCT" + 0.005*"Leaders" + 0.005*"well" + 0.005*"14" + 0.004*"North" + 0.004*"plans" + 0.004*"practice" + 0.004*"However"', '0.014*"’" + 0.007*"well" + 0.007*"Northamptonshire" + 0.007*"quality" + 0.006*"North" + 0.005*"practice" + 0.005*"needs" + 0.005*"plans" + 0.005*"NCT" + 0.005*"e"', '0.021*"’" + 0.009*"Northamptonshire" + 0.008*"North" + 0.006*"well" + 0.006*"quality" + 0.006*"impact" + 0.005*"need" + 0.005*"practice" + 0.005*"needs" + 0.005*"Leaders"']</t>
   </si>
   <si>
     <t>80528</t>
@@ -3229,7 +3229,7 @@
     <t>0.1836</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"quality" + 0.006*"needs" + 0.006*"need" + 0.005*"always" + 0.005*"Somerset" + 0.005*"well" + 0.005*"risk" + 0.004*"oversight" + 0.004*"practice"', '0.014*"’" + 0.009*"quality" + 0.007*"needs" + 0.007*"North" + 0.007*"number" + 0.006*"Somerset" + 0.006*"always" + 0.006*"risk" + 0.006*"experienced" + 0.006*"progress"', '0.020*"’" + 0.006*"needs" + 0.006*"practice" + 0.006*"always" + 0.006*"quality" + 0.005*"Somerset" + 0.005*"North" + 0.005*"number" + 0.005*"well" + 0.005*"progress"']</t>
+    <t>['0.016*"’" + 0.008*"quality" + 0.007*"number" + 0.006*"North" + 0.006*"need" + 0.005*"Somerset" + 0.005*"practice" + 0.005*"experienced" + 0.004*"progress" + 0.004*"13"', '0.019*"’" + 0.007*"needs" + 0.007*"Somerset" + 0.007*"always" + 0.007*"quality" + 0.005*"well" + 0.005*"risk" + 0.005*"North" + 0.005*"number" + 0.005*"effective"', '0.014*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"practice" + 0.006*"always" + 0.006*"North" + 0.006*"progress" + 0.005*"risk" + 0.005*"plans" + 0.005*"experienced"']</t>
   </si>
   <si>
     <t>80529</t>
@@ -3256,7 +3256,7 @@
     <t>0.1847</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"well" + 0.006*"leaders" + 0.005*"make" + 0.005*"needs" + 0.005*"need" + 0.005*"quality" + 0.005*"early" + 0.004*"protection" + 0.004*"progress"', '0.013*"’" + 0.006*"well" + 0.005*"need" + 0.004*"leaders" + 0.004*"make" + 0.004*"quality" + 0.003*"needs" + 0.003*"understand" + 0.003*"foster" + 0.003*"experiences"', '0.016*"’" + 0.005*"need" + 0.005*"well" + 0.005*"leaders" + 0.005*"impact" + 0.005*"quality" + 0.004*"needs" + 0.004*"clear" + 0.004*"make" + 0.003*"carers"']</t>
+    <t>['0.018*"’" + 0.007*"well" + 0.005*"need" + 0.005*"impact" + 0.005*"leaders" + 0.005*"quality" + 0.004*"make" + 0.004*"experiences" + 0.004*"protection" + 0.004*"training"', '0.015*"’" + 0.007*"well" + 0.006*"leaders" + 0.005*"need" + 0.005*"needs" + 0.005*"make" + 0.004*"early" + 0.004*"quality" + 0.004*"clear" + 0.004*"family"', '0.015*"’" + 0.005*"leaders" + 0.005*"well" + 0.005*"progress" + 0.005*"make" + 0.004*"need" + 0.004*"needs" + 0.004*"quality" + 0.004*"protection" + 0.003*"foster"']</t>
   </si>
   <si>
     <t>80530</t>
@@ -3286,7 +3286,7 @@
     <t>18/08/23</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.011*"well" + 0.007*"Yorkshire" + 0.007*"needs" + 0.006*"practice" + 0.006*"North" + 0.006*"family" + 0.005*"‘" + 0.004*"3" + 0.004*"need"', '0.024*"’" + 0.007*"North" + 0.007*"well" + 0.006*"practice" + 0.006*"family" + 0.005*"Yorkshire" + 0.005*"supported" + 0.005*"‘" + 0.005*"needs" + 0.005*"3"', '0.012*"’" + 0.006*"Yorkshire" + 0.005*"well" + 0.005*"family" + 0.005*"North" + 0.004*"practice" + 0.004*"7" + 0.004*"needs" + 0.004*"supported" + 0.004*"ensure"']</t>
+    <t>['0.024*"’" + 0.007*"well" + 0.006*"North" + 0.005*"‘" + 0.005*"needs" + 0.005*"Yorkshire" + 0.005*"practice" + 0.005*"family" + 0.004*"7" + 0.004*"planning"', '0.021*"’" + 0.010*"well" + 0.006*"Yorkshire" + 0.006*"practice" + 0.006*"North" + 0.006*"family" + 0.006*"needs" + 0.005*"3" + 0.004*"need" + 0.004*"2023"', '0.016*"’" + 0.007*"practice" + 0.007*"Yorkshire" + 0.006*"North" + 0.006*"family" + 0.006*"well" + 0.005*"needs" + 0.005*"‘" + 0.004*"3" + 0.004*"supported"']</t>
   </si>
   <si>
     <t>80532</t>
@@ -3313,7 +3313,7 @@
     <t>0.2204</t>
   </si>
   <si>
-    <t>['0.022*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"good" + 0.007*"need" + 0.006*"education" + 0.005*"practice" + 0.005*"impact" + 0.005*"experiences" + 0.005*"quality"', '0.019*"’" + 0.013*"well" + 0.010*"needs" + 0.007*"good" + 0.006*"need" + 0.006*"experiences" + 0.005*"impact" + 0.005*"practice" + 0.005*"quality" + 0.004*"leaders"', '0.025*"’" + 0.009*"needs" + 0.008*"good" + 0.006*"well" + 0.005*"need" + 0.005*"experiences" + 0.005*"practice" + 0.005*"impact" + 0.005*"leaders" + 0.005*"quality"']</t>
+    <t>['0.023*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"good" + 0.006*"experiences" + 0.005*"practice" + 0.005*"need" + 0.005*"education" + 0.005*"leaders" + 0.004*"always"', '0.014*"’" + 0.009*"well" + 0.008*"needs" + 0.007*"good" + 0.007*"need" + 0.005*"experiences" + 0.004*"practice" + 0.004*"education" + 0.004*"impact" + 0.004*"effective"', '0.027*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"good" + 0.007*"impact" + 0.006*"need" + 0.006*"quality" + 0.005*"experiences" + 0.005*"practice" + 0.004*"education"']</t>
   </si>
   <si>
     <t>80533</t>
@@ -3343,7 +3343,7 @@
     <t>0.1774</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"Nottingham" + 0.007*"needs" + 0.007*"plans" + 0.006*"oversight" + 0.006*"effective" + 0.006*"practice" + 0.005*"impact" + 0.005*"City" + 0.005*"11"', '0.011*"’" + 0.008*"needs" + 0.004*"City" + 0.004*"effective" + 0.004*"Nottingham" + 0.004*"impact" + 0.004*"11" + 0.004*"plans" + 0.003*"2022" + 0.003*"However"', '0.015*"’" + 0.009*"needs" + 0.005*"Nottingham" + 0.005*"plans" + 0.005*"2022" + 0.005*"effective" + 0.005*"However" + 0.005*"risk" + 0.004*"protection" + 0.004*"consistently"']</t>
+    <t>['0.014*"’" + 0.008*"needs" + 0.007*"plans" + 0.006*"2022" + 0.005*"effective" + 0.005*"impact" + 0.005*"11" + 0.005*"However" + 0.005*"oversight" + 0.005*"practice"', '0.014*"’" + 0.009*"needs" + 0.007*"Nottingham" + 0.005*"effective" + 0.005*"plans" + 0.005*"oversight" + 0.005*"City" + 0.005*"11" + 0.004*"good" + 0.004*"impact"', '0.013*"’" + 0.007*"needs" + 0.005*"effective" + 0.005*"Nottingham" + 0.005*"July" + 0.005*"impact" + 0.004*"risk" + 0.004*"consistently" + 0.004*"City" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80534</t>
@@ -3367,7 +3367,7 @@
     <t>07/10/2019</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"practice" + 0.008*"well" + 0.006*"needs" + 0.006*"plans" + 0.005*"receive" + 0.005*"progress" + 0.005*"carers" + 0.005*"ensure" + 0.005*"effective"', '0.011*"’" + 0.008*"practice" + 0.008*"well" + 0.006*"receive" + 0.006*"needs" + 0.005*"quality" + 0.005*"ensure" + 0.005*"made" + 0.004*"e" + 0.004*"plans"', '0.012*"’" + 0.008*"well" + 0.007*"practice" + 0.006*"progress" + 0.005*"needs" + 0.005*"e" + 0.005*"ensure" + 0.005*"receive" + 0.005*"made" + 0.004*"areas"']</t>
+    <t>['0.011*"’" + 0.008*"practice" + 0.007*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"made" + 0.005*"ensure" + 0.005*"quality" + 0.005*"good" + 0.004*"receive"', '0.015*"’" + 0.010*"well" + 0.008*"practice" + 0.006*"receive" + 0.006*"needs" + 0.006*"progress" + 0.005*"quality" + 0.005*"placements" + 0.005*"e" + 0.005*"effective"', '0.008*"practice" + 0.007*"’" + 0.005*"well" + 0.005*"ensure" + 0.004*"needs" + 0.004*"areas" + 0.004*"receive" + 0.004*"progress" + 0.004*"meetings" + 0.004*"made"']</t>
   </si>
   <si>
     <t>80535</t>
@@ -3400,7 +3400,7 @@
     <t>04/03/19</t>
   </si>
   <si>
-    <t>['0.009*"’" + 0.007*"practice" + 0.007*"good" + 0.007*"needs" + 0.006*"well" + 0.006*"quality" + 0.006*"effective" + 0.005*"planning" + 0.004*"progress" + 0.004*"many"', '0.013*"’" + 0.010*"needs" + 0.010*"good" + 0.010*"practice" + 0.008*"effective" + 0.007*"planning" + 0.007*"progress" + 0.007*"plans" + 0.006*"well" + 0.006*"quality"', '0.009*"good" + 0.009*"effective" + 0.009*"needs" + 0.008*"practice" + 0.008*"’" + 0.007*"progress" + 0.006*"quality" + 0.006*"plans" + 0.006*"well" + 0.005*"risk"']</t>
+    <t>['0.010*"good" + 0.010*"needs" + 0.010*"effective" + 0.009*"’" + 0.008*"practice" + 0.007*"plans" + 0.006*"well" + 0.005*"progress" + 0.005*"quality" + 0.005*"planning"', '0.011*"’" + 0.009*"good" + 0.007*"practice" + 0.007*"needs" + 0.006*"well" + 0.006*"risk" + 0.005*"effective" + 0.005*"plans" + 0.005*"planning" + 0.005*"quality"', '0.012*"’" + 0.010*"practice" + 0.009*"needs" + 0.008*"good" + 0.008*"progress" + 0.008*"quality" + 0.007*"effective" + 0.007*"planning" + 0.006*"well" + 0.006*"impact"']</t>
   </si>
   <si>
     <t>80536</t>
@@ -3430,7 +3430,7 @@
     <t>0.1755</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.011*"needs" + 0.007*"well" + 0.006*"good" + 0.005*"12" + 0.005*"Oxfordshire" + 0.005*"progress" + 0.005*"supported" + 0.005*"23" + 0.005*"quality"', '0.018*"’" + 0.010*"needs" + 0.008*"risk" + 0.007*"Oxfordshire" + 0.006*"supported" + 0.006*"quality" + 0.005*"well" + 0.005*"practice" + 0.005*"good" + 0.004*"arrangements"', '0.019*"’" + 0.009*"needs" + 0.008*"Oxfordshire" + 0.008*"well" + 0.005*"receive" + 0.005*"supported" + 0.005*"risk" + 0.005*"12" + 0.005*"good" + 0.005*"arrangements"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Oxfordshire" + 0.006*"risk" + 0.005*"good" + 0.005*"arrangements" + 0.005*"receive" + 0.005*"access" + 0.005*"progress"', '0.022*"’" + 0.009*"needs" + 0.008*"Oxfordshire" + 0.007*"well" + 0.005*"quality" + 0.005*"good" + 0.005*"practice" + 0.005*"supported" + 0.005*"23" + 0.004*"receive"', '0.017*"’" + 0.012*"needs" + 0.007*"risk" + 0.006*"supported" + 0.006*"well" + 0.006*"Oxfordshire" + 0.006*"12" + 0.006*"good" + 0.005*"progress" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80537</t>
@@ -3460,7 +3460,7 @@
     <t>30/01/24</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.016*"needs" + 0.008*"Peterborough" + 0.007*"need" + 0.006*"8" + 0.006*"2023" + 0.006*"27" + 0.006*"well" + 0.005*"progress" + 0.005*"receive"', '0.012*"needs" + 0.012*"’" + 0.007*"progress" + 0.007*"Peterborough" + 0.006*"well" + 0.006*"2023" + 0.006*"need" + 0.005*"good" + 0.005*"supported" + 0.005*"education"', '0.013*"’" + 0.010*"needs" + 0.007*"need" + 0.007*"2023" + 0.007*"well" + 0.006*"Peterborough" + 0.005*"plans" + 0.005*"progress" + 0.005*"supported" + 0.005*"8"']</t>
+    <t>['0.008*"’" + 0.007*"needs" + 0.006*"Peterborough" + 0.005*"need" + 0.004*"progress" + 0.004*"receive" + 0.004*"appropriate" + 0.004*"27" + 0.004*"well" + 0.004*"2023"', '0.019*"’" + 0.016*"needs" + 0.009*"2023" + 0.007*"Peterborough" + 0.007*"need" + 0.007*"well" + 0.006*"supported" + 0.005*"good" + 0.005*"8" + 0.005*"plans"', '0.013*"needs" + 0.012*"’" + 0.008*"progress" + 0.007*"need" + 0.007*"well" + 0.006*"Peterborough" + 0.006*"8" + 0.006*"plans" + 0.005*"27" + 0.005*"receive"']</t>
   </si>
   <si>
     <t>80538</t>
@@ -3490,7 +3490,7 @@
     <t>15/03/24</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"Plymouth" + 0.005*"good" + 0.004*"appropriate" + 0.004*"education" + 0.004*"Council" + 0.004*"practice" + 0.004*"quality"', '0.013*"’" + 0.008*"needs" + 0.008*"well" + 0.006*"Plymouth" + 0.006*"practice" + 0.006*"22" + 0.005*"education" + 0.005*"February" + 0.005*"appropriate" + 0.004*"2024"', '0.015*"’" + 0.008*"needs" + 0.007*"Plymouth" + 0.006*"well" + 0.005*"2" + 0.005*"plans" + 0.005*"practice" + 0.005*"January" + 0.004*"effective" + 0.004*"City"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.007*"well" + 0.006*"Plymouth" + 0.006*"appropriate" + 0.005*"practice" + 0.005*"plans" + 0.005*"education" + 0.005*"2" + 0.004*"effective"', '0.013*"’" + 0.009*"needs" + 0.007*"Plymouth" + 0.007*"well" + 0.005*"practice" + 0.005*"22" + 0.005*"risks" + 0.005*"good" + 0.004*"2" + 0.004*"ensure"', '0.012*"’" + 0.007*"Plymouth" + 0.007*"well" + 0.007*"needs" + 0.005*"risks" + 0.005*"2024" + 0.005*"practice" + 0.004*"2" + 0.004*"City" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80539</t>
@@ -3523,7 +3523,7 @@
     <t>0.1859</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"care-experienced" + 0.008*"needs" + 0.008*"Portsmouth" + 0.007*"well" + 0.006*"leaders" + 0.006*"health" + 0.005*"practice" + 0.005*"family" + 0.005*"progress"', '0.019*"’" + 0.008*"well" + 0.006*"care-experienced" + 0.006*"Portsmouth" + 0.006*"plans" + 0.006*"needs" + 0.005*"family" + 0.005*"May" + 0.005*"health" + 0.004*"receive"', '0.014*"’" + 0.008*"care-experienced" + 0.006*"well" + 0.006*"family" + 0.006*"needs" + 0.006*"Portsmouth" + 0.005*"health" + 0.005*"plans" + 0.004*"need" + 0.004*"2023"']</t>
+    <t>['0.015*"’" + 0.008*"care-experienced" + 0.007*"well" + 0.007*"Portsmouth" + 0.007*"needs" + 0.006*"plans" + 0.005*"family" + 0.004*"council" + 0.004*"health" + 0.004*"19"', '0.018*"’" + 0.009*"care-experienced" + 0.007*"well" + 0.006*"health" + 0.006*"needs" + 0.006*"Portsmouth" + 0.005*"family" + 0.005*"leaders" + 0.005*"plans" + 0.004*"receive"', '0.018*"’" + 0.007*"well" + 0.007*"Portsmouth" + 0.007*"care-experienced" + 0.007*"needs" + 0.006*"family" + 0.004*"risk" + 0.004*"good" + 0.004*"need" + 0.004*"practice"']</t>
   </si>
   <si>
     <t>80540</t>
@@ -3559,7 +3559,7 @@
     <t>0.1741</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.008*"quality" + 0.006*"well" + 0.006*"number" + 0.005*"plans" + 0.005*"good" + 0.005*"needs" + 0.005*"effective" + 0.005*"carers" + 0.005*"practice"', '0.016*"’" + 0.008*"number" + 0.007*"plans" + 0.007*"well" + 0.006*"quality" + 0.006*"need" + 0.006*"good" + 0.005*"effective" + 0.005*"ensure" + 0.005*"However"', '0.013*"’" + 0.005*"well" + 0.005*"number" + 0.005*"quality" + 0.005*"good" + 0.005*"plans" + 0.005*"effective" + 0.004*"health" + 0.004*"always" + 0.004*"need"']</t>
+    <t>['0.020*"’" + 0.008*"quality" + 0.007*"number" + 0.007*"good" + 0.006*"well" + 0.006*"plans" + 0.005*"need" + 0.005*"arrangements" + 0.005*"effective" + 0.005*"timely"', '0.009*"’" + 0.007*"number" + 0.006*"plans" + 0.005*"well" + 0.005*"need" + 0.004*"quality" + 0.004*"timely" + 0.004*"However" + 0.004*"effective" + 0.004*"good"', '0.016*"’" + 0.007*"well" + 0.007*"quality" + 0.007*"number" + 0.006*"plans" + 0.006*"effective" + 0.005*"practice" + 0.005*"always" + 0.005*"need" + 0.005*"needs"']</t>
   </si>
   <si>
     <t>80541</t>
@@ -3583,7 +3583,7 @@
     <t>22/09/22</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.006*"consistently" + 0.005*"leaders" + 0.005*"practice" + 0.005*"needs" + 0.005*"carers" + 0.005*"plans" + 0.005*"response" + 0.005*"2022" + 0.005*"20"', '0.019*"’" + 0.007*"plans" + 0.007*"leaders" + 0.006*"However" + 0.006*"needs" + 0.005*"2022" + 0.005*"consistently" + 0.005*"Redcar" + 0.005*"risk" + 0.004*"Cleveland"', '0.017*"’" + 0.006*"leaders" + 0.006*"However" + 0.006*"needs" + 0.005*"20" + 0.005*"practice" + 0.005*"consistently" + 0.005*"2022" + 0.005*"Cleveland" + 0.005*"carers"']</t>
+    <t>['0.019*"’" + 0.007*"However" + 0.006*"leaders" + 0.006*"needs" + 0.006*"consistently" + 0.006*"plans" + 0.005*"practice" + 0.005*"July" + 0.005*"risk" + 0.005*"20"', '0.016*"’" + 0.007*"leaders" + 0.006*"plans" + 0.006*"needs" + 0.005*"However" + 0.005*"1" + 0.005*"Redcar" + 0.005*"20" + 0.005*"consistently" + 0.005*"carers"', '0.017*"’" + 0.005*"leaders" + 0.005*"consistently" + 0.005*"2022" + 0.005*"Redcar" + 0.005*"practice" + 0.004*"Cleveland" + 0.004*"20" + 0.004*"needs" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80542</t>
@@ -3610,7 +3610,7 @@
     <t>17/03/23</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"experienced" + 0.008*"practice" + 0.007*"needs" + 0.006*"consistently" + 0.006*"plans" + 0.005*"Rochdale" + 0.005*"good" + 0.005*"quality" + 0.005*"response"', '0.018*"’" + 0.011*"experienced" + 0.010*"practice" + 0.007*"needs" + 0.006*"plans" + 0.006*"response" + 0.006*"well" + 0.005*"quality" + 0.005*"consistently" + 0.005*"PAs"', '0.023*"’" + 0.009*"needs" + 0.009*"experienced" + 0.006*"response" + 0.006*"practice" + 0.005*"good" + 0.005*"quality" + 0.005*"plans" + 0.005*"progress" + 0.005*"consistently"']</t>
+    <t>['0.021*"’" + 0.008*"experienced" + 0.007*"practice" + 0.007*"needs" + 0.005*"response" + 0.005*"quality" + 0.005*"progress" + 0.005*"consistently" + 0.005*"3" + 0.004*"2023"', '0.015*"’" + 0.008*"experienced" + 0.008*"needs" + 0.007*"practice" + 0.005*"response" + 0.005*"quality" + 0.005*"good" + 0.004*"consistently" + 0.004*"progress" + 0.004*"Rochdale"', '0.023*"’" + 0.011*"experienced" + 0.009*"practice" + 0.008*"needs" + 0.008*"plans" + 0.007*"response" + 0.007*"good" + 0.006*"consistently" + 0.005*"Rochdale" + 0.005*"quality"']</t>
   </si>
   <si>
     <t>80543</t>
@@ -3637,7 +3637,7 @@
     <t>0.1845</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.009*"Rotherham" + 0.006*"good" + 0.006*"well" + 0.006*"needs" + 0.005*"ensure" + 0.004*"plans" + 0.004*"However" + 0.004*"clear" + 0.004*"Council"', '0.014*"’" + 0.008*"needs" + 0.008*"Rotherham" + 0.005*"ensure" + 0.005*"Council" + 0.005*"well" + 0.005*"Borough" + 0.005*"plans" + 0.004*"good" + 0.004*"However"', '0.013*"’" + 0.009*"Rotherham" + 0.005*"needs" + 0.004*"Council" + 0.004*"However" + 0.004*"well" + 0.004*"2022" + 0.004*"1" + 0.004*"Metropolitan" + 0.004*"June"']</t>
+    <t>['0.017*"’" + 0.012*"Rotherham" + 0.007*"needs" + 0.006*"plans" + 0.006*"good" + 0.006*"well" + 0.005*"Council" + 0.005*"ensure" + 0.005*"However" + 0.005*"Borough"', '0.013*"’" + 0.007*"Rotherham" + 0.007*"needs" + 0.005*"well" + 0.005*"good" + 0.005*"ensure" + 0.004*"27" + 0.004*"Metropolitan" + 0.004*"However" + 0.004*"Council"', '0.013*"’" + 0.005*"needs" + 0.005*"Rotherham" + 0.004*"Council" + 0.004*"However" + 0.004*"well" + 0.004*"protection" + 0.004*"Metropolitan" + 0.004*"ensure" + 0.003*"concerns"']</t>
   </si>
   <si>
     <t>80544</t>
@@ -3664,7 +3664,7 @@
     <t>0.222</t>
   </si>
   <si>
-    <t>['0.015*"well" + 0.011*"’" + 0.010*"practice" + 0.006*"effective" + 0.006*"strong" + 0.006*"highly" + 0.005*"needs" + 0.005*"leaders" + 0.005*"high" + 0.004*"professionals"', '0.016*"well" + 0.013*"’" + 0.012*"practice" + 0.008*"highly" + 0.007*"needs" + 0.006*"strong" + 0.005*"leaders" + 0.005*"effective" + 0.004*"high" + 0.004*"progress"', '0.010*"’" + 0.009*"practice" + 0.008*"well" + 0.007*"highly" + 0.006*"strong" + 0.004*"leaders" + 0.004*"timely" + 0.004*"professionals" + 0.004*"effective" + 0.004*"information"']</t>
+    <t>['0.016*"well" + 0.012*"’" + 0.011*"practice" + 0.008*"highly" + 0.006*"needs" + 0.006*"effective" + 0.006*"leaders" + 0.005*"strong" + 0.005*"range" + 0.005*"professionals"', '0.010*"well" + 0.008*"’" + 0.008*"practice" + 0.007*"strong" + 0.006*"highly" + 0.004*"effective" + 0.004*"needs" + 0.004*"improve" + 0.004*"leaders" + 0.004*"professionals"', '0.013*"’" + 0.013*"well" + 0.012*"practice" + 0.008*"highly" + 0.007*"strong" + 0.005*"needs" + 0.005*"high" + 0.005*"effective" + 0.004*"leaders" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80545</t>
@@ -3694,7 +3694,7 @@
     <t>0.2108</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.011*"well" + 0.009*"plans" + 0.009*"needs" + 0.006*"good" + 0.005*"effective" + 0.005*"appropriate" + 0.005*"practice" + 0.004*"information" + 0.004*"risk"', '0.010*"’" + 0.008*"well" + 0.007*"plans" + 0.007*"needs" + 0.004*"effective" + 0.004*"good" + 0.004*"parents" + 0.004*"supported" + 0.004*"need" + 0.004*"clear"', '0.015*"’" + 0.008*"well" + 0.008*"plans" + 0.006*"needs" + 0.005*"practice" + 0.004*"clear" + 0.004*"need" + 0.004*"good" + 0.004*"effective" + 0.004*"risk"']</t>
+    <t>['0.015*"’" + 0.009*"plans" + 0.009*"well" + 0.008*"needs" + 0.006*"good" + 0.005*"practice" + 0.005*"clear" + 0.005*"need" + 0.005*"effective" + 0.005*"parents"', '0.012*"’" + 0.010*"well" + 0.008*"plans" + 0.007*"needs" + 0.005*"supported" + 0.005*"good" + 0.004*"effective" + 0.004*"risk" + 0.004*"clear" + 0.004*"Kingston"', '0.012*"’" + 0.008*"well" + 0.006*"plans" + 0.006*"needs" + 0.004*"risk" + 0.004*"effective" + 0.004*"need" + 0.004*"practice" + 0.003*"appropriate" + 0.003*"good"']</t>
   </si>
   <si>
     <t>80546</t>
@@ -3724,7 +3724,7 @@
     <t>24/02/20</t>
   </si>
   <si>
-    <t>['0.012*"’" + 0.005*"quality" + 0.005*"well" + 0.004*"use" + 0.004*"needs" + 0.004*"benefit" + 0.004*"actions" + 0.004*"early" + 0.004*"effective" + 0.004*"health"', '0.006*"’" + 0.004*"needs" + 0.004*"well" + 0.004*"quality" + 0.004*"always" + 0.004*"information" + 0.003*"effective" + 0.003*"plans" + 0.003*"management" + 0.003*"However"', '0.014*"’" + 0.006*"well" + 0.006*"plans" + 0.005*"needs" + 0.005*"quality" + 0.004*"information" + 0.004*"effective" + 0.004*"benefit" + 0.004*"However" + 0.004*"use"']</t>
+    <t>['0.011*"’" + 0.006*"well" + 0.006*"plans" + 0.004*"needs" + 0.004*"quality" + 0.004*"information" + 0.004*"benefit" + 0.004*"always" + 0.004*"effective" + 0.004*"use"', '0.013*"’" + 0.006*"well" + 0.005*"quality" + 0.004*"benefit" + 0.004*"actions" + 0.004*"needs" + 0.004*"information" + 0.004*"use" + 0.003*"early" + 0.003*"plans"', '0.011*"’" + 0.006*"needs" + 0.005*"quality" + 0.004*"effective" + 0.004*"However" + 0.004*"plans" + 0.004*"use" + 0.004*"well" + 0.004*"informed" + 0.004*"need"']</t>
   </si>
   <si>
     <t>80547</t>
@@ -3748,7 +3748,7 @@
     <t>0.1818</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"needs" + 0.006*"practice" + 0.006*"well" + 0.006*"team" + 0.006*"good" + 0.006*"plans" + 0.005*"protection" + 0.005*"need" + 0.005*"family"', '0.013*"’" + 0.011*"well" + 0.010*"needs" + 0.009*"good" + 0.007*"need" + 0.006*"team" + 0.006*"practice" + 0.006*"effective" + 0.006*"protection" + 0.006*"ensure"', '0.014*"’" + 0.012*"well" + 0.009*"needs" + 0.007*"good" + 0.007*"team" + 0.007*"need" + 0.006*"enough" + 0.006*"ensure" + 0.006*"effective" + 0.006*"plans"']</t>
+    <t>['0.014*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"need" + 0.008*"good" + 0.007*"ensure" + 0.006*"effective" + 0.006*"practice" + 0.006*"protection" + 0.006*"plans"', '0.008*"’" + 0.008*"well" + 0.006*"needs" + 0.005*"enough" + 0.005*"plans" + 0.005*"protection" + 0.005*"need" + 0.005*"good" + 0.005*"team" + 0.004*"However"', '0.013*"’" + 0.010*"well" + 0.009*"needs" + 0.009*"team" + 0.008*"good" + 0.008*"practice" + 0.006*"enough" + 0.006*"effective" + 0.005*"plans" + 0.005*"protection"']</t>
   </si>
   <si>
     <t>80548</t>
@@ -3775,7 +3775,7 @@
     <t>0.2045</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"effective" + 0.006*"Salford" + 0.005*"leaders" + 0.005*"experiences" + 0.004*"10" + 0.004*"planning"', '0.011*"’" + 0.007*"effective" + 0.007*"plans" + 0.007*"needs" + 0.006*"well" + 0.005*"practice" + 0.005*"Salford" + 0.005*"10" + 0.004*"6" + 0.004*"ensure"', '0.014*"’" + 0.009*"plans" + 0.008*"needs" + 0.006*"Salford" + 0.006*"well" + 0.006*"leaders" + 0.006*"planning" + 0.005*"effective" + 0.005*"practice" + 0.005*"quality"']</t>
+    <t>['0.015*"’" + 0.007*"needs" + 0.007*"well" + 0.007*"plans" + 0.006*"Salford" + 0.006*"effective" + 0.004*"leaders" + 0.004*"planning" + 0.004*"quality" + 0.004*"practice"', '0.011*"’" + 0.008*"plans" + 0.007*"effective" + 0.006*"well" + 0.006*"practice" + 0.006*"needs" + 0.005*"planning" + 0.005*"progress" + 0.005*"Salford" + 0.005*"leaders"', '0.014*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"plans" + 0.007*"effective" + 0.006*"Salford" + 0.005*"6" + 0.005*"experiences" + 0.005*"quality" + 0.005*"planning"']</t>
   </si>
   <si>
     <t>80549</t>
@@ -3799,7 +3799,7 @@
     <t>0.1681</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"plans" + 0.006*"Sandwell" + 0.006*"quality" + 0.005*"number" + 0.005*"education" + 0.005*"many" + 0.005*"9"', '0.010*"’" + 0.008*"needs" + 0.007*"Sandwell" + 0.006*"plans" + 0.005*"well" + 0.005*"quality" + 0.005*"many" + 0.005*"9" + 0.004*"Trust" + 0.004*"20"', '0.018*"’" + 0.008*"Sandwell" + 0.008*"needs" + 0.008*"plans" + 0.006*"well" + 0.006*"quality" + 0.005*"Trust" + 0.005*"good" + 0.005*"progress" + 0.004*"changes"']</t>
+    <t>['0.019*"’" + 0.009*"needs" + 0.009*"Sandwell" + 0.008*"plans" + 0.007*"well" + 0.006*"quality" + 0.005*"20" + 0.005*"9" + 0.005*"progress" + 0.005*"effective"', '0.008*"’" + 0.007*"plans" + 0.007*"needs" + 0.006*"Sandwell" + 0.005*"well" + 0.005*"quality" + 0.004*"Trust" + 0.004*"many" + 0.004*"number" + 0.004*"progress"', '0.011*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"Sandwell" + 0.005*"plans" + 0.005*"many" + 0.005*"quality" + 0.004*"Trust" + 0.004*"receive" + 0.004*"changes"']</t>
   </si>
   <si>
     <t>80550</t>
@@ -3823,7 +3823,7 @@
     <t>0.1106</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.008*"needs" + 0.007*"practice" + 0.005*"oversight" + 0.005*"management" + 0.005*"timely" + 0.005*"March" + 0.005*"including" + 0.005*"protection" + 0.004*"plans"', '0.016*"’" + 0.010*"needs" + 0.006*"practice" + 0.005*"Sefton" + 0.005*"lack" + 0.005*"always" + 0.005*"protection" + 0.005*"oversight" + 0.005*"including" + 0.005*"◼"', '0.016*"’" + 0.010*"needs" + 0.006*"oversight" + 0.006*"practice" + 0.005*"lack" + 0.005*"including" + 0.005*"protection" + 0.005*"management" + 0.005*"◼" + 0.005*"21"']</t>
+    <t>['0.013*"’" + 0.010*"needs" + 0.007*"practice" + 0.006*"lack" + 0.006*"protection" + 0.006*"including" + 0.005*"oversight" + 0.005*"◼" + 0.005*"always" + 0.005*"March"', '0.020*"’" + 0.010*"needs" + 0.006*"oversight" + 0.006*"practice" + 0.005*"management" + 0.005*"plans" + 0.005*"timely" + 0.005*"including" + 0.005*"planning" + 0.005*"many"', '0.015*"’" + 0.008*"needs" + 0.006*"practice" + 0.005*"oversight" + 0.004*"many" + 0.004*"lack" + 0.004*"always" + 0.004*"March" + 0.004*"◼" + 0.004*"timely"']</t>
   </si>
   <si>
     <t>80551</t>
@@ -3856,7 +3856,7 @@
     <t>0.2097</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"needs" + 0.005*"health" + 0.005*"well" + 0.005*"Sheffield" + 0.004*"leaders" + 0.004*"quality" + 0.004*"good" + 0.003*"plans" + 0.003*"adviser"', '0.023*"’" + 0.014*"Sheffield" + 0.011*"needs" + 0.008*"well" + 0.007*"practice" + 0.007*"leaders" + 0.006*"experiences" + 0.005*"health" + 0.005*"22" + 0.005*"receive"', '0.020*"’" + 0.011*"Sheffield" + 0.007*"well" + 0.006*"needs" + 0.006*"health" + 0.005*"practice" + 0.005*"11" + 0.005*"leaders" + 0.005*"plans" + 0.004*"effective"']</t>
+    <t>['0.021*"’" + 0.013*"Sheffield" + 0.010*"needs" + 0.008*"well" + 0.007*"health" + 0.005*"practice" + 0.005*"leaders" + 0.005*"ensure" + 0.004*"quality" + 0.004*"experiences"', '0.023*"’" + 0.010*"Sheffield" + 0.009*"needs" + 0.007*"well" + 0.006*"leaders" + 0.005*"health" + 0.005*"practice" + 0.004*"11" + 0.004*"good" + 0.004*"quality"', '0.017*"’" + 0.010*"Sheffield" + 0.007*"practice" + 0.006*"needs" + 0.006*"leaders" + 0.005*"well" + 0.005*"plans" + 0.004*"quality" + 0.004*"receive" + 0.004*"September"']</t>
   </si>
   <si>
     <t>80552</t>
@@ -3886,7 +3886,7 @@
     <t>0.1843</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.009*"needs" + 0.006*"Shropshire" + 0.005*"well" + 0.005*"progress" + 0.005*"making" + 0.005*"need" + 0.005*"7" + 0.004*"leaders" + 0.004*"2022"', '0.019*"’" + 0.010*"needs" + 0.009*"well" + 0.007*"Shropshire" + 0.007*"progress" + 0.006*"plans" + 0.005*"2022" + 0.005*"11" + 0.005*"7" + 0.005*"making"', '0.015*"’" + 0.007*"Shropshire" + 0.005*"needs" + 0.005*"plans" + 0.005*"2022" + 0.005*"well" + 0.005*"arrangements" + 0.005*"making" + 0.005*"progress" + 0.004*"need"']</t>
+    <t>['0.014*"’" + 0.009*"needs" + 0.008*"well" + 0.008*"Shropshire" + 0.006*"plans" + 0.006*"2022" + 0.005*"making" + 0.005*"progress" + 0.005*"7" + 0.004*"11"', '0.018*"’" + 0.007*"needs" + 0.007*"progress" + 0.006*"well" + 0.005*"Shropshire" + 0.005*"plans" + 0.004*"2022" + 0.004*"7" + 0.004*"make" + 0.004*"leaders"', '0.020*"’" + 0.009*"needs" + 0.006*"Shropshire" + 0.006*"well" + 0.005*"progress" + 0.005*"making" + 0.005*"plans" + 0.005*"leaders" + 0.005*"7" + 0.005*"February"']</t>
   </si>
   <si>
     <t>80553</t>
@@ -3910,7 +3910,7 @@
     <t>0.1618</t>
   </si>
   <si>
-    <t>['0.011*"’" + 0.008*"Slough" + 0.006*"needs" + 0.005*"practice" + 0.004*"plans" + 0.004*"supported" + 0.004*"3" + 0.004*"However" + 0.004*"impact" + 0.004*"23"', '0.016*"’" + 0.007*"plans" + 0.007*"Slough" + 0.006*"needs" + 0.005*"quality" + 0.005*"practice" + 0.004*"23" + 0.004*"leaders" + 0.004*"impact" + 0.004*"3"', '0.017*"’" + 0.008*"Slough" + 0.008*"quality" + 0.006*"needs" + 0.006*"plans" + 0.006*"practice" + 0.006*"leaders" + 0.005*"impact" + 0.005*"3" + 0.005*"senior"']</t>
+    <t>['0.016*"’" + 0.009*"Slough" + 0.006*"plans" + 0.006*"quality" + 0.006*"needs" + 0.005*"need" + 0.005*"practice" + 0.005*"timely" + 0.005*"3" + 0.005*"February"', '0.017*"’" + 0.008*"Slough" + 0.007*"needs" + 0.007*"plans" + 0.006*"practice" + 0.006*"quality" + 0.006*"impact" + 0.005*"leaders" + 0.005*"3" + 0.005*"time"', '0.012*"’" + 0.005*"Slough" + 0.005*"plans" + 0.005*"needs" + 0.005*"quality" + 0.004*"impact" + 0.004*"practice" + 0.004*"January" + 0.004*"supported" + 0.004*"planning"']</t>
   </si>
   <si>
     <t>80554</t>
@@ -3934,7 +3934,7 @@
     <t>0.1175</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.011*"lack" + 0.009*"2022" + 0.007*"risk" + 0.006*"Solihull" + 0.006*"quality" + 0.005*"experiences" + 0.005*"need" + 0.005*"effective" + 0.005*"means"', '0.014*"’" + 0.008*"lack" + 0.005*"delay" + 0.005*"practice" + 0.005*"worker" + 0.005*"need" + 0.004*"Solihull" + 0.004*"2022" + 0.004*"11" + 0.004*"quality"', '0.014*"’" + 0.012*"lack" + 0.010*"2022" + 0.008*"need" + 0.007*"Solihull" + 0.006*"risk" + 0.006*"quality" + 0.006*"significant" + 0.006*"effective" + 0.006*"practice"']</t>
+    <t>['0.015*"’" + 0.011*"lack" + 0.008*"2022" + 0.007*"risk" + 0.006*"need" + 0.006*"Solihull" + 0.006*"quality" + 0.005*"practice" + 0.005*"effective" + 0.005*"worker"', '0.012*"’" + 0.011*"lack" + 0.007*"2022" + 0.007*"need" + 0.005*"quality" + 0.005*"practice" + 0.005*"means" + 0.005*"significant" + 0.005*"delay" + 0.005*"experiences"', '0.019*"’" + 0.010*"2022" + 0.009*"lack" + 0.007*"Solihull" + 0.006*"experiences" + 0.005*"significant" + 0.005*"need" + 0.005*"11" + 0.005*"quality" + 0.005*"risk"']</t>
   </si>
   <si>
     <t>80555</t>
@@ -3958,7 +3958,7 @@
     <t>0.198</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.010*"well" + 0.007*"needs" + 0.007*"Somerset" + 0.006*"plans" + 0.006*"leaders" + 0.005*"progress" + 0.005*"good" + 0.005*"supported" + 0.005*"understand"', '0.015*"’" + 0.007*"needs" + 0.006*"well" + 0.006*"good" + 0.005*"including" + 0.005*"plans" + 0.005*"number" + 0.005*"health" + 0.005*"practice" + 0.005*"Somerset"', '0.017*"’" + 0.010*"well" + 0.010*"needs" + 0.008*"Somerset" + 0.006*"good" + 0.006*"plans" + 0.006*"need" + 0.005*"supported" + 0.005*"positive" + 0.005*"range"']</t>
+    <t>['0.016*"’" + 0.007*"needs" + 0.007*"well" + 0.005*"need" + 0.005*"number" + 0.005*"good" + 0.005*"Somerset" + 0.005*"plans" + 0.005*"leaders" + 0.004*"progress"', '0.021*"’" + 0.010*"well" + 0.010*"needs" + 0.007*"plans" + 0.007*"good" + 0.006*"Somerset" + 0.006*"including" + 0.006*"supported" + 0.005*"leaders" + 0.005*"positive"', '0.012*"’" + 0.009*"Somerset" + 0.008*"well" + 0.007*"needs" + 0.006*"plans" + 0.005*"need" + 0.005*"leaders" + 0.005*"good" + 0.005*"supported" + 0.005*"practice"']</t>
   </si>
   <si>
     <t>80556</t>
@@ -3982,7 +3982,7 @@
     <t>0.1515</t>
   </si>
   <si>
-    <t>['0.011*"quality" + 0.011*"well" + 0.008*"plans" + 0.008*"’" + 0.007*"leaders" + 0.006*"good" + 0.006*"needs" + 0.005*"timely" + 0.005*"range" + 0.005*"progress"', '0.010*"quality" + 0.009*"’" + 0.008*"well" + 0.008*"good" + 0.008*"leaders" + 0.006*"plans" + 0.005*"timely" + 0.005*"progress" + 0.005*"practice" + 0.004*"◼"', '0.013*"well" + 0.010*"leaders" + 0.009*"quality" + 0.009*"’" + 0.008*"plans" + 0.007*"timely" + 0.007*"needs" + 0.006*"good" + 0.006*"progress" + 0.005*"practice"']</t>
+    <t>['0.013*"well" + 0.013*"quality" + 0.010*"’" + 0.008*"leaders" + 0.007*"plans" + 0.007*"timely" + 0.007*"needs" + 0.006*"progress" + 0.005*"good" + 0.005*"Senior"', '0.010*"well" + 0.009*"leaders" + 0.008*"good" + 0.008*"quality" + 0.006*"plans" + 0.005*"timely" + 0.005*"’" + 0.005*"progress" + 0.004*"always" + 0.004*"needs"', '0.011*"’" + 0.010*"plans" + 0.009*"quality" + 0.009*"well" + 0.008*"leaders" + 0.007*"good" + 0.006*"timely" + 0.005*"practice" + 0.005*"needs" + 0.005*"always"']</t>
   </si>
   <si>
     <t>80557</t>
@@ -4015,7 +4015,7 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>['0.029*"’" + 0.009*"needs" + 0.008*"Tyneside" + 0.007*"South" + 0.007*"oversight" + 0.005*"However" + 0.005*"carers" + 0.005*"practice" + 0.005*"15" + 0.005*"December"', '0.022*"’" + 0.009*"needs" + 0.008*"South" + 0.007*"Tyneside" + 0.006*"management" + 0.005*"effective" + 0.005*"carers" + 0.005*"2022" + 0.005*"well" + 0.005*"risk"', '0.020*"’" + 0.008*"needs" + 0.007*"South" + 0.006*"Tyneside" + 0.005*"14" + 0.005*"5" + 0.005*"effective" + 0.005*"9" + 0.004*"practice" + 0.004*"plans"']</t>
+    <t>['0.030*"’" + 0.011*"needs" + 0.009*"Tyneside" + 0.009*"South" + 0.006*"oversight" + 0.006*"practice" + 0.006*"effective" + 0.006*"9" + 0.005*"carers" + 0.005*"However"', '0.016*"’" + 0.007*"South" + 0.006*"needs" + 0.006*"Tyneside" + 0.005*"December" + 0.004*"However" + 0.004*"management" + 0.004*"2023" + 0.004*"risk" + 0.004*"plans"', '0.020*"’" + 0.008*"needs" + 0.006*"Tyneside" + 0.005*"management" + 0.005*"carers" + 0.004*"South" + 0.004*"December" + 0.004*"However" + 0.004*"progress" + 0.004*"effective"']</t>
   </si>
   <si>
     <t>80558</t>
@@ -4045,7 +4045,7 @@
     <t>28/07/23</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.005*"plans" + 0.005*"Southampton" + 0.005*"progress" + 0.005*"experiences" + 0.005*"improve" + 0.004*"5" + 0.004*"including" + 0.004*"provide" + 0.004*"needs"', '0.018*"’" + 0.006*"plans" + 0.006*"Southampton" + 0.005*"improve" + 0.005*"needs" + 0.004*"including" + 0.004*"16" + 0.004*"good" + 0.004*"progress" + 0.004*"June"', '0.016*"’" + 0.006*"plans" + 0.006*"Southampton" + 0.005*"5" + 0.005*"progress" + 0.004*"needs" + 0.004*"2023" + 0.004*"including" + 0.004*"improve" + 0.004*"well"']</t>
+    <t>['0.019*"’" + 0.006*"Southampton" + 0.006*"plans" + 0.005*"16" + 0.005*"5" + 0.005*"needs" + 0.005*"timely" + 0.004*"well" + 0.004*"progress" + 0.004*"including"', '0.013*"’" + 0.005*"improve" + 0.005*"Southampton" + 0.005*"progress" + 0.005*"plans" + 0.004*"needs" + 0.004*"experiences" + 0.003*"5" + 0.003*"provided" + 0.003*"leaders"', '0.014*"’" + 0.006*"plans" + 0.005*"Southampton" + 0.005*"including" + 0.005*"improve" + 0.005*"progress" + 0.004*"5" + 0.004*"good" + 0.004*"June" + 0.004*"2023"']</t>
   </si>
   <si>
     <t>80559</t>
@@ -4081,7 +4081,7 @@
     <t>0.1484</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"planning" + 0.006*"practice" + 0.006*"quality" + 0.005*"protection" + 0.005*"leaders" + 0.005*"number" + 0.005*"effective" + 0.005*"need" + 0.005*"risk"', '0.012*"’" + 0.009*"planning" + 0.008*"practice" + 0.008*"quality" + 0.006*"protection" + 0.006*"leaders" + 0.005*"risk" + 0.005*"number" + 0.005*"within" + 0.005*"needs"', '0.014*"’" + 0.007*"planning" + 0.006*"leaders" + 0.006*"practice" + 0.006*"quality" + 0.005*"need" + 0.005*"good" + 0.005*"always" + 0.005*"within" + 0.005*"number"']</t>
+    <t>['0.016*"’" + 0.009*"quality" + 0.008*"planning" + 0.007*"practice" + 0.006*"leaders" + 0.006*"within" + 0.005*"carers" + 0.005*"Southend" + 0.005*"number" + 0.005*"need"', '0.012*"’" + 0.009*"planning" + 0.007*"practice" + 0.006*"protection" + 0.006*"number" + 0.006*"leaders" + 0.006*"effective" + 0.005*"However" + 0.005*"always" + 0.005*"quality"', '0.010*"’" + 0.006*"planning" + 0.006*"leaders" + 0.006*"practice" + 0.005*"protection" + 0.005*"always" + 0.005*"risk" + 0.005*"within" + 0.005*"quality" + 0.004*"well"']</t>
   </si>
   <si>
     <t>80560</t>
@@ -4102,7 +4102,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50227184</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.008*"needs" + 0.007*"Helens" + 0.007*"St" + 0.007*"well" + 0.006*"receive" + 0.006*"good" + 0.005*"need" + 0.005*"risk" + 0.005*"10"', '0.017*"’" + 0.008*"St" + 0.007*"needs" + 0.007*"progress" + 0.007*"Helens" + 0.007*"well" + 0.005*"10" + 0.005*"risk" + 0.005*"21" + 0.005*"effective"', '0.016*"’" + 0.009*"Helens" + 0.007*"St" + 0.006*"21" + 0.006*"need" + 0.006*"well" + 0.006*"needs" + 0.006*"progress" + 0.006*"receive" + 0.005*"good"']</t>
+    <t>['0.018*"’" + 0.008*"St" + 0.008*"well" + 0.008*"Helens" + 0.007*"needs" + 0.006*"risk" + 0.006*"receive" + 0.006*"10" + 0.006*"need" + 0.006*"21"', '0.017*"’" + 0.007*"Helens" + 0.006*"needs" + 0.006*"progress" + 0.005*"St" + 0.005*"21" + 0.005*"good" + 0.005*"well" + 0.004*"need" + 0.004*"receive"', '0.012*"’" + 0.009*"St" + 0.008*"needs" + 0.008*"Helens" + 0.006*"progress" + 0.006*"well" + 0.006*"good" + 0.005*"need" + 0.005*"10" + 0.005*"receive"']</t>
   </si>
   <si>
     <t>80561</t>
@@ -4126,7 +4126,7 @@
     <t>0.1688</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.010*"needs" + 0.007*"quality" + 0.005*"health" + 0.005*"practice" + 0.005*"plans" + 0.004*"Staffordshire" + 0.004*"progress" + 0.004*"10" + 0.004*"ensure"', '0.018*"’" + 0.014*"needs" + 0.007*"ensure" + 0.007*"oversight" + 0.006*"Staffordshire" + 0.006*"progress" + 0.005*"practice" + 0.005*"health" + 0.005*"well" + 0.005*"quality"', '0.017*"’" + 0.010*"needs" + 0.007*"practice" + 0.007*"quality" + 0.006*"progress" + 0.006*"oversight" + 0.005*"health" + 0.005*"plans" + 0.005*"Staffordshire" + 0.005*"good"']</t>
+    <t>['0.021*"’" + 0.011*"needs" + 0.006*"quality" + 0.006*"health" + 0.006*"progress" + 0.005*"oversight" + 0.005*"practice" + 0.005*"ensure" + 0.005*"plans" + 0.005*"Staffordshire"', '0.015*"’" + 0.010*"needs" + 0.007*"quality" + 0.006*"Staffordshire" + 0.005*"practice" + 0.005*"oversight" + 0.005*"ensure" + 0.004*"10" + 0.004*"risk" + 0.004*"health"', '0.015*"’" + 0.013*"needs" + 0.006*"progress" + 0.006*"oversight" + 0.006*"ensure" + 0.006*"practice" + 0.005*"health" + 0.005*"6" + 0.005*"plans" + 0.005*"Staffordshire"']</t>
   </si>
   <si>
     <t>80562</t>
@@ -4156,7 +4156,7 @@
     <t>0.1882</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.007*"well" + 0.007*"needs" + 0.007*"practice" + 0.006*"Stockport" + 0.006*"risk" + 0.005*"quality" + 0.005*"plans" + 0.004*"March" + 0.004*"April"', '0.010*"’" + 0.007*"practice" + 0.007*"well" + 0.007*"Stockport" + 0.006*"needs" + 0.005*"plans" + 0.005*"risk" + 0.005*"strong" + 0.005*"leaders" + 0.005*"ensure"', '0.012*"’" + 0.010*"well" + 0.008*"practice" + 0.007*"strong" + 0.007*"Stockport" + 0.005*"plans" + 0.005*"leaders" + 0.005*"ensure" + 0.005*"28" + 0.005*"needs"']</t>
+    <t>['0.014*"’" + 0.008*"well" + 0.007*"needs" + 0.007*"strong" + 0.007*"practice" + 0.006*"Stockport" + 0.006*"plans" + 0.005*"risk" + 0.005*"team" + 0.005*"need"', '0.009*"’" + 0.008*"practice" + 0.008*"well" + 0.008*"Stockport" + 0.005*"needs" + 0.005*"risk" + 0.005*"strong" + 0.004*"leaders" + 0.004*"ensure" + 0.004*"plans"', '0.008*"well" + 0.008*"’" + 0.007*"practice" + 0.006*"Stockport" + 0.006*"needs" + 0.005*"ensure" + 0.004*"risk" + 0.004*"plans" + 0.004*"quality" + 0.004*"28"']</t>
   </si>
   <si>
     <t>80563</t>
@@ -4192,7 +4192,7 @@
     <t>0.1633</t>
   </si>
   <si>
-    <t>['0.020*"’" + 0.009*"leaders" + 0.008*"plans" + 0.007*"needs" + 0.006*"well" + 0.006*"on-Tees" + 0.006*"Stockton" + 0.006*"quality" + 0.005*"good" + 0.005*"senior"', '0.021*"’" + 0.009*"plans" + 0.009*"leaders" + 0.008*"well" + 0.007*"needs" + 0.007*"quality" + 0.006*"Stockton" + 0.006*"on-Tees" + 0.006*"good" + 0.005*"senior"', '0.017*"’" + 0.006*"leaders" + 0.006*"plans" + 0.005*"Stockton" + 0.005*"good" + 0.005*"on-Tees" + 0.004*"needs" + 0.004*"well" + 0.004*"2023" + 0.004*"education"']</t>
+    <t>['0.016*"’" + 0.009*"leaders" + 0.007*"needs" + 0.006*"plans" + 0.006*"on-Tees" + 0.006*"Stockton" + 0.005*"well" + 0.005*"quality" + 0.005*"good" + 0.005*"senior"', '0.025*"’" + 0.011*"plans" + 0.008*"leaders" + 0.007*"well" + 0.006*"Stockton" + 0.006*"on-Tees" + 0.006*"needs" + 0.006*"good" + 0.005*"senior" + 0.005*"quality"', '0.012*"’" + 0.008*"leaders" + 0.007*"quality" + 0.007*"needs" + 0.006*"well" + 0.005*"on-Tees" + 0.005*"good" + 0.005*"plans" + 0.005*"Stockton" + 0.005*"17"']</t>
   </si>
   <si>
     <t>80564</t>
@@ -4216,7 +4216,7 @@
     <t>0.172</t>
   </si>
   <si>
-    <t>['0.017*"’" + 0.007*"needs" + 0.006*"However" + 0.006*"Stoke" + 0.006*"on-Trent" + 0.006*"plans" + 0.005*"well" + 0.005*"14" + 0.005*"protection" + 0.005*"effectively"', '0.015*"’" + 0.008*"needs" + 0.007*"well" + 0.007*"Stoke" + 0.006*"However" + 0.005*"on-Trent" + 0.005*"progress" + 0.005*"ensure" + 0.005*"protection" + 0.005*"quality"', '0.020*"’" + 0.009*"needs" + 0.008*"plans" + 0.008*"on-Trent" + 0.007*"well" + 0.007*"Stoke" + 0.007*"However" + 0.006*"ensure" + 0.006*"protection" + 0.006*"quality"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.009*"Stoke" + 0.006*"well" + 0.006*"on-Trent" + 0.006*"progress" + 0.006*"However" + 0.006*"plans" + 0.005*"3" + 0.005*"quality"', '0.016*"’" + 0.007*"well" + 0.007*"plans" + 0.006*"on-Trent" + 0.006*"However" + 0.006*"protection" + 0.006*"needs" + 0.006*"Stoke" + 0.005*"progress" + 0.005*"practice"', '0.019*"’" + 0.009*"needs" + 0.007*"on-Trent" + 0.007*"well" + 0.007*"However" + 0.007*"plans" + 0.006*"ensure" + 0.006*"Stoke" + 0.005*"protection" + 0.005*"14"']</t>
   </si>
   <si>
     <t>80565</t>
@@ -4246,7 +4246,7 @@
     <t>21/05/19</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"progress" + 0.006*"well" + 0.006*"leaders" + 0.005*"effective" + 0.004*"needs" + 0.004*"practice" + 0.004*"Suffolk" + 0.004*"need" + 0.004*"high"', '0.014*"’" + 0.007*"well" + 0.006*"progress" + 0.006*"good" + 0.005*"effective" + 0.005*"practice" + 0.005*"leaders" + 0.005*"ensure" + 0.004*"carers" + 0.004*"need"', '0.012*"’" + 0.006*"well" + 0.005*"ensure" + 0.005*"good" + 0.005*"progress" + 0.004*"effective" + 0.003*"high" + 0.003*"effectively" + 0.003*"needs" + 0.003*"new"']</t>
+    <t>['0.017*"’" + 0.008*"well" + 0.006*"progress" + 0.005*"good" + 0.005*"leaders" + 0.004*"high" + 0.004*"Suffolk" + 0.004*"practice" + 0.004*"effective" + 0.004*"need"', '0.011*"’" + 0.006*"progress" + 0.006*"well" + 0.005*"ensure" + 0.005*"effective" + 0.005*"leaders" + 0.004*"good" + 0.004*"carers" + 0.004*"practice" + 0.004*"needs"', '0.012*"’" + 0.006*"progress" + 0.006*"effective" + 0.005*"well" + 0.005*"good" + 0.004*"needs" + 0.004*"ensure" + 0.004*"practice" + 0.004*"leaders" + 0.003*"effectively"']</t>
   </si>
   <si>
     <t>80566</t>
@@ -4279,7 +4279,7 @@
     <t>0.2141</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.007*"Sunderland" + 0.006*"quality" + 0.005*"well" + 0.005*"needs" + 0.005*"experienced" + 0.005*"result" + 0.005*"practice" + 0.004*"training" + 0.004*"highly"', '0.017*"’" + 0.008*"well" + 0.008*"quality" + 0.007*"needs" + 0.005*"good" + 0.005*"protection" + 0.005*"parents" + 0.005*"progress" + 0.005*"TfC" + 0.005*"council"', '0.016*"’" + 0.007*"well" + 0.006*"Sunderland" + 0.006*"needs" + 0.005*"quality" + 0.005*"experienced" + 0.005*"practice" + 0.004*"parents" + 0.004*"council" + 0.004*"highly"']</t>
+    <t>['0.015*"’" + 0.007*"well" + 0.007*"quality" + 0.005*"experienced" + 0.005*"Sunderland" + 0.005*"needs" + 0.005*"practice" + 0.005*"TfC" + 0.005*"protection" + 0.004*"good"', '0.015*"’" + 0.007*"well" + 0.007*"Sunderland" + 0.007*"needs" + 0.006*"quality" + 0.006*"council" + 0.005*"robust" + 0.005*"parents" + 0.005*"experienced" + 0.004*"protection"', '0.019*"’" + 0.007*"needs" + 0.007*"well" + 0.006*"quality" + 0.005*"Sunderland" + 0.004*"experienced" + 0.004*"practice" + 0.004*"TfC" + 0.004*"good" + 0.004*"highly"']</t>
   </si>
   <si>
     <t>80567</t>
@@ -4309,7 +4309,7 @@
     <t>0.1782</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"well" + 0.008*"needs" + 0.008*"practice" + 0.006*"progress" + 0.005*"carers" + 0.005*"effective" + 0.005*"plans" + 0.005*"quality" + 0.004*"Surrey"', '0.013*"’" + 0.013*"needs" + 0.009*"well" + 0.007*"practice" + 0.006*"progress" + 0.006*"plans" + 0.005*"effective" + 0.005*"good" + 0.005*"quality" + 0.005*"However"', '0.012*"’" + 0.009*"well" + 0.007*"progress" + 0.007*"practice" + 0.007*"needs" + 0.006*"17" + 0.005*"quality" + 0.005*"plans" + 0.005*"carers" + 0.005*"good"']</t>
+    <t>['0.015*"’" + 0.011*"needs" + 0.010*"well" + 0.008*"practice" + 0.006*"progress" + 0.006*"carers" + 0.006*"effective" + 0.005*"good" + 0.005*"17" + 0.005*"Surrey"', '0.009*"well" + 0.008*"’" + 0.007*"needs" + 0.006*"progress" + 0.005*"practice" + 0.005*"17" + 0.005*"good" + 0.004*"plans" + 0.004*"quality" + 0.004*"However"', '0.015*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"progress" + 0.006*"practice" + 0.006*"plans" + 0.005*"quality" + 0.005*"However" + 0.004*"effective" + 0.004*"good"']</t>
   </si>
   <si>
     <t>80568</t>
@@ -4333,7 +4333,7 @@
     <t>0.1489</t>
   </si>
   <si>
-    <t>['0.026*"’" + 0.013*"needs" + 0.009*"Swindon" + 0.008*"well" + 0.008*"plans" + 0.007*"always" + 0.007*"need" + 0.006*"health" + 0.005*"impact" + 0.005*"effective"', '0.019*"’" + 0.010*"needs" + 0.009*"Swindon" + 0.007*"well" + 0.007*"need" + 0.006*"plans" + 0.005*"always" + 0.005*"effective" + 0.005*"education" + 0.005*"health"', '0.020*"’" + 0.015*"needs" + 0.011*"need" + 0.009*"Swindon" + 0.008*"well" + 0.007*"always" + 0.006*"impact" + 0.006*"Council" + 0.005*"many" + 0.005*"plans"']</t>
+    <t>['0.025*"’" + 0.013*"needs" + 0.010*"Swindon" + 0.010*"need" + 0.008*"well" + 0.007*"always" + 0.007*"plans" + 0.006*"impact" + 0.006*"health" + 0.005*"effective"', '0.022*"’" + 0.013*"needs" + 0.009*"Swindon" + 0.008*"well" + 0.007*"need" + 0.006*"plans" + 0.006*"always" + 0.006*"17" + 0.006*"effective" + 0.006*"home"', '0.018*"’" + 0.012*"needs" + 0.008*"need" + 0.007*"Swindon" + 0.007*"well" + 0.006*"plans" + 0.006*"always" + 0.005*"risk" + 0.005*"Borough" + 0.005*"lack"']</t>
   </si>
   <si>
     <t>80569</t>
@@ -4360,7 +4360,7 @@
     <t>0.1495</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"needs" + 0.006*"practice" + 0.006*"risk" + 0.005*"4" + 0.005*"2023" + 0.005*"experiences" + 0.005*"impact" + 0.005*"◼" + 0.005*"quality"', '0.016*"’" + 0.008*"needs" + 0.006*"impact" + 0.006*"2023" + 0.005*"understand" + 0.005*"risk" + 0.005*"planning" + 0.005*"response" + 0.004*"protection" + 0.004*"quality"', '0.018*"’" + 0.010*"needs" + 0.007*"risk" + 0.006*"impact" + 0.006*"quality" + 0.006*"experienced" + 0.006*"15" + 0.006*"response" + 0.005*"Tameside" + 0.005*"4"']</t>
+    <t>['0.015*"’" + 0.009*"needs" + 0.006*"2023" + 0.006*"practice" + 0.006*"risk" + 0.005*"progress" + 0.005*"4" + 0.005*"Tameside" + 0.005*"protection" + 0.004*"planning"', '0.018*"’" + 0.008*"needs" + 0.007*"quality" + 0.007*"impact" + 0.007*"risk" + 0.006*"experiences" + 0.005*"experienced" + 0.005*"plans" + 0.005*"4" + 0.005*"practice"', '0.015*"’" + 0.009*"needs" + 0.006*"impact" + 0.006*"experienced" + 0.006*"response" + 0.005*"risk" + 0.005*"15" + 0.005*"practice" + 0.005*"4" + 0.004*"Tameside"']</t>
   </si>
   <si>
     <t>80570</t>
@@ -4384,7 +4384,7 @@
     <t>0.2186</t>
   </si>
   <si>
-    <t>['0.010*"’" + 0.009*"well" + 0.006*"plans" + 0.006*"needs" + 0.005*"effective" + 0.005*"planning" + 0.005*"need" + 0.005*"ensure" + 0.004*"leaders" + 0.004*"Senior"', '0.022*"’" + 0.009*"well" + 0.007*"effective" + 0.006*"needs" + 0.005*"practice" + 0.005*"strong" + 0.005*"ensure" + 0.005*"benefit" + 0.005*"understand" + 0.004*"planning"', '0.015*"’" + 0.014*"well" + 0.010*"needs" + 0.008*"effective" + 0.006*"strong" + 0.006*"plans" + 0.006*"need" + 0.005*"practice" + 0.005*"improve" + 0.005*"ensure"']</t>
+    <t>['0.017*"’" + 0.009*"well" + 0.008*"effective" + 0.008*"needs" + 0.006*"plans" + 0.005*"strong" + 0.005*"practice" + 0.005*"need" + 0.005*"improve" + 0.005*"family"', '0.010*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"effective" + 0.005*"plans" + 0.005*"planning" + 0.005*"ensure" + 0.004*"improve" + 0.004*"carers" + 0.004*"strong"', '0.019*"’" + 0.013*"well" + 0.008*"needs" + 0.007*"effective" + 0.006*"need" + 0.006*"strong" + 0.005*"ensure" + 0.005*"practice" + 0.005*"plans" + 0.005*"timely"']</t>
   </si>
   <si>
     <t>80571</t>
@@ -4408,7 +4408,7 @@
     <t>0.164</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"need" + 0.004*"needs" + 0.004*"ensure" + 0.004*"effective" + 0.004*"leaders" + 0.004*"quality" + 0.004*"protection"', '0.014*"’" + 0.008*"well" + 0.006*"carers" + 0.005*"need" + 0.005*"practice" + 0.004*"needs" + 0.004*"Thurrock" + 0.004*"effective" + 0.004*"protection" + 0.004*"ensure"', '0.012*"’" + 0.008*"well" + 0.005*"need" + 0.005*"carers" + 0.004*"needs" + 0.004*"Thurrock" + 0.004*"ensure" + 0.004*"practice" + 0.004*"leaders" + 0.003*"protect"']</t>
+    <t>['0.016*"’" + 0.010*"well" + 0.007*"carers" + 0.006*"need" + 0.005*"needs" + 0.005*"ensure" + 0.004*"practice" + 0.004*"impact" + 0.003*"parents" + 0.003*"protect"', '0.008*"’" + 0.006*"well" + 0.004*"Thurrock" + 0.004*"carers" + 0.004*"need" + 0.004*"effective" + 0.003*"protection" + 0.003*"needs" + 0.003*"training" + 0.003*"quality"', '0.013*"’" + 0.008*"well" + 0.005*"carers" + 0.005*"leaders" + 0.005*"practice" + 0.004*"need" + 0.004*"effective" + 0.004*"needs" + 0.004*"Thurrock" + 0.003*"ensure"']</t>
   </si>
   <si>
     <t>80572</t>
@@ -4432,7 +4432,7 @@
     <t>0.2197</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.010*"well" + 0.008*"Torbay" + 0.006*"needs" + 0.005*"effective" + 0.005*"team" + 0.005*"good" + 0.005*"progress" + 0.004*"1" + 0.004*"ensure"', '0.017*"’" + 0.009*"well" + 0.007*"Torbay" + 0.007*"good" + 0.006*"needs" + 0.005*"effective" + 0.005*"plans" + 0.005*"timely" + 0.004*"supported" + 0.004*"agencies"', '0.017*"’" + 0.008*"well" + 0.006*"Torbay" + 0.005*"good" + 0.005*"needs" + 0.005*"21" + 0.004*"quality" + 0.004*"2022" + 0.004*"progress" + 0.004*"effective"']</t>
+    <t>['0.014*"’" + 0.008*"Torbay" + 0.006*"well" + 0.006*"good" + 0.005*"effective" + 0.005*"needs" + 0.004*"agencies" + 0.004*"21" + 0.004*"team" + 0.004*"need"', '0.018*"’" + 0.011*"well" + 0.007*"needs" + 0.006*"Torbay" + 0.006*"good" + 0.006*"effective" + 0.005*"team" + 0.005*"21" + 0.005*"timely" + 0.004*"progress"', '0.017*"’" + 0.009*"well" + 0.008*"Torbay" + 0.005*"good" + 0.005*"needs" + 0.005*"progress" + 0.005*"March" + 0.005*"2022" + 0.005*"timely" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>80573</t>
@@ -4456,7 +4456,7 @@
     <t>0.1589</t>
   </si>
   <si>
-    <t>['0.015*"’" + 0.009*"well" + 0.009*"Trafford" + 0.008*"needs" + 0.006*"leaders" + 0.006*"quality" + 0.005*"plans" + 0.005*"team" + 0.004*"November" + 0.004*"education"', '0.012*"’" + 0.009*"needs" + 0.008*"Trafford" + 0.006*"quality" + 0.006*"plans" + 0.006*"well" + 0.005*"leaders" + 0.005*"practice" + 0.005*"21" + 0.004*"education"', '0.020*"’" + 0.010*"needs" + 0.009*"plans" + 0.007*"quality" + 0.007*"Trafford" + 0.006*"practice" + 0.006*"well" + 0.005*"impact" + 0.005*"2" + 0.005*"placed"']</t>
+    <t>['0.013*"’" + 0.007*"needs" + 0.007*"Trafford" + 0.007*"quality" + 0.006*"plans" + 0.006*"well" + 0.005*"team" + 0.005*"practice" + 0.004*"ensure" + 0.004*"impact"', '0.017*"’" + 0.010*"needs" + 0.009*"Trafford" + 0.008*"plans" + 0.007*"quality" + 0.006*"well" + 0.006*"leaders" + 0.005*"placed" + 0.005*"practice" + 0.005*"2"', '0.018*"’" + 0.010*"needs" + 0.008*"well" + 0.007*"Trafford" + 0.006*"plans" + 0.006*"leaders" + 0.006*"quality" + 0.005*"practice" + 0.004*"impact" + 0.004*"21"']</t>
   </si>
   <si>
     <t>80574</t>
@@ -4480,7 +4480,7 @@
     <t>0.1829</t>
   </si>
   <si>
-    <t>['0.025*"’" + 0.007*"needs" + 0.007*"leaders" + 0.006*"well" + 0.006*"Walsall" + 0.005*"4" + 0.005*"Senior" + 0.005*"2021" + 0.005*"information" + 0.005*"good"', '0.018*"’" + 0.007*"leaders" + 0.007*"well" + 0.006*"needs" + 0.005*"Walsall" + 0.005*"4" + 0.004*"15" + 0.004*"oversight" + 0.004*"practice" + 0.004*"October"', '0.019*"’" + 0.008*"leaders" + 0.006*"oversight" + 0.005*"needs" + 0.005*"information" + 0.005*"Walsall" + 0.005*"supported" + 0.004*"well" + 0.004*"good" + 0.004*"Senior"']</t>
+    <t>['0.017*"’" + 0.006*"leaders" + 0.005*"well" + 0.005*"needs" + 0.005*"Walsall" + 0.004*"Senior" + 0.004*"4" + 0.004*"information" + 0.003*"plans" + 0.003*"15"', '0.015*"’" + 0.007*"leaders" + 0.006*"needs" + 0.005*"well" + 0.005*"Walsall" + 0.005*"good" + 0.005*"4" + 0.004*"practice" + 0.004*"information" + 0.004*"Senior"', '0.027*"’" + 0.008*"leaders" + 0.007*"needs" + 0.006*"well" + 0.005*"oversight" + 0.005*"Walsall" + 0.005*"information" + 0.005*"2021" + 0.005*"4" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80575</t>
@@ -4510,7 +4510,7 @@
     <t>19/08/19</t>
   </si>
   <si>
-    <t>['0.019*"’" + 0.008*"well" + 0.006*"practice" + 0.005*"Senior" + 0.005*"carers" + 0.004*"plans" + 0.004*"good" + 0.004*"small" + 0.004*"number" + 0.004*"need"', '0.013*"’" + 0.008*"practice" + 0.007*"well" + 0.006*"plans" + 0.005*"number" + 0.004*"information" + 0.004*"progress" + 0.004*"Senior" + 0.004*"need" + 0.004*"needs"', '0.008*"’" + 0.004*"progress" + 0.004*"practice" + 0.004*"home" + 0.004*"Senior" + 0.004*"well" + 0.004*"number" + 0.004*"good" + 0.003*"need" + 0.003*"carers"']</t>
+    <t>['0.012*"’" + 0.007*"practice" + 0.006*"well" + 0.005*"plans" + 0.005*"good" + 0.004*"number" + 0.004*"information" + 0.004*"progress" + 0.004*"need" + 0.004*"carers"', '0.018*"’" + 0.007*"well" + 0.005*"Senior" + 0.005*"practice" + 0.005*"number" + 0.004*"home" + 0.004*"plans" + 0.004*"need" + 0.004*"carers" + 0.004*"progress"', '0.012*"’" + 0.006*"practice" + 0.006*"well" + 0.004*"information" + 0.004*"needs" + 0.004*"progress" + 0.004*"good" + 0.004*"provided" + 0.004*"plans" + 0.004*"small"']</t>
   </si>
   <si>
     <t>80576</t>
@@ -4540,7 +4540,7 @@
     <t>0.185</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.007*"needs" + 0.006*"Warwickshire" + 0.006*"well" + 0.006*"plans" + 0.005*"good" + 0.005*"practice" + 0.005*"progress" + 0.004*"carers" + 0.004*"November"', '0.013*"’" + 0.007*"plans" + 0.006*"needs" + 0.005*"well" + 0.005*"Warwickshire" + 0.005*"clear" + 0.004*"information" + 0.004*"Senior" + 0.004*"effective" + 0.004*"carers"', '0.009*"’" + 0.008*"well" + 0.006*"Warwickshire" + 0.006*"plans" + 0.006*"needs" + 0.005*"practice" + 0.005*"3" + 0.005*"carers" + 0.004*"good" + 0.004*"2021"']</t>
+    <t>['0.011*"’" + 0.009*"well" + 0.007*"needs" + 0.006*"plans" + 0.006*"Warwickshire" + 0.005*"practice" + 0.004*"3" + 0.004*"effective" + 0.004*"carers" + 0.004*"clear"', '0.013*"’" + 0.007*"Warwickshire" + 0.007*"plans" + 0.006*"needs" + 0.006*"good" + 0.005*"information" + 0.005*"3" + 0.005*"carers" + 0.005*"practice" + 0.005*"supported"', '0.012*"’" + 0.006*"needs" + 0.005*"well" + 0.005*"progress" + 0.005*"plans" + 0.004*"good" + 0.004*"carers" + 0.004*"practice" + 0.004*"22" + 0.004*"Warwickshire"']</t>
   </si>
   <si>
     <t>80577</t>
@@ -4564,7 +4564,7 @@
     <t>14/03/2022</t>
   </si>
   <si>
-    <t>['0.018*"’" + 0.006*"West" + 0.006*"well" + 0.006*"Berkshire" + 0.005*"needs" + 0.004*"18" + 0.004*"plans" + 0.004*"early" + 0.004*"progress" + 0.004*"March"', '0.013*"’" + 0.007*"Berkshire" + 0.006*"West" + 0.006*"well" + 0.004*"need" + 0.004*"working" + 0.004*"14" + 0.004*"agency" + 0.004*"plans" + 0.004*"strong"', '0.012*"’" + 0.007*"West" + 0.006*"Berkshire" + 0.006*"well" + 0.004*"need" + 0.004*"plans" + 0.004*"needs" + 0.004*"working" + 0.004*"14" + 0.004*"2022"']</t>
+    <t>['0.015*"’" + 0.006*"well" + 0.006*"Berkshire" + 0.006*"West" + 0.004*"needs" + 0.004*"14" + 0.004*"plans" + 0.004*"early" + 0.004*"education" + 0.004*"March"', '0.013*"’" + 0.008*"West" + 0.006*"Berkshire" + 0.005*"well" + 0.004*"plans" + 0.004*"18" + 0.004*"need" + 0.004*"practice" + 0.003*"working" + 0.003*"needs"', '0.015*"’" + 0.006*"Berkshire" + 0.006*"West" + 0.006*"well" + 0.005*"need" + 0.005*"agency" + 0.004*"2022" + 0.004*"needs" + 0.004*"working" + 0.004*"plans"']</t>
   </si>
   <si>
     <t>2637548</t>
@@ -4588,7 +4588,7 @@
     <t>0.1588</t>
   </si>
   <si>
-    <t>['0.016*"’" + 0.007*"quality" + 0.006*"Northamptonshire" + 0.005*"practice" + 0.005*"well" + 0.004*"West" + 0.004*"NCT" + 0.004*"needs" + 0.004*"plans" + 0.004*"health"', '0.017*"’" + 0.008*"Northamptonshire" + 0.008*"West" + 0.005*"practice" + 0.005*"well" + 0.005*"quality" + 0.005*"NCT" + 0.005*"experiences" + 0.004*"impact" + 0.004*"2022"', '0.018*"’" + 0.009*"Northamptonshire" + 0.008*"well" + 0.007*"quality" + 0.007*"West" + 0.006*"needs" + 0.005*"practice" + 0.005*"need" + 0.005*"3" + 0.005*"plans"']</t>
+    <t>['0.013*"’" + 0.007*"Northamptonshire" + 0.006*"quality" + 0.006*"West" + 0.005*"well" + 0.005*"practice" + 0.005*"3" + 0.005*"needs" + 0.004*"14" + 0.004*"plans"', '0.019*"’" + 0.008*"Northamptonshire" + 0.007*"West" + 0.006*"quality" + 0.006*"well" + 0.006*"needs" + 0.005*"NCT" + 0.005*"impact" + 0.005*"practice" + 0.005*"experiences"', '0.019*"’" + 0.009*"Northamptonshire" + 0.007*"well" + 0.006*"quality" + 0.006*"West" + 0.005*"practice" + 0.004*"NCT" + 0.004*"needs" + 0.004*"need" + 0.004*"experiences"']</t>
   </si>
   <si>
     <t>80578</t>
@@ -4612,7 +4612,7 @@
     <t>0.1513</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.007*"plans" + 0.006*"well" + 0.006*"needs" + 0.006*"Sussex" + 0.005*"13" + 0.005*"quality" + 0.005*"health" + 0.005*"West" + 0.004*"24"', '0.012*"’" + 0.006*"plans" + 0.005*"well" + 0.005*"West" + 0.004*"needs" + 0.004*"education" + 0.004*"13" + 0.004*"quality" + 0.004*"Sussex" + 0.004*"number"', '0.015*"’" + 0.007*"well" + 0.006*"needs" + 0.005*"plans" + 0.005*"supported" + 0.005*"number" + 0.005*"Sussex" + 0.005*"West" + 0.005*"13" + 0.005*"practice"']</t>
+    <t>['0.010*"’" + 0.006*"well" + 0.006*"plans" + 0.006*"quality" + 0.005*"Sussex" + 0.005*"needs" + 0.005*"health" + 0.004*"13" + 0.004*"supported" + 0.004*"clear"', '0.018*"’" + 0.007*"well" + 0.006*"plans" + 0.005*"West" + 0.005*"needs" + 0.005*"supported" + 0.005*"13" + 0.004*"Sussex" + 0.004*"planning" + 0.004*"number"', '0.013*"’" + 0.007*"needs" + 0.007*"plans" + 0.005*"well" + 0.005*"Sussex" + 0.005*"number" + 0.005*"West" + 0.005*"13" + 0.004*"health" + 0.004*"impact"']</t>
   </si>
   <si>
     <t>80579</t>
@@ -4633,7 +4633,7 @@
     <t>https://files.ofsted.gov.uk/v1/file/50187563</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"practice" + 0.008*"plans" + 0.007*"May" + 0.007*"quality" + 0.006*"Wigan" + 0.006*"needs" + 0.005*"appropriate" + 0.005*"timely" + 0.005*"20"', '0.012*"’" + 0.008*"May" + 0.007*"plans" + 0.006*"needs" + 0.006*"Wigan" + 0.006*"practice" + 0.006*"appropriate" + 0.006*"leaders" + 0.005*"quality" + 0.005*"9"', '0.010*"’" + 0.007*"May" + 0.005*"Wigan" + 0.005*"needs" + 0.005*"practice" + 0.004*"quality" + 0.004*"9" + 0.004*"20" + 0.004*"appropriate" + 0.004*"2022"']</t>
+    <t>['0.012*"’" + 0.007*"practice" + 0.007*"May" + 0.006*"quality" + 0.006*"plans" + 0.005*"Wigan" + 0.005*"needs" + 0.005*"appropriate" + 0.005*"leaders" + 0.005*"timely"', '0.014*"’" + 0.008*"needs" + 0.008*"plans" + 0.007*"May" + 0.006*"practice" + 0.006*"Wigan" + 0.005*"timely" + 0.005*"appropriate" + 0.005*"leaders" + 0.005*"quality"', '0.012*"’" + 0.008*"May" + 0.006*"Wigan" + 0.006*"appropriate" + 0.006*"plans" + 0.006*"practice" + 0.006*"quality" + 0.005*"9" + 0.005*"needs" + 0.004*"due"']</t>
   </si>
   <si>
     <t>80580</t>
@@ -4666,7 +4666,7 @@
     <t>0.1708</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"well" + 0.007*"progress" + 0.007*"need" + 0.006*"needs" + 0.006*"parents" + 0.006*"risk" + 0.006*"including" + 0.005*"supported" + 0.005*"ensure"', '0.019*"’" + 0.010*"well" + 0.006*"needs" + 0.006*"parents" + 0.006*"need" + 0.005*"plans" + 0.005*"Wiltshire" + 0.005*"including" + 0.005*"quality" + 0.004*"progress"', '0.013*"’" + 0.011*"well" + 0.009*"needs" + 0.007*"Wiltshire" + 0.007*"risk" + 0.007*"need" + 0.006*"supported" + 0.006*"plans" + 0.006*"quality" + 0.006*"ensure"']</t>
+    <t>['0.016*"’" + 0.009*"well" + 0.006*"need" + 0.006*"needs" + 0.005*"parents" + 0.005*"progress" + 0.004*"plans" + 0.004*"Wiltshire" + 0.004*"family" + 0.004*"education"', '0.017*"’" + 0.012*"well" + 0.008*"needs" + 0.007*"risk" + 0.007*"need" + 0.007*"progress" + 0.007*"supported" + 0.006*"parents" + 0.006*"ensure" + 0.006*"Wiltshire"', '0.012*"’" + 0.011*"well" + 0.007*"Wiltshire" + 0.007*"needs" + 0.006*"including" + 0.005*"need" + 0.005*"plans" + 0.005*"quality" + 0.005*"parents" + 0.005*"progress"']</t>
   </si>
   <si>
     <t>80581</t>
@@ -4696,7 +4696,7 @@
     <t>0.1655</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.012*"needs" + 0.008*"Wirral" + 0.007*"ensure" + 0.006*"plans" + 0.006*"practice" + 0.006*"small" + 0.005*"response" + 0.005*"good" + 0.005*"well"', '0.009*"needs" + 0.008*"’" + 0.007*"plans" + 0.006*"Wirral" + 0.006*"ensure" + 0.005*"well" + 0.005*"practice" + 0.004*"e" + 0.004*"number" + 0.004*"September"', '0.010*"’" + 0.008*"ensure" + 0.007*"Wirral" + 0.007*"practice" + 0.007*"needs" + 0.006*"plans" + 0.006*"number" + 0.006*"well" + 0.006*"18" + 0.005*"risk"']</t>
+    <t>['0.012*"’" + 0.010*"needs" + 0.008*"Wirral" + 0.006*"ensure" + 0.006*"practice" + 0.006*"small" + 0.005*"plans" + 0.005*"well" + 0.005*"number" + 0.005*"response"', '0.012*"’" + 0.010*"needs" + 0.009*"ensure" + 0.007*"Wirral" + 0.006*"good" + 0.006*"plans" + 0.006*"well" + 0.006*"practice" + 0.005*"risk" + 0.005*"number"', '0.009*"plans" + 0.008*"’" + 0.008*"needs" + 0.006*"Wirral" + 0.006*"ensure" + 0.006*"practice" + 0.005*"18" + 0.005*"well" + 0.005*"number" + 0.004*"appropriate"']</t>
   </si>
   <si>
     <t>80582</t>
@@ -4720,7 +4720,7 @@
     <t>0.1777</t>
   </si>
   <si>
-    <t>['0.013*"’" + 0.008*"plans" + 0.007*"needs" + 0.006*"effective" + 0.005*"progress" + 0.005*"6" + 0.005*"well" + 0.005*"experiences" + 0.005*"17" + 0.005*"provided"', '0.015*"’" + 0.006*"progress" + 0.006*"effective" + 0.006*"needs" + 0.006*"well" + 0.005*"impact" + 0.005*"experiences" + 0.005*"provided" + 0.005*"quality" + 0.005*"plans"', '0.008*"’" + 0.007*"plans" + 0.006*"effective" + 0.005*"provided" + 0.005*"well" + 0.004*"17" + 0.004*"progress" + 0.004*"clear" + 0.004*"appropriate" + 0.004*"needs"']</t>
+    <t>['0.013*"’" + 0.007*"effective" + 0.007*"plans" + 0.006*"needs" + 0.005*"well" + 0.005*"17" + 0.005*"progress" + 0.005*"6" + 0.005*"appropriate" + 0.004*"experiences"', '0.012*"’" + 0.007*"plans" + 0.005*"well" + 0.005*"needs" + 0.005*"effective" + 0.004*"Wokingham" + 0.004*"quality" + 0.004*"protection" + 0.004*"good" + 0.004*"oversight"', '0.013*"’" + 0.007*"progress" + 0.006*"provided" + 0.006*"effective" + 0.006*"needs" + 0.006*"plans" + 0.005*"experiences" + 0.005*"impact" + 0.005*"quality" + 0.005*"well"']</t>
   </si>
   <si>
     <t>80583</t>
@@ -4744,7 +4744,7 @@
     <t>0.1898</t>
   </si>
   <si>
-    <t>['0.014*"’" + 0.009*"needs" + 0.006*"Wolverhampton" + 0.006*"effective" + 0.005*"receive" + 0.005*"risks" + 0.005*"plans" + 0.005*"leaders" + 0.005*"risk" + 0.005*"education"', '0.014*"’" + 0.009*"needs" + 0.007*"effective" + 0.005*"quality" + 0.005*"Wolverhampton" + 0.005*"supported" + 0.005*"strong" + 0.005*"plans" + 0.005*"risks" + 0.004*"City"', '0.015*"’" + 0.005*"Wolverhampton" + 0.005*"leaders" + 0.005*"plans" + 0.005*"needs" + 0.005*"risks" + 0.005*"effective" + 0.005*"supported" + 0.004*"receive" + 0.004*"practice"']</t>
+    <t>['0.010*"’" + 0.006*"needs" + 0.005*"receive" + 0.005*"risks" + 0.005*"Wolverhampton" + 0.005*"risk" + 0.005*"effective" + 0.004*"practice" + 0.004*"strong" + 0.004*"28"', '0.014*"’" + 0.008*"needs" + 0.006*"plans" + 0.006*"Wolverhampton" + 0.005*"effective" + 0.005*"risks" + 0.005*"strong" + 0.004*"practice" + 0.004*"leaders" + 0.004*"quality"', '0.017*"’" + 0.008*"needs" + 0.007*"effective" + 0.006*"Wolverhampton" + 0.005*"quality" + 0.005*"leaders" + 0.005*"education" + 0.005*"supported" + 0.005*"plans" + 0.005*"receive"']</t>
   </si>
   <si>
     <t>80584</t>
@@ -4774,7 +4774,7 @@
     <t>0.1925</t>
   </si>
   <si>
-    <t>['0.021*"’" + 0.009*"plans" + 0.008*"Worcestershire" + 0.007*"well" + 0.007*"progress" + 0.006*"needs" + 0.006*"leaders" + 0.005*"ensure" + 0.005*"26" + 0.005*"appropriate"', '0.021*"’" + 0.010*"needs" + 0.007*"well" + 0.007*"progress" + 0.007*"plans" + 0.007*"leaders" + 0.006*"Worcestershire" + 0.006*"appropriate" + 0.006*"ensure" + 0.005*"Senior"', '0.012*"’" + 0.011*"well" + 0.007*"plans" + 0.007*"leaders" + 0.006*"Worcestershire" + 0.006*"ensure" + 0.005*"needs" + 0.005*"appropriate" + 0.005*"living" + 0.004*"progress"']</t>
+    <t>['0.015*"’" + 0.008*"plans" + 0.006*"needs" + 0.006*"ensure" + 0.006*"well" + 0.006*"appropriate" + 0.006*"progress" + 0.005*"Worcestershire" + 0.005*"PAs" + 0.005*"leaders"', '0.020*"’" + 0.010*"well" + 0.009*"needs" + 0.007*"Worcestershire" + 0.007*"progress" + 0.006*"plans" + 0.006*"leaders" + 0.006*"appropriate" + 0.006*"ensure" + 0.005*"making"', '0.021*"’" + 0.009*"well" + 0.008*"plans" + 0.008*"leaders" + 0.007*"Worcestershire" + 0.007*"progress" + 0.007*"needs" + 0.005*"ensure" + 0.005*"However" + 0.005*"improve"']</t>
   </si>
   <si>
     <t>urn</t>

</xml_diff>